<commit_message>
Manual calibration of the Philippines
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="315" windowWidth="20370" windowHeight="7530" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="375" windowWidth="20370" windowHeight="7470" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="control_panel" sheetId="4" r:id="rId1"/>
     <sheet name="dropdown_lists" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -98,9 +99,6 @@
     <t>country</t>
   </si>
   <si>
-    <t>Fiji</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -114,6 +112,9 @@
   </si>
   <si>
     <t>runge_kutta</t>
+  </si>
+  <si>
+    <t>Philippines</t>
   </si>
 </sst>
 </file>
@@ -123,7 +124,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,8 +160,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +223,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -409,7 +422,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="663">
+  <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -1073,8 +1086,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1118,11 +1132,13 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="663" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="663">
+  <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
     <cellStyle name="Comma 2 2" xfId="5"/>
     <cellStyle name="Input 2" xfId="3"/>
+    <cellStyle name="Neutral" xfId="663" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="6"/>
     <cellStyle name="Normal 2" xfId="2"/>
@@ -2087,16 +2103,16 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2104,7 +2120,7 @@
         <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2156,7 +2172,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="9"/>
     </row>
@@ -2203,7 +2219,9 @@
       <c r="E10" s="42">
         <v>4</v>
       </c>
-      <c r="F10" s="42"/>
+      <c r="F10" s="42">
+        <v>5</v>
+      </c>
       <c r="G10" s="42"/>
       <c r="H10" s="42"/>
       <c r="I10" s="42"/>
@@ -2265,6 +2283,7 @@
       <c r="B17" s="36">
         <v>0.1</v>
       </c>
+      <c r="C17" s="43"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
@@ -2287,7 +2306,7 @@
         <v>11</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -2406,7 +2425,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -2417,21 +2436,21 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow different times to commence treatment
Will allow simulation of decrease in time to starting treatment with
GeneXpert.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2105,7 +2105,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,27 +2214,13 @@
       <c r="B10" s="41">
         <v>1</v>
       </c>
-      <c r="C10" s="42">
-        <v>2</v>
-      </c>
-      <c r="D10" s="42">
-        <v>3</v>
-      </c>
-      <c r="E10" s="42">
-        <v>4</v>
-      </c>
-      <c r="F10" s="42">
-        <v>5</v>
-      </c>
-      <c r="G10" s="42">
-        <v>6</v>
-      </c>
-      <c r="H10" s="42">
-        <v>7</v>
-      </c>
-      <c r="I10" s="42">
-        <v>8</v>
-      </c>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Implement a decreased time to treatment scenario
Still needs work, but the principle of decreasing time to treatment
commencement through GeneXpert is there. (It has no effect.)
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -113,7 +113,7 @@
     <t>runge_kutta</t>
   </si>
   <si>
-    <t>Philippines</t>
+    <t>Fiji</t>
   </si>
 </sst>
 </file>
@@ -2105,7 +2105,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2176,7 +2176,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C6" s="9"/>
     </row>
@@ -2214,8 +2214,12 @@
       <c r="B10" s="41">
         <v>1</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
+      <c r="C10" s="42">
+        <v>2</v>
+      </c>
+      <c r="D10" s="42">
+        <v>3</v>
+      </c>
       <c r="E10" s="42"/>
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>

</xml_diff>

<commit_message>
Separate GeneXpert off as a separate program
Rather than just having a scenario that allows for parameter values to
be modified by Xpert.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2105,7 +2105,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2211,15 +2211,9 @@
       <c r="A10" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="41">
-        <v>1</v>
-      </c>
-      <c r="C10" s="42">
-        <v>2</v>
-      </c>
-      <c r="D10" s="42">
-        <v>3</v>
-      </c>
+      <c r="B10" s="41"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
       <c r="E10" s="42"/>
       <c r="F10" s="42"/>
       <c r="G10" s="42"/>
@@ -2281,7 +2275,7 @@
         <v>23</v>
       </c>
       <c r="B17" s="36">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="C17" s="43"/>
     </row>

</xml_diff>

<commit_message>
Allow time steps/points to be set
Set these as model attributes and move make_times out of __init__, so
that it can be set external to the object.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2211,15 +2211,33 @@
       <c r="A10" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="33"/>
+      <c r="B10" s="41">
+        <v>1</v>
+      </c>
+      <c r="C10" s="42">
+        <v>2</v>
+      </c>
+      <c r="D10" s="42">
+        <v>3</v>
+      </c>
+      <c r="E10" s="42">
+        <v>4</v>
+      </c>
+      <c r="F10" s="42">
+        <v>5</v>
+      </c>
+      <c r="G10" s="42">
+        <v>6</v>
+      </c>
+      <c r="H10" s="42">
+        <v>7</v>
+      </c>
+      <c r="I10" s="42">
+        <v>8</v>
+      </c>
+      <c r="J10" s="33">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">

</xml_diff>

<commit_message>
Allow initial compartment setting outside model
Also some changes to scenarios in spreadsheets.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2105,7 +2105,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2235,9 +2235,7 @@
       <c r="I10" s="42">
         <v>8</v>
       </c>
-      <c r="J10" s="33">
-        <v>9</v>
-      </c>
+      <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">

</xml_diff>

<commit_message>
Fix code that prevents figures overlapping
Fix up the figure number code that prevents figures printing on the same
axes.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2105,7 +2105,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,27 +2214,13 @@
       <c r="B10" s="41">
         <v>1</v>
       </c>
-      <c r="C10" s="42">
-        <v>2</v>
-      </c>
-      <c r="D10" s="42">
-        <v>3</v>
-      </c>
-      <c r="E10" s="42">
-        <v>4</v>
-      </c>
-      <c r="F10" s="42">
-        <v>5</v>
-      </c>
-      <c r="G10" s="42">
-        <v>6</v>
-      </c>
-      <c r="H10" s="42">
-        <v>7</v>
-      </c>
-      <c r="I10" s="42">
-        <v>8</v>
-      </c>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Current scenarios updated in spreadsheets
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2105,7 +2105,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2214,14 +2214,30 @@
       <c r="B10" s="41">
         <v>1</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="33"/>
+      <c r="C10" s="42">
+        <v>2</v>
+      </c>
+      <c r="D10" s="42">
+        <v>3</v>
+      </c>
+      <c r="E10" s="42">
+        <v>4</v>
+      </c>
+      <c r="F10" s="42">
+        <v>5</v>
+      </c>
+      <c r="G10" s="42">
+        <v>6</v>
+      </c>
+      <c r="H10" s="42">
+        <v>7</v>
+      </c>
+      <c r="I10" s="42">
+        <v>8</v>
+      </c>
+      <c r="J10" s="33">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">

</xml_diff>

<commit_message>
No need for any data in control panel
Models will now run with no data included in control panel.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>attribute</t>
   </si>
@@ -2105,7 +2105,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2155,9 +2155,7 @@
       <c r="A4" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5">
-        <v>0</v>
-      </c>
+      <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="3"/>
     </row>
@@ -2165,9 +2163,7 @@
       <c r="A5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6">
-        <v>0</v>
-      </c>
+      <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="7"/>
     </row>
@@ -2175,36 +2171,28 @@
       <c r="A6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="b">
-        <v>0</v>
-      </c>
+      <c r="B6" s="8"/>
       <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="39" t="b">
-        <v>0</v>
-      </c>
+      <c r="B7" s="39"/>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="39" t="b">
-        <v>0</v>
-      </c>
+      <c r="B8" s="39"/>
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="39" t="b">
-        <v>0</v>
-      </c>
+      <c r="B9" s="39"/>
       <c r="C9" s="10"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2217,27 +2205,13 @@
       <c r="C10" s="42">
         <v>2</v>
       </c>
-      <c r="D10" s="42">
-        <v>3</v>
-      </c>
-      <c r="E10" s="42">
-        <v>4</v>
-      </c>
-      <c r="F10" s="42">
-        <v>5</v>
-      </c>
-      <c r="G10" s="42">
-        <v>6</v>
-      </c>
-      <c r="H10" s="42">
-        <v>7</v>
-      </c>
-      <c r="I10" s="42">
-        <v>8</v>
-      </c>
-      <c r="J10" s="33">
-        <v>9</v>
-      </c>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="33"/>
     </row>
     <row r="11" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26" t="s">
@@ -2252,74 +2226,56 @@
       <c r="A12" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="25">
-        <v>1990</v>
-      </c>
+      <c r="B12" s="25"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="4">
-        <v>2015</v>
-      </c>
+      <c r="B13" s="4"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="4">
-        <v>2016</v>
-      </c>
+      <c r="B14" s="4"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="4">
-        <v>2020</v>
-      </c>
+      <c r="B15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="34">
-        <v>2035</v>
-      </c>
+      <c r="B16" s="34"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="36">
-        <v>0.01</v>
-      </c>
+      <c r="B17" s="36"/>
       <c r="C17" s="43"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="31">
-        <v>5</v>
-      </c>
+      <c r="B18" s="31"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B19" s="32">
-        <v>1</v>
-      </c>
+      <c r="B19" s="32"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="28" t="s">
-        <v>31</v>
-      </c>
+      <c r="B20" s="28"/>
     </row>
     <row r="21" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">

</xml_diff>

<commit_message>
Allow changes to all parameters in control panel
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -10,15 +10,15 @@
     <sheet name="control_panel" sheetId="4" r:id="rId1"/>
     <sheet name="dropdown_lists" sheetId="6" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
-  <si>
-    <t>attribute</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
   <si>
     <t>n_comorbidities</t>
   </si>
@@ -44,30 +44,12 @@
     <t>age_breakpoints</t>
   </si>
   <si>
-    <t>age_stratification</t>
-  </si>
-  <si>
-    <t>consecutive age breakpoints</t>
-  </si>
-  <si>
     <t>integration</t>
   </si>
   <si>
     <t>explicit</t>
   </si>
   <si>
-    <t>single value needed</t>
-  </si>
-  <si>
-    <t>first value</t>
-  </si>
-  <si>
-    <t>value at iteration</t>
-  </si>
-  <si>
-    <t>value at second iteration</t>
-  </si>
-  <si>
     <t>fitting_method</t>
   </si>
   <si>
@@ -114,16 +96,122 @@
   </si>
   <si>
     <t>Fiji</t>
+  </si>
+  <si>
+    <t>tb_n_contact</t>
+  </si>
+  <si>
+    <t>tb_multiplier_force_smearneg</t>
+  </si>
+  <si>
+    <t>tb_prop_early_progression</t>
+  </si>
+  <si>
+    <t>tb_prop_casefatality_untreated_smearpos</t>
+  </si>
+  <si>
+    <t>tb_prop_casefatality_untreated_smearneg</t>
+  </si>
+  <si>
+    <t>tb_prop_casefatality_untreated</t>
+  </si>
+  <si>
+    <t>tb_prop_amplification</t>
+  </si>
+  <si>
+    <t>tb_multiplier_latency_protection</t>
+  </si>
+  <si>
+    <t>tb_multiplier_bcg_protection</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_early_latent</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_activeuntreated</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_treatment_ds</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_treatment_mdr</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_treatment_xdr</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_treatment_inappropriate</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_infect_ontreatment_ds</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_infect_ontreatment_mdr</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_infect_ontreatment_xdr</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_infect_ontreatment_inappropriate</t>
+  </si>
+  <si>
+    <t>tb_rate_late_progression</t>
+  </si>
+  <si>
+    <t>tb_prop_ipt_effectiveness</t>
+  </si>
+  <si>
+    <t>tb_prop_ltbi_test_sensitivity</t>
+  </si>
+  <si>
+    <t>tb_prop_contacts_infected</t>
+  </si>
+  <si>
+    <t>program_timeperiod_await_treatment_smearneg_xpert</t>
+  </si>
+  <si>
+    <t>program_rate_start_treatment</t>
+  </si>
+  <si>
+    <t>program_rate_restart_presenting</t>
+  </si>
+  <si>
+    <t>program_rate_leavelowquality</t>
+  </si>
+  <si>
+    <t>program_prop_death_reporting</t>
+  </si>
+  <si>
+    <t>demo_household_size</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>start_mdr_introduce_period</t>
+  </si>
+  <si>
+    <t>end_mdr_introduce_period</t>
+  </si>
+  <si>
+    <t>timepoint_introduce_xdr</t>
+  </si>
+  <si>
+    <t>susceptible_fully</t>
+  </si>
+  <si>
+    <t>active</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,13 +249,54 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="6" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,12 +323,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -218,17 +341,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -253,51 +376,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -315,17 +394,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -356,15 +424,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -372,52 +431,17 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1085,62 +1109,63 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="663" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="9" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="7" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
     <cellStyle name="Comma 2 2" xfId="5"/>
+    <cellStyle name="Input" xfId="663" builtinId="20"/>
     <cellStyle name="Input 2" xfId="3"/>
-    <cellStyle name="Neutral" xfId="663" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="6"/>
     <cellStyle name="Normal 2" xfId="2"/>
@@ -1812,6 +1837,23 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="constants"/>
+      <sheetName val="time_variants"/>
+      <sheetName val="dropdown_lists"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2102,275 +2144,461 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="31" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-    </row>
-    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5">
-        <v>3</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>5</v>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="9"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="37" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="10"/>
+      <c r="C22" s="9"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="10"/>
+      <c r="C23" s="9"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="9"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="9"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="9"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="14"/>
+      <c r="C30" s="13"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="36"/>
+      <c r="C31" s="15"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="17"/>
+      <c r="C32" s="16"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="17"/>
+      <c r="C33" s="16"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="C34" s="16"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="19"/>
+      <c r="C35" s="16"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="19"/>
+      <c r="C36" s="16"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="16"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="17"/>
+      <c r="C38" s="16"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="17"/>
+      <c r="C39" s="16"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="17"/>
+      <c r="C40" s="16"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="17"/>
+      <c r="C41" s="16"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" s="37"/>
+      <c r="C42" s="16"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="35"/>
+      <c r="C43" s="20"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="22"/>
+      <c r="C44" s="21"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="24"/>
+      <c r="C45" s="23"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" s="24"/>
+      <c r="C46" s="23"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47" s="26"/>
+      <c r="C47" s="25"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="39"/>
-      <c r="C7" s="10"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="B50" s="23"/>
+      <c r="C50" s="23"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="28"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="29"/>
+      <c r="C53" s="28"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="28"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" s="38">
+        <v>1</v>
+      </c>
+      <c r="C55" s="39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="10"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="39"/>
-      <c r="C9" s="10"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="41">
-        <v>1</v>
-      </c>
-      <c r="C10" s="42">
-        <v>2</v>
-      </c>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="33"/>
-    </row>
-    <row r="11" spans="1:10" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11" s="27" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="13"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="25"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="34"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="43"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="31"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="32"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="28"/>
-    </row>
-    <row r="21" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
+      <c r="B56" s="34"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="5"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="363" yWindow="440" count="9">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Time to do recent graphs from" prompt="Calendar year that output graphs for recent time start from." sqref="B12:B15">
-      <formula1>-10000</formula1>
-      <formula2>3000</formula2>
+  <dataValidations xWindow="363" yWindow="440" count="5">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45:B47 B52">
+      <formula1>0</formula1>
+      <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Organ stratification" prompt="Number of organs allowed (0: no stratification, 2: smear-positive and smear-negative, 3: smear-positive, smear-negative and extra-pulmonary)." sqref="C3:D3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43:B44">
       <formula1>0</formula1>
-      <formula2>3</formula2>
+      <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Strains" prompt="Number of strains (0: single strain model, 2: DS-TB and MDR-TB, 3: DS-TB, MDR-TB and XDR-TB)." sqref="B4:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Comorbidities" prompt="Number of comorbidities (currently up to three, but will be revised as model develops)." sqref="B5:D5"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Function smoothness" prompt="From zero up, with zero being exact fit and higher values being greater smoothness." sqref="B18:B19">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B53">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Age breakpoints" prompt="Enter consecutively increasing age breakpoints to create age strata. (Can enter any number, don't enter zero and no upper limit is needed.)" sqref="B22:E22"/>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Organ stratification" prompt="Number of organs allowed (0: no stratification, 2: smear-positive and smear-negative, 3: smear-positive, smear-negative and extra-pulmonary). WARNING: No organ stratification should be selected if this is zero (or one)." sqref="B3">
-      <formula1>0</formula1>
-      <formula2>3</formula2>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32:B42">
+      <formula1>-10000</formula1>
+      <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Low quality care access" prompt="Whether to incorporate low quality care access into the model." sqref="C6">
-      <formula1>$B$2:$B$4</formula1>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55:C55">
+      <formula1>1</formula1>
+      <formula2>100</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" sqref="B11:C11"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="363" yWindow="440" count="7">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Amplification" prompt="Whether amplification to progressively more resistant strains permitted.">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="363" yWindow="440" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C7</xm:sqref>
+          <xm:sqref>B48:B51</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Misassignment" prompt="Whether patients can be incorrectly detected with the wrong strain.">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C9</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Integration" prompt="Which integration package. Explicitly coded or Scipy's integration package.">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B20</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Low quality care access" prompt="Whether to incorporate low quality care access into the model.">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$B$2:$B$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B6</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Amplification" prompt="Whether amplification to progressively more resistant strains permitted.">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$B$2:$B$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B7</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Misassignment" prompt="Whether patients can be incorrectly detected with the wrong strain.">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$B$2:$B$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>B8 B9</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Misassignment" prompt="Whether patients can be incorrectly detected with the wrong strain.">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C8</xm:sqref>
+          <xm:sqref>B54</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2393,32 +2621,32 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make Philippines sheet match other sheets
After changing the input sheets so much for the other countries, now do
the same for the Philippines.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -92,112 +92,112 @@
     <t>runge_kutta</t>
   </si>
   <si>
+    <t>tb_n_contact</t>
+  </si>
+  <si>
+    <t>tb_multiplier_force_smearneg</t>
+  </si>
+  <si>
+    <t>tb_prop_early_progression</t>
+  </si>
+  <si>
+    <t>tb_prop_casefatality_untreated_smearpos</t>
+  </si>
+  <si>
+    <t>tb_prop_casefatality_untreated_smearneg</t>
+  </si>
+  <si>
+    <t>tb_prop_casefatality_untreated</t>
+  </si>
+  <si>
+    <t>tb_prop_amplification</t>
+  </si>
+  <si>
+    <t>tb_multiplier_latency_protection</t>
+  </si>
+  <si>
+    <t>tb_multiplier_bcg_protection</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_early_latent</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_activeuntreated</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_treatment_ds</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_treatment_mdr</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_treatment_xdr</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_treatment_inappropriate</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_infect_ontreatment_ds</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_infect_ontreatment_mdr</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_infect_ontreatment_xdr</t>
+  </si>
+  <si>
+    <t>tb_timeperiod_infect_ontreatment_inappropriate</t>
+  </si>
+  <si>
+    <t>tb_rate_late_progression</t>
+  </si>
+  <si>
+    <t>tb_prop_ipt_effectiveness</t>
+  </si>
+  <si>
+    <t>tb_prop_ltbi_test_sensitivity</t>
+  </si>
+  <si>
+    <t>tb_prop_contacts_infected</t>
+  </si>
+  <si>
+    <t>program_timeperiod_await_treatment_smearneg_xpert</t>
+  </si>
+  <si>
+    <t>program_rate_start_treatment</t>
+  </si>
+  <si>
+    <t>program_rate_restart_presenting</t>
+  </si>
+  <si>
+    <t>program_rate_leavelowquality</t>
+  </si>
+  <si>
+    <t>program_prop_death_reporting</t>
+  </si>
+  <si>
+    <t>demo_household_size</t>
+  </si>
+  <si>
+    <t>start_time</t>
+  </si>
+  <si>
+    <t>start_mdr_introduce_period</t>
+  </si>
+  <si>
+    <t>end_mdr_introduce_period</t>
+  </si>
+  <si>
+    <t>timepoint_introduce_xdr</t>
+  </si>
+  <si>
+    <t>susceptible_fully</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
     <t>Fiji</t>
-  </si>
-  <si>
-    <t>tb_n_contact</t>
-  </si>
-  <si>
-    <t>tb_multiplier_force_smearneg</t>
-  </si>
-  <si>
-    <t>tb_prop_early_progression</t>
-  </si>
-  <si>
-    <t>tb_prop_casefatality_untreated_smearpos</t>
-  </si>
-  <si>
-    <t>tb_prop_casefatality_untreated_smearneg</t>
-  </si>
-  <si>
-    <t>tb_prop_casefatality_untreated</t>
-  </si>
-  <si>
-    <t>tb_prop_amplification</t>
-  </si>
-  <si>
-    <t>tb_multiplier_latency_protection</t>
-  </si>
-  <si>
-    <t>tb_multiplier_bcg_protection</t>
-  </si>
-  <si>
-    <t>tb_timeperiod_early_latent</t>
-  </si>
-  <si>
-    <t>tb_timeperiod_activeuntreated</t>
-  </si>
-  <si>
-    <t>tb_timeperiod_treatment_ds</t>
-  </si>
-  <si>
-    <t>tb_timeperiod_treatment_mdr</t>
-  </si>
-  <si>
-    <t>tb_timeperiod_treatment_xdr</t>
-  </si>
-  <si>
-    <t>tb_timeperiod_treatment_inappropriate</t>
-  </si>
-  <si>
-    <t>tb_timeperiod_infect_ontreatment_ds</t>
-  </si>
-  <si>
-    <t>tb_timeperiod_infect_ontreatment_mdr</t>
-  </si>
-  <si>
-    <t>tb_timeperiod_infect_ontreatment_xdr</t>
-  </si>
-  <si>
-    <t>tb_timeperiod_infect_ontreatment_inappropriate</t>
-  </si>
-  <si>
-    <t>tb_rate_late_progression</t>
-  </si>
-  <si>
-    <t>tb_prop_ipt_effectiveness</t>
-  </si>
-  <si>
-    <t>tb_prop_ltbi_test_sensitivity</t>
-  </si>
-  <si>
-    <t>tb_prop_contacts_infected</t>
-  </si>
-  <si>
-    <t>program_timeperiod_await_treatment_smearneg_xpert</t>
-  </si>
-  <si>
-    <t>program_rate_start_treatment</t>
-  </si>
-  <si>
-    <t>program_rate_restart_presenting</t>
-  </si>
-  <si>
-    <t>program_rate_leavelowquality</t>
-  </si>
-  <si>
-    <t>program_prop_death_reporting</t>
-  </si>
-  <si>
-    <t>demo_household_size</t>
-  </si>
-  <si>
-    <t>start_time</t>
-  </si>
-  <si>
-    <t>start_mdr_introduce_period</t>
-  </si>
-  <si>
-    <t>end_mdr_introduce_period</t>
-  </si>
-  <si>
-    <t>timepoint_introduce_xdr</t>
-  </si>
-  <si>
-    <t>susceptible_fully</t>
-  </si>
-  <si>
-    <t>active</t>
   </si>
 </sst>
 </file>
@@ -2127,7 +2127,7 @@
   <dimension ref="A1:E56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2144,210 +2144,210 @@
         <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="9"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="9"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="9"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="9"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="9"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="9"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="9"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="9"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="9"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="9"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B29" s="12"/>
       <c r="C29" s="9"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30" s="14"/>
       <c r="C30" s="13"/>
@@ -2361,7 +2361,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" s="17"/>
       <c r="C32" s="16"/>
@@ -2382,21 +2382,21 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B35" s="19"/>
       <c r="C35" s="16"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B36" s="19"/>
       <c r="C36" s="16"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B37" s="19"/>
       <c r="C37" s="16"/>
@@ -2438,14 +2438,14 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B43" s="35"/>
       <c r="C43" s="20"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B44" s="22"/>
       <c r="C44" s="21"/>

</xml_diff>

<commit_message>
Subtract one from household size
As discussed at teleconference, the number of household contacts should
be household size minus one.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -348,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -441,6 +441,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="664">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1108,13 +1130,10 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1149,14 +1168,16 @@
     <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="8" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="6" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="6" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2124,22 +2145,22 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" style="31" customWidth="1"/>
+    <col min="1" max="1" width="52.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="28" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2150,395 +2171,401 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="9"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="9"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="9"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="9"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="9"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="9"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="9"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="6"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="6"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="9"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="6"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="9"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="6"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="9"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="6"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="6"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="9"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="6"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="14"/>
-      <c r="C30" s="13"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="10"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="36"/>
-      <c r="C31" s="15"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="12"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="16"/>
+      <c r="B32" s="14"/>
+      <c r="C32" s="13"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="16"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="13"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="16"/>
+      <c r="B34" s="14"/>
+      <c r="C34" s="13"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="16"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="13"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="18" t="s">
+      <c r="A37" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B37" s="19"/>
-      <c r="C37" s="16"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="13"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="16"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="13"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B39" s="17"/>
-      <c r="C39" s="16"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="13"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="16"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="13"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="16"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="13"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="37"/>
-      <c r="C42" s="16"/>
+      <c r="B42" s="31"/>
+      <c r="C42" s="13"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="20" t="s">
+      <c r="A43" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="35"/>
-      <c r="C43" s="20"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="17"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="21" t="s">
+      <c r="A44" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B44" s="22"/>
-      <c r="C44" s="21"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="18"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="24"/>
-      <c r="C45" s="23"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="20"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="23" t="s">
+      <c r="A46" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B46" s="24"/>
-      <c r="C46" s="23"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="20"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="25" t="s">
+      <c r="A47" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="26"/>
-      <c r="C47" s="25"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="22"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="23" t="s">
+      <c r="A48" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="23" t="s">
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="23" t="s">
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="23"/>
-      <c r="C50" s="23"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="25" t="s">
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="27" t="s">
+      <c r="B51" s="22"/>
+      <c r="C51" s="22"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="24" t="s">
         <v>10</v>
       </c>
       <c r="B52" s="2"/>
-      <c r="C52" s="28"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="27" t="s">
+      <c r="C52" s="25"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B53" s="29"/>
-      <c r="C53" s="28"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="27" t="s">
+      <c r="B53" s="26"/>
+      <c r="C53" s="25"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="28"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="32" t="s">
+      <c r="B54" s="2"/>
+      <c r="C54" s="25"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B55" s="38">
-        <v>1</v>
-      </c>
-      <c r="C55" s="39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="32">
+        <v>8</v>
+      </c>
+      <c r="C55" s="32">
+        <v>9</v>
+      </c>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="38"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B56" s="34"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="5"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="18"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="35"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">

</xml_diff>

<commit_message>
Tidy control panel file
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -205,7 +205,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -279,12 +279,6 @@
     <font>
       <sz val="11"/>
       <color theme="5" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1127,7 +1121,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1161,7 +1155,6 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2144,16 +2137,15 @@
   </sheetPr>
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.140625" style="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="27" customWidth="1"/>
+    <col min="3" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2172,394 +2164,342 @@
         <v>24</v>
       </c>
       <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="7"/>
-      <c r="C9" s="6"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="7"/>
-      <c r="C10" s="6"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B11" s="7"/>
-      <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="5"/>
-      <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="6"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="6"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="5"/>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B25" s="7"/>
-      <c r="C25" s="6"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B28" s="5"/>
-      <c r="C28" s="6"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>51</v>
       </c>
       <c r="B29" s="9"/>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>52</v>
       </c>
       <c r="B30" s="11"/>
-      <c r="C30" s="10"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="12"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="29"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>53</v>
       </c>
       <c r="B32" s="14"/>
-      <c r="C32" s="13"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B33" s="14"/>
-      <c r="C33" s="13"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B34" s="14"/>
-      <c r="C34" s="13"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B35" s="16"/>
-      <c r="C35" s="13"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>55</v>
       </c>
       <c r="B36" s="16"/>
-      <c r="C36" s="13"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>56</v>
       </c>
       <c r="B37" s="16"/>
-      <c r="C37" s="13"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B38" s="14"/>
-      <c r="C38" s="13"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B39" s="14"/>
-      <c r="C39" s="13"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>14</v>
       </c>
       <c r="B40" s="14"/>
-      <c r="C40" s="13"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B41" s="14"/>
-      <c r="C41" s="13"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="31"/>
-      <c r="C42" s="13"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="30"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B43" s="29"/>
-      <c r="C43" s="17"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="28"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>58</v>
       </c>
       <c r="B44" s="19"/>
-      <c r="C44" s="18"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="21"/>
-      <c r="C45" s="20"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>3</v>
       </c>
       <c r="B46" s="21"/>
-      <c r="C46" s="20"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
         <v>0</v>
       </c>
       <c r="B47" s="23"/>
-      <c r="C47" s="22"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
         <v>6</v>
       </c>
       <c r="B50" s="22"/>
-      <c r="C50" s="22"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="24" t="s">
         <v>10</v>
       </c>
       <c r="B51" s="2"/>
-      <c r="C51" s="25"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="26"/>
-      <c r="C52" s="25"/>
+      <c r="B52" s="25"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B53" s="2"/>
-      <c r="C53" s="25"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="36" t="s">
+      <c r="A54" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B54" s="32">
-        <v>8</v>
-      </c>
-      <c r="C54" s="32">
-        <v>9</v>
-      </c>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="38"/>
+      <c r="B54" s="31">
+        <v>1</v>
+      </c>
+      <c r="C54" s="36"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="36"/>
+      <c r="F54" s="36"/>
+      <c r="G54" s="36"/>
+      <c r="H54" s="36"/>
+      <c r="I54" s="37"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="33" t="s">
+      <c r="A55" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
-      <c r="D55" s="34"/>
-      <c r="E55" s="35"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="33"/>
+      <c r="E55" s="34"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45:B47 B51">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51 B45:B47">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
@@ -2575,11 +2515,11 @@
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54:C54">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 B12:B30">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:B30 B2:B3">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Add option for output spreadsheets to test
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
   <si>
     <t>n_comorbidities</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>Fiji</t>
+  </si>
+  <si>
+    <t>output_spreadsheets</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1124,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1168,6 +1171,8 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2135,10 +2140,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I55"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2496,6 +2501,14 @@
       <c r="C55" s="33"/>
       <c r="D55" s="33"/>
       <c r="E55" s="34"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" s="39" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">
@@ -2541,7 +2554,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B48:B50</xm:sqref>
+          <xm:sqref>B48:B50 B56</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Determine whether to graph from control panel
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -10,12 +10,15 @@
     <sheet name="control_panel" sheetId="4" r:id="rId1"/>
     <sheet name="dropdown_lists" sheetId="6" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>n_comorbidities</t>
   </si>
@@ -198,6 +201,18 @@
   </si>
   <si>
     <t>output_spreadsheets</t>
+  </si>
+  <si>
+    <t>output_gtb_plots</t>
+  </si>
+  <si>
+    <t>output_flow_diagram</t>
+  </si>
+  <si>
+    <t>output_fractions</t>
+  </si>
+  <si>
+    <t>output_scaleups</t>
   </si>
 </sst>
 </file>
@@ -1124,7 +1139,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1171,8 +1186,10 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -1850,6 +1867,23 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="constants"/>
+      <sheetName val="time_variants"/>
+      <sheetName val="dropdown_lists"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2140,10 +2174,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I56"/>
+  <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2426,9 +2460,7 @@
       <c r="A45" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B45" s="21">
-        <v>3</v>
-      </c>
+      <c r="B45" s="21"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
@@ -2506,9 +2538,31 @@
       <c r="A56" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="39" t="b">
-        <v>1</v>
-      </c>
+      <c r="B56" s="39"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" s="2"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="B60" s="41"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">
@@ -2549,18 +2603,24 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="363" yWindow="440" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="363" yWindow="440" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B48:B50 B56</xm:sqref>
+          <xm:sqref>B48:B50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
           <xm:sqref>B53</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B56:B60</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Changes to spreadsheets for age stratification
Needed to match age stratification in model code. However, parameters
are still dummy.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -4,21 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="435" windowWidth="20370" windowHeight="7410" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="control_panel" sheetId="4" r:id="rId1"/>
     <sheet name="dropdown_lists" sheetId="6" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
   <si>
     <t>n_comorbidities</t>
   </si>
@@ -213,6 +210,15 @@
   </si>
   <si>
     <t>output_scaleups</t>
+  </si>
+  <si>
+    <t>tb_prop_early_progression_age0to5</t>
+  </si>
+  <si>
+    <t>tb_prop_early_progression_age5to15</t>
+  </si>
+  <si>
+    <t>tb_prop_early_progression_age15up</t>
   </si>
 </sst>
 </file>
@@ -1139,7 +1145,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1190,6 +1196,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -1867,23 +1874,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="constants"/>
-      <sheetName val="time_variants"/>
-      <sheetName val="dropdown_lists"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2174,10 +2164,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2218,383 +2208,404 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="B5" s="5"/>
+      <c r="C5" s="42"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="B6" s="5"/>
+      <c r="C6" s="42"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="B7" s="5"/>
+      <c r="C7" s="42"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="7"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="5"/>
+      <c r="B14" s="7"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B15" s="5"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16" s="5"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B17" s="5"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="7"/>
+      <c r="A25" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="5"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="7"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="5"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="B30" s="5"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
+      <c r="B31" s="5"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="9"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
+      <c r="B32" s="9"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="11"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+      <c r="B33" s="11"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B31" s="29"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="B34" s="29"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B32" s="14"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="B35" s="14"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="14"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+      <c r="B36" s="14"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="14"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+      <c r="B37" s="14"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="16"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="B38" s="16"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="16"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+      <c r="B39" s="16"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="16"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" s="14"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" s="14"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" s="14"/>
+      <c r="B40" s="16"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B41" s="14"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="14"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="14"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" s="14"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="30"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
+      <c r="B45" s="30"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B43" s="28"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="18" t="s">
+      <c r="B46" s="28"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="19"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45" s="21"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B46" s="21"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47" s="23"/>
+      <c r="B47" s="19"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B48" s="20"/>
+        <v>2</v>
+      </c>
+      <c r="B48" s="21"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="B49" s="21"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B50" s="23"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="20"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="20"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B50" s="22"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="24" t="s">
+      <c r="B53" s="22"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="24" t="s">
+      <c r="B54" s="2"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B52" s="25"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="24" t="s">
+      <c r="B55" s="25"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="35" t="s">
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B54" s="31">
+      <c r="B57" s="31">
         <v>1</v>
       </c>
-      <c r="C54" s="36"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="36"/>
-      <c r="I54" s="37"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="32" t="s">
+      <c r="C57" s="36"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="36"/>
+      <c r="G57" s="36"/>
+      <c r="H57" s="36"/>
+      <c r="I57" s="37"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B55" s="18"/>
-      <c r="C55" s="33"/>
-      <c r="D55" s="33"/>
-      <c r="E55" s="34"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="38" t="s">
+      <c r="B58" s="18"/>
+      <c r="C58" s="33"/>
+      <c r="D58" s="33"/>
+      <c r="E58" s="34"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="39"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="24" t="s">
+      <c r="B59" s="39"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="B57" s="2"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="s">
+      <c r="B60" s="2"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="24" t="s">
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="40" t="s">
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B60" s="41"/>
+      <c r="B63" s="41"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51 B45:B47">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54 B48:B50">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43:B44">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B46:B47">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B52">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B32:B42">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35:B45">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B57">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:B30 B2:B3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:B33 B2:B3">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B11">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 B8:B14">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2603,24 +2614,18 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="363" yWindow="440" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="363" yWindow="440" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B48:B50</xm:sqref>
+          <xm:sqref>B51:B53 B59:B63</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B53</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B56:B60</xm:sqref>
+          <xm:sqref>B56</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Equivalent changes to control panel
Change control panel to make consistent with defaults spreadsheet.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
   <si>
     <t>n_comorbidities</t>
   </si>
@@ -219,6 +219,12 @@
   </si>
   <si>
     <t>tb_prop_early_progression_age15up</t>
+  </si>
+  <si>
+    <t>tb_rate_late_progression_age0to15</t>
+  </si>
+  <si>
+    <t>tb_rate_late_progression_age15up</t>
   </si>
 </sst>
 </file>
@@ -2164,10 +2170,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2281,323 +2287,337 @@
       </c>
       <c r="B16" s="5"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>33</v>
       </c>
       <c r="B17" s="5"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="5"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="5"/>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B23" s="5"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>40</v>
       </c>
       <c r="B24" s="5"/>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B25" s="5"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B26" s="5"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B27" s="5"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="42"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="42"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="7"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="B30" s="7"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="B31" s="5"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="5"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="B32" s="5"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="5"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="8" t="s">
+      <c r="B33" s="5"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="9"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="B34" s="9"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="11"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="12" t="s">
+      <c r="B35" s="11"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="29"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35" s="14"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B36" s="14"/>
+      <c r="B36" s="29"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="14"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="14"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B37" s="14"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="16"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="16"/>
+      <c r="B39" s="14"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="16"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="16"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B40" s="16"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="14"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B42" s="14"/>
+      <c r="B42" s="16"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B43" s="14"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B44" s="14"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="14"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" s="14"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="30"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
+      <c r="B47" s="30"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B46" s="28"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="18" t="s">
+      <c r="B48" s="28"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B47" s="19"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="20" t="s">
+      <c r="B49" s="19"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B48" s="21"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B49" s="21"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B50" s="23"/>
+      <c r="B50" s="21"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="21"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B52" s="23"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B51" s="20"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="20" t="s">
+      <c r="B53" s="20"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="20"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="22" t="s">
+      <c r="B54" s="20"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B53" s="22"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54" s="2"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B55" s="25"/>
+      <c r="B55" s="22"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B56" s="2"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B57" s="25"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="35" t="s">
+      <c r="B58" s="2"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B57" s="31">
+      <c r="B59" s="31">
         <v>1</v>
       </c>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="36"/>
-      <c r="I57" s="37"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="32" t="s">
+      <c r="C59" s="36"/>
+      <c r="D59" s="36"/>
+      <c r="E59" s="36"/>
+      <c r="F59" s="36"/>
+      <c r="G59" s="36"/>
+      <c r="H59" s="36"/>
+      <c r="I59" s="37"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B58" s="18"/>
-      <c r="C58" s="33"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="34"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="38" t="s">
+      <c r="B60" s="18"/>
+      <c r="C60" s="33"/>
+      <c r="D60" s="33"/>
+      <c r="E60" s="34"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="39"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B60" s="2"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B61" s="2"/>
+      <c r="B61" s="39"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" s="2"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B62" s="2"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="40" t="s">
+      <c r="B64" s="2"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="41"/>
+      <c r="B65" s="41"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54 B48:B50">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56 B50:B52">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B46:B47">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48:B49">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B57">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B35:B45">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37:B47">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B57">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B59">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:B33 B2:B3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 B15:B27 B30:B35">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
@@ -2605,7 +2625,7 @@
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2619,13 +2639,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B51:B53 B59:B63</xm:sqref>
+          <xm:sqref>B53:B55 B61:B65</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B56</xm:sqref>
+          <xm:sqref>B58</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Modification of infectiousness by age
Finished code to modify infectiousness depending upon the age profile of
the infectious population.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
   <si>
     <t>n_comorbidities</t>
   </si>
@@ -225,6 +225,15 @@
   </si>
   <si>
     <t>tb_rate_late_progression_age15up</t>
+  </si>
+  <si>
+    <t>tb_multiplier_child_infectiousness</t>
+  </si>
+  <si>
+    <t>tb_multiplier_child_infectiousness_age0to10</t>
+  </si>
+  <si>
+    <t>tb_multiplier_child_infectiousness_age10up</t>
   </si>
 </sst>
 </file>
@@ -2170,10 +2179,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2208,424 +2217,446 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>70</v>
       </c>
       <c r="B4" s="5"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="42"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="42"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="42"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="B8" s="5"/>
+      <c r="C8" s="42"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="B9" s="5"/>
+      <c r="C9" s="42"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="B10" s="5"/>
+      <c r="C10" s="42"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="5"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="5"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="B14" s="5"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="7"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="7"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="B28" s="5"/>
-      <c r="C28" s="42"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="B29" s="5"/>
-      <c r="C29" s="42"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B30" s="7"/>
+      <c r="A30" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="5"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="B31" s="5"/>
+      <c r="C31" s="42"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="42"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="7"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="5"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="5"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="B35" s="5"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="5"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
+      <c r="B36" s="5"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="9"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="10" t="s">
+      <c r="B37" s="9"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="11"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+      <c r="B38" s="11"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="29"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
+      <c r="B39" s="29"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B37" s="14"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
+      <c r="B40" s="14"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="14"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+      <c r="B41" s="14"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="14"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="15" t="s">
+      <c r="B42" s="14"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="16"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="15" t="s">
+      <c r="B43" s="16"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B41" s="16"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
+      <c r="B44" s="16"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="16"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B43" s="14"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="14"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B45" s="14"/>
+      <c r="B45" s="16"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="B46" s="14"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="14"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="14"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49" s="14"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B47" s="30"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
+      <c r="B50" s="30"/>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B48" s="28"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="18" t="s">
+      <c r="B51" s="28"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B49" s="19"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="B50" s="21"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B51" s="21"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="23"/>
+      <c r="B52" s="19"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B53" s="20"/>
+        <v>2</v>
+      </c>
+      <c r="B53" s="21"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" s="20"/>
+        <v>3</v>
+      </c>
+      <c r="B54" s="21"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="23"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="20"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="20"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="B55" s="22"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="24" t="s">
+      <c r="B58" s="22"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B56" s="2"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="24" t="s">
+      <c r="B59" s="2"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B57" s="25"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="24" t="s">
+      <c r="B60" s="25"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="B58" s="2"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="35" t="s">
+      <c r="B61" s="2"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B59" s="31">
+      <c r="B62" s="31">
         <v>1</v>
       </c>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="36"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="36"/>
-      <c r="I59" s="37"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="32" t="s">
+      <c r="C62" s="36"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="36"/>
+      <c r="G62" s="36"/>
+      <c r="H62" s="36"/>
+      <c r="I62" s="37"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B60" s="18"/>
-      <c r="C60" s="33"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="34"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="38" t="s">
+      <c r="B63" s="18">
+        <v>8</v>
+      </c>
+      <c r="C63" s="33"/>
+      <c r="D63" s="33"/>
+      <c r="E63" s="34"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="39"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="24" t="s">
+      <c r="B64" s="39"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="2"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="24" t="s">
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="24" t="s">
+      <c r="B66" s="2"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="2"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="40" t="s">
+      <c r="B67" s="2"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="41"/>
+      <c r="B68" s="41"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="8">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56 B50:B52">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B59 B53:B55">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48:B49">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51:B52">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B57">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B37:B47">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40:B50">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B59">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B62">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B3 B15:B27 B30:B35">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33:B38 B18:B30 B2:B4">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 B8:B14">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7 B11:B17">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B36">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2639,13 +2670,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B53:B55 B61:B65</xm:sqref>
+          <xm:sqref>B56:B58 B64:B68</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B58</xm:sqref>
+          <xm:sqref>B61</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Sync spreadsheet changes to go with code
Sorry Tan, hadn't synced these changes where I have added further
options to control figure outputs.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="495" windowWidth="20370" windowHeight="7350" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="555" windowWidth="20370" windowHeight="7290" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="control_panel" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
   <si>
     <t>n_comorbidities</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>tb_multiplier_child_infectiousness_age10up</t>
+  </si>
+  <si>
+    <t>output_by_age</t>
+  </si>
+  <si>
+    <t>output_age_fractions</t>
   </si>
 </sst>
 </file>
@@ -323,7 +329,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +380,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1160,7 +1172,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1212,6 +1224,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2179,10 +2193,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2194,10 +2208,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="44" t="s">
         <v>59</v>
       </c>
       <c r="C1" s="1"/>
@@ -2589,9 +2603,7 @@
       <c r="A63" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B63" s="18">
-        <v>8</v>
-      </c>
+      <c r="B63" s="18"/>
       <c r="C63" s="33"/>
       <c r="D63" s="33"/>
       <c r="E63" s="34"/>
@@ -2602,32 +2614,46 @@
       </c>
       <c r="B64" s="39"/>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
         <v>61</v>
       </c>
       <c r="B65" s="2"/>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" s="43"/>
+    </row>
+    <row r="67" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" s="43"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B66" s="2"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="24" t="s">
+      <c r="B68" s="2"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B67" s="2"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="40" t="s">
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B68" s="41"/>
+      <c r="B70" s="41"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="363" yWindow="440" count="8">
+  <dataValidations xWindow="363" yWindow="440" count="9">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B59 B53:B55">
       <formula1>0</formula1>
       <formula2>10</formula2>
@@ -2648,17 +2674,21 @@
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33:B38 B18:B30 B2:B4">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33:B38 B18:B30">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7 B11:B17">
-      <formula1>0</formula1>
-      <formula2>1</formula2>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39">
       <formula1>0</formula1>
       <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Override base parameter?" sqref="B2:B6">
+      <formula1>0</formula1>
+      <formula2>10000000000</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Override base parameter?" sqref="B7:B17">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2670,7 +2700,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B56:B58 B64:B68</xm:sqref>
+          <xm:sqref>B56:B58 B64:B70</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Change approach to adding comorbidities
Now allows more flexibility for user to request certain comorbidities.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="75">
-  <si>
-    <t>n_comorbidities</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
   <si>
     <t>recent_time</t>
   </si>
@@ -240,6 +237,21 @@
   </si>
   <si>
     <t>output_age_fractions</t>
+  </si>
+  <si>
+    <t>comorbidity_diabetes</t>
+  </si>
+  <si>
+    <t>comorbidity_hiv</t>
+  </si>
+  <si>
+    <t>comorbidity_prison</t>
+  </si>
+  <si>
+    <t>comorbidity_remote</t>
+  </si>
+  <si>
+    <t>comorbidity_poverty</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1184,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1226,6 +1238,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2193,10 +2209,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,452 +2225,474 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" s="5"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B4" s="5"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="42"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B6" s="5"/>
       <c r="C6" s="42"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="42"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="42"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="42"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="5"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="7"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="7"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="7"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B18" s="5"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="5"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23" s="5"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="5"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="5"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="5"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="5"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29" s="5"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30" s="5"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="42"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B32" s="5"/>
       <c r="C32" s="42"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="7"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="5"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="5"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="5"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="9"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="11"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B39" s="29"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B40" s="14"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B41" s="14"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B42" s="14"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B43" s="16"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B44" s="16"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B45" s="16"/>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B46" s="14"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B47" s="14"/>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48" s="14"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="14"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
-        <v>15</v>
-      </c>
       <c r="B49" s="14"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B50" s="30"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B51" s="28"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="28"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
-        <v>58</v>
-      </c>
       <c r="B52" s="19"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="21"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B53" s="21"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="20" t="s">
+      <c r="B54" s="21"/>
+    </row>
+    <row r="55" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" s="47"/>
+    </row>
+    <row r="56" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B56" s="21"/>
+    </row>
+    <row r="57" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B57" s="21"/>
+    </row>
+    <row r="58" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B58" s="21"/>
+    </row>
+    <row r="59" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B59" s="23"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="21"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="23"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="20" t="s">
+      <c r="B60" s="20"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="20"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="20" t="s">
+      <c r="B61" s="20"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B57" s="20"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="22" t="s">
+      <c r="B62" s="22"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" s="2"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" s="25"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B65" s="2"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="31"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="36"/>
+      <c r="F66" s="36"/>
+      <c r="G66" s="36"/>
+      <c r="H66" s="36"/>
+      <c r="I66" s="37"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="22"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B59" s="2"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B60" s="25"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B61" s="2"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="B62" s="31">
-        <v>1</v>
-      </c>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="36"/>
-      <c r="I62" s="37"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="B63" s="18"/>
-      <c r="C63" s="33"/>
-      <c r="D63" s="33"/>
-      <c r="E63" s="34"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="38" t="s">
+      <c r="B67" s="18"/>
+      <c r="C67" s="33"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="34"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B68" s="39"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B64" s="39"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="24" t="s">
+      <c r="B69" s="2"/>
+    </row>
+    <row r="70" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" s="2"/>
+      <c r="C70" s="43"/>
+    </row>
+    <row r="71" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" s="43"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="B65" s="2"/>
-    </row>
-    <row r="66" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="B66" s="2"/>
-      <c r="C66" s="43"/>
-    </row>
-    <row r="67" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="B67" s="2"/>
-      <c r="C67" s="43"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="24" t="s">
+      <c r="B72" s="2"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B68" s="2"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="24" t="s">
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="B69" s="2"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="40" t="s">
-        <v>64</v>
-      </c>
-      <c r="B70" s="41"/>
+      <c r="B74" s="41"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="9">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B59 B53:B55">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63 B53:B54">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
@@ -2662,7 +2700,7 @@
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B64">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
@@ -2670,7 +2708,7 @@
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B62">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B66">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2700,13 +2738,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B56:B58 B64:B70</xm:sqref>
+          <xm:sqref>B60:B62 B68:B74 B55:B59</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B61</xm:sqref>
+          <xm:sqref>B65</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2729,32 +2767,32 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Vary proportions with certain comorbidities
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
   <si>
     <t>recent_time</t>
   </si>
@@ -252,6 +252,21 @@
   </si>
   <si>
     <t>comorbidity_poverty</t>
+  </si>
+  <si>
+    <t>comorb_prop_prison</t>
+  </si>
+  <si>
+    <t>comorb_prop_poverty</t>
+  </si>
+  <si>
+    <t>comorb_prop_remote</t>
+  </si>
+  <si>
+    <t>comorb_prop_hiv</t>
+  </si>
+  <si>
+    <t>comorb_prop_diabetes</t>
   </si>
 </sst>
 </file>
@@ -1184,7 +1199,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1242,6 +1257,8 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="10" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2209,10 +2226,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2588,111 +2605,143 @@
       </c>
       <c r="B59" s="23"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B60" s="49"/>
+    </row>
+    <row r="61" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B61" s="49"/>
+    </row>
+    <row r="62" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B62" s="49"/>
+    </row>
+    <row r="63" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B63" s="49"/>
+    </row>
+    <row r="64" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B64" s="50"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B60" s="20"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="20" t="s">
+      <c r="B65" s="20"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B61" s="20"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="22" t="s">
+      <c r="B66" s="20"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B62" s="22"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="24" t="s">
+      <c r="B67" s="22"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B63" s="2"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B64" s="25"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="B65" s="2"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="B66" s="31"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="36"/>
-      <c r="E66" s="36"/>
-      <c r="F66" s="36"/>
-      <c r="G66" s="36"/>
-      <c r="H66" s="36"/>
-      <c r="I66" s="37"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B67" s="18"/>
-      <c r="C67" s="33"/>
-      <c r="D67" s="33"/>
-      <c r="E67" s="34"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="B68" s="39"/>
+      <c r="B68" s="2"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B69" s="25"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B70" s="2"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B71" s="31">
+        <v>1</v>
+      </c>
+      <c r="C71" s="36"/>
+      <c r="D71" s="36"/>
+      <c r="E71" s="36"/>
+      <c r="F71" s="36"/>
+      <c r="G71" s="36"/>
+      <c r="H71" s="36"/>
+      <c r="I71" s="37"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B72" s="18"/>
+      <c r="C72" s="33"/>
+      <c r="D72" s="33"/>
+      <c r="E72" s="34"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73" s="39"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B69" s="2"/>
-    </row>
-    <row r="70" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="24" t="s">
+      <c r="B74" s="2"/>
+    </row>
+    <row r="75" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B70" s="2"/>
-      <c r="C70" s="43"/>
-    </row>
-    <row r="71" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="24" t="s">
+      <c r="B75" s="2"/>
+      <c r="C75" s="43"/>
+    </row>
+    <row r="76" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="B71" s="2"/>
-      <c r="C71" s="43"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="24" t="s">
+      <c r="B76" s="2"/>
+      <c r="C76" s="43"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="B72" s="2"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="24" t="s">
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B73" s="2"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="40" t="s">
+      <c r="B78" s="2"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="B74" s="41"/>
+      <c r="B79" s="41"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="363" yWindow="440" count="9">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63 B53:B54">
+  <dataValidations xWindow="363" yWindow="440" count="10">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B68 B53:B54">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
@@ -2700,7 +2749,7 @@
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B64">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B69">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
@@ -2708,7 +2757,7 @@
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B66">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B71">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2728,6 +2777,10 @@
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60:B64">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2738,13 +2791,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B60:B62 B68:B74 B55:B59</xm:sqref>
+          <xm:sqref>B73:B79 B55:B59 B65:B67</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B65</xm:sqref>
+          <xm:sqref>B70</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Separate treatment support as a program
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
   <si>
     <t>recent_time</t>
   </si>
@@ -267,6 +267,9 @@
   </si>
   <si>
     <t>comorb_prop_diabetes</t>
+  </si>
+  <si>
+    <t>program_prop_treatment_support_improvement</t>
   </si>
 </sst>
 </file>
@@ -2226,10 +2229,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2443,329 +2446,336 @@
       <c r="B32" s="5"/>
       <c r="C32" s="42"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>46</v>
       </c>
       <c r="B33" s="7"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B34" s="5"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B35" s="5"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B36" s="5"/>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>50</v>
       </c>
       <c r="B37" s="9"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="42"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B38" s="11"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
+      <c r="B39" s="11"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B39" s="29"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+      <c r="B40" s="29"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B40" s="14"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
+      <c r="B41" s="14"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B41" s="14"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+      <c r="B42" s="14"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B42" s="14"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+      <c r="B43" s="14"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B43" s="16"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
+      <c r="B44" s="16"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B44" s="16"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
+      <c r="B45" s="16"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B45" s="16"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+      <c r="B46" s="16"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B46" s="14"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+      <c r="B47" s="14"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="13" t="s">
         <v>11</v>
-      </c>
-      <c r="B47" s="14"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
-        <v>13</v>
       </c>
       <c r="B48" s="14"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B49" s="14"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" s="14"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B50" s="30"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
+      <c r="B51" s="30"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="28"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
+      <c r="B52" s="28"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="19"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B53" s="21"/>
+      <c r="B53" s="19"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="21"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="21"/>
-    </row>
-    <row r="55" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="46" t="s">
+      <c r="B55" s="21"/>
+    </row>
+    <row r="56" spans="1:2" s="48" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="B55" s="47"/>
-    </row>
-    <row r="56" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B56" s="21"/>
+      <c r="B56" s="47"/>
     </row>
     <row r="57" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B57" s="21"/>
     </row>
     <row r="58" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58" s="21"/>
+    </row>
+    <row r="59" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B58" s="21"/>
-    </row>
-    <row r="59" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="22" t="s">
+      <c r="B59" s="21"/>
+    </row>
+    <row r="60" spans="1:2" s="45" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B59" s="23"/>
-    </row>
-    <row r="60" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B60" s="49"/>
+      <c r="B60" s="23"/>
     </row>
     <row r="61" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B61" s="49"/>
     </row>
     <row r="62" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B62" s="49"/>
     </row>
     <row r="63" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" s="49"/>
+    </row>
+    <row r="64" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="B63" s="49"/>
-    </row>
-    <row r="64" spans="1:2" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="22" t="s">
+      <c r="B64" s="49"/>
+    </row>
+    <row r="65" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B64" s="50"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="B65" s="20"/>
+      <c r="B65" s="50"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="20"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B66" s="20"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="22" t="s">
+      <c r="B67" s="20"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B67" s="22"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B68" s="2"/>
+      <c r="B68" s="22"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B69" s="25"/>
+        <v>9</v>
+      </c>
+      <c r="B69" s="2"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B70" s="25"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B70" s="2"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="35" t="s">
+      <c r="B71" s="2"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B71" s="31">
+      <c r="B72" s="31">
         <v>1</v>
       </c>
-      <c r="C71" s="36"/>
-      <c r="D71" s="36"/>
-      <c r="E71" s="36"/>
-      <c r="F71" s="36"/>
-      <c r="G71" s="36"/>
-      <c r="H71" s="36"/>
-      <c r="I71" s="37"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="32" t="s">
+      <c r="C72" s="36"/>
+      <c r="D72" s="36"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="36"/>
+      <c r="G72" s="36"/>
+      <c r="H72" s="36"/>
+      <c r="I72" s="37"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B72" s="18"/>
-      <c r="C72" s="33"/>
-      <c r="D72" s="33"/>
-      <c r="E72" s="34"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="38" t="s">
+      <c r="B73" s="18"/>
+      <c r="C73" s="33"/>
+      <c r="D73" s="33"/>
+      <c r="E73" s="34"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="B73" s="39"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="24" t="s">
+      <c r="B74" s="39"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="B74" s="2"/>
-    </row>
-    <row r="75" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="24" t="s">
-        <v>72</v>
-      </c>
       <c r="B75" s="2"/>
-      <c r="C75" s="43"/>
     </row>
     <row r="76" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="43"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="24" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="B77" s="2"/>
+      <c r="C77" s="43"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="B78" s="2"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="B78" s="2"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="40" t="s">
+      <c r="B79" s="2"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="B79" s="41"/>
+      <c r="B80" s="41"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="10">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B68 B53:B54">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B69 B54:B55">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B51:B52">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B52:B53">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B69">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B70">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40:B50">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B41:B51">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B71">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B33:B38 B18:B30">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B18:B30 B33:B37 B39">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B39">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B40">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -2777,7 +2787,7 @@
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60:B64">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61:B65">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -2791,13 +2801,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B73:B79 B55:B59 B65:B67</xm:sqref>
+          <xm:sqref>B74:B80 B56:B60 B66:B68</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B70</xm:sqref>
+          <xm:sqref>B71</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Simplify code for age plots
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2232,7 +2232,7 @@
   <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2685,9 +2685,7 @@
       <c r="A72" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="B72" s="31">
-        <v>1</v>
-      </c>
+      <c r="B72" s="31"/>
       <c r="C72" s="36"/>
       <c r="D72" s="36"/>
       <c r="E72" s="36"/>

</xml_diff>

<commit_message>
Revise defaults, remove some code
Revise defaults to a longer time step to focus on running model quickly.
Remove a small amount of unneeded code from economics_lib.py.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2262,8 +2262,8 @@
   </sheetPr>
   <dimension ref="A1:BQ84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3308,9 +3308,7 @@
       <c r="A75" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B75" s="44">
-        <v>2</v>
-      </c>
+      <c r="B75" s="44"/>
       <c r="C75" s="54"/>
       <c r="D75" s="54"/>
       <c r="E75" s="54"/>

</xml_diff>

<commit_message>
Improve consistency of code
Make agegroup follow comorbidity consistently and put last modifiable
parameter into control_panel.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
   <si>
     <t>recent_time</t>
   </si>
@@ -282,6 +282,9 @@
   </si>
   <si>
     <t>program_timeperiod_acf_rounds</t>
+  </si>
+  <si>
+    <t>comorb_multiplier_diabetes_progression</t>
   </si>
 </sst>
 </file>
@@ -2260,10 +2263,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BQ84"/>
+  <dimension ref="A1:BQ85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2566,179 +2569,113 @@
       <c r="C40" s="52"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="28"/>
+      <c r="B41" s="26"/>
       <c r="C41" s="52"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+      <c r="A42" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="28"/>
+      <c r="C42" s="52"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="48"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" s="30"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="48"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="B44" s="30"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>13</v>
+        <v>85</v>
       </c>
       <c r="B45" s="30"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="30"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="30"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B47" s="31"/>
+      <c r="B47" s="30"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B48" s="31"/>
     </row>
     <row r="49" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="31"/>
+    </row>
+    <row r="50" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="31"/>
-    </row>
-    <row r="50" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B50" s="30"/>
+      <c r="B50" s="31"/>
     </row>
     <row r="51" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B51" s="30"/>
     </row>
     <row r="52" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B52" s="30"/>
     </row>
     <row r="53" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B53" s="30"/>
     </row>
     <row r="54" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" s="30"/>
+    </row>
+    <row r="55" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="32"/>
-    </row>
-    <row r="55" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
+      <c r="B55" s="32"/>
+    </row>
+    <row r="56" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A56" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B55" s="33"/>
-    </row>
-    <row r="56" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
+      <c r="B56" s="33"/>
+    </row>
+    <row r="57" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A57" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="34"/>
-    </row>
-    <row r="57" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A57" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B57" s="35"/>
-      <c r="C57" s="48"/>
-      <c r="D57" s="48"/>
-      <c r="E57" s="48"/>
-      <c r="F57" s="48"/>
-      <c r="G57" s="48"/>
-      <c r="H57" s="48"/>
-      <c r="I57" s="48"/>
-      <c r="J57" s="48"/>
-      <c r="K57" s="15"/>
-      <c r="L57" s="15"/>
-      <c r="M57" s="15"/>
-      <c r="N57" s="15"/>
-      <c r="O57" s="15"/>
-      <c r="P57" s="15"/>
-      <c r="Q57" s="15"/>
-      <c r="R57" s="15"/>
-      <c r="S57" s="15"/>
-      <c r="T57" s="15"/>
-      <c r="U57" s="15"/>
-      <c r="V57" s="15"/>
-      <c r="W57" s="15"/>
-      <c r="X57" s="15"/>
-      <c r="Y57" s="15"/>
-      <c r="Z57" s="15"/>
-      <c r="AA57" s="15"/>
-      <c r="AB57" s="15"/>
-      <c r="AC57" s="15"/>
-      <c r="AD57" s="15"/>
-      <c r="AE57" s="15"/>
-      <c r="AF57" s="15"/>
-      <c r="AG57" s="15"/>
-      <c r="AH57" s="15"/>
-      <c r="AI57" s="15"/>
-      <c r="AJ57" s="15"/>
-      <c r="AK57" s="15"/>
-      <c r="AL57" s="15"/>
-      <c r="AM57" s="15"/>
-      <c r="AN57" s="15"/>
-      <c r="AO57" s="15"/>
-      <c r="AP57" s="15"/>
-      <c r="AQ57" s="15"/>
-      <c r="AR57" s="15"/>
-      <c r="AS57" s="15"/>
-      <c r="AT57" s="15"/>
-      <c r="AU57" s="15"/>
-      <c r="AV57" s="15"/>
-      <c r="AW57" s="15"/>
-      <c r="AX57" s="15"/>
-      <c r="AY57" s="15"/>
-      <c r="AZ57" s="15"/>
-      <c r="BA57" s="15"/>
-      <c r="BB57" s="15"/>
-      <c r="BC57" s="15"/>
-      <c r="BD57" s="15"/>
-      <c r="BE57" s="15"/>
-      <c r="BF57" s="15"/>
-      <c r="BG57" s="15"/>
-      <c r="BH57" s="15"/>
-      <c r="BI57" s="15"/>
-      <c r="BJ57" s="15"/>
-      <c r="BK57" s="15"/>
-      <c r="BL57" s="15"/>
-      <c r="BM57" s="15"/>
-      <c r="BN57" s="15"/>
-      <c r="BO57" s="15"/>
-      <c r="BP57" s="15"/>
-      <c r="BQ57" s="15"/>
+      <c r="B57" s="34"/>
     </row>
     <row r="58" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B58" s="35"/>
       <c r="C58" s="48"/>
@@ -2809,11 +2746,11 @@
       <c r="BP58" s="15"/>
       <c r="BQ58" s="15"/>
     </row>
-    <row r="59" spans="1:69" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B59" s="36"/>
+    <row r="59" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="35"/>
       <c r="C59" s="48"/>
       <c r="D59" s="48"/>
       <c r="E59" s="48"/>
@@ -2882,11 +2819,11 @@
       <c r="BP59" s="15"/>
       <c r="BQ59" s="15"/>
     </row>
-    <row r="60" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B60" s="35"/>
+    <row r="60" spans="1:69" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B60" s="36"/>
       <c r="C60" s="48"/>
       <c r="D60" s="48"/>
       <c r="E60" s="48"/>
@@ -2895,10 +2832,69 @@
       <c r="H60" s="48"/>
       <c r="I60" s="48"/>
       <c r="J60" s="48"/>
+      <c r="K60" s="15"/>
+      <c r="L60" s="15"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="15"/>
+      <c r="O60" s="15"/>
+      <c r="P60" s="15"/>
+      <c r="Q60" s="15"/>
+      <c r="R60" s="15"/>
+      <c r="S60" s="15"/>
+      <c r="T60" s="15"/>
+      <c r="U60" s="15"/>
+      <c r="V60" s="15"/>
+      <c r="W60" s="15"/>
+      <c r="X60" s="15"/>
+      <c r="Y60" s="15"/>
+      <c r="Z60" s="15"/>
+      <c r="AA60" s="15"/>
+      <c r="AB60" s="15"/>
+      <c r="AC60" s="15"/>
+      <c r="AD60" s="15"/>
+      <c r="AE60" s="15"/>
+      <c r="AF60" s="15"/>
+      <c r="AG60" s="15"/>
+      <c r="AH60" s="15"/>
+      <c r="AI60" s="15"/>
+      <c r="AJ60" s="15"/>
+      <c r="AK60" s="15"/>
+      <c r="AL60" s="15"/>
+      <c r="AM60" s="15"/>
+      <c r="AN60" s="15"/>
+      <c r="AO60" s="15"/>
+      <c r="AP60" s="15"/>
+      <c r="AQ60" s="15"/>
+      <c r="AR60" s="15"/>
+      <c r="AS60" s="15"/>
+      <c r="AT60" s="15"/>
+      <c r="AU60" s="15"/>
+      <c r="AV60" s="15"/>
+      <c r="AW60" s="15"/>
+      <c r="AX60" s="15"/>
+      <c r="AY60" s="15"/>
+      <c r="AZ60" s="15"/>
+      <c r="BA60" s="15"/>
+      <c r="BB60" s="15"/>
+      <c r="BC60" s="15"/>
+      <c r="BD60" s="15"/>
+      <c r="BE60" s="15"/>
+      <c r="BF60" s="15"/>
+      <c r="BG60" s="15"/>
+      <c r="BH60" s="15"/>
+      <c r="BI60" s="15"/>
+      <c r="BJ60" s="15"/>
+      <c r="BK60" s="15"/>
+      <c r="BL60" s="15"/>
+      <c r="BM60" s="15"/>
+      <c r="BN60" s="15"/>
+      <c r="BO60" s="15"/>
+      <c r="BP60" s="15"/>
+      <c r="BQ60" s="15"/>
     </row>
     <row r="61" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B61" s="35"/>
       <c r="C61" s="48"/>
@@ -2912,7 +2908,7 @@
     </row>
     <row r="62" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B62" s="35"/>
       <c r="C62" s="48"/>
@@ -2924,11 +2920,11 @@
       <c r="I62" s="48"/>
       <c r="J62" s="48"/>
     </row>
-    <row r="63" spans="1:69" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B63" s="37"/>
+    <row r="63" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" s="35"/>
       <c r="C63" s="48"/>
       <c r="D63" s="48"/>
       <c r="E63" s="48"/>
@@ -2937,71 +2933,12 @@
       <c r="H63" s="48"/>
       <c r="I63" s="48"/>
       <c r="J63" s="48"/>
-      <c r="K63" s="15"/>
-      <c r="L63" s="15"/>
-      <c r="M63" s="15"/>
-      <c r="N63" s="15"/>
-      <c r="O63" s="15"/>
-      <c r="P63" s="15"/>
-      <c r="Q63" s="15"/>
-      <c r="R63" s="15"/>
-      <c r="S63" s="15"/>
-      <c r="T63" s="15"/>
-      <c r="U63" s="15"/>
-      <c r="V63" s="15"/>
-      <c r="W63" s="15"/>
-      <c r="X63" s="15"/>
-      <c r="Y63" s="15"/>
-      <c r="Z63" s="15"/>
-      <c r="AA63" s="15"/>
-      <c r="AB63" s="15"/>
-      <c r="AC63" s="15"/>
-      <c r="AD63" s="15"/>
-      <c r="AE63" s="15"/>
-      <c r="AF63" s="15"/>
-      <c r="AG63" s="15"/>
-      <c r="AH63" s="15"/>
-      <c r="AI63" s="15"/>
-      <c r="AJ63" s="15"/>
-      <c r="AK63" s="15"/>
-      <c r="AL63" s="15"/>
-      <c r="AM63" s="15"/>
-      <c r="AN63" s="15"/>
-      <c r="AO63" s="15"/>
-      <c r="AP63" s="15"/>
-      <c r="AQ63" s="15"/>
-      <c r="AR63" s="15"/>
-      <c r="AS63" s="15"/>
-      <c r="AT63" s="15"/>
-      <c r="AU63" s="15"/>
-      <c r="AV63" s="15"/>
-      <c r="AW63" s="15"/>
-      <c r="AX63" s="15"/>
-      <c r="AY63" s="15"/>
-      <c r="AZ63" s="15"/>
-      <c r="BA63" s="15"/>
-      <c r="BB63" s="15"/>
-      <c r="BC63" s="15"/>
-      <c r="BD63" s="15"/>
-      <c r="BE63" s="15"/>
-      <c r="BF63" s="15"/>
-      <c r="BG63" s="15"/>
-      <c r="BH63" s="15"/>
-      <c r="BI63" s="15"/>
-      <c r="BJ63" s="15"/>
-      <c r="BK63" s="15"/>
-      <c r="BL63" s="15"/>
-      <c r="BM63" s="15"/>
-      <c r="BN63" s="15"/>
-      <c r="BO63" s="15"/>
-      <c r="BP63" s="15"/>
-      <c r="BQ63" s="15"/>
-    </row>
-    <row r="64" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B64" s="38"/>
+    </row>
+    <row r="64" spans="1:69" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" s="37"/>
       <c r="C64" s="48"/>
       <c r="D64" s="48"/>
       <c r="E64" s="48"/>
@@ -3010,10 +2947,69 @@
       <c r="H64" s="48"/>
       <c r="I64" s="48"/>
       <c r="J64" s="48"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="15"/>
+      <c r="O64" s="15"/>
+      <c r="P64" s="15"/>
+      <c r="Q64" s="15"/>
+      <c r="R64" s="15"/>
+      <c r="S64" s="15"/>
+      <c r="T64" s="15"/>
+      <c r="U64" s="15"/>
+      <c r="V64" s="15"/>
+      <c r="W64" s="15"/>
+      <c r="X64" s="15"/>
+      <c r="Y64" s="15"/>
+      <c r="Z64" s="15"/>
+      <c r="AA64" s="15"/>
+      <c r="AB64" s="15"/>
+      <c r="AC64" s="15"/>
+      <c r="AD64" s="15"/>
+      <c r="AE64" s="15"/>
+      <c r="AF64" s="15"/>
+      <c r="AG64" s="15"/>
+      <c r="AH64" s="15"/>
+      <c r="AI64" s="15"/>
+      <c r="AJ64" s="15"/>
+      <c r="AK64" s="15"/>
+      <c r="AL64" s="15"/>
+      <c r="AM64" s="15"/>
+      <c r="AN64" s="15"/>
+      <c r="AO64" s="15"/>
+      <c r="AP64" s="15"/>
+      <c r="AQ64" s="15"/>
+      <c r="AR64" s="15"/>
+      <c r="AS64" s="15"/>
+      <c r="AT64" s="15"/>
+      <c r="AU64" s="15"/>
+      <c r="AV64" s="15"/>
+      <c r="AW64" s="15"/>
+      <c r="AX64" s="15"/>
+      <c r="AY64" s="15"/>
+      <c r="AZ64" s="15"/>
+      <c r="BA64" s="15"/>
+      <c r="BB64" s="15"/>
+      <c r="BC64" s="15"/>
+      <c r="BD64" s="15"/>
+      <c r="BE64" s="15"/>
+      <c r="BF64" s="15"/>
+      <c r="BG64" s="15"/>
+      <c r="BH64" s="15"/>
+      <c r="BI64" s="15"/>
+      <c r="BJ64" s="15"/>
+      <c r="BK64" s="15"/>
+      <c r="BL64" s="15"/>
+      <c r="BM64" s="15"/>
+      <c r="BN64" s="15"/>
+      <c r="BO64" s="15"/>
+      <c r="BP64" s="15"/>
+      <c r="BQ64" s="15"/>
     </row>
     <row r="65" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B65" s="38"/>
       <c r="C65" s="48"/>
@@ -3027,7 +3023,7 @@
     </row>
     <row r="66" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B66" s="38"/>
       <c r="C66" s="48"/>
@@ -3041,7 +3037,7 @@
     </row>
     <row r="67" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B67" s="38"/>
       <c r="C67" s="48"/>
@@ -3054,10 +3050,10 @@
       <c r="J67" s="48"/>
     </row>
     <row r="68" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B68" s="39"/>
+      <c r="A68" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68" s="38"/>
       <c r="C68" s="48"/>
       <c r="D68" s="48"/>
       <c r="E68" s="48"/>
@@ -3067,11 +3063,11 @@
       <c r="I68" s="48"/>
       <c r="J68" s="48"/>
     </row>
-    <row r="69" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B69" s="40"/>
+    <row r="69" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B69" s="39"/>
       <c r="C69" s="48"/>
       <c r="D69" s="48"/>
       <c r="E69" s="48"/>
@@ -3080,69 +3076,10 @@
       <c r="H69" s="48"/>
       <c r="I69" s="48"/>
       <c r="J69" s="48"/>
-      <c r="K69" s="15"/>
-      <c r="L69" s="15"/>
-      <c r="M69" s="15"/>
-      <c r="N69" s="15"/>
-      <c r="O69" s="15"/>
-      <c r="P69" s="15"/>
-      <c r="Q69" s="15"/>
-      <c r="R69" s="15"/>
-      <c r="S69" s="15"/>
-      <c r="T69" s="15"/>
-      <c r="U69" s="15"/>
-      <c r="V69" s="15"/>
-      <c r="W69" s="15"/>
-      <c r="X69" s="15"/>
-      <c r="Y69" s="15"/>
-      <c r="Z69" s="15"/>
-      <c r="AA69" s="15"/>
-      <c r="AB69" s="15"/>
-      <c r="AC69" s="15"/>
-      <c r="AD69" s="15"/>
-      <c r="AE69" s="15"/>
-      <c r="AF69" s="15"/>
-      <c r="AG69" s="15"/>
-      <c r="AH69" s="15"/>
-      <c r="AI69" s="15"/>
-      <c r="AJ69" s="15"/>
-      <c r="AK69" s="15"/>
-      <c r="AL69" s="15"/>
-      <c r="AM69" s="15"/>
-      <c r="AN69" s="15"/>
-      <c r="AO69" s="15"/>
-      <c r="AP69" s="15"/>
-      <c r="AQ69" s="15"/>
-      <c r="AR69" s="15"/>
-      <c r="AS69" s="15"/>
-      <c r="AT69" s="15"/>
-      <c r="AU69" s="15"/>
-      <c r="AV69" s="15"/>
-      <c r="AW69" s="15"/>
-      <c r="AX69" s="15"/>
-      <c r="AY69" s="15"/>
-      <c r="AZ69" s="15"/>
-      <c r="BA69" s="15"/>
-      <c r="BB69" s="15"/>
-      <c r="BC69" s="15"/>
-      <c r="BD69" s="15"/>
-      <c r="BE69" s="15"/>
-      <c r="BF69" s="15"/>
-      <c r="BG69" s="15"/>
-      <c r="BH69" s="15"/>
-      <c r="BI69" s="15"/>
-      <c r="BJ69" s="15"/>
-      <c r="BK69" s="15"/>
-      <c r="BL69" s="15"/>
-      <c r="BM69" s="15"/>
-      <c r="BN69" s="15"/>
-      <c r="BO69" s="15"/>
-      <c r="BP69" s="15"/>
-      <c r="BQ69" s="15"/>
     </row>
     <row r="70" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B70" s="40"/>
       <c r="C70" s="48"/>
@@ -3214,10 +3151,10 @@
       <c r="BQ70" s="15"/>
     </row>
     <row r="71" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A71" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B71" s="41"/>
+      <c r="A71" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" s="40"/>
       <c r="C71" s="48"/>
       <c r="D71" s="48"/>
       <c r="E71" s="48"/>
@@ -3287,78 +3224,137 @@
       <c r="BQ71" s="15"/>
     </row>
     <row r="72" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A72" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B72" s="42"/>
+      <c r="A72" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B72" s="41"/>
+      <c r="C72" s="48"/>
+      <c r="D72" s="48"/>
+      <c r="E72" s="48"/>
+      <c r="F72" s="48"/>
+      <c r="G72" s="48"/>
+      <c r="H72" s="48"/>
+      <c r="I72" s="48"/>
+      <c r="J72" s="48"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="15"/>
+      <c r="M72" s="15"/>
+      <c r="N72" s="15"/>
+      <c r="O72" s="15"/>
+      <c r="P72" s="15"/>
+      <c r="Q72" s="15"/>
+      <c r="R72" s="15"/>
+      <c r="S72" s="15"/>
+      <c r="T72" s="15"/>
+      <c r="U72" s="15"/>
+      <c r="V72" s="15"/>
+      <c r="W72" s="15"/>
+      <c r="X72" s="15"/>
+      <c r="Y72" s="15"/>
+      <c r="Z72" s="15"/>
+      <c r="AA72" s="15"/>
+      <c r="AB72" s="15"/>
+      <c r="AC72" s="15"/>
+      <c r="AD72" s="15"/>
+      <c r="AE72" s="15"/>
+      <c r="AF72" s="15"/>
+      <c r="AG72" s="15"/>
+      <c r="AH72" s="15"/>
+      <c r="AI72" s="15"/>
+      <c r="AJ72" s="15"/>
+      <c r="AK72" s="15"/>
+      <c r="AL72" s="15"/>
+      <c r="AM72" s="15"/>
+      <c r="AN72" s="15"/>
+      <c r="AO72" s="15"/>
+      <c r="AP72" s="15"/>
+      <c r="AQ72" s="15"/>
+      <c r="AR72" s="15"/>
+      <c r="AS72" s="15"/>
+      <c r="AT72" s="15"/>
+      <c r="AU72" s="15"/>
+      <c r="AV72" s="15"/>
+      <c r="AW72" s="15"/>
+      <c r="AX72" s="15"/>
+      <c r="AY72" s="15"/>
+      <c r="AZ72" s="15"/>
+      <c r="BA72" s="15"/>
+      <c r="BB72" s="15"/>
+      <c r="BC72" s="15"/>
+      <c r="BD72" s="15"/>
+      <c r="BE72" s="15"/>
+      <c r="BF72" s="15"/>
+      <c r="BG72" s="15"/>
+      <c r="BH72" s="15"/>
+      <c r="BI72" s="15"/>
+      <c r="BJ72" s="15"/>
+      <c r="BK72" s="15"/>
+      <c r="BL72" s="15"/>
+      <c r="BM72" s="15"/>
+      <c r="BN72" s="15"/>
+      <c r="BO72" s="15"/>
+      <c r="BP72" s="15"/>
+      <c r="BQ72" s="15"/>
     </row>
     <row r="73" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A73" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B73" s="43"/>
+        <v>9</v>
+      </c>
+      <c r="B73" s="42"/>
     </row>
     <row r="74" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B74" s="43"/>
+    </row>
+    <row r="75" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A75" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B74" s="42"/>
-    </row>
-    <row r="75" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A75" s="17" t="s">
+      <c r="B75" s="42"/>
+    </row>
+    <row r="76" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A76" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B75" s="44"/>
-      <c r="C75" s="54"/>
-      <c r="D75" s="54"/>
-      <c r="E75" s="54"/>
-      <c r="F75" s="54"/>
-      <c r="G75" s="54"/>
-      <c r="H75" s="54"/>
-      <c r="I75" s="55"/>
-    </row>
-    <row r="76" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A76" s="16" t="s">
+      <c r="B76" s="44"/>
+      <c r="C76" s="54"/>
+      <c r="D76" s="54"/>
+      <c r="E76" s="54"/>
+      <c r="F76" s="54"/>
+      <c r="G76" s="54"/>
+      <c r="H76" s="54"/>
+      <c r="I76" s="55"/>
+    </row>
+    <row r="77" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A77" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="45">
+      <c r="B77" s="45">
         <v>5</v>
       </c>
-      <c r="C76" s="45">
+      <c r="C77" s="45">
         <v>15</v>
       </c>
-      <c r="D76" s="45"/>
-      <c r="E76" s="56"/>
-    </row>
-    <row r="77" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A77" s="18" t="s">
+      <c r="D77" s="45"/>
+      <c r="E77" s="56"/>
+    </row>
+    <row r="78" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A78" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B77" s="46"/>
-    </row>
-    <row r="78" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A78" s="13" t="s">
+      <c r="B78" s="46"/>
+    </row>
+    <row r="79" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A79" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B78" s="42"/>
-    </row>
-    <row r="79" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="13" t="s">
-        <v>71</v>
-      </c>
       <c r="B79" s="42"/>
-      <c r="C79" s="52"/>
-      <c r="D79" s="48"/>
-      <c r="E79" s="48"/>
-      <c r="F79" s="48"/>
-      <c r="G79" s="48"/>
-      <c r="H79" s="48"/>
-      <c r="I79" s="48"/>
-      <c r="J79" s="48"/>
     </row>
     <row r="80" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B80" s="42"/>
       <c r="C80" s="52"/>
@@ -3372,7 +3368,7 @@
     </row>
     <row r="81" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B81" s="42"/>
       <c r="C81" s="52"/>
@@ -3384,51 +3380,65 @@
       <c r="I81" s="48"/>
       <c r="J81" s="48"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="B82" s="42"/>
+      <c r="C82" s="52"/>
+      <c r="D82" s="48"/>
+      <c r="E82" s="48"/>
+      <c r="F82" s="48"/>
+      <c r="G82" s="48"/>
+      <c r="H82" s="48"/>
+      <c r="I82" s="48"/>
+      <c r="J82" s="48"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B83" s="42"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B83" s="42"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A84" s="19" t="s">
+      <c r="B84" s="42"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B84" s="47"/>
+      <c r="B85" s="47"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72 B57:B58">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B73 B58:B59">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B55:B56">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56:B57">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B73">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43:B54">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44:B55">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B76">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B42">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B64:B68">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B65:B69">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -3442,13 +3452,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B77:B84 B59:B63 B69:B71</xm:sqref>
+          <xm:sqref>B78:B85 B60:B64 B70:B72</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B74</xm:sqref>
+          <xm:sqref>B75</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Add economics start time to spreadsheets
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
   <si>
     <t>recent_time</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>comorb_multiplier_diabetes_progression</t>
+  </si>
+  <si>
+    <t>economics_start_time</t>
   </si>
 </sst>
 </file>
@@ -2263,10 +2266,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BQ85"/>
+  <dimension ref="A1:BQ86"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2659,96 +2662,29 @@
       <c r="A55" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B55" s="32"/>
+      <c r="B55" s="30"/>
     </row>
     <row r="56" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
+      <c r="A56" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B56" s="32"/>
+    </row>
+    <row r="57" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B56" s="33"/>
-    </row>
-    <row r="57" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A57" s="10" t="s">
+      <c r="B57" s="33"/>
+    </row>
+    <row r="58" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="34"/>
-    </row>
-    <row r="58" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A58" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B58" s="35"/>
-      <c r="C58" s="48"/>
-      <c r="D58" s="48"/>
-      <c r="E58" s="48"/>
-      <c r="F58" s="48"/>
-      <c r="G58" s="48"/>
-      <c r="H58" s="48"/>
-      <c r="I58" s="48"/>
-      <c r="J58" s="48"/>
-      <c r="K58" s="15"/>
-      <c r="L58" s="15"/>
-      <c r="M58" s="15"/>
-      <c r="N58" s="15"/>
-      <c r="O58" s="15"/>
-      <c r="P58" s="15"/>
-      <c r="Q58" s="15"/>
-      <c r="R58" s="15"/>
-      <c r="S58" s="15"/>
-      <c r="T58" s="15"/>
-      <c r="U58" s="15"/>
-      <c r="V58" s="15"/>
-      <c r="W58" s="15"/>
-      <c r="X58" s="15"/>
-      <c r="Y58" s="15"/>
-      <c r="Z58" s="15"/>
-      <c r="AA58" s="15"/>
-      <c r="AB58" s="15"/>
-      <c r="AC58" s="15"/>
-      <c r="AD58" s="15"/>
-      <c r="AE58" s="15"/>
-      <c r="AF58" s="15"/>
-      <c r="AG58" s="15"/>
-      <c r="AH58" s="15"/>
-      <c r="AI58" s="15"/>
-      <c r="AJ58" s="15"/>
-      <c r="AK58" s="15"/>
-      <c r="AL58" s="15"/>
-      <c r="AM58" s="15"/>
-      <c r="AN58" s="15"/>
-      <c r="AO58" s="15"/>
-      <c r="AP58" s="15"/>
-      <c r="AQ58" s="15"/>
-      <c r="AR58" s="15"/>
-      <c r="AS58" s="15"/>
-      <c r="AT58" s="15"/>
-      <c r="AU58" s="15"/>
-      <c r="AV58" s="15"/>
-      <c r="AW58" s="15"/>
-      <c r="AX58" s="15"/>
-      <c r="AY58" s="15"/>
-      <c r="AZ58" s="15"/>
-      <c r="BA58" s="15"/>
-      <c r="BB58" s="15"/>
-      <c r="BC58" s="15"/>
-      <c r="BD58" s="15"/>
-      <c r="BE58" s="15"/>
-      <c r="BF58" s="15"/>
-      <c r="BG58" s="15"/>
-      <c r="BH58" s="15"/>
-      <c r="BI58" s="15"/>
-      <c r="BJ58" s="15"/>
-      <c r="BK58" s="15"/>
-      <c r="BL58" s="15"/>
-      <c r="BM58" s="15"/>
-      <c r="BN58" s="15"/>
-      <c r="BO58" s="15"/>
-      <c r="BP58" s="15"/>
-      <c r="BQ58" s="15"/>
+      <c r="B58" s="34"/>
     </row>
     <row r="59" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B59" s="35"/>
       <c r="C59" s="48"/>
@@ -2819,11 +2755,11 @@
       <c r="BP59" s="15"/>
       <c r="BQ59" s="15"/>
     </row>
-    <row r="60" spans="1:69" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B60" s="36"/>
+    <row r="60" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="35"/>
       <c r="C60" s="48"/>
       <c r="D60" s="48"/>
       <c r="E60" s="48"/>
@@ -2892,11 +2828,11 @@
       <c r="BP60" s="15"/>
       <c r="BQ60" s="15"/>
     </row>
-    <row r="61" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B61" s="35"/>
+    <row r="61" spans="1:69" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" s="36"/>
       <c r="C61" s="48"/>
       <c r="D61" s="48"/>
       <c r="E61" s="48"/>
@@ -2905,10 +2841,69 @@
       <c r="H61" s="48"/>
       <c r="I61" s="48"/>
       <c r="J61" s="48"/>
+      <c r="K61" s="15"/>
+      <c r="L61" s="15"/>
+      <c r="M61" s="15"/>
+      <c r="N61" s="15"/>
+      <c r="O61" s="15"/>
+      <c r="P61" s="15"/>
+      <c r="Q61" s="15"/>
+      <c r="R61" s="15"/>
+      <c r="S61" s="15"/>
+      <c r="T61" s="15"/>
+      <c r="U61" s="15"/>
+      <c r="V61" s="15"/>
+      <c r="W61" s="15"/>
+      <c r="X61" s="15"/>
+      <c r="Y61" s="15"/>
+      <c r="Z61" s="15"/>
+      <c r="AA61" s="15"/>
+      <c r="AB61" s="15"/>
+      <c r="AC61" s="15"/>
+      <c r="AD61" s="15"/>
+      <c r="AE61" s="15"/>
+      <c r="AF61" s="15"/>
+      <c r="AG61" s="15"/>
+      <c r="AH61" s="15"/>
+      <c r="AI61" s="15"/>
+      <c r="AJ61" s="15"/>
+      <c r="AK61" s="15"/>
+      <c r="AL61" s="15"/>
+      <c r="AM61" s="15"/>
+      <c r="AN61" s="15"/>
+      <c r="AO61" s="15"/>
+      <c r="AP61" s="15"/>
+      <c r="AQ61" s="15"/>
+      <c r="AR61" s="15"/>
+      <c r="AS61" s="15"/>
+      <c r="AT61" s="15"/>
+      <c r="AU61" s="15"/>
+      <c r="AV61" s="15"/>
+      <c r="AW61" s="15"/>
+      <c r="AX61" s="15"/>
+      <c r="AY61" s="15"/>
+      <c r="AZ61" s="15"/>
+      <c r="BA61" s="15"/>
+      <c r="BB61" s="15"/>
+      <c r="BC61" s="15"/>
+      <c r="BD61" s="15"/>
+      <c r="BE61" s="15"/>
+      <c r="BF61" s="15"/>
+      <c r="BG61" s="15"/>
+      <c r="BH61" s="15"/>
+      <c r="BI61" s="15"/>
+      <c r="BJ61" s="15"/>
+      <c r="BK61" s="15"/>
+      <c r="BL61" s="15"/>
+      <c r="BM61" s="15"/>
+      <c r="BN61" s="15"/>
+      <c r="BO61" s="15"/>
+      <c r="BP61" s="15"/>
+      <c r="BQ61" s="15"/>
     </row>
     <row r="62" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B62" s="35"/>
       <c r="C62" s="48"/>
@@ -2922,7 +2917,7 @@
     </row>
     <row r="63" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B63" s="35"/>
       <c r="C63" s="48"/>
@@ -2934,11 +2929,11 @@
       <c r="I63" s="48"/>
       <c r="J63" s="48"/>
     </row>
-    <row r="64" spans="1:69" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B64" s="37"/>
+    <row r="64" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B64" s="35"/>
       <c r="C64" s="48"/>
       <c r="D64" s="48"/>
       <c r="E64" s="48"/>
@@ -2947,71 +2942,12 @@
       <c r="H64" s="48"/>
       <c r="I64" s="48"/>
       <c r="J64" s="48"/>
-      <c r="K64" s="15"/>
-      <c r="L64" s="15"/>
-      <c r="M64" s="15"/>
-      <c r="N64" s="15"/>
-      <c r="O64" s="15"/>
-      <c r="P64" s="15"/>
-      <c r="Q64" s="15"/>
-      <c r="R64" s="15"/>
-      <c r="S64" s="15"/>
-      <c r="T64" s="15"/>
-      <c r="U64" s="15"/>
-      <c r="V64" s="15"/>
-      <c r="W64" s="15"/>
-      <c r="X64" s="15"/>
-      <c r="Y64" s="15"/>
-      <c r="Z64" s="15"/>
-      <c r="AA64" s="15"/>
-      <c r="AB64" s="15"/>
-      <c r="AC64" s="15"/>
-      <c r="AD64" s="15"/>
-      <c r="AE64" s="15"/>
-      <c r="AF64" s="15"/>
-      <c r="AG64" s="15"/>
-      <c r="AH64" s="15"/>
-      <c r="AI64" s="15"/>
-      <c r="AJ64" s="15"/>
-      <c r="AK64" s="15"/>
-      <c r="AL64" s="15"/>
-      <c r="AM64" s="15"/>
-      <c r="AN64" s="15"/>
-      <c r="AO64" s="15"/>
-      <c r="AP64" s="15"/>
-      <c r="AQ64" s="15"/>
-      <c r="AR64" s="15"/>
-      <c r="AS64" s="15"/>
-      <c r="AT64" s="15"/>
-      <c r="AU64" s="15"/>
-      <c r="AV64" s="15"/>
-      <c r="AW64" s="15"/>
-      <c r="AX64" s="15"/>
-      <c r="AY64" s="15"/>
-      <c r="AZ64" s="15"/>
-      <c r="BA64" s="15"/>
-      <c r="BB64" s="15"/>
-      <c r="BC64" s="15"/>
-      <c r="BD64" s="15"/>
-      <c r="BE64" s="15"/>
-      <c r="BF64" s="15"/>
-      <c r="BG64" s="15"/>
-      <c r="BH64" s="15"/>
-      <c r="BI64" s="15"/>
-      <c r="BJ64" s="15"/>
-      <c r="BK64" s="15"/>
-      <c r="BL64" s="15"/>
-      <c r="BM64" s="15"/>
-      <c r="BN64" s="15"/>
-      <c r="BO64" s="15"/>
-      <c r="BP64" s="15"/>
-      <c r="BQ64" s="15"/>
-    </row>
-    <row r="65" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B65" s="38"/>
+    </row>
+    <row r="65" spans="1:69" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B65" s="37"/>
       <c r="C65" s="48"/>
       <c r="D65" s="48"/>
       <c r="E65" s="48"/>
@@ -3020,10 +2956,69 @@
       <c r="H65" s="48"/>
       <c r="I65" s="48"/>
       <c r="J65" s="48"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="15"/>
+      <c r="O65" s="15"/>
+      <c r="P65" s="15"/>
+      <c r="Q65" s="15"/>
+      <c r="R65" s="15"/>
+      <c r="S65" s="15"/>
+      <c r="T65" s="15"/>
+      <c r="U65" s="15"/>
+      <c r="V65" s="15"/>
+      <c r="W65" s="15"/>
+      <c r="X65" s="15"/>
+      <c r="Y65" s="15"/>
+      <c r="Z65" s="15"/>
+      <c r="AA65" s="15"/>
+      <c r="AB65" s="15"/>
+      <c r="AC65" s="15"/>
+      <c r="AD65" s="15"/>
+      <c r="AE65" s="15"/>
+      <c r="AF65" s="15"/>
+      <c r="AG65" s="15"/>
+      <c r="AH65" s="15"/>
+      <c r="AI65" s="15"/>
+      <c r="AJ65" s="15"/>
+      <c r="AK65" s="15"/>
+      <c r="AL65" s="15"/>
+      <c r="AM65" s="15"/>
+      <c r="AN65" s="15"/>
+      <c r="AO65" s="15"/>
+      <c r="AP65" s="15"/>
+      <c r="AQ65" s="15"/>
+      <c r="AR65" s="15"/>
+      <c r="AS65" s="15"/>
+      <c r="AT65" s="15"/>
+      <c r="AU65" s="15"/>
+      <c r="AV65" s="15"/>
+      <c r="AW65" s="15"/>
+      <c r="AX65" s="15"/>
+      <c r="AY65" s="15"/>
+      <c r="AZ65" s="15"/>
+      <c r="BA65" s="15"/>
+      <c r="BB65" s="15"/>
+      <c r="BC65" s="15"/>
+      <c r="BD65" s="15"/>
+      <c r="BE65" s="15"/>
+      <c r="BF65" s="15"/>
+      <c r="BG65" s="15"/>
+      <c r="BH65" s="15"/>
+      <c r="BI65" s="15"/>
+      <c r="BJ65" s="15"/>
+      <c r="BK65" s="15"/>
+      <c r="BL65" s="15"/>
+      <c r="BM65" s="15"/>
+      <c r="BN65" s="15"/>
+      <c r="BO65" s="15"/>
+      <c r="BP65" s="15"/>
+      <c r="BQ65" s="15"/>
     </row>
     <row r="66" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B66" s="38"/>
       <c r="C66" s="48"/>
@@ -3037,7 +3032,7 @@
     </row>
     <row r="67" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B67" s="38"/>
       <c r="C67" s="48"/>
@@ -3051,7 +3046,7 @@
     </row>
     <row r="68" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B68" s="38"/>
       <c r="C68" s="48"/>
@@ -3064,10 +3059,10 @@
       <c r="J68" s="48"/>
     </row>
     <row r="69" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B69" s="39"/>
+      <c r="A69" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B69" s="38"/>
       <c r="C69" s="48"/>
       <c r="D69" s="48"/>
       <c r="E69" s="48"/>
@@ -3077,11 +3072,11 @@
       <c r="I69" s="48"/>
       <c r="J69" s="48"/>
     </row>
-    <row r="70" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B70" s="40"/>
+    <row r="70" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B70" s="39"/>
       <c r="C70" s="48"/>
       <c r="D70" s="48"/>
       <c r="E70" s="48"/>
@@ -3090,69 +3085,10 @@
       <c r="H70" s="48"/>
       <c r="I70" s="48"/>
       <c r="J70" s="48"/>
-      <c r="K70" s="15"/>
-      <c r="L70" s="15"/>
-      <c r="M70" s="15"/>
-      <c r="N70" s="15"/>
-      <c r="O70" s="15"/>
-      <c r="P70" s="15"/>
-      <c r="Q70" s="15"/>
-      <c r="R70" s="15"/>
-      <c r="S70" s="15"/>
-      <c r="T70" s="15"/>
-      <c r="U70" s="15"/>
-      <c r="V70" s="15"/>
-      <c r="W70" s="15"/>
-      <c r="X70" s="15"/>
-      <c r="Y70" s="15"/>
-      <c r="Z70" s="15"/>
-      <c r="AA70" s="15"/>
-      <c r="AB70" s="15"/>
-      <c r="AC70" s="15"/>
-      <c r="AD70" s="15"/>
-      <c r="AE70" s="15"/>
-      <c r="AF70" s="15"/>
-      <c r="AG70" s="15"/>
-      <c r="AH70" s="15"/>
-      <c r="AI70" s="15"/>
-      <c r="AJ70" s="15"/>
-      <c r="AK70" s="15"/>
-      <c r="AL70" s="15"/>
-      <c r="AM70" s="15"/>
-      <c r="AN70" s="15"/>
-      <c r="AO70" s="15"/>
-      <c r="AP70" s="15"/>
-      <c r="AQ70" s="15"/>
-      <c r="AR70" s="15"/>
-      <c r="AS70" s="15"/>
-      <c r="AT70" s="15"/>
-      <c r="AU70" s="15"/>
-      <c r="AV70" s="15"/>
-      <c r="AW70" s="15"/>
-      <c r="AX70" s="15"/>
-      <c r="AY70" s="15"/>
-      <c r="AZ70" s="15"/>
-      <c r="BA70" s="15"/>
-      <c r="BB70" s="15"/>
-      <c r="BC70" s="15"/>
-      <c r="BD70" s="15"/>
-      <c r="BE70" s="15"/>
-      <c r="BF70" s="15"/>
-      <c r="BG70" s="15"/>
-      <c r="BH70" s="15"/>
-      <c r="BI70" s="15"/>
-      <c r="BJ70" s="15"/>
-      <c r="BK70" s="15"/>
-      <c r="BL70" s="15"/>
-      <c r="BM70" s="15"/>
-      <c r="BN70" s="15"/>
-      <c r="BO70" s="15"/>
-      <c r="BP70" s="15"/>
-      <c r="BQ70" s="15"/>
     </row>
     <row r="71" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B71" s="40"/>
       <c r="C71" s="48"/>
@@ -3224,10 +3160,10 @@
       <c r="BQ71" s="15"/>
     </row>
     <row r="72" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A72" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B72" s="41"/>
+      <c r="A72" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72" s="40"/>
       <c r="C72" s="48"/>
       <c r="D72" s="48"/>
       <c r="E72" s="48"/>
@@ -3297,78 +3233,133 @@
       <c r="BQ72" s="15"/>
     </row>
     <row r="73" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A73" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B73" s="42"/>
+      <c r="A73" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="41"/>
+      <c r="C73" s="48"/>
+      <c r="D73" s="48"/>
+      <c r="E73" s="48"/>
+      <c r="F73" s="48"/>
+      <c r="G73" s="48"/>
+      <c r="H73" s="48"/>
+      <c r="I73" s="48"/>
+      <c r="J73" s="48"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="15"/>
+      <c r="O73" s="15"/>
+      <c r="P73" s="15"/>
+      <c r="Q73" s="15"/>
+      <c r="R73" s="15"/>
+      <c r="S73" s="15"/>
+      <c r="T73" s="15"/>
+      <c r="U73" s="15"/>
+      <c r="V73" s="15"/>
+      <c r="W73" s="15"/>
+      <c r="X73" s="15"/>
+      <c r="Y73" s="15"/>
+      <c r="Z73" s="15"/>
+      <c r="AA73" s="15"/>
+      <c r="AB73" s="15"/>
+      <c r="AC73" s="15"/>
+      <c r="AD73" s="15"/>
+      <c r="AE73" s="15"/>
+      <c r="AF73" s="15"/>
+      <c r="AG73" s="15"/>
+      <c r="AH73" s="15"/>
+      <c r="AI73" s="15"/>
+      <c r="AJ73" s="15"/>
+      <c r="AK73" s="15"/>
+      <c r="AL73" s="15"/>
+      <c r="AM73" s="15"/>
+      <c r="AN73" s="15"/>
+      <c r="AO73" s="15"/>
+      <c r="AP73" s="15"/>
+      <c r="AQ73" s="15"/>
+      <c r="AR73" s="15"/>
+      <c r="AS73" s="15"/>
+      <c r="AT73" s="15"/>
+      <c r="AU73" s="15"/>
+      <c r="AV73" s="15"/>
+      <c r="AW73" s="15"/>
+      <c r="AX73" s="15"/>
+      <c r="AY73" s="15"/>
+      <c r="AZ73" s="15"/>
+      <c r="BA73" s="15"/>
+      <c r="BB73" s="15"/>
+      <c r="BC73" s="15"/>
+      <c r="BD73" s="15"/>
+      <c r="BE73" s="15"/>
+      <c r="BF73" s="15"/>
+      <c r="BG73" s="15"/>
+      <c r="BH73" s="15"/>
+      <c r="BI73" s="15"/>
+      <c r="BJ73" s="15"/>
+      <c r="BK73" s="15"/>
+      <c r="BL73" s="15"/>
+      <c r="BM73" s="15"/>
+      <c r="BN73" s="15"/>
+      <c r="BO73" s="15"/>
+      <c r="BP73" s="15"/>
+      <c r="BQ73" s="15"/>
     </row>
     <row r="74" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A74" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B74" s="43"/>
+        <v>9</v>
+      </c>
+      <c r="B74" s="42"/>
     </row>
     <row r="75" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A75" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B75" s="43"/>
+    </row>
+    <row r="76" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A76" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B75" s="42"/>
-    </row>
-    <row r="76" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A76" s="17" t="s">
+      <c r="B76" s="42"/>
+    </row>
+    <row r="77" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A77" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B76" s="44"/>
-      <c r="C76" s="54"/>
-      <c r="D76" s="54"/>
-      <c r="E76" s="54"/>
-      <c r="F76" s="54"/>
-      <c r="G76" s="54"/>
-      <c r="H76" s="54"/>
-      <c r="I76" s="55"/>
-    </row>
-    <row r="77" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A77" s="16" t="s">
+      <c r="B77" s="44"/>
+      <c r="C77" s="54"/>
+      <c r="D77" s="54"/>
+      <c r="E77" s="54"/>
+      <c r="F77" s="54"/>
+      <c r="G77" s="54"/>
+      <c r="H77" s="54"/>
+      <c r="I77" s="55"/>
+    </row>
+    <row r="78" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B77" s="45">
-        <v>5</v>
-      </c>
-      <c r="C77" s="45">
-        <v>15</v>
-      </c>
-      <c r="D77" s="45"/>
-      <c r="E77" s="56"/>
-    </row>
-    <row r="78" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A78" s="18" t="s">
+      <c r="B78" s="45"/>
+      <c r="C78" s="45"/>
+      <c r="D78" s="45"/>
+      <c r="E78" s="56"/>
+    </row>
+    <row r="79" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A79" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B78" s="46"/>
-    </row>
-    <row r="79" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A79" s="13" t="s">
+      <c r="B79" s="46"/>
+    </row>
+    <row r="80" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A80" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B79" s="42"/>
-    </row>
-    <row r="80" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="13" t="s">
-        <v>71</v>
-      </c>
       <c r="B80" s="42"/>
-      <c r="C80" s="52"/>
-      <c r="D80" s="48"/>
-      <c r="E80" s="48"/>
-      <c r="F80" s="48"/>
-      <c r="G80" s="48"/>
-      <c r="H80" s="48"/>
-      <c r="I80" s="48"/>
-      <c r="J80" s="48"/>
     </row>
     <row r="81" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B81" s="42"/>
       <c r="C81" s="52"/>
@@ -3382,7 +3373,7 @@
     </row>
     <row r="82" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B82" s="42"/>
       <c r="C82" s="52"/>
@@ -3394,43 +3385,57 @@
       <c r="I82" s="48"/>
       <c r="J82" s="48"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="B83" s="42"/>
+      <c r="C83" s="52"/>
+      <c r="D83" s="48"/>
+      <c r="E83" s="48"/>
+      <c r="F83" s="48"/>
+      <c r="G83" s="48"/>
+      <c r="H83" s="48"/>
+      <c r="I83" s="48"/>
+      <c r="J83" s="48"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B84" s="42"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B84" s="42"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A85" s="19" t="s">
+      <c r="B85" s="42"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B85" s="47"/>
+      <c r="B86" s="47"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B73 B58:B59">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74 B59:B60">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B56:B57">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B57:B58">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44:B55">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44:B56">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B76">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B77">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3438,7 +3443,7 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B65:B69">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B66:B70">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -3452,13 +3457,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B78:B85 B60:B64 B70:B72</xm:sqref>
+          <xm:sqref>B79:B86 B61:B65 B71:B73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B75</xm:sqref>
+          <xm:sqref>B76</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Move discounting rate to control panel
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
   <si>
     <t>recent_time</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>economics_start_time</t>
+  </si>
+  <si>
+    <t>econ_discount_rate</t>
   </si>
 </sst>
 </file>
@@ -390,7 +393,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -447,6 +450,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1233,7 +1242,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1299,6 +1308,8 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2266,10 +2277,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BQ86"/>
+  <dimension ref="A1:BQ87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3416,6 +3427,12 @@
         <v>62</v>
       </c>
       <c r="B86" s="47"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="B87" s="58"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">

</xml_diff>

<commit_message>
Read unit costs from main spreadsheet readers
Economic unit costs now read in as constant parameters from the default
or control panel sheets.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
   <si>
     <t>recent_time</t>
   </si>
@@ -291,6 +291,24 @@
   </si>
   <si>
     <t>econ_discount_rate</t>
+  </si>
+  <si>
+    <t>econ_unitcost_vaccination</t>
+  </si>
+  <si>
+    <t>econ_unitcost_ipt</t>
+  </si>
+  <si>
+    <t>econ_unitcost_xpert</t>
+  </si>
+  <si>
+    <t>econ_unitcost_treatment_support</t>
+  </si>
+  <si>
+    <t>econ_unitcost_smearacf</t>
+  </si>
+  <si>
+    <t>econ_unitcost_xpertacf</t>
   </si>
 </sst>
 </file>
@@ -1242,7 +1260,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1308,8 +1326,13 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2277,10 +2300,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BQ87"/>
+  <dimension ref="A1:BQ93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3436,7 +3459,43 @@
       <c r="A87" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="B87" s="58"/>
+      <c r="B87" s="63"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="58" t="s">
+        <v>92</v>
+      </c>
+      <c r="B88" s="61"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89" s="61"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90" s="61"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="59" t="s">
+        <v>95</v>
+      </c>
+      <c r="B91" s="61"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="59" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92" s="61"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B93" s="62"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">

</xml_diff>

<commit_message>
Fully reconcile epi and economics inputs
All economics sheets now redundant, with data entered through common
inputs sheets.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="110">
   <si>
     <t>recent_time</t>
   </si>
@@ -309,6 +309,42 @@
   </si>
   <si>
     <t>econ_unitcost_xpertacf</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_vaccination</t>
+  </si>
+  <si>
+    <t>econ_saturation_vaccination</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_ipt</t>
+  </si>
+  <si>
+    <t>econ_saturation_ipt</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_xpert</t>
+  </si>
+  <si>
+    <t>econ_saturation_xpert</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_treatment_support</t>
+  </si>
+  <si>
+    <t>econ_saturation_treatment_support</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_smearacf</t>
+  </si>
+  <si>
+    <t>econ_saturation_smearacf</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_xpertacf</t>
+  </si>
+  <si>
+    <t>econ_saturation_xpertacf</t>
   </si>
 </sst>
 </file>
@@ -1260,7 +1296,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1316,7 +1352,6 @@
     <xf numFmtId="1" fontId="12" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2300,19 +2335,19 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BQ93"/>
+  <dimension ref="A1:BQ105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" style="48" customWidth="1"/>
-    <col min="3" max="4" width="23.28515625" style="53" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="53" customWidth="1"/>
-    <col min="6" max="10" width="9.140625" style="53"/>
+    <col min="2" max="2" width="25.5703125" style="47" customWidth="1"/>
+    <col min="3" max="4" width="23.28515625" style="52" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="52" customWidth="1"/>
+    <col min="6" max="10" width="9.140625" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -2322,309 +2357,309 @@
       <c r="B1" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="25"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="48"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="47"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="25"/>
-      <c r="C3" s="52"/>
+      <c r="C3" s="51"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B4" s="25"/>
-      <c r="C4" s="52"/>
+      <c r="C4" s="51"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B5" s="25"/>
-      <c r="C5" s="52"/>
+      <c r="C5" s="51"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B6" s="25"/>
-      <c r="C6" s="52"/>
+      <c r="C6" s="51"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="25"/>
-      <c r="C7" s="52"/>
+      <c r="C7" s="51"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
       <c r="B8" s="25"/>
-      <c r="C8" s="52"/>
+      <c r="C8" s="51"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B9" s="25"/>
-      <c r="C9" s="52"/>
+      <c r="C9" s="51"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B10" s="25"/>
-      <c r="C10" s="52"/>
+      <c r="C10" s="51"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B11" s="25"/>
-      <c r="C11" s="52"/>
+      <c r="C11" s="51"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="25"/>
-      <c r="C12" s="52"/>
+      <c r="C12" s="51"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="25"/>
-      <c r="C13" s="52"/>
+      <c r="C13" s="51"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B14" s="25"/>
-      <c r="C14" s="52"/>
+      <c r="C14" s="51"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="26"/>
-      <c r="C15" s="52"/>
+      <c r="C15" s="51"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="26"/>
-      <c r="C16" s="52"/>
+      <c r="C16" s="51"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="26"/>
-      <c r="C17" s="52"/>
+      <c r="C17" s="51"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="25"/>
-      <c r="C18" s="52"/>
+      <c r="C18" s="51"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="25"/>
-      <c r="C19" s="52"/>
+      <c r="C19" s="51"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B20" s="25"/>
-      <c r="C20" s="52"/>
+      <c r="C20" s="51"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="25"/>
-      <c r="C21" s="52"/>
+      <c r="C21" s="51"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B22" s="25"/>
-      <c r="C22" s="52"/>
+      <c r="C22" s="51"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B23" s="25"/>
-      <c r="C23" s="52"/>
+      <c r="C23" s="51"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B24" s="25"/>
-      <c r="C24" s="52"/>
+      <c r="C24" s="51"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B25" s="25"/>
-      <c r="C25" s="52"/>
+      <c r="C25" s="51"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B26" s="25"/>
-      <c r="C26" s="52"/>
+      <c r="C26" s="51"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B27" s="25"/>
-      <c r="C27" s="52"/>
+      <c r="C27" s="51"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B28" s="25"/>
-      <c r="C28" s="52"/>
+      <c r="C28" s="51"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B29" s="25"/>
-      <c r="C29" s="52"/>
+      <c r="C29" s="51"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B30" s="25"/>
-      <c r="C30" s="52"/>
+      <c r="C30" s="51"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B31" s="25"/>
-      <c r="C31" s="52"/>
+      <c r="C31" s="51"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B32" s="25"/>
-      <c r="C32" s="52"/>
+      <c r="C32" s="51"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B33" s="26"/>
-      <c r="C33" s="52"/>
+      <c r="C33" s="51"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B34" s="25"/>
-      <c r="C34" s="52"/>
+      <c r="C34" s="51"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B35" s="25"/>
-      <c r="C35" s="52"/>
+      <c r="C35" s="51"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B36" s="25"/>
-      <c r="C36" s="52"/>
+      <c r="C36" s="51"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B37" s="27"/>
-      <c r="C37" s="52"/>
+      <c r="C37" s="51"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>83</v>
       </c>
       <c r="B38" s="27"/>
-      <c r="C38" s="52"/>
+      <c r="C38" s="51"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>87</v>
       </c>
       <c r="B39" s="27"/>
-      <c r="C39" s="52"/>
+      <c r="C39" s="51"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B40" s="27"/>
-      <c r="C40" s="52"/>
+      <c r="C40" s="51"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B41" s="26"/>
-      <c r="C41" s="52"/>
+      <c r="C41" s="51"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B42" s="28"/>
-      <c r="C42" s="52"/>
+      <c r="C42" s="51"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B43" s="29"/>
-      <c r="C43" s="48"/>
+      <c r="C43" s="47"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
@@ -2721,14 +2756,14 @@
         <v>1</v>
       </c>
       <c r="B59" s="35"/>
-      <c r="C59" s="48"/>
-      <c r="D59" s="48"/>
-      <c r="E59" s="48"/>
-      <c r="F59" s="48"/>
-      <c r="G59" s="48"/>
-      <c r="H59" s="48"/>
-      <c r="I59" s="48"/>
-      <c r="J59" s="48"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="47"/>
+      <c r="H59" s="47"/>
+      <c r="I59" s="47"/>
+      <c r="J59" s="47"/>
       <c r="K59" s="15"/>
       <c r="L59" s="15"/>
       <c r="M59" s="15"/>
@@ -2794,14 +2829,14 @@
         <v>2</v>
       </c>
       <c r="B60" s="35"/>
-      <c r="C60" s="48"/>
-      <c r="D60" s="48"/>
-      <c r="E60" s="48"/>
-      <c r="F60" s="48"/>
-      <c r="G60" s="48"/>
-      <c r="H60" s="48"/>
-      <c r="I60" s="48"/>
-      <c r="J60" s="48"/>
+      <c r="C60" s="47"/>
+      <c r="D60" s="47"/>
+      <c r="E60" s="47"/>
+      <c r="F60" s="47"/>
+      <c r="G60" s="47"/>
+      <c r="H60" s="47"/>
+      <c r="I60" s="47"/>
+      <c r="J60" s="47"/>
       <c r="K60" s="15"/>
       <c r="L60" s="15"/>
       <c r="M60" s="15"/>
@@ -2867,14 +2902,14 @@
         <v>75</v>
       </c>
       <c r="B61" s="36"/>
-      <c r="C61" s="48"/>
-      <c r="D61" s="48"/>
-      <c r="E61" s="48"/>
-      <c r="F61" s="48"/>
-      <c r="G61" s="48"/>
-      <c r="H61" s="48"/>
-      <c r="I61" s="48"/>
-      <c r="J61" s="48"/>
+      <c r="C61" s="47"/>
+      <c r="D61" s="47"/>
+      <c r="E61" s="47"/>
+      <c r="F61" s="47"/>
+      <c r="G61" s="47"/>
+      <c r="H61" s="47"/>
+      <c r="I61" s="47"/>
+      <c r="J61" s="47"/>
       <c r="K61" s="15"/>
       <c r="L61" s="15"/>
       <c r="M61" s="15"/>
@@ -2940,56 +2975,56 @@
         <v>77</v>
       </c>
       <c r="B62" s="35"/>
-      <c r="C62" s="48"/>
-      <c r="D62" s="48"/>
-      <c r="E62" s="48"/>
-      <c r="F62" s="48"/>
-      <c r="G62" s="48"/>
-      <c r="H62" s="48"/>
-      <c r="I62" s="48"/>
-      <c r="J62" s="48"/>
+      <c r="C62" s="47"/>
+      <c r="D62" s="47"/>
+      <c r="E62" s="47"/>
+      <c r="F62" s="47"/>
+      <c r="G62" s="47"/>
+      <c r="H62" s="47"/>
+      <c r="I62" s="47"/>
+      <c r="J62" s="47"/>
     </row>
     <row r="63" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>76</v>
       </c>
       <c r="B63" s="35"/>
-      <c r="C63" s="48"/>
-      <c r="D63" s="48"/>
-      <c r="E63" s="48"/>
-      <c r="F63" s="48"/>
-      <c r="G63" s="48"/>
-      <c r="H63" s="48"/>
-      <c r="I63" s="48"/>
-      <c r="J63" s="48"/>
+      <c r="C63" s="47"/>
+      <c r="D63" s="47"/>
+      <c r="E63" s="47"/>
+      <c r="F63" s="47"/>
+      <c r="G63" s="47"/>
+      <c r="H63" s="47"/>
+      <c r="I63" s="47"/>
+      <c r="J63" s="47"/>
     </row>
     <row r="64" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
         <v>74</v>
       </c>
       <c r="B64" s="35"/>
-      <c r="C64" s="48"/>
-      <c r="D64" s="48"/>
-      <c r="E64" s="48"/>
-      <c r="F64" s="48"/>
-      <c r="G64" s="48"/>
-      <c r="H64" s="48"/>
-      <c r="I64" s="48"/>
-      <c r="J64" s="48"/>
+      <c r="C64" s="47"/>
+      <c r="D64" s="47"/>
+      <c r="E64" s="47"/>
+      <c r="F64" s="47"/>
+      <c r="G64" s="47"/>
+      <c r="H64" s="47"/>
+      <c r="I64" s="47"/>
+      <c r="J64" s="47"/>
     </row>
     <row r="65" spans="1:69" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>73</v>
       </c>
       <c r="B65" s="37"/>
-      <c r="C65" s="48"/>
-      <c r="D65" s="48"/>
-      <c r="E65" s="48"/>
-      <c r="F65" s="48"/>
-      <c r="G65" s="48"/>
-      <c r="H65" s="48"/>
-      <c r="I65" s="48"/>
-      <c r="J65" s="48"/>
+      <c r="C65" s="47"/>
+      <c r="D65" s="47"/>
+      <c r="E65" s="47"/>
+      <c r="F65" s="47"/>
+      <c r="G65" s="47"/>
+      <c r="H65" s="47"/>
+      <c r="I65" s="47"/>
+      <c r="J65" s="47"/>
       <c r="K65" s="15"/>
       <c r="L65" s="15"/>
       <c r="M65" s="15"/>
@@ -3055,84 +3090,84 @@
         <v>78</v>
       </c>
       <c r="B66" s="38"/>
-      <c r="C66" s="48"/>
-      <c r="D66" s="48"/>
-      <c r="E66" s="48"/>
-      <c r="F66" s="48"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="48"/>
-      <c r="I66" s="48"/>
-      <c r="J66" s="48"/>
+      <c r="C66" s="47"/>
+      <c r="D66" s="47"/>
+      <c r="E66" s="47"/>
+      <c r="F66" s="47"/>
+      <c r="G66" s="47"/>
+      <c r="H66" s="47"/>
+      <c r="I66" s="47"/>
+      <c r="J66" s="47"/>
     </row>
     <row r="67" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>79</v>
       </c>
       <c r="B67" s="38"/>
-      <c r="C67" s="48"/>
-      <c r="D67" s="48"/>
-      <c r="E67" s="48"/>
-      <c r="F67" s="48"/>
-      <c r="G67" s="48"/>
-      <c r="H67" s="48"/>
-      <c r="I67" s="48"/>
-      <c r="J67" s="48"/>
+      <c r="C67" s="47"/>
+      <c r="D67" s="47"/>
+      <c r="E67" s="47"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="47"/>
+      <c r="H67" s="47"/>
+      <c r="I67" s="47"/>
+      <c r="J67" s="47"/>
     </row>
     <row r="68" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>80</v>
       </c>
       <c r="B68" s="38"/>
-      <c r="C68" s="48"/>
-      <c r="D68" s="48"/>
-      <c r="E68" s="48"/>
-      <c r="F68" s="48"/>
-      <c r="G68" s="48"/>
-      <c r="H68" s="48"/>
-      <c r="I68" s="48"/>
-      <c r="J68" s="48"/>
+      <c r="C68" s="47"/>
+      <c r="D68" s="47"/>
+      <c r="E68" s="47"/>
+      <c r="F68" s="47"/>
+      <c r="G68" s="47"/>
+      <c r="H68" s="47"/>
+      <c r="I68" s="47"/>
+      <c r="J68" s="47"/>
     </row>
     <row r="69" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
         <v>81</v>
       </c>
       <c r="B69" s="38"/>
-      <c r="C69" s="48"/>
-      <c r="D69" s="48"/>
-      <c r="E69" s="48"/>
-      <c r="F69" s="48"/>
-      <c r="G69" s="48"/>
-      <c r="H69" s="48"/>
-      <c r="I69" s="48"/>
-      <c r="J69" s="48"/>
+      <c r="C69" s="47"/>
+      <c r="D69" s="47"/>
+      <c r="E69" s="47"/>
+      <c r="F69" s="47"/>
+      <c r="G69" s="47"/>
+      <c r="H69" s="47"/>
+      <c r="I69" s="47"/>
+      <c r="J69" s="47"/>
     </row>
     <row r="70" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="12" t="s">
         <v>82</v>
       </c>
       <c r="B70" s="39"/>
-      <c r="C70" s="48"/>
-      <c r="D70" s="48"/>
-      <c r="E70" s="48"/>
-      <c r="F70" s="48"/>
-      <c r="G70" s="48"/>
-      <c r="H70" s="48"/>
-      <c r="I70" s="48"/>
-      <c r="J70" s="48"/>
+      <c r="C70" s="47"/>
+      <c r="D70" s="47"/>
+      <c r="E70" s="47"/>
+      <c r="F70" s="47"/>
+      <c r="G70" s="47"/>
+      <c r="H70" s="47"/>
+      <c r="I70" s="47"/>
+      <c r="J70" s="47"/>
     </row>
     <row r="71" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B71" s="40"/>
-      <c r="C71" s="48"/>
-      <c r="D71" s="48"/>
-      <c r="E71" s="48"/>
-      <c r="F71" s="48"/>
-      <c r="G71" s="48"/>
-      <c r="H71" s="48"/>
-      <c r="I71" s="48"/>
-      <c r="J71" s="48"/>
+      <c r="C71" s="47"/>
+      <c r="D71" s="47"/>
+      <c r="E71" s="47"/>
+      <c r="F71" s="47"/>
+      <c r="G71" s="47"/>
+      <c r="H71" s="47"/>
+      <c r="I71" s="47"/>
+      <c r="J71" s="47"/>
       <c r="K71" s="15"/>
       <c r="L71" s="15"/>
       <c r="M71" s="15"/>
@@ -3198,14 +3233,14 @@
         <v>4</v>
       </c>
       <c r="B72" s="40"/>
-      <c r="C72" s="48"/>
-      <c r="D72" s="48"/>
-      <c r="E72" s="48"/>
-      <c r="F72" s="48"/>
-      <c r="G72" s="48"/>
-      <c r="H72" s="48"/>
-      <c r="I72" s="48"/>
-      <c r="J72" s="48"/>
+      <c r="C72" s="47"/>
+      <c r="D72" s="47"/>
+      <c r="E72" s="47"/>
+      <c r="F72" s="47"/>
+      <c r="G72" s="47"/>
+      <c r="H72" s="47"/>
+      <c r="I72" s="47"/>
+      <c r="J72" s="47"/>
       <c r="K72" s="15"/>
       <c r="L72" s="15"/>
       <c r="M72" s="15"/>
@@ -3271,14 +3306,14 @@
         <v>5</v>
       </c>
       <c r="B73" s="41"/>
-      <c r="C73" s="48"/>
-      <c r="D73" s="48"/>
-      <c r="E73" s="48"/>
-      <c r="F73" s="48"/>
-      <c r="G73" s="48"/>
-      <c r="H73" s="48"/>
-      <c r="I73" s="48"/>
-      <c r="J73" s="48"/>
+      <c r="C73" s="47"/>
+      <c r="D73" s="47"/>
+      <c r="E73" s="47"/>
+      <c r="F73" s="47"/>
+      <c r="G73" s="47"/>
+      <c r="H73" s="47"/>
+      <c r="I73" s="47"/>
+      <c r="J73" s="47"/>
       <c r="K73" s="15"/>
       <c r="L73" s="15"/>
       <c r="M73" s="15"/>
@@ -3362,13 +3397,13 @@
         <v>12</v>
       </c>
       <c r="B77" s="44"/>
-      <c r="C77" s="54"/>
-      <c r="D77" s="54"/>
-      <c r="E77" s="54"/>
-      <c r="F77" s="54"/>
-      <c r="G77" s="54"/>
-      <c r="H77" s="54"/>
-      <c r="I77" s="55"/>
+      <c r="C77" s="53"/>
+      <c r="D77" s="53"/>
+      <c r="E77" s="53"/>
+      <c r="F77" s="53"/>
+      <c r="G77" s="53"/>
+      <c r="H77" s="53"/>
+      <c r="I77" s="54"/>
     </row>
     <row r="78" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
@@ -3381,7 +3416,7 @@
         <v>15</v>
       </c>
       <c r="D78" s="45"/>
-      <c r="E78" s="56"/>
+      <c r="E78" s="55"/>
     </row>
     <row r="79" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A79" s="18" t="s">
@@ -3400,42 +3435,42 @@
         <v>71</v>
       </c>
       <c r="B81" s="42"/>
-      <c r="C81" s="52"/>
-      <c r="D81" s="48"/>
-      <c r="E81" s="48"/>
-      <c r="F81" s="48"/>
-      <c r="G81" s="48"/>
-      <c r="H81" s="48"/>
-      <c r="I81" s="48"/>
-      <c r="J81" s="48"/>
+      <c r="C81" s="51"/>
+      <c r="D81" s="47"/>
+      <c r="E81" s="47"/>
+      <c r="F81" s="47"/>
+      <c r="G81" s="47"/>
+      <c r="H81" s="47"/>
+      <c r="I81" s="47"/>
+      <c r="J81" s="47"/>
     </row>
     <row r="82" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>72</v>
       </c>
       <c r="B82" s="42"/>
-      <c r="C82" s="52"/>
-      <c r="D82" s="48"/>
-      <c r="E82" s="48"/>
-      <c r="F82" s="48"/>
-      <c r="G82" s="48"/>
-      <c r="H82" s="48"/>
-      <c r="I82" s="48"/>
-      <c r="J82" s="48"/>
+      <c r="C82" s="51"/>
+      <c r="D82" s="47"/>
+      <c r="E82" s="47"/>
+      <c r="F82" s="47"/>
+      <c r="G82" s="47"/>
+      <c r="H82" s="47"/>
+      <c r="I82" s="47"/>
+      <c r="J82" s="47"/>
     </row>
     <row r="83" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
         <v>86</v>
       </c>
       <c r="B83" s="42"/>
-      <c r="C83" s="52"/>
-      <c r="D83" s="48"/>
-      <c r="E83" s="48"/>
-      <c r="F83" s="48"/>
-      <c r="G83" s="48"/>
-      <c r="H83" s="48"/>
-      <c r="I83" s="48"/>
-      <c r="J83" s="48"/>
+      <c r="C83" s="51"/>
+      <c r="D83" s="47"/>
+      <c r="E83" s="47"/>
+      <c r="F83" s="47"/>
+      <c r="G83" s="47"/>
+      <c r="H83" s="47"/>
+      <c r="I83" s="47"/>
+      <c r="J83" s="47"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
@@ -3453,49 +3488,121 @@
       <c r="A86" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B86" s="47"/>
+      <c r="B86" s="42"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="57" t="s">
+      <c r="A87" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="B87" s="63"/>
+      <c r="B87" s="62"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="58" t="s">
+      <c r="A88" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="B88" s="61"/>
+      <c r="B88" s="60"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="58" t="s">
+      <c r="A89" s="57" t="s">
+        <v>98</v>
+      </c>
+      <c r="B89" s="60"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B90" s="60"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="B89" s="61"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="59" t="s">
+      <c r="B91" s="60"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="B92" s="60"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="57" t="s">
+        <v>101</v>
+      </c>
+      <c r="B93" s="60"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="B90" s="61"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="59" t="s">
+      <c r="B94" s="60"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="58" t="s">
+        <v>102</v>
+      </c>
+      <c r="B95" s="60"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="B96" s="60"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="B91" s="61"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="59" t="s">
+      <c r="B97" s="60"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="58" t="s">
+        <v>104</v>
+      </c>
+      <c r="B98" s="60"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="B99" s="60"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="B92" s="61"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="60" t="s">
+      <c r="B100" s="60"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="B101" s="60"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="58" t="s">
+        <v>107</v>
+      </c>
+      <c r="B102" s="60"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="B93" s="62"/>
+      <c r="B103" s="60"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="B104" s="60"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="B105" s="61"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">

</xml_diff>

<commit_message>
Started better object-oriented outputs module
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2337,8 +2337,8 @@
   </sheetPr>
   <dimension ref="A1:BQ105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3396,7 +3396,9 @@
       <c r="A77" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B77" s="44"/>
+      <c r="B77" s="44">
+        <v>1</v>
+      </c>
       <c r="C77" s="53"/>
       <c r="D77" s="53"/>
       <c r="E77" s="53"/>
@@ -3409,12 +3411,8 @@
       <c r="A78" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B78" s="45">
-        <v>5</v>
-      </c>
-      <c r="C78" s="45">
-        <v>15</v>
-      </c>
+      <c r="B78" s="45"/>
+      <c r="C78" s="45"/>
       <c r="D78" s="45"/>
       <c r="E78" s="55"/>
     </row>
@@ -3422,7 +3420,9 @@
       <c r="A79" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B79" s="46"/>
+      <c r="B79" s="46" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="80" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">

</xml_diff>

<commit_message>
Add method for processing eonomics outputs
Method added to the main analysis object to add economics dictionaries
to the main output dictionary with the same format as for the original
(i.e. epi outputs) dictionaries.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -3396,9 +3396,7 @@
       <c r="A77" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B77" s="44">
-        <v>1</v>
-      </c>
+      <c r="B77" s="44"/>
       <c r="C77" s="53"/>
       <c r="D77" s="53"/>
       <c r="E77" s="53"/>
@@ -3411,8 +3409,12 @@
       <c r="A78" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B78" s="45"/>
-      <c r="C78" s="45"/>
+      <c r="B78" s="45">
+        <v>5</v>
+      </c>
+      <c r="C78" s="45">
+        <v>15</v>
+      </c>
       <c r="D78" s="45"/>
       <c r="E78" s="55"/>
     </row>
@@ -3420,9 +3422,7 @@
       <c r="A79" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B79" s="46" t="b">
-        <v>1</v>
-      </c>
+      <c r="B79" s="46"/>
     </row>
     <row r="80" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">

</xml_diff>

<commit_message>
Get running again for all scenarios
In changing outputs code, I didn't have everything running properly.
Quick fix so others can use.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2338,7 +2338,7 @@
   <dimension ref="A1:BQ105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3396,7 +3396,9 @@
       <c r="A77" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B77" s="44"/>
+      <c r="B77" s="44">
+        <v>1</v>
+      </c>
       <c r="C77" s="53"/>
       <c r="D77" s="53"/>
       <c r="E77" s="53"/>

</xml_diff>

<commit_message>
Output module works directly with inputs
Outputs module now takes arguments directly from the spreadsheets.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="111">
   <si>
     <t>recent_time</t>
   </si>
@@ -345,6 +345,9 @@
   </si>
   <si>
     <t>econ_saturation_xpertacf</t>
+  </si>
+  <si>
+    <t>output_by_scenario</t>
   </si>
 </sst>
 </file>
@@ -2335,10 +2338,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BQ105"/>
+  <dimension ref="A1:BQ106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3396,9 +3399,7 @@
       <c r="A77" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B77" s="44">
-        <v>1</v>
-      </c>
+      <c r="B77" s="44"/>
       <c r="C77" s="53"/>
       <c r="D77" s="53"/>
       <c r="E77" s="53"/>
@@ -3428,27 +3429,19 @@
     </row>
     <row r="80" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B80" s="42"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B80" s="42"/>
-    </row>
-    <row r="81" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="13" t="s">
-        <v>71</v>
-      </c>
       <c r="B81" s="42"/>
-      <c r="C81" s="51"/>
-      <c r="D81" s="47"/>
-      <c r="E81" s="47"/>
-      <c r="F81" s="47"/>
-      <c r="G81" s="47"/>
-      <c r="H81" s="47"/>
-      <c r="I81" s="47"/>
-      <c r="J81" s="47"/>
     </row>
     <row r="82" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B82" s="42"/>
       <c r="C82" s="51"/>
@@ -3462,7 +3455,7 @@
     </row>
     <row r="83" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B83" s="42"/>
       <c r="C83" s="51"/>
@@ -3474,137 +3467,151 @@
       <c r="I83" s="47"/>
       <c r="J83" s="47"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="B84" s="42"/>
+      <c r="C84" s="51"/>
+      <c r="D84" s="47"/>
+      <c r="E84" s="47"/>
+      <c r="F84" s="47"/>
+      <c r="G84" s="47"/>
+      <c r="H84" s="47"/>
+      <c r="I84" s="47"/>
+      <c r="J84" s="47"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B85" s="42"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B85" s="42"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="19" t="s">
+      <c r="B86" s="42"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B86" s="42"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="56" t="s">
+      <c r="B87" s="42"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="B87" s="62"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="57" t="s">
-        <v>92</v>
-      </c>
-      <c r="B88" s="60"/>
+      <c r="B88" s="62"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="57" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B89" s="60"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="57" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B90" s="60"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="57" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B91" s="60"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="57" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B92" s="60"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="B93" s="60"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="57" t="s">
         <v>101</v>
-      </c>
-      <c r="B93" s="60"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="58" t="s">
-        <v>94</v>
       </c>
       <c r="B94" s="60"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="58" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B95" s="60"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B96" s="60"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="58" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B97" s="60"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="58" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B98" s="60"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B99" s="60"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="58" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B100" s="60"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="58" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B101" s="60"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B102" s="60"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="58" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B103" s="60"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B104" s="60"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="B104" s="60"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="59" t="s">
+      <c r="B105" s="60"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="B105" s="61"/>
+      <c r="B106" s="61"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
@@ -3646,7 +3653,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B79:B86 B61:B65 B71:B73</xm:sqref>
+          <xm:sqref>B79:B87 B61:B65 B71:B73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Set write direction through control panel
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
   <si>
     <t>recent_time</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>output_by_scenario</t>
+  </si>
+  <si>
+    <t>output_horizontally</t>
   </si>
 </sst>
 </file>
@@ -2338,10 +2341,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BQ106"/>
+  <dimension ref="A1:BQ107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3399,9 +3402,7 @@
       <c r="A77" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B77" s="44">
-        <v>1</v>
-      </c>
+      <c r="B77" s="44"/>
       <c r="C77" s="53"/>
       <c r="D77" s="53"/>
       <c r="E77" s="53"/>
@@ -3437,27 +3438,19 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B81" s="42"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B81" s="42"/>
-    </row>
-    <row r="82" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="13" t="s">
-        <v>71</v>
-      </c>
       <c r="B82" s="42"/>
-      <c r="C82" s="51"/>
-      <c r="D82" s="47"/>
-      <c r="E82" s="47"/>
-      <c r="F82" s="47"/>
-      <c r="G82" s="47"/>
-      <c r="H82" s="47"/>
-      <c r="I82" s="47"/>
-      <c r="J82" s="47"/>
     </row>
     <row r="83" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B83" s="42"/>
       <c r="C83" s="51"/>
@@ -3471,7 +3464,7 @@
     </row>
     <row r="84" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B84" s="42"/>
       <c r="C84" s="51"/>
@@ -3483,137 +3476,151 @@
       <c r="I84" s="47"/>
       <c r="J84" s="47"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="B85" s="42"/>
+      <c r="C85" s="51"/>
+      <c r="D85" s="47"/>
+      <c r="E85" s="47"/>
+      <c r="F85" s="47"/>
+      <c r="G85" s="47"/>
+      <c r="H85" s="47"/>
+      <c r="I85" s="47"/>
+      <c r="J85" s="47"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B86" s="42"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B86" s="42"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="19" t="s">
+      <c r="B87" s="42"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A88" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B87" s="42"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="56" t="s">
+      <c r="B88" s="42"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="B88" s="62"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="57" t="s">
-        <v>92</v>
-      </c>
-      <c r="B89" s="60"/>
+      <c r="B89" s="62"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="57" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B90" s="60"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="57" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B91" s="60"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="57" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B92" s="60"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="57" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B93" s="60"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="B94" s="60"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A95" s="57" t="s">
         <v>101</v>
-      </c>
-      <c r="B94" s="60"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="58" t="s">
-        <v>94</v>
       </c>
       <c r="B95" s="60"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="58" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B96" s="60"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B97" s="60"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="58" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B98" s="60"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="58" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B99" s="60"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B100" s="60"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="58" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B101" s="60"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="58" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B102" s="60"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B103" s="60"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="58" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B104" s="60"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B105" s="60"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="B105" s="60"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="59" t="s">
+      <c r="B106" s="60"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="B106" s="61"/>
+      <c r="B107" s="61"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
@@ -3655,7 +3662,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B79:B87 B61:B65 B71:B73</xm:sqref>
+          <xm:sqref>B79:B88 B61:B65 B71:B73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Set times to write sheets through control panel
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="115">
   <si>
     <t>recent_time</t>
   </si>
@@ -351,6 +351,15 @@
   </si>
   <si>
     <t>output_horizontally</t>
+  </si>
+  <si>
+    <t>report_start_time</t>
+  </si>
+  <si>
+    <t>report_end_time</t>
+  </si>
+  <si>
+    <t>report_step_time</t>
   </si>
 </sst>
 </file>
@@ -2341,10 +2350,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BQ107"/>
+  <dimension ref="A1:BQ110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2741,244 +2750,43 @@
     </row>
     <row r="56" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" s="30"/>
+    </row>
+    <row r="57" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" s="30"/>
+    </row>
+    <row r="58" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" s="30"/>
+    </row>
+    <row r="59" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B56" s="32"/>
-    </row>
-    <row r="57" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
+      <c r="B59" s="32"/>
+    </row>
+    <row r="60" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="33"/>
-    </row>
-    <row r="58" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A58" s="10" t="s">
+      <c r="B60" s="33"/>
+    </row>
+    <row r="61" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A61" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="34"/>
-    </row>
-    <row r="59" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
+      <c r="B61" s="34"/>
+    </row>
+    <row r="62" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A62" s="11" t="s">
         <v>1</v>
-      </c>
-      <c r="B59" s="35"/>
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
-      <c r="E59" s="47"/>
-      <c r="F59" s="47"/>
-      <c r="G59" s="47"/>
-      <c r="H59" s="47"/>
-      <c r="I59" s="47"/>
-      <c r="J59" s="47"/>
-      <c r="K59" s="15"/>
-      <c r="L59" s="15"/>
-      <c r="M59" s="15"/>
-      <c r="N59" s="15"/>
-      <c r="O59" s="15"/>
-      <c r="P59" s="15"/>
-      <c r="Q59" s="15"/>
-      <c r="R59" s="15"/>
-      <c r="S59" s="15"/>
-      <c r="T59" s="15"/>
-      <c r="U59" s="15"/>
-      <c r="V59" s="15"/>
-      <c r="W59" s="15"/>
-      <c r="X59" s="15"/>
-      <c r="Y59" s="15"/>
-      <c r="Z59" s="15"/>
-      <c r="AA59" s="15"/>
-      <c r="AB59" s="15"/>
-      <c r="AC59" s="15"/>
-      <c r="AD59" s="15"/>
-      <c r="AE59" s="15"/>
-      <c r="AF59" s="15"/>
-      <c r="AG59" s="15"/>
-      <c r="AH59" s="15"/>
-      <c r="AI59" s="15"/>
-      <c r="AJ59" s="15"/>
-      <c r="AK59" s="15"/>
-      <c r="AL59" s="15"/>
-      <c r="AM59" s="15"/>
-      <c r="AN59" s="15"/>
-      <c r="AO59" s="15"/>
-      <c r="AP59" s="15"/>
-      <c r="AQ59" s="15"/>
-      <c r="AR59" s="15"/>
-      <c r="AS59" s="15"/>
-      <c r="AT59" s="15"/>
-      <c r="AU59" s="15"/>
-      <c r="AV59" s="15"/>
-      <c r="AW59" s="15"/>
-      <c r="AX59" s="15"/>
-      <c r="AY59" s="15"/>
-      <c r="AZ59" s="15"/>
-      <c r="BA59" s="15"/>
-      <c r="BB59" s="15"/>
-      <c r="BC59" s="15"/>
-      <c r="BD59" s="15"/>
-      <c r="BE59" s="15"/>
-      <c r="BF59" s="15"/>
-      <c r="BG59" s="15"/>
-      <c r="BH59" s="15"/>
-      <c r="BI59" s="15"/>
-      <c r="BJ59" s="15"/>
-      <c r="BK59" s="15"/>
-      <c r="BL59" s="15"/>
-      <c r="BM59" s="15"/>
-      <c r="BN59" s="15"/>
-      <c r="BO59" s="15"/>
-      <c r="BP59" s="15"/>
-      <c r="BQ59" s="15"/>
-    </row>
-    <row r="60" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B60" s="35"/>
-      <c r="C60" s="47"/>
-      <c r="D60" s="47"/>
-      <c r="E60" s="47"/>
-      <c r="F60" s="47"/>
-      <c r="G60" s="47"/>
-      <c r="H60" s="47"/>
-      <c r="I60" s="47"/>
-      <c r="J60" s="47"/>
-      <c r="K60" s="15"/>
-      <c r="L60" s="15"/>
-      <c r="M60" s="15"/>
-      <c r="N60" s="15"/>
-      <c r="O60" s="15"/>
-      <c r="P60" s="15"/>
-      <c r="Q60" s="15"/>
-      <c r="R60" s="15"/>
-      <c r="S60" s="15"/>
-      <c r="T60" s="15"/>
-      <c r="U60" s="15"/>
-      <c r="V60" s="15"/>
-      <c r="W60" s="15"/>
-      <c r="X60" s="15"/>
-      <c r="Y60" s="15"/>
-      <c r="Z60" s="15"/>
-      <c r="AA60" s="15"/>
-      <c r="AB60" s="15"/>
-      <c r="AC60" s="15"/>
-      <c r="AD60" s="15"/>
-      <c r="AE60" s="15"/>
-      <c r="AF60" s="15"/>
-      <c r="AG60" s="15"/>
-      <c r="AH60" s="15"/>
-      <c r="AI60" s="15"/>
-      <c r="AJ60" s="15"/>
-      <c r="AK60" s="15"/>
-      <c r="AL60" s="15"/>
-      <c r="AM60" s="15"/>
-      <c r="AN60" s="15"/>
-      <c r="AO60" s="15"/>
-      <c r="AP60" s="15"/>
-      <c r="AQ60" s="15"/>
-      <c r="AR60" s="15"/>
-      <c r="AS60" s="15"/>
-      <c r="AT60" s="15"/>
-      <c r="AU60" s="15"/>
-      <c r="AV60" s="15"/>
-      <c r="AW60" s="15"/>
-      <c r="AX60" s="15"/>
-      <c r="AY60" s="15"/>
-      <c r="AZ60" s="15"/>
-      <c r="BA60" s="15"/>
-      <c r="BB60" s="15"/>
-      <c r="BC60" s="15"/>
-      <c r="BD60" s="15"/>
-      <c r="BE60" s="15"/>
-      <c r="BF60" s="15"/>
-      <c r="BG60" s="15"/>
-      <c r="BH60" s="15"/>
-      <c r="BI60" s="15"/>
-      <c r="BJ60" s="15"/>
-      <c r="BK60" s="15"/>
-      <c r="BL60" s="15"/>
-      <c r="BM60" s="15"/>
-      <c r="BN60" s="15"/>
-      <c r="BO60" s="15"/>
-      <c r="BP60" s="15"/>
-      <c r="BQ60" s="15"/>
-    </row>
-    <row r="61" spans="1:69" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="B61" s="36"/>
-      <c r="C61" s="47"/>
-      <c r="D61" s="47"/>
-      <c r="E61" s="47"/>
-      <c r="F61" s="47"/>
-      <c r="G61" s="47"/>
-      <c r="H61" s="47"/>
-      <c r="I61" s="47"/>
-      <c r="J61" s="47"/>
-      <c r="K61" s="15"/>
-      <c r="L61" s="15"/>
-      <c r="M61" s="15"/>
-      <c r="N61" s="15"/>
-      <c r="O61" s="15"/>
-      <c r="P61" s="15"/>
-      <c r="Q61" s="15"/>
-      <c r="R61" s="15"/>
-      <c r="S61" s="15"/>
-      <c r="T61" s="15"/>
-      <c r="U61" s="15"/>
-      <c r="V61" s="15"/>
-      <c r="W61" s="15"/>
-      <c r="X61" s="15"/>
-      <c r="Y61" s="15"/>
-      <c r="Z61" s="15"/>
-      <c r="AA61" s="15"/>
-      <c r="AB61" s="15"/>
-      <c r="AC61" s="15"/>
-      <c r="AD61" s="15"/>
-      <c r="AE61" s="15"/>
-      <c r="AF61" s="15"/>
-      <c r="AG61" s="15"/>
-      <c r="AH61" s="15"/>
-      <c r="AI61" s="15"/>
-      <c r="AJ61" s="15"/>
-      <c r="AK61" s="15"/>
-      <c r="AL61" s="15"/>
-      <c r="AM61" s="15"/>
-      <c r="AN61" s="15"/>
-      <c r="AO61" s="15"/>
-      <c r="AP61" s="15"/>
-      <c r="AQ61" s="15"/>
-      <c r="AR61" s="15"/>
-      <c r="AS61" s="15"/>
-      <c r="AT61" s="15"/>
-      <c r="AU61" s="15"/>
-      <c r="AV61" s="15"/>
-      <c r="AW61" s="15"/>
-      <c r="AX61" s="15"/>
-      <c r="AY61" s="15"/>
-      <c r="AZ61" s="15"/>
-      <c r="BA61" s="15"/>
-      <c r="BB61" s="15"/>
-      <c r="BC61" s="15"/>
-      <c r="BD61" s="15"/>
-      <c r="BE61" s="15"/>
-      <c r="BF61" s="15"/>
-      <c r="BG61" s="15"/>
-      <c r="BH61" s="15"/>
-      <c r="BI61" s="15"/>
-      <c r="BJ61" s="15"/>
-      <c r="BK61" s="15"/>
-      <c r="BL61" s="15"/>
-      <c r="BM61" s="15"/>
-      <c r="BN61" s="15"/>
-      <c r="BO61" s="15"/>
-      <c r="BP61" s="15"/>
-      <c r="BQ61" s="15"/>
-    </row>
-    <row r="62" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
-        <v>77</v>
       </c>
       <c r="B62" s="35"/>
       <c r="C62" s="47"/>
@@ -2989,10 +2797,69 @@
       <c r="H62" s="47"/>
       <c r="I62" s="47"/>
       <c r="J62" s="47"/>
-    </row>
-    <row r="63" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K62" s="15"/>
+      <c r="L62" s="15"/>
+      <c r="M62" s="15"/>
+      <c r="N62" s="15"/>
+      <c r="O62" s="15"/>
+      <c r="P62" s="15"/>
+      <c r="Q62" s="15"/>
+      <c r="R62" s="15"/>
+      <c r="S62" s="15"/>
+      <c r="T62" s="15"/>
+      <c r="U62" s="15"/>
+      <c r="V62" s="15"/>
+      <c r="W62" s="15"/>
+      <c r="X62" s="15"/>
+      <c r="Y62" s="15"/>
+      <c r="Z62" s="15"/>
+      <c r="AA62" s="15"/>
+      <c r="AB62" s="15"/>
+      <c r="AC62" s="15"/>
+      <c r="AD62" s="15"/>
+      <c r="AE62" s="15"/>
+      <c r="AF62" s="15"/>
+      <c r="AG62" s="15"/>
+      <c r="AH62" s="15"/>
+      <c r="AI62" s="15"/>
+      <c r="AJ62" s="15"/>
+      <c r="AK62" s="15"/>
+      <c r="AL62" s="15"/>
+      <c r="AM62" s="15"/>
+      <c r="AN62" s="15"/>
+      <c r="AO62" s="15"/>
+      <c r="AP62" s="15"/>
+      <c r="AQ62" s="15"/>
+      <c r="AR62" s="15"/>
+      <c r="AS62" s="15"/>
+      <c r="AT62" s="15"/>
+      <c r="AU62" s="15"/>
+      <c r="AV62" s="15"/>
+      <c r="AW62" s="15"/>
+      <c r="AX62" s="15"/>
+      <c r="AY62" s="15"/>
+      <c r="AZ62" s="15"/>
+      <c r="BA62" s="15"/>
+      <c r="BB62" s="15"/>
+      <c r="BC62" s="15"/>
+      <c r="BD62" s="15"/>
+      <c r="BE62" s="15"/>
+      <c r="BF62" s="15"/>
+      <c r="BG62" s="15"/>
+      <c r="BH62" s="15"/>
+      <c r="BI62" s="15"/>
+      <c r="BJ62" s="15"/>
+      <c r="BK62" s="15"/>
+      <c r="BL62" s="15"/>
+      <c r="BM62" s="15"/>
+      <c r="BN62" s="15"/>
+      <c r="BO62" s="15"/>
+      <c r="BP62" s="15"/>
+      <c r="BQ62" s="15"/>
+    </row>
+    <row r="63" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="B63" s="35"/>
       <c r="C63" s="47"/>
@@ -3003,12 +2870,71 @@
       <c r="H63" s="47"/>
       <c r="I63" s="47"/>
       <c r="J63" s="47"/>
-    </row>
-    <row r="64" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B64" s="35"/>
+      <c r="K63" s="15"/>
+      <c r="L63" s="15"/>
+      <c r="M63" s="15"/>
+      <c r="N63" s="15"/>
+      <c r="O63" s="15"/>
+      <c r="P63" s="15"/>
+      <c r="Q63" s="15"/>
+      <c r="R63" s="15"/>
+      <c r="S63" s="15"/>
+      <c r="T63" s="15"/>
+      <c r="U63" s="15"/>
+      <c r="V63" s="15"/>
+      <c r="W63" s="15"/>
+      <c r="X63" s="15"/>
+      <c r="Y63" s="15"/>
+      <c r="Z63" s="15"/>
+      <c r="AA63" s="15"/>
+      <c r="AB63" s="15"/>
+      <c r="AC63" s="15"/>
+      <c r="AD63" s="15"/>
+      <c r="AE63" s="15"/>
+      <c r="AF63" s="15"/>
+      <c r="AG63" s="15"/>
+      <c r="AH63" s="15"/>
+      <c r="AI63" s="15"/>
+      <c r="AJ63" s="15"/>
+      <c r="AK63" s="15"/>
+      <c r="AL63" s="15"/>
+      <c r="AM63" s="15"/>
+      <c r="AN63" s="15"/>
+      <c r="AO63" s="15"/>
+      <c r="AP63" s="15"/>
+      <c r="AQ63" s="15"/>
+      <c r="AR63" s="15"/>
+      <c r="AS63" s="15"/>
+      <c r="AT63" s="15"/>
+      <c r="AU63" s="15"/>
+      <c r="AV63" s="15"/>
+      <c r="AW63" s="15"/>
+      <c r="AX63" s="15"/>
+      <c r="AY63" s="15"/>
+      <c r="AZ63" s="15"/>
+      <c r="BA63" s="15"/>
+      <c r="BB63" s="15"/>
+      <c r="BC63" s="15"/>
+      <c r="BD63" s="15"/>
+      <c r="BE63" s="15"/>
+      <c r="BF63" s="15"/>
+      <c r="BG63" s="15"/>
+      <c r="BH63" s="15"/>
+      <c r="BI63" s="15"/>
+      <c r="BJ63" s="15"/>
+      <c r="BK63" s="15"/>
+      <c r="BL63" s="15"/>
+      <c r="BM63" s="15"/>
+      <c r="BN63" s="15"/>
+      <c r="BO63" s="15"/>
+      <c r="BP63" s="15"/>
+      <c r="BQ63" s="15"/>
+    </row>
+    <row r="64" spans="1:69" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64" s="36"/>
       <c r="C64" s="47"/>
       <c r="D64" s="47"/>
       <c r="E64" s="47"/>
@@ -3017,12 +2943,71 @@
       <c r="H64" s="47"/>
       <c r="I64" s="47"/>
       <c r="J64" s="47"/>
-    </row>
-    <row r="65" spans="1:69" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B65" s="37"/>
+      <c r="K64" s="15"/>
+      <c r="L64" s="15"/>
+      <c r="M64" s="15"/>
+      <c r="N64" s="15"/>
+      <c r="O64" s="15"/>
+      <c r="P64" s="15"/>
+      <c r="Q64" s="15"/>
+      <c r="R64" s="15"/>
+      <c r="S64" s="15"/>
+      <c r="T64" s="15"/>
+      <c r="U64" s="15"/>
+      <c r="V64" s="15"/>
+      <c r="W64" s="15"/>
+      <c r="X64" s="15"/>
+      <c r="Y64" s="15"/>
+      <c r="Z64" s="15"/>
+      <c r="AA64" s="15"/>
+      <c r="AB64" s="15"/>
+      <c r="AC64" s="15"/>
+      <c r="AD64" s="15"/>
+      <c r="AE64" s="15"/>
+      <c r="AF64" s="15"/>
+      <c r="AG64" s="15"/>
+      <c r="AH64" s="15"/>
+      <c r="AI64" s="15"/>
+      <c r="AJ64" s="15"/>
+      <c r="AK64" s="15"/>
+      <c r="AL64" s="15"/>
+      <c r="AM64" s="15"/>
+      <c r="AN64" s="15"/>
+      <c r="AO64" s="15"/>
+      <c r="AP64" s="15"/>
+      <c r="AQ64" s="15"/>
+      <c r="AR64" s="15"/>
+      <c r="AS64" s="15"/>
+      <c r="AT64" s="15"/>
+      <c r="AU64" s="15"/>
+      <c r="AV64" s="15"/>
+      <c r="AW64" s="15"/>
+      <c r="AX64" s="15"/>
+      <c r="AY64" s="15"/>
+      <c r="AZ64" s="15"/>
+      <c r="BA64" s="15"/>
+      <c r="BB64" s="15"/>
+      <c r="BC64" s="15"/>
+      <c r="BD64" s="15"/>
+      <c r="BE64" s="15"/>
+      <c r="BF64" s="15"/>
+      <c r="BG64" s="15"/>
+      <c r="BH64" s="15"/>
+      <c r="BI64" s="15"/>
+      <c r="BJ64" s="15"/>
+      <c r="BK64" s="15"/>
+      <c r="BL64" s="15"/>
+      <c r="BM64" s="15"/>
+      <c r="BN64" s="15"/>
+      <c r="BO64" s="15"/>
+      <c r="BP64" s="15"/>
+      <c r="BQ64" s="15"/>
+    </row>
+    <row r="65" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B65" s="35"/>
       <c r="C65" s="47"/>
       <c r="D65" s="47"/>
       <c r="E65" s="47"/>
@@ -3031,71 +3016,12 @@
       <c r="H65" s="47"/>
       <c r="I65" s="47"/>
       <c r="J65" s="47"/>
-      <c r="K65" s="15"/>
-      <c r="L65" s="15"/>
-      <c r="M65" s="15"/>
-      <c r="N65" s="15"/>
-      <c r="O65" s="15"/>
-      <c r="P65" s="15"/>
-      <c r="Q65" s="15"/>
-      <c r="R65" s="15"/>
-      <c r="S65" s="15"/>
-      <c r="T65" s="15"/>
-      <c r="U65" s="15"/>
-      <c r="V65" s="15"/>
-      <c r="W65" s="15"/>
-      <c r="X65" s="15"/>
-      <c r="Y65" s="15"/>
-      <c r="Z65" s="15"/>
-      <c r="AA65" s="15"/>
-      <c r="AB65" s="15"/>
-      <c r="AC65" s="15"/>
-      <c r="AD65" s="15"/>
-      <c r="AE65" s="15"/>
-      <c r="AF65" s="15"/>
-      <c r="AG65" s="15"/>
-      <c r="AH65" s="15"/>
-      <c r="AI65" s="15"/>
-      <c r="AJ65" s="15"/>
-      <c r="AK65" s="15"/>
-      <c r="AL65" s="15"/>
-      <c r="AM65" s="15"/>
-      <c r="AN65" s="15"/>
-      <c r="AO65" s="15"/>
-      <c r="AP65" s="15"/>
-      <c r="AQ65" s="15"/>
-      <c r="AR65" s="15"/>
-      <c r="AS65" s="15"/>
-      <c r="AT65" s="15"/>
-      <c r="AU65" s="15"/>
-      <c r="AV65" s="15"/>
-      <c r="AW65" s="15"/>
-      <c r="AX65" s="15"/>
-      <c r="AY65" s="15"/>
-      <c r="AZ65" s="15"/>
-      <c r="BA65" s="15"/>
-      <c r="BB65" s="15"/>
-      <c r="BC65" s="15"/>
-      <c r="BD65" s="15"/>
-      <c r="BE65" s="15"/>
-      <c r="BF65" s="15"/>
-      <c r="BG65" s="15"/>
-      <c r="BH65" s="15"/>
-      <c r="BI65" s="15"/>
-      <c r="BJ65" s="15"/>
-      <c r="BK65" s="15"/>
-      <c r="BL65" s="15"/>
-      <c r="BM65" s="15"/>
-      <c r="BN65" s="15"/>
-      <c r="BO65" s="15"/>
-      <c r="BP65" s="15"/>
-      <c r="BQ65" s="15"/>
     </row>
     <row r="66" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B66" s="38"/>
+        <v>76</v>
+      </c>
+      <c r="B66" s="35"/>
       <c r="C66" s="47"/>
       <c r="D66" s="47"/>
       <c r="E66" s="47"/>
@@ -3107,9 +3033,9 @@
     </row>
     <row r="67" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B67" s="38"/>
+        <v>74</v>
+      </c>
+      <c r="B67" s="35"/>
       <c r="C67" s="47"/>
       <c r="D67" s="47"/>
       <c r="E67" s="47"/>
@@ -3119,11 +3045,11 @@
       <c r="I67" s="47"/>
       <c r="J67" s="47"/>
     </row>
-    <row r="68" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B68" s="38"/>
+    <row r="68" spans="1:69" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B68" s="37"/>
       <c r="C68" s="47"/>
       <c r="D68" s="47"/>
       <c r="E68" s="47"/>
@@ -3132,10 +3058,69 @@
       <c r="H68" s="47"/>
       <c r="I68" s="47"/>
       <c r="J68" s="47"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="15"/>
+      <c r="M68" s="15"/>
+      <c r="N68" s="15"/>
+      <c r="O68" s="15"/>
+      <c r="P68" s="15"/>
+      <c r="Q68" s="15"/>
+      <c r="R68" s="15"/>
+      <c r="S68" s="15"/>
+      <c r="T68" s="15"/>
+      <c r="U68" s="15"/>
+      <c r="V68" s="15"/>
+      <c r="W68" s="15"/>
+      <c r="X68" s="15"/>
+      <c r="Y68" s="15"/>
+      <c r="Z68" s="15"/>
+      <c r="AA68" s="15"/>
+      <c r="AB68" s="15"/>
+      <c r="AC68" s="15"/>
+      <c r="AD68" s="15"/>
+      <c r="AE68" s="15"/>
+      <c r="AF68" s="15"/>
+      <c r="AG68" s="15"/>
+      <c r="AH68" s="15"/>
+      <c r="AI68" s="15"/>
+      <c r="AJ68" s="15"/>
+      <c r="AK68" s="15"/>
+      <c r="AL68" s="15"/>
+      <c r="AM68" s="15"/>
+      <c r="AN68" s="15"/>
+      <c r="AO68" s="15"/>
+      <c r="AP68" s="15"/>
+      <c r="AQ68" s="15"/>
+      <c r="AR68" s="15"/>
+      <c r="AS68" s="15"/>
+      <c r="AT68" s="15"/>
+      <c r="AU68" s="15"/>
+      <c r="AV68" s="15"/>
+      <c r="AW68" s="15"/>
+      <c r="AX68" s="15"/>
+      <c r="AY68" s="15"/>
+      <c r="AZ68" s="15"/>
+      <c r="BA68" s="15"/>
+      <c r="BB68" s="15"/>
+      <c r="BC68" s="15"/>
+      <c r="BD68" s="15"/>
+      <c r="BE68" s="15"/>
+      <c r="BF68" s="15"/>
+      <c r="BG68" s="15"/>
+      <c r="BH68" s="15"/>
+      <c r="BI68" s="15"/>
+      <c r="BJ68" s="15"/>
+      <c r="BK68" s="15"/>
+      <c r="BL68" s="15"/>
+      <c r="BM68" s="15"/>
+      <c r="BN68" s="15"/>
+      <c r="BO68" s="15"/>
+      <c r="BP68" s="15"/>
+      <c r="BQ68" s="15"/>
     </row>
     <row r="69" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B69" s="38"/>
       <c r="C69" s="47"/>
@@ -3148,10 +3133,10 @@
       <c r="J69" s="47"/>
     </row>
     <row r="70" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="B70" s="39"/>
+      <c r="A70" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70" s="38"/>
       <c r="C70" s="47"/>
       <c r="D70" s="47"/>
       <c r="E70" s="47"/>
@@ -3161,11 +3146,11 @@
       <c r="I70" s="47"/>
       <c r="J70" s="47"/>
     </row>
-    <row r="71" spans="1:69" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B71" s="40"/>
+        <v>80</v>
+      </c>
+      <c r="B71" s="38"/>
       <c r="C71" s="47"/>
       <c r="D71" s="47"/>
       <c r="E71" s="47"/>
@@ -3174,71 +3159,12 @@
       <c r="H71" s="47"/>
       <c r="I71" s="47"/>
       <c r="J71" s="47"/>
-      <c r="K71" s="15"/>
-      <c r="L71" s="15"/>
-      <c r="M71" s="15"/>
-      <c r="N71" s="15"/>
-      <c r="O71" s="15"/>
-      <c r="P71" s="15"/>
-      <c r="Q71" s="15"/>
-      <c r="R71" s="15"/>
-      <c r="S71" s="15"/>
-      <c r="T71" s="15"/>
-      <c r="U71" s="15"/>
-      <c r="V71" s="15"/>
-      <c r="W71" s="15"/>
-      <c r="X71" s="15"/>
-      <c r="Y71" s="15"/>
-      <c r="Z71" s="15"/>
-      <c r="AA71" s="15"/>
-      <c r="AB71" s="15"/>
-      <c r="AC71" s="15"/>
-      <c r="AD71" s="15"/>
-      <c r="AE71" s="15"/>
-      <c r="AF71" s="15"/>
-      <c r="AG71" s="15"/>
-      <c r="AH71" s="15"/>
-      <c r="AI71" s="15"/>
-      <c r="AJ71" s="15"/>
-      <c r="AK71" s="15"/>
-      <c r="AL71" s="15"/>
-      <c r="AM71" s="15"/>
-      <c r="AN71" s="15"/>
-      <c r="AO71" s="15"/>
-      <c r="AP71" s="15"/>
-      <c r="AQ71" s="15"/>
-      <c r="AR71" s="15"/>
-      <c r="AS71" s="15"/>
-      <c r="AT71" s="15"/>
-      <c r="AU71" s="15"/>
-      <c r="AV71" s="15"/>
-      <c r="AW71" s="15"/>
-      <c r="AX71" s="15"/>
-      <c r="AY71" s="15"/>
-      <c r="AZ71" s="15"/>
-      <c r="BA71" s="15"/>
-      <c r="BB71" s="15"/>
-      <c r="BC71" s="15"/>
-      <c r="BD71" s="15"/>
-      <c r="BE71" s="15"/>
-      <c r="BF71" s="15"/>
-      <c r="BG71" s="15"/>
-      <c r="BH71" s="15"/>
-      <c r="BI71" s="15"/>
-      <c r="BJ71" s="15"/>
-      <c r="BK71" s="15"/>
-      <c r="BL71" s="15"/>
-      <c r="BM71" s="15"/>
-      <c r="BN71" s="15"/>
-      <c r="BO71" s="15"/>
-      <c r="BP71" s="15"/>
-      <c r="BQ71" s="15"/>
-    </row>
-    <row r="72" spans="1:69" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B72" s="40"/>
+        <v>81</v>
+      </c>
+      <c r="B72" s="38"/>
       <c r="C72" s="47"/>
       <c r="D72" s="47"/>
       <c r="E72" s="47"/>
@@ -3247,71 +3173,12 @@
       <c r="H72" s="47"/>
       <c r="I72" s="47"/>
       <c r="J72" s="47"/>
-      <c r="K72" s="15"/>
-      <c r="L72" s="15"/>
-      <c r="M72" s="15"/>
-      <c r="N72" s="15"/>
-      <c r="O72" s="15"/>
-      <c r="P72" s="15"/>
-      <c r="Q72" s="15"/>
-      <c r="R72" s="15"/>
-      <c r="S72" s="15"/>
-      <c r="T72" s="15"/>
-      <c r="U72" s="15"/>
-      <c r="V72" s="15"/>
-      <c r="W72" s="15"/>
-      <c r="X72" s="15"/>
-      <c r="Y72" s="15"/>
-      <c r="Z72" s="15"/>
-      <c r="AA72" s="15"/>
-      <c r="AB72" s="15"/>
-      <c r="AC72" s="15"/>
-      <c r="AD72" s="15"/>
-      <c r="AE72" s="15"/>
-      <c r="AF72" s="15"/>
-      <c r="AG72" s="15"/>
-      <c r="AH72" s="15"/>
-      <c r="AI72" s="15"/>
-      <c r="AJ72" s="15"/>
-      <c r="AK72" s="15"/>
-      <c r="AL72" s="15"/>
-      <c r="AM72" s="15"/>
-      <c r="AN72" s="15"/>
-      <c r="AO72" s="15"/>
-      <c r="AP72" s="15"/>
-      <c r="AQ72" s="15"/>
-      <c r="AR72" s="15"/>
-      <c r="AS72" s="15"/>
-      <c r="AT72" s="15"/>
-      <c r="AU72" s="15"/>
-      <c r="AV72" s="15"/>
-      <c r="AW72" s="15"/>
-      <c r="AX72" s="15"/>
-      <c r="AY72" s="15"/>
-      <c r="AZ72" s="15"/>
-      <c r="BA72" s="15"/>
-      <c r="BB72" s="15"/>
-      <c r="BC72" s="15"/>
-      <c r="BD72" s="15"/>
-      <c r="BE72" s="15"/>
-      <c r="BF72" s="15"/>
-      <c r="BG72" s="15"/>
-      <c r="BH72" s="15"/>
-      <c r="BI72" s="15"/>
-      <c r="BJ72" s="15"/>
-      <c r="BK72" s="15"/>
-      <c r="BL72" s="15"/>
-      <c r="BM72" s="15"/>
-      <c r="BN72" s="15"/>
-      <c r="BO72" s="15"/>
-      <c r="BP72" s="15"/>
-      <c r="BQ72" s="15"/>
-    </row>
-    <row r="73" spans="1:69" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B73" s="41"/>
+        <v>82</v>
+      </c>
+      <c r="B73" s="39"/>
       <c r="C73" s="47"/>
       <c r="D73" s="47"/>
       <c r="E73" s="47"/>
@@ -3320,327 +3187,487 @@
       <c r="H73" s="47"/>
       <c r="I73" s="47"/>
       <c r="J73" s="47"/>
-      <c r="K73" s="15"/>
-      <c r="L73" s="15"/>
-      <c r="M73" s="15"/>
-      <c r="N73" s="15"/>
-      <c r="O73" s="15"/>
-      <c r="P73" s="15"/>
-      <c r="Q73" s="15"/>
-      <c r="R73" s="15"/>
-      <c r="S73" s="15"/>
-      <c r="T73" s="15"/>
-      <c r="U73" s="15"/>
-      <c r="V73" s="15"/>
-      <c r="W73" s="15"/>
-      <c r="X73" s="15"/>
-      <c r="Y73" s="15"/>
-      <c r="Z73" s="15"/>
-      <c r="AA73" s="15"/>
-      <c r="AB73" s="15"/>
-      <c r="AC73" s="15"/>
-      <c r="AD73" s="15"/>
-      <c r="AE73" s="15"/>
-      <c r="AF73" s="15"/>
-      <c r="AG73" s="15"/>
-      <c r="AH73" s="15"/>
-      <c r="AI73" s="15"/>
-      <c r="AJ73" s="15"/>
-      <c r="AK73" s="15"/>
-      <c r="AL73" s="15"/>
-      <c r="AM73" s="15"/>
-      <c r="AN73" s="15"/>
-      <c r="AO73" s="15"/>
-      <c r="AP73" s="15"/>
-      <c r="AQ73" s="15"/>
-      <c r="AR73" s="15"/>
-      <c r="AS73" s="15"/>
-      <c r="AT73" s="15"/>
-      <c r="AU73" s="15"/>
-      <c r="AV73" s="15"/>
-      <c r="AW73" s="15"/>
-      <c r="AX73" s="15"/>
-      <c r="AY73" s="15"/>
-      <c r="AZ73" s="15"/>
-      <c r="BA73" s="15"/>
-      <c r="BB73" s="15"/>
-      <c r="BC73" s="15"/>
-      <c r="BD73" s="15"/>
-      <c r="BE73" s="15"/>
-      <c r="BF73" s="15"/>
-      <c r="BG73" s="15"/>
-      <c r="BH73" s="15"/>
-      <c r="BI73" s="15"/>
-      <c r="BJ73" s="15"/>
-      <c r="BK73" s="15"/>
-      <c r="BL73" s="15"/>
-      <c r="BM73" s="15"/>
-      <c r="BN73" s="15"/>
-      <c r="BO73" s="15"/>
-      <c r="BP73" s="15"/>
-      <c r="BQ73" s="15"/>
     </row>
     <row r="74" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A74" s="13" t="s">
+      <c r="A74" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" s="40"/>
+      <c r="C74" s="47"/>
+      <c r="D74" s="47"/>
+      <c r="E74" s="47"/>
+      <c r="F74" s="47"/>
+      <c r="G74" s="47"/>
+      <c r="H74" s="47"/>
+      <c r="I74" s="47"/>
+      <c r="J74" s="47"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="15"/>
+      <c r="M74" s="15"/>
+      <c r="N74" s="15"/>
+      <c r="O74" s="15"/>
+      <c r="P74" s="15"/>
+      <c r="Q74" s="15"/>
+      <c r="R74" s="15"/>
+      <c r="S74" s="15"/>
+      <c r="T74" s="15"/>
+      <c r="U74" s="15"/>
+      <c r="V74" s="15"/>
+      <c r="W74" s="15"/>
+      <c r="X74" s="15"/>
+      <c r="Y74" s="15"/>
+      <c r="Z74" s="15"/>
+      <c r="AA74" s="15"/>
+      <c r="AB74" s="15"/>
+      <c r="AC74" s="15"/>
+      <c r="AD74" s="15"/>
+      <c r="AE74" s="15"/>
+      <c r="AF74" s="15"/>
+      <c r="AG74" s="15"/>
+      <c r="AH74" s="15"/>
+      <c r="AI74" s="15"/>
+      <c r="AJ74" s="15"/>
+      <c r="AK74" s="15"/>
+      <c r="AL74" s="15"/>
+      <c r="AM74" s="15"/>
+      <c r="AN74" s="15"/>
+      <c r="AO74" s="15"/>
+      <c r="AP74" s="15"/>
+      <c r="AQ74" s="15"/>
+      <c r="AR74" s="15"/>
+      <c r="AS74" s="15"/>
+      <c r="AT74" s="15"/>
+      <c r="AU74" s="15"/>
+      <c r="AV74" s="15"/>
+      <c r="AW74" s="15"/>
+      <c r="AX74" s="15"/>
+      <c r="AY74" s="15"/>
+      <c r="AZ74" s="15"/>
+      <c r="BA74" s="15"/>
+      <c r="BB74" s="15"/>
+      <c r="BC74" s="15"/>
+      <c r="BD74" s="15"/>
+      <c r="BE74" s="15"/>
+      <c r="BF74" s="15"/>
+      <c r="BG74" s="15"/>
+      <c r="BH74" s="15"/>
+      <c r="BI74" s="15"/>
+      <c r="BJ74" s="15"/>
+      <c r="BK74" s="15"/>
+      <c r="BL74" s="15"/>
+      <c r="BM74" s="15"/>
+      <c r="BN74" s="15"/>
+      <c r="BO74" s="15"/>
+      <c r="BP74" s="15"/>
+      <c r="BQ74" s="15"/>
+    </row>
+    <row r="75" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A75" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" s="40"/>
+      <c r="C75" s="47"/>
+      <c r="D75" s="47"/>
+      <c r="E75" s="47"/>
+      <c r="F75" s="47"/>
+      <c r="G75" s="47"/>
+      <c r="H75" s="47"/>
+      <c r="I75" s="47"/>
+      <c r="J75" s="47"/>
+      <c r="K75" s="15"/>
+      <c r="L75" s="15"/>
+      <c r="M75" s="15"/>
+      <c r="N75" s="15"/>
+      <c r="O75" s="15"/>
+      <c r="P75" s="15"/>
+      <c r="Q75" s="15"/>
+      <c r="R75" s="15"/>
+      <c r="S75" s="15"/>
+      <c r="T75" s="15"/>
+      <c r="U75" s="15"/>
+      <c r="V75" s="15"/>
+      <c r="W75" s="15"/>
+      <c r="X75" s="15"/>
+      <c r="Y75" s="15"/>
+      <c r="Z75" s="15"/>
+      <c r="AA75" s="15"/>
+      <c r="AB75" s="15"/>
+      <c r="AC75" s="15"/>
+      <c r="AD75" s="15"/>
+      <c r="AE75" s="15"/>
+      <c r="AF75" s="15"/>
+      <c r="AG75" s="15"/>
+      <c r="AH75" s="15"/>
+      <c r="AI75" s="15"/>
+      <c r="AJ75" s="15"/>
+      <c r="AK75" s="15"/>
+      <c r="AL75" s="15"/>
+      <c r="AM75" s="15"/>
+      <c r="AN75" s="15"/>
+      <c r="AO75" s="15"/>
+      <c r="AP75" s="15"/>
+      <c r="AQ75" s="15"/>
+      <c r="AR75" s="15"/>
+      <c r="AS75" s="15"/>
+      <c r="AT75" s="15"/>
+      <c r="AU75" s="15"/>
+      <c r="AV75" s="15"/>
+      <c r="AW75" s="15"/>
+      <c r="AX75" s="15"/>
+      <c r="AY75" s="15"/>
+      <c r="AZ75" s="15"/>
+      <c r="BA75" s="15"/>
+      <c r="BB75" s="15"/>
+      <c r="BC75" s="15"/>
+      <c r="BD75" s="15"/>
+      <c r="BE75" s="15"/>
+      <c r="BF75" s="15"/>
+      <c r="BG75" s="15"/>
+      <c r="BH75" s="15"/>
+      <c r="BI75" s="15"/>
+      <c r="BJ75" s="15"/>
+      <c r="BK75" s="15"/>
+      <c r="BL75" s="15"/>
+      <c r="BM75" s="15"/>
+      <c r="BN75" s="15"/>
+      <c r="BO75" s="15"/>
+      <c r="BP75" s="15"/>
+      <c r="BQ75" s="15"/>
+    </row>
+    <row r="76" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A76" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" s="41"/>
+      <c r="C76" s="47"/>
+      <c r="D76" s="47"/>
+      <c r="E76" s="47"/>
+      <c r="F76" s="47"/>
+      <c r="G76" s="47"/>
+      <c r="H76" s="47"/>
+      <c r="I76" s="47"/>
+      <c r="J76" s="47"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="15"/>
+      <c r="M76" s="15"/>
+      <c r="N76" s="15"/>
+      <c r="O76" s="15"/>
+      <c r="P76" s="15"/>
+      <c r="Q76" s="15"/>
+      <c r="R76" s="15"/>
+      <c r="S76" s="15"/>
+      <c r="T76" s="15"/>
+      <c r="U76" s="15"/>
+      <c r="V76" s="15"/>
+      <c r="W76" s="15"/>
+      <c r="X76" s="15"/>
+      <c r="Y76" s="15"/>
+      <c r="Z76" s="15"/>
+      <c r="AA76" s="15"/>
+      <c r="AB76" s="15"/>
+      <c r="AC76" s="15"/>
+      <c r="AD76" s="15"/>
+      <c r="AE76" s="15"/>
+      <c r="AF76" s="15"/>
+      <c r="AG76" s="15"/>
+      <c r="AH76" s="15"/>
+      <c r="AI76" s="15"/>
+      <c r="AJ76" s="15"/>
+      <c r="AK76" s="15"/>
+      <c r="AL76" s="15"/>
+      <c r="AM76" s="15"/>
+      <c r="AN76" s="15"/>
+      <c r="AO76" s="15"/>
+      <c r="AP76" s="15"/>
+      <c r="AQ76" s="15"/>
+      <c r="AR76" s="15"/>
+      <c r="AS76" s="15"/>
+      <c r="AT76" s="15"/>
+      <c r="AU76" s="15"/>
+      <c r="AV76" s="15"/>
+      <c r="AW76" s="15"/>
+      <c r="AX76" s="15"/>
+      <c r="AY76" s="15"/>
+      <c r="AZ76" s="15"/>
+      <c r="BA76" s="15"/>
+      <c r="BB76" s="15"/>
+      <c r="BC76" s="15"/>
+      <c r="BD76" s="15"/>
+      <c r="BE76" s="15"/>
+      <c r="BF76" s="15"/>
+      <c r="BG76" s="15"/>
+      <c r="BH76" s="15"/>
+      <c r="BI76" s="15"/>
+      <c r="BJ76" s="15"/>
+      <c r="BK76" s="15"/>
+      <c r="BL76" s="15"/>
+      <c r="BM76" s="15"/>
+      <c r="BN76" s="15"/>
+      <c r="BO76" s="15"/>
+      <c r="BP76" s="15"/>
+      <c r="BQ76" s="15"/>
+    </row>
+    <row r="77" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A77" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B74" s="42"/>
-    </row>
-    <row r="75" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A75" s="13" t="s">
+      <c r="B77" s="42"/>
+    </row>
+    <row r="78" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A78" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B75" s="43"/>
-    </row>
-    <row r="76" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A76" s="13" t="s">
+      <c r="B78" s="43"/>
+    </row>
+    <row r="79" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A79" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B76" s="42"/>
-    </row>
-    <row r="77" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A77" s="17" t="s">
+      <c r="B79" s="42"/>
+    </row>
+    <row r="80" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A80" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B77" s="44"/>
-      <c r="C77" s="53"/>
-      <c r="D77" s="53"/>
-      <c r="E77" s="53"/>
-      <c r="F77" s="53"/>
-      <c r="G77" s="53"/>
-      <c r="H77" s="53"/>
-      <c r="I77" s="54"/>
-    </row>
-    <row r="78" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
+      <c r="B80" s="44"/>
+      <c r="C80" s="53"/>
+      <c r="D80" s="53"/>
+      <c r="E80" s="53"/>
+      <c r="F80" s="53"/>
+      <c r="G80" s="53"/>
+      <c r="H80" s="53"/>
+      <c r="I80" s="54"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B78" s="45">
+      <c r="B81" s="45">
         <v>5</v>
       </c>
-      <c r="C78" s="45">
+      <c r="C81" s="45">
         <v>15</v>
       </c>
-      <c r="D78" s="45"/>
-      <c r="E78" s="55"/>
-    </row>
-    <row r="79" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A79" s="18" t="s">
+      <c r="D81" s="45"/>
+      <c r="E81" s="55"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B79" s="46"/>
-    </row>
-    <row r="80" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A80" s="13" t="s">
+      <c r="B82" s="46"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="B80" s="42"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="13" t="s">
+      <c r="B83" s="42"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A84" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="B81" s="42"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="13" t="s">
+      <c r="B84" s="42"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A85" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B82" s="42"/>
-    </row>
-    <row r="83" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="13" t="s">
+      <c r="B85" s="42"/>
+    </row>
+    <row r="86" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="B83" s="42"/>
-      <c r="C83" s="51"/>
-      <c r="D83" s="47"/>
-      <c r="E83" s="47"/>
-      <c r="F83" s="47"/>
-      <c r="G83" s="47"/>
-      <c r="H83" s="47"/>
-      <c r="I83" s="47"/>
-      <c r="J83" s="47"/>
-    </row>
-    <row r="84" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="13" t="s">
+      <c r="B86" s="42"/>
+      <c r="C86" s="51"/>
+      <c r="D86" s="47"/>
+      <c r="E86" s="47"/>
+      <c r="F86" s="47"/>
+      <c r="G86" s="47"/>
+      <c r="H86" s="47"/>
+      <c r="I86" s="47"/>
+      <c r="J86" s="47"/>
+    </row>
+    <row r="87" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="B84" s="42"/>
-      <c r="C84" s="51"/>
-      <c r="D84" s="47"/>
-      <c r="E84" s="47"/>
-      <c r="F84" s="47"/>
-      <c r="G84" s="47"/>
-      <c r="H84" s="47"/>
-      <c r="I84" s="47"/>
-      <c r="J84" s="47"/>
-    </row>
-    <row r="85" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="13" t="s">
+      <c r="B87" s="42"/>
+      <c r="C87" s="51"/>
+      <c r="D87" s="47"/>
+      <c r="E87" s="47"/>
+      <c r="F87" s="47"/>
+      <c r="G87" s="47"/>
+      <c r="H87" s="47"/>
+      <c r="I87" s="47"/>
+      <c r="J87" s="47"/>
+    </row>
+    <row r="88" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B85" s="42"/>
-      <c r="C85" s="51"/>
-      <c r="D85" s="47"/>
-      <c r="E85" s="47"/>
-      <c r="F85" s="47"/>
-      <c r="G85" s="47"/>
-      <c r="H85" s="47"/>
-      <c r="I85" s="47"/>
-      <c r="J85" s="47"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" s="13" t="s">
+      <c r="B88" s="42"/>
+      <c r="C88" s="51"/>
+      <c r="D88" s="47"/>
+      <c r="E88" s="47"/>
+      <c r="F88" s="47"/>
+      <c r="G88" s="47"/>
+      <c r="H88" s="47"/>
+      <c r="I88" s="47"/>
+      <c r="J88" s="47"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A89" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B86" s="42"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A87" s="13" t="s">
+      <c r="B89" s="42"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A90" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B87" s="42"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="19" t="s">
+      <c r="B90" s="42"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B88" s="42"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A89" s="56" t="s">
+      <c r="B91" s="42"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="B89" s="62"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A90" s="57" t="s">
-        <v>92</v>
-      </c>
-      <c r="B90" s="60"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="57" t="s">
-        <v>98</v>
-      </c>
-      <c r="B91" s="60"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="57" t="s">
-        <v>99</v>
-      </c>
-      <c r="B92" s="60"/>
+      <c r="B92" s="62"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B93" s="60"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="57" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B94" s="60"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B95" s="60"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A96" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="B96" s="60"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="B97" s="60"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="57" t="s">
         <v>101</v>
-      </c>
-      <c r="B95" s="60"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="58" t="s">
-        <v>94</v>
-      </c>
-      <c r="B96" s="60"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="58" t="s">
-        <v>102</v>
-      </c>
-      <c r="B97" s="60"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="58" t="s">
-        <v>103</v>
       </c>
       <c r="B98" s="60"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B99" s="60"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="58" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B100" s="60"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="58" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B101" s="60"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B102" s="60"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="58" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B103" s="60"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B104" s="60"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B105" s="60"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106" s="60"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="58" t="s">
+        <v>107</v>
+      </c>
+      <c r="B107" s="60"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B108" s="60"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="B106" s="60"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="59" t="s">
+      <c r="B109" s="60"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="B107" s="61"/>
+      <c r="B110" s="61"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74 B59:B60">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B77 B62:B63">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B57:B58">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60:B61">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B78">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44:B56">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44:B59">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B77">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B80">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3648,7 +3675,7 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B66:B70">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B69:B73">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -3662,13 +3689,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B79:B88 B61:B65 B71:B73</xm:sqref>
+          <xm:sqref>B82:B91 B64:B68 B74:B76</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B76</xm:sqref>
+          <xm:sqref>B79</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
First write documents method complete
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
   <si>
     <t>recent_time</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t>report_step_time</t>
+  </si>
+  <si>
+    <t>output_documents</t>
   </si>
 </sst>
 </file>
@@ -2350,10 +2353,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BQ110"/>
+  <dimension ref="A1:BQ111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3459,39 +3462,31 @@
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B83" s="42"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B84" s="42"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="B85" s="42"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A86" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B85" s="42"/>
-    </row>
-    <row r="86" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="13" t="s">
-        <v>71</v>
-      </c>
       <c r="B86" s="42"/>
-      <c r="C86" s="51"/>
-      <c r="D86" s="47"/>
-      <c r="E86" s="47"/>
-      <c r="F86" s="47"/>
-      <c r="G86" s="47"/>
-      <c r="H86" s="47"/>
-      <c r="I86" s="47"/>
-      <c r="J86" s="47"/>
     </row>
     <row r="87" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B87" s="42"/>
       <c r="C87" s="51"/>
@@ -3505,7 +3500,7 @@
     </row>
     <row r="88" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B88" s="42"/>
       <c r="C88" s="51"/>
@@ -3517,137 +3512,151 @@
       <c r="I88" s="47"/>
       <c r="J88" s="47"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="B89" s="42"/>
+      <c r="C89" s="51"/>
+      <c r="D89" s="47"/>
+      <c r="E89" s="47"/>
+      <c r="F89" s="47"/>
+      <c r="G89" s="47"/>
+      <c r="H89" s="47"/>
+      <c r="I89" s="47"/>
+      <c r="J89" s="47"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B90" s="42"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A91" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B90" s="42"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A91" s="19" t="s">
+      <c r="B91" s="42"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B91" s="42"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="56" t="s">
+      <c r="B92" s="42"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="56" t="s">
         <v>91</v>
       </c>
-      <c r="B92" s="62"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="57" t="s">
-        <v>92</v>
-      </c>
-      <c r="B93" s="60"/>
+      <c r="B93" s="62"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="57" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B94" s="60"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="57" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B95" s="60"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="57" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B96" s="60"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="57" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B97" s="60"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98" s="60"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="57" t="s">
         <v>101</v>
-      </c>
-      <c r="B98" s="60"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="58" t="s">
-        <v>94</v>
       </c>
       <c r="B99" s="60"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="58" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B100" s="60"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B101" s="60"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="58" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B102" s="60"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="58" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="B103" s="60"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B104" s="60"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="58" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="B105" s="60"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="58" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B106" s="60"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="58" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B107" s="60"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="58" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B108" s="60"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B109" s="60"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="B109" s="60"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="59" t="s">
+      <c r="B110" s="60"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="B110" s="61"/>
+      <c r="B111" s="61"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
@@ -3689,7 +3698,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B82:B91 B64:B68 B74:B76</xm:sqref>
+          <xm:sqref>B82:B92 B64:B68 B74:B76</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Renaming for consistency and checks
Making sure all inputted timepoints end in time, so that they can be
consistently checked in data processing.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -176,15 +176,6 @@
     <t>start_time</t>
   </si>
   <si>
-    <t>start_mdr_introduce_period</t>
-  </si>
-  <si>
-    <t>end_mdr_introduce_period</t>
-  </si>
-  <si>
-    <t>timepoint_introduce_xdr</t>
-  </si>
-  <si>
     <t>susceptible_fully</t>
   </si>
   <si>
@@ -363,6 +354,15 @@
   </si>
   <si>
     <t>output_documents</t>
+  </si>
+  <si>
+    <t>start_mdr_introduce_time</t>
+  </si>
+  <si>
+    <t>end_mdr_introduce_time</t>
+  </si>
+  <si>
+    <t>xdr_introduce_time</t>
   </si>
 </sst>
 </file>
@@ -2355,8 +2355,8 @@
   </sheetPr>
   <dimension ref="A1:BQ111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2373,7 +2373,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C1" s="48"/>
       <c r="D1" s="49"/>
@@ -2401,21 +2401,21 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B4" s="25"/>
       <c r="C4" s="51"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" s="25"/>
       <c r="C5" s="51"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="51"/>
@@ -2429,21 +2429,21 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="51"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B9" s="25"/>
       <c r="C9" s="51"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B10" s="25"/>
       <c r="C10" s="51"/>
@@ -2590,14 +2590,14 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B31" s="25"/>
       <c r="C31" s="51"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B32" s="25"/>
       <c r="C32" s="51"/>
@@ -2639,21 +2639,21 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B38" s="27"/>
       <c r="C38" s="51"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B39" s="27"/>
       <c r="C39" s="51"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B40" s="27"/>
       <c r="C40" s="51"/>
@@ -2667,7 +2667,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B42" s="28"/>
       <c r="C42" s="51"/>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B45" s="30"/>
     </row>
@@ -2705,19 +2705,19 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>53</v>
+        <v>113</v>
       </c>
       <c r="B48" s="31"/>
     </row>
     <row r="49" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>54</v>
+        <v>114</v>
       </c>
       <c r="B49" s="31"/>
     </row>
     <row r="50" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="B50" s="31"/>
     </row>
@@ -2753,37 +2753,37 @@
     </row>
     <row r="56" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B56" s="30"/>
     </row>
     <row r="57" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B57" s="30"/>
     </row>
     <row r="58" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B58" s="30"/>
     </row>
     <row r="59" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B59" s="32"/>
     </row>
     <row r="60" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B60" s="33"/>
     </row>
     <row r="61" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B61" s="34"/>
     </row>
@@ -2935,7 +2935,7 @@
     </row>
     <row r="64" spans="1:69" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="22" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B64" s="36"/>
       <c r="C64" s="47"/>
@@ -3008,7 +3008,7 @@
     </row>
     <row r="65" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B65" s="35"/>
       <c r="C65" s="47"/>
@@ -3022,7 +3022,7 @@
     </row>
     <row r="66" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B66" s="35"/>
       <c r="C66" s="47"/>
@@ -3036,7 +3036,7 @@
     </row>
     <row r="67" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B67" s="35"/>
       <c r="C67" s="47"/>
@@ -3050,7 +3050,7 @@
     </row>
     <row r="68" spans="1:69" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B68" s="37"/>
       <c r="C68" s="47"/>
@@ -3123,7 +3123,7 @@
     </row>
     <row r="69" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B69" s="38"/>
       <c r="C69" s="47"/>
@@ -3137,7 +3137,7 @@
     </row>
     <row r="70" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B70" s="38"/>
       <c r="C70" s="47"/>
@@ -3151,7 +3151,7 @@
     </row>
     <row r="71" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B71" s="38"/>
       <c r="C71" s="47"/>
@@ -3165,7 +3165,7 @@
     </row>
     <row r="72" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B72" s="38"/>
       <c r="C72" s="47"/>
@@ -3179,7 +3179,7 @@
     </row>
     <row r="73" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B73" s="39"/>
       <c r="C73" s="47"/>
@@ -3432,7 +3432,9 @@
       <c r="A80" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B80" s="44"/>
+      <c r="B80" s="44">
+        <v>1</v>
+      </c>
       <c r="C80" s="53"/>
       <c r="D80" s="53"/>
       <c r="E80" s="53"/>
@@ -3445,48 +3447,44 @@
       <c r="A81" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B81" s="45">
-        <v>5</v>
-      </c>
-      <c r="C81" s="45">
-        <v>15</v>
-      </c>
+      <c r="B81" s="45"/>
+      <c r="C81" s="45"/>
       <c r="D81" s="45"/>
       <c r="E81" s="55"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B82" s="46"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="13" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B83" s="42"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B84" s="42"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B85" s="42"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B86" s="42"/>
     </row>
     <row r="87" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B87" s="42"/>
       <c r="C87" s="51"/>
@@ -3500,7 +3498,7 @@
     </row>
     <row r="88" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B88" s="42"/>
       <c r="C88" s="51"/>
@@ -3514,7 +3512,7 @@
     </row>
     <row r="89" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B89" s="42"/>
       <c r="C89" s="51"/>
@@ -3528,133 +3526,135 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B90" s="42"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B91" s="42"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="B92" s="42"/>
+        <v>59</v>
+      </c>
+      <c r="B92" s="42" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="56" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B93" s="62"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="57" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B94" s="60"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="57" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B95" s="60"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="57" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B96" s="60"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="57" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B97" s="60"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="57" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B98" s="60"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="57" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B99" s="60"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="58" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B100" s="60"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="58" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B101" s="60"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="58" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B102" s="60"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="58" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B103" s="60"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="58" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B104" s="60"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="58" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B105" s="60"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="58" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B106" s="60"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="58" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B107" s="60"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="58" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B108" s="60"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="58" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B109" s="60"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="58" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B110" s="60"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="59" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B111" s="61"/>
     </row>

</xml_diff>

<commit_message>
Return control panel to baseline
Must have synced with changes in control_panel.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2355,8 +2355,8 @@
   </sheetPr>
   <dimension ref="A1:BQ111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3432,9 +3432,7 @@
       <c r="A80" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B80" s="44">
-        <v>1</v>
-      </c>
+      <c r="B80" s="44"/>
       <c r="C80" s="53"/>
       <c r="D80" s="53"/>
       <c r="E80" s="53"/>
@@ -3447,8 +3445,12 @@
       <c r="A81" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B81" s="45"/>
-      <c r="C81" s="45"/>
+      <c r="B81" s="45">
+        <v>5</v>
+      </c>
+      <c r="C81" s="45">
+        <v>15</v>
+      </c>
       <c r="D81" s="45"/>
       <c r="E81" s="55"/>
     </row>
@@ -3540,9 +3542,7 @@
       <c r="A92" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B92" s="42" t="b">
-        <v>1</v>
-      </c>
+      <c r="B92" s="42"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="56" t="s">

</xml_diff>

<commit_message>
Debug and allow modifcation of diabetes start age
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="117">
   <si>
     <t>recent_time</t>
   </si>
@@ -363,6 +363,9 @@
   </si>
   <si>
     <t>xdr_introduce_time</t>
+  </si>
+  <si>
+    <t>comorb_startage_diabetes</t>
   </si>
 </sst>
 </file>
@@ -2353,10 +2356,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BQ111"/>
+  <dimension ref="A1:BQ112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2666,203 +2669,137 @@
       <c r="C41" s="51"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B42" s="26"/>
+      <c r="C42" s="51"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B42" s="28"/>
-      <c r="C42" s="51"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
+      <c r="B43" s="28"/>
+      <c r="C43" s="51"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B43" s="29"/>
-      <c r="C43" s="47"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="30"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="47"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B45" s="30"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="B46" s="30"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" s="30"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="30"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B48" s="31"/>
+      <c r="B48" s="30"/>
     </row>
     <row r="49" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B49" s="31"/>
     </row>
     <row r="50" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B50" s="31"/>
+    </row>
+    <row r="51" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="31"/>
-    </row>
-    <row r="51" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51" s="30"/>
+      <c r="B51" s="31"/>
     </row>
     <row r="52" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B52" s="30"/>
     </row>
     <row r="53" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B53" s="30"/>
     </row>
     <row r="54" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B54" s="30"/>
     </row>
     <row r="55" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B55" s="30"/>
     </row>
     <row r="56" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>109</v>
+        <v>10</v>
       </c>
       <c r="B56" s="30"/>
     </row>
     <row r="57" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B57" s="30"/>
     </row>
     <row r="58" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B58" s="30"/>
     </row>
     <row r="59" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B59" s="30"/>
+    </row>
+    <row r="60" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B59" s="32"/>
-    </row>
-    <row r="60" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+      <c r="B60" s="32"/>
+    </row>
+    <row r="61" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B60" s="33"/>
-    </row>
-    <row r="61" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A61" s="10" t="s">
+      <c r="B61" s="33"/>
+    </row>
+    <row r="62" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A62" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B61" s="34"/>
-    </row>
-    <row r="62" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B62" s="35"/>
-      <c r="C62" s="47"/>
-      <c r="D62" s="47"/>
-      <c r="E62" s="47"/>
-      <c r="F62" s="47"/>
-      <c r="G62" s="47"/>
-      <c r="H62" s="47"/>
-      <c r="I62" s="47"/>
-      <c r="J62" s="47"/>
-      <c r="K62" s="15"/>
-      <c r="L62" s="15"/>
-      <c r="M62" s="15"/>
-      <c r="N62" s="15"/>
-      <c r="O62" s="15"/>
-      <c r="P62" s="15"/>
-      <c r="Q62" s="15"/>
-      <c r="R62" s="15"/>
-      <c r="S62" s="15"/>
-      <c r="T62" s="15"/>
-      <c r="U62" s="15"/>
-      <c r="V62" s="15"/>
-      <c r="W62" s="15"/>
-      <c r="X62" s="15"/>
-      <c r="Y62" s="15"/>
-      <c r="Z62" s="15"/>
-      <c r="AA62" s="15"/>
-      <c r="AB62" s="15"/>
-      <c r="AC62" s="15"/>
-      <c r="AD62" s="15"/>
-      <c r="AE62" s="15"/>
-      <c r="AF62" s="15"/>
-      <c r="AG62" s="15"/>
-      <c r="AH62" s="15"/>
-      <c r="AI62" s="15"/>
-      <c r="AJ62" s="15"/>
-      <c r="AK62" s="15"/>
-      <c r="AL62" s="15"/>
-      <c r="AM62" s="15"/>
-      <c r="AN62" s="15"/>
-      <c r="AO62" s="15"/>
-      <c r="AP62" s="15"/>
-      <c r="AQ62" s="15"/>
-      <c r="AR62" s="15"/>
-      <c r="AS62" s="15"/>
-      <c r="AT62" s="15"/>
-      <c r="AU62" s="15"/>
-      <c r="AV62" s="15"/>
-      <c r="AW62" s="15"/>
-      <c r="AX62" s="15"/>
-      <c r="AY62" s="15"/>
-      <c r="AZ62" s="15"/>
-      <c r="BA62" s="15"/>
-      <c r="BB62" s="15"/>
-      <c r="BC62" s="15"/>
-      <c r="BD62" s="15"/>
-      <c r="BE62" s="15"/>
-      <c r="BF62" s="15"/>
-      <c r="BG62" s="15"/>
-      <c r="BH62" s="15"/>
-      <c r="BI62" s="15"/>
-      <c r="BJ62" s="15"/>
-      <c r="BK62" s="15"/>
-      <c r="BL62" s="15"/>
-      <c r="BM62" s="15"/>
-      <c r="BN62" s="15"/>
-      <c r="BO62" s="15"/>
-      <c r="BP62" s="15"/>
-      <c r="BQ62" s="15"/>
+      <c r="B62" s="34"/>
     </row>
     <row r="63" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B63" s="35"/>
       <c r="C63" s="47"/>
@@ -2933,11 +2870,11 @@
       <c r="BP63" s="15"/>
       <c r="BQ63" s="15"/>
     </row>
-    <row r="64" spans="1:69" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B64" s="36"/>
+    <row r="64" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B64" s="35"/>
       <c r="C64" s="47"/>
       <c r="D64" s="47"/>
       <c r="E64" s="47"/>
@@ -3006,11 +2943,11 @@
       <c r="BP64" s="15"/>
       <c r="BQ64" s="15"/>
     </row>
-    <row r="65" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B65" s="35"/>
+    <row r="65" spans="1:69" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65" s="36"/>
       <c r="C65" s="47"/>
       <c r="D65" s="47"/>
       <c r="E65" s="47"/>
@@ -3019,10 +2956,69 @@
       <c r="H65" s="47"/>
       <c r="I65" s="47"/>
       <c r="J65" s="47"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
+      <c r="M65" s="15"/>
+      <c r="N65" s="15"/>
+      <c r="O65" s="15"/>
+      <c r="P65" s="15"/>
+      <c r="Q65" s="15"/>
+      <c r="R65" s="15"/>
+      <c r="S65" s="15"/>
+      <c r="T65" s="15"/>
+      <c r="U65" s="15"/>
+      <c r="V65" s="15"/>
+      <c r="W65" s="15"/>
+      <c r="X65" s="15"/>
+      <c r="Y65" s="15"/>
+      <c r="Z65" s="15"/>
+      <c r="AA65" s="15"/>
+      <c r="AB65" s="15"/>
+      <c r="AC65" s="15"/>
+      <c r="AD65" s="15"/>
+      <c r="AE65" s="15"/>
+      <c r="AF65" s="15"/>
+      <c r="AG65" s="15"/>
+      <c r="AH65" s="15"/>
+      <c r="AI65" s="15"/>
+      <c r="AJ65" s="15"/>
+      <c r="AK65" s="15"/>
+      <c r="AL65" s="15"/>
+      <c r="AM65" s="15"/>
+      <c r="AN65" s="15"/>
+      <c r="AO65" s="15"/>
+      <c r="AP65" s="15"/>
+      <c r="AQ65" s="15"/>
+      <c r="AR65" s="15"/>
+      <c r="AS65" s="15"/>
+      <c r="AT65" s="15"/>
+      <c r="AU65" s="15"/>
+      <c r="AV65" s="15"/>
+      <c r="AW65" s="15"/>
+      <c r="AX65" s="15"/>
+      <c r="AY65" s="15"/>
+      <c r="AZ65" s="15"/>
+      <c r="BA65" s="15"/>
+      <c r="BB65" s="15"/>
+      <c r="BC65" s="15"/>
+      <c r="BD65" s="15"/>
+      <c r="BE65" s="15"/>
+      <c r="BF65" s="15"/>
+      <c r="BG65" s="15"/>
+      <c r="BH65" s="15"/>
+      <c r="BI65" s="15"/>
+      <c r="BJ65" s="15"/>
+      <c r="BK65" s="15"/>
+      <c r="BL65" s="15"/>
+      <c r="BM65" s="15"/>
+      <c r="BN65" s="15"/>
+      <c r="BO65" s="15"/>
+      <c r="BP65" s="15"/>
+      <c r="BQ65" s="15"/>
     </row>
     <row r="66" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B66" s="35"/>
       <c r="C66" s="47"/>
@@ -3036,7 +3032,7 @@
     </row>
     <row r="67" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B67" s="35"/>
       <c r="C67" s="47"/>
@@ -3048,11 +3044,11 @@
       <c r="I67" s="47"/>
       <c r="J67" s="47"/>
     </row>
-    <row r="68" spans="1:69" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B68" s="37"/>
+    <row r="68" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" s="35"/>
       <c r="C68" s="47"/>
       <c r="D68" s="47"/>
       <c r="E68" s="47"/>
@@ -3061,71 +3057,12 @@
       <c r="H68" s="47"/>
       <c r="I68" s="47"/>
       <c r="J68" s="47"/>
-      <c r="K68" s="15"/>
-      <c r="L68" s="15"/>
-      <c r="M68" s="15"/>
-      <c r="N68" s="15"/>
-      <c r="O68" s="15"/>
-      <c r="P68" s="15"/>
-      <c r="Q68" s="15"/>
-      <c r="R68" s="15"/>
-      <c r="S68" s="15"/>
-      <c r="T68" s="15"/>
-      <c r="U68" s="15"/>
-      <c r="V68" s="15"/>
-      <c r="W68" s="15"/>
-      <c r="X68" s="15"/>
-      <c r="Y68" s="15"/>
-      <c r="Z68" s="15"/>
-      <c r="AA68" s="15"/>
-      <c r="AB68" s="15"/>
-      <c r="AC68" s="15"/>
-      <c r="AD68" s="15"/>
-      <c r="AE68" s="15"/>
-      <c r="AF68" s="15"/>
-      <c r="AG68" s="15"/>
-      <c r="AH68" s="15"/>
-      <c r="AI68" s="15"/>
-      <c r="AJ68" s="15"/>
-      <c r="AK68" s="15"/>
-      <c r="AL68" s="15"/>
-      <c r="AM68" s="15"/>
-      <c r="AN68" s="15"/>
-      <c r="AO68" s="15"/>
-      <c r="AP68" s="15"/>
-      <c r="AQ68" s="15"/>
-      <c r="AR68" s="15"/>
-      <c r="AS68" s="15"/>
-      <c r="AT68" s="15"/>
-      <c r="AU68" s="15"/>
-      <c r="AV68" s="15"/>
-      <c r="AW68" s="15"/>
-      <c r="AX68" s="15"/>
-      <c r="AY68" s="15"/>
-      <c r="AZ68" s="15"/>
-      <c r="BA68" s="15"/>
-      <c r="BB68" s="15"/>
-      <c r="BC68" s="15"/>
-      <c r="BD68" s="15"/>
-      <c r="BE68" s="15"/>
-      <c r="BF68" s="15"/>
-      <c r="BG68" s="15"/>
-      <c r="BH68" s="15"/>
-      <c r="BI68" s="15"/>
-      <c r="BJ68" s="15"/>
-      <c r="BK68" s="15"/>
-      <c r="BL68" s="15"/>
-      <c r="BM68" s="15"/>
-      <c r="BN68" s="15"/>
-      <c r="BO68" s="15"/>
-      <c r="BP68" s="15"/>
-      <c r="BQ68" s="15"/>
-    </row>
-    <row r="69" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B69" s="38"/>
+    </row>
+    <row r="69" spans="1:69" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" s="37"/>
       <c r="C69" s="47"/>
       <c r="D69" s="47"/>
       <c r="E69" s="47"/>
@@ -3134,10 +3071,69 @@
       <c r="H69" s="47"/>
       <c r="I69" s="47"/>
       <c r="J69" s="47"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="15"/>
+      <c r="M69" s="15"/>
+      <c r="N69" s="15"/>
+      <c r="O69" s="15"/>
+      <c r="P69" s="15"/>
+      <c r="Q69" s="15"/>
+      <c r="R69" s="15"/>
+      <c r="S69" s="15"/>
+      <c r="T69" s="15"/>
+      <c r="U69" s="15"/>
+      <c r="V69" s="15"/>
+      <c r="W69" s="15"/>
+      <c r="X69" s="15"/>
+      <c r="Y69" s="15"/>
+      <c r="Z69" s="15"/>
+      <c r="AA69" s="15"/>
+      <c r="AB69" s="15"/>
+      <c r="AC69" s="15"/>
+      <c r="AD69" s="15"/>
+      <c r="AE69" s="15"/>
+      <c r="AF69" s="15"/>
+      <c r="AG69" s="15"/>
+      <c r="AH69" s="15"/>
+      <c r="AI69" s="15"/>
+      <c r="AJ69" s="15"/>
+      <c r="AK69" s="15"/>
+      <c r="AL69" s="15"/>
+      <c r="AM69" s="15"/>
+      <c r="AN69" s="15"/>
+      <c r="AO69" s="15"/>
+      <c r="AP69" s="15"/>
+      <c r="AQ69" s="15"/>
+      <c r="AR69" s="15"/>
+      <c r="AS69" s="15"/>
+      <c r="AT69" s="15"/>
+      <c r="AU69" s="15"/>
+      <c r="AV69" s="15"/>
+      <c r="AW69" s="15"/>
+      <c r="AX69" s="15"/>
+      <c r="AY69" s="15"/>
+      <c r="AZ69" s="15"/>
+      <c r="BA69" s="15"/>
+      <c r="BB69" s="15"/>
+      <c r="BC69" s="15"/>
+      <c r="BD69" s="15"/>
+      <c r="BE69" s="15"/>
+      <c r="BF69" s="15"/>
+      <c r="BG69" s="15"/>
+      <c r="BH69" s="15"/>
+      <c r="BI69" s="15"/>
+      <c r="BJ69" s="15"/>
+      <c r="BK69" s="15"/>
+      <c r="BL69" s="15"/>
+      <c r="BM69" s="15"/>
+      <c r="BN69" s="15"/>
+      <c r="BO69" s="15"/>
+      <c r="BP69" s="15"/>
+      <c r="BQ69" s="15"/>
     </row>
     <row r="70" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B70" s="38"/>
       <c r="C70" s="47"/>
@@ -3151,7 +3147,7 @@
     </row>
     <row r="71" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B71" s="38"/>
       <c r="C71" s="47"/>
@@ -3165,7 +3161,7 @@
     </row>
     <row r="72" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B72" s="38"/>
       <c r="C72" s="47"/>
@@ -3178,10 +3174,10 @@
       <c r="J72" s="47"/>
     </row>
     <row r="73" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B73" s="39"/>
+      <c r="A73" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B73" s="38"/>
       <c r="C73" s="47"/>
       <c r="D73" s="47"/>
       <c r="E73" s="47"/>
@@ -3191,11 +3187,11 @@
       <c r="I73" s="47"/>
       <c r="J73" s="47"/>
     </row>
-    <row r="74" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B74" s="40"/>
+    <row r="74" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" s="39"/>
       <c r="C74" s="47"/>
       <c r="D74" s="47"/>
       <c r="E74" s="47"/>
@@ -3204,69 +3200,10 @@
       <c r="H74" s="47"/>
       <c r="I74" s="47"/>
       <c r="J74" s="47"/>
-      <c r="K74" s="15"/>
-      <c r="L74" s="15"/>
-      <c r="M74" s="15"/>
-      <c r="N74" s="15"/>
-      <c r="O74" s="15"/>
-      <c r="P74" s="15"/>
-      <c r="Q74" s="15"/>
-      <c r="R74" s="15"/>
-      <c r="S74" s="15"/>
-      <c r="T74" s="15"/>
-      <c r="U74" s="15"/>
-      <c r="V74" s="15"/>
-      <c r="W74" s="15"/>
-      <c r="X74" s="15"/>
-      <c r="Y74" s="15"/>
-      <c r="Z74" s="15"/>
-      <c r="AA74" s="15"/>
-      <c r="AB74" s="15"/>
-      <c r="AC74" s="15"/>
-      <c r="AD74" s="15"/>
-      <c r="AE74" s="15"/>
-      <c r="AF74" s="15"/>
-      <c r="AG74" s="15"/>
-      <c r="AH74" s="15"/>
-      <c r="AI74" s="15"/>
-      <c r="AJ74" s="15"/>
-      <c r="AK74" s="15"/>
-      <c r="AL74" s="15"/>
-      <c r="AM74" s="15"/>
-      <c r="AN74" s="15"/>
-      <c r="AO74" s="15"/>
-      <c r="AP74" s="15"/>
-      <c r="AQ74" s="15"/>
-      <c r="AR74" s="15"/>
-      <c r="AS74" s="15"/>
-      <c r="AT74" s="15"/>
-      <c r="AU74" s="15"/>
-      <c r="AV74" s="15"/>
-      <c r="AW74" s="15"/>
-      <c r="AX74" s="15"/>
-      <c r="AY74" s="15"/>
-      <c r="AZ74" s="15"/>
-      <c r="BA74" s="15"/>
-      <c r="BB74" s="15"/>
-      <c r="BC74" s="15"/>
-      <c r="BD74" s="15"/>
-      <c r="BE74" s="15"/>
-      <c r="BF74" s="15"/>
-      <c r="BG74" s="15"/>
-      <c r="BH74" s="15"/>
-      <c r="BI74" s="15"/>
-      <c r="BJ74" s="15"/>
-      <c r="BK74" s="15"/>
-      <c r="BL74" s="15"/>
-      <c r="BM74" s="15"/>
-      <c r="BN74" s="15"/>
-      <c r="BO74" s="15"/>
-      <c r="BP74" s="15"/>
-      <c r="BQ74" s="15"/>
     </row>
     <row r="75" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B75" s="40"/>
       <c r="C75" s="47"/>
@@ -3338,10 +3275,10 @@
       <c r="BQ75" s="15"/>
     </row>
     <row r="76" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A76" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B76" s="41"/>
+      <c r="A76" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76" s="40"/>
       <c r="C76" s="47"/>
       <c r="D76" s="47"/>
       <c r="E76" s="47"/>
@@ -3411,96 +3348,155 @@
       <c r="BQ76" s="15"/>
     </row>
     <row r="77" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A77" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B77" s="42"/>
+      <c r="A77" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" s="41"/>
+      <c r="C77" s="47"/>
+      <c r="D77" s="47"/>
+      <c r="E77" s="47"/>
+      <c r="F77" s="47"/>
+      <c r="G77" s="47"/>
+      <c r="H77" s="47"/>
+      <c r="I77" s="47"/>
+      <c r="J77" s="47"/>
+      <c r="K77" s="15"/>
+      <c r="L77" s="15"/>
+      <c r="M77" s="15"/>
+      <c r="N77" s="15"/>
+      <c r="O77" s="15"/>
+      <c r="P77" s="15"/>
+      <c r="Q77" s="15"/>
+      <c r="R77" s="15"/>
+      <c r="S77" s="15"/>
+      <c r="T77" s="15"/>
+      <c r="U77" s="15"/>
+      <c r="V77" s="15"/>
+      <c r="W77" s="15"/>
+      <c r="X77" s="15"/>
+      <c r="Y77" s="15"/>
+      <c r="Z77" s="15"/>
+      <c r="AA77" s="15"/>
+      <c r="AB77" s="15"/>
+      <c r="AC77" s="15"/>
+      <c r="AD77" s="15"/>
+      <c r="AE77" s="15"/>
+      <c r="AF77" s="15"/>
+      <c r="AG77" s="15"/>
+      <c r="AH77" s="15"/>
+      <c r="AI77" s="15"/>
+      <c r="AJ77" s="15"/>
+      <c r="AK77" s="15"/>
+      <c r="AL77" s="15"/>
+      <c r="AM77" s="15"/>
+      <c r="AN77" s="15"/>
+      <c r="AO77" s="15"/>
+      <c r="AP77" s="15"/>
+      <c r="AQ77" s="15"/>
+      <c r="AR77" s="15"/>
+      <c r="AS77" s="15"/>
+      <c r="AT77" s="15"/>
+      <c r="AU77" s="15"/>
+      <c r="AV77" s="15"/>
+      <c r="AW77" s="15"/>
+      <c r="AX77" s="15"/>
+      <c r="AY77" s="15"/>
+      <c r="AZ77" s="15"/>
+      <c r="BA77" s="15"/>
+      <c r="BB77" s="15"/>
+      <c r="BC77" s="15"/>
+      <c r="BD77" s="15"/>
+      <c r="BE77" s="15"/>
+      <c r="BF77" s="15"/>
+      <c r="BG77" s="15"/>
+      <c r="BH77" s="15"/>
+      <c r="BI77" s="15"/>
+      <c r="BJ77" s="15"/>
+      <c r="BK77" s="15"/>
+      <c r="BL77" s="15"/>
+      <c r="BM77" s="15"/>
+      <c r="BN77" s="15"/>
+      <c r="BO77" s="15"/>
+      <c r="BP77" s="15"/>
+      <c r="BQ77" s="15"/>
     </row>
     <row r="78" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B78" s="43"/>
+        <v>9</v>
+      </c>
+      <c r="B78" s="42"/>
     </row>
     <row r="79" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B79" s="43"/>
+    </row>
+    <row r="80" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="A80" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B79" s="42"/>
-    </row>
-    <row r="80" spans="1:69" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
+      <c r="B80" s="42"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A81" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B80" s="44"/>
-      <c r="C80" s="53"/>
-      <c r="D80" s="53"/>
-      <c r="E80" s="53"/>
-      <c r="F80" s="53"/>
-      <c r="G80" s="53"/>
-      <c r="H80" s="53"/>
-      <c r="I80" s="54"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A81" s="16" t="s">
+      <c r="B81" s="44"/>
+      <c r="C81" s="53"/>
+      <c r="D81" s="53"/>
+      <c r="E81" s="53"/>
+      <c r="F81" s="53"/>
+      <c r="G81" s="53"/>
+      <c r="H81" s="53"/>
+      <c r="I81" s="54"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A82" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B81" s="45">
+      <c r="B82" s="45">
         <v>5</v>
       </c>
-      <c r="C81" s="45">
+      <c r="C82" s="45">
         <v>15</v>
       </c>
-      <c r="D81" s="45"/>
-      <c r="E81" s="55"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A82" s="18" t="s">
+      <c r="D82" s="45"/>
+      <c r="E82" s="55"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A83" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B82" s="46"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A83" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B83" s="42"/>
+      <c r="B83" s="46"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B84" s="42"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B85" s="42"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="B86" s="42"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A87" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B86" s="42"/>
-    </row>
-    <row r="87" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="13" t="s">
-        <v>68</v>
-      </c>
       <c r="B87" s="42"/>
-      <c r="C87" s="51"/>
-      <c r="D87" s="47"/>
-      <c r="E87" s="47"/>
-      <c r="F87" s="47"/>
-      <c r="G87" s="47"/>
-      <c r="H87" s="47"/>
-      <c r="I87" s="47"/>
-      <c r="J87" s="47"/>
     </row>
     <row r="88" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B88" s="42"/>
       <c r="C88" s="51"/>
@@ -3514,7 +3510,7 @@
     </row>
     <row r="89" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B89" s="42"/>
       <c r="C89" s="51"/>
@@ -3526,165 +3522,179 @@
       <c r="I89" s="47"/>
       <c r="J89" s="47"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="B90" s="42"/>
+      <c r="C90" s="51"/>
+      <c r="D90" s="47"/>
+      <c r="E90" s="47"/>
+      <c r="F90" s="47"/>
+      <c r="G90" s="47"/>
+      <c r="H90" s="47"/>
+      <c r="I90" s="47"/>
+      <c r="J90" s="47"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B91" s="42"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A92" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B91" s="42"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A92" s="19" t="s">
+      <c r="B92" s="42"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A93" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B92" s="42"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="56" t="s">
+      <c r="B93" s="42"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A94" s="56" t="s">
         <v>88</v>
       </c>
-      <c r="B93" s="62"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="57" t="s">
-        <v>89</v>
-      </c>
-      <c r="B94" s="60"/>
+      <c r="B94" s="62"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="57" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B95" s="60"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="57" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B96" s="60"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="57" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B97" s="60"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="57" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B98" s="60"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="57" t="s">
+        <v>97</v>
+      </c>
+      <c r="B99" s="60"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="57" t="s">
         <v>98</v>
-      </c>
-      <c r="B99" s="60"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="58" t="s">
-        <v>91</v>
       </c>
       <c r="B100" s="60"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="58" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B101" s="60"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B102" s="60"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="58" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B103" s="60"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="58" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B104" s="60"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="58" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B105" s="60"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="58" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B106" s="60"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="58" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B107" s="60"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B108" s="60"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="58" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B109" s="60"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="58" t="s">
+        <v>94</v>
+      </c>
+      <c r="B110" s="60"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="58" t="s">
         <v>105</v>
       </c>
-      <c r="B110" s="60"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="59" t="s">
+      <c r="B111" s="60"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="B111" s="61"/>
+      <c r="B112" s="61"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B77 B62:B63">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B78 B63:B64">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60:B61">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61:B62">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B78">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44:B59">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45:B60">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B80">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B81">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B43">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B69:B73">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B70:B74">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -3698,13 +3708,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B82:B92 B64:B68 B74:B76</xm:sqref>
+          <xm:sqref>B83:B93 B65:B69 B75:B77</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B79</xm:sqref>
+          <xm:sqref>B80</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Allow importation of uncertainty dictionaries
Wow, that shouldn't have been so hard.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2358,8 +2358,8 @@
   </sheetPr>
   <dimension ref="A1:BQ112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Move uncertainty Boolean to inputs
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="555" windowWidth="20370" windowHeight="7290" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="20370" windowHeight="7230" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="control_panel" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="119">
   <si>
     <t>recent_time</t>
   </si>
@@ -366,6 +366,12 @@
   </si>
   <si>
     <t>comorb_startage_diabetes</t>
+  </si>
+  <si>
+    <t>output_uncertainty</t>
+  </si>
+  <si>
+    <t>output_uncertainty_all_scenarios</t>
   </si>
 </sst>
 </file>
@@ -1317,7 +1323,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1341,7 +1347,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1389,6 +1394,12 @@
     <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2356,462 +2367,586 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BQ112"/>
+  <dimension ref="A1:BS114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" style="47" customWidth="1"/>
-    <col min="3" max="4" width="23.28515625" style="52" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" style="52" customWidth="1"/>
-    <col min="6" max="10" width="9.140625" style="52"/>
+    <col min="2" max="4" width="25.5703125" style="46" customWidth="1"/>
+    <col min="5" max="6" width="23.28515625" style="51" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" style="51" customWidth="1"/>
+    <col min="8" max="12" width="9.140625" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="47"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="46"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="51"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="50"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="51"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="50"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="51"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="50"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="51"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="50"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="51"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="50"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="51"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="50"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="51"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="50"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="51"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="50"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="51"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="50"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="51"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="50"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="51"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="50"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="51"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="50"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="26"/>
-      <c r="C15" s="51"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="25"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="50"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="51"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="50"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="51"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="50"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="51"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="50"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="51"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="50"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="51"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="50"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="51"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="50"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="51"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="50"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="51"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="50"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="51"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="50"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="51"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="50"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="25"/>
-      <c r="C26" s="51"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="50"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="25"/>
-      <c r="C27" s="51"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="50"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="51"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="50"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="25"/>
-      <c r="C29" s="51"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="50"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="51"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="50"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="51"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="50"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B32" s="25"/>
-      <c r="C32" s="51"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
+      <c r="D32" s="24"/>
+      <c r="E32" s="50"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="26"/>
-      <c r="C33" s="51"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="50"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="51"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="24"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="50"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="25"/>
-      <c r="C35" s="51"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="50"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="51"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="50"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="51"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="50"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="51"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="50"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="27"/>
-      <c r="C39" s="51"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="50"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B40" s="27"/>
-      <c r="C40" s="51"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="26"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="50"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="26"/>
-      <c r="C41" s="51"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="50"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B42" s="26"/>
-      <c r="C42" s="51"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="50"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B43" s="28"/>
-      <c r="C43" s="51"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="50"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="29"/>
-      <c r="C44" s="47"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="28"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="46"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="30"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="29"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="62"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B46" s="30"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="29"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="62"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B47" s="30"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="29"/>
+      <c r="C47" s="62"/>
+      <c r="D47" s="62"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="30"/>
-    </row>
-    <row r="49" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B48" s="29"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="62"/>
+    </row>
+    <row r="49" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="31"/>
-    </row>
-    <row r="50" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B49" s="30"/>
+      <c r="C49" s="63"/>
+      <c r="D49" s="63"/>
+    </row>
+    <row r="50" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B50" s="31"/>
-    </row>
-    <row r="51" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B50" s="30"/>
+      <c r="C50" s="63"/>
+      <c r="D50" s="63"/>
+    </row>
+    <row r="51" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B51" s="31"/>
-    </row>
-    <row r="52" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B51" s="30"/>
+      <c r="C51" s="63"/>
+      <c r="D51" s="63"/>
+    </row>
+    <row r="52" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B52" s="30"/>
-    </row>
-    <row r="53" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B52" s="29"/>
+      <c r="C52" s="62"/>
+      <c r="D52" s="62"/>
+    </row>
+    <row r="53" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="30"/>
-    </row>
-    <row r="54" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B53" s="29"/>
+      <c r="C53" s="62"/>
+      <c r="D53" s="62"/>
+    </row>
+    <row r="54" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B54" s="30"/>
-    </row>
-    <row r="55" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B54" s="29"/>
+      <c r="C54" s="62"/>
+      <c r="D54" s="62"/>
+    </row>
+    <row r="55" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B55" s="30"/>
-    </row>
-    <row r="56" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B55" s="29"/>
+      <c r="C55" s="62"/>
+      <c r="D55" s="62"/>
+    </row>
+    <row r="56" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B56" s="30"/>
-    </row>
-    <row r="57" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B56" s="29"/>
+      <c r="C56" s="62"/>
+      <c r="D56" s="62"/>
+    </row>
+    <row r="57" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B57" s="30"/>
-    </row>
-    <row r="58" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B57" s="29"/>
+      <c r="C57" s="62"/>
+      <c r="D57" s="62"/>
+    </row>
+    <row r="58" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B58" s="30"/>
-    </row>
-    <row r="59" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B58" s="29"/>
+      <c r="C58" s="62"/>
+      <c r="D58" s="62"/>
+    </row>
+    <row r="59" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B59" s="30"/>
-    </row>
-    <row r="60" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B59" s="29"/>
+      <c r="C59" s="62"/>
+      <c r="D59" s="62"/>
+    </row>
+    <row r="60" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B60" s="32"/>
-    </row>
-    <row r="61" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B60" s="31"/>
+      <c r="C60" s="62"/>
+      <c r="D60" s="62"/>
+    </row>
+    <row r="61" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B61" s="33"/>
-    </row>
-    <row r="62" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B61" s="32"/>
+      <c r="C61" s="62"/>
+      <c r="D61" s="62"/>
+    </row>
+    <row r="62" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B62" s="34"/>
-    </row>
-    <row r="63" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B62" s="33"/>
+      <c r="C62" s="62"/>
+      <c r="D62" s="62"/>
+    </row>
+    <row r="63" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B63" s="35"/>
-      <c r="C63" s="47"/>
-      <c r="D63" s="47"/>
-      <c r="E63" s="47"/>
-      <c r="F63" s="47"/>
-      <c r="G63" s="47"/>
-      <c r="H63" s="47"/>
-      <c r="I63" s="47"/>
-      <c r="J63" s="47"/>
-      <c r="K63" s="15"/>
-      <c r="L63" s="15"/>
+      <c r="B63" s="34"/>
+      <c r="C63" s="62"/>
+      <c r="D63" s="62"/>
+      <c r="E63" s="46"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="46"/>
+      <c r="H63" s="46"/>
+      <c r="I63" s="46"/>
+      <c r="J63" s="46"/>
+      <c r="K63" s="46"/>
+      <c r="L63" s="46"/>
       <c r="M63" s="15"/>
       <c r="N63" s="15"/>
       <c r="O63" s="15"/>
@@ -2869,22 +3004,24 @@
       <c r="BO63" s="15"/>
       <c r="BP63" s="15"/>
       <c r="BQ63" s="15"/>
-    </row>
-    <row r="64" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR63" s="15"/>
+      <c r="BS63" s="15"/>
+    </row>
+    <row r="64" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B64" s="35"/>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
-      <c r="E64" s="47"/>
-      <c r="F64" s="47"/>
-      <c r="G64" s="47"/>
-      <c r="H64" s="47"/>
-      <c r="I64" s="47"/>
-      <c r="J64" s="47"/>
-      <c r="K64" s="15"/>
-      <c r="L64" s="15"/>
+      <c r="B64" s="34"/>
+      <c r="C64" s="62"/>
+      <c r="D64" s="62"/>
+      <c r="E64" s="46"/>
+      <c r="F64" s="46"/>
+      <c r="G64" s="46"/>
+      <c r="H64" s="46"/>
+      <c r="I64" s="46"/>
+      <c r="J64" s="46"/>
+      <c r="K64" s="46"/>
+      <c r="L64" s="46"/>
       <c r="M64" s="15"/>
       <c r="N64" s="15"/>
       <c r="O64" s="15"/>
@@ -2942,22 +3079,24 @@
       <c r="BO64" s="15"/>
       <c r="BP64" s="15"/>
       <c r="BQ64" s="15"/>
-    </row>
-    <row r="65" spans="1:69" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="22" t="s">
+      <c r="BR64" s="15"/>
+      <c r="BS64" s="15"/>
+    </row>
+    <row r="65" spans="1:71" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B65" s="36"/>
-      <c r="C65" s="47"/>
-      <c r="D65" s="47"/>
-      <c r="E65" s="47"/>
-      <c r="F65" s="47"/>
-      <c r="G65" s="47"/>
-      <c r="H65" s="47"/>
-      <c r="I65" s="47"/>
-      <c r="J65" s="47"/>
-      <c r="K65" s="15"/>
-      <c r="L65" s="15"/>
+      <c r="B65" s="35"/>
+      <c r="C65" s="62"/>
+      <c r="D65" s="62"/>
+      <c r="E65" s="46"/>
+      <c r="F65" s="46"/>
+      <c r="G65" s="46"/>
+      <c r="H65" s="46"/>
+      <c r="I65" s="46"/>
+      <c r="J65" s="46"/>
+      <c r="K65" s="46"/>
+      <c r="L65" s="46"/>
       <c r="M65" s="15"/>
       <c r="N65" s="15"/>
       <c r="O65" s="15"/>
@@ -3015,64 +3154,72 @@
       <c r="BO65" s="15"/>
       <c r="BP65" s="15"/>
       <c r="BQ65" s="15"/>
-    </row>
-    <row r="66" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR65" s="15"/>
+      <c r="BS65" s="15"/>
+    </row>
+    <row r="66" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B66" s="35"/>
-      <c r="C66" s="47"/>
-      <c r="D66" s="47"/>
-      <c r="E66" s="47"/>
-      <c r="F66" s="47"/>
-      <c r="G66" s="47"/>
-      <c r="H66" s="47"/>
-      <c r="I66" s="47"/>
-      <c r="J66" s="47"/>
-    </row>
-    <row r="67" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="34"/>
+      <c r="C66" s="62"/>
+      <c r="D66" s="62"/>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="46"/>
+      <c r="I66" s="46"/>
+      <c r="J66" s="46"/>
+      <c r="K66" s="46"/>
+      <c r="L66" s="46"/>
+    </row>
+    <row r="67" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B67" s="35"/>
-      <c r="C67" s="47"/>
-      <c r="D67" s="47"/>
-      <c r="E67" s="47"/>
-      <c r="F67" s="47"/>
-      <c r="G67" s="47"/>
-      <c r="H67" s="47"/>
-      <c r="I67" s="47"/>
-      <c r="J67" s="47"/>
-    </row>
-    <row r="68" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="34"/>
+      <c r="C67" s="62"/>
+      <c r="D67" s="62"/>
+      <c r="E67" s="46"/>
+      <c r="F67" s="46"/>
+      <c r="G67" s="46"/>
+      <c r="H67" s="46"/>
+      <c r="I67" s="46"/>
+      <c r="J67" s="46"/>
+      <c r="K67" s="46"/>
+      <c r="L67" s="46"/>
+    </row>
+    <row r="68" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B68" s="35"/>
-      <c r="C68" s="47"/>
-      <c r="D68" s="47"/>
-      <c r="E68" s="47"/>
-      <c r="F68" s="47"/>
-      <c r="G68" s="47"/>
-      <c r="H68" s="47"/>
-      <c r="I68" s="47"/>
-      <c r="J68" s="47"/>
-    </row>
-    <row r="69" spans="1:69" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="34"/>
+      <c r="C68" s="62"/>
+      <c r="D68" s="62"/>
+      <c r="E68" s="46"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="46"/>
+      <c r="H68" s="46"/>
+      <c r="I68" s="46"/>
+      <c r="J68" s="46"/>
+      <c r="K68" s="46"/>
+      <c r="L68" s="46"/>
+    </row>
+    <row r="69" spans="1:71" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="37"/>
-      <c r="C69" s="47"/>
-      <c r="D69" s="47"/>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="47"/>
-      <c r="H69" s="47"/>
-      <c r="I69" s="47"/>
-      <c r="J69" s="47"/>
-      <c r="K69" s="15"/>
-      <c r="L69" s="15"/>
+      <c r="B69" s="36"/>
+      <c r="C69" s="62"/>
+      <c r="D69" s="62"/>
+      <c r="E69" s="46"/>
+      <c r="F69" s="46"/>
+      <c r="G69" s="46"/>
+      <c r="H69" s="46"/>
+      <c r="I69" s="46"/>
+      <c r="J69" s="46"/>
+      <c r="K69" s="46"/>
+      <c r="L69" s="46"/>
       <c r="M69" s="15"/>
       <c r="N69" s="15"/>
       <c r="O69" s="15"/>
@@ -3130,92 +3277,104 @@
       <c r="BO69" s="15"/>
       <c r="BP69" s="15"/>
       <c r="BQ69" s="15"/>
-    </row>
-    <row r="70" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BR69" s="15"/>
+      <c r="BS69" s="15"/>
+    </row>
+    <row r="70" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B70" s="38"/>
-      <c r="C70" s="47"/>
-      <c r="D70" s="47"/>
-      <c r="E70" s="47"/>
-      <c r="F70" s="47"/>
-      <c r="G70" s="47"/>
-      <c r="H70" s="47"/>
-      <c r="I70" s="47"/>
-      <c r="J70" s="47"/>
-    </row>
-    <row r="71" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="37"/>
+      <c r="C70" s="64"/>
+      <c r="D70" s="64"/>
+      <c r="E70" s="46"/>
+      <c r="F70" s="46"/>
+      <c r="G70" s="46"/>
+      <c r="H70" s="46"/>
+      <c r="I70" s="46"/>
+      <c r="J70" s="46"/>
+      <c r="K70" s="46"/>
+      <c r="L70" s="46"/>
+    </row>
+    <row r="71" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B71" s="38"/>
-      <c r="C71" s="47"/>
-      <c r="D71" s="47"/>
-      <c r="E71" s="47"/>
-      <c r="F71" s="47"/>
-      <c r="G71" s="47"/>
-      <c r="H71" s="47"/>
-      <c r="I71" s="47"/>
-      <c r="J71" s="47"/>
-    </row>
-    <row r="72" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="37"/>
+      <c r="C71" s="64"/>
+      <c r="D71" s="64"/>
+      <c r="E71" s="46"/>
+      <c r="F71" s="46"/>
+      <c r="G71" s="46"/>
+      <c r="H71" s="46"/>
+      <c r="I71" s="46"/>
+      <c r="J71" s="46"/>
+      <c r="K71" s="46"/>
+      <c r="L71" s="46"/>
+    </row>
+    <row r="72" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B72" s="38"/>
-      <c r="C72" s="47"/>
-      <c r="D72" s="47"/>
-      <c r="E72" s="47"/>
-      <c r="F72" s="47"/>
-      <c r="G72" s="47"/>
-      <c r="H72" s="47"/>
-      <c r="I72" s="47"/>
-      <c r="J72" s="47"/>
-    </row>
-    <row r="73" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="37"/>
+      <c r="C72" s="64"/>
+      <c r="D72" s="64"/>
+      <c r="E72" s="46"/>
+      <c r="F72" s="46"/>
+      <c r="G72" s="46"/>
+      <c r="H72" s="46"/>
+      <c r="I72" s="46"/>
+      <c r="J72" s="46"/>
+      <c r="K72" s="46"/>
+      <c r="L72" s="46"/>
+    </row>
+    <row r="73" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B73" s="38"/>
-      <c r="C73" s="47"/>
-      <c r="D73" s="47"/>
-      <c r="E73" s="47"/>
-      <c r="F73" s="47"/>
-      <c r="G73" s="47"/>
-      <c r="H73" s="47"/>
-      <c r="I73" s="47"/>
-      <c r="J73" s="47"/>
-    </row>
-    <row r="74" spans="1:69" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="37"/>
+      <c r="C73" s="64"/>
+      <c r="D73" s="64"/>
+      <c r="E73" s="46"/>
+      <c r="F73" s="46"/>
+      <c r="G73" s="46"/>
+      <c r="H73" s="46"/>
+      <c r="I73" s="46"/>
+      <c r="J73" s="46"/>
+      <c r="K73" s="46"/>
+      <c r="L73" s="46"/>
+    </row>
+    <row r="74" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B74" s="39"/>
-      <c r="C74" s="47"/>
-      <c r="D74" s="47"/>
-      <c r="E74" s="47"/>
-      <c r="F74" s="47"/>
-      <c r="G74" s="47"/>
-      <c r="H74" s="47"/>
-      <c r="I74" s="47"/>
-      <c r="J74" s="47"/>
-    </row>
-    <row r="75" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B74" s="38"/>
+      <c r="C74" s="64"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="46"/>
+      <c r="F74" s="46"/>
+      <c r="G74" s="46"/>
+      <c r="H74" s="46"/>
+      <c r="I74" s="46"/>
+      <c r="J74" s="46"/>
+      <c r="K74" s="46"/>
+      <c r="L74" s="46"/>
+    </row>
+    <row r="75" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B75" s="40"/>
-      <c r="C75" s="47"/>
-      <c r="D75" s="47"/>
-      <c r="E75" s="47"/>
-      <c r="F75" s="47"/>
-      <c r="G75" s="47"/>
-      <c r="H75" s="47"/>
-      <c r="I75" s="47"/>
-      <c r="J75" s="47"/>
-      <c r="K75" s="15"/>
-      <c r="L75" s="15"/>
+      <c r="B75" s="39"/>
+      <c r="C75" s="50"/>
+      <c r="D75" s="50"/>
+      <c r="E75" s="46"/>
+      <c r="F75" s="46"/>
+      <c r="G75" s="46"/>
+      <c r="H75" s="46"/>
+      <c r="I75" s="46"/>
+      <c r="J75" s="46"/>
+      <c r="K75" s="46"/>
+      <c r="L75" s="46"/>
       <c r="M75" s="15"/>
       <c r="N75" s="15"/>
       <c r="O75" s="15"/>
@@ -3273,22 +3432,24 @@
       <c r="BO75" s="15"/>
       <c r="BP75" s="15"/>
       <c r="BQ75" s="15"/>
-    </row>
-    <row r="76" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR75" s="15"/>
+      <c r="BS75" s="15"/>
+    </row>
+    <row r="76" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B76" s="40"/>
-      <c r="C76" s="47"/>
-      <c r="D76" s="47"/>
-      <c r="E76" s="47"/>
-      <c r="F76" s="47"/>
-      <c r="G76" s="47"/>
-      <c r="H76" s="47"/>
-      <c r="I76" s="47"/>
-      <c r="J76" s="47"/>
-      <c r="K76" s="15"/>
-      <c r="L76" s="15"/>
+      <c r="B76" s="39"/>
+      <c r="C76" s="50"/>
+      <c r="D76" s="50"/>
+      <c r="E76" s="46"/>
+      <c r="F76" s="46"/>
+      <c r="G76" s="46"/>
+      <c r="H76" s="46"/>
+      <c r="I76" s="46"/>
+      <c r="J76" s="46"/>
+      <c r="K76" s="46"/>
+      <c r="L76" s="46"/>
       <c r="M76" s="15"/>
       <c r="N76" s="15"/>
       <c r="O76" s="15"/>
@@ -3346,22 +3507,24 @@
       <c r="BO76" s="15"/>
       <c r="BP76" s="15"/>
       <c r="BQ76" s="15"/>
-    </row>
-    <row r="77" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR76" s="15"/>
+      <c r="BS76" s="15"/>
+    </row>
+    <row r="77" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B77" s="41"/>
-      <c r="C77" s="47"/>
-      <c r="D77" s="47"/>
-      <c r="E77" s="47"/>
-      <c r="F77" s="47"/>
-      <c r="G77" s="47"/>
-      <c r="H77" s="47"/>
-      <c r="I77" s="47"/>
-      <c r="J77" s="47"/>
-      <c r="K77" s="15"/>
-      <c r="L77" s="15"/>
+      <c r="B77" s="40"/>
+      <c r="C77" s="50"/>
+      <c r="D77" s="50"/>
+      <c r="E77" s="46"/>
+      <c r="F77" s="46"/>
+      <c r="G77" s="46"/>
+      <c r="H77" s="46"/>
+      <c r="I77" s="46"/>
+      <c r="J77" s="46"/>
+      <c r="K77" s="46"/>
+      <c r="L77" s="46"/>
       <c r="M77" s="15"/>
       <c r="N77" s="15"/>
       <c r="O77" s="15"/>
@@ -3419,282 +3582,372 @@
       <c r="BO77" s="15"/>
       <c r="BP77" s="15"/>
       <c r="BQ77" s="15"/>
-    </row>
-    <row r="78" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="BR77" s="15"/>
+      <c r="BS77" s="15"/>
+    </row>
+    <row r="78" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A78" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B78" s="42"/>
-    </row>
-    <row r="79" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B78" s="41"/>
+      <c r="C78" s="50"/>
+      <c r="D78" s="50"/>
+    </row>
+    <row r="79" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A79" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B79" s="43"/>
-    </row>
-    <row r="80" spans="1:69" x14ac:dyDescent="0.25">
+      <c r="B79" s="42"/>
+      <c r="C79" s="65"/>
+      <c r="D79" s="65"/>
+    </row>
+    <row r="80" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B80" s="42"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B80" s="41"/>
+      <c r="C80" s="50"/>
+      <c r="D80" s="50"/>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B81" s="44"/>
-      <c r="C81" s="53"/>
-      <c r="D81" s="53"/>
-      <c r="E81" s="53"/>
-      <c r="F81" s="53"/>
-      <c r="G81" s="53"/>
-      <c r="H81" s="53"/>
-      <c r="I81" s="54"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B81" s="43"/>
+      <c r="C81" s="43"/>
+      <c r="D81" s="43"/>
+      <c r="E81" s="52"/>
+      <c r="F81" s="52"/>
+      <c r="G81" s="52"/>
+      <c r="H81" s="52"/>
+      <c r="I81" s="52"/>
+      <c r="J81" s="52"/>
+      <c r="K81" s="53"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B82" s="45">
+      <c r="B82" s="44">
         <v>5</v>
       </c>
-      <c r="C82" s="45">
+      <c r="C82" s="44">
         <v>15</v>
       </c>
-      <c r="D82" s="45"/>
-      <c r="E82" s="55"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D82" s="44"/>
+      <c r="E82" s="44"/>
+      <c r="F82" s="44"/>
+      <c r="G82" s="54"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B83" s="46"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B83" s="45"/>
+      <c r="C83" s="50"/>
+      <c r="D83" s="50"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B84" s="42"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B84" s="41"/>
+      <c r="C84" s="50"/>
+      <c r="D84" s="50"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="B85" s="42"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B85" s="41"/>
+      <c r="C85" s="50"/>
+      <c r="D85" s="50"/>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="B86" s="42"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B86" s="41"/>
+      <c r="C86" s="50"/>
+      <c r="D86" s="50"/>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B87" s="42"/>
-    </row>
-    <row r="88" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="41"/>
+      <c r="C87" s="50"/>
+      <c r="D87" s="50"/>
+    </row>
+    <row r="88" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B88" s="42"/>
-      <c r="C88" s="51"/>
-      <c r="D88" s="47"/>
-      <c r="E88" s="47"/>
-      <c r="F88" s="47"/>
-      <c r="G88" s="47"/>
-      <c r="H88" s="47"/>
-      <c r="I88" s="47"/>
-      <c r="J88" s="47"/>
-    </row>
-    <row r="89" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="41"/>
+      <c r="C88" s="50"/>
+      <c r="D88" s="50"/>
+      <c r="E88" s="50"/>
+      <c r="F88" s="46"/>
+      <c r="G88" s="46"/>
+      <c r="H88" s="46"/>
+      <c r="I88" s="46"/>
+      <c r="J88" s="46"/>
+      <c r="K88" s="46"/>
+      <c r="L88" s="46"/>
+    </row>
+    <row r="89" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="B89" s="42"/>
-      <c r="C89" s="51"/>
-      <c r="D89" s="47"/>
-      <c r="E89" s="47"/>
-      <c r="F89" s="47"/>
-      <c r="G89" s="47"/>
-      <c r="H89" s="47"/>
-      <c r="I89" s="47"/>
-      <c r="J89" s="47"/>
-    </row>
-    <row r="90" spans="1:10" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="41"/>
+      <c r="C89" s="50"/>
+      <c r="D89" s="50"/>
+      <c r="E89" s="50"/>
+      <c r="F89" s="46"/>
+      <c r="G89" s="46"/>
+      <c r="H89" s="46"/>
+      <c r="I89" s="46"/>
+      <c r="J89" s="46"/>
+      <c r="K89" s="46"/>
+      <c r="L89" s="46"/>
+    </row>
+    <row r="90" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="B90" s="42"/>
-      <c r="C90" s="51"/>
-      <c r="D90" s="47"/>
-      <c r="E90" s="47"/>
-      <c r="F90" s="47"/>
-      <c r="G90" s="47"/>
-      <c r="H90" s="47"/>
-      <c r="I90" s="47"/>
-      <c r="J90" s="47"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B90" s="41"/>
+      <c r="C90" s="50"/>
+      <c r="D90" s="50"/>
+      <c r="E90" s="50"/>
+      <c r="F90" s="46"/>
+      <c r="G90" s="46"/>
+      <c r="H90" s="46"/>
+      <c r="I90" s="46"/>
+      <c r="J90" s="46"/>
+      <c r="K90" s="46"/>
+      <c r="L90" s="46"/>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B91" s="42"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B91" s="41"/>
+      <c r="C91" s="50"/>
+      <c r="D91" s="50"/>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B92" s="42"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A93" s="19" t="s">
+      <c r="B92" s="41"/>
+      <c r="C92" s="50"/>
+      <c r="D92" s="50"/>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B93" s="42"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A94" s="56" t="s">
+      <c r="B93" s="41"/>
+      <c r="C93" s="50"/>
+      <c r="D93" s="50"/>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B94" s="41" t="b">
+        <v>1</v>
+      </c>
+      <c r="C94" s="50"/>
+      <c r="D94" s="50"/>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B95" s="41"/>
+      <c r="C95" s="50"/>
+      <c r="D95" s="50"/>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B94" s="62"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A95" s="57" t="s">
+      <c r="B96" s="61"/>
+      <c r="C96" s="50"/>
+      <c r="D96" s="50"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="B95" s="60"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A96" s="57" t="s">
+      <c r="B97" s="59"/>
+      <c r="C97" s="50"/>
+      <c r="D97" s="50"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="B96" s="60"/>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="57" t="s">
+      <c r="B98" s="59"/>
+      <c r="C98" s="50"/>
+      <c r="D98" s="50"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="B97" s="60"/>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="57" t="s">
+      <c r="B99" s="59"/>
+      <c r="C99" s="50"/>
+      <c r="D99" s="50"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="B98" s="60"/>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="57" t="s">
+      <c r="B100" s="59"/>
+      <c r="C100" s="50"/>
+      <c r="D100" s="50"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="B99" s="60"/>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="57" t="s">
+      <c r="B101" s="59"/>
+      <c r="C101" s="50"/>
+      <c r="D101" s="50"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="B100" s="60"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="58" t="s">
+      <c r="B102" s="59"/>
+      <c r="C102" s="50"/>
+      <c r="D102" s="50"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="B101" s="60"/>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="58" t="s">
+      <c r="B103" s="59"/>
+      <c r="C103" s="50"/>
+      <c r="D103" s="50"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="B102" s="60"/>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="58" t="s">
+      <c r="B104" s="59"/>
+      <c r="C104" s="50"/>
+      <c r="D104" s="50"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="B103" s="60"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="58" t="s">
+      <c r="B105" s="59"/>
+      <c r="C105" s="50"/>
+      <c r="D105" s="50"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="B104" s="60"/>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="58" t="s">
+      <c r="B106" s="59"/>
+      <c r="C106" s="50"/>
+      <c r="D106" s="50"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="B105" s="60"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="58" t="s">
+      <c r="B107" s="59"/>
+      <c r="C107" s="50"/>
+      <c r="D107" s="50"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="B106" s="60"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="58" t="s">
+      <c r="B108" s="59"/>
+      <c r="C108" s="50"/>
+      <c r="D108" s="50"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="B107" s="60"/>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="58" t="s">
+      <c r="B109" s="59"/>
+      <c r="C109" s="50"/>
+      <c r="D109" s="50"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="B108" s="60"/>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="58" t="s">
+      <c r="B110" s="59"/>
+      <c r="C110" s="50"/>
+      <c r="D110" s="50"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="B109" s="60"/>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="58" t="s">
+      <c r="B111" s="59"/>
+      <c r="C111" s="50"/>
+      <c r="D111" s="50"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="B110" s="60"/>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="58" t="s">
+      <c r="B112" s="59"/>
+      <c r="C112" s="50"/>
+      <c r="D112" s="50"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="B111" s="60"/>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="59" t="s">
+      <c r="B113" s="59"/>
+      <c r="C113" s="50"/>
+      <c r="D113" s="50"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="B112" s="61"/>
+      <c r="B114" s="60"/>
+      <c r="C114" s="50"/>
+      <c r="D114" s="50"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B78 B63:B64">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B78:D78 B63:D64">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61:B62">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61:D62">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79:D79">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45:B60">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45:D60">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B81">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B81:D81">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44:D44">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B70:B74">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B70:D74">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -3708,13 +3961,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B83:B93 B65:B69 B75:B77</xm:sqref>
+          <xm:sqref>B83:D95 B65:D69 B75:D77</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B80</xm:sqref>
+          <xm:sqref>B80:D80</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Object-orient main output plotting
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2369,8 +2369,8 @@
   </sheetPr>
   <dimension ref="A1:BS114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3755,9 +3755,7 @@
       <c r="A94" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="B94" s="41" t="b">
-        <v>1</v>
-      </c>
+      <c r="B94" s="41"/>
       <c r="C94" s="50"/>
       <c r="D94" s="50"/>
     </row>

</xml_diff>

<commit_message>
More tidying of main outputs plotting function
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="121">
   <si>
     <t>recent_time</t>
   </si>
@@ -372,6 +372,12 @@
   </si>
   <si>
     <t>output_uncertainty_all_scenarios</t>
+  </si>
+  <si>
+    <t>plot_end_time</t>
+  </si>
+  <si>
+    <t>plot_start_time</t>
   </si>
 </sst>
 </file>
@@ -2367,10 +2373,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BS114"/>
+  <dimension ref="A1:BS116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2820,7 +2826,7 @@
       <c r="C48" s="62"/>
       <c r="D48" s="62"/>
     </row>
-    <row r="49" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>113</v>
       </c>
@@ -2828,7 +2834,7 @@
       <c r="C49" s="63"/>
       <c r="D49" s="63"/>
     </row>
-    <row r="50" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>114</v>
       </c>
@@ -2836,7 +2842,7 @@
       <c r="C50" s="63"/>
       <c r="D50" s="63"/>
     </row>
-    <row r="51" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>115</v>
       </c>
@@ -2844,7 +2850,7 @@
       <c r="C51" s="63"/>
       <c r="D51" s="63"/>
     </row>
-    <row r="52" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>0</v>
       </c>
@@ -2852,7 +2858,7 @@
       <c r="C52" s="62"/>
       <c r="D52" s="62"/>
     </row>
-    <row r="53" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>11</v>
       </c>
@@ -2860,7 +2866,7 @@
       <c r="C53" s="62"/>
       <c r="D53" s="62"/>
     </row>
-    <row r="54" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>13</v>
       </c>
@@ -2868,7 +2874,7 @@
       <c r="C54" s="62"/>
       <c r="D54" s="62"/>
     </row>
-    <row r="55" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>14</v>
       </c>
@@ -2876,7 +2882,7 @@
       <c r="C55" s="62"/>
       <c r="D55" s="62"/>
     </row>
-    <row r="56" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>10</v>
       </c>
@@ -2884,7 +2890,7 @@
       <c r="C56" s="62"/>
       <c r="D56" s="62"/>
     </row>
-    <row r="57" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>109</v>
       </c>
@@ -2892,7 +2898,7 @@
       <c r="C57" s="62"/>
       <c r="D57" s="62"/>
     </row>
-    <row r="58" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>110</v>
       </c>
@@ -2900,7 +2906,7 @@
       <c r="C58" s="62"/>
       <c r="D58" s="62"/>
     </row>
-    <row r="59" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>111</v>
       </c>
@@ -2908,185 +2914,51 @@
       <c r="C59" s="62"/>
       <c r="D59" s="62"/>
     </row>
-    <row r="60" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B60" s="31"/>
+        <v>120</v>
+      </c>
+      <c r="B60" s="29"/>
       <c r="C60" s="62"/>
       <c r="D60" s="62"/>
     </row>
-    <row r="61" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B61" s="32"/>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B61" s="29"/>
       <c r="C61" s="62"/>
       <c r="D61" s="62"/>
     </row>
-    <row r="62" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A62" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B62" s="33"/>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B62" s="31"/>
       <c r="C62" s="62"/>
       <c r="D62" s="62"/>
     </row>
-    <row r="63" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B63" s="34"/>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B63" s="32"/>
       <c r="C63" s="62"/>
       <c r="D63" s="62"/>
-      <c r="E63" s="46"/>
-      <c r="F63" s="46"/>
-      <c r="G63" s="46"/>
-      <c r="H63" s="46"/>
-      <c r="I63" s="46"/>
-      <c r="J63" s="46"/>
-      <c r="K63" s="46"/>
-      <c r="L63" s="46"/>
-      <c r="M63" s="15"/>
-      <c r="N63" s="15"/>
-      <c r="O63" s="15"/>
-      <c r="P63" s="15"/>
-      <c r="Q63" s="15"/>
-      <c r="R63" s="15"/>
-      <c r="S63" s="15"/>
-      <c r="T63" s="15"/>
-      <c r="U63" s="15"/>
-      <c r="V63" s="15"/>
-      <c r="W63" s="15"/>
-      <c r="X63" s="15"/>
-      <c r="Y63" s="15"/>
-      <c r="Z63" s="15"/>
-      <c r="AA63" s="15"/>
-      <c r="AB63" s="15"/>
-      <c r="AC63" s="15"/>
-      <c r="AD63" s="15"/>
-      <c r="AE63" s="15"/>
-      <c r="AF63" s="15"/>
-      <c r="AG63" s="15"/>
-      <c r="AH63" s="15"/>
-      <c r="AI63" s="15"/>
-      <c r="AJ63" s="15"/>
-      <c r="AK63" s="15"/>
-      <c r="AL63" s="15"/>
-      <c r="AM63" s="15"/>
-      <c r="AN63" s="15"/>
-      <c r="AO63" s="15"/>
-      <c r="AP63" s="15"/>
-      <c r="AQ63" s="15"/>
-      <c r="AR63" s="15"/>
-      <c r="AS63" s="15"/>
-      <c r="AT63" s="15"/>
-      <c r="AU63" s="15"/>
-      <c r="AV63" s="15"/>
-      <c r="AW63" s="15"/>
-      <c r="AX63" s="15"/>
-      <c r="AY63" s="15"/>
-      <c r="AZ63" s="15"/>
-      <c r="BA63" s="15"/>
-      <c r="BB63" s="15"/>
-      <c r="BC63" s="15"/>
-      <c r="BD63" s="15"/>
-      <c r="BE63" s="15"/>
-      <c r="BF63" s="15"/>
-      <c r="BG63" s="15"/>
-      <c r="BH63" s="15"/>
-      <c r="BI63" s="15"/>
-      <c r="BJ63" s="15"/>
-      <c r="BK63" s="15"/>
-      <c r="BL63" s="15"/>
-      <c r="BM63" s="15"/>
-      <c r="BN63" s="15"/>
-      <c r="BO63" s="15"/>
-      <c r="BP63" s="15"/>
-      <c r="BQ63" s="15"/>
-      <c r="BR63" s="15"/>
-      <c r="BS63" s="15"/>
-    </row>
-    <row r="64" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B64" s="34"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B64" s="33"/>
       <c r="C64" s="62"/>
       <c r="D64" s="62"/>
-      <c r="E64" s="46"/>
-      <c r="F64" s="46"/>
-      <c r="G64" s="46"/>
-      <c r="H64" s="46"/>
-      <c r="I64" s="46"/>
-      <c r="J64" s="46"/>
-      <c r="K64" s="46"/>
-      <c r="L64" s="46"/>
-      <c r="M64" s="15"/>
-      <c r="N64" s="15"/>
-      <c r="O64" s="15"/>
-      <c r="P64" s="15"/>
-      <c r="Q64" s="15"/>
-      <c r="R64" s="15"/>
-      <c r="S64" s="15"/>
-      <c r="T64" s="15"/>
-      <c r="U64" s="15"/>
-      <c r="V64" s="15"/>
-      <c r="W64" s="15"/>
-      <c r="X64" s="15"/>
-      <c r="Y64" s="15"/>
-      <c r="Z64" s="15"/>
-      <c r="AA64" s="15"/>
-      <c r="AB64" s="15"/>
-      <c r="AC64" s="15"/>
-      <c r="AD64" s="15"/>
-      <c r="AE64" s="15"/>
-      <c r="AF64" s="15"/>
-      <c r="AG64" s="15"/>
-      <c r="AH64" s="15"/>
-      <c r="AI64" s="15"/>
-      <c r="AJ64" s="15"/>
-      <c r="AK64" s="15"/>
-      <c r="AL64" s="15"/>
-      <c r="AM64" s="15"/>
-      <c r="AN64" s="15"/>
-      <c r="AO64" s="15"/>
-      <c r="AP64" s="15"/>
-      <c r="AQ64" s="15"/>
-      <c r="AR64" s="15"/>
-      <c r="AS64" s="15"/>
-      <c r="AT64" s="15"/>
-      <c r="AU64" s="15"/>
-      <c r="AV64" s="15"/>
-      <c r="AW64" s="15"/>
-      <c r="AX64" s="15"/>
-      <c r="AY64" s="15"/>
-      <c r="AZ64" s="15"/>
-      <c r="BA64" s="15"/>
-      <c r="BB64" s="15"/>
-      <c r="BC64" s="15"/>
-      <c r="BD64" s="15"/>
-      <c r="BE64" s="15"/>
-      <c r="BF64" s="15"/>
-      <c r="BG64" s="15"/>
-      <c r="BH64" s="15"/>
-      <c r="BI64" s="15"/>
-      <c r="BJ64" s="15"/>
-      <c r="BK64" s="15"/>
-      <c r="BL64" s="15"/>
-      <c r="BM64" s="15"/>
-      <c r="BN64" s="15"/>
-      <c r="BO64" s="15"/>
-      <c r="BP64" s="15"/>
-      <c r="BQ64" s="15"/>
-      <c r="BR64" s="15"/>
-      <c r="BS64" s="15"/>
-    </row>
-    <row r="65" spans="1:71" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B65" s="35"/>
+    </row>
+    <row r="65" spans="1:71" x14ac:dyDescent="0.25">
+      <c r="A65" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="34"/>
       <c r="C65" s="62"/>
       <c r="D65" s="62"/>
       <c r="E65" s="46"/>
@@ -3157,9 +3029,9 @@
       <c r="BR65" s="15"/>
       <c r="BS65" s="15"/>
     </row>
-    <row r="66" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
-        <v>74</v>
+        <v>2</v>
       </c>
       <c r="B66" s="34"/>
       <c r="C66" s="62"/>
@@ -3172,12 +3044,71 @@
       <c r="J66" s="46"/>
       <c r="K66" s="46"/>
       <c r="L66" s="46"/>
-    </row>
-    <row r="67" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B67" s="34"/>
+      <c r="M66" s="15"/>
+      <c r="N66" s="15"/>
+      <c r="O66" s="15"/>
+      <c r="P66" s="15"/>
+      <c r="Q66" s="15"/>
+      <c r="R66" s="15"/>
+      <c r="S66" s="15"/>
+      <c r="T66" s="15"/>
+      <c r="U66" s="15"/>
+      <c r="V66" s="15"/>
+      <c r="W66" s="15"/>
+      <c r="X66" s="15"/>
+      <c r="Y66" s="15"/>
+      <c r="Z66" s="15"/>
+      <c r="AA66" s="15"/>
+      <c r="AB66" s="15"/>
+      <c r="AC66" s="15"/>
+      <c r="AD66" s="15"/>
+      <c r="AE66" s="15"/>
+      <c r="AF66" s="15"/>
+      <c r="AG66" s="15"/>
+      <c r="AH66" s="15"/>
+      <c r="AI66" s="15"/>
+      <c r="AJ66" s="15"/>
+      <c r="AK66" s="15"/>
+      <c r="AL66" s="15"/>
+      <c r="AM66" s="15"/>
+      <c r="AN66" s="15"/>
+      <c r="AO66" s="15"/>
+      <c r="AP66" s="15"/>
+      <c r="AQ66" s="15"/>
+      <c r="AR66" s="15"/>
+      <c r="AS66" s="15"/>
+      <c r="AT66" s="15"/>
+      <c r="AU66" s="15"/>
+      <c r="AV66" s="15"/>
+      <c r="AW66" s="15"/>
+      <c r="AX66" s="15"/>
+      <c r="AY66" s="15"/>
+      <c r="AZ66" s="15"/>
+      <c r="BA66" s="15"/>
+      <c r="BB66" s="15"/>
+      <c r="BC66" s="15"/>
+      <c r="BD66" s="15"/>
+      <c r="BE66" s="15"/>
+      <c r="BF66" s="15"/>
+      <c r="BG66" s="15"/>
+      <c r="BH66" s="15"/>
+      <c r="BI66" s="15"/>
+      <c r="BJ66" s="15"/>
+      <c r="BK66" s="15"/>
+      <c r="BL66" s="15"/>
+      <c r="BM66" s="15"/>
+      <c r="BN66" s="15"/>
+      <c r="BO66" s="15"/>
+      <c r="BP66" s="15"/>
+      <c r="BQ66" s="15"/>
+      <c r="BR66" s="15"/>
+      <c r="BS66" s="15"/>
+    </row>
+    <row r="67" spans="1:71" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67" s="35"/>
       <c r="C67" s="62"/>
       <c r="D67" s="62"/>
       <c r="E67" s="46"/>
@@ -3188,10 +3119,69 @@
       <c r="J67" s="46"/>
       <c r="K67" s="46"/>
       <c r="L67" s="46"/>
+      <c r="M67" s="15"/>
+      <c r="N67" s="15"/>
+      <c r="O67" s="15"/>
+      <c r="P67" s="15"/>
+      <c r="Q67" s="15"/>
+      <c r="R67" s="15"/>
+      <c r="S67" s="15"/>
+      <c r="T67" s="15"/>
+      <c r="U67" s="15"/>
+      <c r="V67" s="15"/>
+      <c r="W67" s="15"/>
+      <c r="X67" s="15"/>
+      <c r="Y67" s="15"/>
+      <c r="Z67" s="15"/>
+      <c r="AA67" s="15"/>
+      <c r="AB67" s="15"/>
+      <c r="AC67" s="15"/>
+      <c r="AD67" s="15"/>
+      <c r="AE67" s="15"/>
+      <c r="AF67" s="15"/>
+      <c r="AG67" s="15"/>
+      <c r="AH67" s="15"/>
+      <c r="AI67" s="15"/>
+      <c r="AJ67" s="15"/>
+      <c r="AK67" s="15"/>
+      <c r="AL67" s="15"/>
+      <c r="AM67" s="15"/>
+      <c r="AN67" s="15"/>
+      <c r="AO67" s="15"/>
+      <c r="AP67" s="15"/>
+      <c r="AQ67" s="15"/>
+      <c r="AR67" s="15"/>
+      <c r="AS67" s="15"/>
+      <c r="AT67" s="15"/>
+      <c r="AU67" s="15"/>
+      <c r="AV67" s="15"/>
+      <c r="AW67" s="15"/>
+      <c r="AX67" s="15"/>
+      <c r="AY67" s="15"/>
+      <c r="AZ67" s="15"/>
+      <c r="BA67" s="15"/>
+      <c r="BB67" s="15"/>
+      <c r="BC67" s="15"/>
+      <c r="BD67" s="15"/>
+      <c r="BE67" s="15"/>
+      <c r="BF67" s="15"/>
+      <c r="BG67" s="15"/>
+      <c r="BH67" s="15"/>
+      <c r="BI67" s="15"/>
+      <c r="BJ67" s="15"/>
+      <c r="BK67" s="15"/>
+      <c r="BL67" s="15"/>
+      <c r="BM67" s="15"/>
+      <c r="BN67" s="15"/>
+      <c r="BO67" s="15"/>
+      <c r="BP67" s="15"/>
+      <c r="BQ67" s="15"/>
+      <c r="BR67" s="15"/>
+      <c r="BS67" s="15"/>
     </row>
     <row r="68" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B68" s="34"/>
       <c r="C68" s="62"/>
@@ -3205,11 +3195,11 @@
       <c r="K68" s="46"/>
       <c r="L68" s="46"/>
     </row>
-    <row r="69" spans="1:71" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B69" s="36"/>
+    <row r="69" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69" s="34"/>
       <c r="C69" s="62"/>
       <c r="D69" s="62"/>
       <c r="E69" s="46"/>
@@ -3220,73 +3210,14 @@
       <c r="J69" s="46"/>
       <c r="K69" s="46"/>
       <c r="L69" s="46"/>
-      <c r="M69" s="15"/>
-      <c r="N69" s="15"/>
-      <c r="O69" s="15"/>
-      <c r="P69" s="15"/>
-      <c r="Q69" s="15"/>
-      <c r="R69" s="15"/>
-      <c r="S69" s="15"/>
-      <c r="T69" s="15"/>
-      <c r="U69" s="15"/>
-      <c r="V69" s="15"/>
-      <c r="W69" s="15"/>
-      <c r="X69" s="15"/>
-      <c r="Y69" s="15"/>
-      <c r="Z69" s="15"/>
-      <c r="AA69" s="15"/>
-      <c r="AB69" s="15"/>
-      <c r="AC69" s="15"/>
-      <c r="AD69" s="15"/>
-      <c r="AE69" s="15"/>
-      <c r="AF69" s="15"/>
-      <c r="AG69" s="15"/>
-      <c r="AH69" s="15"/>
-      <c r="AI69" s="15"/>
-      <c r="AJ69" s="15"/>
-      <c r="AK69" s="15"/>
-      <c r="AL69" s="15"/>
-      <c r="AM69" s="15"/>
-      <c r="AN69" s="15"/>
-      <c r="AO69" s="15"/>
-      <c r="AP69" s="15"/>
-      <c r="AQ69" s="15"/>
-      <c r="AR69" s="15"/>
-      <c r="AS69" s="15"/>
-      <c r="AT69" s="15"/>
-      <c r="AU69" s="15"/>
-      <c r="AV69" s="15"/>
-      <c r="AW69" s="15"/>
-      <c r="AX69" s="15"/>
-      <c r="AY69" s="15"/>
-      <c r="AZ69" s="15"/>
-      <c r="BA69" s="15"/>
-      <c r="BB69" s="15"/>
-      <c r="BC69" s="15"/>
-      <c r="BD69" s="15"/>
-      <c r="BE69" s="15"/>
-      <c r="BF69" s="15"/>
-      <c r="BG69" s="15"/>
-      <c r="BH69" s="15"/>
-      <c r="BI69" s="15"/>
-      <c r="BJ69" s="15"/>
-      <c r="BK69" s="15"/>
-      <c r="BL69" s="15"/>
-      <c r="BM69" s="15"/>
-      <c r="BN69" s="15"/>
-      <c r="BO69" s="15"/>
-      <c r="BP69" s="15"/>
-      <c r="BQ69" s="15"/>
-      <c r="BR69" s="15"/>
-      <c r="BS69" s="15"/>
     </row>
     <row r="70" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B70" s="37"/>
-      <c r="C70" s="64"/>
-      <c r="D70" s="64"/>
+        <v>71</v>
+      </c>
+      <c r="B70" s="34"/>
+      <c r="C70" s="62"/>
+      <c r="D70" s="62"/>
       <c r="E70" s="46"/>
       <c r="F70" s="46"/>
       <c r="G70" s="46"/>
@@ -3296,13 +3227,13 @@
       <c r="K70" s="46"/>
       <c r="L70" s="46"/>
     </row>
-    <row r="71" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B71" s="37"/>
-      <c r="C71" s="64"/>
-      <c r="D71" s="64"/>
+    <row r="71" spans="1:71" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71" s="36"/>
+      <c r="C71" s="62"/>
+      <c r="D71" s="62"/>
       <c r="E71" s="46"/>
       <c r="F71" s="46"/>
       <c r="G71" s="46"/>
@@ -3311,10 +3242,69 @@
       <c r="J71" s="46"/>
       <c r="K71" s="46"/>
       <c r="L71" s="46"/>
+      <c r="M71" s="15"/>
+      <c r="N71" s="15"/>
+      <c r="O71" s="15"/>
+      <c r="P71" s="15"/>
+      <c r="Q71" s="15"/>
+      <c r="R71" s="15"/>
+      <c r="S71" s="15"/>
+      <c r="T71" s="15"/>
+      <c r="U71" s="15"/>
+      <c r="V71" s="15"/>
+      <c r="W71" s="15"/>
+      <c r="X71" s="15"/>
+      <c r="Y71" s="15"/>
+      <c r="Z71" s="15"/>
+      <c r="AA71" s="15"/>
+      <c r="AB71" s="15"/>
+      <c r="AC71" s="15"/>
+      <c r="AD71" s="15"/>
+      <c r="AE71" s="15"/>
+      <c r="AF71" s="15"/>
+      <c r="AG71" s="15"/>
+      <c r="AH71" s="15"/>
+      <c r="AI71" s="15"/>
+      <c r="AJ71" s="15"/>
+      <c r="AK71" s="15"/>
+      <c r="AL71" s="15"/>
+      <c r="AM71" s="15"/>
+      <c r="AN71" s="15"/>
+      <c r="AO71" s="15"/>
+      <c r="AP71" s="15"/>
+      <c r="AQ71" s="15"/>
+      <c r="AR71" s="15"/>
+      <c r="AS71" s="15"/>
+      <c r="AT71" s="15"/>
+      <c r="AU71" s="15"/>
+      <c r="AV71" s="15"/>
+      <c r="AW71" s="15"/>
+      <c r="AX71" s="15"/>
+      <c r="AY71" s="15"/>
+      <c r="AZ71" s="15"/>
+      <c r="BA71" s="15"/>
+      <c r="BB71" s="15"/>
+      <c r="BC71" s="15"/>
+      <c r="BD71" s="15"/>
+      <c r="BE71" s="15"/>
+      <c r="BF71" s="15"/>
+      <c r="BG71" s="15"/>
+      <c r="BH71" s="15"/>
+      <c r="BI71" s="15"/>
+      <c r="BJ71" s="15"/>
+      <c r="BK71" s="15"/>
+      <c r="BL71" s="15"/>
+      <c r="BM71" s="15"/>
+      <c r="BN71" s="15"/>
+      <c r="BO71" s="15"/>
+      <c r="BP71" s="15"/>
+      <c r="BQ71" s="15"/>
+      <c r="BR71" s="15"/>
+      <c r="BS71" s="15"/>
     </row>
     <row r="72" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B72" s="37"/>
       <c r="C72" s="64"/>
@@ -3330,7 +3320,7 @@
     </row>
     <row r="73" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B73" s="37"/>
       <c r="C73" s="64"/>
@@ -3345,10 +3335,10 @@
       <c r="L73" s="46"/>
     </row>
     <row r="74" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B74" s="38"/>
+      <c r="A74" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74" s="37"/>
       <c r="C74" s="64"/>
       <c r="D74" s="64"/>
       <c r="E74" s="46"/>
@@ -3360,13 +3350,13 @@
       <c r="K74" s="46"/>
       <c r="L74" s="46"/>
     </row>
-    <row r="75" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B75" s="39"/>
-      <c r="C75" s="50"/>
-      <c r="D75" s="50"/>
+        <v>78</v>
+      </c>
+      <c r="B75" s="37"/>
+      <c r="C75" s="64"/>
+      <c r="D75" s="64"/>
       <c r="E75" s="46"/>
       <c r="F75" s="46"/>
       <c r="G75" s="46"/>
@@ -3375,73 +3365,14 @@
       <c r="J75" s="46"/>
       <c r="K75" s="46"/>
       <c r="L75" s="46"/>
-      <c r="M75" s="15"/>
-      <c r="N75" s="15"/>
-      <c r="O75" s="15"/>
-      <c r="P75" s="15"/>
-      <c r="Q75" s="15"/>
-      <c r="R75" s="15"/>
-      <c r="S75" s="15"/>
-      <c r="T75" s="15"/>
-      <c r="U75" s="15"/>
-      <c r="V75" s="15"/>
-      <c r="W75" s="15"/>
-      <c r="X75" s="15"/>
-      <c r="Y75" s="15"/>
-      <c r="Z75" s="15"/>
-      <c r="AA75" s="15"/>
-      <c r="AB75" s="15"/>
-      <c r="AC75" s="15"/>
-      <c r="AD75" s="15"/>
-      <c r="AE75" s="15"/>
-      <c r="AF75" s="15"/>
-      <c r="AG75" s="15"/>
-      <c r="AH75" s="15"/>
-      <c r="AI75" s="15"/>
-      <c r="AJ75" s="15"/>
-      <c r="AK75" s="15"/>
-      <c r="AL75" s="15"/>
-      <c r="AM75" s="15"/>
-      <c r="AN75" s="15"/>
-      <c r="AO75" s="15"/>
-      <c r="AP75" s="15"/>
-      <c r="AQ75" s="15"/>
-      <c r="AR75" s="15"/>
-      <c r="AS75" s="15"/>
-      <c r="AT75" s="15"/>
-      <c r="AU75" s="15"/>
-      <c r="AV75" s="15"/>
-      <c r="AW75" s="15"/>
-      <c r="AX75" s="15"/>
-      <c r="AY75" s="15"/>
-      <c r="AZ75" s="15"/>
-      <c r="BA75" s="15"/>
-      <c r="BB75" s="15"/>
-      <c r="BC75" s="15"/>
-      <c r="BD75" s="15"/>
-      <c r="BE75" s="15"/>
-      <c r="BF75" s="15"/>
-      <c r="BG75" s="15"/>
-      <c r="BH75" s="15"/>
-      <c r="BI75" s="15"/>
-      <c r="BJ75" s="15"/>
-      <c r="BK75" s="15"/>
-      <c r="BL75" s="15"/>
-      <c r="BM75" s="15"/>
-      <c r="BN75" s="15"/>
-      <c r="BO75" s="15"/>
-      <c r="BP75" s="15"/>
-      <c r="BQ75" s="15"/>
-      <c r="BR75" s="15"/>
-      <c r="BS75" s="15"/>
-    </row>
-    <row r="76" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B76" s="39"/>
-      <c r="C76" s="50"/>
-      <c r="D76" s="50"/>
+    </row>
+    <row r="76" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" s="38"/>
+      <c r="C76" s="64"/>
+      <c r="D76" s="64"/>
       <c r="E76" s="46"/>
       <c r="F76" s="46"/>
       <c r="G76" s="46"/>
@@ -3450,71 +3381,12 @@
       <c r="J76" s="46"/>
       <c r="K76" s="46"/>
       <c r="L76" s="46"/>
-      <c r="M76" s="15"/>
-      <c r="N76" s="15"/>
-      <c r="O76" s="15"/>
-      <c r="P76" s="15"/>
-      <c r="Q76" s="15"/>
-      <c r="R76" s="15"/>
-      <c r="S76" s="15"/>
-      <c r="T76" s="15"/>
-      <c r="U76" s="15"/>
-      <c r="V76" s="15"/>
-      <c r="W76" s="15"/>
-      <c r="X76" s="15"/>
-      <c r="Y76" s="15"/>
-      <c r="Z76" s="15"/>
-      <c r="AA76" s="15"/>
-      <c r="AB76" s="15"/>
-      <c r="AC76" s="15"/>
-      <c r="AD76" s="15"/>
-      <c r="AE76" s="15"/>
-      <c r="AF76" s="15"/>
-      <c r="AG76" s="15"/>
-      <c r="AH76" s="15"/>
-      <c r="AI76" s="15"/>
-      <c r="AJ76" s="15"/>
-      <c r="AK76" s="15"/>
-      <c r="AL76" s="15"/>
-      <c r="AM76" s="15"/>
-      <c r="AN76" s="15"/>
-      <c r="AO76" s="15"/>
-      <c r="AP76" s="15"/>
-      <c r="AQ76" s="15"/>
-      <c r="AR76" s="15"/>
-      <c r="AS76" s="15"/>
-      <c r="AT76" s="15"/>
-      <c r="AU76" s="15"/>
-      <c r="AV76" s="15"/>
-      <c r="AW76" s="15"/>
-      <c r="AX76" s="15"/>
-      <c r="AY76" s="15"/>
-      <c r="AZ76" s="15"/>
-      <c r="BA76" s="15"/>
-      <c r="BB76" s="15"/>
-      <c r="BC76" s="15"/>
-      <c r="BD76" s="15"/>
-      <c r="BE76" s="15"/>
-      <c r="BF76" s="15"/>
-      <c r="BG76" s="15"/>
-      <c r="BH76" s="15"/>
-      <c r="BI76" s="15"/>
-      <c r="BJ76" s="15"/>
-      <c r="BK76" s="15"/>
-      <c r="BL76" s="15"/>
-      <c r="BM76" s="15"/>
-      <c r="BN76" s="15"/>
-      <c r="BO76" s="15"/>
-      <c r="BP76" s="15"/>
-      <c r="BQ76" s="15"/>
-      <c r="BR76" s="15"/>
-      <c r="BS76" s="15"/>
     </row>
     <row r="77" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A77" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B77" s="40"/>
+      <c r="A77" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77" s="39"/>
       <c r="C77" s="50"/>
       <c r="D77" s="50"/>
       <c r="E77" s="46"/>
@@ -3586,86 +3458,220 @@
       <c r="BS77" s="15"/>
     </row>
     <row r="78" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A78" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B78" s="41"/>
+      <c r="A78" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B78" s="39"/>
       <c r="C78" s="50"/>
       <c r="D78" s="50"/>
+      <c r="E78" s="46"/>
+      <c r="F78" s="46"/>
+      <c r="G78" s="46"/>
+      <c r="H78" s="46"/>
+      <c r="I78" s="46"/>
+      <c r="J78" s="46"/>
+      <c r="K78" s="46"/>
+      <c r="L78" s="46"/>
+      <c r="M78" s="15"/>
+      <c r="N78" s="15"/>
+      <c r="O78" s="15"/>
+      <c r="P78" s="15"/>
+      <c r="Q78" s="15"/>
+      <c r="R78" s="15"/>
+      <c r="S78" s="15"/>
+      <c r="T78" s="15"/>
+      <c r="U78" s="15"/>
+      <c r="V78" s="15"/>
+      <c r="W78" s="15"/>
+      <c r="X78" s="15"/>
+      <c r="Y78" s="15"/>
+      <c r="Z78" s="15"/>
+      <c r="AA78" s="15"/>
+      <c r="AB78" s="15"/>
+      <c r="AC78" s="15"/>
+      <c r="AD78" s="15"/>
+      <c r="AE78" s="15"/>
+      <c r="AF78" s="15"/>
+      <c r="AG78" s="15"/>
+      <c r="AH78" s="15"/>
+      <c r="AI78" s="15"/>
+      <c r="AJ78" s="15"/>
+      <c r="AK78" s="15"/>
+      <c r="AL78" s="15"/>
+      <c r="AM78" s="15"/>
+      <c r="AN78" s="15"/>
+      <c r="AO78" s="15"/>
+      <c r="AP78" s="15"/>
+      <c r="AQ78" s="15"/>
+      <c r="AR78" s="15"/>
+      <c r="AS78" s="15"/>
+      <c r="AT78" s="15"/>
+      <c r="AU78" s="15"/>
+      <c r="AV78" s="15"/>
+      <c r="AW78" s="15"/>
+      <c r="AX78" s="15"/>
+      <c r="AY78" s="15"/>
+      <c r="AZ78" s="15"/>
+      <c r="BA78" s="15"/>
+      <c r="BB78" s="15"/>
+      <c r="BC78" s="15"/>
+      <c r="BD78" s="15"/>
+      <c r="BE78" s="15"/>
+      <c r="BF78" s="15"/>
+      <c r="BG78" s="15"/>
+      <c r="BH78" s="15"/>
+      <c r="BI78" s="15"/>
+      <c r="BJ78" s="15"/>
+      <c r="BK78" s="15"/>
+      <c r="BL78" s="15"/>
+      <c r="BM78" s="15"/>
+      <c r="BN78" s="15"/>
+      <c r="BO78" s="15"/>
+      <c r="BP78" s="15"/>
+      <c r="BQ78" s="15"/>
+      <c r="BR78" s="15"/>
+      <c r="BS78" s="15"/>
     </row>
     <row r="79" spans="1:71" x14ac:dyDescent="0.25">
-      <c r="A79" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B79" s="42"/>
-      <c r="C79" s="65"/>
-      <c r="D79" s="65"/>
+      <c r="A79" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" s="40"/>
+      <c r="C79" s="50"/>
+      <c r="D79" s="50"/>
+      <c r="E79" s="46"/>
+      <c r="F79" s="46"/>
+      <c r="G79" s="46"/>
+      <c r="H79" s="46"/>
+      <c r="I79" s="46"/>
+      <c r="J79" s="46"/>
+      <c r="K79" s="46"/>
+      <c r="L79" s="46"/>
+      <c r="M79" s="15"/>
+      <c r="N79" s="15"/>
+      <c r="O79" s="15"/>
+      <c r="P79" s="15"/>
+      <c r="Q79" s="15"/>
+      <c r="R79" s="15"/>
+      <c r="S79" s="15"/>
+      <c r="T79" s="15"/>
+      <c r="U79" s="15"/>
+      <c r="V79" s="15"/>
+      <c r="W79" s="15"/>
+      <c r="X79" s="15"/>
+      <c r="Y79" s="15"/>
+      <c r="Z79" s="15"/>
+      <c r="AA79" s="15"/>
+      <c r="AB79" s="15"/>
+      <c r="AC79" s="15"/>
+      <c r="AD79" s="15"/>
+      <c r="AE79" s="15"/>
+      <c r="AF79" s="15"/>
+      <c r="AG79" s="15"/>
+      <c r="AH79" s="15"/>
+      <c r="AI79" s="15"/>
+      <c r="AJ79" s="15"/>
+      <c r="AK79" s="15"/>
+      <c r="AL79" s="15"/>
+      <c r="AM79" s="15"/>
+      <c r="AN79" s="15"/>
+      <c r="AO79" s="15"/>
+      <c r="AP79" s="15"/>
+      <c r="AQ79" s="15"/>
+      <c r="AR79" s="15"/>
+      <c r="AS79" s="15"/>
+      <c r="AT79" s="15"/>
+      <c r="AU79" s="15"/>
+      <c r="AV79" s="15"/>
+      <c r="AW79" s="15"/>
+      <c r="AX79" s="15"/>
+      <c r="AY79" s="15"/>
+      <c r="AZ79" s="15"/>
+      <c r="BA79" s="15"/>
+      <c r="BB79" s="15"/>
+      <c r="BC79" s="15"/>
+      <c r="BD79" s="15"/>
+      <c r="BE79" s="15"/>
+      <c r="BF79" s="15"/>
+      <c r="BG79" s="15"/>
+      <c r="BH79" s="15"/>
+      <c r="BI79" s="15"/>
+      <c r="BJ79" s="15"/>
+      <c r="BK79" s="15"/>
+      <c r="BL79" s="15"/>
+      <c r="BM79" s="15"/>
+      <c r="BN79" s="15"/>
+      <c r="BO79" s="15"/>
+      <c r="BP79" s="15"/>
+      <c r="BQ79" s="15"/>
+      <c r="BR79" s="15"/>
+      <c r="BS79" s="15"/>
     </row>
     <row r="80" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B80" s="41"/>
       <c r="C80" s="50"/>
       <c r="D80" s="50"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A81" s="17" t="s">
+      <c r="A81" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B81" s="42"/>
+      <c r="C81" s="65"/>
+      <c r="D81" s="65"/>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B82" s="41"/>
+      <c r="C82" s="50"/>
+      <c r="D82" s="50"/>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B81" s="43"/>
-      <c r="C81" s="43"/>
-      <c r="D81" s="43"/>
-      <c r="E81" s="52"/>
-      <c r="F81" s="52"/>
-      <c r="G81" s="52"/>
-      <c r="H81" s="52"/>
-      <c r="I81" s="52"/>
-      <c r="J81" s="52"/>
-      <c r="K81" s="53"/>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A82" s="16" t="s">
+      <c r="B83" s="43"/>
+      <c r="C83" s="43"/>
+      <c r="D83" s="43"/>
+      <c r="E83" s="52"/>
+      <c r="F83" s="52"/>
+      <c r="G83" s="52"/>
+      <c r="H83" s="52"/>
+      <c r="I83" s="52"/>
+      <c r="J83" s="52"/>
+      <c r="K83" s="53"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B82" s="44">
+      <c r="B84" s="44">
         <v>5</v>
       </c>
-      <c r="C82" s="44">
+      <c r="C84" s="44">
         <v>15</v>
       </c>
-      <c r="D82" s="44"/>
-      <c r="E82" s="44"/>
-      <c r="F82" s="44"/>
-      <c r="G82" s="54"/>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A83" s="18" t="s">
+      <c r="D84" s="44"/>
+      <c r="E84" s="44"/>
+      <c r="F84" s="44"/>
+      <c r="G84" s="54"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B83" s="45"/>
-      <c r="C83" s="50"/>
-      <c r="D83" s="50"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A84" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B84" s="41"/>
-      <c r="C84" s="50"/>
-      <c r="D84" s="50"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B85" s="41"/>
+      <c r="B85" s="45"/>
       <c r="C85" s="50"/>
       <c r="D85" s="50"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B86" s="41"/>
       <c r="C86" s="50"/>
@@ -3673,47 +3679,31 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="B87" s="41"/>
       <c r="C87" s="50"/>
       <c r="D87" s="50"/>
     </row>
-    <row r="88" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="B88" s="41"/>
       <c r="C88" s="50"/>
       <c r="D88" s="50"/>
-      <c r="E88" s="50"/>
-      <c r="F88" s="46"/>
-      <c r="G88" s="46"/>
-      <c r="H88" s="46"/>
-      <c r="I88" s="46"/>
-      <c r="J88" s="46"/>
-      <c r="K88" s="46"/>
-      <c r="L88" s="46"/>
-    </row>
-    <row r="89" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B89" s="41"/>
       <c r="C89" s="50"/>
       <c r="D89" s="50"/>
-      <c r="E89" s="50"/>
-      <c r="F89" s="46"/>
-      <c r="G89" s="46"/>
-      <c r="H89" s="46"/>
-      <c r="I89" s="46"/>
-      <c r="J89" s="46"/>
-      <c r="K89" s="46"/>
-      <c r="L89" s="46"/>
     </row>
     <row r="90" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B90" s="41"/>
       <c r="C90" s="50"/>
@@ -3727,25 +3717,41 @@
       <c r="K90" s="46"/>
       <c r="L90" s="46"/>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B91" s="41"/>
       <c r="C91" s="50"/>
       <c r="D91" s="50"/>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E91" s="50"/>
+      <c r="F91" s="46"/>
+      <c r="G91" s="46"/>
+      <c r="H91" s="46"/>
+      <c r="I91" s="46"/>
+      <c r="J91" s="46"/>
+      <c r="K91" s="46"/>
+      <c r="L91" s="46"/>
+    </row>
+    <row r="92" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="B92" s="41"/>
       <c r="C92" s="50"/>
       <c r="D92" s="50"/>
+      <c r="E92" s="50"/>
+      <c r="F92" s="46"/>
+      <c r="G92" s="46"/>
+      <c r="H92" s="46"/>
+      <c r="I92" s="46"/>
+      <c r="J92" s="46"/>
+      <c r="K92" s="46"/>
+      <c r="L92" s="46"/>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B93" s="41"/>
       <c r="C93" s="50"/>
@@ -3753,7 +3759,7 @@
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>117</v>
+        <v>58</v>
       </c>
       <c r="B94" s="41"/>
       <c r="C94" s="50"/>
@@ -3761,39 +3767,39 @@
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>118</v>
+        <v>59</v>
       </c>
       <c r="B95" s="41"/>
       <c r="C95" s="50"/>
       <c r="D95" s="50"/>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A96" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B96" s="61"/>
+      <c r="A96" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B96" s="41"/>
       <c r="C96" s="50"/>
       <c r="D96" s="50"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="B97" s="59"/>
+      <c r="A97" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B97" s="41"/>
       <c r="C97" s="50"/>
       <c r="D97" s="50"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="56" t="s">
-        <v>95</v>
-      </c>
-      <c r="B98" s="59"/>
+      <c r="A98" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="B98" s="61"/>
       <c r="C98" s="50"/>
       <c r="D98" s="50"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="56" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B99" s="59"/>
       <c r="C99" s="50"/>
@@ -3801,7 +3807,7 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="56" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B100" s="59"/>
       <c r="C100" s="50"/>
@@ -3809,7 +3815,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B101" s="59"/>
       <c r="C101" s="50"/>
@@ -3817,23 +3823,23 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="56" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B102" s="59"/>
       <c r="C102" s="50"/>
       <c r="D102" s="50"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="57" t="s">
-        <v>91</v>
+      <c r="A103" s="56" t="s">
+        <v>97</v>
       </c>
       <c r="B103" s="59"/>
       <c r="C103" s="50"/>
       <c r="D103" s="50"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="57" t="s">
-        <v>99</v>
+      <c r="A104" s="56" t="s">
+        <v>98</v>
       </c>
       <c r="B104" s="59"/>
       <c r="C104" s="50"/>
@@ -3841,7 +3847,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="57" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B105" s="59"/>
       <c r="C105" s="50"/>
@@ -3849,7 +3855,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="57" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B106" s="59"/>
       <c r="C106" s="50"/>
@@ -3857,7 +3863,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="57" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B107" s="59"/>
       <c r="C107" s="50"/>
@@ -3865,7 +3871,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="57" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B108" s="59"/>
       <c r="C108" s="50"/>
@@ -3873,7 +3879,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="57" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B109" s="59"/>
       <c r="C109" s="50"/>
@@ -3881,7 +3887,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B110" s="59"/>
       <c r="C110" s="50"/>
@@ -3889,7 +3895,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="57" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B111" s="59"/>
       <c r="C111" s="50"/>
@@ -3897,7 +3903,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="57" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B112" s="59"/>
       <c r="C112" s="50"/>
@@ -3905,39 +3911,55 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B113" s="59"/>
       <c r="C113" s="50"/>
       <c r="D113" s="50"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="58" t="s">
-        <v>106</v>
-      </c>
-      <c r="B114" s="60"/>
+      <c r="A114" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B114" s="59"/>
       <c r="C114" s="50"/>
       <c r="D114" s="50"/>
     </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="B115" s="59"/>
+      <c r="C115" s="50"/>
+      <c r="D115" s="50"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="B116" s="60"/>
+      <c r="C116" s="50"/>
+      <c r="D116" s="50"/>
+    </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B78:D78 B63:D64">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B80:D80 B65:D66">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B61:D62">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63:D64">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79:D79">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B81:D81">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45:D60">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45:D61 B62:D62">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B81:D81">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83:D83">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3945,7 +3967,7 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B70:D74">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72:D76">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -3959,13 +3981,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B83:D95 B65:D69 B75:D77</xm:sqref>
+          <xm:sqref>B85:D97 B67:D71 B77:D79</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B80:D80</xm:sqref>
+          <xm:sqref>B82:D82</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Enable suppresssion of age calculation plots
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="122">
   <si>
     <t>recent_time</t>
   </si>
@@ -378,6 +378,9 @@
   </si>
   <si>
     <t>plot_start_time</t>
+  </si>
+  <si>
+    <t>output_age_calculations</t>
   </si>
 </sst>
 </file>
@@ -2373,22 +2376,24 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BS116"/>
+  <dimension ref="A1:BP117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.140625" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="25.5703125" style="46" customWidth="1"/>
-    <col min="5" max="6" width="23.28515625" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" style="51" customWidth="1"/>
-    <col min="8" max="12" width="9.140625" style="51"/>
+    <col min="5" max="5" width="23.28515625" style="51" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="51" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="51" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="51" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>17</v>
       </c>
@@ -2398,15 +2403,12 @@
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
       <c r="E1" s="47"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="49"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="48"/>
       <c r="H1" s="49"/>
       <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -2414,9 +2416,10 @@
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
       <c r="E2" s="50"/>
-      <c r="F2" s="46"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F2" s="50"/>
+      <c r="G2" s="46"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -2424,8 +2427,9 @@
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
       <c r="E3" s="50"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F3" s="50"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>65</v>
       </c>
@@ -2433,8 +2437,9 @@
       <c r="C4" s="24"/>
       <c r="D4" s="24"/>
       <c r="E4" s="50"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F4" s="50"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>66</v>
       </c>
@@ -2442,8 +2447,9 @@
       <c r="C5" s="24"/>
       <c r="D5" s="24"/>
       <c r="E5" s="50"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F5" s="50"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>67</v>
       </c>
@@ -2451,8 +2457,9 @@
       <c r="C6" s="24"/>
       <c r="D6" s="24"/>
       <c r="E6" s="50"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F6" s="50"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -2460,8 +2467,9 @@
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
       <c r="E7" s="50"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F7" s="50"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>60</v>
       </c>
@@ -2469,8 +2477,9 @@
       <c r="C8" s="24"/>
       <c r="D8" s="24"/>
       <c r="E8" s="50"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F8" s="50"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>61</v>
       </c>
@@ -2478,8 +2487,9 @@
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
       <c r="E9" s="50"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F9" s="50"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>62</v>
       </c>
@@ -2487,8 +2497,9 @@
       <c r="C10" s="24"/>
       <c r="D10" s="24"/>
       <c r="E10" s="50"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F10" s="50"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -2496,8 +2507,9 @@
       <c r="C11" s="24"/>
       <c r="D11" s="24"/>
       <c r="E11" s="50"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F11" s="50"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -2505,8 +2517,9 @@
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
       <c r="E12" s="50"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F12" s="50"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
@@ -2514,8 +2527,9 @@
       <c r="C13" s="24"/>
       <c r="D13" s="24"/>
       <c r="E13" s="50"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F13" s="50"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
@@ -2523,8 +2537,9 @@
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
       <c r="E14" s="50"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F14" s="50"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -2532,8 +2547,9 @@
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
       <c r="E15" s="50"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F15" s="50"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
@@ -2541,8 +2557,9 @@
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
       <c r="E16" s="50"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="50"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -2550,8 +2567,9 @@
       <c r="C17" s="25"/>
       <c r="D17" s="25"/>
       <c r="E17" s="50"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="50"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
@@ -2559,8 +2577,9 @@
       <c r="C18" s="24"/>
       <c r="D18" s="24"/>
       <c r="E18" s="50"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="50"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
@@ -2568,8 +2587,9 @@
       <c r="C19" s="24"/>
       <c r="D19" s="24"/>
       <c r="E19" s="50"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="50"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
@@ -2577,8 +2597,9 @@
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
       <c r="E20" s="50"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="50"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -2586,8 +2607,9 @@
       <c r="C21" s="24"/>
       <c r="D21" s="24"/>
       <c r="E21" s="50"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="50"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -2595,8 +2617,9 @@
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
       <c r="E22" s="50"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="50"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
@@ -2604,8 +2627,9 @@
       <c r="C23" s="24"/>
       <c r="D23" s="24"/>
       <c r="E23" s="50"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="50"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
@@ -2613,8 +2637,9 @@
       <c r="C24" s="24"/>
       <c r="D24" s="24"/>
       <c r="E24" s="50"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="50"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
@@ -2622,8 +2647,9 @@
       <c r="C25" s="24"/>
       <c r="D25" s="24"/>
       <c r="E25" s="50"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="50"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
@@ -2631,8 +2657,9 @@
       <c r="C26" s="24"/>
       <c r="D26" s="24"/>
       <c r="E26" s="50"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="50"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
@@ -2640,8 +2667,9 @@
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
       <c r="E27" s="50"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="50"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
@@ -2649,8 +2677,9 @@
       <c r="C28" s="24"/>
       <c r="D28" s="24"/>
       <c r="E28" s="50"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="50"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
@@ -2658,8 +2687,9 @@
       <c r="C29" s="24"/>
       <c r="D29" s="24"/>
       <c r="E29" s="50"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="50"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
@@ -2667,8 +2697,9 @@
       <c r="C30" s="24"/>
       <c r="D30" s="24"/>
       <c r="E30" s="50"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="50"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>63</v>
       </c>
@@ -2676,8 +2707,9 @@
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
       <c r="E31" s="50"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="50"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>64</v>
       </c>
@@ -2685,8 +2717,9 @@
       <c r="C32" s="24"/>
       <c r="D32" s="24"/>
       <c r="E32" s="50"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="50"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
@@ -2694,8 +2727,9 @@
       <c r="C33" s="25"/>
       <c r="D33" s="25"/>
       <c r="E33" s="50"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="50"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
@@ -2703,8 +2737,9 @@
       <c r="C34" s="24"/>
       <c r="D34" s="24"/>
       <c r="E34" s="50"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="50"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>48</v>
       </c>
@@ -2712,8 +2747,9 @@
       <c r="C35" s="24"/>
       <c r="D35" s="24"/>
       <c r="E35" s="50"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="50"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>49</v>
       </c>
@@ -2721,8 +2757,9 @@
       <c r="C36" s="24"/>
       <c r="D36" s="24"/>
       <c r="E36" s="50"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="50"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
@@ -2730,8 +2767,9 @@
       <c r="C37" s="26"/>
       <c r="D37" s="26"/>
       <c r="E37" s="50"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="50"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>80</v>
       </c>
@@ -2739,8 +2777,9 @@
       <c r="C38" s="26"/>
       <c r="D38" s="26"/>
       <c r="E38" s="50"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="50"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>84</v>
       </c>
@@ -2748,8 +2787,9 @@
       <c r="C39" s="26"/>
       <c r="D39" s="26"/>
       <c r="E39" s="50"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="50"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>85</v>
       </c>
@@ -2757,8 +2797,9 @@
       <c r="C40" s="26"/>
       <c r="D40" s="26"/>
       <c r="E40" s="50"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40" s="50"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>51</v>
       </c>
@@ -2766,8 +2807,9 @@
       <c r="C41" s="25"/>
       <c r="D41" s="25"/>
       <c r="E41" s="50"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41" s="50"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>116</v>
       </c>
@@ -2775,8 +2817,9 @@
       <c r="C42" s="25"/>
       <c r="D42" s="25"/>
       <c r="E42" s="50"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42" s="50"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>86</v>
       </c>
@@ -2784,8 +2827,9 @@
       <c r="C43" s="27"/>
       <c r="D43" s="27"/>
       <c r="E43" s="50"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43" s="50"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>15</v>
       </c>
@@ -2793,8 +2837,9 @@
       <c r="C44" s="50"/>
       <c r="D44" s="50"/>
       <c r="E44" s="46"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44" s="46"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>52</v>
       </c>
@@ -2802,7 +2847,7 @@
       <c r="C45" s="62"/>
       <c r="D45" s="62"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>82</v>
       </c>
@@ -2810,7 +2855,7 @@
       <c r="C46" s="62"/>
       <c r="D46" s="62"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>13</v>
       </c>
@@ -2818,7 +2863,7 @@
       <c r="C47" s="62"/>
       <c r="D47" s="62"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>14</v>
       </c>
@@ -2954,7 +2999,7 @@
       <c r="C64" s="62"/>
       <c r="D64" s="62"/>
     </row>
-    <row r="65" spans="1:71" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>1</v>
       </c>
@@ -2966,9 +3011,9 @@
       <c r="G65" s="46"/>
       <c r="H65" s="46"/>
       <c r="I65" s="46"/>
-      <c r="J65" s="46"/>
-      <c r="K65" s="46"/>
-      <c r="L65" s="46"/>
+      <c r="J65" s="15"/>
+      <c r="K65" s="15"/>
+      <c r="L65" s="15"/>
       <c r="M65" s="15"/>
       <c r="N65" s="15"/>
       <c r="O65" s="15"/>
@@ -3025,11 +3070,8 @@
       <c r="BN65" s="15"/>
       <c r="BO65" s="15"/>
       <c r="BP65" s="15"/>
-      <c r="BQ65" s="15"/>
-      <c r="BR65" s="15"/>
-      <c r="BS65" s="15"/>
-    </row>
-    <row r="66" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>2</v>
       </c>
@@ -3041,9 +3083,9 @@
       <c r="G66" s="46"/>
       <c r="H66" s="46"/>
       <c r="I66" s="46"/>
-      <c r="J66" s="46"/>
-      <c r="K66" s="46"/>
-      <c r="L66" s="46"/>
+      <c r="J66" s="15"/>
+      <c r="K66" s="15"/>
+      <c r="L66" s="15"/>
       <c r="M66" s="15"/>
       <c r="N66" s="15"/>
       <c r="O66" s="15"/>
@@ -3100,11 +3142,8 @@
       <c r="BN66" s="15"/>
       <c r="BO66" s="15"/>
       <c r="BP66" s="15"/>
-      <c r="BQ66" s="15"/>
-      <c r="BR66" s="15"/>
-      <c r="BS66" s="15"/>
-    </row>
-    <row r="67" spans="1:71" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
         <v>72</v>
       </c>
@@ -3116,9 +3155,9 @@
       <c r="G67" s="46"/>
       <c r="H67" s="46"/>
       <c r="I67" s="46"/>
-      <c r="J67" s="46"/>
-      <c r="K67" s="46"/>
-      <c r="L67" s="46"/>
+      <c r="J67" s="15"/>
+      <c r="K67" s="15"/>
+      <c r="L67" s="15"/>
       <c r="M67" s="15"/>
       <c r="N67" s="15"/>
       <c r="O67" s="15"/>
@@ -3175,11 +3214,8 @@
       <c r="BN67" s="15"/>
       <c r="BO67" s="15"/>
       <c r="BP67" s="15"/>
-      <c r="BQ67" s="15"/>
-      <c r="BR67" s="15"/>
-      <c r="BS67" s="15"/>
-    </row>
-    <row r="68" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>74</v>
       </c>
@@ -3191,11 +3227,8 @@
       <c r="G68" s="46"/>
       <c r="H68" s="46"/>
       <c r="I68" s="46"/>
-      <c r="J68" s="46"/>
-      <c r="K68" s="46"/>
-      <c r="L68" s="46"/>
-    </row>
-    <row r="69" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
         <v>73</v>
       </c>
@@ -3207,11 +3240,8 @@
       <c r="G69" s="46"/>
       <c r="H69" s="46"/>
       <c r="I69" s="46"/>
-      <c r="J69" s="46"/>
-      <c r="K69" s="46"/>
-      <c r="L69" s="46"/>
-    </row>
-    <row r="70" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>71</v>
       </c>
@@ -3223,11 +3253,8 @@
       <c r="G70" s="46"/>
       <c r="H70" s="46"/>
       <c r="I70" s="46"/>
-      <c r="J70" s="46"/>
-      <c r="K70" s="46"/>
-      <c r="L70" s="46"/>
-    </row>
-    <row r="71" spans="1:71" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>70</v>
       </c>
@@ -3239,9 +3266,9 @@
       <c r="G71" s="46"/>
       <c r="H71" s="46"/>
       <c r="I71" s="46"/>
-      <c r="J71" s="46"/>
-      <c r="K71" s="46"/>
-      <c r="L71" s="46"/>
+      <c r="J71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="15"/>
       <c r="M71" s="15"/>
       <c r="N71" s="15"/>
       <c r="O71" s="15"/>
@@ -3298,11 +3325,8 @@
       <c r="BN71" s="15"/>
       <c r="BO71" s="15"/>
       <c r="BP71" s="15"/>
-      <c r="BQ71" s="15"/>
-      <c r="BR71" s="15"/>
-      <c r="BS71" s="15"/>
-    </row>
-    <row r="72" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>75</v>
       </c>
@@ -3314,11 +3338,8 @@
       <c r="G72" s="46"/>
       <c r="H72" s="46"/>
       <c r="I72" s="46"/>
-      <c r="J72" s="46"/>
-      <c r="K72" s="46"/>
-      <c r="L72" s="46"/>
-    </row>
-    <row r="73" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>76</v>
       </c>
@@ -3330,11 +3351,8 @@
       <c r="G73" s="46"/>
       <c r="H73" s="46"/>
       <c r="I73" s="46"/>
-      <c r="J73" s="46"/>
-      <c r="K73" s="46"/>
-      <c r="L73" s="46"/>
-    </row>
-    <row r="74" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>77</v>
       </c>
@@ -3346,11 +3364,8 @@
       <c r="G74" s="46"/>
       <c r="H74" s="46"/>
       <c r="I74" s="46"/>
-      <c r="J74" s="46"/>
-      <c r="K74" s="46"/>
-      <c r="L74" s="46"/>
-    </row>
-    <row r="75" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>78</v>
       </c>
@@ -3362,11 +3377,8 @@
       <c r="G75" s="46"/>
       <c r="H75" s="46"/>
       <c r="I75" s="46"/>
-      <c r="J75" s="46"/>
-      <c r="K75" s="46"/>
-      <c r="L75" s="46"/>
-    </row>
-    <row r="76" spans="1:71" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
         <v>79</v>
       </c>
@@ -3378,11 +3390,8 @@
       <c r="G76" s="46"/>
       <c r="H76" s="46"/>
       <c r="I76" s="46"/>
-      <c r="J76" s="46"/>
-      <c r="K76" s="46"/>
-      <c r="L76" s="46"/>
-    </row>
-    <row r="77" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>3</v>
       </c>
@@ -3394,9 +3403,9 @@
       <c r="G77" s="46"/>
       <c r="H77" s="46"/>
       <c r="I77" s="46"/>
-      <c r="J77" s="46"/>
-      <c r="K77" s="46"/>
-      <c r="L77" s="46"/>
+      <c r="J77" s="15"/>
+      <c r="K77" s="15"/>
+      <c r="L77" s="15"/>
       <c r="M77" s="15"/>
       <c r="N77" s="15"/>
       <c r="O77" s="15"/>
@@ -3453,11 +3462,8 @@
       <c r="BN77" s="15"/>
       <c r="BO77" s="15"/>
       <c r="BP77" s="15"/>
-      <c r="BQ77" s="15"/>
-      <c r="BR77" s="15"/>
-      <c r="BS77" s="15"/>
-    </row>
-    <row r="78" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>4</v>
       </c>
@@ -3469,9 +3475,9 @@
       <c r="G78" s="46"/>
       <c r="H78" s="46"/>
       <c r="I78" s="46"/>
-      <c r="J78" s="46"/>
-      <c r="K78" s="46"/>
-      <c r="L78" s="46"/>
+      <c r="J78" s="15"/>
+      <c r="K78" s="15"/>
+      <c r="L78" s="15"/>
       <c r="M78" s="15"/>
       <c r="N78" s="15"/>
       <c r="O78" s="15"/>
@@ -3528,11 +3534,8 @@
       <c r="BN78" s="15"/>
       <c r="BO78" s="15"/>
       <c r="BP78" s="15"/>
-      <c r="BQ78" s="15"/>
-      <c r="BR78" s="15"/>
-      <c r="BS78" s="15"/>
-    </row>
-    <row r="79" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>5</v>
       </c>
@@ -3544,9 +3547,9 @@
       <c r="G79" s="46"/>
       <c r="H79" s="46"/>
       <c r="I79" s="46"/>
-      <c r="J79" s="46"/>
-      <c r="K79" s="46"/>
-      <c r="L79" s="46"/>
+      <c r="J79" s="15"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="15"/>
       <c r="M79" s="15"/>
       <c r="N79" s="15"/>
       <c r="O79" s="15"/>
@@ -3603,11 +3606,8 @@
       <c r="BN79" s="15"/>
       <c r="BO79" s="15"/>
       <c r="BP79" s="15"/>
-      <c r="BQ79" s="15"/>
-      <c r="BR79" s="15"/>
-      <c r="BS79" s="15"/>
-    </row>
-    <row r="80" spans="1:71" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>9</v>
       </c>
@@ -3615,7 +3615,7 @@
       <c r="C80" s="50"/>
       <c r="D80" s="50"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>16</v>
       </c>
@@ -3623,7 +3623,7 @@
       <c r="C81" s="65"/>
       <c r="D81" s="65"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>7</v>
       </c>
@@ -3631,7 +3631,7 @@
       <c r="C82" s="50"/>
       <c r="D82" s="50"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
         <v>12</v>
       </c>
@@ -3641,12 +3641,9 @@
       <c r="E83" s="52"/>
       <c r="F83" s="52"/>
       <c r="G83" s="52"/>
-      <c r="H83" s="52"/>
-      <c r="I83" s="52"/>
-      <c r="J83" s="52"/>
-      <c r="K83" s="53"/>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H83" s="53"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="16" t="s">
         <v>6</v>
       </c>
@@ -3659,9 +3656,10 @@
       <c r="D84" s="44"/>
       <c r="E84" s="44"/>
       <c r="F84" s="44"/>
-      <c r="G84" s="54"/>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G84" s="44"/>
+      <c r="H84" s="54"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
         <v>55</v>
       </c>
@@ -3669,7 +3667,7 @@
       <c r="C85" s="50"/>
       <c r="D85" s="50"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>112</v>
       </c>
@@ -3677,7 +3675,7 @@
       <c r="C86" s="50"/>
       <c r="D86" s="50"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>107</v>
       </c>
@@ -3685,7 +3683,7 @@
       <c r="C87" s="50"/>
       <c r="D87" s="50"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>108</v>
       </c>
@@ -3693,7 +3691,7 @@
       <c r="C88" s="50"/>
       <c r="D88" s="50"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>56</v>
       </c>
@@ -3701,7 +3699,7 @@
       <c r="C89" s="50"/>
       <c r="D89" s="50"/>
     </row>
-    <row r="90" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>68</v>
       </c>
@@ -3709,15 +3707,12 @@
       <c r="C90" s="50"/>
       <c r="D90" s="50"/>
       <c r="E90" s="50"/>
-      <c r="F90" s="46"/>
+      <c r="F90" s="50"/>
       <c r="G90" s="46"/>
       <c r="H90" s="46"/>
       <c r="I90" s="46"/>
-      <c r="J90" s="46"/>
-      <c r="K90" s="46"/>
-      <c r="L90" s="46"/>
-    </row>
-    <row r="91" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>69</v>
       </c>
@@ -3725,57 +3720,56 @@
       <c r="C91" s="50"/>
       <c r="D91" s="50"/>
       <c r="E91" s="50"/>
-      <c r="F91" s="46"/>
+      <c r="F91" s="50"/>
       <c r="G91" s="46"/>
       <c r="H91" s="46"/>
       <c r="I91" s="46"/>
-      <c r="J91" s="46"/>
-      <c r="K91" s="46"/>
-      <c r="L91" s="46"/>
-    </row>
-    <row r="92" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="B92" s="41"/>
       <c r="C92" s="50"/>
       <c r="D92" s="50"/>
       <c r="E92" s="50"/>
-      <c r="F92" s="46"/>
+      <c r="F92" s="50"/>
       <c r="G92" s="46"/>
       <c r="H92" s="46"/>
       <c r="I92" s="46"/>
-      <c r="J92" s="46"/>
-      <c r="K92" s="46"/>
-      <c r="L92" s="46"/>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="B93" s="41"/>
       <c r="C93" s="50"/>
       <c r="D93" s="50"/>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E93" s="50"/>
+      <c r="F93" s="50"/>
+      <c r="G93" s="46"/>
+      <c r="H93" s="46"/>
+      <c r="I93" s="46"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B94" s="41"/>
       <c r="C94" s="50"/>
       <c r="D94" s="50"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B95" s="41"/>
       <c r="C95" s="50"/>
       <c r="D95" s="50"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>117</v>
+        <v>59</v>
       </c>
       <c r="B96" s="41"/>
       <c r="C96" s="50"/>
@@ -3783,31 +3777,31 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B97" s="41"/>
       <c r="C97" s="50"/>
       <c r="D97" s="50"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B98" s="61"/>
+      <c r="A98" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B98" s="41"/>
       <c r="C98" s="50"/>
       <c r="D98" s="50"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="B99" s="59"/>
+      <c r="A99" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="B99" s="61"/>
       <c r="C99" s="50"/>
       <c r="D99" s="50"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="56" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B100" s="59"/>
       <c r="C100" s="50"/>
@@ -3815,7 +3809,7 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B101" s="59"/>
       <c r="C101" s="50"/>
@@ -3823,7 +3817,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="56" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B102" s="59"/>
       <c r="C102" s="50"/>
@@ -3831,7 +3825,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="56" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B103" s="59"/>
       <c r="C103" s="50"/>
@@ -3839,15 +3833,15 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B104" s="59"/>
       <c r="C104" s="50"/>
       <c r="D104" s="50"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="57" t="s">
-        <v>91</v>
+      <c r="A105" s="56" t="s">
+        <v>98</v>
       </c>
       <c r="B105" s="59"/>
       <c r="C105" s="50"/>
@@ -3855,7 +3849,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="57" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B106" s="59"/>
       <c r="C106" s="50"/>
@@ -3863,7 +3857,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B107" s="59"/>
       <c r="C107" s="50"/>
@@ -3871,7 +3865,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="57" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B108" s="59"/>
       <c r="C108" s="50"/>
@@ -3879,7 +3873,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="57" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B109" s="59"/>
       <c r="C109" s="50"/>
@@ -3887,7 +3881,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B110" s="59"/>
       <c r="C110" s="50"/>
@@ -3895,7 +3889,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="57" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B111" s="59"/>
       <c r="C111" s="50"/>
@@ -3903,7 +3897,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="57" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B112" s="59"/>
       <c r="C112" s="50"/>
@@ -3911,7 +3905,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B113" s="59"/>
       <c r="C113" s="50"/>
@@ -3919,7 +3913,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="57" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B114" s="59"/>
       <c r="C114" s="50"/>
@@ -3927,19 +3921,27 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="57" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B115" s="59"/>
       <c r="C115" s="50"/>
       <c r="D115" s="50"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="58" t="s">
-        <v>106</v>
-      </c>
-      <c r="B116" s="60"/>
+      <c r="A116" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="B116" s="59"/>
       <c r="C116" s="50"/>
       <c r="D116" s="50"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="B117" s="60"/>
+      <c r="C117" s="50"/>
+      <c r="D117" s="50"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
@@ -3981,7 +3983,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B85:D97 B67:D71 B77:D79</xm:sqref>
+          <xm:sqref>B85:D98 B67:D71 B77:D79</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Recalibrated model due to new start age for diabetes
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="615" windowWidth="20370" windowHeight="7230" tabRatio="807"/>
   </bookViews>
@@ -10,7 +15,7 @@
     <sheet name="control_panel" sheetId="4" r:id="rId1"/>
     <sheet name="dropdown_lists" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -2082,6 +2087,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2129,7 +2137,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2164,7 +2172,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2378,7 +2386,7 @@
   </sheetPr>
   <dimension ref="A1:BP117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
       <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
@@ -2813,7 +2821,9 @@
       <c r="A42" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B42" s="25"/>
+      <c r="B42" s="25">
+        <v>40</v>
+      </c>
       <c r="C42" s="25"/>
       <c r="D42" s="25"/>
       <c r="E42" s="50"/>
@@ -2833,7 +2843,9 @@
       <c r="A44" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="28"/>
+      <c r="B44" s="28">
+        <v>0.01</v>
+      </c>
       <c r="C44" s="50"/>
       <c r="D44" s="50"/>
       <c r="E44" s="46"/>
@@ -3258,7 +3270,9 @@
       <c r="A71" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="36"/>
+      <c r="B71" s="36" t="b">
+        <v>1</v>
+      </c>
       <c r="C71" s="62"/>
       <c r="D71" s="62"/>
       <c r="E71" s="46"/>
@@ -3382,7 +3396,9 @@
       <c r="A76" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B76" s="38"/>
+      <c r="B76" s="38">
+        <v>0.17</v>
+      </c>
       <c r="C76" s="64"/>
       <c r="D76" s="64"/>
       <c r="E76" s="46"/>

</xml_diff>

<commit_message>
Re-calibrate model with new diabetes prevalence and age
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2386,8 +2386,8 @@
   </sheetPr>
   <dimension ref="A1:BP117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2822,7 +2822,7 @@
         <v>116</v>
       </c>
       <c r="B42" s="25">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C42" s="25"/>
       <c r="D42" s="25"/>
@@ -3397,7 +3397,7 @@
         <v>79</v>
       </c>
       <c r="B76" s="38">
-        <v>0.17</v>
+        <v>0.156</v>
       </c>
       <c r="C76" s="64"/>
       <c r="D76" s="64"/>
@@ -3669,7 +3669,9 @@
       <c r="C84" s="44">
         <v>15</v>
       </c>
-      <c r="D84" s="44"/>
+      <c r="D84" s="44">
+        <v>25</v>
+      </c>
       <c r="E84" s="44"/>
       <c r="F84" s="44"/>
       <c r="G84" s="44"/>
@@ -3679,7 +3681,9 @@
       <c r="A85" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B85" s="45"/>
+      <c r="B85" s="45" t="b">
+        <v>1</v>
+      </c>
       <c r="C85" s="50"/>
       <c r="D85" s="50"/>
     </row>

</xml_diff>

<commit_message>
Cost-coverage curve plots tidying
Should be enough for Tan to look at now.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="615" windowWidth="20370" windowHeight="7230" tabRatio="807"/>
   </bookViews>
@@ -15,12 +10,12 @@
     <sheet name="control_panel" sheetId="4" r:id="rId1"/>
     <sheet name="dropdown_lists" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="123">
   <si>
     <t>recent_time</t>
   </si>
@@ -386,6 +381,9 @@
   </si>
   <si>
     <t>output_age_calculations</t>
+  </si>
+  <si>
+    <t>output_plot_economics</t>
   </si>
 </sst>
 </file>
@@ -2137,7 +2135,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2172,7 +2170,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2384,9 +2382,9 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP117"/>
+  <dimension ref="A1:BP118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
@@ -3681,9 +3679,7 @@
       <c r="A85" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B85" s="45" t="b">
-        <v>1</v>
-      </c>
+      <c r="B85" s="45"/>
       <c r="C85" s="50"/>
       <c r="D85" s="50"/>
     </row>
@@ -3797,7 +3793,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B97" s="41"/>
       <c r="C97" s="50"/>
@@ -3805,31 +3801,31 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B98" s="41"/>
       <c r="C98" s="50"/>
       <c r="D98" s="50"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B99" s="61"/>
+      <c r="A99" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B99" s="41"/>
       <c r="C99" s="50"/>
       <c r="D99" s="50"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="B100" s="59"/>
+      <c r="A100" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="B100" s="61"/>
       <c r="C100" s="50"/>
       <c r="D100" s="50"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="56" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B101" s="59"/>
       <c r="C101" s="50"/>
@@ -3837,7 +3833,7 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="56" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B102" s="59"/>
       <c r="C102" s="50"/>
@@ -3845,7 +3841,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="56" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B103" s="59"/>
       <c r="C103" s="50"/>
@@ -3853,7 +3849,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="56" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B104" s="59"/>
       <c r="C104" s="50"/>
@@ -3861,15 +3857,15 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B105" s="59"/>
       <c r="C105" s="50"/>
       <c r="D105" s="50"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="57" t="s">
-        <v>91</v>
+      <c r="A106" s="56" t="s">
+        <v>98</v>
       </c>
       <c r="B106" s="59"/>
       <c r="C106" s="50"/>
@@ -3877,7 +3873,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="57" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B107" s="59"/>
       <c r="C107" s="50"/>
@@ -3885,7 +3881,7 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="57" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B108" s="59"/>
       <c r="C108" s="50"/>
@@ -3893,7 +3889,7 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="57" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B109" s="59"/>
       <c r="C109" s="50"/>
@@ -3901,7 +3897,7 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="57" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B110" s="59"/>
       <c r="C110" s="50"/>
@@ -3909,7 +3905,7 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="57" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B111" s="59"/>
       <c r="C111" s="50"/>
@@ -3917,7 +3913,7 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="57" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B112" s="59"/>
       <c r="C112" s="50"/>
@@ -3925,7 +3921,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="57" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B113" s="59"/>
       <c r="C113" s="50"/>
@@ -3933,7 +3929,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B114" s="59"/>
       <c r="C114" s="50"/>
@@ -3941,7 +3937,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="57" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B115" s="59"/>
       <c r="C115" s="50"/>
@@ -3949,19 +3945,27 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="57" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B116" s="59"/>
       <c r="C116" s="50"/>
       <c r="D116" s="50"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="58" t="s">
-        <v>106</v>
-      </c>
-      <c r="B117" s="60"/>
+      <c r="A117" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="B117" s="59"/>
       <c r="C117" s="50"/>
       <c r="D117" s="50"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="B118" s="60"/>
+      <c r="C118" s="50"/>
+      <c r="D118" s="50"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
@@ -4003,7 +4007,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B85:D98 B67:D71 B77:D79</xm:sqref>
+          <xm:sqref>B85:D99 B67:D71 B77:D79</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Update clibration - minor changes to Romain's values
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="615" windowWidth="20370" windowHeight="7230" tabRatio="807"/>
   </bookViews>
@@ -2135,7 +2140,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2170,7 +2175,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2384,8 +2389,8 @@
   </sheetPr>
   <dimension ref="A1:BP118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2949,7 +2954,9 @@
       <c r="A57" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B57" s="29"/>
+      <c r="B57" s="29">
+        <v>1865</v>
+      </c>
       <c r="C57" s="62"/>
       <c r="D57" s="62"/>
     </row>
@@ -2957,7 +2964,9 @@
       <c r="A58" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B58" s="29"/>
+      <c r="B58" s="29">
+        <v>2036</v>
+      </c>
       <c r="C58" s="62"/>
       <c r="D58" s="62"/>
     </row>
@@ -2965,7 +2974,9 @@
       <c r="A59" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B59" s="29"/>
+      <c r="B59" s="29">
+        <v>1</v>
+      </c>
       <c r="C59" s="62"/>
       <c r="D59" s="62"/>
     </row>
@@ -3679,7 +3690,9 @@
       <c r="A85" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B85" s="45"/>
+      <c r="B85" s="45" t="b">
+        <v>1</v>
+      </c>
       <c r="C85" s="50"/>
       <c r="D85" s="50"/>
     </row>

</xml_diff>

<commit_message>
Update spreadsheets for starting costs
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN_new\AuTuMN\autumn\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="615" windowWidth="20370" windowHeight="7230" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="612" windowWidth="20376" windowHeight="7236" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="control_panel" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="128">
   <si>
     <t>recent_time</t>
   </si>
@@ -389,6 +389,21 @@
   </si>
   <si>
     <t>output_plot_economics</t>
+  </si>
+  <si>
+    <t>econ_sartingcost_duration_vaccination</t>
+  </si>
+  <si>
+    <t>econ_sartingcost_duration_ipt</t>
+  </si>
+  <si>
+    <t>econ_sartingcost_duration_xpert</t>
+  </si>
+  <si>
+    <t>econ_sartingcost_duration_treatment_support</t>
+  </si>
+  <si>
+    <t>econ_sartingcost_duration_xpertacf</t>
   </si>
 </sst>
 </file>
@@ -2387,24 +2402,24 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP118"/>
+  <dimension ref="A1:BP123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="52.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="25.5703125" style="46" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="51" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="51" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="51" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="51" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="51"/>
+    <col min="1" max="1" width="52.109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="25.5546875" style="46" customWidth="1"/>
+    <col min="5" max="5" width="23.33203125" style="51" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" style="51" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" style="51" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" style="51" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>17</v>
       </c>
@@ -2419,7 +2434,7 @@
       <c r="H1" s="49"/>
       <c r="I1" s="49"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -2430,7 +2445,7 @@
       <c r="F2" s="50"/>
       <c r="G2" s="46"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -2440,7 +2455,7 @@
       <c r="E3" s="50"/>
       <c r="F3" s="50"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>65</v>
       </c>
@@ -2450,7 +2465,7 @@
       <c r="E4" s="50"/>
       <c r="F4" s="50"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>66</v>
       </c>
@@ -2460,7 +2475,7 @@
       <c r="E5" s="50"/>
       <c r="F5" s="50"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>67</v>
       </c>
@@ -2470,7 +2485,7 @@
       <c r="E6" s="50"/>
       <c r="F6" s="50"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -2480,7 +2495,7 @@
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>60</v>
       </c>
@@ -2490,7 +2505,7 @@
       <c r="E8" s="50"/>
       <c r="F8" s="50"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>61</v>
       </c>
@@ -2500,7 +2515,7 @@
       <c r="E9" s="50"/>
       <c r="F9" s="50"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>62</v>
       </c>
@@ -2510,7 +2525,7 @@
       <c r="E10" s="50"/>
       <c r="F10" s="50"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -2520,7 +2535,7 @@
       <c r="E11" s="50"/>
       <c r="F11" s="50"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -2530,7 +2545,7 @@
       <c r="E12" s="50"/>
       <c r="F12" s="50"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
@@ -2540,7 +2555,7 @@
       <c r="E13" s="50"/>
       <c r="F13" s="50"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
@@ -2550,7 +2565,7 @@
       <c r="E14" s="50"/>
       <c r="F14" s="50"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -2560,7 +2575,7 @@
       <c r="E15" s="50"/>
       <c r="F15" s="50"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
@@ -2570,7 +2585,7 @@
       <c r="E16" s="50"/>
       <c r="F16" s="50"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -2580,7 +2595,7 @@
       <c r="E17" s="50"/>
       <c r="F17" s="50"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
@@ -2590,7 +2605,7 @@
       <c r="E18" s="50"/>
       <c r="F18" s="50"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
@@ -2600,7 +2615,7 @@
       <c r="E19" s="50"/>
       <c r="F19" s="50"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
@@ -2610,7 +2625,7 @@
       <c r="E20" s="50"/>
       <c r="F20" s="50"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -2620,7 +2635,7 @@
       <c r="E21" s="50"/>
       <c r="F21" s="50"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -2630,7 +2645,7 @@
       <c r="E22" s="50"/>
       <c r="F22" s="50"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
@@ -2640,7 +2655,7 @@
       <c r="E23" s="50"/>
       <c r="F23" s="50"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
@@ -2650,7 +2665,7 @@
       <c r="E24" s="50"/>
       <c r="F24" s="50"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
@@ -2660,7 +2675,7 @@
       <c r="E25" s="50"/>
       <c r="F25" s="50"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
@@ -2670,7 +2685,7 @@
       <c r="E26" s="50"/>
       <c r="F26" s="50"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
@@ -2680,7 +2695,7 @@
       <c r="E27" s="50"/>
       <c r="F27" s="50"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
@@ -2690,7 +2705,7 @@
       <c r="E28" s="50"/>
       <c r="F28" s="50"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
@@ -2700,7 +2715,7 @@
       <c r="E29" s="50"/>
       <c r="F29" s="50"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
@@ -2710,7 +2725,7 @@
       <c r="E30" s="50"/>
       <c r="F30" s="50"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>63</v>
       </c>
@@ -2720,7 +2735,7 @@
       <c r="E31" s="50"/>
       <c r="F31" s="50"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>64</v>
       </c>
@@ -2730,7 +2745,7 @@
       <c r="E32" s="50"/>
       <c r="F32" s="50"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
@@ -2740,7 +2755,7 @@
       <c r="E33" s="50"/>
       <c r="F33" s="50"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
@@ -2750,7 +2765,7 @@
       <c r="E34" s="50"/>
       <c r="F34" s="50"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>48</v>
       </c>
@@ -2760,7 +2775,7 @@
       <c r="E35" s="50"/>
       <c r="F35" s="50"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>49</v>
       </c>
@@ -2770,7 +2785,7 @@
       <c r="E36" s="50"/>
       <c r="F36" s="50"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
@@ -2780,7 +2795,7 @@
       <c r="E37" s="50"/>
       <c r="F37" s="50"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>80</v>
       </c>
@@ -2790,7 +2805,7 @@
       <c r="E38" s="50"/>
       <c r="F38" s="50"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>84</v>
       </c>
@@ -2800,7 +2815,7 @@
       <c r="E39" s="50"/>
       <c r="F39" s="50"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>85</v>
       </c>
@@ -2810,7 +2825,7 @@
       <c r="E40" s="50"/>
       <c r="F40" s="50"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>51</v>
       </c>
@@ -2820,7 +2835,7 @@
       <c r="E41" s="50"/>
       <c r="F41" s="50"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>116</v>
       </c>
@@ -2832,7 +2847,7 @@
       <c r="E42" s="50"/>
       <c r="F42" s="50"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>86</v>
       </c>
@@ -2842,19 +2857,19 @@
       <c r="E43" s="50"/>
       <c r="F43" s="50"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B44" s="28">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="C44" s="50"/>
       <c r="D44" s="50"/>
       <c r="E44" s="46"/>
       <c r="F44" s="46"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>52</v>
       </c>
@@ -2862,7 +2877,7 @@
       <c r="C45" s="62"/>
       <c r="D45" s="62"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>82</v>
       </c>
@@ -2870,7 +2885,7 @@
       <c r="C46" s="62"/>
       <c r="D46" s="62"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>13</v>
       </c>
@@ -2878,7 +2893,7 @@
       <c r="C47" s="62"/>
       <c r="D47" s="62"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>14</v>
       </c>
@@ -2886,7 +2901,7 @@
       <c r="C48" s="62"/>
       <c r="D48" s="62"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="s">
         <v>113</v>
       </c>
@@ -2894,7 +2909,7 @@
       <c r="C49" s="63"/>
       <c r="D49" s="63"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="s">
         <v>114</v>
       </c>
@@ -2902,7 +2917,7 @@
       <c r="C50" s="63"/>
       <c r="D50" s="63"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="s">
         <v>115</v>
       </c>
@@ -2910,7 +2925,7 @@
       <c r="C51" s="63"/>
       <c r="D51" s="63"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
         <v>0</v>
       </c>
@@ -2918,7 +2933,7 @@
       <c r="C52" s="62"/>
       <c r="D52" s="62"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
         <v>11</v>
       </c>
@@ -2926,7 +2941,7 @@
       <c r="C53" s="62"/>
       <c r="D53" s="62"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>13</v>
       </c>
@@ -2934,7 +2949,7 @@
       <c r="C54" s="62"/>
       <c r="D54" s="62"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>14</v>
       </c>
@@ -2942,7 +2957,7 @@
       <c r="C55" s="62"/>
       <c r="D55" s="62"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>10</v>
       </c>
@@ -2950,7 +2965,7 @@
       <c r="C56" s="62"/>
       <c r="D56" s="62"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
         <v>109</v>
       </c>
@@ -2960,7 +2975,7 @@
       <c r="C57" s="62"/>
       <c r="D57" s="62"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
         <v>110</v>
       </c>
@@ -2970,7 +2985,7 @@
       <c r="C58" s="62"/>
       <c r="D58" s="62"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
         <v>111</v>
       </c>
@@ -2980,7 +2995,7 @@
       <c r="C59" s="62"/>
       <c r="D59" s="62"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
         <v>120</v>
       </c>
@@ -2988,7 +3003,7 @@
       <c r="C60" s="62"/>
       <c r="D60" s="62"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
         <v>119</v>
       </c>
@@ -2996,7 +3011,7 @@
       <c r="C61" s="62"/>
       <c r="D61" s="62"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
         <v>87</v>
       </c>
@@ -3004,7 +3019,7 @@
       <c r="C62" s="62"/>
       <c r="D62" s="62"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="9" t="s">
         <v>53</v>
       </c>
@@ -3012,7 +3027,7 @@
       <c r="C63" s="62"/>
       <c r="D63" s="62"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
         <v>54</v>
       </c>
@@ -3020,7 +3035,7 @@
       <c r="C64" s="62"/>
       <c r="D64" s="62"/>
     </row>
-    <row r="65" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A65" s="11" t="s">
         <v>1</v>
       </c>
@@ -3092,7 +3107,7 @@
       <c r="BO65" s="15"/>
       <c r="BP65" s="15"/>
     </row>
-    <row r="66" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A66" s="11" t="s">
         <v>2</v>
       </c>
@@ -3164,7 +3179,7 @@
       <c r="BO66" s="15"/>
       <c r="BP66" s="15"/>
     </row>
-    <row r="67" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="21" t="s">
         <v>72</v>
       </c>
@@ -3236,7 +3251,7 @@
       <c r="BO67" s="15"/>
       <c r="BP67" s="15"/>
     </row>
-    <row r="68" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="11" t="s">
         <v>74</v>
       </c>
@@ -3249,7 +3264,7 @@
       <c r="H68" s="46"/>
       <c r="I68" s="46"/>
     </row>
-    <row r="69" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="11" t="s">
         <v>73</v>
       </c>
@@ -3262,7 +3277,7 @@
       <c r="H69" s="46"/>
       <c r="I69" s="46"/>
     </row>
-    <row r="70" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="11" t="s">
         <v>71</v>
       </c>
@@ -3275,7 +3290,7 @@
       <c r="H70" s="46"/>
       <c r="I70" s="46"/>
     </row>
-    <row r="71" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A71" s="12" t="s">
         <v>70</v>
       </c>
@@ -3349,7 +3364,7 @@
       <c r="BO71" s="15"/>
       <c r="BP71" s="15"/>
     </row>
-    <row r="72" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A72" s="11" t="s">
         <v>75</v>
       </c>
@@ -3362,7 +3377,7 @@
       <c r="H72" s="46"/>
       <c r="I72" s="46"/>
     </row>
-    <row r="73" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="11" t="s">
         <v>76</v>
       </c>
@@ -3375,7 +3390,7 @@
       <c r="H73" s="46"/>
       <c r="I73" s="46"/>
     </row>
-    <row r="74" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A74" s="11" t="s">
         <v>77</v>
       </c>
@@ -3388,7 +3403,7 @@
       <c r="H74" s="46"/>
       <c r="I74" s="46"/>
     </row>
-    <row r="75" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A75" s="11" t="s">
         <v>78</v>
       </c>
@@ -3401,7 +3416,7 @@
       <c r="H75" s="46"/>
       <c r="I75" s="46"/>
     </row>
-    <row r="76" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="12" t="s">
         <v>79</v>
       </c>
@@ -3416,7 +3431,7 @@
       <c r="H76" s="46"/>
       <c r="I76" s="46"/>
     </row>
-    <row r="77" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A77" s="11" t="s">
         <v>3</v>
       </c>
@@ -3488,7 +3503,7 @@
       <c r="BO77" s="15"/>
       <c r="BP77" s="15"/>
     </row>
-    <row r="78" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A78" s="11" t="s">
         <v>4</v>
       </c>
@@ -3560,7 +3575,7 @@
       <c r="BO78" s="15"/>
       <c r="BP78" s="15"/>
     </row>
-    <row r="79" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A79" s="12" t="s">
         <v>5</v>
       </c>
@@ -3632,7 +3647,7 @@
       <c r="BO79" s="15"/>
       <c r="BP79" s="15"/>
     </row>
-    <row r="80" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:68" x14ac:dyDescent="0.3">
       <c r="A80" s="13" t="s">
         <v>9</v>
       </c>
@@ -3640,7 +3655,7 @@
       <c r="C80" s="50"/>
       <c r="D80" s="50"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="13" t="s">
         <v>16</v>
       </c>
@@ -3648,7 +3663,7 @@
       <c r="C81" s="65"/>
       <c r="D81" s="65"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="13" t="s">
         <v>7</v>
       </c>
@@ -3656,11 +3671,13 @@
       <c r="C82" s="50"/>
       <c r="D82" s="50"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B83" s="43"/>
+      <c r="B83" s="43">
+        <v>2</v>
+      </c>
       <c r="C83" s="43"/>
       <c r="D83" s="43"/>
       <c r="E83" s="52"/>
@@ -3668,35 +3685,29 @@
       <c r="G83" s="52"/>
       <c r="H83" s="53"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B84" s="44">
-        <v>5</v>
-      </c>
-      <c r="C84" s="44">
-        <v>15</v>
-      </c>
-      <c r="D84" s="44">
-        <v>25</v>
-      </c>
+      <c r="B84" s="44"/>
+      <c r="C84" s="44"/>
+      <c r="D84" s="44"/>
       <c r="E84" s="44"/>
       <c r="F84" s="44"/>
       <c r="G84" s="44"/>
       <c r="H84" s="54"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="18" t="s">
         <v>55</v>
       </c>
       <c r="B85" s="45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C85" s="50"/>
       <c r="D85" s="50"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="13" t="s">
         <v>112</v>
       </c>
@@ -3704,7 +3715,7 @@
       <c r="C86" s="50"/>
       <c r="D86" s="50"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="13" t="s">
         <v>107</v>
       </c>
@@ -3712,7 +3723,7 @@
       <c r="C87" s="50"/>
       <c r="D87" s="50"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="13" t="s">
         <v>108</v>
       </c>
@@ -3720,7 +3731,7 @@
       <c r="C88" s="50"/>
       <c r="D88" s="50"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="13" t="s">
         <v>56</v>
       </c>
@@ -3728,7 +3739,7 @@
       <c r="C89" s="50"/>
       <c r="D89" s="50"/>
     </row>
-    <row r="90" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90" s="13" t="s">
         <v>68</v>
       </c>
@@ -3741,7 +3752,7 @@
       <c r="H90" s="46"/>
       <c r="I90" s="46"/>
     </row>
-    <row r="91" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91" s="13" t="s">
         <v>69</v>
       </c>
@@ -3754,7 +3765,7 @@
       <c r="H91" s="46"/>
       <c r="I91" s="46"/>
     </row>
-    <row r="92" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A92" s="13" t="s">
         <v>121</v>
       </c>
@@ -3767,7 +3778,7 @@
       <c r="H92" s="46"/>
       <c r="I92" s="46"/>
     </row>
-    <row r="93" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A93" s="13" t="s">
         <v>83</v>
       </c>
@@ -3780,7 +3791,7 @@
       <c r="H93" s="46"/>
       <c r="I93" s="46"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="13" t="s">
         <v>57</v>
       </c>
@@ -3788,7 +3799,7 @@
       <c r="C94" s="50"/>
       <c r="D94" s="50"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="13" t="s">
         <v>58</v>
       </c>
@@ -3796,7 +3807,7 @@
       <c r="C95" s="50"/>
       <c r="D95" s="50"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="13" t="s">
         <v>59</v>
       </c>
@@ -3804,7 +3815,7 @@
       <c r="C96" s="50"/>
       <c r="D96" s="50"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="13" t="s">
         <v>122</v>
       </c>
@@ -3812,7 +3823,7 @@
       <c r="C97" s="50"/>
       <c r="D97" s="50"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
         <v>117</v>
       </c>
@@ -3820,7 +3831,7 @@
       <c r="C98" s="50"/>
       <c r="D98" s="50"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
         <v>118</v>
       </c>
@@ -3828,7 +3839,7 @@
       <c r="C99" s="50"/>
       <c r="D99" s="50"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" s="55" t="s">
         <v>88</v>
       </c>
@@ -3836,7 +3847,7 @@
       <c r="C100" s="50"/>
       <c r="D100" s="50"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="56" t="s">
         <v>89</v>
       </c>
@@ -3844,7 +3855,7 @@
       <c r="C101" s="50"/>
       <c r="D101" s="50"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="56" t="s">
         <v>95</v>
       </c>
@@ -3852,133 +3863,163 @@
       <c r="C102" s="50"/>
       <c r="D102" s="50"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="56" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="B103" s="59"/>
       <c r="C103" s="50"/>
       <c r="D103" s="50"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" s="56" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B104" s="59"/>
       <c r="C104" s="50"/>
       <c r="D104" s="50"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="56" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B105" s="59"/>
       <c r="C105" s="50"/>
       <c r="D105" s="50"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="56" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B106" s="59"/>
       <c r="C106" s="50"/>
       <c r="D106" s="50"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="57" t="s">
-        <v>91</v>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="56" t="s">
+        <v>124</v>
       </c>
       <c r="B107" s="59"/>
       <c r="C107" s="50"/>
       <c r="D107" s="50"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="57" t="s">
-        <v>99</v>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="56" t="s">
+        <v>98</v>
       </c>
       <c r="B108" s="59"/>
       <c r="C108" s="50"/>
       <c r="D108" s="50"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="57" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B109" s="59"/>
       <c r="C109" s="50"/>
       <c r="D109" s="50"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="57" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B110" s="59"/>
       <c r="C110" s="50"/>
       <c r="D110" s="50"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="57" t="s">
-        <v>101</v>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="56" t="s">
+        <v>125</v>
       </c>
       <c r="B111" s="59"/>
       <c r="C111" s="50"/>
       <c r="D111" s="50"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="57" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B112" s="59"/>
       <c r="C112" s="50"/>
       <c r="D112" s="50"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="57" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B113" s="59"/>
       <c r="C113" s="50"/>
       <c r="D113" s="50"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="57" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B114" s="59"/>
       <c r="C114" s="50"/>
       <c r="D114" s="50"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="57" t="s">
-        <v>104</v>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="56" t="s">
+        <v>126</v>
       </c>
       <c r="B115" s="59"/>
       <c r="C115" s="50"/>
       <c r="D115" s="50"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="57" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="B116" s="59"/>
       <c r="C116" s="50"/>
       <c r="D116" s="50"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="57" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B117" s="59"/>
       <c r="C117" s="50"/>
       <c r="D117" s="50"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="58" t="s">
-        <v>106</v>
-      </c>
-      <c r="B118" s="60"/>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="B118" s="59"/>
       <c r="C118" s="50"/>
       <c r="D118" s="50"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="B119" s="59"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B120" s="59"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="B121" s="59"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="B122" s="59"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="B123" s="60"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
@@ -3994,7 +4035,7 @@
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45:D61 B62:D62">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45:D62">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
@@ -4045,9 +4086,9 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -4058,7 +4099,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -4069,7 +4110,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>

</xml_diff>

<commit_message>
Enable freezing of times
Can specify a year for a scenario at which the input data is frozen.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rragonnet\Google Drive\GitHub\AuTuMN_new\AuTuMN\autumn\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="612" windowWidth="20376" windowHeight="7236" tabRatio="807"/>
+    <workbookView xWindow="120" yWindow="615" windowWidth="20370" windowHeight="7230" tabRatio="807"/>
   </bookViews>
   <sheets>
     <sheet name="control_panel" sheetId="4" r:id="rId1"/>
@@ -2158,7 +2153,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2193,7 +2188,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2407,22 +2402,22 @@
   </sheetPr>
   <dimension ref="A1:BP124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="25.5546875" style="46" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" style="51" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" style="51" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" style="51" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" style="51" customWidth="1"/>
-    <col min="9" max="9" width="9.109375" style="51"/>
+    <col min="1" max="1" width="52.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="25.5703125" style="46" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="51" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="51" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="51" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="51" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="51"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>17</v>
       </c>
@@ -2437,7 +2432,7 @@
       <c r="H1" s="49"/>
       <c r="I1" s="49"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
@@ -2448,7 +2443,7 @@
       <c r="F2" s="50"/>
       <c r="G2" s="46"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
@@ -2458,7 +2453,7 @@
       <c r="E3" s="50"/>
       <c r="F3" s="50"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>65</v>
       </c>
@@ -2468,7 +2463,7 @@
       <c r="E4" s="50"/>
       <c r="F4" s="50"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>66</v>
       </c>
@@ -2478,7 +2473,7 @@
       <c r="E5" s="50"/>
       <c r="F5" s="50"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>67</v>
       </c>
@@ -2488,7 +2483,7 @@
       <c r="E6" s="50"/>
       <c r="F6" s="50"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
@@ -2498,7 +2493,7 @@
       <c r="E7" s="50"/>
       <c r="F7" s="50"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>60</v>
       </c>
@@ -2508,7 +2503,7 @@
       <c r="E8" s="50"/>
       <c r="F8" s="50"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>61</v>
       </c>
@@ -2518,7 +2513,7 @@
       <c r="E9" s="50"/>
       <c r="F9" s="50"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>62</v>
       </c>
@@ -2528,7 +2523,7 @@
       <c r="E10" s="50"/>
       <c r="F10" s="50"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
@@ -2538,7 +2533,7 @@
       <c r="E11" s="50"/>
       <c r="F11" s="50"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -2548,7 +2543,7 @@
       <c r="E12" s="50"/>
       <c r="F12" s="50"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
@@ -2558,7 +2553,7 @@
       <c r="E13" s="50"/>
       <c r="F13" s="50"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
@@ -2568,7 +2563,7 @@
       <c r="E14" s="50"/>
       <c r="F14" s="50"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -2578,7 +2573,7 @@
       <c r="E15" s="50"/>
       <c r="F15" s="50"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
@@ -2588,7 +2583,7 @@
       <c r="E16" s="50"/>
       <c r="F16" s="50"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
@@ -2598,7 +2593,7 @@
       <c r="E17" s="50"/>
       <c r="F17" s="50"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
@@ -2608,7 +2603,7 @@
       <c r="E18" s="50"/>
       <c r="F18" s="50"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
@@ -2618,7 +2613,7 @@
       <c r="E19" s="50"/>
       <c r="F19" s="50"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
@@ -2628,7 +2623,7 @@
       <c r="E20" s="50"/>
       <c r="F20" s="50"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
@@ -2638,7 +2633,7 @@
       <c r="E21" s="50"/>
       <c r="F21" s="50"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
@@ -2648,7 +2643,7 @@
       <c r="E22" s="50"/>
       <c r="F22" s="50"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
@@ -2658,7 +2653,7 @@
       <c r="E23" s="50"/>
       <c r="F23" s="50"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
@@ -2668,7 +2663,7 @@
       <c r="E24" s="50"/>
       <c r="F24" s="50"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
@@ -2678,7 +2673,7 @@
       <c r="E25" s="50"/>
       <c r="F25" s="50"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
@@ -2688,7 +2683,7 @@
       <c r="E26" s="50"/>
       <c r="F26" s="50"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
@@ -2698,7 +2693,7 @@
       <c r="E27" s="50"/>
       <c r="F27" s="50"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
@@ -2708,7 +2703,7 @@
       <c r="E28" s="50"/>
       <c r="F28" s="50"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
@@ -2718,7 +2713,7 @@
       <c r="E29" s="50"/>
       <c r="F29" s="50"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
@@ -2728,7 +2723,7 @@
       <c r="E30" s="50"/>
       <c r="F30" s="50"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>63</v>
       </c>
@@ -2738,7 +2733,7 @@
       <c r="E31" s="50"/>
       <c r="F31" s="50"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>64</v>
       </c>
@@ -2748,7 +2743,7 @@
       <c r="E32" s="50"/>
       <c r="F32" s="50"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
@@ -2758,7 +2753,7 @@
       <c r="E33" s="50"/>
       <c r="F33" s="50"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
@@ -2768,7 +2763,7 @@
       <c r="E34" s="50"/>
       <c r="F34" s="50"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>48</v>
       </c>
@@ -2778,7 +2773,7 @@
       <c r="E35" s="50"/>
       <c r="F35" s="50"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>49</v>
       </c>
@@ -2788,7 +2783,7 @@
       <c r="E36" s="50"/>
       <c r="F36" s="50"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
@@ -2798,7 +2793,7 @@
       <c r="E37" s="50"/>
       <c r="F37" s="50"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>80</v>
       </c>
@@ -2808,7 +2803,7 @@
       <c r="E38" s="50"/>
       <c r="F38" s="50"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>84</v>
       </c>
@@ -2818,7 +2813,7 @@
       <c r="E39" s="50"/>
       <c r="F39" s="50"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>85</v>
       </c>
@@ -2828,7 +2823,7 @@
       <c r="E40" s="50"/>
       <c r="F40" s="50"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>51</v>
       </c>
@@ -2838,7 +2833,7 @@
       <c r="E41" s="50"/>
       <c r="F41" s="50"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>116</v>
       </c>
@@ -2850,7 +2845,7 @@
       <c r="E42" s="50"/>
       <c r="F42" s="50"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
         <v>86</v>
       </c>
@@ -2860,7 +2855,7 @@
       <c r="E43" s="50"/>
       <c r="F43" s="50"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>15</v>
       </c>
@@ -2872,7 +2867,7 @@
       <c r="E44" s="46"/>
       <c r="F44" s="46"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>52</v>
       </c>
@@ -2880,7 +2875,7 @@
       <c r="C45" s="62"/>
       <c r="D45" s="62"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>82</v>
       </c>
@@ -2888,7 +2883,7 @@
       <c r="C46" s="62"/>
       <c r="D46" s="62"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
         <v>13</v>
       </c>
@@ -2896,7 +2891,7 @@
       <c r="C47" s="62"/>
       <c r="D47" s="62"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>14</v>
       </c>
@@ -2904,7 +2899,7 @@
       <c r="C48" s="62"/>
       <c r="D48" s="62"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>113</v>
       </c>
@@ -2912,7 +2907,7 @@
       <c r="C49" s="63"/>
       <c r="D49" s="63"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>114</v>
       </c>
@@ -2920,7 +2915,7 @@
       <c r="C50" s="63"/>
       <c r="D50" s="63"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>115</v>
       </c>
@@ -2928,7 +2923,7 @@
       <c r="C51" s="63"/>
       <c r="D51" s="63"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>0</v>
       </c>
@@ -2936,7 +2931,7 @@
       <c r="C52" s="62"/>
       <c r="D52" s="62"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>11</v>
       </c>
@@ -2944,7 +2939,7 @@
       <c r="C53" s="62"/>
       <c r="D53" s="62"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>13</v>
       </c>
@@ -2952,7 +2947,7 @@
       <c r="C54" s="62"/>
       <c r="D54" s="62"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>14</v>
       </c>
@@ -2960,7 +2955,7 @@
       <c r="C55" s="62"/>
       <c r="D55" s="62"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>10</v>
       </c>
@@ -2968,7 +2963,7 @@
       <c r="C56" s="62"/>
       <c r="D56" s="62"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>109</v>
       </c>
@@ -2978,7 +2973,7 @@
       <c r="C57" s="62"/>
       <c r="D57" s="62"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>110</v>
       </c>
@@ -2988,7 +2983,7 @@
       <c r="C58" s="62"/>
       <c r="D58" s="62"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>111</v>
       </c>
@@ -2998,7 +2993,7 @@
       <c r="C59" s="62"/>
       <c r="D59" s="62"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>120</v>
       </c>
@@ -3006,7 +3001,7 @@
       <c r="C60" s="62"/>
       <c r="D60" s="62"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>119</v>
       </c>
@@ -3014,7 +3009,7 @@
       <c r="C61" s="62"/>
       <c r="D61" s="62"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>87</v>
       </c>
@@ -3022,7 +3017,7 @@
       <c r="C62" s="62"/>
       <c r="D62" s="62"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>53</v>
       </c>
@@ -3030,7 +3025,7 @@
       <c r="C63" s="62"/>
       <c r="D63" s="62"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
         <v>54</v>
       </c>
@@ -3038,7 +3033,7 @@
       <c r="C64" s="62"/>
       <c r="D64" s="62"/>
     </row>
-    <row r="65" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A65" s="11" t="s">
         <v>1</v>
       </c>
@@ -3110,7 +3105,7 @@
       <c r="BO65" s="15"/>
       <c r="BP65" s="15"/>
     </row>
-    <row r="66" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A66" s="11" t="s">
         <v>2</v>
       </c>
@@ -3182,7 +3177,7 @@
       <c r="BO66" s="15"/>
       <c r="BP66" s="15"/>
     </row>
-    <row r="67" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="21" t="s">
         <v>72</v>
       </c>
@@ -3254,7 +3249,7 @@
       <c r="BO67" s="15"/>
       <c r="BP67" s="15"/>
     </row>
-    <row r="68" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
         <v>74</v>
       </c>
@@ -3267,7 +3262,7 @@
       <c r="H68" s="46"/>
       <c r="I68" s="46"/>
     </row>
-    <row r="69" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
         <v>73</v>
       </c>
@@ -3280,7 +3275,7 @@
       <c r="H69" s="46"/>
       <c r="I69" s="46"/>
     </row>
-    <row r="70" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>71</v>
       </c>
@@ -3293,7 +3288,7 @@
       <c r="H70" s="46"/>
       <c r="I70" s="46"/>
     </row>
-    <row r="71" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>70</v>
       </c>
@@ -3367,7 +3362,7 @@
       <c r="BO71" s="15"/>
       <c r="BP71" s="15"/>
     </row>
-    <row r="72" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>75</v>
       </c>
@@ -3380,7 +3375,7 @@
       <c r="H72" s="46"/>
       <c r="I72" s="46"/>
     </row>
-    <row r="73" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>76</v>
       </c>
@@ -3393,7 +3388,7 @@
       <c r="H73" s="46"/>
       <c r="I73" s="46"/>
     </row>
-    <row r="74" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>77</v>
       </c>
@@ -3406,7 +3401,7 @@
       <c r="H74" s="46"/>
       <c r="I74" s="46"/>
     </row>
-    <row r="75" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>78</v>
       </c>
@@ -3419,7 +3414,7 @@
       <c r="H75" s="46"/>
       <c r="I75" s="46"/>
     </row>
-    <row r="76" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="12" t="s">
         <v>79</v>
       </c>
@@ -3434,7 +3429,7 @@
       <c r="H76" s="46"/>
       <c r="I76" s="46"/>
     </row>
-    <row r="77" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>3</v>
       </c>
@@ -3506,7 +3501,7 @@
       <c r="BO77" s="15"/>
       <c r="BP77" s="15"/>
     </row>
-    <row r="78" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>4</v>
       </c>
@@ -3578,7 +3573,7 @@
       <c r="BO78" s="15"/>
       <c r="BP78" s="15"/>
     </row>
-    <row r="79" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>5</v>
       </c>
@@ -3650,7 +3645,7 @@
       <c r="BO79" s="15"/>
       <c r="BP79" s="15"/>
     </row>
-    <row r="80" spans="1:68" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A80" s="13" t="s">
         <v>9</v>
       </c>
@@ -3658,7 +3653,7 @@
       <c r="C80" s="50"/>
       <c r="D80" s="50"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="13" t="s">
         <v>16</v>
       </c>
@@ -3666,7 +3661,7 @@
       <c r="C81" s="65"/>
       <c r="D81" s="65"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="13" t="s">
         <v>7</v>
       </c>
@@ -3674,21 +3669,23 @@
       <c r="C82" s="50"/>
       <c r="D82" s="50"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B83" s="43">
+        <v>1</v>
+      </c>
+      <c r="C83" s="43">
         <v>2</v>
       </c>
-      <c r="C83" s="43"/>
       <c r="D83" s="43"/>
       <c r="E83" s="52"/>
       <c r="F83" s="52"/>
       <c r="G83" s="52"/>
       <c r="H83" s="53"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="16" t="s">
         <v>6</v>
       </c>
@@ -3706,17 +3703,15 @@
       <c r="G84" s="44"/>
       <c r="H84" s="54"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B85" s="45" t="b">
-        <v>1</v>
-      </c>
+      <c r="B85" s="45"/>
       <c r="C85" s="50"/>
       <c r="D85" s="50"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="13" t="s">
         <v>112</v>
       </c>
@@ -3724,7 +3719,7 @@
       <c r="C86" s="50"/>
       <c r="D86" s="50"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="13" t="s">
         <v>107</v>
       </c>
@@ -3732,7 +3727,7 @@
       <c r="C87" s="50"/>
       <c r="D87" s="50"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
         <v>108</v>
       </c>
@@ -3740,7 +3735,7 @@
       <c r="C88" s="50"/>
       <c r="D88" s="50"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
         <v>56</v>
       </c>
@@ -3748,7 +3743,7 @@
       <c r="C89" s="50"/>
       <c r="D89" s="50"/>
     </row>
-    <row r="90" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>68</v>
       </c>
@@ -3761,7 +3756,7 @@
       <c r="H90" s="46"/>
       <c r="I90" s="46"/>
     </row>
-    <row r="91" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>69</v>
       </c>
@@ -3774,7 +3769,7 @@
       <c r="H91" s="46"/>
       <c r="I91" s="46"/>
     </row>
-    <row r="92" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>121</v>
       </c>
@@ -3787,7 +3782,7 @@
       <c r="H92" s="46"/>
       <c r="I92" s="46"/>
     </row>
-    <row r="93" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
         <v>83</v>
       </c>
@@ -3800,7 +3795,7 @@
       <c r="H93" s="46"/>
       <c r="I93" s="46"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>57</v>
       </c>
@@ -3808,7 +3803,7 @@
       <c r="C94" s="50"/>
       <c r="D94" s="50"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
         <v>58</v>
       </c>
@@ -3816,7 +3811,7 @@
       <c r="C95" s="50"/>
       <c r="D95" s="50"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
         <v>59</v>
       </c>
@@ -3824,7 +3819,7 @@
       <c r="C96" s="50"/>
       <c r="D96" s="50"/>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
         <v>122</v>
       </c>
@@ -3832,7 +3827,7 @@
       <c r="C97" s="50"/>
       <c r="D97" s="50"/>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
         <v>117</v>
       </c>
@@ -3840,7 +3835,7 @@
       <c r="C98" s="50"/>
       <c r="D98" s="50"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
         <v>118</v>
       </c>
@@ -3848,7 +3843,7 @@
       <c r="C99" s="50"/>
       <c r="D99" s="50"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="55" t="s">
         <v>88</v>
       </c>
@@ -3856,7 +3851,7 @@
       <c r="C100" s="50"/>
       <c r="D100" s="50"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="56" t="s">
         <v>89</v>
       </c>
@@ -3864,7 +3859,7 @@
       <c r="C101" s="50"/>
       <c r="D101" s="50"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="56" t="s">
         <v>95</v>
       </c>
@@ -3872,7 +3867,7 @@
       <c r="C102" s="50"/>
       <c r="D102" s="50"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="56" t="s">
         <v>123</v>
       </c>
@@ -3880,7 +3875,7 @@
       <c r="C103" s="50"/>
       <c r="D103" s="50"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="56" t="s">
         <v>96</v>
       </c>
@@ -3888,7 +3883,7 @@
       <c r="C104" s="50"/>
       <c r="D104" s="50"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="56" t="s">
         <v>90</v>
       </c>
@@ -3896,7 +3891,7 @@
       <c r="C105" s="50"/>
       <c r="D105" s="50"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="56" t="s">
         <v>97</v>
       </c>
@@ -3904,7 +3899,7 @@
       <c r="C106" s="50"/>
       <c r="D106" s="50"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="56" t="s">
         <v>124</v>
       </c>
@@ -3912,7 +3907,7 @@
       <c r="C107" s="50"/>
       <c r="D107" s="50"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="56" t="s">
         <v>98</v>
       </c>
@@ -3920,7 +3915,7 @@
       <c r="C108" s="50"/>
       <c r="D108" s="50"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="57" t="s">
         <v>91</v>
       </c>
@@ -3928,7 +3923,7 @@
       <c r="C109" s="50"/>
       <c r="D109" s="50"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="57" t="s">
         <v>99</v>
       </c>
@@ -3936,7 +3931,7 @@
       <c r="C110" s="50"/>
       <c r="D110" s="50"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="56" t="s">
         <v>125</v>
       </c>
@@ -3944,7 +3939,7 @@
       <c r="C111" s="50"/>
       <c r="D111" s="50"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="57" t="s">
         <v>100</v>
       </c>
@@ -3952,7 +3947,7 @@
       <c r="C112" s="50"/>
       <c r="D112" s="50"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="57" t="s">
         <v>92</v>
       </c>
@@ -3960,7 +3955,7 @@
       <c r="C113" s="50"/>
       <c r="D113" s="50"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="57" t="s">
         <v>101</v>
       </c>
@@ -3968,7 +3963,7 @@
       <c r="C114" s="50"/>
       <c r="D114" s="50"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="56" t="s">
         <v>126</v>
       </c>
@@ -3976,7 +3971,7 @@
       <c r="C115" s="50"/>
       <c r="D115" s="50"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="57" t="s">
         <v>102</v>
       </c>
@@ -3984,7 +3979,7 @@
       <c r="C116" s="50"/>
       <c r="D116" s="50"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="57" t="s">
         <v>93</v>
       </c>
@@ -3992,7 +3987,7 @@
       <c r="C117" s="50"/>
       <c r="D117" s="50"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="57" t="s">
         <v>103</v>
       </c>
@@ -4000,37 +3995,37 @@
       <c r="C118" s="50"/>
       <c r="D118" s="50"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="56" t="s">
         <v>127</v>
       </c>
       <c r="B119" s="59"/>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="57" t="s">
         <v>104</v>
       </c>
       <c r="B120" s="59"/>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="57" t="s">
         <v>94</v>
       </c>
       <c r="B121" s="59"/>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="57" t="s">
         <v>105</v>
       </c>
       <c r="B122" s="59"/>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="56" t="s">
         <v>128</v>
       </c>
       <c r="B123" s="59"/>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="58" t="s">
         <v>106</v>
       </c>
@@ -4101,7 +4096,7 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
Bring compartment sizes into line
Ensure compartment size plotting for outputs is coded consistently with
the other plotting methods.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="130">
   <si>
     <t>recent_time</t>
   </si>
@@ -402,6 +402,9 @@
   </si>
   <si>
     <t>econ_startingcost_duration_xpertacf</t>
+  </si>
+  <si>
+    <t>output_compartment_populations</t>
   </si>
 </sst>
 </file>
@@ -2400,10 +2403,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP124"/>
+  <dimension ref="A1:BP125"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2693,7 +2696,7 @@
       <c r="E27" s="50"/>
       <c r="F27" s="50"/>
     </row>
-    <row r="28" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
@@ -2703,7 +2706,7 @@
       <c r="E28" s="50"/>
       <c r="F28" s="50"/>
     </row>
-    <row r="29" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
@@ -2713,7 +2716,7 @@
       <c r="E29" s="50"/>
       <c r="F29" s="50"/>
     </row>
-    <row r="30" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
@@ -2723,7 +2726,7 @@
       <c r="E30" s="50"/>
       <c r="F30" s="50"/>
     </row>
-    <row r="31" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>63</v>
       </c>
@@ -2733,7 +2736,7 @@
       <c r="E31" s="50"/>
       <c r="F31" s="50"/>
     </row>
-    <row r="32" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>64</v>
       </c>
@@ -2743,7 +2746,7 @@
       <c r="E32" s="50"/>
       <c r="F32" s="50"/>
     </row>
-    <row r="33" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
@@ -2753,7 +2756,7 @@
       <c r="E33" s="50"/>
       <c r="F33" s="50"/>
     </row>
-    <row r="34" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
@@ -2763,7 +2766,7 @@
       <c r="E34" s="50"/>
       <c r="F34" s="50"/>
     </row>
-    <row r="35" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>48</v>
       </c>
@@ -2773,7 +2776,7 @@
       <c r="E35" s="50"/>
       <c r="F35" s="50"/>
     </row>
-    <row r="36" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>49</v>
       </c>
@@ -2783,7 +2786,7 @@
       <c r="E36" s="50"/>
       <c r="F36" s="50"/>
     </row>
-    <row r="37" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
@@ -2793,7 +2796,7 @@
       <c r="E37" s="50"/>
       <c r="F37" s="50"/>
     </row>
-    <row r="38" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>80</v>
       </c>
@@ -2803,7 +2806,7 @@
       <c r="E38" s="50"/>
       <c r="F38" s="50"/>
     </row>
-    <row r="39" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>84</v>
       </c>
@@ -2813,7 +2816,7 @@
       <c r="E39" s="50"/>
       <c r="F39" s="50"/>
     </row>
-    <row r="40" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>85</v>
       </c>
@@ -2823,7 +2826,7 @@
       <c r="E40" s="50"/>
       <c r="F40" s="50"/>
     </row>
-    <row r="41" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>51</v>
       </c>
@@ -2833,7 +2836,7 @@
       <c r="E41" s="50"/>
       <c r="F41" s="50"/>
     </row>
-    <row r="42" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>116</v>
       </c>
@@ -2845,7 +2848,7 @@
       <c r="E42" s="50"/>
       <c r="F42" s="50"/>
     </row>
-    <row r="43" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>86</v>
       </c>
@@ -2855,7 +2858,7 @@
       <c r="E43" s="50"/>
       <c r="F43" s="50"/>
     </row>
-    <row r="44" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>15</v>
       </c>
@@ -2867,7 +2870,7 @@
       <c r="E44" s="46"/>
       <c r="F44" s="46"/>
     </row>
-    <row r="45" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>52</v>
       </c>
@@ -2875,7 +2878,7 @@
       <c r="C45" s="62"/>
       <c r="D45" s="62"/>
     </row>
-    <row r="46" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>82</v>
       </c>
@@ -2883,7 +2886,7 @@
       <c r="C46" s="62"/>
       <c r="D46" s="62"/>
     </row>
-    <row r="47" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>13</v>
       </c>
@@ -3743,22 +3746,17 @@
       <c r="C89" s="50"/>
       <c r="D89" s="50"/>
     </row>
-    <row r="90" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
       <c r="B90" s="41"/>
       <c r="C90" s="50"/>
       <c r="D90" s="50"/>
-      <c r="E90" s="50"/>
-      <c r="F90" s="50"/>
-      <c r="G90" s="46"/>
-      <c r="H90" s="46"/>
-      <c r="I90" s="46"/>
     </row>
     <row r="91" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B91" s="41"/>
       <c r="C91" s="50"/>
@@ -3771,7 +3769,7 @@
     </row>
     <row r="92" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>121</v>
+        <v>69</v>
       </c>
       <c r="B92" s="41"/>
       <c r="C92" s="50"/>
@@ -3784,7 +3782,7 @@
     </row>
     <row r="93" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="B93" s="41"/>
       <c r="C93" s="50"/>
@@ -3795,17 +3793,22 @@
       <c r="H93" s="46"/>
       <c r="I93" s="46"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="B94" s="41"/>
       <c r="C94" s="50"/>
       <c r="D94" s="50"/>
+      <c r="E94" s="50"/>
+      <c r="F94" s="50"/>
+      <c r="G94" s="46"/>
+      <c r="H94" s="46"/>
+      <c r="I94" s="46"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B95" s="41"/>
       <c r="C95" s="50"/>
@@ -3813,7 +3816,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B96" s="41"/>
       <c r="C96" s="50"/>
@@ -3821,7 +3824,7 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="B97" s="41"/>
       <c r="C97" s="50"/>
@@ -3829,7 +3832,7 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B98" s="41"/>
       <c r="C98" s="50"/>
@@ -3837,31 +3840,31 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B99" s="41"/>
       <c r="C99" s="50"/>
       <c r="D99" s="50"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B100" s="61"/>
+      <c r="A100" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B100" s="41"/>
       <c r="C100" s="50"/>
       <c r="D100" s="50"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="B101" s="59"/>
+      <c r="A101" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="B101" s="61"/>
       <c r="C101" s="50"/>
       <c r="D101" s="50"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="56" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B102" s="59"/>
       <c r="C102" s="50"/>
@@ -3869,7 +3872,7 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="56" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="B103" s="59"/>
       <c r="C103" s="50"/>
@@ -3877,7 +3880,7 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="56" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="B104" s="59"/>
       <c r="C104" s="50"/>
@@ -3885,7 +3888,7 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="56" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B105" s="59"/>
       <c r="C105" s="50"/>
@@ -3893,7 +3896,7 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="56" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B106" s="59"/>
       <c r="C106" s="50"/>
@@ -3901,7 +3904,7 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="56" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B107" s="59"/>
       <c r="C107" s="50"/>
@@ -3909,15 +3912,15 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="56" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="B108" s="59"/>
       <c r="C108" s="50"/>
       <c r="D108" s="50"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="57" t="s">
-        <v>91</v>
+      <c r="A109" s="56" t="s">
+        <v>98</v>
       </c>
       <c r="B109" s="59"/>
       <c r="C109" s="50"/>
@@ -3925,23 +3928,23 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="57" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B110" s="59"/>
       <c r="C110" s="50"/>
       <c r="D110" s="50"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="56" t="s">
-        <v>125</v>
+      <c r="A111" s="57" t="s">
+        <v>99</v>
       </c>
       <c r="B111" s="59"/>
       <c r="C111" s="50"/>
       <c r="D111" s="50"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="57" t="s">
-        <v>100</v>
+      <c r="A112" s="56" t="s">
+        <v>125</v>
       </c>
       <c r="B112" s="59"/>
       <c r="C112" s="50"/>
@@ -3949,7 +3952,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="57" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B113" s="59"/>
       <c r="C113" s="50"/>
@@ -3957,23 +3960,23 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="57" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B114" s="59"/>
       <c r="C114" s="50"/>
       <c r="D114" s="50"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="56" t="s">
-        <v>126</v>
+      <c r="A115" s="57" t="s">
+        <v>101</v>
       </c>
       <c r="B115" s="59"/>
       <c r="C115" s="50"/>
       <c r="D115" s="50"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="57" t="s">
-        <v>102</v>
+      <c r="A116" s="56" t="s">
+        <v>126</v>
       </c>
       <c r="B116" s="59"/>
       <c r="C116" s="50"/>
@@ -3981,7 +3984,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="57" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B117" s="59"/>
       <c r="C117" s="50"/>
@@ -3989,47 +3992,55 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="57" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B118" s="59"/>
       <c r="C118" s="50"/>
       <c r="D118" s="50"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="56" t="s">
+      <c r="A119" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="B119" s="59"/>
+      <c r="C119" s="50"/>
+      <c r="D119" s="50"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="56" t="s">
         <v>127</v>
-      </c>
-      <c r="B119" s="59"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="57" t="s">
-        <v>104</v>
       </c>
       <c r="B120" s="59"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="57" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B121" s="59"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B122" s="59"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="B122" s="59"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="56" t="s">
+      <c r="B123" s="59"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="B123" s="59"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="58" t="s">
+      <c r="B124" s="59"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="B124" s="60"/>
+      <c r="B125" s="60"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
@@ -4071,7 +4082,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B85:D99 B67:D71 B77:D79</xm:sqref>
+          <xm:sqref>B85:D100 B67:D71 B77:D79</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Revise popsize calculation for Xpert-based ACF
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="133">
   <si>
     <t>recent_time</t>
   </si>
@@ -405,6 +405,15 @@
   </si>
   <si>
     <t>output_compartment_populations</t>
+  </si>
+  <si>
+    <t>program_nns_smearacf</t>
+  </si>
+  <si>
+    <t>program_nns_xpertacf_smearpos</t>
+  </si>
+  <si>
+    <t>program_nns_xpertacf_smearneg</t>
   </si>
 </sst>
 </file>
@@ -1356,7 +1365,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1433,6 +1442,8 @@
     </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2403,10 +2414,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP125"/>
+  <dimension ref="A1:BP128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2746,7 +2757,7 @@
       <c r="E32" s="50"/>
       <c r="F32" s="50"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
@@ -2756,7 +2767,7 @@
       <c r="E33" s="50"/>
       <c r="F33" s="50"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
@@ -2766,7 +2777,7 @@
       <c r="E34" s="50"/>
       <c r="F34" s="50"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>48</v>
       </c>
@@ -2776,7 +2787,7 @@
       <c r="E35" s="50"/>
       <c r="F35" s="50"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>49</v>
       </c>
@@ -2786,7 +2797,7 @@
       <c r="E36" s="50"/>
       <c r="F36" s="50"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
@@ -2796,7 +2807,7 @@
       <c r="E37" s="50"/>
       <c r="F37" s="50"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>80</v>
       </c>
@@ -2806,7 +2817,7 @@
       <c r="E38" s="50"/>
       <c r="F38" s="50"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>84</v>
       </c>
@@ -2816,7 +2827,7 @@
       <c r="E39" s="50"/>
       <c r="F39" s="50"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>85</v>
       </c>
@@ -2826,133 +2837,148 @@
       <c r="E40" s="50"/>
       <c r="F40" s="50"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B41" s="66"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="67"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="67"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="67"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B42" s="25">
+      <c r="B45" s="25">
         <v>25</v>
       </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="50"/>
-      <c r="F42" s="50"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="50"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="50"/>
-      <c r="F43" s="50"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
+      <c r="B46" s="27"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="28">
+      <c r="B47" s="28">
         <v>0.05</v>
       </c>
-      <c r="C44" s="50"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="46"/>
-      <c r="F44" s="46"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="B45" s="29"/>
-      <c r="C45" s="62"/>
-      <c r="D45" s="62"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B46" s="29"/>
-      <c r="C46" s="62"/>
-      <c r="D46" s="62"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B47" s="29"/>
-      <c r="C47" s="62"/>
-      <c r="D47" s="62"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>14</v>
       </c>
       <c r="B48" s="29"/>
       <c r="C48" s="62"/>
       <c r="D48" s="62"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" s="29"/>
+      <c r="C49" s="62"/>
+      <c r="D49" s="62"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B50" s="29"/>
+      <c r="C50" s="62"/>
+      <c r="D50" s="62"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" s="29"/>
+      <c r="C51" s="62"/>
+      <c r="D51" s="62"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="B49" s="30"/>
-      <c r="C49" s="63"/>
-      <c r="D49" s="63"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="B52" s="30"/>
+      <c r="C52" s="63"/>
+      <c r="D52" s="63"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B50" s="30"/>
-      <c r="C50" s="63"/>
-      <c r="D50" s="63"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
+      <c r="B53" s="30"/>
+      <c r="C53" s="63"/>
+      <c r="D53" s="63"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="B51" s="30"/>
-      <c r="C51" s="63"/>
-      <c r="D51" s="63"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B52" s="29"/>
-      <c r="C52" s="62"/>
-      <c r="D52" s="62"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B53" s="29"/>
-      <c r="C53" s="62"/>
-      <c r="D53" s="62"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B54" s="29"/>
-      <c r="C54" s="62"/>
-      <c r="D54" s="62"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="63"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B55" s="29"/>
       <c r="C55" s="62"/>
@@ -2960,7 +2986,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B56" s="29"/>
       <c r="C56" s="62"/>
@@ -2968,293 +2994,101 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B57" s="29">
-        <v>1865</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B57" s="29"/>
       <c r="C57" s="62"/>
       <c r="D57" s="62"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B58" s="29">
-        <v>2036</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B58" s="29"/>
       <c r="C58" s="62"/>
       <c r="D58" s="62"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B59" s="29">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B59" s="29"/>
       <c r="C59" s="62"/>
       <c r="D59" s="62"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B60" s="29"/>
+        <v>109</v>
+      </c>
+      <c r="B60" s="29">
+        <v>1865</v>
+      </c>
       <c r="C60" s="62"/>
       <c r="D60" s="62"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="B61" s="29"/>
+        <v>110</v>
+      </c>
+      <c r="B61" s="29">
+        <v>2036</v>
+      </c>
       <c r="C61" s="62"/>
       <c r="D61" s="62"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B62" s="31"/>
+        <v>111</v>
+      </c>
+      <c r="B62" s="29">
+        <v>1</v>
+      </c>
       <c r="C62" s="62"/>
       <c r="D62" s="62"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B63" s="32"/>
+      <c r="A63" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" s="29"/>
       <c r="C63" s="62"/>
       <c r="D63" s="62"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B64" s="33"/>
+      <c r="A64" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64" s="29"/>
       <c r="C64" s="62"/>
       <c r="D64" s="62"/>
     </row>
     <row r="65" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B65" s="34"/>
+      <c r="A65" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B65" s="31"/>
       <c r="C65" s="62"/>
       <c r="D65" s="62"/>
-      <c r="E65" s="46"/>
-      <c r="F65" s="46"/>
-      <c r="G65" s="46"/>
-      <c r="H65" s="46"/>
-      <c r="I65" s="46"/>
-      <c r="J65" s="15"/>
-      <c r="K65" s="15"/>
-      <c r="L65" s="15"/>
-      <c r="M65" s="15"/>
-      <c r="N65" s="15"/>
-      <c r="O65" s="15"/>
-      <c r="P65" s="15"/>
-      <c r="Q65" s="15"/>
-      <c r="R65" s="15"/>
-      <c r="S65" s="15"/>
-      <c r="T65" s="15"/>
-      <c r="U65" s="15"/>
-      <c r="V65" s="15"/>
-      <c r="W65" s="15"/>
-      <c r="X65" s="15"/>
-      <c r="Y65" s="15"/>
-      <c r="Z65" s="15"/>
-      <c r="AA65" s="15"/>
-      <c r="AB65" s="15"/>
-      <c r="AC65" s="15"/>
-      <c r="AD65" s="15"/>
-      <c r="AE65" s="15"/>
-      <c r="AF65" s="15"/>
-      <c r="AG65" s="15"/>
-      <c r="AH65" s="15"/>
-      <c r="AI65" s="15"/>
-      <c r="AJ65" s="15"/>
-      <c r="AK65" s="15"/>
-      <c r="AL65" s="15"/>
-      <c r="AM65" s="15"/>
-      <c r="AN65" s="15"/>
-      <c r="AO65" s="15"/>
-      <c r="AP65" s="15"/>
-      <c r="AQ65" s="15"/>
-      <c r="AR65" s="15"/>
-      <c r="AS65" s="15"/>
-      <c r="AT65" s="15"/>
-      <c r="AU65" s="15"/>
-      <c r="AV65" s="15"/>
-      <c r="AW65" s="15"/>
-      <c r="AX65" s="15"/>
-      <c r="AY65" s="15"/>
-      <c r="AZ65" s="15"/>
-      <c r="BA65" s="15"/>
-      <c r="BB65" s="15"/>
-      <c r="BC65" s="15"/>
-      <c r="BD65" s="15"/>
-      <c r="BE65" s="15"/>
-      <c r="BF65" s="15"/>
-      <c r="BG65" s="15"/>
-      <c r="BH65" s="15"/>
-      <c r="BI65" s="15"/>
-      <c r="BJ65" s="15"/>
-      <c r="BK65" s="15"/>
-      <c r="BL65" s="15"/>
-      <c r="BM65" s="15"/>
-      <c r="BN65" s="15"/>
-      <c r="BO65" s="15"/>
-      <c r="BP65" s="15"/>
     </row>
     <row r="66" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A66" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B66" s="34"/>
+      <c r="A66" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B66" s="32"/>
       <c r="C66" s="62"/>
       <c r="D66" s="62"/>
-      <c r="E66" s="46"/>
-      <c r="F66" s="46"/>
-      <c r="G66" s="46"/>
-      <c r="H66" s="46"/>
-      <c r="I66" s="46"/>
-      <c r="J66" s="15"/>
-      <c r="K66" s="15"/>
-      <c r="L66" s="15"/>
-      <c r="M66" s="15"/>
-      <c r="N66" s="15"/>
-      <c r="O66" s="15"/>
-      <c r="P66" s="15"/>
-      <c r="Q66" s="15"/>
-      <c r="R66" s="15"/>
-      <c r="S66" s="15"/>
-      <c r="T66" s="15"/>
-      <c r="U66" s="15"/>
-      <c r="V66" s="15"/>
-      <c r="W66" s="15"/>
-      <c r="X66" s="15"/>
-      <c r="Y66" s="15"/>
-      <c r="Z66" s="15"/>
-      <c r="AA66" s="15"/>
-      <c r="AB66" s="15"/>
-      <c r="AC66" s="15"/>
-      <c r="AD66" s="15"/>
-      <c r="AE66" s="15"/>
-      <c r="AF66" s="15"/>
-      <c r="AG66" s="15"/>
-      <c r="AH66" s="15"/>
-      <c r="AI66" s="15"/>
-      <c r="AJ66" s="15"/>
-      <c r="AK66" s="15"/>
-      <c r="AL66" s="15"/>
-      <c r="AM66" s="15"/>
-      <c r="AN66" s="15"/>
-      <c r="AO66" s="15"/>
-      <c r="AP66" s="15"/>
-      <c r="AQ66" s="15"/>
-      <c r="AR66" s="15"/>
-      <c r="AS66" s="15"/>
-      <c r="AT66" s="15"/>
-      <c r="AU66" s="15"/>
-      <c r="AV66" s="15"/>
-      <c r="AW66" s="15"/>
-      <c r="AX66" s="15"/>
-      <c r="AY66" s="15"/>
-      <c r="AZ66" s="15"/>
-      <c r="BA66" s="15"/>
-      <c r="BB66" s="15"/>
-      <c r="BC66" s="15"/>
-      <c r="BD66" s="15"/>
-      <c r="BE66" s="15"/>
-      <c r="BF66" s="15"/>
-      <c r="BG66" s="15"/>
-      <c r="BH66" s="15"/>
-      <c r="BI66" s="15"/>
-      <c r="BJ66" s="15"/>
-      <c r="BK66" s="15"/>
-      <c r="BL66" s="15"/>
-      <c r="BM66" s="15"/>
-      <c r="BN66" s="15"/>
-      <c r="BO66" s="15"/>
-      <c r="BP66" s="15"/>
-    </row>
-    <row r="67" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B67" s="35"/>
+    </row>
+    <row r="67" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A67" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B67" s="33"/>
       <c r="C67" s="62"/>
       <c r="D67" s="62"/>
-      <c r="E67" s="46"/>
-      <c r="F67" s="46"/>
-      <c r="G67" s="46"/>
-      <c r="H67" s="46"/>
-      <c r="I67" s="46"/>
-      <c r="J67" s="15"/>
-      <c r="K67" s="15"/>
-      <c r="L67" s="15"/>
-      <c r="M67" s="15"/>
-      <c r="N67" s="15"/>
-      <c r="O67" s="15"/>
-      <c r="P67" s="15"/>
-      <c r="Q67" s="15"/>
-      <c r="R67" s="15"/>
-      <c r="S67" s="15"/>
-      <c r="T67" s="15"/>
-      <c r="U67" s="15"/>
-      <c r="V67" s="15"/>
-      <c r="W67" s="15"/>
-      <c r="X67" s="15"/>
-      <c r="Y67" s="15"/>
-      <c r="Z67" s="15"/>
-      <c r="AA67" s="15"/>
-      <c r="AB67" s="15"/>
-      <c r="AC67" s="15"/>
-      <c r="AD67" s="15"/>
-      <c r="AE67" s="15"/>
-      <c r="AF67" s="15"/>
-      <c r="AG67" s="15"/>
-      <c r="AH67" s="15"/>
-      <c r="AI67" s="15"/>
-      <c r="AJ67" s="15"/>
-      <c r="AK67" s="15"/>
-      <c r="AL67" s="15"/>
-      <c r="AM67" s="15"/>
-      <c r="AN67" s="15"/>
-      <c r="AO67" s="15"/>
-      <c r="AP67" s="15"/>
-      <c r="AQ67" s="15"/>
-      <c r="AR67" s="15"/>
-      <c r="AS67" s="15"/>
-      <c r="AT67" s="15"/>
-      <c r="AU67" s="15"/>
-      <c r="AV67" s="15"/>
-      <c r="AW67" s="15"/>
-      <c r="AX67" s="15"/>
-      <c r="AY67" s="15"/>
-      <c r="AZ67" s="15"/>
-      <c r="BA67" s="15"/>
-      <c r="BB67" s="15"/>
-      <c r="BC67" s="15"/>
-      <c r="BD67" s="15"/>
-      <c r="BE67" s="15"/>
-      <c r="BF67" s="15"/>
-      <c r="BG67" s="15"/>
-      <c r="BH67" s="15"/>
-      <c r="BI67" s="15"/>
-      <c r="BJ67" s="15"/>
-      <c r="BK67" s="15"/>
-      <c r="BL67" s="15"/>
-      <c r="BM67" s="15"/>
-      <c r="BN67" s="15"/>
-      <c r="BO67" s="15"/>
-      <c r="BP67" s="15"/>
-    </row>
-    <row r="68" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A68" s="11" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="B68" s="34"/>
       <c r="C68" s="62"/>
@@ -3264,10 +3098,69 @@
       <c r="G68" s="46"/>
       <c r="H68" s="46"/>
       <c r="I68" s="46"/>
-    </row>
-    <row r="69" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J68" s="15"/>
+      <c r="K68" s="15"/>
+      <c r="L68" s="15"/>
+      <c r="M68" s="15"/>
+      <c r="N68" s="15"/>
+      <c r="O68" s="15"/>
+      <c r="P68" s="15"/>
+      <c r="Q68" s="15"/>
+      <c r="R68" s="15"/>
+      <c r="S68" s="15"/>
+      <c r="T68" s="15"/>
+      <c r="U68" s="15"/>
+      <c r="V68" s="15"/>
+      <c r="W68" s="15"/>
+      <c r="X68" s="15"/>
+      <c r="Y68" s="15"/>
+      <c r="Z68" s="15"/>
+      <c r="AA68" s="15"/>
+      <c r="AB68" s="15"/>
+      <c r="AC68" s="15"/>
+      <c r="AD68" s="15"/>
+      <c r="AE68" s="15"/>
+      <c r="AF68" s="15"/>
+      <c r="AG68" s="15"/>
+      <c r="AH68" s="15"/>
+      <c r="AI68" s="15"/>
+      <c r="AJ68" s="15"/>
+      <c r="AK68" s="15"/>
+      <c r="AL68" s="15"/>
+      <c r="AM68" s="15"/>
+      <c r="AN68" s="15"/>
+      <c r="AO68" s="15"/>
+      <c r="AP68" s="15"/>
+      <c r="AQ68" s="15"/>
+      <c r="AR68" s="15"/>
+      <c r="AS68" s="15"/>
+      <c r="AT68" s="15"/>
+      <c r="AU68" s="15"/>
+      <c r="AV68" s="15"/>
+      <c r="AW68" s="15"/>
+      <c r="AX68" s="15"/>
+      <c r="AY68" s="15"/>
+      <c r="AZ68" s="15"/>
+      <c r="BA68" s="15"/>
+      <c r="BB68" s="15"/>
+      <c r="BC68" s="15"/>
+      <c r="BD68" s="15"/>
+      <c r="BE68" s="15"/>
+      <c r="BF68" s="15"/>
+      <c r="BG68" s="15"/>
+      <c r="BH68" s="15"/>
+      <c r="BI68" s="15"/>
+      <c r="BJ68" s="15"/>
+      <c r="BK68" s="15"/>
+      <c r="BL68" s="15"/>
+      <c r="BM68" s="15"/>
+      <c r="BN68" s="15"/>
+      <c r="BO68" s="15"/>
+      <c r="BP68" s="15"/>
+    </row>
+    <row r="69" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="B69" s="34"/>
       <c r="C69" s="62"/>
@@ -3277,12 +3170,71 @@
       <c r="G69" s="46"/>
       <c r="H69" s="46"/>
       <c r="I69" s="46"/>
-    </row>
-    <row r="70" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B70" s="34"/>
+      <c r="J69" s="15"/>
+      <c r="K69" s="15"/>
+      <c r="L69" s="15"/>
+      <c r="M69" s="15"/>
+      <c r="N69" s="15"/>
+      <c r="O69" s="15"/>
+      <c r="P69" s="15"/>
+      <c r="Q69" s="15"/>
+      <c r="R69" s="15"/>
+      <c r="S69" s="15"/>
+      <c r="T69" s="15"/>
+      <c r="U69" s="15"/>
+      <c r="V69" s="15"/>
+      <c r="W69" s="15"/>
+      <c r="X69" s="15"/>
+      <c r="Y69" s="15"/>
+      <c r="Z69" s="15"/>
+      <c r="AA69" s="15"/>
+      <c r="AB69" s="15"/>
+      <c r="AC69" s="15"/>
+      <c r="AD69" s="15"/>
+      <c r="AE69" s="15"/>
+      <c r="AF69" s="15"/>
+      <c r="AG69" s="15"/>
+      <c r="AH69" s="15"/>
+      <c r="AI69" s="15"/>
+      <c r="AJ69" s="15"/>
+      <c r="AK69" s="15"/>
+      <c r="AL69" s="15"/>
+      <c r="AM69" s="15"/>
+      <c r="AN69" s="15"/>
+      <c r="AO69" s="15"/>
+      <c r="AP69" s="15"/>
+      <c r="AQ69" s="15"/>
+      <c r="AR69" s="15"/>
+      <c r="AS69" s="15"/>
+      <c r="AT69" s="15"/>
+      <c r="AU69" s="15"/>
+      <c r="AV69" s="15"/>
+      <c r="AW69" s="15"/>
+      <c r="AX69" s="15"/>
+      <c r="AY69" s="15"/>
+      <c r="AZ69" s="15"/>
+      <c r="BA69" s="15"/>
+      <c r="BB69" s="15"/>
+      <c r="BC69" s="15"/>
+      <c r="BD69" s="15"/>
+      <c r="BE69" s="15"/>
+      <c r="BF69" s="15"/>
+      <c r="BG69" s="15"/>
+      <c r="BH69" s="15"/>
+      <c r="BI69" s="15"/>
+      <c r="BJ69" s="15"/>
+      <c r="BK69" s="15"/>
+      <c r="BL69" s="15"/>
+      <c r="BM69" s="15"/>
+      <c r="BN69" s="15"/>
+      <c r="BO69" s="15"/>
+      <c r="BP69" s="15"/>
+    </row>
+    <row r="70" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B70" s="35"/>
       <c r="C70" s="62"/>
       <c r="D70" s="62"/>
       <c r="E70" s="46"/>
@@ -3290,14 +3242,71 @@
       <c r="G70" s="46"/>
       <c r="H70" s="46"/>
       <c r="I70" s="46"/>
-    </row>
-    <row r="71" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B71" s="36" t="b">
-        <v>1</v>
-      </c>
+      <c r="J70" s="15"/>
+      <c r="K70" s="15"/>
+      <c r="L70" s="15"/>
+      <c r="M70" s="15"/>
+      <c r="N70" s="15"/>
+      <c r="O70" s="15"/>
+      <c r="P70" s="15"/>
+      <c r="Q70" s="15"/>
+      <c r="R70" s="15"/>
+      <c r="S70" s="15"/>
+      <c r="T70" s="15"/>
+      <c r="U70" s="15"/>
+      <c r="V70" s="15"/>
+      <c r="W70" s="15"/>
+      <c r="X70" s="15"/>
+      <c r="Y70" s="15"/>
+      <c r="Z70" s="15"/>
+      <c r="AA70" s="15"/>
+      <c r="AB70" s="15"/>
+      <c r="AC70" s="15"/>
+      <c r="AD70" s="15"/>
+      <c r="AE70" s="15"/>
+      <c r="AF70" s="15"/>
+      <c r="AG70" s="15"/>
+      <c r="AH70" s="15"/>
+      <c r="AI70" s="15"/>
+      <c r="AJ70" s="15"/>
+      <c r="AK70" s="15"/>
+      <c r="AL70" s="15"/>
+      <c r="AM70" s="15"/>
+      <c r="AN70" s="15"/>
+      <c r="AO70" s="15"/>
+      <c r="AP70" s="15"/>
+      <c r="AQ70" s="15"/>
+      <c r="AR70" s="15"/>
+      <c r="AS70" s="15"/>
+      <c r="AT70" s="15"/>
+      <c r="AU70" s="15"/>
+      <c r="AV70" s="15"/>
+      <c r="AW70" s="15"/>
+      <c r="AX70" s="15"/>
+      <c r="AY70" s="15"/>
+      <c r="AZ70" s="15"/>
+      <c r="BA70" s="15"/>
+      <c r="BB70" s="15"/>
+      <c r="BC70" s="15"/>
+      <c r="BD70" s="15"/>
+      <c r="BE70" s="15"/>
+      <c r="BF70" s="15"/>
+      <c r="BG70" s="15"/>
+      <c r="BH70" s="15"/>
+      <c r="BI70" s="15"/>
+      <c r="BJ70" s="15"/>
+      <c r="BK70" s="15"/>
+      <c r="BL70" s="15"/>
+      <c r="BM70" s="15"/>
+      <c r="BN70" s="15"/>
+      <c r="BO70" s="15"/>
+      <c r="BP70" s="15"/>
+    </row>
+    <row r="71" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="34"/>
       <c r="C71" s="62"/>
       <c r="D71" s="62"/>
       <c r="E71" s="46"/>
@@ -3305,73 +3314,14 @@
       <c r="G71" s="46"/>
       <c r="H71" s="46"/>
       <c r="I71" s="46"/>
-      <c r="J71" s="15"/>
-      <c r="K71" s="15"/>
-      <c r="L71" s="15"/>
-      <c r="M71" s="15"/>
-      <c r="N71" s="15"/>
-      <c r="O71" s="15"/>
-      <c r="P71" s="15"/>
-      <c r="Q71" s="15"/>
-      <c r="R71" s="15"/>
-      <c r="S71" s="15"/>
-      <c r="T71" s="15"/>
-      <c r="U71" s="15"/>
-      <c r="V71" s="15"/>
-      <c r="W71" s="15"/>
-      <c r="X71" s="15"/>
-      <c r="Y71" s="15"/>
-      <c r="Z71" s="15"/>
-      <c r="AA71" s="15"/>
-      <c r="AB71" s="15"/>
-      <c r="AC71" s="15"/>
-      <c r="AD71" s="15"/>
-      <c r="AE71" s="15"/>
-      <c r="AF71" s="15"/>
-      <c r="AG71" s="15"/>
-      <c r="AH71" s="15"/>
-      <c r="AI71" s="15"/>
-      <c r="AJ71" s="15"/>
-      <c r="AK71" s="15"/>
-      <c r="AL71" s="15"/>
-      <c r="AM71" s="15"/>
-      <c r="AN71" s="15"/>
-      <c r="AO71" s="15"/>
-      <c r="AP71" s="15"/>
-      <c r="AQ71" s="15"/>
-      <c r="AR71" s="15"/>
-      <c r="AS71" s="15"/>
-      <c r="AT71" s="15"/>
-      <c r="AU71" s="15"/>
-      <c r="AV71" s="15"/>
-      <c r="AW71" s="15"/>
-      <c r="AX71" s="15"/>
-      <c r="AY71" s="15"/>
-      <c r="AZ71" s="15"/>
-      <c r="BA71" s="15"/>
-      <c r="BB71" s="15"/>
-      <c r="BC71" s="15"/>
-      <c r="BD71" s="15"/>
-      <c r="BE71" s="15"/>
-      <c r="BF71" s="15"/>
-      <c r="BG71" s="15"/>
-      <c r="BH71" s="15"/>
-      <c r="BI71" s="15"/>
-      <c r="BJ71" s="15"/>
-      <c r="BK71" s="15"/>
-      <c r="BL71" s="15"/>
-      <c r="BM71" s="15"/>
-      <c r="BN71" s="15"/>
-      <c r="BO71" s="15"/>
-      <c r="BP71" s="15"/>
     </row>
     <row r="72" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B72" s="37"/>
-      <c r="C72" s="64"/>
-      <c r="D72" s="64"/>
+        <v>73</v>
+      </c>
+      <c r="B72" s="34"/>
+      <c r="C72" s="62"/>
+      <c r="D72" s="62"/>
       <c r="E72" s="46"/>
       <c r="F72" s="46"/>
       <c r="G72" s="46"/>
@@ -3380,33 +3330,94 @@
     </row>
     <row r="73" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B73" s="37"/>
-      <c r="C73" s="64"/>
-      <c r="D73" s="64"/>
+        <v>71</v>
+      </c>
+      <c r="B73" s="34"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="62"/>
       <c r="E73" s="46"/>
       <c r="F73" s="46"/>
       <c r="G73" s="46"/>
       <c r="H73" s="46"/>
       <c r="I73" s="46"/>
     </row>
-    <row r="74" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B74" s="37"/>
-      <c r="C74" s="64"/>
-      <c r="D74" s="64"/>
+    <row r="74" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B74" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="C74" s="62"/>
+      <c r="D74" s="62"/>
       <c r="E74" s="46"/>
       <c r="F74" s="46"/>
       <c r="G74" s="46"/>
       <c r="H74" s="46"/>
       <c r="I74" s="46"/>
+      <c r="J74" s="15"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="15"/>
+      <c r="M74" s="15"/>
+      <c r="N74" s="15"/>
+      <c r="O74" s="15"/>
+      <c r="P74" s="15"/>
+      <c r="Q74" s="15"/>
+      <c r="R74" s="15"/>
+      <c r="S74" s="15"/>
+      <c r="T74" s="15"/>
+      <c r="U74" s="15"/>
+      <c r="V74" s="15"/>
+      <c r="W74" s="15"/>
+      <c r="X74" s="15"/>
+      <c r="Y74" s="15"/>
+      <c r="Z74" s="15"/>
+      <c r="AA74" s="15"/>
+      <c r="AB74" s="15"/>
+      <c r="AC74" s="15"/>
+      <c r="AD74" s="15"/>
+      <c r="AE74" s="15"/>
+      <c r="AF74" s="15"/>
+      <c r="AG74" s="15"/>
+      <c r="AH74" s="15"/>
+      <c r="AI74" s="15"/>
+      <c r="AJ74" s="15"/>
+      <c r="AK74" s="15"/>
+      <c r="AL74" s="15"/>
+      <c r="AM74" s="15"/>
+      <c r="AN74" s="15"/>
+      <c r="AO74" s="15"/>
+      <c r="AP74" s="15"/>
+      <c r="AQ74" s="15"/>
+      <c r="AR74" s="15"/>
+      <c r="AS74" s="15"/>
+      <c r="AT74" s="15"/>
+      <c r="AU74" s="15"/>
+      <c r="AV74" s="15"/>
+      <c r="AW74" s="15"/>
+      <c r="AX74" s="15"/>
+      <c r="AY74" s="15"/>
+      <c r="AZ74" s="15"/>
+      <c r="BA74" s="15"/>
+      <c r="BB74" s="15"/>
+      <c r="BC74" s="15"/>
+      <c r="BD74" s="15"/>
+      <c r="BE74" s="15"/>
+      <c r="BF74" s="15"/>
+      <c r="BG74" s="15"/>
+      <c r="BH74" s="15"/>
+      <c r="BI74" s="15"/>
+      <c r="BJ74" s="15"/>
+      <c r="BK74" s="15"/>
+      <c r="BL74" s="15"/>
+      <c r="BM74" s="15"/>
+      <c r="BN74" s="15"/>
+      <c r="BO74" s="15"/>
+      <c r="BP74" s="15"/>
     </row>
     <row r="75" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B75" s="37"/>
       <c r="C75" s="64"/>
@@ -3418,12 +3429,10 @@
       <c r="I75" s="46"/>
     </row>
     <row r="76" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B76" s="38">
-        <v>0.156</v>
-      </c>
+      <c r="A76" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" s="37"/>
       <c r="C76" s="64"/>
       <c r="D76" s="64"/>
       <c r="E76" s="46"/>
@@ -3432,370 +3441,372 @@
       <c r="H76" s="46"/>
       <c r="I76" s="46"/>
     </row>
-    <row r="77" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B77" s="39"/>
-      <c r="C77" s="50"/>
-      <c r="D77" s="50"/>
+        <v>77</v>
+      </c>
+      <c r="B77" s="37"/>
+      <c r="C77" s="64"/>
+      <c r="D77" s="64"/>
       <c r="E77" s="46"/>
       <c r="F77" s="46"/>
       <c r="G77" s="46"/>
       <c r="H77" s="46"/>
       <c r="I77" s="46"/>
-      <c r="J77" s="15"/>
-      <c r="K77" s="15"/>
-      <c r="L77" s="15"/>
-      <c r="M77" s="15"/>
-      <c r="N77" s="15"/>
-      <c r="O77" s="15"/>
-      <c r="P77" s="15"/>
-      <c r="Q77" s="15"/>
-      <c r="R77" s="15"/>
-      <c r="S77" s="15"/>
-      <c r="T77" s="15"/>
-      <c r="U77" s="15"/>
-      <c r="V77" s="15"/>
-      <c r="W77" s="15"/>
-      <c r="X77" s="15"/>
-      <c r="Y77" s="15"/>
-      <c r="Z77" s="15"/>
-      <c r="AA77" s="15"/>
-      <c r="AB77" s="15"/>
-      <c r="AC77" s="15"/>
-      <c r="AD77" s="15"/>
-      <c r="AE77" s="15"/>
-      <c r="AF77" s="15"/>
-      <c r="AG77" s="15"/>
-      <c r="AH77" s="15"/>
-      <c r="AI77" s="15"/>
-      <c r="AJ77" s="15"/>
-      <c r="AK77" s="15"/>
-      <c r="AL77" s="15"/>
-      <c r="AM77" s="15"/>
-      <c r="AN77" s="15"/>
-      <c r="AO77" s="15"/>
-      <c r="AP77" s="15"/>
-      <c r="AQ77" s="15"/>
-      <c r="AR77" s="15"/>
-      <c r="AS77" s="15"/>
-      <c r="AT77" s="15"/>
-      <c r="AU77" s="15"/>
-      <c r="AV77" s="15"/>
-      <c r="AW77" s="15"/>
-      <c r="AX77" s="15"/>
-      <c r="AY77" s="15"/>
-      <c r="AZ77" s="15"/>
-      <c r="BA77" s="15"/>
-      <c r="BB77" s="15"/>
-      <c r="BC77" s="15"/>
-      <c r="BD77" s="15"/>
-      <c r="BE77" s="15"/>
-      <c r="BF77" s="15"/>
-      <c r="BG77" s="15"/>
-      <c r="BH77" s="15"/>
-      <c r="BI77" s="15"/>
-      <c r="BJ77" s="15"/>
-      <c r="BK77" s="15"/>
-      <c r="BL77" s="15"/>
-      <c r="BM77" s="15"/>
-      <c r="BN77" s="15"/>
-      <c r="BO77" s="15"/>
-      <c r="BP77" s="15"/>
-    </row>
-    <row r="78" spans="1:68" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B78" s="39"/>
-      <c r="C78" s="50"/>
-      <c r="D78" s="50"/>
+        <v>78</v>
+      </c>
+      <c r="B78" s="37"/>
+      <c r="C78" s="64"/>
+      <c r="D78" s="64"/>
       <c r="E78" s="46"/>
       <c r="F78" s="46"/>
       <c r="G78" s="46"/>
       <c r="H78" s="46"/>
       <c r="I78" s="46"/>
-      <c r="J78" s="15"/>
-      <c r="K78" s="15"/>
-      <c r="L78" s="15"/>
-      <c r="M78" s="15"/>
-      <c r="N78" s="15"/>
-      <c r="O78" s="15"/>
-      <c r="P78" s="15"/>
-      <c r="Q78" s="15"/>
-      <c r="R78" s="15"/>
-      <c r="S78" s="15"/>
-      <c r="T78" s="15"/>
-      <c r="U78" s="15"/>
-      <c r="V78" s="15"/>
-      <c r="W78" s="15"/>
-      <c r="X78" s="15"/>
-      <c r="Y78" s="15"/>
-      <c r="Z78" s="15"/>
-      <c r="AA78" s="15"/>
-      <c r="AB78" s="15"/>
-      <c r="AC78" s="15"/>
-      <c r="AD78" s="15"/>
-      <c r="AE78" s="15"/>
-      <c r="AF78" s="15"/>
-      <c r="AG78" s="15"/>
-      <c r="AH78" s="15"/>
-      <c r="AI78" s="15"/>
-      <c r="AJ78" s="15"/>
-      <c r="AK78" s="15"/>
-      <c r="AL78" s="15"/>
-      <c r="AM78" s="15"/>
-      <c r="AN78" s="15"/>
-      <c r="AO78" s="15"/>
-      <c r="AP78" s="15"/>
-      <c r="AQ78" s="15"/>
-      <c r="AR78" s="15"/>
-      <c r="AS78" s="15"/>
-      <c r="AT78" s="15"/>
-      <c r="AU78" s="15"/>
-      <c r="AV78" s="15"/>
-      <c r="AW78" s="15"/>
-      <c r="AX78" s="15"/>
-      <c r="AY78" s="15"/>
-      <c r="AZ78" s="15"/>
-      <c r="BA78" s="15"/>
-      <c r="BB78" s="15"/>
-      <c r="BC78" s="15"/>
-      <c r="BD78" s="15"/>
-      <c r="BE78" s="15"/>
-      <c r="BF78" s="15"/>
-      <c r="BG78" s="15"/>
-      <c r="BH78" s="15"/>
-      <c r="BI78" s="15"/>
-      <c r="BJ78" s="15"/>
-      <c r="BK78" s="15"/>
-      <c r="BL78" s="15"/>
-      <c r="BM78" s="15"/>
-      <c r="BN78" s="15"/>
-      <c r="BO78" s="15"/>
-      <c r="BP78" s="15"/>
-    </row>
-    <row r="79" spans="1:68" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B79" s="40"/>
-      <c r="C79" s="50"/>
-      <c r="D79" s="50"/>
+        <v>79</v>
+      </c>
+      <c r="B79" s="38">
+        <v>0.156</v>
+      </c>
+      <c r="C79" s="64"/>
+      <c r="D79" s="64"/>
       <c r="E79" s="46"/>
       <c r="F79" s="46"/>
       <c r="G79" s="46"/>
       <c r="H79" s="46"/>
       <c r="I79" s="46"/>
-      <c r="J79" s="15"/>
-      <c r="K79" s="15"/>
-      <c r="L79" s="15"/>
-      <c r="M79" s="15"/>
-      <c r="N79" s="15"/>
-      <c r="O79" s="15"/>
-      <c r="P79" s="15"/>
-      <c r="Q79" s="15"/>
-      <c r="R79" s="15"/>
-      <c r="S79" s="15"/>
-      <c r="T79" s="15"/>
-      <c r="U79" s="15"/>
-      <c r="V79" s="15"/>
-      <c r="W79" s="15"/>
-      <c r="X79" s="15"/>
-      <c r="Y79" s="15"/>
-      <c r="Z79" s="15"/>
-      <c r="AA79" s="15"/>
-      <c r="AB79" s="15"/>
-      <c r="AC79" s="15"/>
-      <c r="AD79" s="15"/>
-      <c r="AE79" s="15"/>
-      <c r="AF79" s="15"/>
-      <c r="AG79" s="15"/>
-      <c r="AH79" s="15"/>
-      <c r="AI79" s="15"/>
-      <c r="AJ79" s="15"/>
-      <c r="AK79" s="15"/>
-      <c r="AL79" s="15"/>
-      <c r="AM79" s="15"/>
-      <c r="AN79" s="15"/>
-      <c r="AO79" s="15"/>
-      <c r="AP79" s="15"/>
-      <c r="AQ79" s="15"/>
-      <c r="AR79" s="15"/>
-      <c r="AS79" s="15"/>
-      <c r="AT79" s="15"/>
-      <c r="AU79" s="15"/>
-      <c r="AV79" s="15"/>
-      <c r="AW79" s="15"/>
-      <c r="AX79" s="15"/>
-      <c r="AY79" s="15"/>
-      <c r="AZ79" s="15"/>
-      <c r="BA79" s="15"/>
-      <c r="BB79" s="15"/>
-      <c r="BC79" s="15"/>
-      <c r="BD79" s="15"/>
-      <c r="BE79" s="15"/>
-      <c r="BF79" s="15"/>
-      <c r="BG79" s="15"/>
-      <c r="BH79" s="15"/>
-      <c r="BI79" s="15"/>
-      <c r="BJ79" s="15"/>
-      <c r="BK79" s="15"/>
-      <c r="BL79" s="15"/>
-      <c r="BM79" s="15"/>
-      <c r="BN79" s="15"/>
-      <c r="BO79" s="15"/>
-      <c r="BP79" s="15"/>
     </row>
     <row r="80" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A80" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B80" s="41"/>
+      <c r="A80" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80" s="39"/>
       <c r="C80" s="50"/>
       <c r="D80" s="50"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B81" s="42"/>
-      <c r="C81" s="65"/>
-      <c r="D81" s="65"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B82" s="41"/>
+      <c r="E80" s="46"/>
+      <c r="F80" s="46"/>
+      <c r="G80" s="46"/>
+      <c r="H80" s="46"/>
+      <c r="I80" s="46"/>
+      <c r="J80" s="15"/>
+      <c r="K80" s="15"/>
+      <c r="L80" s="15"/>
+      <c r="M80" s="15"/>
+      <c r="N80" s="15"/>
+      <c r="O80" s="15"/>
+      <c r="P80" s="15"/>
+      <c r="Q80" s="15"/>
+      <c r="R80" s="15"/>
+      <c r="S80" s="15"/>
+      <c r="T80" s="15"/>
+      <c r="U80" s="15"/>
+      <c r="V80" s="15"/>
+      <c r="W80" s="15"/>
+      <c r="X80" s="15"/>
+      <c r="Y80" s="15"/>
+      <c r="Z80" s="15"/>
+      <c r="AA80" s="15"/>
+      <c r="AB80" s="15"/>
+      <c r="AC80" s="15"/>
+      <c r="AD80" s="15"/>
+      <c r="AE80" s="15"/>
+      <c r="AF80" s="15"/>
+      <c r="AG80" s="15"/>
+      <c r="AH80" s="15"/>
+      <c r="AI80" s="15"/>
+      <c r="AJ80" s="15"/>
+      <c r="AK80" s="15"/>
+      <c r="AL80" s="15"/>
+      <c r="AM80" s="15"/>
+      <c r="AN80" s="15"/>
+      <c r="AO80" s="15"/>
+      <c r="AP80" s="15"/>
+      <c r="AQ80" s="15"/>
+      <c r="AR80" s="15"/>
+      <c r="AS80" s="15"/>
+      <c r="AT80" s="15"/>
+      <c r="AU80" s="15"/>
+      <c r="AV80" s="15"/>
+      <c r="AW80" s="15"/>
+      <c r="AX80" s="15"/>
+      <c r="AY80" s="15"/>
+      <c r="AZ80" s="15"/>
+      <c r="BA80" s="15"/>
+      <c r="BB80" s="15"/>
+      <c r="BC80" s="15"/>
+      <c r="BD80" s="15"/>
+      <c r="BE80" s="15"/>
+      <c r="BF80" s="15"/>
+      <c r="BG80" s="15"/>
+      <c r="BH80" s="15"/>
+      <c r="BI80" s="15"/>
+      <c r="BJ80" s="15"/>
+      <c r="BK80" s="15"/>
+      <c r="BL80" s="15"/>
+      <c r="BM80" s="15"/>
+      <c r="BN80" s="15"/>
+      <c r="BO80" s="15"/>
+      <c r="BP80" s="15"/>
+    </row>
+    <row r="81" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A81" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B81" s="39"/>
+      <c r="C81" s="50"/>
+      <c r="D81" s="50"/>
+      <c r="E81" s="46"/>
+      <c r="F81" s="46"/>
+      <c r="G81" s="46"/>
+      <c r="H81" s="46"/>
+      <c r="I81" s="46"/>
+      <c r="J81" s="15"/>
+      <c r="K81" s="15"/>
+      <c r="L81" s="15"/>
+      <c r="M81" s="15"/>
+      <c r="N81" s="15"/>
+      <c r="O81" s="15"/>
+      <c r="P81" s="15"/>
+      <c r="Q81" s="15"/>
+      <c r="R81" s="15"/>
+      <c r="S81" s="15"/>
+      <c r="T81" s="15"/>
+      <c r="U81" s="15"/>
+      <c r="V81" s="15"/>
+      <c r="W81" s="15"/>
+      <c r="X81" s="15"/>
+      <c r="Y81" s="15"/>
+      <c r="Z81" s="15"/>
+      <c r="AA81" s="15"/>
+      <c r="AB81" s="15"/>
+      <c r="AC81" s="15"/>
+      <c r="AD81" s="15"/>
+      <c r="AE81" s="15"/>
+      <c r="AF81" s="15"/>
+      <c r="AG81" s="15"/>
+      <c r="AH81" s="15"/>
+      <c r="AI81" s="15"/>
+      <c r="AJ81" s="15"/>
+      <c r="AK81" s="15"/>
+      <c r="AL81" s="15"/>
+      <c r="AM81" s="15"/>
+      <c r="AN81" s="15"/>
+      <c r="AO81" s="15"/>
+      <c r="AP81" s="15"/>
+      <c r="AQ81" s="15"/>
+      <c r="AR81" s="15"/>
+      <c r="AS81" s="15"/>
+      <c r="AT81" s="15"/>
+      <c r="AU81" s="15"/>
+      <c r="AV81" s="15"/>
+      <c r="AW81" s="15"/>
+      <c r="AX81" s="15"/>
+      <c r="AY81" s="15"/>
+      <c r="AZ81" s="15"/>
+      <c r="BA81" s="15"/>
+      <c r="BB81" s="15"/>
+      <c r="BC81" s="15"/>
+      <c r="BD81" s="15"/>
+      <c r="BE81" s="15"/>
+      <c r="BF81" s="15"/>
+      <c r="BG81" s="15"/>
+      <c r="BH81" s="15"/>
+      <c r="BI81" s="15"/>
+      <c r="BJ81" s="15"/>
+      <c r="BK81" s="15"/>
+      <c r="BL81" s="15"/>
+      <c r="BM81" s="15"/>
+      <c r="BN81" s="15"/>
+      <c r="BO81" s="15"/>
+      <c r="BP81" s="15"/>
+    </row>
+    <row r="82" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A82" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" s="40"/>
       <c r="C82" s="50"/>
       <c r="D82" s="50"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B83" s="43">
-        <v>1</v>
-      </c>
-      <c r="C83" s="43">
-        <v>2</v>
-      </c>
-      <c r="D83" s="43"/>
-      <c r="E83" s="52"/>
-      <c r="F83" s="52"/>
-      <c r="G83" s="52"/>
-      <c r="H83" s="53"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B84" s="44">
-        <v>5</v>
-      </c>
-      <c r="C84" s="44">
-        <v>15</v>
-      </c>
-      <c r="D84" s="44">
-        <v>25</v>
-      </c>
-      <c r="E84" s="44"/>
-      <c r="F84" s="44"/>
-      <c r="G84" s="44"/>
-      <c r="H84" s="54"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B85" s="45"/>
+      <c r="E82" s="46"/>
+      <c r="F82" s="46"/>
+      <c r="G82" s="46"/>
+      <c r="H82" s="46"/>
+      <c r="I82" s="46"/>
+      <c r="J82" s="15"/>
+      <c r="K82" s="15"/>
+      <c r="L82" s="15"/>
+      <c r="M82" s="15"/>
+      <c r="N82" s="15"/>
+      <c r="O82" s="15"/>
+      <c r="P82" s="15"/>
+      <c r="Q82" s="15"/>
+      <c r="R82" s="15"/>
+      <c r="S82" s="15"/>
+      <c r="T82" s="15"/>
+      <c r="U82" s="15"/>
+      <c r="V82" s="15"/>
+      <c r="W82" s="15"/>
+      <c r="X82" s="15"/>
+      <c r="Y82" s="15"/>
+      <c r="Z82" s="15"/>
+      <c r="AA82" s="15"/>
+      <c r="AB82" s="15"/>
+      <c r="AC82" s="15"/>
+      <c r="AD82" s="15"/>
+      <c r="AE82" s="15"/>
+      <c r="AF82" s="15"/>
+      <c r="AG82" s="15"/>
+      <c r="AH82" s="15"/>
+      <c r="AI82" s="15"/>
+      <c r="AJ82" s="15"/>
+      <c r="AK82" s="15"/>
+      <c r="AL82" s="15"/>
+      <c r="AM82" s="15"/>
+      <c r="AN82" s="15"/>
+      <c r="AO82" s="15"/>
+      <c r="AP82" s="15"/>
+      <c r="AQ82" s="15"/>
+      <c r="AR82" s="15"/>
+      <c r="AS82" s="15"/>
+      <c r="AT82" s="15"/>
+      <c r="AU82" s="15"/>
+      <c r="AV82" s="15"/>
+      <c r="AW82" s="15"/>
+      <c r="AX82" s="15"/>
+      <c r="AY82" s="15"/>
+      <c r="AZ82" s="15"/>
+      <c r="BA82" s="15"/>
+      <c r="BB82" s="15"/>
+      <c r="BC82" s="15"/>
+      <c r="BD82" s="15"/>
+      <c r="BE82" s="15"/>
+      <c r="BF82" s="15"/>
+      <c r="BG82" s="15"/>
+      <c r="BH82" s="15"/>
+      <c r="BI82" s="15"/>
+      <c r="BJ82" s="15"/>
+      <c r="BK82" s="15"/>
+      <c r="BL82" s="15"/>
+      <c r="BM82" s="15"/>
+      <c r="BN82" s="15"/>
+      <c r="BO82" s="15"/>
+      <c r="BP82" s="15"/>
+    </row>
+    <row r="83" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A83" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B83" s="41"/>
+      <c r="C83" s="50"/>
+      <c r="D83" s="50"/>
+    </row>
+    <row r="84" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A84" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B84" s="42"/>
+      <c r="C84" s="65"/>
+      <c r="D84" s="65"/>
+    </row>
+    <row r="85" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A85" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B85" s="41"/>
       <c r="C85" s="50"/>
       <c r="D85" s="50"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B86" s="41"/>
-      <c r="C86" s="50"/>
-      <c r="D86" s="50"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B87" s="41"/>
-      <c r="C87" s="50"/>
-      <c r="D87" s="50"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B88" s="41"/>
+    <row r="86" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A86" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B86" s="43">
+        <v>1</v>
+      </c>
+      <c r="C86" s="43">
+        <v>2</v>
+      </c>
+      <c r="D86" s="43"/>
+      <c r="E86" s="52"/>
+      <c r="F86" s="52"/>
+      <c r="G86" s="52"/>
+      <c r="H86" s="53"/>
+    </row>
+    <row r="87" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A87" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B87" s="44">
+        <v>5</v>
+      </c>
+      <c r="C87" s="44">
+        <v>15</v>
+      </c>
+      <c r="D87" s="44">
+        <v>25</v>
+      </c>
+      <c r="E87" s="44"/>
+      <c r="F87" s="44"/>
+      <c r="G87" s="44"/>
+      <c r="H87" s="54"/>
+    </row>
+    <row r="88" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A88" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B88" s="45"/>
       <c r="C88" s="50"/>
       <c r="D88" s="50"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="B89" s="41"/>
       <c r="C89" s="50"/>
       <c r="D89" s="50"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="B90" s="41"/>
       <c r="C90" s="50"/>
       <c r="D90" s="50"/>
     </row>
-    <row r="91" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="B91" s="41"/>
       <c r="C91" s="50"/>
       <c r="D91" s="50"/>
-      <c r="E91" s="50"/>
-      <c r="F91" s="50"/>
-      <c r="G91" s="46"/>
-      <c r="H91" s="46"/>
-      <c r="I91" s="46"/>
-    </row>
-    <row r="92" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B92" s="41"/>
       <c r="C92" s="50"/>
       <c r="D92" s="50"/>
-      <c r="E92" s="50"/>
-      <c r="F92" s="50"/>
-      <c r="G92" s="46"/>
-      <c r="H92" s="46"/>
-      <c r="I92" s="46"/>
-    </row>
-    <row r="93" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B93" s="41"/>
       <c r="C93" s="50"/>
       <c r="D93" s="50"/>
-      <c r="E93" s="50"/>
-      <c r="F93" s="50"/>
-      <c r="G93" s="46"/>
-      <c r="H93" s="46"/>
-      <c r="I93" s="46"/>
-    </row>
-    <row r="94" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B94" s="41"/>
       <c r="C94" s="50"/>
@@ -3806,145 +3817,160 @@
       <c r="H94" s="46"/>
       <c r="I94" s="46"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B95" s="41"/>
       <c r="C95" s="50"/>
       <c r="D95" s="50"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E95" s="50"/>
+      <c r="F95" s="50"/>
+      <c r="G95" s="46"/>
+      <c r="H95" s="46"/>
+      <c r="I95" s="46"/>
+    </row>
+    <row r="96" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>58</v>
+        <v>121</v>
       </c>
       <c r="B96" s="41"/>
       <c r="C96" s="50"/>
       <c r="D96" s="50"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" s="50"/>
+      <c r="F96" s="50"/>
+      <c r="G96" s="46"/>
+      <c r="H96" s="46"/>
+      <c r="I96" s="46"/>
+    </row>
+    <row r="97" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B97" s="41"/>
       <c r="C97" s="50"/>
       <c r="D97" s="50"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" s="50"/>
+      <c r="F97" s="50"/>
+      <c r="G97" s="46"/>
+      <c r="H97" s="46"/>
+      <c r="I97" s="46"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
-        <v>122</v>
+        <v>57</v>
       </c>
       <c r="B98" s="41"/>
       <c r="C98" s="50"/>
       <c r="D98" s="50"/>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
-        <v>117</v>
+        <v>58</v>
       </c>
       <c r="B99" s="41"/>
       <c r="C99" s="50"/>
       <c r="D99" s="50"/>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
-        <v>118</v>
+        <v>59</v>
       </c>
       <c r="B100" s="41"/>
       <c r="C100" s="50"/>
       <c r="D100" s="50"/>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B101" s="61"/>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B101" s="41"/>
       <c r="C101" s="50"/>
       <c r="D101" s="50"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="B102" s="59"/>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B102" s="41"/>
       <c r="C102" s="50"/>
       <c r="D102" s="50"/>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="56" t="s">
-        <v>95</v>
-      </c>
-      <c r="B103" s="59"/>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B103" s="41"/>
       <c r="C103" s="50"/>
       <c r="D103" s="50"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="56" t="s">
-        <v>123</v>
-      </c>
-      <c r="B104" s="59"/>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="B104" s="61"/>
       <c r="C104" s="50"/>
       <c r="D104" s="50"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="56" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B105" s="59"/>
       <c r="C105" s="50"/>
       <c r="D105" s="50"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="56" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B106" s="59"/>
       <c r="C106" s="50"/>
       <c r="D106" s="50"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="56" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="B107" s="59"/>
       <c r="C107" s="50"/>
       <c r="D107" s="50"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="56" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="B108" s="59"/>
       <c r="C108" s="50"/>
       <c r="D108" s="50"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="56" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B109" s="59"/>
       <c r="C109" s="50"/>
       <c r="D109" s="50"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="57" t="s">
-        <v>91</v>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="56" t="s">
+        <v>97</v>
       </c>
       <c r="B110" s="59"/>
       <c r="C110" s="50"/>
       <c r="D110" s="50"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="57" t="s">
-        <v>99</v>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="56" t="s">
+        <v>124</v>
       </c>
       <c r="B111" s="59"/>
       <c r="C111" s="50"/>
       <c r="D111" s="50"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="56" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="B112" s="59"/>
       <c r="C112" s="50"/>
@@ -3952,7 +3978,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="57" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B113" s="59"/>
       <c r="C113" s="50"/>
@@ -3960,23 +3986,23 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="57" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B114" s="59"/>
       <c r="C114" s="50"/>
       <c r="D114" s="50"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="57" t="s">
-        <v>101</v>
+      <c r="A115" s="56" t="s">
+        <v>125</v>
       </c>
       <c r="B115" s="59"/>
       <c r="C115" s="50"/>
       <c r="D115" s="50"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="56" t="s">
-        <v>126</v>
+      <c r="A116" s="57" t="s">
+        <v>100</v>
       </c>
       <c r="B116" s="59"/>
       <c r="C116" s="50"/>
@@ -3984,7 +4010,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="57" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B117" s="59"/>
       <c r="C117" s="50"/>
@@ -3992,83 +4018,107 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="57" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B118" s="59"/>
       <c r="C118" s="50"/>
       <c r="D118" s="50"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="57" t="s">
-        <v>103</v>
+      <c r="A119" s="56" t="s">
+        <v>126</v>
       </c>
       <c r="B119" s="59"/>
       <c r="C119" s="50"/>
       <c r="D119" s="50"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="56" t="s">
-        <v>127</v>
+      <c r="A120" s="57" t="s">
+        <v>102</v>
       </c>
       <c r="B120" s="59"/>
+      <c r="C120" s="50"/>
+      <c r="D120" s="50"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="57" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B121" s="59"/>
+      <c r="C121" s="50"/>
+      <c r="D121" s="50"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="B122" s="59"/>
+      <c r="C122" s="50"/>
+      <c r="D122" s="50"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="B123" s="59"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="57" t="s">
+        <v>104</v>
+      </c>
+      <c r="B124" s="59"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="B122" s="59"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="57" t="s">
+      <c r="B125" s="59"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="B123" s="59"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="56" t="s">
+      <c r="B126" s="59"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="B124" s="59"/>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="58" t="s">
+      <c r="B127" s="59"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="58" t="s">
         <v>106</v>
       </c>
-      <c r="B125" s="60"/>
+      <c r="B128" s="60"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B80:D80 B65:D66">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83:D83 B68:D69">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B63:D64">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B66:D67">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B81:D81">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B84:D84">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B45:D62">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48:D65">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83:D83">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B86:D86">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B44:D44">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B47:D47">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72:D76">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75:D79">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -4082,13 +4132,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B85:D100 B67:D71 B77:D79</xm:sqref>
+          <xm:sqref>B88:D103 B70:D74 B80:D82</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B82:D82</xm:sqref>
+          <xm:sqref>B85:D85</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Various bits of tidying
New methods to tool_kit to make other code a little simpler.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="138">
   <si>
     <t>recent_time</t>
   </si>
@@ -414,6 +414,21 @@
   </si>
   <si>
     <t>program_nns_xpertacf_smearneg</t>
+  </si>
+  <si>
+    <t>program_ideal_detection</t>
+  </si>
+  <si>
+    <t>econ_unitcost_decentralisation</t>
+  </si>
+  <si>
+    <t>econ_inflectioncost_decentralisation</t>
+  </si>
+  <si>
+    <t>econ_saturation_decentralisation</t>
+  </si>
+  <si>
+    <t>econ_startingcost_duration_decentralisation</t>
   </si>
 </sst>
 </file>
@@ -2414,10 +2429,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP128"/>
+  <dimension ref="A1:BP133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,60 +2892,65 @@
       <c r="I43"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="50"/>
+      <c r="A44" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="66"/>
+      <c r="C44" s="66"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="67"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B45" s="25">
-        <v>25</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B45" s="25"/>
       <c r="C45" s="25"/>
       <c r="D45" s="25"/>
       <c r="E45" s="50"/>
       <c r="F45" s="50"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
+      <c r="A46" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" s="25">
+        <v>25</v>
+      </c>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
       <c r="E46" s="50"/>
       <c r="F46" s="50"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B47" s="28">
+      <c r="B48" s="28">
         <v>0.05</v>
       </c>
-      <c r="C47" s="50"/>
-      <c r="D47" s="50"/>
-      <c r="E47" s="46"/>
-      <c r="F47" s="46"/>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" s="29"/>
-      <c r="C48" s="62"/>
-      <c r="D48" s="62"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B49" s="29"/>
       <c r="C49" s="62"/>
@@ -2938,7 +2958,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="B50" s="29"/>
       <c r="C50" s="62"/>
@@ -2946,23 +2966,23 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B51" s="29"/>
       <c r="C51" s="62"/>
       <c r="D51" s="62"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B52" s="30"/>
-      <c r="C52" s="63"/>
-      <c r="D52" s="63"/>
+      <c r="A52" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" s="29"/>
+      <c r="C52" s="62"/>
+      <c r="D52" s="62"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B53" s="30"/>
       <c r="C53" s="63"/>
@@ -2970,23 +2990,23 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B54" s="30"/>
       <c r="C54" s="63"/>
       <c r="D54" s="63"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="29"/>
-      <c r="C55" s="62"/>
-      <c r="D55" s="62"/>
+      <c r="A55" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="30"/>
+      <c r="C55" s="63"/>
+      <c r="D55" s="63"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B56" s="29"/>
       <c r="C56" s="62"/>
@@ -2994,7 +3014,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B57" s="29"/>
       <c r="C57" s="62"/>
@@ -3002,7 +3022,7 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B58" s="29"/>
       <c r="C58" s="62"/>
@@ -3010,7 +3030,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B59" s="29"/>
       <c r="C59" s="62"/>
@@ -3018,45 +3038,45 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B60" s="29">
-        <v>1865</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B60" s="29"/>
       <c r="C60" s="62"/>
       <c r="D60" s="62"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B61" s="29">
-        <v>2036</v>
+        <v>1865</v>
       </c>
       <c r="C61" s="62"/>
       <c r="D61" s="62"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B62" s="29">
-        <v>1</v>
+        <v>2036</v>
       </c>
       <c r="C62" s="62"/>
       <c r="D62" s="62"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B63" s="29"/>
+        <v>111</v>
+      </c>
+      <c r="B63" s="29">
+        <v>1</v>
+      </c>
       <c r="C63" s="62"/>
       <c r="D63" s="62"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B64" s="29"/>
       <c r="C64" s="62"/>
@@ -3064,103 +3084,39 @@
     </row>
     <row r="65" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B65" s="31"/>
+        <v>119</v>
+      </c>
+      <c r="B65" s="29"/>
       <c r="C65" s="62"/>
       <c r="D65" s="62"/>
     </row>
     <row r="66" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A66" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B66" s="32"/>
+      <c r="A66" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B66" s="31"/>
       <c r="C66" s="62"/>
       <c r="D66" s="62"/>
     </row>
     <row r="67" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A67" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B67" s="33"/>
+      <c r="A67" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B67" s="32"/>
       <c r="C67" s="62"/>
       <c r="D67" s="62"/>
     </row>
     <row r="68" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B68" s="34"/>
+      <c r="A68" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B68" s="33"/>
       <c r="C68" s="62"/>
       <c r="D68" s="62"/>
-      <c r="E68" s="46"/>
-      <c r="F68" s="46"/>
-      <c r="G68" s="46"/>
-      <c r="H68" s="46"/>
-      <c r="I68" s="46"/>
-      <c r="J68" s="15"/>
-      <c r="K68" s="15"/>
-      <c r="L68" s="15"/>
-      <c r="M68" s="15"/>
-      <c r="N68" s="15"/>
-      <c r="O68" s="15"/>
-      <c r="P68" s="15"/>
-      <c r="Q68" s="15"/>
-      <c r="R68" s="15"/>
-      <c r="S68" s="15"/>
-      <c r="T68" s="15"/>
-      <c r="U68" s="15"/>
-      <c r="V68" s="15"/>
-      <c r="W68" s="15"/>
-      <c r="X68" s="15"/>
-      <c r="Y68" s="15"/>
-      <c r="Z68" s="15"/>
-      <c r="AA68" s="15"/>
-      <c r="AB68" s="15"/>
-      <c r="AC68" s="15"/>
-      <c r="AD68" s="15"/>
-      <c r="AE68" s="15"/>
-      <c r="AF68" s="15"/>
-      <c r="AG68" s="15"/>
-      <c r="AH68" s="15"/>
-      <c r="AI68" s="15"/>
-      <c r="AJ68" s="15"/>
-      <c r="AK68" s="15"/>
-      <c r="AL68" s="15"/>
-      <c r="AM68" s="15"/>
-      <c r="AN68" s="15"/>
-      <c r="AO68" s="15"/>
-      <c r="AP68" s="15"/>
-      <c r="AQ68" s="15"/>
-      <c r="AR68" s="15"/>
-      <c r="AS68" s="15"/>
-      <c r="AT68" s="15"/>
-      <c r="AU68" s="15"/>
-      <c r="AV68" s="15"/>
-      <c r="AW68" s="15"/>
-      <c r="AX68" s="15"/>
-      <c r="AY68" s="15"/>
-      <c r="AZ68" s="15"/>
-      <c r="BA68" s="15"/>
-      <c r="BB68" s="15"/>
-      <c r="BC68" s="15"/>
-      <c r="BD68" s="15"/>
-      <c r="BE68" s="15"/>
-      <c r="BF68" s="15"/>
-      <c r="BG68" s="15"/>
-      <c r="BH68" s="15"/>
-      <c r="BI68" s="15"/>
-      <c r="BJ68" s="15"/>
-      <c r="BK68" s="15"/>
-      <c r="BL68" s="15"/>
-      <c r="BM68" s="15"/>
-      <c r="BN68" s="15"/>
-      <c r="BO68" s="15"/>
-      <c r="BP68" s="15"/>
     </row>
     <row r="69" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A69" s="11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B69" s="34"/>
       <c r="C69" s="62"/>
@@ -3230,11 +3186,11 @@
       <c r="BO69" s="15"/>
       <c r="BP69" s="15"/>
     </row>
-    <row r="70" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B70" s="35"/>
+    <row r="70" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A70" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B70" s="34"/>
       <c r="C70" s="62"/>
       <c r="D70" s="62"/>
       <c r="E70" s="46"/>
@@ -3302,11 +3258,11 @@
       <c r="BO70" s="15"/>
       <c r="BP70" s="15"/>
     </row>
-    <row r="71" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B71" s="34"/>
+    <row r="71" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" s="35"/>
       <c r="C71" s="62"/>
       <c r="D71" s="62"/>
       <c r="E71" s="46"/>
@@ -3314,10 +3270,69 @@
       <c r="G71" s="46"/>
       <c r="H71" s="46"/>
       <c r="I71" s="46"/>
+      <c r="J71" s="15"/>
+      <c r="K71" s="15"/>
+      <c r="L71" s="15"/>
+      <c r="M71" s="15"/>
+      <c r="N71" s="15"/>
+      <c r="O71" s="15"/>
+      <c r="P71" s="15"/>
+      <c r="Q71" s="15"/>
+      <c r="R71" s="15"/>
+      <c r="S71" s="15"/>
+      <c r="T71" s="15"/>
+      <c r="U71" s="15"/>
+      <c r="V71" s="15"/>
+      <c r="W71" s="15"/>
+      <c r="X71" s="15"/>
+      <c r="Y71" s="15"/>
+      <c r="Z71" s="15"/>
+      <c r="AA71" s="15"/>
+      <c r="AB71" s="15"/>
+      <c r="AC71" s="15"/>
+      <c r="AD71" s="15"/>
+      <c r="AE71" s="15"/>
+      <c r="AF71" s="15"/>
+      <c r="AG71" s="15"/>
+      <c r="AH71" s="15"/>
+      <c r="AI71" s="15"/>
+      <c r="AJ71" s="15"/>
+      <c r="AK71" s="15"/>
+      <c r="AL71" s="15"/>
+      <c r="AM71" s="15"/>
+      <c r="AN71" s="15"/>
+      <c r="AO71" s="15"/>
+      <c r="AP71" s="15"/>
+      <c r="AQ71" s="15"/>
+      <c r="AR71" s="15"/>
+      <c r="AS71" s="15"/>
+      <c r="AT71" s="15"/>
+      <c r="AU71" s="15"/>
+      <c r="AV71" s="15"/>
+      <c r="AW71" s="15"/>
+      <c r="AX71" s="15"/>
+      <c r="AY71" s="15"/>
+      <c r="AZ71" s="15"/>
+      <c r="BA71" s="15"/>
+      <c r="BB71" s="15"/>
+      <c r="BC71" s="15"/>
+      <c r="BD71" s="15"/>
+      <c r="BE71" s="15"/>
+      <c r="BF71" s="15"/>
+      <c r="BG71" s="15"/>
+      <c r="BH71" s="15"/>
+      <c r="BI71" s="15"/>
+      <c r="BJ71" s="15"/>
+      <c r="BK71" s="15"/>
+      <c r="BL71" s="15"/>
+      <c r="BM71" s="15"/>
+      <c r="BN71" s="15"/>
+      <c r="BO71" s="15"/>
+      <c r="BP71" s="15"/>
     </row>
     <row r="72" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B72" s="34"/>
       <c r="C72" s="62"/>
@@ -3330,7 +3345,7 @@
     </row>
     <row r="73" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B73" s="34"/>
       <c r="C73" s="62"/>
@@ -3341,13 +3356,11 @@
       <c r="H73" s="46"/>
       <c r="I73" s="46"/>
     </row>
-    <row r="74" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B74" s="36" t="b">
-        <v>1</v>
-      </c>
+    <row r="74" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B74" s="34"/>
       <c r="C74" s="62"/>
       <c r="D74" s="62"/>
       <c r="E74" s="46"/>
@@ -3355,82 +3368,84 @@
       <c r="G74" s="46"/>
       <c r="H74" s="46"/>
       <c r="I74" s="46"/>
-      <c r="J74" s="15"/>
-      <c r="K74" s="15"/>
-      <c r="L74" s="15"/>
-      <c r="M74" s="15"/>
-      <c r="N74" s="15"/>
-      <c r="O74" s="15"/>
-      <c r="P74" s="15"/>
-      <c r="Q74" s="15"/>
-      <c r="R74" s="15"/>
-      <c r="S74" s="15"/>
-      <c r="T74" s="15"/>
-      <c r="U74" s="15"/>
-      <c r="V74" s="15"/>
-      <c r="W74" s="15"/>
-      <c r="X74" s="15"/>
-      <c r="Y74" s="15"/>
-      <c r="Z74" s="15"/>
-      <c r="AA74" s="15"/>
-      <c r="AB74" s="15"/>
-      <c r="AC74" s="15"/>
-      <c r="AD74" s="15"/>
-      <c r="AE74" s="15"/>
-      <c r="AF74" s="15"/>
-      <c r="AG74" s="15"/>
-      <c r="AH74" s="15"/>
-      <c r="AI74" s="15"/>
-      <c r="AJ74" s="15"/>
-      <c r="AK74" s="15"/>
-      <c r="AL74" s="15"/>
-      <c r="AM74" s="15"/>
-      <c r="AN74" s="15"/>
-      <c r="AO74" s="15"/>
-      <c r="AP74" s="15"/>
-      <c r="AQ74" s="15"/>
-      <c r="AR74" s="15"/>
-      <c r="AS74" s="15"/>
-      <c r="AT74" s="15"/>
-      <c r="AU74" s="15"/>
-      <c r="AV74" s="15"/>
-      <c r="AW74" s="15"/>
-      <c r="AX74" s="15"/>
-      <c r="AY74" s="15"/>
-      <c r="AZ74" s="15"/>
-      <c r="BA74" s="15"/>
-      <c r="BB74" s="15"/>
-      <c r="BC74" s="15"/>
-      <c r="BD74" s="15"/>
-      <c r="BE74" s="15"/>
-      <c r="BF74" s="15"/>
-      <c r="BG74" s="15"/>
-      <c r="BH74" s="15"/>
-      <c r="BI74" s="15"/>
-      <c r="BJ74" s="15"/>
-      <c r="BK74" s="15"/>
-      <c r="BL74" s="15"/>
-      <c r="BM74" s="15"/>
-      <c r="BN74" s="15"/>
-      <c r="BO74" s="15"/>
-      <c r="BP74" s="15"/>
-    </row>
-    <row r="75" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B75" s="37"/>
-      <c r="C75" s="64"/>
-      <c r="D75" s="64"/>
+    </row>
+    <row r="75" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B75" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="C75" s="62"/>
+      <c r="D75" s="62"/>
       <c r="E75" s="46"/>
       <c r="F75" s="46"/>
       <c r="G75" s="46"/>
       <c r="H75" s="46"/>
       <c r="I75" s="46"/>
+      <c r="J75" s="15"/>
+      <c r="K75" s="15"/>
+      <c r="L75" s="15"/>
+      <c r="M75" s="15"/>
+      <c r="N75" s="15"/>
+      <c r="O75" s="15"/>
+      <c r="P75" s="15"/>
+      <c r="Q75" s="15"/>
+      <c r="R75" s="15"/>
+      <c r="S75" s="15"/>
+      <c r="T75" s="15"/>
+      <c r="U75" s="15"/>
+      <c r="V75" s="15"/>
+      <c r="W75" s="15"/>
+      <c r="X75" s="15"/>
+      <c r="Y75" s="15"/>
+      <c r="Z75" s="15"/>
+      <c r="AA75" s="15"/>
+      <c r="AB75" s="15"/>
+      <c r="AC75" s="15"/>
+      <c r="AD75" s="15"/>
+      <c r="AE75" s="15"/>
+      <c r="AF75" s="15"/>
+      <c r="AG75" s="15"/>
+      <c r="AH75" s="15"/>
+      <c r="AI75" s="15"/>
+      <c r="AJ75" s="15"/>
+      <c r="AK75" s="15"/>
+      <c r="AL75" s="15"/>
+      <c r="AM75" s="15"/>
+      <c r="AN75" s="15"/>
+      <c r="AO75" s="15"/>
+      <c r="AP75" s="15"/>
+      <c r="AQ75" s="15"/>
+      <c r="AR75" s="15"/>
+      <c r="AS75" s="15"/>
+      <c r="AT75" s="15"/>
+      <c r="AU75" s="15"/>
+      <c r="AV75" s="15"/>
+      <c r="AW75" s="15"/>
+      <c r="AX75" s="15"/>
+      <c r="AY75" s="15"/>
+      <c r="AZ75" s="15"/>
+      <c r="BA75" s="15"/>
+      <c r="BB75" s="15"/>
+      <c r="BC75" s="15"/>
+      <c r="BD75" s="15"/>
+      <c r="BE75" s="15"/>
+      <c r="BF75" s="15"/>
+      <c r="BG75" s="15"/>
+      <c r="BH75" s="15"/>
+      <c r="BI75" s="15"/>
+      <c r="BJ75" s="15"/>
+      <c r="BK75" s="15"/>
+      <c r="BL75" s="15"/>
+      <c r="BM75" s="15"/>
+      <c r="BN75" s="15"/>
+      <c r="BO75" s="15"/>
+      <c r="BP75" s="15"/>
     </row>
     <row r="76" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B76" s="37"/>
       <c r="C76" s="64"/>
@@ -3443,7 +3458,7 @@
     </row>
     <row r="77" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" s="37"/>
       <c r="C77" s="64"/>
@@ -3456,7 +3471,7 @@
     </row>
     <row r="78" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" s="37"/>
       <c r="C78" s="64"/>
@@ -3468,12 +3483,10 @@
       <c r="I78" s="46"/>
     </row>
     <row r="79" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B79" s="38">
-        <v>0.156</v>
-      </c>
+      <c r="A79" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79" s="37"/>
       <c r="C79" s="64"/>
       <c r="D79" s="64"/>
       <c r="E79" s="46"/>
@@ -3482,81 +3495,24 @@
       <c r="H79" s="46"/>
       <c r="I79" s="46"/>
     </row>
-    <row r="80" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B80" s="39"/>
-      <c r="C80" s="50"/>
-      <c r="D80" s="50"/>
+    <row r="80" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" s="38">
+        <v>0.156</v>
+      </c>
+      <c r="C80" s="64"/>
+      <c r="D80" s="64"/>
       <c r="E80" s="46"/>
       <c r="F80" s="46"/>
       <c r="G80" s="46"/>
       <c r="H80" s="46"/>
       <c r="I80" s="46"/>
-      <c r="J80" s="15"/>
-      <c r="K80" s="15"/>
-      <c r="L80" s="15"/>
-      <c r="M80" s="15"/>
-      <c r="N80" s="15"/>
-      <c r="O80" s="15"/>
-      <c r="P80" s="15"/>
-      <c r="Q80" s="15"/>
-      <c r="R80" s="15"/>
-      <c r="S80" s="15"/>
-      <c r="T80" s="15"/>
-      <c r="U80" s="15"/>
-      <c r="V80" s="15"/>
-      <c r="W80" s="15"/>
-      <c r="X80" s="15"/>
-      <c r="Y80" s="15"/>
-      <c r="Z80" s="15"/>
-      <c r="AA80" s="15"/>
-      <c r="AB80" s="15"/>
-      <c r="AC80" s="15"/>
-      <c r="AD80" s="15"/>
-      <c r="AE80" s="15"/>
-      <c r="AF80" s="15"/>
-      <c r="AG80" s="15"/>
-      <c r="AH80" s="15"/>
-      <c r="AI80" s="15"/>
-      <c r="AJ80" s="15"/>
-      <c r="AK80" s="15"/>
-      <c r="AL80" s="15"/>
-      <c r="AM80" s="15"/>
-      <c r="AN80" s="15"/>
-      <c r="AO80" s="15"/>
-      <c r="AP80" s="15"/>
-      <c r="AQ80" s="15"/>
-      <c r="AR80" s="15"/>
-      <c r="AS80" s="15"/>
-      <c r="AT80" s="15"/>
-      <c r="AU80" s="15"/>
-      <c r="AV80" s="15"/>
-      <c r="AW80" s="15"/>
-      <c r="AX80" s="15"/>
-      <c r="AY80" s="15"/>
-      <c r="AZ80" s="15"/>
-      <c r="BA80" s="15"/>
-      <c r="BB80" s="15"/>
-      <c r="BC80" s="15"/>
-      <c r="BD80" s="15"/>
-      <c r="BE80" s="15"/>
-      <c r="BF80" s="15"/>
-      <c r="BG80" s="15"/>
-      <c r="BH80" s="15"/>
-      <c r="BI80" s="15"/>
-      <c r="BJ80" s="15"/>
-      <c r="BK80" s="15"/>
-      <c r="BL80" s="15"/>
-      <c r="BM80" s="15"/>
-      <c r="BN80" s="15"/>
-      <c r="BO80" s="15"/>
-      <c r="BP80" s="15"/>
     </row>
     <row r="81" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B81" s="39"/>
       <c r="C81" s="50"/>
@@ -3627,10 +3583,10 @@
       <c r="BP81" s="15"/>
     </row>
     <row r="82" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A82" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B82" s="40"/>
+      <c r="A82" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82" s="39"/>
       <c r="C82" s="50"/>
       <c r="D82" s="50"/>
       <c r="E82" s="46"/>
@@ -3699,82 +3655,146 @@
       <c r="BP82" s="15"/>
     </row>
     <row r="83" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A83" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B83" s="41"/>
+      <c r="A83" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" s="40"/>
       <c r="C83" s="50"/>
       <c r="D83" s="50"/>
+      <c r="E83" s="46"/>
+      <c r="F83" s="46"/>
+      <c r="G83" s="46"/>
+      <c r="H83" s="46"/>
+      <c r="I83" s="46"/>
+      <c r="J83" s="15"/>
+      <c r="K83" s="15"/>
+      <c r="L83" s="15"/>
+      <c r="M83" s="15"/>
+      <c r="N83" s="15"/>
+      <c r="O83" s="15"/>
+      <c r="P83" s="15"/>
+      <c r="Q83" s="15"/>
+      <c r="R83" s="15"/>
+      <c r="S83" s="15"/>
+      <c r="T83" s="15"/>
+      <c r="U83" s="15"/>
+      <c r="V83" s="15"/>
+      <c r="W83" s="15"/>
+      <c r="X83" s="15"/>
+      <c r="Y83" s="15"/>
+      <c r="Z83" s="15"/>
+      <c r="AA83" s="15"/>
+      <c r="AB83" s="15"/>
+      <c r="AC83" s="15"/>
+      <c r="AD83" s="15"/>
+      <c r="AE83" s="15"/>
+      <c r="AF83" s="15"/>
+      <c r="AG83" s="15"/>
+      <c r="AH83" s="15"/>
+      <c r="AI83" s="15"/>
+      <c r="AJ83" s="15"/>
+      <c r="AK83" s="15"/>
+      <c r="AL83" s="15"/>
+      <c r="AM83" s="15"/>
+      <c r="AN83" s="15"/>
+      <c r="AO83" s="15"/>
+      <c r="AP83" s="15"/>
+      <c r="AQ83" s="15"/>
+      <c r="AR83" s="15"/>
+      <c r="AS83" s="15"/>
+      <c r="AT83" s="15"/>
+      <c r="AU83" s="15"/>
+      <c r="AV83" s="15"/>
+      <c r="AW83" s="15"/>
+      <c r="AX83" s="15"/>
+      <c r="AY83" s="15"/>
+      <c r="AZ83" s="15"/>
+      <c r="BA83" s="15"/>
+      <c r="BB83" s="15"/>
+      <c r="BC83" s="15"/>
+      <c r="BD83" s="15"/>
+      <c r="BE83" s="15"/>
+      <c r="BF83" s="15"/>
+      <c r="BG83" s="15"/>
+      <c r="BH83" s="15"/>
+      <c r="BI83" s="15"/>
+      <c r="BJ83" s="15"/>
+      <c r="BK83" s="15"/>
+      <c r="BL83" s="15"/>
+      <c r="BM83" s="15"/>
+      <c r="BN83" s="15"/>
+      <c r="BO83" s="15"/>
+      <c r="BP83" s="15"/>
     </row>
     <row r="84" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A84" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B84" s="42"/>
-      <c r="C84" s="65"/>
-      <c r="D84" s="65"/>
+        <v>9</v>
+      </c>
+      <c r="B84" s="41"/>
+      <c r="C84" s="50"/>
+      <c r="D84" s="50"/>
     </row>
     <row r="85" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A85" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B85" s="42"/>
+      <c r="C85" s="65"/>
+      <c r="D85" s="65"/>
+    </row>
+    <row r="86" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A86" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B85" s="41"/>
-      <c r="C85" s="50"/>
-      <c r="D85" s="50"/>
-    </row>
-    <row r="86" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A86" s="17" t="s">
+      <c r="B86" s="41"/>
+      <c r="C86" s="50"/>
+      <c r="D86" s="50"/>
+    </row>
+    <row r="87" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A87" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B86" s="43">
+      <c r="B87" s="43">
         <v>1</v>
       </c>
-      <c r="C86" s="43">
+      <c r="C87" s="43">
         <v>2</v>
       </c>
-      <c r="D86" s="43"/>
-      <c r="E86" s="52"/>
-      <c r="F86" s="52"/>
-      <c r="G86" s="52"/>
-      <c r="H86" s="53"/>
-    </row>
-    <row r="87" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A87" s="16" t="s">
+      <c r="D87" s="43"/>
+      <c r="E87" s="52"/>
+      <c r="F87" s="52"/>
+      <c r="G87" s="52"/>
+      <c r="H87" s="53"/>
+    </row>
+    <row r="88" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A88" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B87" s="44">
+      <c r="B88" s="44">
         <v>5</v>
       </c>
-      <c r="C87" s="44">
+      <c r="C88" s="44">
         <v>15</v>
       </c>
-      <c r="D87" s="44">
+      <c r="D88" s="44">
         <v>25</v>
       </c>
-      <c r="E87" s="44"/>
-      <c r="F87" s="44"/>
-      <c r="G87" s="44"/>
-      <c r="H87" s="54"/>
-    </row>
-    <row r="88" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A88" s="18" t="s">
+      <c r="E88" s="44"/>
+      <c r="F88" s="44"/>
+      <c r="G88" s="44"/>
+      <c r="H88" s="54"/>
+    </row>
+    <row r="89" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A89" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B88" s="45"/>
-      <c r="C88" s="50"/>
-      <c r="D88" s="50"/>
-    </row>
-    <row r="89" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A89" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B89" s="41"/>
+      <c r="B89" s="45"/>
       <c r="C89" s="50"/>
       <c r="D89" s="50"/>
     </row>
     <row r="90" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B90" s="41"/>
       <c r="C90" s="50"/>
@@ -3782,7 +3802,7 @@
     </row>
     <row r="91" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B91" s="41"/>
       <c r="C91" s="50"/>
@@ -3790,7 +3810,7 @@
     </row>
     <row r="92" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="B92" s="41"/>
       <c r="C92" s="50"/>
@@ -3798,28 +3818,23 @@
     </row>
     <row r="93" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="B93" s="41"/>
       <c r="C93" s="50"/>
       <c r="D93" s="50"/>
     </row>
-    <row r="94" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
       <c r="B94" s="41"/>
       <c r="C94" s="50"/>
       <c r="D94" s="50"/>
-      <c r="E94" s="50"/>
-      <c r="F94" s="50"/>
-      <c r="G94" s="46"/>
-      <c r="H94" s="46"/>
-      <c r="I94" s="46"/>
     </row>
     <row r="95" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B95" s="41"/>
       <c r="C95" s="50"/>
@@ -3832,7 +3847,7 @@
     </row>
     <row r="96" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>121</v>
+        <v>69</v>
       </c>
       <c r="B96" s="41"/>
       <c r="C96" s="50"/>
@@ -3845,7 +3860,7 @@
     </row>
     <row r="97" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="B97" s="41"/>
       <c r="C97" s="50"/>
@@ -3856,17 +3871,22 @@
       <c r="H97" s="46"/>
       <c r="I97" s="46"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="B98" s="41"/>
       <c r="C98" s="50"/>
       <c r="D98" s="50"/>
+      <c r="E98" s="50"/>
+      <c r="F98" s="50"/>
+      <c r="G98" s="46"/>
+      <c r="H98" s="46"/>
+      <c r="I98" s="46"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B99" s="41"/>
       <c r="C99" s="50"/>
@@ -3874,7 +3894,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B100" s="41"/>
       <c r="C100" s="50"/>
@@ -3882,7 +3902,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="B101" s="41"/>
       <c r="C101" s="50"/>
@@ -3890,7 +3910,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="B102" s="41"/>
       <c r="C102" s="50"/>
@@ -3898,31 +3918,31 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B103" s="41"/>
       <c r="C103" s="50"/>
       <c r="D103" s="50"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B104" s="61"/>
+      <c r="A104" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B104" s="41"/>
       <c r="C104" s="50"/>
       <c r="D104" s="50"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="B105" s="59"/>
+      <c r="A105" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="B105" s="61"/>
       <c r="C105" s="50"/>
       <c r="D105" s="50"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="56" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B106" s="59"/>
       <c r="C106" s="50"/>
@@ -3930,7 +3950,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="56" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="B107" s="59"/>
       <c r="C107" s="50"/>
@@ -3938,7 +3958,7 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="56" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="B108" s="59"/>
       <c r="C108" s="50"/>
@@ -3946,7 +3966,7 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="56" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B109" s="59"/>
       <c r="C109" s="50"/>
@@ -3954,7 +3974,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="56" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B110" s="59"/>
       <c r="C110" s="50"/>
@@ -3962,7 +3982,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="56" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B111" s="59"/>
       <c r="C111" s="50"/>
@@ -3970,15 +3990,15 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="56" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="B112" s="59"/>
       <c r="C112" s="50"/>
       <c r="D112" s="50"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="57" t="s">
-        <v>91</v>
+      <c r="A113" s="56" t="s">
+        <v>98</v>
       </c>
       <c r="B113" s="59"/>
       <c r="C113" s="50"/>
@@ -3986,23 +4006,23 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="57" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B114" s="59"/>
       <c r="C114" s="50"/>
       <c r="D114" s="50"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="56" t="s">
-        <v>125</v>
+      <c r="A115" s="57" t="s">
+        <v>99</v>
       </c>
       <c r="B115" s="59"/>
       <c r="C115" s="50"/>
       <c r="D115" s="50"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="57" t="s">
-        <v>100</v>
+      <c r="A116" s="56" t="s">
+        <v>125</v>
       </c>
       <c r="B116" s="59"/>
       <c r="C116" s="50"/>
@@ -4010,7 +4030,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="57" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B117" s="59"/>
       <c r="C117" s="50"/>
@@ -4018,23 +4038,23 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="57" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B118" s="59"/>
       <c r="C118" s="50"/>
       <c r="D118" s="50"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="56" t="s">
-        <v>126</v>
+      <c r="A119" s="57" t="s">
+        <v>101</v>
       </c>
       <c r="B119" s="59"/>
       <c r="C119" s="50"/>
       <c r="D119" s="50"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="57" t="s">
-        <v>102</v>
+      <c r="A120" s="56" t="s">
+        <v>126</v>
       </c>
       <c r="B120" s="59"/>
       <c r="C120" s="50"/>
@@ -4042,7 +4062,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="57" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B121" s="59"/>
       <c r="C121" s="50"/>
@@ -4050,75 +4070,107 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="57" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B122" s="59"/>
       <c r="C122" s="50"/>
       <c r="D122" s="50"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="56" t="s">
+      <c r="A123" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="B123" s="59"/>
+      <c r="C123" s="50"/>
+      <c r="D123" s="50"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="56" t="s">
         <v>127</v>
-      </c>
-      <c r="B123" s="59"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="57" t="s">
-        <v>104</v>
       </c>
       <c r="B124" s="59"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="57" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B125" s="59"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B126" s="59"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="B126" s="59"/>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="56" t="s">
+      <c r="B127" s="59"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="B127" s="59"/>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="58" t="s">
+      <c r="B128" s="59"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="B128" s="60"/>
+      <c r="B129" s="59"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="B130" s="59"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="57" t="s">
+        <v>135</v>
+      </c>
+      <c r="B131" s="59"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="B132" s="59"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="B133" s="60"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83:D83 B68:D69">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B84:D84 B69:D70">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B66:D67">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B67:D68">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B84:D84">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B85:D85">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48:D65">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B49:D66">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B86:D86">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87:D87">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B47:D47">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48:D48">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75:D79">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B76:D80">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -4132,13 +4184,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B88:D103 B70:D74 B80:D82</xm:sqref>
+          <xm:sqref>B89:D104 B71:D75 B81:D83</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B85:D85</xm:sqref>
+          <xm:sqref>B86:D86</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Allow separate years for cost-curve plotting
Previously kept plotting from very early in model with rapid time steps.
Avoid this behaviour, by separating the time inputs for cost-coverage
curves from those for the report.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="141">
   <si>
     <t>recent_time</t>
   </si>
@@ -429,6 +429,15 @@
   </si>
   <si>
     <t>econ_startingcost_duration_decentralisation</t>
+  </si>
+  <si>
+    <t>cost_curve_start_time</t>
+  </si>
+  <si>
+    <t>cost_curve_end_time</t>
+  </si>
+  <si>
+    <t>cost_curve_step_time</t>
   </si>
 </sst>
 </file>
@@ -1380,7 +1389,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1459,6 +1468,11 @@
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2429,10 +2443,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP133"/>
+  <dimension ref="A1:BP136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2948,7 +2962,7 @@
       <c r="E48" s="46"/>
       <c r="F48" s="46"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>52</v>
       </c>
@@ -2956,7 +2970,7 @@
       <c r="C49" s="62"/>
       <c r="D49" s="62"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>82</v>
       </c>
@@ -2964,7 +2978,7 @@
       <c r="C50" s="62"/>
       <c r="D50" s="62"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>13</v>
       </c>
@@ -2972,7 +2986,7 @@
       <c r="C51" s="62"/>
       <c r="D51" s="62"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>14</v>
       </c>
@@ -2980,7 +2994,7 @@
       <c r="C52" s="62"/>
       <c r="D52" s="62"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>113</v>
       </c>
@@ -2988,7 +3002,7 @@
       <c r="C53" s="63"/>
       <c r="D53" s="63"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>114</v>
       </c>
@@ -2996,7 +3010,7 @@
       <c r="C54" s="63"/>
       <c r="D54" s="63"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>115</v>
       </c>
@@ -3004,7 +3018,7 @@
       <c r="C55" s="63"/>
       <c r="D55" s="63"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>0</v>
       </c>
@@ -3012,7 +3026,7 @@
       <c r="C56" s="62"/>
       <c r="D56" s="62"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>11</v>
       </c>
@@ -3020,7 +3034,7 @@
       <c r="C57" s="62"/>
       <c r="D57" s="62"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>13</v>
       </c>
@@ -3028,23 +3042,29 @@
       <c r="C58" s="62"/>
       <c r="D58" s="62"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B59" s="29"/>
       <c r="C59" s="62"/>
       <c r="D59" s="62"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="69"/>
+      <c r="F59" s="69"/>
+      <c r="G59" s="69"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B60" s="29"/>
       <c r="C60" s="62"/>
       <c r="D60" s="62"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="69"/>
+      <c r="F60" s="69"/>
+      <c r="G60" s="69"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>109</v>
       </c>
@@ -3053,8 +3073,11 @@
       </c>
       <c r="C61" s="62"/>
       <c r="D61" s="62"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="69"/>
+      <c r="F61" s="69"/>
+      <c r="G61" s="69"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>110</v>
       </c>
@@ -3063,8 +3086,11 @@
       </c>
       <c r="C62" s="62"/>
       <c r="D62" s="62"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="69"/>
+      <c r="F62" s="69"/>
+      <c r="G62" s="69"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>111</v>
       </c>
@@ -3073,309 +3099,325 @@
       </c>
       <c r="C63" s="62"/>
       <c r="D63" s="62"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="69"/>
+      <c r="F63" s="69"/>
+      <c r="G63" s="69"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B64" s="29"/>
-      <c r="C64" s="62"/>
-      <c r="D64" s="62"/>
+        <v>138</v>
+      </c>
+      <c r="B64" s="68"/>
+      <c r="C64" s="70"/>
+      <c r="D64" s="70"/>
+      <c r="E64" s="71"/>
+      <c r="F64" s="72"/>
+      <c r="G64" s="72"/>
+      <c r="H64"/>
+      <c r="I64"/>
     </row>
     <row r="65" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="B65" s="29"/>
-      <c r="C65" s="62"/>
-      <c r="D65" s="62"/>
+        <v>139</v>
+      </c>
+      <c r="B65" s="68"/>
+      <c r="C65" s="70"/>
+      <c r="D65" s="70"/>
+      <c r="E65" s="71"/>
+      <c r="F65" s="72"/>
+      <c r="G65" s="72"/>
+      <c r="H65"/>
+      <c r="I65"/>
     </row>
     <row r="66" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B66" s="31"/>
-      <c r="C66" s="62"/>
-      <c r="D66" s="62"/>
+        <v>140</v>
+      </c>
+      <c r="B66" s="68"/>
+      <c r="C66" s="70"/>
+      <c r="D66" s="70"/>
+      <c r="E66" s="71"/>
+      <c r="F66" s="72"/>
+      <c r="G66" s="72"/>
+      <c r="H66"/>
+      <c r="I66"/>
     </row>
     <row r="67" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A67" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B67" s="32"/>
+      <c r="A67" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B67" s="29"/>
       <c r="C67" s="62"/>
       <c r="D67" s="62"/>
+      <c r="E67" s="69"/>
+      <c r="F67" s="69"/>
+      <c r="G67" s="69"/>
     </row>
     <row r="68" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A68" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B68" s="33"/>
+      <c r="A68" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B68" s="29"/>
       <c r="C68" s="62"/>
       <c r="D68" s="62"/>
+      <c r="E68" s="69"/>
+      <c r="F68" s="69"/>
+      <c r="G68" s="69"/>
     </row>
     <row r="69" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A69" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B69" s="34"/>
+      <c r="A69" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B69" s="31"/>
       <c r="C69" s="62"/>
       <c r="D69" s="62"/>
-      <c r="E69" s="46"/>
-      <c r="F69" s="46"/>
-      <c r="G69" s="46"/>
-      <c r="H69" s="46"/>
-      <c r="I69" s="46"/>
-      <c r="J69" s="15"/>
-      <c r="K69" s="15"/>
-      <c r="L69" s="15"/>
-      <c r="M69" s="15"/>
-      <c r="N69" s="15"/>
-      <c r="O69" s="15"/>
-      <c r="P69" s="15"/>
-      <c r="Q69" s="15"/>
-      <c r="R69" s="15"/>
-      <c r="S69" s="15"/>
-      <c r="T69" s="15"/>
-      <c r="U69" s="15"/>
-      <c r="V69" s="15"/>
-      <c r="W69" s="15"/>
-      <c r="X69" s="15"/>
-      <c r="Y69" s="15"/>
-      <c r="Z69" s="15"/>
-      <c r="AA69" s="15"/>
-      <c r="AB69" s="15"/>
-      <c r="AC69" s="15"/>
-      <c r="AD69" s="15"/>
-      <c r="AE69" s="15"/>
-      <c r="AF69" s="15"/>
-      <c r="AG69" s="15"/>
-      <c r="AH69" s="15"/>
-      <c r="AI69" s="15"/>
-      <c r="AJ69" s="15"/>
-      <c r="AK69" s="15"/>
-      <c r="AL69" s="15"/>
-      <c r="AM69" s="15"/>
-      <c r="AN69" s="15"/>
-      <c r="AO69" s="15"/>
-      <c r="AP69" s="15"/>
-      <c r="AQ69" s="15"/>
-      <c r="AR69" s="15"/>
-      <c r="AS69" s="15"/>
-      <c r="AT69" s="15"/>
-      <c r="AU69" s="15"/>
-      <c r="AV69" s="15"/>
-      <c r="AW69" s="15"/>
-      <c r="AX69" s="15"/>
-      <c r="AY69" s="15"/>
-      <c r="AZ69" s="15"/>
-      <c r="BA69" s="15"/>
-      <c r="BB69" s="15"/>
-      <c r="BC69" s="15"/>
-      <c r="BD69" s="15"/>
-      <c r="BE69" s="15"/>
-      <c r="BF69" s="15"/>
-      <c r="BG69" s="15"/>
-      <c r="BH69" s="15"/>
-      <c r="BI69" s="15"/>
-      <c r="BJ69" s="15"/>
-      <c r="BK69" s="15"/>
-      <c r="BL69" s="15"/>
-      <c r="BM69" s="15"/>
-      <c r="BN69" s="15"/>
-      <c r="BO69" s="15"/>
-      <c r="BP69" s="15"/>
+      <c r="E69" s="69"/>
+      <c r="F69" s="69"/>
+      <c r="G69" s="69"/>
     </row>
     <row r="70" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A70" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B70" s="34"/>
+      <c r="A70" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B70" s="32"/>
       <c r="C70" s="62"/>
       <c r="D70" s="62"/>
-      <c r="E70" s="46"/>
-      <c r="F70" s="46"/>
-      <c r="G70" s="46"/>
-      <c r="H70" s="46"/>
-      <c r="I70" s="46"/>
-      <c r="J70" s="15"/>
-      <c r="K70" s="15"/>
-      <c r="L70" s="15"/>
-      <c r="M70" s="15"/>
-      <c r="N70" s="15"/>
-      <c r="O70" s="15"/>
-      <c r="P70" s="15"/>
-      <c r="Q70" s="15"/>
-      <c r="R70" s="15"/>
-      <c r="S70" s="15"/>
-      <c r="T70" s="15"/>
-      <c r="U70" s="15"/>
-      <c r="V70" s="15"/>
-      <c r="W70" s="15"/>
-      <c r="X70" s="15"/>
-      <c r="Y70" s="15"/>
-      <c r="Z70" s="15"/>
-      <c r="AA70" s="15"/>
-      <c r="AB70" s="15"/>
-      <c r="AC70" s="15"/>
-      <c r="AD70" s="15"/>
-      <c r="AE70" s="15"/>
-      <c r="AF70" s="15"/>
-      <c r="AG70" s="15"/>
-      <c r="AH70" s="15"/>
-      <c r="AI70" s="15"/>
-      <c r="AJ70" s="15"/>
-      <c r="AK70" s="15"/>
-      <c r="AL70" s="15"/>
-      <c r="AM70" s="15"/>
-      <c r="AN70" s="15"/>
-      <c r="AO70" s="15"/>
-      <c r="AP70" s="15"/>
-      <c r="AQ70" s="15"/>
-      <c r="AR70" s="15"/>
-      <c r="AS70" s="15"/>
-      <c r="AT70" s="15"/>
-      <c r="AU70" s="15"/>
-      <c r="AV70" s="15"/>
-      <c r="AW70" s="15"/>
-      <c r="AX70" s="15"/>
-      <c r="AY70" s="15"/>
-      <c r="AZ70" s="15"/>
-      <c r="BA70" s="15"/>
-      <c r="BB70" s="15"/>
-      <c r="BC70" s="15"/>
-      <c r="BD70" s="15"/>
-      <c r="BE70" s="15"/>
-      <c r="BF70" s="15"/>
-      <c r="BG70" s="15"/>
-      <c r="BH70" s="15"/>
-      <c r="BI70" s="15"/>
-      <c r="BJ70" s="15"/>
-      <c r="BK70" s="15"/>
-      <c r="BL70" s="15"/>
-      <c r="BM70" s="15"/>
-      <c r="BN70" s="15"/>
-      <c r="BO70" s="15"/>
-      <c r="BP70" s="15"/>
-    </row>
-    <row r="71" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B71" s="35"/>
+      <c r="E70" s="69"/>
+      <c r="F70" s="69"/>
+      <c r="G70" s="69"/>
+    </row>
+    <row r="71" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A71" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B71" s="33"/>
       <c r="C71" s="62"/>
       <c r="D71" s="62"/>
-      <c r="E71" s="46"/>
-      <c r="F71" s="46"/>
-      <c r="G71" s="46"/>
-      <c r="H71" s="46"/>
-      <c r="I71" s="46"/>
-      <c r="J71" s="15"/>
-      <c r="K71" s="15"/>
-      <c r="L71" s="15"/>
-      <c r="M71" s="15"/>
-      <c r="N71" s="15"/>
-      <c r="O71" s="15"/>
-      <c r="P71" s="15"/>
-      <c r="Q71" s="15"/>
-      <c r="R71" s="15"/>
-      <c r="S71" s="15"/>
-      <c r="T71" s="15"/>
-      <c r="U71" s="15"/>
-      <c r="V71" s="15"/>
-      <c r="W71" s="15"/>
-      <c r="X71" s="15"/>
-      <c r="Y71" s="15"/>
-      <c r="Z71" s="15"/>
-      <c r="AA71" s="15"/>
-      <c r="AB71" s="15"/>
-      <c r="AC71" s="15"/>
-      <c r="AD71" s="15"/>
-      <c r="AE71" s="15"/>
-      <c r="AF71" s="15"/>
-      <c r="AG71" s="15"/>
-      <c r="AH71" s="15"/>
-      <c r="AI71" s="15"/>
-      <c r="AJ71" s="15"/>
-      <c r="AK71" s="15"/>
-      <c r="AL71" s="15"/>
-      <c r="AM71" s="15"/>
-      <c r="AN71" s="15"/>
-      <c r="AO71" s="15"/>
-      <c r="AP71" s="15"/>
-      <c r="AQ71" s="15"/>
-      <c r="AR71" s="15"/>
-      <c r="AS71" s="15"/>
-      <c r="AT71" s="15"/>
-      <c r="AU71" s="15"/>
-      <c r="AV71" s="15"/>
-      <c r="AW71" s="15"/>
-      <c r="AX71" s="15"/>
-      <c r="AY71" s="15"/>
-      <c r="AZ71" s="15"/>
-      <c r="BA71" s="15"/>
-      <c r="BB71" s="15"/>
-      <c r="BC71" s="15"/>
-      <c r="BD71" s="15"/>
-      <c r="BE71" s="15"/>
-      <c r="BF71" s="15"/>
-      <c r="BG71" s="15"/>
-      <c r="BH71" s="15"/>
-      <c r="BI71" s="15"/>
-      <c r="BJ71" s="15"/>
-      <c r="BK71" s="15"/>
-      <c r="BL71" s="15"/>
-      <c r="BM71" s="15"/>
-      <c r="BN71" s="15"/>
-      <c r="BO71" s="15"/>
-      <c r="BP71" s="15"/>
-    </row>
-    <row r="72" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E71" s="69"/>
+      <c r="F71" s="69"/>
+      <c r="G71" s="69"/>
+    </row>
+    <row r="72" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>74</v>
+        <v>1</v>
       </c>
       <c r="B72" s="34"/>
       <c r="C72" s="62"/>
       <c r="D72" s="62"/>
-      <c r="E72" s="46"/>
-      <c r="F72" s="46"/>
-      <c r="G72" s="46"/>
+      <c r="E72" s="50"/>
+      <c r="F72" s="50"/>
+      <c r="G72" s="50"/>
       <c r="H72" s="46"/>
       <c r="I72" s="46"/>
-    </row>
-    <row r="73" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J72" s="15"/>
+      <c r="K72" s="15"/>
+      <c r="L72" s="15"/>
+      <c r="M72" s="15"/>
+      <c r="N72" s="15"/>
+      <c r="O72" s="15"/>
+      <c r="P72" s="15"/>
+      <c r="Q72" s="15"/>
+      <c r="R72" s="15"/>
+      <c r="S72" s="15"/>
+      <c r="T72" s="15"/>
+      <c r="U72" s="15"/>
+      <c r="V72" s="15"/>
+      <c r="W72" s="15"/>
+      <c r="X72" s="15"/>
+      <c r="Y72" s="15"/>
+      <c r="Z72" s="15"/>
+      <c r="AA72" s="15"/>
+      <c r="AB72" s="15"/>
+      <c r="AC72" s="15"/>
+      <c r="AD72" s="15"/>
+      <c r="AE72" s="15"/>
+      <c r="AF72" s="15"/>
+      <c r="AG72" s="15"/>
+      <c r="AH72" s="15"/>
+      <c r="AI72" s="15"/>
+      <c r="AJ72" s="15"/>
+      <c r="AK72" s="15"/>
+      <c r="AL72" s="15"/>
+      <c r="AM72" s="15"/>
+      <c r="AN72" s="15"/>
+      <c r="AO72" s="15"/>
+      <c r="AP72" s="15"/>
+      <c r="AQ72" s="15"/>
+      <c r="AR72" s="15"/>
+      <c r="AS72" s="15"/>
+      <c r="AT72" s="15"/>
+      <c r="AU72" s="15"/>
+      <c r="AV72" s="15"/>
+      <c r="AW72" s="15"/>
+      <c r="AX72" s="15"/>
+      <c r="AY72" s="15"/>
+      <c r="AZ72" s="15"/>
+      <c r="BA72" s="15"/>
+      <c r="BB72" s="15"/>
+      <c r="BC72" s="15"/>
+      <c r="BD72" s="15"/>
+      <c r="BE72" s="15"/>
+      <c r="BF72" s="15"/>
+      <c r="BG72" s="15"/>
+      <c r="BH72" s="15"/>
+      <c r="BI72" s="15"/>
+      <c r="BJ72" s="15"/>
+      <c r="BK72" s="15"/>
+      <c r="BL72" s="15"/>
+      <c r="BM72" s="15"/>
+      <c r="BN72" s="15"/>
+      <c r="BO72" s="15"/>
+      <c r="BP72" s="15"/>
+    </row>
+    <row r="73" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>73</v>
+        <v>2</v>
       </c>
       <c r="B73" s="34"/>
       <c r="C73" s="62"/>
       <c r="D73" s="62"/>
-      <c r="E73" s="46"/>
-      <c r="F73" s="46"/>
-      <c r="G73" s="46"/>
+      <c r="E73" s="50"/>
+      <c r="F73" s="50"/>
+      <c r="G73" s="50"/>
       <c r="H73" s="46"/>
       <c r="I73" s="46"/>
-    </row>
-    <row r="74" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B74" s="34"/>
+      <c r="J73" s="15"/>
+      <c r="K73" s="15"/>
+      <c r="L73" s="15"/>
+      <c r="M73" s="15"/>
+      <c r="N73" s="15"/>
+      <c r="O73" s="15"/>
+      <c r="P73" s="15"/>
+      <c r="Q73" s="15"/>
+      <c r="R73" s="15"/>
+      <c r="S73" s="15"/>
+      <c r="T73" s="15"/>
+      <c r="U73" s="15"/>
+      <c r="V73" s="15"/>
+      <c r="W73" s="15"/>
+      <c r="X73" s="15"/>
+      <c r="Y73" s="15"/>
+      <c r="Z73" s="15"/>
+      <c r="AA73" s="15"/>
+      <c r="AB73" s="15"/>
+      <c r="AC73" s="15"/>
+      <c r="AD73" s="15"/>
+      <c r="AE73" s="15"/>
+      <c r="AF73" s="15"/>
+      <c r="AG73" s="15"/>
+      <c r="AH73" s="15"/>
+      <c r="AI73" s="15"/>
+      <c r="AJ73" s="15"/>
+      <c r="AK73" s="15"/>
+      <c r="AL73" s="15"/>
+      <c r="AM73" s="15"/>
+      <c r="AN73" s="15"/>
+      <c r="AO73" s="15"/>
+      <c r="AP73" s="15"/>
+      <c r="AQ73" s="15"/>
+      <c r="AR73" s="15"/>
+      <c r="AS73" s="15"/>
+      <c r="AT73" s="15"/>
+      <c r="AU73" s="15"/>
+      <c r="AV73" s="15"/>
+      <c r="AW73" s="15"/>
+      <c r="AX73" s="15"/>
+      <c r="AY73" s="15"/>
+      <c r="AZ73" s="15"/>
+      <c r="BA73" s="15"/>
+      <c r="BB73" s="15"/>
+      <c r="BC73" s="15"/>
+      <c r="BD73" s="15"/>
+      <c r="BE73" s="15"/>
+      <c r="BF73" s="15"/>
+      <c r="BG73" s="15"/>
+      <c r="BH73" s="15"/>
+      <c r="BI73" s="15"/>
+      <c r="BJ73" s="15"/>
+      <c r="BK73" s="15"/>
+      <c r="BL73" s="15"/>
+      <c r="BM73" s="15"/>
+      <c r="BN73" s="15"/>
+      <c r="BO73" s="15"/>
+      <c r="BP73" s="15"/>
+    </row>
+    <row r="74" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B74" s="35"/>
       <c r="C74" s="62"/>
       <c r="D74" s="62"/>
-      <c r="E74" s="46"/>
-      <c r="F74" s="46"/>
-      <c r="G74" s="46"/>
+      <c r="E74" s="50"/>
+      <c r="F74" s="50"/>
+      <c r="G74" s="50"/>
       <c r="H74" s="46"/>
       <c r="I74" s="46"/>
-    </row>
-    <row r="75" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B75" s="36" t="b">
-        <v>1</v>
-      </c>
+      <c r="J74" s="15"/>
+      <c r="K74" s="15"/>
+      <c r="L74" s="15"/>
+      <c r="M74" s="15"/>
+      <c r="N74" s="15"/>
+      <c r="O74" s="15"/>
+      <c r="P74" s="15"/>
+      <c r="Q74" s="15"/>
+      <c r="R74" s="15"/>
+      <c r="S74" s="15"/>
+      <c r="T74" s="15"/>
+      <c r="U74" s="15"/>
+      <c r="V74" s="15"/>
+      <c r="W74" s="15"/>
+      <c r="X74" s="15"/>
+      <c r="Y74" s="15"/>
+      <c r="Z74" s="15"/>
+      <c r="AA74" s="15"/>
+      <c r="AB74" s="15"/>
+      <c r="AC74" s="15"/>
+      <c r="AD74" s="15"/>
+      <c r="AE74" s="15"/>
+      <c r="AF74" s="15"/>
+      <c r="AG74" s="15"/>
+      <c r="AH74" s="15"/>
+      <c r="AI74" s="15"/>
+      <c r="AJ74" s="15"/>
+      <c r="AK74" s="15"/>
+      <c r="AL74" s="15"/>
+      <c r="AM74" s="15"/>
+      <c r="AN74" s="15"/>
+      <c r="AO74" s="15"/>
+      <c r="AP74" s="15"/>
+      <c r="AQ74" s="15"/>
+      <c r="AR74" s="15"/>
+      <c r="AS74" s="15"/>
+      <c r="AT74" s="15"/>
+      <c r="AU74" s="15"/>
+      <c r="AV74" s="15"/>
+      <c r="AW74" s="15"/>
+      <c r="AX74" s="15"/>
+      <c r="AY74" s="15"/>
+      <c r="AZ74" s="15"/>
+      <c r="BA74" s="15"/>
+      <c r="BB74" s="15"/>
+      <c r="BC74" s="15"/>
+      <c r="BD74" s="15"/>
+      <c r="BE74" s="15"/>
+      <c r="BF74" s="15"/>
+      <c r="BG74" s="15"/>
+      <c r="BH74" s="15"/>
+      <c r="BI74" s="15"/>
+      <c r="BJ74" s="15"/>
+      <c r="BK74" s="15"/>
+      <c r="BL74" s="15"/>
+      <c r="BM74" s="15"/>
+      <c r="BN74" s="15"/>
+      <c r="BO74" s="15"/>
+      <c r="BP74" s="15"/>
+    </row>
+    <row r="75" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75" s="34"/>
       <c r="C75" s="62"/>
       <c r="D75" s="62"/>
       <c r="E75" s="46"/>
@@ -3383,73 +3425,14 @@
       <c r="G75" s="46"/>
       <c r="H75" s="46"/>
       <c r="I75" s="46"/>
-      <c r="J75" s="15"/>
-      <c r="K75" s="15"/>
-      <c r="L75" s="15"/>
-      <c r="M75" s="15"/>
-      <c r="N75" s="15"/>
-      <c r="O75" s="15"/>
-      <c r="P75" s="15"/>
-      <c r="Q75" s="15"/>
-      <c r="R75" s="15"/>
-      <c r="S75" s="15"/>
-      <c r="T75" s="15"/>
-      <c r="U75" s="15"/>
-      <c r="V75" s="15"/>
-      <c r="W75" s="15"/>
-      <c r="X75" s="15"/>
-      <c r="Y75" s="15"/>
-      <c r="Z75" s="15"/>
-      <c r="AA75" s="15"/>
-      <c r="AB75" s="15"/>
-      <c r="AC75" s="15"/>
-      <c r="AD75" s="15"/>
-      <c r="AE75" s="15"/>
-      <c r="AF75" s="15"/>
-      <c r="AG75" s="15"/>
-      <c r="AH75" s="15"/>
-      <c r="AI75" s="15"/>
-      <c r="AJ75" s="15"/>
-      <c r="AK75" s="15"/>
-      <c r="AL75" s="15"/>
-      <c r="AM75" s="15"/>
-      <c r="AN75" s="15"/>
-      <c r="AO75" s="15"/>
-      <c r="AP75" s="15"/>
-      <c r="AQ75" s="15"/>
-      <c r="AR75" s="15"/>
-      <c r="AS75" s="15"/>
-      <c r="AT75" s="15"/>
-      <c r="AU75" s="15"/>
-      <c r="AV75" s="15"/>
-      <c r="AW75" s="15"/>
-      <c r="AX75" s="15"/>
-      <c r="AY75" s="15"/>
-      <c r="AZ75" s="15"/>
-      <c r="BA75" s="15"/>
-      <c r="BB75" s="15"/>
-      <c r="BC75" s="15"/>
-      <c r="BD75" s="15"/>
-      <c r="BE75" s="15"/>
-      <c r="BF75" s="15"/>
-      <c r="BG75" s="15"/>
-      <c r="BH75" s="15"/>
-      <c r="BI75" s="15"/>
-      <c r="BJ75" s="15"/>
-      <c r="BK75" s="15"/>
-      <c r="BL75" s="15"/>
-      <c r="BM75" s="15"/>
-      <c r="BN75" s="15"/>
-      <c r="BO75" s="15"/>
-      <c r="BP75" s="15"/>
     </row>
     <row r="76" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B76" s="37"/>
-      <c r="C76" s="64"/>
-      <c r="D76" s="64"/>
+        <v>73</v>
+      </c>
+      <c r="B76" s="34"/>
+      <c r="C76" s="62"/>
+      <c r="D76" s="62"/>
       <c r="E76" s="46"/>
       <c r="F76" s="46"/>
       <c r="G76" s="46"/>
@@ -3458,33 +3441,94 @@
     </row>
     <row r="77" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B77" s="37"/>
-      <c r="C77" s="64"/>
-      <c r="D77" s="64"/>
+        <v>71</v>
+      </c>
+      <c r="B77" s="34"/>
+      <c r="C77" s="62"/>
+      <c r="D77" s="62"/>
       <c r="E77" s="46"/>
       <c r="F77" s="46"/>
       <c r="G77" s="46"/>
       <c r="H77" s="46"/>
       <c r="I77" s="46"/>
     </row>
-    <row r="78" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B78" s="37"/>
-      <c r="C78" s="64"/>
-      <c r="D78" s="64"/>
+    <row r="78" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B78" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="C78" s="62"/>
+      <c r="D78" s="62"/>
       <c r="E78" s="46"/>
       <c r="F78" s="46"/>
       <c r="G78" s="46"/>
       <c r="H78" s="46"/>
       <c r="I78" s="46"/>
+      <c r="J78" s="15"/>
+      <c r="K78" s="15"/>
+      <c r="L78" s="15"/>
+      <c r="M78" s="15"/>
+      <c r="N78" s="15"/>
+      <c r="O78" s="15"/>
+      <c r="P78" s="15"/>
+      <c r="Q78" s="15"/>
+      <c r="R78" s="15"/>
+      <c r="S78" s="15"/>
+      <c r="T78" s="15"/>
+      <c r="U78" s="15"/>
+      <c r="V78" s="15"/>
+      <c r="W78" s="15"/>
+      <c r="X78" s="15"/>
+      <c r="Y78" s="15"/>
+      <c r="Z78" s="15"/>
+      <c r="AA78" s="15"/>
+      <c r="AB78" s="15"/>
+      <c r="AC78" s="15"/>
+      <c r="AD78" s="15"/>
+      <c r="AE78" s="15"/>
+      <c r="AF78" s="15"/>
+      <c r="AG78" s="15"/>
+      <c r="AH78" s="15"/>
+      <c r="AI78" s="15"/>
+      <c r="AJ78" s="15"/>
+      <c r="AK78" s="15"/>
+      <c r="AL78" s="15"/>
+      <c r="AM78" s="15"/>
+      <c r="AN78" s="15"/>
+      <c r="AO78" s="15"/>
+      <c r="AP78" s="15"/>
+      <c r="AQ78" s="15"/>
+      <c r="AR78" s="15"/>
+      <c r="AS78" s="15"/>
+      <c r="AT78" s="15"/>
+      <c r="AU78" s="15"/>
+      <c r="AV78" s="15"/>
+      <c r="AW78" s="15"/>
+      <c r="AX78" s="15"/>
+      <c r="AY78" s="15"/>
+      <c r="AZ78" s="15"/>
+      <c r="BA78" s="15"/>
+      <c r="BB78" s="15"/>
+      <c r="BC78" s="15"/>
+      <c r="BD78" s="15"/>
+      <c r="BE78" s="15"/>
+      <c r="BF78" s="15"/>
+      <c r="BG78" s="15"/>
+      <c r="BH78" s="15"/>
+      <c r="BI78" s="15"/>
+      <c r="BJ78" s="15"/>
+      <c r="BK78" s="15"/>
+      <c r="BL78" s="15"/>
+      <c r="BM78" s="15"/>
+      <c r="BN78" s="15"/>
+      <c r="BO78" s="15"/>
+      <c r="BP78" s="15"/>
     </row>
     <row r="79" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B79" s="37"/>
       <c r="C79" s="64"/>
@@ -3496,12 +3540,10 @@
       <c r="I79" s="46"/>
     </row>
     <row r="80" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B80" s="38">
-        <v>0.156</v>
-      </c>
+      <c r="A80" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B80" s="37"/>
       <c r="C80" s="64"/>
       <c r="D80" s="64"/>
       <c r="E80" s="46"/>
@@ -3510,315 +3552,332 @@
       <c r="H80" s="46"/>
       <c r="I80" s="46"/>
     </row>
-    <row r="81" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B81" s="39"/>
-      <c r="C81" s="50"/>
-      <c r="D81" s="50"/>
+        <v>77</v>
+      </c>
+      <c r="B81" s="37"/>
+      <c r="C81" s="64"/>
+      <c r="D81" s="64"/>
       <c r="E81" s="46"/>
       <c r="F81" s="46"/>
       <c r="G81" s="46"/>
       <c r="H81" s="46"/>
       <c r="I81" s="46"/>
-      <c r="J81" s="15"/>
-      <c r="K81" s="15"/>
-      <c r="L81" s="15"/>
-      <c r="M81" s="15"/>
-      <c r="N81" s="15"/>
-      <c r="O81" s="15"/>
-      <c r="P81" s="15"/>
-      <c r="Q81" s="15"/>
-      <c r="R81" s="15"/>
-      <c r="S81" s="15"/>
-      <c r="T81" s="15"/>
-      <c r="U81" s="15"/>
-      <c r="V81" s="15"/>
-      <c r="W81" s="15"/>
-      <c r="X81" s="15"/>
-      <c r="Y81" s="15"/>
-      <c r="Z81" s="15"/>
-      <c r="AA81" s="15"/>
-      <c r="AB81" s="15"/>
-      <c r="AC81" s="15"/>
-      <c r="AD81" s="15"/>
-      <c r="AE81" s="15"/>
-      <c r="AF81" s="15"/>
-      <c r="AG81" s="15"/>
-      <c r="AH81" s="15"/>
-      <c r="AI81" s="15"/>
-      <c r="AJ81" s="15"/>
-      <c r="AK81" s="15"/>
-      <c r="AL81" s="15"/>
-      <c r="AM81" s="15"/>
-      <c r="AN81" s="15"/>
-      <c r="AO81" s="15"/>
-      <c r="AP81" s="15"/>
-      <c r="AQ81" s="15"/>
-      <c r="AR81" s="15"/>
-      <c r="AS81" s="15"/>
-      <c r="AT81" s="15"/>
-      <c r="AU81" s="15"/>
-      <c r="AV81" s="15"/>
-      <c r="AW81" s="15"/>
-      <c r="AX81" s="15"/>
-      <c r="AY81" s="15"/>
-      <c r="AZ81" s="15"/>
-      <c r="BA81" s="15"/>
-      <c r="BB81" s="15"/>
-      <c r="BC81" s="15"/>
-      <c r="BD81" s="15"/>
-      <c r="BE81" s="15"/>
-      <c r="BF81" s="15"/>
-      <c r="BG81" s="15"/>
-      <c r="BH81" s="15"/>
-      <c r="BI81" s="15"/>
-      <c r="BJ81" s="15"/>
-      <c r="BK81" s="15"/>
-      <c r="BL81" s="15"/>
-      <c r="BM81" s="15"/>
-      <c r="BN81" s="15"/>
-      <c r="BO81" s="15"/>
-      <c r="BP81" s="15"/>
-    </row>
-    <row r="82" spans="1:68" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B82" s="39"/>
-      <c r="C82" s="50"/>
-      <c r="D82" s="50"/>
+        <v>78</v>
+      </c>
+      <c r="B82" s="37"/>
+      <c r="C82" s="64"/>
+      <c r="D82" s="64"/>
       <c r="E82" s="46"/>
       <c r="F82" s="46"/>
       <c r="G82" s="46"/>
       <c r="H82" s="46"/>
       <c r="I82" s="46"/>
-      <c r="J82" s="15"/>
-      <c r="K82" s="15"/>
-      <c r="L82" s="15"/>
-      <c r="M82" s="15"/>
-      <c r="N82" s="15"/>
-      <c r="O82" s="15"/>
-      <c r="P82" s="15"/>
-      <c r="Q82" s="15"/>
-      <c r="R82" s="15"/>
-      <c r="S82" s="15"/>
-      <c r="T82" s="15"/>
-      <c r="U82" s="15"/>
-      <c r="V82" s="15"/>
-      <c r="W82" s="15"/>
-      <c r="X82" s="15"/>
-      <c r="Y82" s="15"/>
-      <c r="Z82" s="15"/>
-      <c r="AA82" s="15"/>
-      <c r="AB82" s="15"/>
-      <c r="AC82" s="15"/>
-      <c r="AD82" s="15"/>
-      <c r="AE82" s="15"/>
-      <c r="AF82" s="15"/>
-      <c r="AG82" s="15"/>
-      <c r="AH82" s="15"/>
-      <c r="AI82" s="15"/>
-      <c r="AJ82" s="15"/>
-      <c r="AK82" s="15"/>
-      <c r="AL82" s="15"/>
-      <c r="AM82" s="15"/>
-      <c r="AN82" s="15"/>
-      <c r="AO82" s="15"/>
-      <c r="AP82" s="15"/>
-      <c r="AQ82" s="15"/>
-      <c r="AR82" s="15"/>
-      <c r="AS82" s="15"/>
-      <c r="AT82" s="15"/>
-      <c r="AU82" s="15"/>
-      <c r="AV82" s="15"/>
-      <c r="AW82" s="15"/>
-      <c r="AX82" s="15"/>
-      <c r="AY82" s="15"/>
-      <c r="AZ82" s="15"/>
-      <c r="BA82" s="15"/>
-      <c r="BB82" s="15"/>
-      <c r="BC82" s="15"/>
-      <c r="BD82" s="15"/>
-      <c r="BE82" s="15"/>
-      <c r="BF82" s="15"/>
-      <c r="BG82" s="15"/>
-      <c r="BH82" s="15"/>
-      <c r="BI82" s="15"/>
-      <c r="BJ82" s="15"/>
-      <c r="BK82" s="15"/>
-      <c r="BL82" s="15"/>
-      <c r="BM82" s="15"/>
-      <c r="BN82" s="15"/>
-      <c r="BO82" s="15"/>
-      <c r="BP82" s="15"/>
-    </row>
-    <row r="83" spans="1:68" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B83" s="40"/>
-      <c r="C83" s="50"/>
-      <c r="D83" s="50"/>
+        <v>79</v>
+      </c>
+      <c r="B83" s="38">
+        <v>0.156</v>
+      </c>
+      <c r="C83" s="64"/>
+      <c r="D83" s="64"/>
       <c r="E83" s="46"/>
       <c r="F83" s="46"/>
       <c r="G83" s="46"/>
       <c r="H83" s="46"/>
       <c r="I83" s="46"/>
-      <c r="J83" s="15"/>
-      <c r="K83" s="15"/>
-      <c r="L83" s="15"/>
-      <c r="M83" s="15"/>
-      <c r="N83" s="15"/>
-      <c r="O83" s="15"/>
-      <c r="P83" s="15"/>
-      <c r="Q83" s="15"/>
-      <c r="R83" s="15"/>
-      <c r="S83" s="15"/>
-      <c r="T83" s="15"/>
-      <c r="U83" s="15"/>
-      <c r="V83" s="15"/>
-      <c r="W83" s="15"/>
-      <c r="X83" s="15"/>
-      <c r="Y83" s="15"/>
-      <c r="Z83" s="15"/>
-      <c r="AA83" s="15"/>
-      <c r="AB83" s="15"/>
-      <c r="AC83" s="15"/>
-      <c r="AD83" s="15"/>
-      <c r="AE83" s="15"/>
-      <c r="AF83" s="15"/>
-      <c r="AG83" s="15"/>
-      <c r="AH83" s="15"/>
-      <c r="AI83" s="15"/>
-      <c r="AJ83" s="15"/>
-      <c r="AK83" s="15"/>
-      <c r="AL83" s="15"/>
-      <c r="AM83" s="15"/>
-      <c r="AN83" s="15"/>
-      <c r="AO83" s="15"/>
-      <c r="AP83" s="15"/>
-      <c r="AQ83" s="15"/>
-      <c r="AR83" s="15"/>
-      <c r="AS83" s="15"/>
-      <c r="AT83" s="15"/>
-      <c r="AU83" s="15"/>
-      <c r="AV83" s="15"/>
-      <c r="AW83" s="15"/>
-      <c r="AX83" s="15"/>
-      <c r="AY83" s="15"/>
-      <c r="AZ83" s="15"/>
-      <c r="BA83" s="15"/>
-      <c r="BB83" s="15"/>
-      <c r="BC83" s="15"/>
-      <c r="BD83" s="15"/>
-      <c r="BE83" s="15"/>
-      <c r="BF83" s="15"/>
-      <c r="BG83" s="15"/>
-      <c r="BH83" s="15"/>
-      <c r="BI83" s="15"/>
-      <c r="BJ83" s="15"/>
-      <c r="BK83" s="15"/>
-      <c r="BL83" s="15"/>
-      <c r="BM83" s="15"/>
-      <c r="BN83" s="15"/>
-      <c r="BO83" s="15"/>
-      <c r="BP83" s="15"/>
     </row>
     <row r="84" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A84" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B84" s="41"/>
+      <c r="A84" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84" s="39"/>
       <c r="C84" s="50"/>
       <c r="D84" s="50"/>
+      <c r="E84" s="46"/>
+      <c r="F84" s="46"/>
+      <c r="G84" s="46"/>
+      <c r="H84" s="46"/>
+      <c r="I84" s="46"/>
+      <c r="J84" s="15"/>
+      <c r="K84" s="15"/>
+      <c r="L84" s="15"/>
+      <c r="M84" s="15"/>
+      <c r="N84" s="15"/>
+      <c r="O84" s="15"/>
+      <c r="P84" s="15"/>
+      <c r="Q84" s="15"/>
+      <c r="R84" s="15"/>
+      <c r="S84" s="15"/>
+      <c r="T84" s="15"/>
+      <c r="U84" s="15"/>
+      <c r="V84" s="15"/>
+      <c r="W84" s="15"/>
+      <c r="X84" s="15"/>
+      <c r="Y84" s="15"/>
+      <c r="Z84" s="15"/>
+      <c r="AA84" s="15"/>
+      <c r="AB84" s="15"/>
+      <c r="AC84" s="15"/>
+      <c r="AD84" s="15"/>
+      <c r="AE84" s="15"/>
+      <c r="AF84" s="15"/>
+      <c r="AG84" s="15"/>
+      <c r="AH84" s="15"/>
+      <c r="AI84" s="15"/>
+      <c r="AJ84" s="15"/>
+      <c r="AK84" s="15"/>
+      <c r="AL84" s="15"/>
+      <c r="AM84" s="15"/>
+      <c r="AN84" s="15"/>
+      <c r="AO84" s="15"/>
+      <c r="AP84" s="15"/>
+      <c r="AQ84" s="15"/>
+      <c r="AR84" s="15"/>
+      <c r="AS84" s="15"/>
+      <c r="AT84" s="15"/>
+      <c r="AU84" s="15"/>
+      <c r="AV84" s="15"/>
+      <c r="AW84" s="15"/>
+      <c r="AX84" s="15"/>
+      <c r="AY84" s="15"/>
+      <c r="AZ84" s="15"/>
+      <c r="BA84" s="15"/>
+      <c r="BB84" s="15"/>
+      <c r="BC84" s="15"/>
+      <c r="BD84" s="15"/>
+      <c r="BE84" s="15"/>
+      <c r="BF84" s="15"/>
+      <c r="BG84" s="15"/>
+      <c r="BH84" s="15"/>
+      <c r="BI84" s="15"/>
+      <c r="BJ84" s="15"/>
+      <c r="BK84" s="15"/>
+      <c r="BL84" s="15"/>
+      <c r="BM84" s="15"/>
+      <c r="BN84" s="15"/>
+      <c r="BO84" s="15"/>
+      <c r="BP84" s="15"/>
     </row>
     <row r="85" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A85" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B85" s="42"/>
-      <c r="C85" s="65"/>
-      <c r="D85" s="65"/>
+      <c r="A85" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B85" s="39"/>
+      <c r="C85" s="50"/>
+      <c r="D85" s="50"/>
+      <c r="E85" s="46"/>
+      <c r="F85" s="46"/>
+      <c r="G85" s="46"/>
+      <c r="H85" s="46"/>
+      <c r="I85" s="46"/>
+      <c r="J85" s="15"/>
+      <c r="K85" s="15"/>
+      <c r="L85" s="15"/>
+      <c r="M85" s="15"/>
+      <c r="N85" s="15"/>
+      <c r="O85" s="15"/>
+      <c r="P85" s="15"/>
+      <c r="Q85" s="15"/>
+      <c r="R85" s="15"/>
+      <c r="S85" s="15"/>
+      <c r="T85" s="15"/>
+      <c r="U85" s="15"/>
+      <c r="V85" s="15"/>
+      <c r="W85" s="15"/>
+      <c r="X85" s="15"/>
+      <c r="Y85" s="15"/>
+      <c r="Z85" s="15"/>
+      <c r="AA85" s="15"/>
+      <c r="AB85" s="15"/>
+      <c r="AC85" s="15"/>
+      <c r="AD85" s="15"/>
+      <c r="AE85" s="15"/>
+      <c r="AF85" s="15"/>
+      <c r="AG85" s="15"/>
+      <c r="AH85" s="15"/>
+      <c r="AI85" s="15"/>
+      <c r="AJ85" s="15"/>
+      <c r="AK85" s="15"/>
+      <c r="AL85" s="15"/>
+      <c r="AM85" s="15"/>
+      <c r="AN85" s="15"/>
+      <c r="AO85" s="15"/>
+      <c r="AP85" s="15"/>
+      <c r="AQ85" s="15"/>
+      <c r="AR85" s="15"/>
+      <c r="AS85" s="15"/>
+      <c r="AT85" s="15"/>
+      <c r="AU85" s="15"/>
+      <c r="AV85" s="15"/>
+      <c r="AW85" s="15"/>
+      <c r="AX85" s="15"/>
+      <c r="AY85" s="15"/>
+      <c r="AZ85" s="15"/>
+      <c r="BA85" s="15"/>
+      <c r="BB85" s="15"/>
+      <c r="BC85" s="15"/>
+      <c r="BD85" s="15"/>
+      <c r="BE85" s="15"/>
+      <c r="BF85" s="15"/>
+      <c r="BG85" s="15"/>
+      <c r="BH85" s="15"/>
+      <c r="BI85" s="15"/>
+      <c r="BJ85" s="15"/>
+      <c r="BK85" s="15"/>
+      <c r="BL85" s="15"/>
+      <c r="BM85" s="15"/>
+      <c r="BN85" s="15"/>
+      <c r="BO85" s="15"/>
+      <c r="BP85" s="15"/>
     </row>
     <row r="86" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A86" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B86" s="41"/>
+      <c r="A86" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" s="40"/>
       <c r="C86" s="50"/>
       <c r="D86" s="50"/>
+      <c r="E86" s="46"/>
+      <c r="F86" s="46"/>
+      <c r="G86" s="46"/>
+      <c r="H86" s="46"/>
+      <c r="I86" s="46"/>
+      <c r="J86" s="15"/>
+      <c r="K86" s="15"/>
+      <c r="L86" s="15"/>
+      <c r="M86" s="15"/>
+      <c r="N86" s="15"/>
+      <c r="O86" s="15"/>
+      <c r="P86" s="15"/>
+      <c r="Q86" s="15"/>
+      <c r="R86" s="15"/>
+      <c r="S86" s="15"/>
+      <c r="T86" s="15"/>
+      <c r="U86" s="15"/>
+      <c r="V86" s="15"/>
+      <c r="W86" s="15"/>
+      <c r="X86" s="15"/>
+      <c r="Y86" s="15"/>
+      <c r="Z86" s="15"/>
+      <c r="AA86" s="15"/>
+      <c r="AB86" s="15"/>
+      <c r="AC86" s="15"/>
+      <c r="AD86" s="15"/>
+      <c r="AE86" s="15"/>
+      <c r="AF86" s="15"/>
+      <c r="AG86" s="15"/>
+      <c r="AH86" s="15"/>
+      <c r="AI86" s="15"/>
+      <c r="AJ86" s="15"/>
+      <c r="AK86" s="15"/>
+      <c r="AL86" s="15"/>
+      <c r="AM86" s="15"/>
+      <c r="AN86" s="15"/>
+      <c r="AO86" s="15"/>
+      <c r="AP86" s="15"/>
+      <c r="AQ86" s="15"/>
+      <c r="AR86" s="15"/>
+      <c r="AS86" s="15"/>
+      <c r="AT86" s="15"/>
+      <c r="AU86" s="15"/>
+      <c r="AV86" s="15"/>
+      <c r="AW86" s="15"/>
+      <c r="AX86" s="15"/>
+      <c r="AY86" s="15"/>
+      <c r="AZ86" s="15"/>
+      <c r="BA86" s="15"/>
+      <c r="BB86" s="15"/>
+      <c r="BC86" s="15"/>
+      <c r="BD86" s="15"/>
+      <c r="BE86" s="15"/>
+      <c r="BF86" s="15"/>
+      <c r="BG86" s="15"/>
+      <c r="BH86" s="15"/>
+      <c r="BI86" s="15"/>
+      <c r="BJ86" s="15"/>
+      <c r="BK86" s="15"/>
+      <c r="BL86" s="15"/>
+      <c r="BM86" s="15"/>
+      <c r="BN86" s="15"/>
+      <c r="BO86" s="15"/>
+      <c r="BP86" s="15"/>
     </row>
     <row r="87" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A87" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B87" s="43">
-        <v>1</v>
-      </c>
-      <c r="C87" s="43">
-        <v>2</v>
-      </c>
-      <c r="D87" s="43"/>
-      <c r="E87" s="52"/>
-      <c r="F87" s="52"/>
-      <c r="G87" s="52"/>
-      <c r="H87" s="53"/>
+      <c r="A87" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B87" s="41"/>
+      <c r="C87" s="50"/>
+      <c r="D87" s="50"/>
     </row>
     <row r="88" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A88" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B88" s="44">
-        <v>5</v>
-      </c>
-      <c r="C88" s="44">
-        <v>15</v>
-      </c>
-      <c r="D88" s="44">
-        <v>25</v>
-      </c>
-      <c r="E88" s="44"/>
-      <c r="F88" s="44"/>
-      <c r="G88" s="44"/>
-      <c r="H88" s="54"/>
+      <c r="A88" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B88" s="42"/>
+      <c r="C88" s="65"/>
+      <c r="D88" s="65"/>
     </row>
     <row r="89" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A89" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B89" s="45"/>
+      <c r="A89" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B89" s="41"/>
       <c r="C89" s="50"/>
       <c r="D89" s="50"/>
     </row>
     <row r="90" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A90" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B90" s="41"/>
-      <c r="C90" s="50"/>
-      <c r="D90" s="50"/>
+      <c r="A90" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B90" s="43">
+        <v>1</v>
+      </c>
+      <c r="C90" s="43">
+        <v>2</v>
+      </c>
+      <c r="D90" s="43"/>
+      <c r="E90" s="52"/>
+      <c r="F90" s="52"/>
+      <c r="G90" s="52"/>
+      <c r="H90" s="53"/>
     </row>
     <row r="91" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A91" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B91" s="41"/>
-      <c r="C91" s="50"/>
-      <c r="D91" s="50"/>
+      <c r="A91" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B91" s="44">
+        <v>5</v>
+      </c>
+      <c r="C91" s="44">
+        <v>15</v>
+      </c>
+      <c r="D91" s="44">
+        <v>25</v>
+      </c>
+      <c r="E91" s="44"/>
+      <c r="F91" s="44"/>
+      <c r="G91" s="44"/>
+      <c r="H91" s="54"/>
     </row>
     <row r="92" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A92" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B92" s="41"/>
+      <c r="A92" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B92" s="45"/>
       <c r="C92" s="50"/>
       <c r="D92" s="50"/>
     </row>
     <row r="93" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="B93" s="41"/>
       <c r="C93" s="50"/>
@@ -3826,54 +3885,39 @@
     </row>
     <row r="94" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="B94" s="41"/>
       <c r="C94" s="50"/>
       <c r="D94" s="50"/>
     </row>
-    <row r="95" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="B95" s="41"/>
       <c r="C95" s="50"/>
       <c r="D95" s="50"/>
-      <c r="E95" s="50"/>
-      <c r="F95" s="50"/>
-      <c r="G95" s="46"/>
-      <c r="H95" s="46"/>
-      <c r="I95" s="46"/>
-    </row>
-    <row r="96" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B96" s="41"/>
       <c r="C96" s="50"/>
       <c r="D96" s="50"/>
-      <c r="E96" s="50"/>
-      <c r="F96" s="50"/>
-      <c r="G96" s="46"/>
-      <c r="H96" s="46"/>
-      <c r="I96" s="46"/>
-    </row>
-    <row r="97" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="B97" s="41"/>
       <c r="C97" s="50"/>
       <c r="D97" s="50"/>
-      <c r="E97" s="50"/>
-      <c r="F97" s="50"/>
-      <c r="G97" s="46"/>
-      <c r="H97" s="46"/>
-      <c r="I97" s="46"/>
     </row>
     <row r="98" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B98" s="41"/>
       <c r="C98" s="50"/>
@@ -3884,33 +3928,48 @@
       <c r="H98" s="46"/>
       <c r="I98" s="46"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B99" s="41"/>
       <c r="C99" s="50"/>
       <c r="D99" s="50"/>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E99" s="50"/>
+      <c r="F99" s="50"/>
+      <c r="G99" s="46"/>
+      <c r="H99" s="46"/>
+      <c r="I99" s="46"/>
+    </row>
+    <row r="100" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
-        <v>58</v>
+        <v>121</v>
       </c>
       <c r="B100" s="41"/>
       <c r="C100" s="50"/>
       <c r="D100" s="50"/>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E100" s="50"/>
+      <c r="F100" s="50"/>
+      <c r="G100" s="46"/>
+      <c r="H100" s="46"/>
+      <c r="I100" s="46"/>
+    </row>
+    <row r="101" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B101" s="41"/>
       <c r="C101" s="50"/>
       <c r="D101" s="50"/>
+      <c r="E101" s="50"/>
+      <c r="F101" s="50"/>
+      <c r="G101" s="46"/>
+      <c r="H101" s="46"/>
+      <c r="I101" s="46"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
-        <v>122</v>
+        <v>57</v>
       </c>
       <c r="B102" s="41"/>
       <c r="C102" s="50"/>
@@ -3918,7 +3977,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
-        <v>117</v>
+        <v>58</v>
       </c>
       <c r="B103" s="41"/>
       <c r="C103" s="50"/>
@@ -3926,47 +3985,47 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
-        <v>118</v>
+        <v>59</v>
       </c>
       <c r="B104" s="41"/>
       <c r="C104" s="50"/>
       <c r="D104" s="50"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B105" s="61"/>
+      <c r="A105" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B105" s="41"/>
       <c r="C105" s="50"/>
       <c r="D105" s="50"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="B106" s="59"/>
+      <c r="A106" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="B106" s="41"/>
       <c r="C106" s="50"/>
       <c r="D106" s="50"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="56" t="s">
-        <v>95</v>
-      </c>
-      <c r="B107" s="59"/>
+      <c r="A107" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B107" s="41"/>
       <c r="C107" s="50"/>
       <c r="D107" s="50"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="56" t="s">
-        <v>123</v>
-      </c>
-      <c r="B108" s="59"/>
+      <c r="A108" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="B108" s="61"/>
       <c r="C108" s="50"/>
       <c r="D108" s="50"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="56" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="B109" s="59"/>
       <c r="C109" s="50"/>
@@ -3974,7 +4033,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="56" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B110" s="59"/>
       <c r="C110" s="50"/>
@@ -3982,7 +4041,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="56" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="B111" s="59"/>
       <c r="C111" s="50"/>
@@ -3990,7 +4049,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="56" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="B112" s="59"/>
       <c r="C112" s="50"/>
@@ -3998,23 +4057,23 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="56" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B113" s="59"/>
       <c r="C113" s="50"/>
       <c r="D113" s="50"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="57" t="s">
-        <v>91</v>
+      <c r="A114" s="56" t="s">
+        <v>97</v>
       </c>
       <c r="B114" s="59"/>
       <c r="C114" s="50"/>
       <c r="D114" s="50"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="57" t="s">
-        <v>99</v>
+      <c r="A115" s="56" t="s">
+        <v>124</v>
       </c>
       <c r="B115" s="59"/>
       <c r="C115" s="50"/>
@@ -4022,7 +4081,7 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="56" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="B116" s="59"/>
       <c r="C116" s="50"/>
@@ -4030,7 +4089,7 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="57" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B117" s="59"/>
       <c r="C117" s="50"/>
@@ -4038,23 +4097,23 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="57" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B118" s="59"/>
       <c r="C118" s="50"/>
       <c r="D118" s="50"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="57" t="s">
-        <v>101</v>
+      <c r="A119" s="56" t="s">
+        <v>125</v>
       </c>
       <c r="B119" s="59"/>
       <c r="C119" s="50"/>
       <c r="D119" s="50"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="56" t="s">
-        <v>126</v>
+      <c r="A120" s="57" t="s">
+        <v>100</v>
       </c>
       <c r="B120" s="59"/>
       <c r="C120" s="50"/>
@@ -4062,7 +4121,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="57" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B121" s="59"/>
       <c r="C121" s="50"/>
@@ -4070,99 +4129,123 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="57" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B122" s="59"/>
       <c r="C122" s="50"/>
       <c r="D122" s="50"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="57" t="s">
-        <v>103</v>
+      <c r="A123" s="56" t="s">
+        <v>126</v>
       </c>
       <c r="B123" s="59"/>
       <c r="C123" s="50"/>
       <c r="D123" s="50"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="56" t="s">
-        <v>127</v>
+      <c r="A124" s="57" t="s">
+        <v>102</v>
       </c>
       <c r="B124" s="59"/>
+      <c r="C124" s="50"/>
+      <c r="D124" s="50"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="57" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B125" s="59"/>
+      <c r="C125" s="50"/>
+      <c r="D125" s="50"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="57" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B126" s="59"/>
+      <c r="C126" s="50"/>
+      <c r="D126" s="50"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="57" t="s">
-        <v>105</v>
+      <c r="A127" s="56" t="s">
+        <v>127</v>
       </c>
       <c r="B127" s="59"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="56" t="s">
-        <v>128</v>
+      <c r="A128" s="57" t="s">
+        <v>104</v>
       </c>
       <c r="B128" s="59"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="57" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B129" s="59"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="57" t="s">
+        <v>105</v>
+      </c>
+      <c r="B130" s="59"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="56" t="s">
+        <v>128</v>
+      </c>
+      <c r="B131" s="59"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="B132" s="59"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" s="57" t="s">
         <v>134</v>
       </c>
-      <c r="B130" s="59"/>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="57" t="s">
+      <c r="B133" s="59"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="B131" s="59"/>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="56" t="s">
+      <c r="B134" s="59"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="B132" s="59"/>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="58" t="s">
+      <c r="B135" s="59"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="B133" s="60"/>
+      <c r="B136" s="60"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B84:D84 B69:D70">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87:D87 B72:D73">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B67:D68">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B70:D71">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B85:D85">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B88:D88">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B49:D66">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B49:D69">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87:D87">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B90:D90">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -4170,7 +4253,7 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B76:D80">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79:D83">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -4184,13 +4267,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B89:D104 B71:D75 B81:D83</xm:sqref>
+          <xm:sqref>B92:D107 B74:D78 B84:D86</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B86:D86</xm:sqref>
+          <xm:sqref>B89:D89</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Simplifying code around start-up costs
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="142">
   <si>
     <t>recent_time</t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>cost_curve_step_time</t>
+  </si>
+  <si>
+    <t>reference_time</t>
   </si>
 </sst>
 </file>
@@ -2443,10 +2446,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP136"/>
+  <dimension ref="A1:BP137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2962,7 +2965,7 @@
       <c r="E48" s="46"/>
       <c r="F48" s="46"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>52</v>
       </c>
@@ -2970,7 +2973,7 @@
       <c r="C49" s="62"/>
       <c r="D49" s="62"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>82</v>
       </c>
@@ -2978,7 +2981,7 @@
       <c r="C50" s="62"/>
       <c r="D50" s="62"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>13</v>
       </c>
@@ -2986,7 +2989,7 @@
       <c r="C51" s="62"/>
       <c r="D51" s="62"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>14</v>
       </c>
@@ -2994,7 +2997,7 @@
       <c r="C52" s="62"/>
       <c r="D52" s="62"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>113</v>
       </c>
@@ -3002,7 +3005,7 @@
       <c r="C53" s="63"/>
       <c r="D53" s="63"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>114</v>
       </c>
@@ -3010,7 +3013,7 @@
       <c r="C54" s="63"/>
       <c r="D54" s="63"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>115</v>
       </c>
@@ -3018,7 +3021,7 @@
       <c r="C55" s="63"/>
       <c r="D55" s="63"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>0</v>
       </c>
@@ -3026,7 +3029,7 @@
       <c r="C56" s="62"/>
       <c r="D56" s="62"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>11</v>
       </c>
@@ -3034,28 +3037,25 @@
       <c r="C57" s="62"/>
       <c r="D57" s="62"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="B58" s="29"/>
       <c r="C58" s="62"/>
       <c r="D58" s="62"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B59" s="29"/>
       <c r="C59" s="62"/>
       <c r="D59" s="62"/>
-      <c r="E59" s="69"/>
-      <c r="F59" s="69"/>
-      <c r="G59" s="69"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B60" s="29"/>
       <c r="C60" s="62"/>
@@ -3064,25 +3064,23 @@
       <c r="F60" s="69"/>
       <c r="G60" s="69"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B61" s="29">
-        <v>1865</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B61" s="29"/>
       <c r="C61" s="62"/>
       <c r="D61" s="62"/>
       <c r="E61" s="69"/>
       <c r="F61" s="69"/>
       <c r="G61" s="69"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B62" s="29">
-        <v>2036</v>
+        <v>1865</v>
       </c>
       <c r="C62" s="62"/>
       <c r="D62" s="62"/>
@@ -3090,12 +3088,12 @@
       <c r="F62" s="69"/>
       <c r="G62" s="69"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B63" s="29">
-        <v>1</v>
+        <v>2036</v>
       </c>
       <c r="C63" s="62"/>
       <c r="D63" s="62"/>
@@ -3103,22 +3101,22 @@
       <c r="F63" s="69"/>
       <c r="G63" s="69"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="B64" s="68"/>
-      <c r="C64" s="70"/>
-      <c r="D64" s="70"/>
-      <c r="E64" s="71"/>
-      <c r="F64" s="72"/>
-      <c r="G64" s="72"/>
-      <c r="H64"/>
-      <c r="I64"/>
+        <v>111</v>
+      </c>
+      <c r="B64" s="29">
+        <v>1</v>
+      </c>
+      <c r="C64" s="62"/>
+      <c r="D64" s="62"/>
+      <c r="E64" s="69"/>
+      <c r="F64" s="69"/>
+      <c r="G64" s="69"/>
     </row>
     <row r="65" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B65" s="68"/>
       <c r="C65" s="70"/>
@@ -3131,7 +3129,7 @@
     </row>
     <row r="66" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B66" s="68"/>
       <c r="C66" s="70"/>
@@ -3144,18 +3142,20 @@
     </row>
     <row r="67" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B67" s="29"/>
-      <c r="C67" s="62"/>
-      <c r="D67" s="62"/>
-      <c r="E67" s="69"/>
-      <c r="F67" s="69"/>
-      <c r="G67" s="69"/>
+        <v>140</v>
+      </c>
+      <c r="B67" s="68"/>
+      <c r="C67" s="70"/>
+      <c r="D67" s="70"/>
+      <c r="E67" s="71"/>
+      <c r="F67" s="72"/>
+      <c r="G67" s="72"/>
+      <c r="H67"/>
+      <c r="I67"/>
     </row>
     <row r="68" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B68" s="29"/>
       <c r="C68" s="62"/>
@@ -3166,9 +3166,9 @@
     </row>
     <row r="69" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B69" s="31"/>
+        <v>119</v>
+      </c>
+      <c r="B69" s="29"/>
       <c r="C69" s="62"/>
       <c r="D69" s="62"/>
       <c r="E69" s="69"/>
@@ -3176,10 +3176,10 @@
       <c r="G69" s="69"/>
     </row>
     <row r="70" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B70" s="32"/>
+      <c r="A70" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70" s="31"/>
       <c r="C70" s="62"/>
       <c r="D70" s="62"/>
       <c r="E70" s="69"/>
@@ -3187,10 +3187,10 @@
       <c r="G70" s="69"/>
     </row>
     <row r="71" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A71" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B71" s="33"/>
+      <c r="A71" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B71" s="32"/>
       <c r="C71" s="62"/>
       <c r="D71" s="62"/>
       <c r="E71" s="69"/>
@@ -3198,80 +3198,19 @@
       <c r="G71" s="69"/>
     </row>
     <row r="72" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A72" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B72" s="34"/>
+      <c r="A72" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B72" s="33"/>
       <c r="C72" s="62"/>
       <c r="D72" s="62"/>
-      <c r="E72" s="50"/>
-      <c r="F72" s="50"/>
-      <c r="G72" s="50"/>
-      <c r="H72" s="46"/>
-      <c r="I72" s="46"/>
-      <c r="J72" s="15"/>
-      <c r="K72" s="15"/>
-      <c r="L72" s="15"/>
-      <c r="M72" s="15"/>
-      <c r="N72" s="15"/>
-      <c r="O72" s="15"/>
-      <c r="P72" s="15"/>
-      <c r="Q72" s="15"/>
-      <c r="R72" s="15"/>
-      <c r="S72" s="15"/>
-      <c r="T72" s="15"/>
-      <c r="U72" s="15"/>
-      <c r="V72" s="15"/>
-      <c r="W72" s="15"/>
-      <c r="X72" s="15"/>
-      <c r="Y72" s="15"/>
-      <c r="Z72" s="15"/>
-      <c r="AA72" s="15"/>
-      <c r="AB72" s="15"/>
-      <c r="AC72" s="15"/>
-      <c r="AD72" s="15"/>
-      <c r="AE72" s="15"/>
-      <c r="AF72" s="15"/>
-      <c r="AG72" s="15"/>
-      <c r="AH72" s="15"/>
-      <c r="AI72" s="15"/>
-      <c r="AJ72" s="15"/>
-      <c r="AK72" s="15"/>
-      <c r="AL72" s="15"/>
-      <c r="AM72" s="15"/>
-      <c r="AN72" s="15"/>
-      <c r="AO72" s="15"/>
-      <c r="AP72" s="15"/>
-      <c r="AQ72" s="15"/>
-      <c r="AR72" s="15"/>
-      <c r="AS72" s="15"/>
-      <c r="AT72" s="15"/>
-      <c r="AU72" s="15"/>
-      <c r="AV72" s="15"/>
-      <c r="AW72" s="15"/>
-      <c r="AX72" s="15"/>
-      <c r="AY72" s="15"/>
-      <c r="AZ72" s="15"/>
-      <c r="BA72" s="15"/>
-      <c r="BB72" s="15"/>
-      <c r="BC72" s="15"/>
-      <c r="BD72" s="15"/>
-      <c r="BE72" s="15"/>
-      <c r="BF72" s="15"/>
-      <c r="BG72" s="15"/>
-      <c r="BH72" s="15"/>
-      <c r="BI72" s="15"/>
-      <c r="BJ72" s="15"/>
-      <c r="BK72" s="15"/>
-      <c r="BL72" s="15"/>
-      <c r="BM72" s="15"/>
-      <c r="BN72" s="15"/>
-      <c r="BO72" s="15"/>
-      <c r="BP72" s="15"/>
+      <c r="E72" s="69"/>
+      <c r="F72" s="69"/>
+      <c r="G72" s="69"/>
     </row>
     <row r="73" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B73" s="34"/>
       <c r="C73" s="62"/>
@@ -3341,11 +3280,11 @@
       <c r="BO73" s="15"/>
       <c r="BP73" s="15"/>
     </row>
-    <row r="74" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B74" s="35"/>
+    <row r="74" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A74" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B74" s="34"/>
       <c r="C74" s="62"/>
       <c r="D74" s="62"/>
       <c r="E74" s="50"/>
@@ -3413,22 +3352,81 @@
       <c r="BO74" s="15"/>
       <c r="BP74" s="15"/>
     </row>
-    <row r="75" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B75" s="34"/>
+    <row r="75" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B75" s="35"/>
       <c r="C75" s="62"/>
       <c r="D75" s="62"/>
-      <c r="E75" s="46"/>
-      <c r="F75" s="46"/>
-      <c r="G75" s="46"/>
+      <c r="E75" s="50"/>
+      <c r="F75" s="50"/>
+      <c r="G75" s="50"/>
       <c r="H75" s="46"/>
       <c r="I75" s="46"/>
+      <c r="J75" s="15"/>
+      <c r="K75" s="15"/>
+      <c r="L75" s="15"/>
+      <c r="M75" s="15"/>
+      <c r="N75" s="15"/>
+      <c r="O75" s="15"/>
+      <c r="P75" s="15"/>
+      <c r="Q75" s="15"/>
+      <c r="R75" s="15"/>
+      <c r="S75" s="15"/>
+      <c r="T75" s="15"/>
+      <c r="U75" s="15"/>
+      <c r="V75" s="15"/>
+      <c r="W75" s="15"/>
+      <c r="X75" s="15"/>
+      <c r="Y75" s="15"/>
+      <c r="Z75" s="15"/>
+      <c r="AA75" s="15"/>
+      <c r="AB75" s="15"/>
+      <c r="AC75" s="15"/>
+      <c r="AD75" s="15"/>
+      <c r="AE75" s="15"/>
+      <c r="AF75" s="15"/>
+      <c r="AG75" s="15"/>
+      <c r="AH75" s="15"/>
+      <c r="AI75" s="15"/>
+      <c r="AJ75" s="15"/>
+      <c r="AK75" s="15"/>
+      <c r="AL75" s="15"/>
+      <c r="AM75" s="15"/>
+      <c r="AN75" s="15"/>
+      <c r="AO75" s="15"/>
+      <c r="AP75" s="15"/>
+      <c r="AQ75" s="15"/>
+      <c r="AR75" s="15"/>
+      <c r="AS75" s="15"/>
+      <c r="AT75" s="15"/>
+      <c r="AU75" s="15"/>
+      <c r="AV75" s="15"/>
+      <c r="AW75" s="15"/>
+      <c r="AX75" s="15"/>
+      <c r="AY75" s="15"/>
+      <c r="AZ75" s="15"/>
+      <c r="BA75" s="15"/>
+      <c r="BB75" s="15"/>
+      <c r="BC75" s="15"/>
+      <c r="BD75" s="15"/>
+      <c r="BE75" s="15"/>
+      <c r="BF75" s="15"/>
+      <c r="BG75" s="15"/>
+      <c r="BH75" s="15"/>
+      <c r="BI75" s="15"/>
+      <c r="BJ75" s="15"/>
+      <c r="BK75" s="15"/>
+      <c r="BL75" s="15"/>
+      <c r="BM75" s="15"/>
+      <c r="BN75" s="15"/>
+      <c r="BO75" s="15"/>
+      <c r="BP75" s="15"/>
     </row>
     <row r="76" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B76" s="34"/>
       <c r="C76" s="62"/>
@@ -3441,7 +3439,7 @@
     </row>
     <row r="77" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B77" s="34"/>
       <c r="C77" s="62"/>
@@ -3452,13 +3450,11 @@
       <c r="H77" s="46"/>
       <c r="I77" s="46"/>
     </row>
-    <row r="78" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B78" s="36" t="b">
-        <v>1</v>
-      </c>
+    <row r="78" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B78" s="34"/>
       <c r="C78" s="62"/>
       <c r="D78" s="62"/>
       <c r="E78" s="46"/>
@@ -3466,82 +3462,84 @@
       <c r="G78" s="46"/>
       <c r="H78" s="46"/>
       <c r="I78" s="46"/>
-      <c r="J78" s="15"/>
-      <c r="K78" s="15"/>
-      <c r="L78" s="15"/>
-      <c r="M78" s="15"/>
-      <c r="N78" s="15"/>
-      <c r="O78" s="15"/>
-      <c r="P78" s="15"/>
-      <c r="Q78" s="15"/>
-      <c r="R78" s="15"/>
-      <c r="S78" s="15"/>
-      <c r="T78" s="15"/>
-      <c r="U78" s="15"/>
-      <c r="V78" s="15"/>
-      <c r="W78" s="15"/>
-      <c r="X78" s="15"/>
-      <c r="Y78" s="15"/>
-      <c r="Z78" s="15"/>
-      <c r="AA78" s="15"/>
-      <c r="AB78" s="15"/>
-      <c r="AC78" s="15"/>
-      <c r="AD78" s="15"/>
-      <c r="AE78" s="15"/>
-      <c r="AF78" s="15"/>
-      <c r="AG78" s="15"/>
-      <c r="AH78" s="15"/>
-      <c r="AI78" s="15"/>
-      <c r="AJ78" s="15"/>
-      <c r="AK78" s="15"/>
-      <c r="AL78" s="15"/>
-      <c r="AM78" s="15"/>
-      <c r="AN78" s="15"/>
-      <c r="AO78" s="15"/>
-      <c r="AP78" s="15"/>
-      <c r="AQ78" s="15"/>
-      <c r="AR78" s="15"/>
-      <c r="AS78" s="15"/>
-      <c r="AT78" s="15"/>
-      <c r="AU78" s="15"/>
-      <c r="AV78" s="15"/>
-      <c r="AW78" s="15"/>
-      <c r="AX78" s="15"/>
-      <c r="AY78" s="15"/>
-      <c r="AZ78" s="15"/>
-      <c r="BA78" s="15"/>
-      <c r="BB78" s="15"/>
-      <c r="BC78" s="15"/>
-      <c r="BD78" s="15"/>
-      <c r="BE78" s="15"/>
-      <c r="BF78" s="15"/>
-      <c r="BG78" s="15"/>
-      <c r="BH78" s="15"/>
-      <c r="BI78" s="15"/>
-      <c r="BJ78" s="15"/>
-      <c r="BK78" s="15"/>
-      <c r="BL78" s="15"/>
-      <c r="BM78" s="15"/>
-      <c r="BN78" s="15"/>
-      <c r="BO78" s="15"/>
-      <c r="BP78" s="15"/>
-    </row>
-    <row r="79" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B79" s="37"/>
-      <c r="C79" s="64"/>
-      <c r="D79" s="64"/>
+    </row>
+    <row r="79" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B79" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="C79" s="62"/>
+      <c r="D79" s="62"/>
       <c r="E79" s="46"/>
       <c r="F79" s="46"/>
       <c r="G79" s="46"/>
       <c r="H79" s="46"/>
       <c r="I79" s="46"/>
+      <c r="J79" s="15"/>
+      <c r="K79" s="15"/>
+      <c r="L79" s="15"/>
+      <c r="M79" s="15"/>
+      <c r="N79" s="15"/>
+      <c r="O79" s="15"/>
+      <c r="P79" s="15"/>
+      <c r="Q79" s="15"/>
+      <c r="R79" s="15"/>
+      <c r="S79" s="15"/>
+      <c r="T79" s="15"/>
+      <c r="U79" s="15"/>
+      <c r="V79" s="15"/>
+      <c r="W79" s="15"/>
+      <c r="X79" s="15"/>
+      <c r="Y79" s="15"/>
+      <c r="Z79" s="15"/>
+      <c r="AA79" s="15"/>
+      <c r="AB79" s="15"/>
+      <c r="AC79" s="15"/>
+      <c r="AD79" s="15"/>
+      <c r="AE79" s="15"/>
+      <c r="AF79" s="15"/>
+      <c r="AG79" s="15"/>
+      <c r="AH79" s="15"/>
+      <c r="AI79" s="15"/>
+      <c r="AJ79" s="15"/>
+      <c r="AK79" s="15"/>
+      <c r="AL79" s="15"/>
+      <c r="AM79" s="15"/>
+      <c r="AN79" s="15"/>
+      <c r="AO79" s="15"/>
+      <c r="AP79" s="15"/>
+      <c r="AQ79" s="15"/>
+      <c r="AR79" s="15"/>
+      <c r="AS79" s="15"/>
+      <c r="AT79" s="15"/>
+      <c r="AU79" s="15"/>
+      <c r="AV79" s="15"/>
+      <c r="AW79" s="15"/>
+      <c r="AX79" s="15"/>
+      <c r="AY79" s="15"/>
+      <c r="AZ79" s="15"/>
+      <c r="BA79" s="15"/>
+      <c r="BB79" s="15"/>
+      <c r="BC79" s="15"/>
+      <c r="BD79" s="15"/>
+      <c r="BE79" s="15"/>
+      <c r="BF79" s="15"/>
+      <c r="BG79" s="15"/>
+      <c r="BH79" s="15"/>
+      <c r="BI79" s="15"/>
+      <c r="BJ79" s="15"/>
+      <c r="BK79" s="15"/>
+      <c r="BL79" s="15"/>
+      <c r="BM79" s="15"/>
+      <c r="BN79" s="15"/>
+      <c r="BO79" s="15"/>
+      <c r="BP79" s="15"/>
     </row>
     <row r="80" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B80" s="37"/>
       <c r="C80" s="64"/>
@@ -3554,7 +3552,7 @@
     </row>
     <row r="81" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B81" s="37"/>
       <c r="C81" s="64"/>
@@ -3567,7 +3565,7 @@
     </row>
     <row r="82" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B82" s="37"/>
       <c r="C82" s="64"/>
@@ -3579,12 +3577,10 @@
       <c r="I82" s="46"/>
     </row>
     <row r="83" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B83" s="38">
-        <v>0.156</v>
-      </c>
+      <c r="A83" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B83" s="37"/>
       <c r="C83" s="64"/>
       <c r="D83" s="64"/>
       <c r="E83" s="46"/>
@@ -3593,81 +3589,24 @@
       <c r="H83" s="46"/>
       <c r="I83" s="46"/>
     </row>
-    <row r="84" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B84" s="39"/>
-      <c r="C84" s="50"/>
-      <c r="D84" s="50"/>
+    <row r="84" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B84" s="38">
+        <v>0.156</v>
+      </c>
+      <c r="C84" s="64"/>
+      <c r="D84" s="64"/>
       <c r="E84" s="46"/>
       <c r="F84" s="46"/>
       <c r="G84" s="46"/>
       <c r="H84" s="46"/>
       <c r="I84" s="46"/>
-      <c r="J84" s="15"/>
-      <c r="K84" s="15"/>
-      <c r="L84" s="15"/>
-      <c r="M84" s="15"/>
-      <c r="N84" s="15"/>
-      <c r="O84" s="15"/>
-      <c r="P84" s="15"/>
-      <c r="Q84" s="15"/>
-      <c r="R84" s="15"/>
-      <c r="S84" s="15"/>
-      <c r="T84" s="15"/>
-      <c r="U84" s="15"/>
-      <c r="V84" s="15"/>
-      <c r="W84" s="15"/>
-      <c r="X84" s="15"/>
-      <c r="Y84" s="15"/>
-      <c r="Z84" s="15"/>
-      <c r="AA84" s="15"/>
-      <c r="AB84" s="15"/>
-      <c r="AC84" s="15"/>
-      <c r="AD84" s="15"/>
-      <c r="AE84" s="15"/>
-      <c r="AF84" s="15"/>
-      <c r="AG84" s="15"/>
-      <c r="AH84" s="15"/>
-      <c r="AI84" s="15"/>
-      <c r="AJ84" s="15"/>
-      <c r="AK84" s="15"/>
-      <c r="AL84" s="15"/>
-      <c r="AM84" s="15"/>
-      <c r="AN84" s="15"/>
-      <c r="AO84" s="15"/>
-      <c r="AP84" s="15"/>
-      <c r="AQ84" s="15"/>
-      <c r="AR84" s="15"/>
-      <c r="AS84" s="15"/>
-      <c r="AT84" s="15"/>
-      <c r="AU84" s="15"/>
-      <c r="AV84" s="15"/>
-      <c r="AW84" s="15"/>
-      <c r="AX84" s="15"/>
-      <c r="AY84" s="15"/>
-      <c r="AZ84" s="15"/>
-      <c r="BA84" s="15"/>
-      <c r="BB84" s="15"/>
-      <c r="BC84" s="15"/>
-      <c r="BD84" s="15"/>
-      <c r="BE84" s="15"/>
-      <c r="BF84" s="15"/>
-      <c r="BG84" s="15"/>
-      <c r="BH84" s="15"/>
-      <c r="BI84" s="15"/>
-      <c r="BJ84" s="15"/>
-      <c r="BK84" s="15"/>
-      <c r="BL84" s="15"/>
-      <c r="BM84" s="15"/>
-      <c r="BN84" s="15"/>
-      <c r="BO84" s="15"/>
-      <c r="BP84" s="15"/>
     </row>
     <row r="85" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B85" s="39"/>
       <c r="C85" s="50"/>
@@ -3738,10 +3677,10 @@
       <c r="BP85" s="15"/>
     </row>
     <row r="86" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A86" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B86" s="40"/>
+      <c r="A86" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B86" s="39"/>
       <c r="C86" s="50"/>
       <c r="D86" s="50"/>
       <c r="E86" s="46"/>
@@ -3810,82 +3749,142 @@
       <c r="BP86" s="15"/>
     </row>
     <row r="87" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A87" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B87" s="41"/>
+      <c r="A87" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" s="40"/>
       <c r="C87" s="50"/>
       <c r="D87" s="50"/>
+      <c r="E87" s="46"/>
+      <c r="F87" s="46"/>
+      <c r="G87" s="46"/>
+      <c r="H87" s="46"/>
+      <c r="I87" s="46"/>
+      <c r="J87" s="15"/>
+      <c r="K87" s="15"/>
+      <c r="L87" s="15"/>
+      <c r="M87" s="15"/>
+      <c r="N87" s="15"/>
+      <c r="O87" s="15"/>
+      <c r="P87" s="15"/>
+      <c r="Q87" s="15"/>
+      <c r="R87" s="15"/>
+      <c r="S87" s="15"/>
+      <c r="T87" s="15"/>
+      <c r="U87" s="15"/>
+      <c r="V87" s="15"/>
+      <c r="W87" s="15"/>
+      <c r="X87" s="15"/>
+      <c r="Y87" s="15"/>
+      <c r="Z87" s="15"/>
+      <c r="AA87" s="15"/>
+      <c r="AB87" s="15"/>
+      <c r="AC87" s="15"/>
+      <c r="AD87" s="15"/>
+      <c r="AE87" s="15"/>
+      <c r="AF87" s="15"/>
+      <c r="AG87" s="15"/>
+      <c r="AH87" s="15"/>
+      <c r="AI87" s="15"/>
+      <c r="AJ87" s="15"/>
+      <c r="AK87" s="15"/>
+      <c r="AL87" s="15"/>
+      <c r="AM87" s="15"/>
+      <c r="AN87" s="15"/>
+      <c r="AO87" s="15"/>
+      <c r="AP87" s="15"/>
+      <c r="AQ87" s="15"/>
+      <c r="AR87" s="15"/>
+      <c r="AS87" s="15"/>
+      <c r="AT87" s="15"/>
+      <c r="AU87" s="15"/>
+      <c r="AV87" s="15"/>
+      <c r="AW87" s="15"/>
+      <c r="AX87" s="15"/>
+      <c r="AY87" s="15"/>
+      <c r="AZ87" s="15"/>
+      <c r="BA87" s="15"/>
+      <c r="BB87" s="15"/>
+      <c r="BC87" s="15"/>
+      <c r="BD87" s="15"/>
+      <c r="BE87" s="15"/>
+      <c r="BF87" s="15"/>
+      <c r="BG87" s="15"/>
+      <c r="BH87" s="15"/>
+      <c r="BI87" s="15"/>
+      <c r="BJ87" s="15"/>
+      <c r="BK87" s="15"/>
+      <c r="BL87" s="15"/>
+      <c r="BM87" s="15"/>
+      <c r="BN87" s="15"/>
+      <c r="BO87" s="15"/>
+      <c r="BP87" s="15"/>
     </row>
     <row r="88" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A88" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B88" s="42"/>
-      <c r="C88" s="65"/>
-      <c r="D88" s="65"/>
+        <v>9</v>
+      </c>
+      <c r="B88" s="41"/>
+      <c r="C88" s="50"/>
+      <c r="D88" s="50"/>
     </row>
     <row r="89" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B89" s="42"/>
+      <c r="C89" s="65"/>
+      <c r="D89" s="65"/>
+    </row>
+    <row r="90" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A90" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B89" s="41"/>
-      <c r="C89" s="50"/>
-      <c r="D89" s="50"/>
-    </row>
-    <row r="90" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A90" s="17" t="s">
+      <c r="B90" s="41"/>
+      <c r="C90" s="50"/>
+      <c r="D90" s="50"/>
+    </row>
+    <row r="91" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A91" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B90" s="43">
-        <v>1</v>
-      </c>
-      <c r="C90" s="43">
-        <v>2</v>
-      </c>
-      <c r="D90" s="43"/>
-      <c r="E90" s="52"/>
-      <c r="F90" s="52"/>
-      <c r="G90" s="52"/>
-      <c r="H90" s="53"/>
-    </row>
-    <row r="91" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A91" s="16" t="s">
+      <c r="B91" s="43"/>
+      <c r="C91" s="43"/>
+      <c r="D91" s="43"/>
+      <c r="E91" s="52"/>
+      <c r="F91" s="52"/>
+      <c r="G91" s="52"/>
+      <c r="H91" s="53"/>
+    </row>
+    <row r="92" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A92" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B91" s="44">
+      <c r="B92" s="44">
         <v>5</v>
       </c>
-      <c r="C91" s="44">
+      <c r="C92" s="44">
         <v>15</v>
       </c>
-      <c r="D91" s="44">
+      <c r="D92" s="44">
         <v>25</v>
       </c>
-      <c r="E91" s="44"/>
-      <c r="F91" s="44"/>
-      <c r="G91" s="44"/>
-      <c r="H91" s="54"/>
-    </row>
-    <row r="92" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A92" s="18" t="s">
+      <c r="E92" s="44"/>
+      <c r="F92" s="44"/>
+      <c r="G92" s="44"/>
+      <c r="H92" s="54"/>
+    </row>
+    <row r="93" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A93" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B92" s="45"/>
-      <c r="C92" s="50"/>
-      <c r="D92" s="50"/>
-    </row>
-    <row r="93" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A93" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B93" s="41"/>
+      <c r="B93" s="45"/>
       <c r="C93" s="50"/>
       <c r="D93" s="50"/>
     </row>
     <row r="94" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B94" s="41"/>
       <c r="C94" s="50"/>
@@ -3893,7 +3892,7 @@
     </row>
     <row r="95" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B95" s="41"/>
       <c r="C95" s="50"/>
@@ -3901,7 +3900,7 @@
     </row>
     <row r="96" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="B96" s="41"/>
       <c r="C96" s="50"/>
@@ -3909,28 +3908,23 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="B97" s="41"/>
       <c r="C97" s="50"/>
       <c r="D97" s="50"/>
     </row>
-    <row r="98" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
       <c r="B98" s="41"/>
       <c r="C98" s="50"/>
       <c r="D98" s="50"/>
-      <c r="E98" s="50"/>
-      <c r="F98" s="50"/>
-      <c r="G98" s="46"/>
-      <c r="H98" s="46"/>
-      <c r="I98" s="46"/>
     </row>
     <row r="99" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B99" s="41"/>
       <c r="C99" s="50"/>
@@ -3943,7 +3937,7 @@
     </row>
     <row r="100" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
-        <v>121</v>
+        <v>69</v>
       </c>
       <c r="B100" s="41"/>
       <c r="C100" s="50"/>
@@ -3956,7 +3950,7 @@
     </row>
     <row r="101" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="B101" s="41"/>
       <c r="C101" s="50"/>
@@ -3967,17 +3961,22 @@
       <c r="H101" s="46"/>
       <c r="I101" s="46"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="B102" s="41"/>
       <c r="C102" s="50"/>
       <c r="D102" s="50"/>
+      <c r="E102" s="50"/>
+      <c r="F102" s="50"/>
+      <c r="G102" s="46"/>
+      <c r="H102" s="46"/>
+      <c r="I102" s="46"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B103" s="41"/>
       <c r="C103" s="50"/>
@@ -3985,7 +3984,7 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B104" s="41"/>
       <c r="C104" s="50"/>
@@ -3993,7 +3992,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="B105" s="41"/>
       <c r="C105" s="50"/>
@@ -4001,39 +4000,41 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B106" s="41"/>
+        <v>122</v>
+      </c>
+      <c r="B106" s="41" t="b">
+        <v>1</v>
+      </c>
       <c r="C106" s="50"/>
       <c r="D106" s="50"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B107" s="41"/>
       <c r="C107" s="50"/>
       <c r="D107" s="50"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B108" s="61"/>
+      <c r="A108" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B108" s="41"/>
       <c r="C108" s="50"/>
       <c r="D108" s="50"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="B109" s="59"/>
+      <c r="A109" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="B109" s="61"/>
       <c r="C109" s="50"/>
       <c r="D109" s="50"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="56" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B110" s="59"/>
       <c r="C110" s="50"/>
@@ -4041,7 +4042,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="56" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="B111" s="59"/>
       <c r="C111" s="50"/>
@@ -4049,7 +4050,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="56" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="B112" s="59"/>
       <c r="C112" s="50"/>
@@ -4057,7 +4058,7 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="56" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B113" s="59"/>
       <c r="C113" s="50"/>
@@ -4065,7 +4066,7 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="56" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B114" s="59"/>
       <c r="C114" s="50"/>
@@ -4073,7 +4074,7 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="56" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="B115" s="59"/>
       <c r="C115" s="50"/>
@@ -4081,15 +4082,15 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="56" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="B116" s="59"/>
       <c r="C116" s="50"/>
       <c r="D116" s="50"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="57" t="s">
-        <v>91</v>
+      <c r="A117" s="56" t="s">
+        <v>98</v>
       </c>
       <c r="B117" s="59"/>
       <c r="C117" s="50"/>
@@ -4097,23 +4098,23 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="57" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B118" s="59"/>
       <c r="C118" s="50"/>
       <c r="D118" s="50"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="56" t="s">
-        <v>125</v>
+      <c r="A119" s="57" t="s">
+        <v>99</v>
       </c>
       <c r="B119" s="59"/>
       <c r="C119" s="50"/>
       <c r="D119" s="50"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="57" t="s">
-        <v>100</v>
+      <c r="A120" s="56" t="s">
+        <v>125</v>
       </c>
       <c r="B120" s="59"/>
       <c r="C120" s="50"/>
@@ -4121,7 +4122,7 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="57" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B121" s="59"/>
       <c r="C121" s="50"/>
@@ -4129,23 +4130,23 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="57" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B122" s="59"/>
       <c r="C122" s="50"/>
       <c r="D122" s="50"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="56" t="s">
-        <v>126</v>
+      <c r="A123" s="57" t="s">
+        <v>101</v>
       </c>
       <c r="B123" s="59"/>
       <c r="C123" s="50"/>
       <c r="D123" s="50"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="57" t="s">
-        <v>102</v>
+      <c r="A124" s="56" t="s">
+        <v>126</v>
       </c>
       <c r="B124" s="59"/>
       <c r="C124" s="50"/>
@@ -4153,7 +4154,7 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="57" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B125" s="59"/>
       <c r="C125" s="50"/>
@@ -4161,91 +4162,99 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="57" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B126" s="59"/>
       <c r="C126" s="50"/>
       <c r="D126" s="50"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="56" t="s">
+      <c r="A127" s="57" t="s">
+        <v>103</v>
+      </c>
+      <c r="B127" s="59"/>
+      <c r="C127" s="50"/>
+      <c r="D127" s="50"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="56" t="s">
         <v>127</v>
-      </c>
-      <c r="B127" s="59"/>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="57" t="s">
-        <v>104</v>
       </c>
       <c r="B128" s="59"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="57" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="B129" s="59"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B130" s="59"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="B130" s="59"/>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="56" t="s">
+      <c r="B131" s="59"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" s="56" t="s">
         <v>128</v>
-      </c>
-      <c r="B131" s="59"/>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="57" t="s">
-        <v>106</v>
       </c>
       <c r="B132" s="59"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="57" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="B133" s="59"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="B134" s="59"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="B134" s="59"/>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="56" t="s">
+      <c r="B135" s="59"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="B135" s="59"/>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="58" t="s">
+      <c r="B136" s="59"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="B136" s="60"/>
+      <c r="B137" s="60"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87:D87 B72:D73">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B88:D88 B73:D74">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B70:D71">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B71:D72">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B88:D88">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89:D89">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B49:D69">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B49:D70">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B90:D90">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B91:D91">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -4253,7 +4262,7 @@
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79:D83">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B80:D84">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -4267,13 +4276,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B92:D107 B74:D78 B84:D86</xm:sqref>
+          <xm:sqref>B93:D108 B75:D79 B85:D87</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B89:D89</xm:sqref>
+          <xm:sqref>B90:D90</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Separate inflection cost from start-up cost
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="149">
   <si>
     <t>recent_time</t>
   </si>
@@ -441,6 +441,27 @@
   </si>
   <si>
     <t>reference_time</t>
+  </si>
+  <si>
+    <t>econ_startupcost_vaccination</t>
+  </si>
+  <si>
+    <t>econ_startupcost_ipt</t>
+  </si>
+  <si>
+    <t>econ_startupcost_xpert</t>
+  </si>
+  <si>
+    <t>econ_startupcost_treatment_support</t>
+  </si>
+  <si>
+    <t>econ_startupcost_smearacf</t>
+  </si>
+  <si>
+    <t>econ_startupcost_xpertacf</t>
+  </si>
+  <si>
+    <t>econ_startupcost_decentralisation</t>
   </si>
 </sst>
 </file>
@@ -1392,7 +1413,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1460,9 +1481,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -1476,6 +1494,16 @@
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2446,10 +2474,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP137"/>
+  <dimension ref="A1:BP146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2873,10 +2901,10 @@
       <c r="A41" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B41" s="66"/>
-      <c r="C41" s="66"/>
-      <c r="D41" s="66"/>
-      <c r="E41" s="67"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="63"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="64"/>
       <c r="F41"/>
       <c r="G41"/>
       <c r="H41"/>
@@ -2886,10 +2914,10 @@
       <c r="A42" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="B42" s="66"/>
-      <c r="C42" s="66"/>
-      <c r="D42" s="66"/>
-      <c r="E42" s="67"/>
+      <c r="B42" s="63"/>
+      <c r="C42" s="63"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="64"/>
       <c r="F42"/>
       <c r="G42"/>
       <c r="H42"/>
@@ -2899,10 +2927,10 @@
       <c r="A43" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B43" s="66"/>
-      <c r="C43" s="66"/>
-      <c r="D43" s="66"/>
-      <c r="E43" s="67"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="63"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="64"/>
       <c r="F43"/>
       <c r="G43"/>
       <c r="H43"/>
@@ -2912,10 +2940,10 @@
       <c r="A44" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="B44" s="66"/>
-      <c r="C44" s="66"/>
-      <c r="D44" s="66"/>
-      <c r="E44" s="67"/>
+      <c r="B44" s="63"/>
+      <c r="C44" s="63"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="64"/>
       <c r="F44"/>
       <c r="G44"/>
       <c r="H44"/>
@@ -2970,110 +2998,110 @@
         <v>52</v>
       </c>
       <c r="B49" s="29"/>
-      <c r="C49" s="62"/>
-      <c r="D49" s="62"/>
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B50" s="29"/>
-      <c r="C50" s="62"/>
-      <c r="D50" s="62"/>
+      <c r="C50" s="59"/>
+      <c r="D50" s="59"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B51" s="29"/>
-      <c r="C51" s="62"/>
-      <c r="D51" s="62"/>
+      <c r="C51" s="59"/>
+      <c r="D51" s="59"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B52" s="29"/>
-      <c r="C52" s="62"/>
-      <c r="D52" s="62"/>
+      <c r="C52" s="59"/>
+      <c r="D52" s="59"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>113</v>
       </c>
       <c r="B53" s="30"/>
-      <c r="C53" s="63"/>
-      <c r="D53" s="63"/>
+      <c r="C53" s="60"/>
+      <c r="D53" s="60"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>114</v>
       </c>
       <c r="B54" s="30"/>
-      <c r="C54" s="63"/>
-      <c r="D54" s="63"/>
+      <c r="C54" s="60"/>
+      <c r="D54" s="60"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>115</v>
       </c>
       <c r="B55" s="30"/>
-      <c r="C55" s="63"/>
-      <c r="D55" s="63"/>
+      <c r="C55" s="60"/>
+      <c r="D55" s="60"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B56" s="29"/>
-      <c r="C56" s="62"/>
-      <c r="D56" s="62"/>
+      <c r="C56" s="59"/>
+      <c r="D56" s="59"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B57" s="29"/>
-      <c r="C57" s="62"/>
-      <c r="D57" s="62"/>
+      <c r="C57" s="59"/>
+      <c r="D57" s="59"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>141</v>
       </c>
       <c r="B58" s="29"/>
-      <c r="C58" s="62"/>
-      <c r="D58" s="62"/>
+      <c r="C58" s="59"/>
+      <c r="D58" s="59"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B59" s="29"/>
-      <c r="C59" s="62"/>
-      <c r="D59" s="62"/>
+      <c r="C59" s="59"/>
+      <c r="D59" s="59"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B60" s="29"/>
-      <c r="C60" s="62"/>
-      <c r="D60" s="62"/>
-      <c r="E60" s="69"/>
-      <c r="F60" s="69"/>
-      <c r="G60" s="69"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="66"/>
+      <c r="F60" s="66"/>
+      <c r="G60" s="66"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>10</v>
       </c>
       <c r="B61" s="29"/>
-      <c r="C61" s="62"/>
-      <c r="D61" s="62"/>
-      <c r="E61" s="69"/>
-      <c r="F61" s="69"/>
-      <c r="G61" s="69"/>
+      <c r="C61" s="59"/>
+      <c r="D61" s="59"/>
+      <c r="E61" s="66"/>
+      <c r="F61" s="66"/>
+      <c r="G61" s="66"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
@@ -3082,11 +3110,11 @@
       <c r="B62" s="29">
         <v>1865</v>
       </c>
-      <c r="C62" s="62"/>
-      <c r="D62" s="62"/>
-      <c r="E62" s="69"/>
-      <c r="F62" s="69"/>
-      <c r="G62" s="69"/>
+      <c r="C62" s="59"/>
+      <c r="D62" s="59"/>
+      <c r="E62" s="66"/>
+      <c r="F62" s="66"/>
+      <c r="G62" s="66"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
@@ -3095,11 +3123,11 @@
       <c r="B63" s="29">
         <v>2036</v>
       </c>
-      <c r="C63" s="62"/>
-      <c r="D63" s="62"/>
-      <c r="E63" s="69"/>
-      <c r="F63" s="69"/>
-      <c r="G63" s="69"/>
+      <c r="C63" s="59"/>
+      <c r="D63" s="59"/>
+      <c r="E63" s="66"/>
+      <c r="F63" s="66"/>
+      <c r="G63" s="66"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
@@ -3108,22 +3136,22 @@
       <c r="B64" s="29">
         <v>1</v>
       </c>
-      <c r="C64" s="62"/>
-      <c r="D64" s="62"/>
-      <c r="E64" s="69"/>
-      <c r="F64" s="69"/>
-      <c r="G64" s="69"/>
+      <c r="C64" s="59"/>
+      <c r="D64" s="59"/>
+      <c r="E64" s="66"/>
+      <c r="F64" s="66"/>
+      <c r="G64" s="66"/>
     </row>
     <row r="65" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="B65" s="68"/>
-      <c r="C65" s="70"/>
-      <c r="D65" s="70"/>
-      <c r="E65" s="71"/>
-      <c r="F65" s="72"/>
-      <c r="G65" s="72"/>
+      <c r="B65" s="65"/>
+      <c r="C65" s="67"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="68"/>
+      <c r="F65" s="69"/>
+      <c r="G65" s="69"/>
       <c r="H65"/>
       <c r="I65"/>
     </row>
@@ -3131,12 +3159,12 @@
       <c r="A66" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="B66" s="68"/>
-      <c r="C66" s="70"/>
-      <c r="D66" s="70"/>
-      <c r="E66" s="71"/>
-      <c r="F66" s="72"/>
-      <c r="G66" s="72"/>
+      <c r="B66" s="65"/>
+      <c r="C66" s="67"/>
+      <c r="D66" s="67"/>
+      <c r="E66" s="68"/>
+      <c r="F66" s="69"/>
+      <c r="G66" s="69"/>
       <c r="H66"/>
       <c r="I66"/>
     </row>
@@ -3144,12 +3172,12 @@
       <c r="A67" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="B67" s="68"/>
-      <c r="C67" s="70"/>
-      <c r="D67" s="70"/>
-      <c r="E67" s="71"/>
-      <c r="F67" s="72"/>
-      <c r="G67" s="72"/>
+      <c r="B67" s="65"/>
+      <c r="C67" s="67"/>
+      <c r="D67" s="67"/>
+      <c r="E67" s="68"/>
+      <c r="F67" s="69"/>
+      <c r="G67" s="69"/>
       <c r="H67"/>
       <c r="I67"/>
     </row>
@@ -3158,63 +3186,63 @@
         <v>120</v>
       </c>
       <c r="B68" s="29"/>
-      <c r="C68" s="62"/>
-      <c r="D68" s="62"/>
-      <c r="E68" s="69"/>
-      <c r="F68" s="69"/>
-      <c r="G68" s="69"/>
+      <c r="C68" s="59"/>
+      <c r="D68" s="59"/>
+      <c r="E68" s="66"/>
+      <c r="F68" s="66"/>
+      <c r="G68" s="66"/>
     </row>
     <row r="69" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>119</v>
       </c>
       <c r="B69" s="29"/>
-      <c r="C69" s="62"/>
-      <c r="D69" s="62"/>
-      <c r="E69" s="69"/>
-      <c r="F69" s="69"/>
-      <c r="G69" s="69"/>
+      <c r="C69" s="59"/>
+      <c r="D69" s="59"/>
+      <c r="E69" s="66"/>
+      <c r="F69" s="66"/>
+      <c r="G69" s="66"/>
     </row>
     <row r="70" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>87</v>
       </c>
       <c r="B70" s="31"/>
-      <c r="C70" s="62"/>
-      <c r="D70" s="62"/>
-      <c r="E70" s="69"/>
-      <c r="F70" s="69"/>
-      <c r="G70" s="69"/>
+      <c r="C70" s="59"/>
+      <c r="D70" s="59"/>
+      <c r="E70" s="66"/>
+      <c r="F70" s="66"/>
+      <c r="G70" s="66"/>
     </row>
     <row r="71" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>53</v>
       </c>
       <c r="B71" s="32"/>
-      <c r="C71" s="62"/>
-      <c r="D71" s="62"/>
-      <c r="E71" s="69"/>
-      <c r="F71" s="69"/>
-      <c r="G71" s="69"/>
+      <c r="C71" s="59"/>
+      <c r="D71" s="59"/>
+      <c r="E71" s="66"/>
+      <c r="F71" s="66"/>
+      <c r="G71" s="66"/>
     </row>
     <row r="72" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>54</v>
       </c>
       <c r="B72" s="33"/>
-      <c r="C72" s="62"/>
-      <c r="D72" s="62"/>
-      <c r="E72" s="69"/>
-      <c r="F72" s="69"/>
-      <c r="G72" s="69"/>
+      <c r="C72" s="59"/>
+      <c r="D72" s="59"/>
+      <c r="E72" s="66"/>
+      <c r="F72" s="66"/>
+      <c r="G72" s="66"/>
     </row>
     <row r="73" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>1</v>
       </c>
       <c r="B73" s="34"/>
-      <c r="C73" s="62"/>
-      <c r="D73" s="62"/>
+      <c r="C73" s="59"/>
+      <c r="D73" s="59"/>
       <c r="E73" s="50"/>
       <c r="F73" s="50"/>
       <c r="G73" s="50"/>
@@ -3285,8 +3313,8 @@
         <v>2</v>
       </c>
       <c r="B74" s="34"/>
-      <c r="C74" s="62"/>
-      <c r="D74" s="62"/>
+      <c r="C74" s="59"/>
+      <c r="D74" s="59"/>
       <c r="E74" s="50"/>
       <c r="F74" s="50"/>
       <c r="G74" s="50"/>
@@ -3357,8 +3385,8 @@
         <v>72</v>
       </c>
       <c r="B75" s="35"/>
-      <c r="C75" s="62"/>
-      <c r="D75" s="62"/>
+      <c r="C75" s="59"/>
+      <c r="D75" s="59"/>
       <c r="E75" s="50"/>
       <c r="F75" s="50"/>
       <c r="G75" s="50"/>
@@ -3429,8 +3457,8 @@
         <v>74</v>
       </c>
       <c r="B76" s="34"/>
-      <c r="C76" s="62"/>
-      <c r="D76" s="62"/>
+      <c r="C76" s="59"/>
+      <c r="D76" s="59"/>
       <c r="E76" s="46"/>
       <c r="F76" s="46"/>
       <c r="G76" s="46"/>
@@ -3442,8 +3470,8 @@
         <v>73</v>
       </c>
       <c r="B77" s="34"/>
-      <c r="C77" s="62"/>
-      <c r="D77" s="62"/>
+      <c r="C77" s="59"/>
+      <c r="D77" s="59"/>
       <c r="E77" s="46"/>
       <c r="F77" s="46"/>
       <c r="G77" s="46"/>
@@ -3455,8 +3483,8 @@
         <v>71</v>
       </c>
       <c r="B78" s="34"/>
-      <c r="C78" s="62"/>
-      <c r="D78" s="62"/>
+      <c r="C78" s="59"/>
+      <c r="D78" s="59"/>
       <c r="E78" s="46"/>
       <c r="F78" s="46"/>
       <c r="G78" s="46"/>
@@ -3470,8 +3498,8 @@
       <c r="B79" s="36" t="b">
         <v>1</v>
       </c>
-      <c r="C79" s="62"/>
-      <c r="D79" s="62"/>
+      <c r="C79" s="59"/>
+      <c r="D79" s="59"/>
       <c r="E79" s="46"/>
       <c r="F79" s="46"/>
       <c r="G79" s="46"/>
@@ -3542,8 +3570,8 @@
         <v>75</v>
       </c>
       <c r="B80" s="37"/>
-      <c r="C80" s="64"/>
-      <c r="D80" s="64"/>
+      <c r="C80" s="61"/>
+      <c r="D80" s="61"/>
       <c r="E80" s="46"/>
       <c r="F80" s="46"/>
       <c r="G80" s="46"/>
@@ -3555,8 +3583,8 @@
         <v>76</v>
       </c>
       <c r="B81" s="37"/>
-      <c r="C81" s="64"/>
-      <c r="D81" s="64"/>
+      <c r="C81" s="61"/>
+      <c r="D81" s="61"/>
       <c r="E81" s="46"/>
       <c r="F81" s="46"/>
       <c r="G81" s="46"/>
@@ -3568,8 +3596,8 @@
         <v>77</v>
       </c>
       <c r="B82" s="37"/>
-      <c r="C82" s="64"/>
-      <c r="D82" s="64"/>
+      <c r="C82" s="61"/>
+      <c r="D82" s="61"/>
       <c r="E82" s="46"/>
       <c r="F82" s="46"/>
       <c r="G82" s="46"/>
@@ -3581,8 +3609,8 @@
         <v>78</v>
       </c>
       <c r="B83" s="37"/>
-      <c r="C83" s="64"/>
-      <c r="D83" s="64"/>
+      <c r="C83" s="61"/>
+      <c r="D83" s="61"/>
       <c r="E83" s="46"/>
       <c r="F83" s="46"/>
       <c r="G83" s="46"/>
@@ -3596,8 +3624,8 @@
       <c r="B84" s="38">
         <v>0.156</v>
       </c>
-      <c r="C84" s="64"/>
-      <c r="D84" s="64"/>
+      <c r="C84" s="61"/>
+      <c r="D84" s="61"/>
       <c r="E84" s="46"/>
       <c r="F84" s="46"/>
       <c r="G84" s="46"/>
@@ -3833,8 +3861,8 @@
         <v>16</v>
       </c>
       <c r="B89" s="42"/>
-      <c r="C89" s="65"/>
-      <c r="D89" s="65"/>
+      <c r="C89" s="62"/>
+      <c r="D89" s="62"/>
     </row>
     <row r="90" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
@@ -4002,11 +4030,11 @@
       <c r="A106" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B106" s="41" t="b">
-        <v>1</v>
-      </c>
+      <c r="B106" s="41"/>
       <c r="C106" s="50"/>
       <c r="D106" s="50"/>
+      <c r="E106" s="50"/>
+      <c r="F106" s="50"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
@@ -4015,6 +4043,8 @@
       <c r="B107" s="41"/>
       <c r="C107" s="50"/>
       <c r="D107" s="50"/>
+      <c r="E107" s="50"/>
+      <c r="F107" s="50"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
@@ -4023,218 +4053,488 @@
       <c r="B108" s="41"/>
       <c r="C108" s="50"/>
       <c r="D108" s="50"/>
+      <c r="E108" s="50"/>
+      <c r="F108" s="50"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B109" s="61"/>
-      <c r="C109" s="50"/>
-      <c r="D109" s="50"/>
+      <c r="B109" s="70"/>
+      <c r="C109" s="74"/>
+      <c r="D109" s="74"/>
+      <c r="E109" s="74"/>
+      <c r="F109" s="74"/>
+      <c r="G109"/>
+      <c r="H109"/>
+      <c r="I109"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="56" t="s">
         <v>89</v>
       </c>
-      <c r="B110" s="59"/>
-      <c r="C110" s="50"/>
-      <c r="D110" s="50"/>
+      <c r="B110" s="56"/>
+      <c r="C110" s="73"/>
+      <c r="D110" s="73"/>
+      <c r="E110" s="74"/>
+      <c r="F110" s="74"/>
+      <c r="G110"/>
+      <c r="H110"/>
+      <c r="I110"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="56" t="s">
         <v>95</v>
       </c>
-      <c r="B111" s="59"/>
-      <c r="C111" s="50"/>
-      <c r="D111" s="50"/>
+      <c r="B111" s="56"/>
+      <c r="C111" s="74"/>
+      <c r="D111" s="74"/>
+      <c r="E111" s="74"/>
+      <c r="F111" s="74"/>
+      <c r="G111"/>
+      <c r="H111"/>
+      <c r="I111"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="B112" s="56"/>
+      <c r="C112" s="74"/>
+      <c r="D112" s="74"/>
+      <c r="E112" s="74"/>
+      <c r="F112" s="74"/>
+      <c r="G112"/>
+      <c r="H112"/>
+      <c r="I112"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="56" t="s">
         <v>123</v>
       </c>
-      <c r="B112" s="59"/>
-      <c r="C112" s="50"/>
-      <c r="D112" s="50"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="56" t="s">
+      <c r="B113" s="56"/>
+      <c r="C113" s="74"/>
+      <c r="D113" s="74"/>
+      <c r="E113" s="74"/>
+      <c r="F113" s="74"/>
+      <c r="G113"/>
+      <c r="H113"/>
+      <c r="I113"/>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="B113" s="59"/>
-      <c r="C113" s="50"/>
-      <c r="D113" s="50"/>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="56" t="s">
+      <c r="B114" s="56"/>
+      <c r="C114" s="74"/>
+      <c r="D114" s="74"/>
+      <c r="E114" s="74"/>
+      <c r="F114" s="74"/>
+      <c r="G114"/>
+      <c r="H114"/>
+      <c r="I114"/>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="56" t="s">
         <v>90</v>
       </c>
-      <c r="B114" s="59"/>
-      <c r="C114" s="50"/>
-      <c r="D114" s="50"/>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="56" t="s">
+      <c r="B115" s="56"/>
+      <c r="C115" s="73"/>
+      <c r="D115" s="73"/>
+      <c r="E115" s="74"/>
+      <c r="F115" s="74"/>
+      <c r="G115"/>
+      <c r="H115"/>
+      <c r="I115"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="B115" s="59"/>
-      <c r="C115" s="50"/>
-      <c r="D115" s="50"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="56" t="s">
+      <c r="B116" s="56"/>
+      <c r="C116" s="74"/>
+      <c r="D116" s="74"/>
+      <c r="E116" s="74"/>
+      <c r="F116" s="74"/>
+      <c r="G116"/>
+      <c r="H116"/>
+      <c r="I116"/>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="56" t="s">
+        <v>143</v>
+      </c>
+      <c r="B117" s="56"/>
+      <c r="C117" s="74"/>
+      <c r="D117" s="74"/>
+      <c r="E117" s="74"/>
+      <c r="F117" s="74"/>
+      <c r="G117"/>
+      <c r="H117"/>
+      <c r="I117"/>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="56" t="s">
         <v>124</v>
       </c>
-      <c r="B116" s="59"/>
-      <c r="C116" s="50"/>
-      <c r="D116" s="50"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="56" t="s">
+      <c r="B118" s="56"/>
+      <c r="C118" s="74"/>
+      <c r="D118" s="74"/>
+      <c r="E118" s="74"/>
+      <c r="F118" s="74"/>
+      <c r="G118"/>
+      <c r="H118"/>
+      <c r="I118"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="B117" s="59"/>
-      <c r="C117" s="50"/>
-      <c r="D117" s="50"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="57" t="s">
+      <c r="B119" s="56"/>
+      <c r="C119" s="74"/>
+      <c r="D119" s="74"/>
+      <c r="E119" s="74"/>
+      <c r="F119" s="74"/>
+      <c r="G119"/>
+      <c r="H119"/>
+      <c r="I119"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="57" t="s">
         <v>91</v>
       </c>
-      <c r="B118" s="59"/>
-      <c r="C118" s="50"/>
-      <c r="D118" s="50"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="57" t="s">
+      <c r="B120" s="71"/>
+      <c r="C120" s="74"/>
+      <c r="D120" s="74"/>
+      <c r="E120" s="74"/>
+      <c r="F120" s="74"/>
+      <c r="G120"/>
+      <c r="H120"/>
+      <c r="I120"/>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="57" t="s">
         <v>99</v>
       </c>
-      <c r="B119" s="59"/>
-      <c r="C119" s="50"/>
-      <c r="D119" s="50"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="56" t="s">
+      <c r="B121" s="71"/>
+      <c r="C121" s="74"/>
+      <c r="D121" s="74"/>
+      <c r="E121" s="74"/>
+      <c r="F121" s="74"/>
+      <c r="G121"/>
+      <c r="H121"/>
+      <c r="I121"/>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="B122" s="71"/>
+      <c r="C122" s="74"/>
+      <c r="D122" s="74"/>
+      <c r="E122" s="74"/>
+      <c r="F122" s="74"/>
+      <c r="G122"/>
+      <c r="H122"/>
+      <c r="I122"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="56" t="s">
         <v>125</v>
       </c>
-      <c r="B120" s="59"/>
-      <c r="C120" s="50"/>
-      <c r="D120" s="50"/>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="57" t="s">
+      <c r="B123" s="71"/>
+      <c r="C123" s="74"/>
+      <c r="D123" s="74"/>
+      <c r="E123" s="74"/>
+      <c r="F123" s="74"/>
+      <c r="G123"/>
+      <c r="H123"/>
+      <c r="I123"/>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="B121" s="59"/>
-      <c r="C121" s="50"/>
-      <c r="D121" s="50"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="57" t="s">
+      <c r="B124" s="71"/>
+      <c r="C124" s="74"/>
+      <c r="D124" s="74"/>
+      <c r="E124" s="74"/>
+      <c r="F124" s="74"/>
+      <c r="G124"/>
+      <c r="H124"/>
+      <c r="I124"/>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="57" t="s">
         <v>92</v>
       </c>
-      <c r="B122" s="59"/>
-      <c r="C122" s="50"/>
-      <c r="D122" s="50"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="57" t="s">
+      <c r="B125" s="71"/>
+      <c r="C125" s="74"/>
+      <c r="D125" s="74"/>
+      <c r="E125" s="74"/>
+      <c r="F125" s="74"/>
+      <c r="G125"/>
+      <c r="H125"/>
+      <c r="I125"/>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="B123" s="59"/>
-      <c r="C123" s="50"/>
-      <c r="D123" s="50"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="56" t="s">
+      <c r="B126" s="71"/>
+      <c r="C126" s="74"/>
+      <c r="D126" s="74"/>
+      <c r="E126" s="74"/>
+      <c r="F126" s="74"/>
+      <c r="G126"/>
+      <c r="H126"/>
+      <c r="I126"/>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A127" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="B127" s="71"/>
+      <c r="C127" s="74"/>
+      <c r="D127" s="74"/>
+      <c r="E127" s="74"/>
+      <c r="F127" s="74"/>
+      <c r="G127"/>
+      <c r="H127"/>
+      <c r="I127"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A128" s="56" t="s">
         <v>126</v>
       </c>
-      <c r="B124" s="59"/>
-      <c r="C124" s="50"/>
-      <c r="D124" s="50"/>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="57" t="s">
+      <c r="B128" s="71"/>
+      <c r="C128" s="74"/>
+      <c r="D128" s="74"/>
+      <c r="E128" s="74"/>
+      <c r="F128" s="74"/>
+      <c r="G128"/>
+      <c r="H128"/>
+      <c r="I128"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A129" s="57" t="s">
         <v>102</v>
       </c>
-      <c r="B125" s="59"/>
-      <c r="C125" s="50"/>
-      <c r="D125" s="50"/>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="57" t="s">
+      <c r="B129" s="71"/>
+      <c r="C129" s="74"/>
+      <c r="D129" s="74"/>
+      <c r="E129" s="74"/>
+      <c r="F129" s="74"/>
+      <c r="G129"/>
+      <c r="H129"/>
+      <c r="I129"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A130" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="B126" s="59"/>
-      <c r="C126" s="50"/>
-      <c r="D126" s="50"/>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="57" t="s">
+      <c r="B130" s="71"/>
+      <c r="C130" s="74"/>
+      <c r="D130" s="74"/>
+      <c r="E130" s="74"/>
+      <c r="F130" s="74"/>
+      <c r="G130"/>
+      <c r="H130"/>
+      <c r="I130"/>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A131" s="57" t="s">
         <v>103</v>
       </c>
-      <c r="B127" s="59"/>
-      <c r="C127" s="50"/>
-      <c r="D127" s="50"/>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="56" t="s">
+      <c r="B131" s="71"/>
+      <c r="C131" s="74"/>
+      <c r="D131" s="74"/>
+      <c r="E131" s="75"/>
+      <c r="F131" s="74"/>
+      <c r="G131"/>
+      <c r="H131"/>
+      <c r="I131"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A132" s="57" t="s">
+        <v>146</v>
+      </c>
+      <c r="B132" s="71"/>
+      <c r="C132" s="74"/>
+      <c r="D132" s="74"/>
+      <c r="E132" s="75"/>
+      <c r="F132" s="74"/>
+      <c r="G132"/>
+      <c r="H132"/>
+      <c r="I132"/>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A133" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="B128" s="59"/>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="57" t="s">
+      <c r="B133" s="71"/>
+      <c r="C133" s="74"/>
+      <c r="D133" s="74"/>
+      <c r="E133" s="74"/>
+      <c r="F133" s="74"/>
+      <c r="G133"/>
+      <c r="H133"/>
+      <c r="I133"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A134" s="57" t="s">
         <v>104</v>
       </c>
-      <c r="B129" s="59"/>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="57" t="s">
+      <c r="B134" s="71"/>
+      <c r="C134" s="74"/>
+      <c r="D134" s="74"/>
+      <c r="E134" s="74"/>
+      <c r="F134" s="74"/>
+      <c r="G134"/>
+      <c r="H134"/>
+      <c r="I134"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A135" s="57" t="s">
         <v>94</v>
       </c>
-      <c r="B130" s="59"/>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="57" t="s">
+      <c r="B135" s="56"/>
+      <c r="C135" s="74"/>
+      <c r="D135" s="74"/>
+      <c r="E135" s="74"/>
+      <c r="F135" s="74"/>
+      <c r="G135"/>
+      <c r="H135"/>
+      <c r="I135"/>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A136" s="57" t="s">
         <v>105</v>
       </c>
-      <c r="B131" s="59"/>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="56" t="s">
+      <c r="B136" s="56"/>
+      <c r="C136" s="74"/>
+      <c r="D136" s="74"/>
+      <c r="E136" s="74"/>
+      <c r="F136" s="74"/>
+      <c r="G136"/>
+      <c r="H136"/>
+      <c r="I136"/>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A137" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="B137" s="56"/>
+      <c r="C137" s="74"/>
+      <c r="D137" s="74"/>
+      <c r="E137" s="74"/>
+      <c r="F137" s="74"/>
+      <c r="G137"/>
+      <c r="H137"/>
+      <c r="I137"/>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A138" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="B132" s="59"/>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="57" t="s">
+      <c r="B138" s="56"/>
+      <c r="C138" s="74"/>
+      <c r="D138" s="74"/>
+      <c r="E138" s="74"/>
+      <c r="F138" s="74"/>
+      <c r="G138"/>
+      <c r="H138"/>
+      <c r="I138"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A139" s="57" t="s">
         <v>106</v>
       </c>
-      <c r="B133" s="59"/>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="57" t="s">
+      <c r="B139" s="56"/>
+      <c r="C139" s="74"/>
+      <c r="D139" s="74"/>
+      <c r="E139" s="74"/>
+      <c r="F139" s="74"/>
+      <c r="G139"/>
+      <c r="H139"/>
+      <c r="I139"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A140" s="57" t="s">
         <v>134</v>
       </c>
-      <c r="B134" s="59"/>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="57" t="s">
+      <c r="B140" s="56"/>
+      <c r="C140" s="74"/>
+      <c r="D140" s="74"/>
+      <c r="E140" s="74"/>
+      <c r="F140" s="74"/>
+      <c r="G140"/>
+      <c r="H140"/>
+      <c r="I140"/>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A141" s="57" t="s">
         <v>135</v>
       </c>
-      <c r="B135" s="59"/>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="56" t="s">
+      <c r="B141" s="56"/>
+      <c r="C141" s="74"/>
+      <c r="D141" s="74"/>
+      <c r="E141" s="74"/>
+      <c r="F141" s="74"/>
+      <c r="G141"/>
+      <c r="H141"/>
+      <c r="I141"/>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A142" s="57" t="s">
+        <v>148</v>
+      </c>
+      <c r="B142" s="56"/>
+      <c r="C142" s="74"/>
+      <c r="D142" s="74"/>
+      <c r="E142" s="74"/>
+      <c r="F142" s="74"/>
+      <c r="G142"/>
+      <c r="H142"/>
+      <c r="I142"/>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A143" s="56" t="s">
         <v>137</v>
       </c>
-      <c r="B136" s="59"/>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="58" t="s">
+      <c r="B143" s="56"/>
+      <c r="C143" s="74"/>
+      <c r="D143" s="74"/>
+      <c r="E143" s="74"/>
+      <c r="F143" s="74"/>
+      <c r="G143"/>
+      <c r="H143"/>
+      <c r="I143"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A144" s="58" t="s">
         <v>136</v>
       </c>
-      <c r="B137" s="60"/>
+      <c r="B144" s="72"/>
+      <c r="C144" s="74"/>
+      <c r="D144" s="74"/>
+      <c r="E144" s="74"/>
+      <c r="F144" s="74"/>
+      <c r="G144"/>
+      <c r="H144"/>
+      <c r="I144"/>
+    </row>
+    <row r="145" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C145" s="50"/>
+      <c r="D145" s="50"/>
+      <c r="E145" s="50"/>
+      <c r="F145" s="50"/>
+    </row>
+    <row r="146" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C146" s="50"/>
+      <c r="D146" s="50"/>
+      <c r="E146" s="50"/>
+      <c r="F146" s="50"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">

</xml_diff>

<commit_message>
Renaming and correction to startup calculations
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2476,8 +2476,8 @@
   </sheetPr>
   <dimension ref="A1:BP146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revise popsize calculation for Xpert
And remove very old code for simple model.
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="150">
   <si>
     <t>recent_time</t>
   </si>
@@ -462,6 +462,9 @@
   </si>
   <si>
     <t>econ_startupcost_decentralisation</t>
+  </si>
+  <si>
+    <t>program_number_tests_per_tb_presentation</t>
   </si>
 </sst>
 </file>
@@ -2474,10 +2477,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP146"/>
+  <dimension ref="A1:BP147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2938,7 +2941,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="B44" s="63"/>
       <c r="C44" s="63"/>
@@ -2950,60 +2953,65 @@
       <c r="I44"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="50"/>
+      <c r="A45" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B45" s="63"/>
+      <c r="C45" s="63"/>
+      <c r="D45" s="63"/>
+      <c r="E45" s="64"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B46" s="25">
-        <v>25</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B46" s="25"/>
       <c r="C46" s="25"/>
       <c r="D46" s="25"/>
       <c r="E46" s="50"/>
       <c r="F46" s="50"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
+      <c r="A47" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B47" s="25">
+        <v>25</v>
+      </c>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
       <c r="E47" s="50"/>
       <c r="F47" s="50"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="27"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="50"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="28">
+      <c r="B49" s="28">
         <v>0.05</v>
       </c>
-      <c r="C48" s="50"/>
-      <c r="D48" s="50"/>
-      <c r="E48" s="46"/>
-      <c r="F48" s="46"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="29"/>
-      <c r="C49" s="59"/>
-      <c r="D49" s="59"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="46"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B50" s="29"/>
       <c r="C50" s="59"/>
@@ -3011,7 +3019,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>13</v>
+        <v>82</v>
       </c>
       <c r="B51" s="29"/>
       <c r="C51" s="59"/>
@@ -3019,23 +3027,23 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B52" s="29"/>
       <c r="C52" s="59"/>
       <c r="D52" s="59"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B53" s="30"/>
-      <c r="C53" s="60"/>
-      <c r="D53" s="60"/>
+      <c r="A53" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="29"/>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B54" s="30"/>
       <c r="C54" s="60"/>
@@ -3043,23 +3051,23 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B55" s="30"/>
       <c r="C55" s="60"/>
       <c r="D55" s="60"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B56" s="29"/>
-      <c r="C56" s="59"/>
-      <c r="D56" s="59"/>
+      <c r="A56" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B56" s="30"/>
+      <c r="C56" s="60"/>
+      <c r="D56" s="60"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B57" s="29"/>
       <c r="C57" s="59"/>
@@ -3067,7 +3075,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>141</v>
+        <v>11</v>
       </c>
       <c r="B58" s="29"/>
       <c r="C58" s="59"/>
@@ -3075,7 +3083,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>13</v>
+        <v>141</v>
       </c>
       <c r="B59" s="29"/>
       <c r="C59" s="59"/>
@@ -3083,18 +3091,15 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B60" s="29"/>
       <c r="C60" s="59"/>
       <c r="D60" s="59"/>
-      <c r="E60" s="66"/>
-      <c r="F60" s="66"/>
-      <c r="G60" s="66"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B61" s="29"/>
       <c r="C61" s="59"/>
@@ -3105,11 +3110,9 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B62" s="29">
-        <v>1865</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B62" s="29"/>
       <c r="C62" s="59"/>
       <c r="D62" s="59"/>
       <c r="E62" s="66"/>
@@ -3118,10 +3121,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B63" s="29">
-        <v>2036</v>
+        <v>1865</v>
       </c>
       <c r="C63" s="59"/>
       <c r="D63" s="59"/>
@@ -3131,10 +3134,10 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B64" s="29">
-        <v>1</v>
+        <v>2036</v>
       </c>
       <c r="C64" s="59"/>
       <c r="D64" s="59"/>
@@ -3144,20 +3147,20 @@
     </row>
     <row r="65" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="B65" s="65"/>
-      <c r="C65" s="67"/>
-      <c r="D65" s="67"/>
-      <c r="E65" s="68"/>
-      <c r="F65" s="69"/>
-      <c r="G65" s="69"/>
-      <c r="H65"/>
-      <c r="I65"/>
+        <v>111</v>
+      </c>
+      <c r="B65" s="29">
+        <v>1</v>
+      </c>
+      <c r="C65" s="59"/>
+      <c r="D65" s="59"/>
+      <c r="E65" s="66"/>
+      <c r="F65" s="66"/>
+      <c r="G65" s="66"/>
     </row>
     <row r="66" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B66" s="65"/>
       <c r="C66" s="67"/>
@@ -3170,7 +3173,7 @@
     </row>
     <row r="67" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B67" s="65"/>
       <c r="C67" s="67"/>
@@ -3183,18 +3186,20 @@
     </row>
     <row r="68" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B68" s="29"/>
-      <c r="C68" s="59"/>
-      <c r="D68" s="59"/>
-      <c r="E68" s="66"/>
-      <c r="F68" s="66"/>
-      <c r="G68" s="66"/>
+        <v>140</v>
+      </c>
+      <c r="B68" s="65"/>
+      <c r="C68" s="67"/>
+      <c r="D68" s="67"/>
+      <c r="E68" s="68"/>
+      <c r="F68" s="69"/>
+      <c r="G68" s="69"/>
+      <c r="H68"/>
+      <c r="I68"/>
     </row>
     <row r="69" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B69" s="29"/>
       <c r="C69" s="59"/>
@@ -3205,9 +3210,9 @@
     </row>
     <row r="70" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B70" s="31"/>
+        <v>119</v>
+      </c>
+      <c r="B70" s="29"/>
       <c r="C70" s="59"/>
       <c r="D70" s="59"/>
       <c r="E70" s="66"/>
@@ -3215,10 +3220,10 @@
       <c r="G70" s="66"/>
     </row>
     <row r="71" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B71" s="32"/>
+      <c r="A71" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B71" s="31"/>
       <c r="C71" s="59"/>
       <c r="D71" s="59"/>
       <c r="E71" s="66"/>
@@ -3226,10 +3231,10 @@
       <c r="G71" s="66"/>
     </row>
     <row r="72" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A72" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B72" s="33"/>
+      <c r="A72" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B72" s="32"/>
       <c r="C72" s="59"/>
       <c r="D72" s="59"/>
       <c r="E72" s="66"/>
@@ -3237,80 +3242,19 @@
       <c r="G72" s="66"/>
     </row>
     <row r="73" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A73" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B73" s="34"/>
+      <c r="A73" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B73" s="33"/>
       <c r="C73" s="59"/>
       <c r="D73" s="59"/>
-      <c r="E73" s="50"/>
-      <c r="F73" s="50"/>
-      <c r="G73" s="50"/>
-      <c r="H73" s="46"/>
-      <c r="I73" s="46"/>
-      <c r="J73" s="15"/>
-      <c r="K73" s="15"/>
-      <c r="L73" s="15"/>
-      <c r="M73" s="15"/>
-      <c r="N73" s="15"/>
-      <c r="O73" s="15"/>
-      <c r="P73" s="15"/>
-      <c r="Q73" s="15"/>
-      <c r="R73" s="15"/>
-      <c r="S73" s="15"/>
-      <c r="T73" s="15"/>
-      <c r="U73" s="15"/>
-      <c r="V73" s="15"/>
-      <c r="W73" s="15"/>
-      <c r="X73" s="15"/>
-      <c r="Y73" s="15"/>
-      <c r="Z73" s="15"/>
-      <c r="AA73" s="15"/>
-      <c r="AB73" s="15"/>
-      <c r="AC73" s="15"/>
-      <c r="AD73" s="15"/>
-      <c r="AE73" s="15"/>
-      <c r="AF73" s="15"/>
-      <c r="AG73" s="15"/>
-      <c r="AH73" s="15"/>
-      <c r="AI73" s="15"/>
-      <c r="AJ73" s="15"/>
-      <c r="AK73" s="15"/>
-      <c r="AL73" s="15"/>
-      <c r="AM73" s="15"/>
-      <c r="AN73" s="15"/>
-      <c r="AO73" s="15"/>
-      <c r="AP73" s="15"/>
-      <c r="AQ73" s="15"/>
-      <c r="AR73" s="15"/>
-      <c r="AS73" s="15"/>
-      <c r="AT73" s="15"/>
-      <c r="AU73" s="15"/>
-      <c r="AV73" s="15"/>
-      <c r="AW73" s="15"/>
-      <c r="AX73" s="15"/>
-      <c r="AY73" s="15"/>
-      <c r="AZ73" s="15"/>
-      <c r="BA73" s="15"/>
-      <c r="BB73" s="15"/>
-      <c r="BC73" s="15"/>
-      <c r="BD73" s="15"/>
-      <c r="BE73" s="15"/>
-      <c r="BF73" s="15"/>
-      <c r="BG73" s="15"/>
-      <c r="BH73" s="15"/>
-      <c r="BI73" s="15"/>
-      <c r="BJ73" s="15"/>
-      <c r="BK73" s="15"/>
-      <c r="BL73" s="15"/>
-      <c r="BM73" s="15"/>
-      <c r="BN73" s="15"/>
-      <c r="BO73" s="15"/>
-      <c r="BP73" s="15"/>
+      <c r="E73" s="66"/>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
     </row>
     <row r="74" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B74" s="34"/>
       <c r="C74" s="59"/>
@@ -3380,11 +3324,11 @@
       <c r="BO74" s="15"/>
       <c r="BP74" s="15"/>
     </row>
-    <row r="75" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B75" s="35"/>
+    <row r="75" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A75" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B75" s="34"/>
       <c r="C75" s="59"/>
       <c r="D75" s="59"/>
       <c r="E75" s="50"/>
@@ -3452,22 +3396,81 @@
       <c r="BO75" s="15"/>
       <c r="BP75" s="15"/>
     </row>
-    <row r="76" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B76" s="34"/>
+    <row r="76" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B76" s="35"/>
       <c r="C76" s="59"/>
       <c r="D76" s="59"/>
-      <c r="E76" s="46"/>
-      <c r="F76" s="46"/>
-      <c r="G76" s="46"/>
+      <c r="E76" s="50"/>
+      <c r="F76" s="50"/>
+      <c r="G76" s="50"/>
       <c r="H76" s="46"/>
       <c r="I76" s="46"/>
+      <c r="J76" s="15"/>
+      <c r="K76" s="15"/>
+      <c r="L76" s="15"/>
+      <c r="M76" s="15"/>
+      <c r="N76" s="15"/>
+      <c r="O76" s="15"/>
+      <c r="P76" s="15"/>
+      <c r="Q76" s="15"/>
+      <c r="R76" s="15"/>
+      <c r="S76" s="15"/>
+      <c r="T76" s="15"/>
+      <c r="U76" s="15"/>
+      <c r="V76" s="15"/>
+      <c r="W76" s="15"/>
+      <c r="X76" s="15"/>
+      <c r="Y76" s="15"/>
+      <c r="Z76" s="15"/>
+      <c r="AA76" s="15"/>
+      <c r="AB76" s="15"/>
+      <c r="AC76" s="15"/>
+      <c r="AD76" s="15"/>
+      <c r="AE76" s="15"/>
+      <c r="AF76" s="15"/>
+      <c r="AG76" s="15"/>
+      <c r="AH76" s="15"/>
+      <c r="AI76" s="15"/>
+      <c r="AJ76" s="15"/>
+      <c r="AK76" s="15"/>
+      <c r="AL76" s="15"/>
+      <c r="AM76" s="15"/>
+      <c r="AN76" s="15"/>
+      <c r="AO76" s="15"/>
+      <c r="AP76" s="15"/>
+      <c r="AQ76" s="15"/>
+      <c r="AR76" s="15"/>
+      <c r="AS76" s="15"/>
+      <c r="AT76" s="15"/>
+      <c r="AU76" s="15"/>
+      <c r="AV76" s="15"/>
+      <c r="AW76" s="15"/>
+      <c r="AX76" s="15"/>
+      <c r="AY76" s="15"/>
+      <c r="AZ76" s="15"/>
+      <c r="BA76" s="15"/>
+      <c r="BB76" s="15"/>
+      <c r="BC76" s="15"/>
+      <c r="BD76" s="15"/>
+      <c r="BE76" s="15"/>
+      <c r="BF76" s="15"/>
+      <c r="BG76" s="15"/>
+      <c r="BH76" s="15"/>
+      <c r="BI76" s="15"/>
+      <c r="BJ76" s="15"/>
+      <c r="BK76" s="15"/>
+      <c r="BL76" s="15"/>
+      <c r="BM76" s="15"/>
+      <c r="BN76" s="15"/>
+      <c r="BO76" s="15"/>
+      <c r="BP76" s="15"/>
     </row>
     <row r="77" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B77" s="34"/>
       <c r="C77" s="59"/>
@@ -3480,7 +3483,7 @@
     </row>
     <row r="78" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B78" s="34"/>
       <c r="C78" s="59"/>
@@ -3491,13 +3494,11 @@
       <c r="H78" s="46"/>
       <c r="I78" s="46"/>
     </row>
-    <row r="79" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B79" s="36" t="b">
-        <v>1</v>
-      </c>
+    <row r="79" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B79" s="34"/>
       <c r="C79" s="59"/>
       <c r="D79" s="59"/>
       <c r="E79" s="46"/>
@@ -3505,82 +3506,84 @@
       <c r="G79" s="46"/>
       <c r="H79" s="46"/>
       <c r="I79" s="46"/>
-      <c r="J79" s="15"/>
-      <c r="K79" s="15"/>
-      <c r="L79" s="15"/>
-      <c r="M79" s="15"/>
-      <c r="N79" s="15"/>
-      <c r="O79" s="15"/>
-      <c r="P79" s="15"/>
-      <c r="Q79" s="15"/>
-      <c r="R79" s="15"/>
-      <c r="S79" s="15"/>
-      <c r="T79" s="15"/>
-      <c r="U79" s="15"/>
-      <c r="V79" s="15"/>
-      <c r="W79" s="15"/>
-      <c r="X79" s="15"/>
-      <c r="Y79" s="15"/>
-      <c r="Z79" s="15"/>
-      <c r="AA79" s="15"/>
-      <c r="AB79" s="15"/>
-      <c r="AC79" s="15"/>
-      <c r="AD79" s="15"/>
-      <c r="AE79" s="15"/>
-      <c r="AF79" s="15"/>
-      <c r="AG79" s="15"/>
-      <c r="AH79" s="15"/>
-      <c r="AI79" s="15"/>
-      <c r="AJ79" s="15"/>
-      <c r="AK79" s="15"/>
-      <c r="AL79" s="15"/>
-      <c r="AM79" s="15"/>
-      <c r="AN79" s="15"/>
-      <c r="AO79" s="15"/>
-      <c r="AP79" s="15"/>
-      <c r="AQ79" s="15"/>
-      <c r="AR79" s="15"/>
-      <c r="AS79" s="15"/>
-      <c r="AT79" s="15"/>
-      <c r="AU79" s="15"/>
-      <c r="AV79" s="15"/>
-      <c r="AW79" s="15"/>
-      <c r="AX79" s="15"/>
-      <c r="AY79" s="15"/>
-      <c r="AZ79" s="15"/>
-      <c r="BA79" s="15"/>
-      <c r="BB79" s="15"/>
-      <c r="BC79" s="15"/>
-      <c r="BD79" s="15"/>
-      <c r="BE79" s="15"/>
-      <c r="BF79" s="15"/>
-      <c r="BG79" s="15"/>
-      <c r="BH79" s="15"/>
-      <c r="BI79" s="15"/>
-      <c r="BJ79" s="15"/>
-      <c r="BK79" s="15"/>
-      <c r="BL79" s="15"/>
-      <c r="BM79" s="15"/>
-      <c r="BN79" s="15"/>
-      <c r="BO79" s="15"/>
-      <c r="BP79" s="15"/>
-    </row>
-    <row r="80" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B80" s="37"/>
-      <c r="C80" s="61"/>
-      <c r="D80" s="61"/>
+    </row>
+    <row r="80" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B80" s="36" t="b">
+        <v>1</v>
+      </c>
+      <c r="C80" s="59"/>
+      <c r="D80" s="59"/>
       <c r="E80" s="46"/>
       <c r="F80" s="46"/>
       <c r="G80" s="46"/>
       <c r="H80" s="46"/>
       <c r="I80" s="46"/>
+      <c r="J80" s="15"/>
+      <c r="K80" s="15"/>
+      <c r="L80" s="15"/>
+      <c r="M80" s="15"/>
+      <c r="N80" s="15"/>
+      <c r="O80" s="15"/>
+      <c r="P80" s="15"/>
+      <c r="Q80" s="15"/>
+      <c r="R80" s="15"/>
+      <c r="S80" s="15"/>
+      <c r="T80" s="15"/>
+      <c r="U80" s="15"/>
+      <c r="V80" s="15"/>
+      <c r="W80" s="15"/>
+      <c r="X80" s="15"/>
+      <c r="Y80" s="15"/>
+      <c r="Z80" s="15"/>
+      <c r="AA80" s="15"/>
+      <c r="AB80" s="15"/>
+      <c r="AC80" s="15"/>
+      <c r="AD80" s="15"/>
+      <c r="AE80" s="15"/>
+      <c r="AF80" s="15"/>
+      <c r="AG80" s="15"/>
+      <c r="AH80" s="15"/>
+      <c r="AI80" s="15"/>
+      <c r="AJ80" s="15"/>
+      <c r="AK80" s="15"/>
+      <c r="AL80" s="15"/>
+      <c r="AM80" s="15"/>
+      <c r="AN80" s="15"/>
+      <c r="AO80" s="15"/>
+      <c r="AP80" s="15"/>
+      <c r="AQ80" s="15"/>
+      <c r="AR80" s="15"/>
+      <c r="AS80" s="15"/>
+      <c r="AT80" s="15"/>
+      <c r="AU80" s="15"/>
+      <c r="AV80" s="15"/>
+      <c r="AW80" s="15"/>
+      <c r="AX80" s="15"/>
+      <c r="AY80" s="15"/>
+      <c r="AZ80" s="15"/>
+      <c r="BA80" s="15"/>
+      <c r="BB80" s="15"/>
+      <c r="BC80" s="15"/>
+      <c r="BD80" s="15"/>
+      <c r="BE80" s="15"/>
+      <c r="BF80" s="15"/>
+      <c r="BG80" s="15"/>
+      <c r="BH80" s="15"/>
+      <c r="BI80" s="15"/>
+      <c r="BJ80" s="15"/>
+      <c r="BK80" s="15"/>
+      <c r="BL80" s="15"/>
+      <c r="BM80" s="15"/>
+      <c r="BN80" s="15"/>
+      <c r="BO80" s="15"/>
+      <c r="BP80" s="15"/>
     </row>
     <row r="81" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B81" s="37"/>
       <c r="C81" s="61"/>
@@ -3593,7 +3596,7 @@
     </row>
     <row r="82" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B82" s="37"/>
       <c r="C82" s="61"/>
@@ -3606,7 +3609,7 @@
     </row>
     <row r="83" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B83" s="37"/>
       <c r="C83" s="61"/>
@@ -3618,12 +3621,10 @@
       <c r="I83" s="46"/>
     </row>
     <row r="84" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B84" s="38">
-        <v>0.156</v>
-      </c>
+      <c r="A84" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B84" s="37"/>
       <c r="C84" s="61"/>
       <c r="D84" s="61"/>
       <c r="E84" s="46"/>
@@ -3632,81 +3633,24 @@
       <c r="H84" s="46"/>
       <c r="I84" s="46"/>
     </row>
-    <row r="85" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A85" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B85" s="39"/>
-      <c r="C85" s="50"/>
-      <c r="D85" s="50"/>
+    <row r="85" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B85" s="38">
+        <v>0.156</v>
+      </c>
+      <c r="C85" s="61"/>
+      <c r="D85" s="61"/>
       <c r="E85" s="46"/>
       <c r="F85" s="46"/>
       <c r="G85" s="46"/>
       <c r="H85" s="46"/>
       <c r="I85" s="46"/>
-      <c r="J85" s="15"/>
-      <c r="K85" s="15"/>
-      <c r="L85" s="15"/>
-      <c r="M85" s="15"/>
-      <c r="N85" s="15"/>
-      <c r="O85" s="15"/>
-      <c r="P85" s="15"/>
-      <c r="Q85" s="15"/>
-      <c r="R85" s="15"/>
-      <c r="S85" s="15"/>
-      <c r="T85" s="15"/>
-      <c r="U85" s="15"/>
-      <c r="V85" s="15"/>
-      <c r="W85" s="15"/>
-      <c r="X85" s="15"/>
-      <c r="Y85" s="15"/>
-      <c r="Z85" s="15"/>
-      <c r="AA85" s="15"/>
-      <c r="AB85" s="15"/>
-      <c r="AC85" s="15"/>
-      <c r="AD85" s="15"/>
-      <c r="AE85" s="15"/>
-      <c r="AF85" s="15"/>
-      <c r="AG85" s="15"/>
-      <c r="AH85" s="15"/>
-      <c r="AI85" s="15"/>
-      <c r="AJ85" s="15"/>
-      <c r="AK85" s="15"/>
-      <c r="AL85" s="15"/>
-      <c r="AM85" s="15"/>
-      <c r="AN85" s="15"/>
-      <c r="AO85" s="15"/>
-      <c r="AP85" s="15"/>
-      <c r="AQ85" s="15"/>
-      <c r="AR85" s="15"/>
-      <c r="AS85" s="15"/>
-      <c r="AT85" s="15"/>
-      <c r="AU85" s="15"/>
-      <c r="AV85" s="15"/>
-      <c r="AW85" s="15"/>
-      <c r="AX85" s="15"/>
-      <c r="AY85" s="15"/>
-      <c r="AZ85" s="15"/>
-      <c r="BA85" s="15"/>
-      <c r="BB85" s="15"/>
-      <c r="BC85" s="15"/>
-      <c r="BD85" s="15"/>
-      <c r="BE85" s="15"/>
-      <c r="BF85" s="15"/>
-      <c r="BG85" s="15"/>
-      <c r="BH85" s="15"/>
-      <c r="BI85" s="15"/>
-      <c r="BJ85" s="15"/>
-      <c r="BK85" s="15"/>
-      <c r="BL85" s="15"/>
-      <c r="BM85" s="15"/>
-      <c r="BN85" s="15"/>
-      <c r="BO85" s="15"/>
-      <c r="BP85" s="15"/>
     </row>
     <row r="86" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B86" s="39"/>
       <c r="C86" s="50"/>
@@ -3777,10 +3721,10 @@
       <c r="BP86" s="15"/>
     </row>
     <row r="87" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A87" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B87" s="40"/>
+      <c r="A87" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B87" s="39"/>
       <c r="C87" s="50"/>
       <c r="D87" s="50"/>
       <c r="E87" s="46"/>
@@ -3849,78 +3793,142 @@
       <c r="BP87" s="15"/>
     </row>
     <row r="88" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A88" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B88" s="41"/>
+      <c r="A88" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" s="40"/>
       <c r="C88" s="50"/>
       <c r="D88" s="50"/>
+      <c r="E88" s="46"/>
+      <c r="F88" s="46"/>
+      <c r="G88" s="46"/>
+      <c r="H88" s="46"/>
+      <c r="I88" s="46"/>
+      <c r="J88" s="15"/>
+      <c r="K88" s="15"/>
+      <c r="L88" s="15"/>
+      <c r="M88" s="15"/>
+      <c r="N88" s="15"/>
+      <c r="O88" s="15"/>
+      <c r="P88" s="15"/>
+      <c r="Q88" s="15"/>
+      <c r="R88" s="15"/>
+      <c r="S88" s="15"/>
+      <c r="T88" s="15"/>
+      <c r="U88" s="15"/>
+      <c r="V88" s="15"/>
+      <c r="W88" s="15"/>
+      <c r="X88" s="15"/>
+      <c r="Y88" s="15"/>
+      <c r="Z88" s="15"/>
+      <c r="AA88" s="15"/>
+      <c r="AB88" s="15"/>
+      <c r="AC88" s="15"/>
+      <c r="AD88" s="15"/>
+      <c r="AE88" s="15"/>
+      <c r="AF88" s="15"/>
+      <c r="AG88" s="15"/>
+      <c r="AH88" s="15"/>
+      <c r="AI88" s="15"/>
+      <c r="AJ88" s="15"/>
+      <c r="AK88" s="15"/>
+      <c r="AL88" s="15"/>
+      <c r="AM88" s="15"/>
+      <c r="AN88" s="15"/>
+      <c r="AO88" s="15"/>
+      <c r="AP88" s="15"/>
+      <c r="AQ88" s="15"/>
+      <c r="AR88" s="15"/>
+      <c r="AS88" s="15"/>
+      <c r="AT88" s="15"/>
+      <c r="AU88" s="15"/>
+      <c r="AV88" s="15"/>
+      <c r="AW88" s="15"/>
+      <c r="AX88" s="15"/>
+      <c r="AY88" s="15"/>
+      <c r="AZ88" s="15"/>
+      <c r="BA88" s="15"/>
+      <c r="BB88" s="15"/>
+      <c r="BC88" s="15"/>
+      <c r="BD88" s="15"/>
+      <c r="BE88" s="15"/>
+      <c r="BF88" s="15"/>
+      <c r="BG88" s="15"/>
+      <c r="BH88" s="15"/>
+      <c r="BI88" s="15"/>
+      <c r="BJ88" s="15"/>
+      <c r="BK88" s="15"/>
+      <c r="BL88" s="15"/>
+      <c r="BM88" s="15"/>
+      <c r="BN88" s="15"/>
+      <c r="BO88" s="15"/>
+      <c r="BP88" s="15"/>
     </row>
     <row r="89" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B89" s="42"/>
-      <c r="C89" s="62"/>
-      <c r="D89" s="62"/>
+        <v>9</v>
+      </c>
+      <c r="B89" s="41"/>
+      <c r="C89" s="50"/>
+      <c r="D89" s="50"/>
     </row>
     <row r="90" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B90" s="42"/>
+      <c r="C90" s="62"/>
+      <c r="D90" s="62"/>
+    </row>
+    <row r="91" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A91" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="41"/>
-      <c r="C90" s="50"/>
-      <c r="D90" s="50"/>
-    </row>
-    <row r="91" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A91" s="17" t="s">
+      <c r="B91" s="41"/>
+      <c r="C91" s="50"/>
+      <c r="D91" s="50"/>
+    </row>
+    <row r="92" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A92" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B91" s="43"/>
-      <c r="C91" s="43"/>
-      <c r="D91" s="43"/>
-      <c r="E91" s="52"/>
-      <c r="F91" s="52"/>
-      <c r="G91" s="52"/>
-      <c r="H91" s="53"/>
-    </row>
-    <row r="92" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A92" s="16" t="s">
+      <c r="B92" s="43"/>
+      <c r="C92" s="43"/>
+      <c r="D92" s="43"/>
+      <c r="E92" s="52"/>
+      <c r="F92" s="52"/>
+      <c r="G92" s="52"/>
+      <c r="H92" s="53"/>
+    </row>
+    <row r="93" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A93" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B92" s="44">
+      <c r="B93" s="44">
         <v>5</v>
       </c>
-      <c r="C92" s="44">
+      <c r="C93" s="44">
         <v>15</v>
       </c>
-      <c r="D92" s="44">
+      <c r="D93" s="44">
         <v>25</v>
       </c>
-      <c r="E92" s="44"/>
-      <c r="F92" s="44"/>
-      <c r="G92" s="44"/>
-      <c r="H92" s="54"/>
-    </row>
-    <row r="93" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A93" s="18" t="s">
+      <c r="E93" s="44"/>
+      <c r="F93" s="44"/>
+      <c r="G93" s="44"/>
+      <c r="H93" s="54"/>
+    </row>
+    <row r="94" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A94" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B93" s="45"/>
-      <c r="C93" s="50"/>
-      <c r="D93" s="50"/>
-    </row>
-    <row r="94" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A94" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B94" s="41"/>
+      <c r="B94" s="45"/>
       <c r="C94" s="50"/>
       <c r="D94" s="50"/>
     </row>
     <row r="95" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B95" s="41"/>
       <c r="C95" s="50"/>
@@ -3928,7 +3936,7 @@
     </row>
     <row r="96" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B96" s="41"/>
       <c r="C96" s="50"/>
@@ -3936,7 +3944,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
       <c r="B97" s="41"/>
       <c r="C97" s="50"/>
@@ -3944,28 +3952,23 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="B98" s="41"/>
       <c r="C98" s="50"/>
       <c r="D98" s="50"/>
     </row>
-    <row r="99" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
-        <v>68</v>
+        <v>129</v>
       </c>
       <c r="B99" s="41"/>
       <c r="C99" s="50"/>
       <c r="D99" s="50"/>
-      <c r="E99" s="50"/>
-      <c r="F99" s="50"/>
-      <c r="G99" s="46"/>
-      <c r="H99" s="46"/>
-      <c r="I99" s="46"/>
     </row>
     <row r="100" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B100" s="41"/>
       <c r="C100" s="50"/>
@@ -3978,7 +3981,7 @@
     </row>
     <row r="101" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
-        <v>121</v>
+        <v>69</v>
       </c>
       <c r="B101" s="41"/>
       <c r="C101" s="50"/>
@@ -3991,7 +3994,7 @@
     </row>
     <row r="102" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="B102" s="41"/>
       <c r="C102" s="50"/>
@@ -4002,17 +4005,22 @@
       <c r="H102" s="46"/>
       <c r="I102" s="46"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="B103" s="41"/>
       <c r="C103" s="50"/>
       <c r="D103" s="50"/>
+      <c r="E103" s="50"/>
+      <c r="F103" s="50"/>
+      <c r="G103" s="46"/>
+      <c r="H103" s="46"/>
+      <c r="I103" s="46"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B104" s="41"/>
       <c r="C104" s="50"/>
@@ -4020,7 +4028,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B105" s="41"/>
       <c r="C105" s="50"/>
@@ -4028,19 +4036,19 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="13" t="s">
-        <v>122</v>
+        <v>59</v>
       </c>
       <c r="B106" s="41"/>
       <c r="C106" s="50"/>
       <c r="D106" s="50"/>
-      <c r="E106" s="50"/>
-      <c r="F106" s="50"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B107" s="41"/>
+        <v>122</v>
+      </c>
+      <c r="B107" s="41" t="b">
+        <v>1</v>
+      </c>
       <c r="C107" s="50"/>
       <c r="D107" s="50"/>
       <c r="E107" s="50"/>
@@ -4048,7 +4056,7 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B108" s="41"/>
       <c r="C108" s="50"/>
@@ -4057,25 +4065,22 @@
       <c r="F108" s="50"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="55" t="s">
+      <c r="A109" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B109" s="41"/>
+      <c r="C109" s="50"/>
+      <c r="D109" s="50"/>
+      <c r="E109" s="50"/>
+      <c r="F109" s="50"/>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="B109" s="70"/>
-      <c r="C109" s="74"/>
-      <c r="D109" s="74"/>
-      <c r="E109" s="74"/>
-      <c r="F109" s="74"/>
-      <c r="G109"/>
-      <c r="H109"/>
-      <c r="I109"/>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="B110" s="56"/>
-      <c r="C110" s="73"/>
-      <c r="D110" s="73"/>
+      <c r="B110" s="70"/>
+      <c r="C110" s="74"/>
+      <c r="D110" s="74"/>
       <c r="E110" s="74"/>
       <c r="F110" s="74"/>
       <c r="G110"/>
@@ -4084,11 +4089,11 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="56" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B111" s="56"/>
-      <c r="C111" s="74"/>
-      <c r="D111" s="74"/>
+      <c r="C111" s="73"/>
+      <c r="D111" s="73"/>
       <c r="E111" s="74"/>
       <c r="F111" s="74"/>
       <c r="G111"/>
@@ -4097,7 +4102,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="56" t="s">
-        <v>142</v>
+        <v>95</v>
       </c>
       <c r="B112" s="56"/>
       <c r="C112" s="74"/>
@@ -4110,7 +4115,7 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="56" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="B113" s="56"/>
       <c r="C113" s="74"/>
@@ -4123,7 +4128,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="56" t="s">
-        <v>96</v>
+        <v>123</v>
       </c>
       <c r="B114" s="56"/>
       <c r="C114" s="74"/>
@@ -4136,11 +4141,11 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="56" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B115" s="56"/>
-      <c r="C115" s="73"/>
-      <c r="D115" s="73"/>
+      <c r="C115" s="74"/>
+      <c r="D115" s="74"/>
       <c r="E115" s="74"/>
       <c r="F115" s="74"/>
       <c r="G115"/>
@@ -4149,11 +4154,11 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="56" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B116" s="56"/>
-      <c r="C116" s="74"/>
-      <c r="D116" s="74"/>
+      <c r="C116" s="73"/>
+      <c r="D116" s="73"/>
       <c r="E116" s="74"/>
       <c r="F116" s="74"/>
       <c r="G116"/>
@@ -4162,7 +4167,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="56" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="B117" s="56"/>
       <c r="C117" s="74"/>
@@ -4175,7 +4180,7 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="56" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="B118" s="56"/>
       <c r="C118" s="74"/>
@@ -4188,7 +4193,7 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="56" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="B119" s="56"/>
       <c r="C119" s="74"/>
@@ -4200,10 +4205,10 @@
       <c r="I119"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="57" t="s">
-        <v>91</v>
-      </c>
-      <c r="B120" s="71"/>
+      <c r="A120" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="B120" s="56"/>
       <c r="C120" s="74"/>
       <c r="D120" s="74"/>
       <c r="E120" s="74"/>
@@ -4214,7 +4219,7 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="57" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B121" s="71"/>
       <c r="C121" s="74"/>
@@ -4227,7 +4232,7 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="57" t="s">
-        <v>144</v>
+        <v>99</v>
       </c>
       <c r="B122" s="71"/>
       <c r="C122" s="74"/>
@@ -4239,8 +4244,8 @@
       <c r="I122"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="56" t="s">
-        <v>125</v>
+      <c r="A123" s="57" t="s">
+        <v>144</v>
       </c>
       <c r="B123" s="71"/>
       <c r="C123" s="74"/>
@@ -4252,8 +4257,8 @@
       <c r="I123"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="57" t="s">
-        <v>100</v>
+      <c r="A124" s="56" t="s">
+        <v>125</v>
       </c>
       <c r="B124" s="71"/>
       <c r="C124" s="74"/>
@@ -4266,7 +4271,7 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="57" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="B125" s="71"/>
       <c r="C125" s="74"/>
@@ -4279,7 +4284,7 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="57" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B126" s="71"/>
       <c r="C126" s="74"/>
@@ -4292,7 +4297,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="57" t="s">
-        <v>145</v>
+        <v>101</v>
       </c>
       <c r="B127" s="71"/>
       <c r="C127" s="74"/>
@@ -4304,8 +4309,8 @@
       <c r="I127"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" s="56" t="s">
-        <v>126</v>
+      <c r="A128" s="57" t="s">
+        <v>145</v>
       </c>
       <c r="B128" s="71"/>
       <c r="C128" s="74"/>
@@ -4317,8 +4322,8 @@
       <c r="I128"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="57" t="s">
-        <v>102</v>
+      <c r="A129" s="56" t="s">
+        <v>126</v>
       </c>
       <c r="B129" s="71"/>
       <c r="C129" s="74"/>
@@ -4331,7 +4336,7 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="57" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B130" s="71"/>
       <c r="C130" s="74"/>
@@ -4344,12 +4349,12 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="57" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B131" s="71"/>
       <c r="C131" s="74"/>
       <c r="D131" s="74"/>
-      <c r="E131" s="75"/>
+      <c r="E131" s="74"/>
       <c r="F131" s="74"/>
       <c r="G131"/>
       <c r="H131"/>
@@ -4357,7 +4362,7 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="57" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="B132" s="71"/>
       <c r="C132" s="74"/>
@@ -4369,21 +4374,21 @@
       <c r="I132"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="56" t="s">
-        <v>127</v>
+      <c r="A133" s="57" t="s">
+        <v>146</v>
       </c>
       <c r="B133" s="71"/>
       <c r="C133" s="74"/>
       <c r="D133" s="74"/>
-      <c r="E133" s="74"/>
+      <c r="E133" s="75"/>
       <c r="F133" s="74"/>
       <c r="G133"/>
       <c r="H133"/>
       <c r="I133"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="57" t="s">
-        <v>104</v>
+      <c r="A134" s="56" t="s">
+        <v>127</v>
       </c>
       <c r="B134" s="71"/>
       <c r="C134" s="74"/>
@@ -4396,9 +4401,9 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="57" t="s">
-        <v>94</v>
-      </c>
-      <c r="B135" s="56"/>
+        <v>104</v>
+      </c>
+      <c r="B135" s="71"/>
       <c r="C135" s="74"/>
       <c r="D135" s="74"/>
       <c r="E135" s="74"/>
@@ -4409,7 +4414,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="57" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B136" s="56"/>
       <c r="C136" s="74"/>
@@ -4422,7 +4427,7 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="57" t="s">
-        <v>147</v>
+        <v>105</v>
       </c>
       <c r="B137" s="56"/>
       <c r="C137" s="74"/>
@@ -4434,8 +4439,8 @@
       <c r="I137"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="56" t="s">
-        <v>128</v>
+      <c r="A138" s="57" t="s">
+        <v>147</v>
       </c>
       <c r="B138" s="56"/>
       <c r="C138" s="74"/>
@@ -4447,8 +4452,8 @@
       <c r="I138"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A139" s="57" t="s">
-        <v>106</v>
+      <c r="A139" s="56" t="s">
+        <v>128</v>
       </c>
       <c r="B139" s="56"/>
       <c r="C139" s="74"/>
@@ -4461,7 +4466,7 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="57" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="B140" s="56"/>
       <c r="C140" s="74"/>
@@ -4474,7 +4479,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B141" s="56"/>
       <c r="C141" s="74"/>
@@ -4487,7 +4492,7 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="57" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="B142" s="56"/>
       <c r="C142" s="74"/>
@@ -4499,8 +4504,8 @@
       <c r="I142"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A143" s="56" t="s">
-        <v>137</v>
+      <c r="A143" s="57" t="s">
+        <v>148</v>
       </c>
       <c r="B143" s="56"/>
       <c r="C143" s="74"/>
@@ -4512,10 +4517,10 @@
       <c r="I143"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A144" s="58" t="s">
-        <v>136</v>
-      </c>
-      <c r="B144" s="72"/>
+      <c r="A144" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="B144" s="56"/>
       <c r="C144" s="74"/>
       <c r="D144" s="74"/>
       <c r="E144" s="74"/>
@@ -4524,45 +4529,58 @@
       <c r="H144"/>
       <c r="I144"/>
     </row>
-    <row r="145" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C145" s="50"/>
-      <c r="D145" s="50"/>
-      <c r="E145" s="50"/>
-      <c r="F145" s="50"/>
-    </row>
-    <row r="146" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="B145" s="72"/>
+      <c r="C145" s="74"/>
+      <c r="D145" s="74"/>
+      <c r="E145" s="74"/>
+      <c r="F145" s="74"/>
+      <c r="G145"/>
+      <c r="H145"/>
+      <c r="I145"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C146" s="50"/>
       <c r="D146" s="50"/>
       <c r="E146" s="50"/>
       <c r="F146" s="50"/>
     </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C147" s="50"/>
+      <c r="D147" s="50"/>
+      <c r="E147" s="50"/>
+      <c r="F147" s="50"/>
+    </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B88:D88 B73:D74">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89:D89 B74:D75">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B71:D72">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72:D73">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89:D89">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B90:D90">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B49:D70">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B50:D71">
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B91:D91">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B92:D92">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48:D48">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B49:D49">
       <formula1>0</formula1>
       <formula2>100</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B80:D84">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B81:D85">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -4576,13 +4594,13 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B93:D108 B75:D79 B85:D87</xm:sqref>
+          <xm:sqref>B94:D109 B76:D80 B86:D88</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B90:D90</xm:sqref>
+          <xm:sqref>B91:D91</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Fix start-up cost inclusion
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -386,24 +386,6 @@
     <t>output_plot_economics</t>
   </si>
   <si>
-    <t>econ_startingcost_duration_vaccination</t>
-  </si>
-  <si>
-    <t>econ_startingcost_duration_ipt</t>
-  </si>
-  <si>
-    <t>econ_startingcost_duration_xpert</t>
-  </si>
-  <si>
-    <t>econ_startingcost_duration_treatment_support</t>
-  </si>
-  <si>
-    <t>econ_startingcost_duration_smearacf</t>
-  </si>
-  <si>
-    <t>econ_startingcost_duration_xpertacf</t>
-  </si>
-  <si>
     <t>output_compartment_populations</t>
   </si>
   <si>
@@ -428,9 +410,6 @@
     <t>econ_saturation_decentralisation</t>
   </si>
   <si>
-    <t>econ_startingcost_duration_decentralisation</t>
-  </si>
-  <si>
     <t>cost_curve_start_time</t>
   </si>
   <si>
@@ -465,6 +444,27 @@
   </si>
   <si>
     <t>program_number_tests_per_tb_presentation</t>
+  </si>
+  <si>
+    <t>econ_startupduration_vaccination</t>
+  </si>
+  <si>
+    <t>econ_startupduration_ipt</t>
+  </si>
+  <si>
+    <t>econ_startupduration_xpert</t>
+  </si>
+  <si>
+    <t>econ_startupduration_treatment_support</t>
+  </si>
+  <si>
+    <t>econ_startupduration_smearacf</t>
+  </si>
+  <si>
+    <t>econ_startupduration_xpertacf</t>
+  </si>
+  <si>
+    <t>econ_startupduration_decentralisation</t>
   </si>
 </sst>
 </file>
@@ -2479,7 +2479,7 @@
   </sheetPr>
   <dimension ref="A1:BP147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
       <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
@@ -2902,7 +2902,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B41" s="63"/>
       <c r="C41" s="63"/>
@@ -2915,7 +2915,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B42" s="63"/>
       <c r="C42" s="63"/>
@@ -2928,7 +2928,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B43" s="63"/>
       <c r="C43" s="63"/>
@@ -2941,7 +2941,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="B44" s="63"/>
       <c r="C44" s="63"/>
@@ -2954,7 +2954,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B45" s="63"/>
       <c r="C45" s="63"/>
@@ -3083,7 +3083,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B59" s="29"/>
       <c r="C59" s="59"/>
@@ -3160,7 +3160,7 @@
     </row>
     <row r="66" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B66" s="65"/>
       <c r="C66" s="67"/>
@@ -3173,7 +3173,7 @@
     </row>
     <row r="67" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B67" s="65"/>
       <c r="C67" s="67"/>
@@ -3186,7 +3186,7 @@
     </row>
     <row r="68" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B68" s="65"/>
       <c r="C68" s="67"/>
@@ -3892,7 +3892,9 @@
       <c r="A92" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B92" s="43"/>
+      <c r="B92" s="43">
+        <v>12</v>
+      </c>
       <c r="C92" s="43"/>
       <c r="D92" s="43"/>
       <c r="E92" s="52"/>
@@ -3960,7 +3962,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B99" s="41"/>
       <c r="C99" s="50"/>
@@ -4115,7 +4117,7 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="56" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B113" s="56"/>
       <c r="C113" s="74"/>
@@ -4128,7 +4130,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="56" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="B114" s="56"/>
       <c r="C114" s="74"/>
@@ -4180,7 +4182,7 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="56" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B118" s="56"/>
       <c r="C118" s="74"/>
@@ -4193,7 +4195,7 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="56" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="B119" s="56"/>
       <c r="C119" s="74"/>
@@ -4245,7 +4247,7 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="57" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="B123" s="71"/>
       <c r="C123" s="74"/>
@@ -4258,7 +4260,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="56" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="B124" s="71"/>
       <c r="C124" s="74"/>
@@ -4310,7 +4312,7 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="57" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="B128" s="71"/>
       <c r="C128" s="74"/>
@@ -4323,7 +4325,7 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="56" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="B129" s="71"/>
       <c r="C129" s="74"/>
@@ -4375,7 +4377,7 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="57" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="B133" s="71"/>
       <c r="C133" s="74"/>
@@ -4388,7 +4390,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="56" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="B134" s="71"/>
       <c r="C134" s="74"/>
@@ -4440,7 +4442,7 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="57" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B138" s="56"/>
       <c r="C138" s="74"/>
@@ -4453,7 +4455,7 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="56" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="B139" s="56"/>
       <c r="C139" s="74"/>
@@ -4479,7 +4481,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="57" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="B141" s="56"/>
       <c r="C141" s="74"/>
@@ -4492,7 +4494,7 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="57" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="B142" s="56"/>
       <c r="C142" s="74"/>
@@ -4505,7 +4507,7 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="57" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="B143" s="56"/>
       <c r="C143" s="74"/>
@@ -4518,7 +4520,7 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="56" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="B144" s="56"/>
       <c r="C144" s="74"/>
@@ -4531,7 +4533,7 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="58" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B145" s="72"/>
       <c r="C145" s="74"/>

</xml_diff>

<commit_message>
Move Fiji-specific data into country sheet
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -2479,8 +2479,8 @@
   </sheetPr>
   <dimension ref="A1:BP147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2979,9 +2979,7 @@
       <c r="A47" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B47" s="25">
-        <v>25</v>
-      </c>
+      <c r="B47" s="25"/>
       <c r="C47" s="25"/>
       <c r="D47" s="25"/>
       <c r="E47" s="50"/>
@@ -3123,9 +3121,7 @@
       <c r="A63" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="B63" s="29">
-        <v>1865</v>
-      </c>
+      <c r="B63" s="29"/>
       <c r="C63" s="59"/>
       <c r="D63" s="59"/>
       <c r="E63" s="66"/>
@@ -3136,9 +3132,7 @@
       <c r="A64" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="B64" s="29">
-        <v>2036</v>
-      </c>
+      <c r="B64" s="29"/>
       <c r="C64" s="59"/>
       <c r="D64" s="59"/>
       <c r="E64" s="66"/>
@@ -3149,9 +3143,7 @@
       <c r="A65" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="B65" s="29">
-        <v>1</v>
-      </c>
+      <c r="B65" s="29"/>
       <c r="C65" s="59"/>
       <c r="D65" s="59"/>
       <c r="E65" s="66"/>
@@ -3511,9 +3503,7 @@
       <c r="A80" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B80" s="36" t="b">
-        <v>1</v>
-      </c>
+      <c r="B80" s="36"/>
       <c r="C80" s="59"/>
       <c r="D80" s="59"/>
       <c r="E80" s="46"/>
@@ -3637,9 +3627,7 @@
       <c r="A85" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="B85" s="38">
-        <v>0.156</v>
-      </c>
+      <c r="B85" s="38"/>
       <c r="C85" s="61"/>
       <c r="D85" s="61"/>
       <c r="E85" s="46"/>
@@ -3892,9 +3880,7 @@
       <c r="A92" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B92" s="43">
-        <v>12</v>
-      </c>
+      <c r="B92" s="43"/>
       <c r="C92" s="43"/>
       <c r="D92" s="43"/>
       <c r="E92" s="52"/>
@@ -4048,9 +4034,7 @@
       <c r="A107" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B107" s="41" t="b">
-        <v>1</v>
-      </c>
+      <c r="B107" s="41"/>
       <c r="C107" s="50"/>
       <c r="D107" s="50"/>
       <c r="E107" s="50"/>

</xml_diff>

<commit_message>
Add scenarios 12 and 13 for decentralization
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="615" windowWidth="20370" windowHeight="7230" tabRatio="807"/>
   </bookViews>
@@ -2230,7 +2235,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2265,7 +2270,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2479,8 +2484,8 @@
   </sheetPr>
   <dimension ref="A1:BP147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="B87" sqref="B87"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3504,7 +3509,7 @@
         <v>70</v>
       </c>
       <c r="B80" s="36" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C80" s="59"/>
       <c r="D80" s="59"/>
@@ -3894,9 +3899,15 @@
       <c r="A93" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B93" s="44"/>
-      <c r="C93" s="44"/>
-      <c r="D93" s="44"/>
+      <c r="B93" s="44">
+        <v>5</v>
+      </c>
+      <c r="C93" s="44">
+        <v>15</v>
+      </c>
+      <c r="D93" s="44">
+        <v>25</v>
+      </c>
       <c r="E93" s="44"/>
       <c r="F93" s="44"/>
       <c r="G93" s="44"/>
@@ -4030,7 +4041,9 @@
       <c r="A107" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B107" s="41"/>
+      <c r="B107" s="41" t="b">
+        <v>1</v>
+      </c>
       <c r="C107" s="50"/>
       <c r="D107" s="50"/>
       <c r="E107" s="50"/>

</xml_diff>

<commit_message>
Actually make GUI function for something
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntdoan\Github\AuTuMN\autumn\xls\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="615" windowWidth="20370" windowHeight="7230" tabRatio="807"/>
   </bookViews>
@@ -20,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="148">
   <si>
     <t>recent_time</t>
   </si>
@@ -371,12 +366,6 @@
   </si>
   <si>
     <t>comorb_startage_diabetes</t>
-  </si>
-  <si>
-    <t>output_uncertainty</t>
-  </si>
-  <si>
-    <t>output_uncertainty_all_scenarios</t>
   </si>
   <si>
     <t>plot_end_time</t>
@@ -2235,7 +2224,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2270,7 +2259,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2482,10 +2471,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP147"/>
+  <dimension ref="A1:BP145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2907,7 +2896,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B41" s="63"/>
       <c r="C41" s="63"/>
@@ -2920,7 +2909,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B42" s="63"/>
       <c r="C42" s="63"/>
@@ -2933,7 +2922,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B43" s="63"/>
       <c r="C43" s="63"/>
@@ -2946,7 +2935,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B44" s="63"/>
       <c r="C44" s="63"/>
@@ -2959,7 +2948,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B45" s="63"/>
       <c r="C45" s="63"/>
@@ -3086,7 +3075,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B59" s="29"/>
       <c r="C59" s="59"/>
@@ -3157,7 +3146,7 @@
     </row>
     <row r="66" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B66" s="65"/>
       <c r="C66" s="67"/>
@@ -3170,7 +3159,7 @@
     </row>
     <row r="67" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B67" s="65"/>
       <c r="C67" s="67"/>
@@ -3183,7 +3172,7 @@
     </row>
     <row r="68" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B68" s="65"/>
       <c r="C68" s="67"/>
@@ -3196,7 +3185,7 @@
     </row>
     <row r="69" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B69" s="29"/>
       <c r="C69" s="59"/>
@@ -3207,7 +3196,7 @@
     </row>
     <row r="70" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B70" s="29"/>
       <c r="C70" s="59"/>
@@ -3508,9 +3497,7 @@
       <c r="A80" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B80" s="36" t="b">
-        <v>1</v>
-      </c>
+      <c r="B80" s="36"/>
       <c r="C80" s="59"/>
       <c r="D80" s="59"/>
       <c r="E80" s="46"/>
@@ -3899,15 +3886,9 @@
       <c r="A93" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B93" s="44">
-        <v>5</v>
-      </c>
-      <c r="C93" s="44">
-        <v>15</v>
-      </c>
-      <c r="D93" s="44">
-        <v>25</v>
-      </c>
+      <c r="B93" s="44"/>
+      <c r="C93" s="44"/>
+      <c r="D93" s="44"/>
       <c r="E93" s="44"/>
       <c r="F93" s="44"/>
       <c r="G93" s="44"/>
@@ -3955,7 +3936,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B99" s="41"/>
       <c r="C99" s="50"/>
@@ -3989,7 +3970,7 @@
     </row>
     <row r="102" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B102" s="41"/>
       <c r="C102" s="50"/>
@@ -4039,41 +4020,45 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="B107" s="41" t="b">
-        <v>1</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="B107" s="41"/>
       <c r="C107" s="50"/>
       <c r="D107" s="50"/>
       <c r="E107" s="50"/>
       <c r="F107" s="50"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B108" s="41"/>
-      <c r="C108" s="50"/>
-      <c r="D108" s="50"/>
-      <c r="E108" s="50"/>
-      <c r="F108" s="50"/>
+      <c r="A108" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="B108" s="70"/>
+      <c r="C108" s="74"/>
+      <c r="D108" s="74"/>
+      <c r="E108" s="74"/>
+      <c r="F108" s="74"/>
+      <c r="G108"/>
+      <c r="H108"/>
+      <c r="I108"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="B109" s="41"/>
-      <c r="C109" s="50"/>
-      <c r="D109" s="50"/>
-      <c r="E109" s="50"/>
-      <c r="F109" s="50"/>
+      <c r="A109" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="B109" s="56"/>
+      <c r="C109" s="73"/>
+      <c r="D109" s="73"/>
+      <c r="E109" s="74"/>
+      <c r="F109" s="74"/>
+      <c r="G109"/>
+      <c r="H109"/>
+      <c r="I109"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B110" s="70"/>
+      <c r="A110" s="56" t="s">
+        <v>95</v>
+      </c>
+      <c r="B110" s="56"/>
       <c r="C110" s="74"/>
       <c r="D110" s="74"/>
       <c r="E110" s="74"/>
@@ -4084,11 +4069,11 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="56" t="s">
-        <v>89</v>
+        <v>133</v>
       </c>
       <c r="B111" s="56"/>
-      <c r="C111" s="73"/>
-      <c r="D111" s="73"/>
+      <c r="C111" s="74"/>
+      <c r="D111" s="74"/>
       <c r="E111" s="74"/>
       <c r="F111" s="74"/>
       <c r="G111"/>
@@ -4097,7 +4082,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="56" t="s">
-        <v>95</v>
+        <v>141</v>
       </c>
       <c r="B112" s="56"/>
       <c r="C112" s="74"/>
@@ -4110,7 +4095,7 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="56" t="s">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="B113" s="56"/>
       <c r="C113" s="74"/>
@@ -4123,11 +4108,11 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="56" t="s">
-        <v>143</v>
+        <v>90</v>
       </c>
       <c r="B114" s="56"/>
-      <c r="C114" s="74"/>
-      <c r="D114" s="74"/>
+      <c r="C114" s="73"/>
+      <c r="D114" s="73"/>
       <c r="E114" s="74"/>
       <c r="F114" s="74"/>
       <c r="G114"/>
@@ -4136,7 +4121,7 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="56" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B115" s="56"/>
       <c r="C115" s="74"/>
@@ -4149,11 +4134,11 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="56" t="s">
-        <v>90</v>
+        <v>134</v>
       </c>
       <c r="B116" s="56"/>
-      <c r="C116" s="73"/>
-      <c r="D116" s="73"/>
+      <c r="C116" s="74"/>
+      <c r="D116" s="74"/>
       <c r="E116" s="74"/>
       <c r="F116" s="74"/>
       <c r="G116"/>
@@ -4162,7 +4147,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="56" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="B117" s="56"/>
       <c r="C117" s="74"/>
@@ -4175,7 +4160,7 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="56" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="B118" s="56"/>
       <c r="C118" s="74"/>
@@ -4187,10 +4172,10 @@
       <c r="I118"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="B119" s="56"/>
+      <c r="A119" s="57" t="s">
+        <v>91</v>
+      </c>
+      <c r="B119" s="71"/>
       <c r="C119" s="74"/>
       <c r="D119" s="74"/>
       <c r="E119" s="74"/>
@@ -4200,10 +4185,10 @@
       <c r="I119"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="56" t="s">
-        <v>98</v>
-      </c>
-      <c r="B120" s="56"/>
+      <c r="A120" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B120" s="71"/>
       <c r="C120" s="74"/>
       <c r="D120" s="74"/>
       <c r="E120" s="74"/>
@@ -4214,7 +4199,7 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="57" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="B121" s="71"/>
       <c r="C121" s="74"/>
@@ -4226,8 +4211,8 @@
       <c r="I121"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="57" t="s">
-        <v>99</v>
+      <c r="A122" s="56" t="s">
+        <v>143</v>
       </c>
       <c r="B122" s="71"/>
       <c r="C122" s="74"/>
@@ -4240,7 +4225,7 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="57" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="B123" s="71"/>
       <c r="C123" s="74"/>
@@ -4252,8 +4237,8 @@
       <c r="I123"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="56" t="s">
-        <v>145</v>
+      <c r="A124" s="57" t="s">
+        <v>92</v>
       </c>
       <c r="B124" s="71"/>
       <c r="C124" s="74"/>
@@ -4266,7 +4251,7 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="57" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B125" s="71"/>
       <c r="C125" s="74"/>
@@ -4279,7 +4264,7 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="57" t="s">
-        <v>92</v>
+        <v>136</v>
       </c>
       <c r="B126" s="71"/>
       <c r="C126" s="74"/>
@@ -4291,8 +4276,8 @@
       <c r="I126"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A127" s="57" t="s">
-        <v>101</v>
+      <c r="A127" s="56" t="s">
+        <v>144</v>
       </c>
       <c r="B127" s="71"/>
       <c r="C127" s="74"/>
@@ -4305,7 +4290,7 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="57" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="B128" s="71"/>
       <c r="C128" s="74"/>
@@ -4317,8 +4302,8 @@
       <c r="I128"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="56" t="s">
-        <v>146</v>
+      <c r="A129" s="57" t="s">
+        <v>93</v>
       </c>
       <c r="B129" s="71"/>
       <c r="C129" s="74"/>
@@ -4331,12 +4316,12 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="57" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B130" s="71"/>
       <c r="C130" s="74"/>
       <c r="D130" s="74"/>
-      <c r="E130" s="74"/>
+      <c r="E130" s="75"/>
       <c r="F130" s="74"/>
       <c r="G130"/>
       <c r="H130"/>
@@ -4344,25 +4329,25 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="57" t="s">
-        <v>93</v>
+        <v>137</v>
       </c>
       <c r="B131" s="71"/>
       <c r="C131" s="74"/>
       <c r="D131" s="74"/>
-      <c r="E131" s="74"/>
+      <c r="E131" s="75"/>
       <c r="F131" s="74"/>
       <c r="G131"/>
       <c r="H131"/>
       <c r="I131"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="57" t="s">
-        <v>103</v>
+      <c r="A132" s="56" t="s">
+        <v>145</v>
       </c>
       <c r="B132" s="71"/>
       <c r="C132" s="74"/>
       <c r="D132" s="74"/>
-      <c r="E132" s="75"/>
+      <c r="E132" s="74"/>
       <c r="F132" s="74"/>
       <c r="G132"/>
       <c r="H132"/>
@@ -4370,22 +4355,22 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="57" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="B133" s="71"/>
       <c r="C133" s="74"/>
       <c r="D133" s="74"/>
-      <c r="E133" s="75"/>
+      <c r="E133" s="74"/>
       <c r="F133" s="74"/>
       <c r="G133"/>
       <c r="H133"/>
       <c r="I133"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="56" t="s">
-        <v>147</v>
-      </c>
-      <c r="B134" s="71"/>
+      <c r="A134" s="57" t="s">
+        <v>94</v>
+      </c>
+      <c r="B134" s="56"/>
       <c r="C134" s="74"/>
       <c r="D134" s="74"/>
       <c r="E134" s="74"/>
@@ -4396,9 +4381,9 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="57" t="s">
-        <v>104</v>
-      </c>
-      <c r="B135" s="71"/>
+        <v>105</v>
+      </c>
+      <c r="B135" s="56"/>
       <c r="C135" s="74"/>
       <c r="D135" s="74"/>
       <c r="E135" s="74"/>
@@ -4409,7 +4394,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="57" t="s">
-        <v>94</v>
+        <v>138</v>
       </c>
       <c r="B136" s="56"/>
       <c r="C136" s="74"/>
@@ -4421,8 +4406,8 @@
       <c r="I136"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A137" s="57" t="s">
-        <v>105</v>
+      <c r="A137" s="56" t="s">
+        <v>146</v>
       </c>
       <c r="B137" s="56"/>
       <c r="C137" s="74"/>
@@ -4435,7 +4420,7 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="57" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="B138" s="56"/>
       <c r="C138" s="74"/>
@@ -4447,8 +4432,8 @@
       <c r="I138"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A139" s="56" t="s">
-        <v>148</v>
+      <c r="A139" s="57" t="s">
+        <v>126</v>
       </c>
       <c r="B139" s="56"/>
       <c r="C139" s="74"/>
@@ -4461,7 +4446,7 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="57" t="s">
-        <v>106</v>
+        <v>127</v>
       </c>
       <c r="B140" s="56"/>
       <c r="C140" s="74"/>
@@ -4474,7 +4459,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="57" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="B141" s="56"/>
       <c r="C141" s="74"/>
@@ -4486,8 +4471,8 @@
       <c r="I141"/>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A142" s="57" t="s">
-        <v>129</v>
+      <c r="A142" s="56" t="s">
+        <v>147</v>
       </c>
       <c r="B142" s="56"/>
       <c r="C142" s="74"/>
@@ -4499,10 +4484,10 @@
       <c r="I142"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A143" s="57" t="s">
-        <v>141</v>
-      </c>
-      <c r="B143" s="56"/>
+      <c r="A143" s="58" t="s">
+        <v>128</v>
+      </c>
+      <c r="B143" s="72"/>
       <c r="C143" s="74"/>
       <c r="D143" s="74"/>
       <c r="E143" s="74"/>
@@ -4512,42 +4497,16 @@
       <c r="I143"/>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A144" s="56" t="s">
-        <v>149</v>
-      </c>
-      <c r="B144" s="56"/>
-      <c r="C144" s="74"/>
-      <c r="D144" s="74"/>
-      <c r="E144" s="74"/>
-      <c r="F144" s="74"/>
-      <c r="G144"/>
-      <c r="H144"/>
-      <c r="I144"/>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A145" s="58" t="s">
-        <v>130</v>
-      </c>
-      <c r="B145" s="72"/>
-      <c r="C145" s="74"/>
-      <c r="D145" s="74"/>
-      <c r="E145" s="74"/>
-      <c r="F145" s="74"/>
-      <c r="G145"/>
-      <c r="H145"/>
-      <c r="I145"/>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C146" s="50"/>
-      <c r="D146" s="50"/>
-      <c r="E146" s="50"/>
-      <c r="F146" s="50"/>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C147" s="50"/>
-      <c r="D147" s="50"/>
-      <c r="E147" s="50"/>
-      <c r="F147" s="50"/>
+      <c r="C144" s="50"/>
+      <c r="D144" s="50"/>
+      <c r="E144" s="50"/>
+      <c r="F144" s="50"/>
+    </row>
+    <row r="145" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C145" s="50"/>
+      <c r="D145" s="50"/>
+      <c r="E145" s="50"/>
+      <c r="F145" s="50"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
@@ -4589,7 +4548,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B94:D109 B76:D80 B86:D88</xm:sqref>
+          <xm:sqref>B94:D107 B76:D80 B86:D88</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Output documents to GUI
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
   <si>
     <t>recent_time</t>
   </si>
@@ -182,9 +182,6 @@
     <t>active</t>
   </si>
   <si>
-    <t>output_spreadsheets</t>
-  </si>
-  <si>
     <t>output_gtb_plots</t>
   </si>
   <si>
@@ -351,9 +348,6 @@
   </si>
   <si>
     <t>report_step_time</t>
-  </si>
-  <si>
-    <t>output_documents</t>
   </si>
   <si>
     <t>start_mdr_introduce_time</t>
@@ -1410,7 +1404,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1433,7 +1427,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1464,7 +1457,6 @@
     <xf numFmtId="165" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="12" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2471,437 +2463,437 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP145"/>
+  <dimension ref="A1:BP143"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A101" sqref="A101"/>
+      <selection activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="25.5703125" style="46" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="51" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="51" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="51" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="51" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="51"/>
+    <col min="2" max="4" width="25.5703125" style="44" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="49" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="49" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="49" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="49" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="49"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
+      <c r="B1" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
     </row>
     <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="46"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="44"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
     </row>
     <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
+        <v>64</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
     </row>
     <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
+        <v>65</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
     </row>
     <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
+        <v>66</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
     </row>
     <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
     </row>
     <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
+        <v>59</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="48"/>
     </row>
     <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
+        <v>60</v>
+      </c>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
     </row>
     <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="50"/>
+        <v>61</v>
+      </c>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
     </row>
     <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
     </row>
     <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="50"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
     </row>
     <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="50"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
     </row>
     <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
     </row>
     <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="50"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
     </row>
     <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="50"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="48"/>
+      <c r="F16" s="48"/>
     </row>
     <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="48"/>
     </row>
     <row r="18" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="50"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
     </row>
     <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="50"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
     </row>
     <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
     </row>
     <row r="21" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="50"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="48"/>
+      <c r="F21" s="48"/>
     </row>
     <row r="22" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="48"/>
+      <c r="F22" s="48"/>
     </row>
     <row r="23" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="48"/>
+      <c r="F23" s="48"/>
     </row>
     <row r="24" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="50"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="48"/>
+      <c r="F24" s="48"/>
     </row>
     <row r="25" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
     </row>
     <row r="26" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="50"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="48"/>
+      <c r="F26" s="48"/>
     </row>
     <row r="27" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="48"/>
+      <c r="F28" s="48"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="48"/>
+      <c r="F29" s="48"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="48"/>
+      <c r="F30" s="48"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
+        <v>62</v>
+      </c>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="50"/>
+        <v>63</v>
+      </c>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B33" s="25"/>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="48"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="24"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="24"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="48"/>
+      <c r="F35" s="48"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="48"/>
+      <c r="F36" s="48"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="48"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38" s="26"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50"/>
+        <v>79</v>
+      </c>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
+        <v>83</v>
+      </c>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="48"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B40" s="26"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="50"/>
+        <v>84</v>
+      </c>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="48"/>
+      <c r="F40" s="48"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B41" s="63"/>
-      <c r="C41" s="63"/>
-      <c r="D41" s="63"/>
-      <c r="E41" s="64"/>
+        <v>120</v>
+      </c>
+      <c r="B41" s="61"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="62"/>
       <c r="F41"/>
       <c r="G41"/>
       <c r="H41"/>
@@ -2909,12 +2901,12 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B42" s="63"/>
-      <c r="C42" s="63"/>
-      <c r="D42" s="63"/>
-      <c r="E42" s="64"/>
+        <v>121</v>
+      </c>
+      <c r="B42" s="61"/>
+      <c r="C42" s="61"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="62"/>
       <c r="F42"/>
       <c r="G42"/>
       <c r="H42"/>
@@ -2922,12 +2914,12 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B43" s="63"/>
-      <c r="C43" s="63"/>
-      <c r="D43" s="63"/>
-      <c r="E43" s="64"/>
+        <v>122</v>
+      </c>
+      <c r="B43" s="61"/>
+      <c r="C43" s="61"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="62"/>
       <c r="F43"/>
       <c r="G43"/>
       <c r="H43"/>
@@ -2935,12 +2927,12 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B44" s="63"/>
-      <c r="C44" s="63"/>
-      <c r="D44" s="63"/>
-      <c r="E44" s="64"/>
+        <v>138</v>
+      </c>
+      <c r="B44" s="61"/>
+      <c r="C44" s="61"/>
+      <c r="D44" s="61"/>
+      <c r="E44" s="62"/>
       <c r="F44"/>
       <c r="G44"/>
       <c r="H44"/>
@@ -2948,12 +2940,12 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B45" s="63"/>
-      <c r="C45" s="63"/>
-      <c r="D45" s="63"/>
-      <c r="E45" s="64"/>
+        <v>123</v>
+      </c>
+      <c r="B45" s="61"/>
+      <c r="C45" s="61"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="62"/>
       <c r="F45"/>
       <c r="G45"/>
       <c r="H45"/>
@@ -2963,293 +2955,293 @@
       <c r="A46" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="50"/>
-      <c r="F46" s="50"/>
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="48"/>
+      <c r="F46" s="48"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="50"/>
+        <v>114</v>
+      </c>
+      <c r="B47" s="24"/>
+      <c r="C47" s="24"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="48"/>
+      <c r="F47" s="48"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="50"/>
-      <c r="F48" s="50"/>
+        <v>85</v>
+      </c>
+      <c r="B48" s="26"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="48"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="28">
+      <c r="B49" s="27">
         <v>0.05</v>
       </c>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
-      <c r="E49" s="46"/>
-      <c r="F49" s="46"/>
+      <c r="C49" s="48"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="44"/>
+      <c r="F49" s="44"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B50" s="29"/>
-      <c r="C50" s="59"/>
-      <c r="D50" s="59"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="57"/>
+      <c r="D50" s="57"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B51" s="29"/>
-      <c r="C51" s="59"/>
-      <c r="D51" s="59"/>
+        <v>81</v>
+      </c>
+      <c r="B51" s="28"/>
+      <c r="C51" s="57"/>
+      <c r="D51" s="57"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B52" s="29"/>
-      <c r="C52" s="59"/>
-      <c r="D52" s="59"/>
+      <c r="B52" s="28"/>
+      <c r="C52" s="57"/>
+      <c r="D52" s="57"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="29"/>
-      <c r="C53" s="59"/>
-      <c r="D53" s="59"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="57"/>
+      <c r="D53" s="57"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B54" s="30"/>
-      <c r="C54" s="60"/>
-      <c r="D54" s="60"/>
+        <v>111</v>
+      </c>
+      <c r="B54" s="29"/>
+      <c r="C54" s="58"/>
+      <c r="D54" s="58"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="60"/>
-      <c r="D55" s="60"/>
+        <v>112</v>
+      </c>
+      <c r="B55" s="29"/>
+      <c r="C55" s="58"/>
+      <c r="D55" s="58"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>115</v>
-      </c>
-      <c r="B56" s="30"/>
-      <c r="C56" s="60"/>
-      <c r="D56" s="60"/>
+        <v>113</v>
+      </c>
+      <c r="B56" s="29"/>
+      <c r="C56" s="58"/>
+      <c r="D56" s="58"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="29"/>
-      <c r="C57" s="59"/>
-      <c r="D57" s="59"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="57"/>
+      <c r="D57" s="57"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B58" s="29"/>
-      <c r="C58" s="59"/>
-      <c r="D58" s="59"/>
+      <c r="B58" s="28"/>
+      <c r="C58" s="57"/>
+      <c r="D58" s="57"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B59" s="29"/>
-      <c r="C59" s="59"/>
-      <c r="D59" s="59"/>
+        <v>130</v>
+      </c>
+      <c r="B59" s="28"/>
+      <c r="C59" s="57"/>
+      <c r="D59" s="57"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B60" s="29"/>
-      <c r="C60" s="59"/>
-      <c r="D60" s="59"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="57"/>
+      <c r="D60" s="57"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B61" s="29"/>
-      <c r="C61" s="59"/>
-      <c r="D61" s="59"/>
-      <c r="E61" s="66"/>
-      <c r="F61" s="66"/>
-      <c r="G61" s="66"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="57"/>
+      <c r="D61" s="57"/>
+      <c r="E61" s="64"/>
+      <c r="F61" s="64"/>
+      <c r="G61" s="64"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B62" s="29"/>
-      <c r="C62" s="59"/>
-      <c r="D62" s="59"/>
-      <c r="E62" s="66"/>
-      <c r="F62" s="66"/>
-      <c r="G62" s="66"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="57"/>
+      <c r="D62" s="57"/>
+      <c r="E62" s="64"/>
+      <c r="F62" s="64"/>
+      <c r="G62" s="64"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B63" s="29"/>
-      <c r="C63" s="59"/>
-      <c r="D63" s="59"/>
-      <c r="E63" s="66"/>
-      <c r="F63" s="66"/>
-      <c r="G63" s="66"/>
+        <v>108</v>
+      </c>
+      <c r="B63" s="28"/>
+      <c r="C63" s="57"/>
+      <c r="D63" s="57"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="64"/>
+      <c r="G63" s="64"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B64" s="29"/>
-      <c r="C64" s="59"/>
-      <c r="D64" s="59"/>
-      <c r="E64" s="66"/>
-      <c r="F64" s="66"/>
-      <c r="G64" s="66"/>
+        <v>109</v>
+      </c>
+      <c r="B64" s="28"/>
+      <c r="C64" s="57"/>
+      <c r="D64" s="57"/>
+      <c r="E64" s="64"/>
+      <c r="F64" s="64"/>
+      <c r="G64" s="64"/>
     </row>
     <row r="65" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B65" s="29"/>
-      <c r="C65" s="59"/>
-      <c r="D65" s="59"/>
-      <c r="E65" s="66"/>
-      <c r="F65" s="66"/>
-      <c r="G65" s="66"/>
+        <v>110</v>
+      </c>
+      <c r="B65" s="28"/>
+      <c r="C65" s="57"/>
+      <c r="D65" s="57"/>
+      <c r="E65" s="64"/>
+      <c r="F65" s="64"/>
+      <c r="G65" s="64"/>
     </row>
     <row r="66" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B66" s="65"/>
-      <c r="C66" s="67"/>
-      <c r="D66" s="67"/>
-      <c r="E66" s="68"/>
-      <c r="F66" s="69"/>
-      <c r="G66" s="69"/>
+        <v>127</v>
+      </c>
+      <c r="B66" s="63"/>
+      <c r="C66" s="65"/>
+      <c r="D66" s="65"/>
+      <c r="E66" s="66"/>
+      <c r="F66" s="67"/>
+      <c r="G66" s="67"/>
       <c r="H66"/>
       <c r="I66"/>
     </row>
     <row r="67" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B67" s="65"/>
-      <c r="C67" s="67"/>
-      <c r="D67" s="67"/>
-      <c r="E67" s="68"/>
-      <c r="F67" s="69"/>
-      <c r="G67" s="69"/>
+        <v>128</v>
+      </c>
+      <c r="B67" s="63"/>
+      <c r="C67" s="65"/>
+      <c r="D67" s="65"/>
+      <c r="E67" s="66"/>
+      <c r="F67" s="67"/>
+      <c r="G67" s="67"/>
       <c r="H67"/>
       <c r="I67"/>
     </row>
     <row r="68" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B68" s="65"/>
-      <c r="C68" s="67"/>
-      <c r="D68" s="67"/>
-      <c r="E68" s="68"/>
-      <c r="F68" s="69"/>
-      <c r="G68" s="69"/>
+        <v>129</v>
+      </c>
+      <c r="B68" s="63"/>
+      <c r="C68" s="65"/>
+      <c r="D68" s="65"/>
+      <c r="E68" s="66"/>
+      <c r="F68" s="67"/>
+      <c r="G68" s="67"/>
       <c r="H68"/>
       <c r="I68"/>
     </row>
     <row r="69" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="B69" s="29"/>
-      <c r="C69" s="59"/>
-      <c r="D69" s="59"/>
-      <c r="E69" s="66"/>
-      <c r="F69" s="66"/>
-      <c r="G69" s="66"/>
+        <v>116</v>
+      </c>
+      <c r="B69" s="28"/>
+      <c r="C69" s="57"/>
+      <c r="D69" s="57"/>
+      <c r="E69" s="64"/>
+      <c r="F69" s="64"/>
+      <c r="G69" s="64"/>
     </row>
     <row r="70" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B70" s="29"/>
-      <c r="C70" s="59"/>
-      <c r="D70" s="59"/>
-      <c r="E70" s="66"/>
-      <c r="F70" s="66"/>
-      <c r="G70" s="66"/>
+        <v>115</v>
+      </c>
+      <c r="B70" s="28"/>
+      <c r="C70" s="57"/>
+      <c r="D70" s="57"/>
+      <c r="E70" s="64"/>
+      <c r="F70" s="64"/>
+      <c r="G70" s="64"/>
     </row>
     <row r="71" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B71" s="31"/>
-      <c r="C71" s="59"/>
-      <c r="D71" s="59"/>
-      <c r="E71" s="66"/>
-      <c r="F71" s="66"/>
-      <c r="G71" s="66"/>
+        <v>86</v>
+      </c>
+      <c r="B71" s="30"/>
+      <c r="C71" s="57"/>
+      <c r="D71" s="57"/>
+      <c r="E71" s="64"/>
+      <c r="F71" s="64"/>
+      <c r="G71" s="64"/>
     </row>
     <row r="72" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B72" s="32"/>
-      <c r="C72" s="59"/>
-      <c r="D72" s="59"/>
-      <c r="E72" s="66"/>
-      <c r="F72" s="66"/>
-      <c r="G72" s="66"/>
+      <c r="B72" s="31"/>
+      <c r="C72" s="57"/>
+      <c r="D72" s="57"/>
+      <c r="E72" s="64"/>
+      <c r="F72" s="64"/>
+      <c r="G72" s="64"/>
     </row>
     <row r="73" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B73" s="33"/>
-      <c r="C73" s="59"/>
-      <c r="D73" s="59"/>
-      <c r="E73" s="66"/>
-      <c r="F73" s="66"/>
-      <c r="G73" s="66"/>
+      <c r="B73" s="32"/>
+      <c r="C73" s="57"/>
+      <c r="D73" s="57"/>
+      <c r="E73" s="64"/>
+      <c r="F73" s="64"/>
+      <c r="G73" s="64"/>
     </row>
     <row r="74" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B74" s="34"/>
-      <c r="C74" s="59"/>
-      <c r="D74" s="59"/>
-      <c r="E74" s="50"/>
-      <c r="F74" s="50"/>
-      <c r="G74" s="50"/>
-      <c r="H74" s="46"/>
-      <c r="I74" s="46"/>
+      <c r="B74" s="33"/>
+      <c r="C74" s="57"/>
+      <c r="D74" s="57"/>
+      <c r="E74" s="48"/>
+      <c r="F74" s="48"/>
+      <c r="G74" s="48"/>
+      <c r="H74" s="44"/>
+      <c r="I74" s="44"/>
       <c r="J74" s="15"/>
       <c r="K74" s="15"/>
       <c r="L74" s="15"/>
@@ -3314,14 +3306,14 @@
       <c r="A75" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B75" s="34"/>
-      <c r="C75" s="59"/>
-      <c r="D75" s="59"/>
-      <c r="E75" s="50"/>
-      <c r="F75" s="50"/>
-      <c r="G75" s="50"/>
-      <c r="H75" s="46"/>
-      <c r="I75" s="46"/>
+      <c r="B75" s="33"/>
+      <c r="C75" s="57"/>
+      <c r="D75" s="57"/>
+      <c r="E75" s="48"/>
+      <c r="F75" s="48"/>
+      <c r="G75" s="48"/>
+      <c r="H75" s="44"/>
+      <c r="I75" s="44"/>
       <c r="J75" s="15"/>
       <c r="K75" s="15"/>
       <c r="L75" s="15"/>
@@ -3382,18 +3374,18 @@
       <c r="BO75" s="15"/>
       <c r="BP75" s="15"/>
     </row>
-    <row r="76" spans="1:68" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B76" s="35"/>
-      <c r="C76" s="59"/>
-      <c r="D76" s="59"/>
-      <c r="E76" s="50"/>
-      <c r="F76" s="50"/>
-      <c r="G76" s="50"/>
-      <c r="H76" s="46"/>
-      <c r="I76" s="46"/>
+    <row r="76" spans="1:68" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B76" s="34"/>
+      <c r="C76" s="57"/>
+      <c r="D76" s="57"/>
+      <c r="E76" s="48"/>
+      <c r="F76" s="48"/>
+      <c r="G76" s="48"/>
+      <c r="H76" s="44"/>
+      <c r="I76" s="44"/>
       <c r="J76" s="15"/>
       <c r="K76" s="15"/>
       <c r="L76" s="15"/>
@@ -3456,55 +3448,55 @@
     </row>
     <row r="77" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B77" s="34"/>
-      <c r="C77" s="59"/>
-      <c r="D77" s="59"/>
-      <c r="E77" s="46"/>
-      <c r="F77" s="46"/>
-      <c r="G77" s="46"/>
-      <c r="H77" s="46"/>
-      <c r="I77" s="46"/>
+        <v>73</v>
+      </c>
+      <c r="B77" s="33"/>
+      <c r="C77" s="57"/>
+      <c r="D77" s="57"/>
+      <c r="E77" s="44"/>
+      <c r="F77" s="44"/>
+      <c r="G77" s="44"/>
+      <c r="H77" s="44"/>
+      <c r="I77" s="44"/>
     </row>
     <row r="78" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B78" s="34"/>
-      <c r="C78" s="59"/>
-      <c r="D78" s="59"/>
-      <c r="E78" s="46"/>
-      <c r="F78" s="46"/>
-      <c r="G78" s="46"/>
-      <c r="H78" s="46"/>
-      <c r="I78" s="46"/>
+        <v>72</v>
+      </c>
+      <c r="B78" s="33"/>
+      <c r="C78" s="57"/>
+      <c r="D78" s="57"/>
+      <c r="E78" s="44"/>
+      <c r="F78" s="44"/>
+      <c r="G78" s="44"/>
+      <c r="H78" s="44"/>
+      <c r="I78" s="44"/>
     </row>
     <row r="79" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B79" s="34"/>
-      <c r="C79" s="59"/>
-      <c r="D79" s="59"/>
-      <c r="E79" s="46"/>
-      <c r="F79" s="46"/>
-      <c r="G79" s="46"/>
-      <c r="H79" s="46"/>
-      <c r="I79" s="46"/>
-    </row>
-    <row r="80" spans="1:68" s="20" customFormat="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="B79" s="33"/>
+      <c r="C79" s="57"/>
+      <c r="D79" s="57"/>
+      <c r="E79" s="44"/>
+      <c r="F79" s="44"/>
+      <c r="G79" s="44"/>
+      <c r="H79" s="44"/>
+      <c r="I79" s="44"/>
+    </row>
+    <row r="80" spans="1:68" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B80" s="36"/>
-      <c r="C80" s="59"/>
-      <c r="D80" s="59"/>
-      <c r="E80" s="46"/>
-      <c r="F80" s="46"/>
-      <c r="G80" s="46"/>
-      <c r="H80" s="46"/>
-      <c r="I80" s="46"/>
+        <v>69</v>
+      </c>
+      <c r="B80" s="35"/>
+      <c r="C80" s="57"/>
+      <c r="D80" s="57"/>
+      <c r="E80" s="44"/>
+      <c r="F80" s="44"/>
+      <c r="G80" s="44"/>
+      <c r="H80" s="44"/>
+      <c r="I80" s="44"/>
       <c r="J80" s="15"/>
       <c r="K80" s="15"/>
       <c r="L80" s="15"/>
@@ -3567,81 +3559,81 @@
     </row>
     <row r="81" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B81" s="37"/>
-      <c r="C81" s="61"/>
-      <c r="D81" s="61"/>
-      <c r="E81" s="46"/>
-      <c r="F81" s="46"/>
-      <c r="G81" s="46"/>
-      <c r="H81" s="46"/>
-      <c r="I81" s="46"/>
+        <v>74</v>
+      </c>
+      <c r="B81" s="36"/>
+      <c r="C81" s="59"/>
+      <c r="D81" s="59"/>
+      <c r="E81" s="44"/>
+      <c r="F81" s="44"/>
+      <c r="G81" s="44"/>
+      <c r="H81" s="44"/>
+      <c r="I81" s="44"/>
     </row>
     <row r="82" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B82" s="37"/>
-      <c r="C82" s="61"/>
-      <c r="D82" s="61"/>
-      <c r="E82" s="46"/>
-      <c r="F82" s="46"/>
-      <c r="G82" s="46"/>
-      <c r="H82" s="46"/>
-      <c r="I82" s="46"/>
+        <v>75</v>
+      </c>
+      <c r="B82" s="36"/>
+      <c r="C82" s="59"/>
+      <c r="D82" s="59"/>
+      <c r="E82" s="44"/>
+      <c r="F82" s="44"/>
+      <c r="G82" s="44"/>
+      <c r="H82" s="44"/>
+      <c r="I82" s="44"/>
     </row>
     <row r="83" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B83" s="37"/>
-      <c r="C83" s="61"/>
-      <c r="D83" s="61"/>
-      <c r="E83" s="46"/>
-      <c r="F83" s="46"/>
-      <c r="G83" s="46"/>
-      <c r="H83" s="46"/>
-      <c r="I83" s="46"/>
+        <v>76</v>
+      </c>
+      <c r="B83" s="36"/>
+      <c r="C83" s="59"/>
+      <c r="D83" s="59"/>
+      <c r="E83" s="44"/>
+      <c r="F83" s="44"/>
+      <c r="G83" s="44"/>
+      <c r="H83" s="44"/>
+      <c r="I83" s="44"/>
     </row>
     <row r="84" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B84" s="37"/>
-      <c r="C84" s="61"/>
-      <c r="D84" s="61"/>
-      <c r="E84" s="46"/>
-      <c r="F84" s="46"/>
-      <c r="G84" s="46"/>
-      <c r="H84" s="46"/>
-      <c r="I84" s="46"/>
+        <v>77</v>
+      </c>
+      <c r="B84" s="36"/>
+      <c r="C84" s="59"/>
+      <c r="D84" s="59"/>
+      <c r="E84" s="44"/>
+      <c r="F84" s="44"/>
+      <c r="G84" s="44"/>
+      <c r="H84" s="44"/>
+      <c r="I84" s="44"/>
     </row>
     <row r="85" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B85" s="38"/>
-      <c r="C85" s="61"/>
-      <c r="D85" s="61"/>
-      <c r="E85" s="46"/>
-      <c r="F85" s="46"/>
-      <c r="G85" s="46"/>
-      <c r="H85" s="46"/>
-      <c r="I85" s="46"/>
+        <v>78</v>
+      </c>
+      <c r="B85" s="37"/>
+      <c r="C85" s="59"/>
+      <c r="D85" s="59"/>
+      <c r="E85" s="44"/>
+      <c r="F85" s="44"/>
+      <c r="G85" s="44"/>
+      <c r="H85" s="44"/>
+      <c r="I85" s="44"/>
     </row>
     <row r="86" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B86" s="39"/>
-      <c r="C86" s="50"/>
-      <c r="D86" s="50"/>
-      <c r="E86" s="46"/>
-      <c r="F86" s="46"/>
-      <c r="G86" s="46"/>
-      <c r="H86" s="46"/>
-      <c r="I86" s="46"/>
+      <c r="B86" s="38"/>
+      <c r="C86" s="48"/>
+      <c r="D86" s="48"/>
+      <c r="E86" s="44"/>
+      <c r="F86" s="44"/>
+      <c r="G86" s="44"/>
+      <c r="H86" s="44"/>
+      <c r="I86" s="44"/>
       <c r="J86" s="15"/>
       <c r="K86" s="15"/>
       <c r="L86" s="15"/>
@@ -3706,14 +3698,14 @@
       <c r="A87" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B87" s="39"/>
-      <c r="C87" s="50"/>
-      <c r="D87" s="50"/>
-      <c r="E87" s="46"/>
-      <c r="F87" s="46"/>
-      <c r="G87" s="46"/>
-      <c r="H87" s="46"/>
-      <c r="I87" s="46"/>
+      <c r="B87" s="38"/>
+      <c r="C87" s="48"/>
+      <c r="D87" s="48"/>
+      <c r="E87" s="44"/>
+      <c r="F87" s="44"/>
+      <c r="G87" s="44"/>
+      <c r="H87" s="44"/>
+      <c r="I87" s="44"/>
       <c r="J87" s="15"/>
       <c r="K87" s="15"/>
       <c r="L87" s="15"/>
@@ -3778,14 +3770,14 @@
       <c r="A88" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B88" s="40"/>
-      <c r="C88" s="50"/>
-      <c r="D88" s="50"/>
-      <c r="E88" s="46"/>
-      <c r="F88" s="46"/>
-      <c r="G88" s="46"/>
-      <c r="H88" s="46"/>
-      <c r="I88" s="46"/>
+      <c r="B88" s="39"/>
+      <c r="C88" s="48"/>
+      <c r="D88" s="48"/>
+      <c r="E88" s="44"/>
+      <c r="F88" s="44"/>
+      <c r="G88" s="44"/>
+      <c r="H88" s="44"/>
+      <c r="I88" s="44"/>
       <c r="J88" s="15"/>
       <c r="K88" s="15"/>
       <c r="L88" s="15"/>
@@ -3850,663 +3842,647 @@
       <c r="A89" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B89" s="41"/>
-      <c r="C89" s="50"/>
-      <c r="D89" s="50"/>
+      <c r="B89" s="40"/>
+      <c r="C89" s="48"/>
+      <c r="D89" s="48"/>
     </row>
     <row r="90" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B90" s="42"/>
-      <c r="C90" s="62"/>
-      <c r="D90" s="62"/>
+      <c r="B90" s="41"/>
+      <c r="C90" s="60"/>
+      <c r="D90" s="60"/>
     </row>
     <row r="91" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A91" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B91" s="41"/>
-      <c r="C91" s="50"/>
-      <c r="D91" s="50"/>
+      <c r="B91" s="40"/>
+      <c r="C91" s="48"/>
+      <c r="D91" s="48"/>
     </row>
     <row r="92" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B92" s="43"/>
-      <c r="C92" s="43"/>
-      <c r="D92" s="43"/>
-      <c r="E92" s="52"/>
-      <c r="F92" s="52"/>
-      <c r="G92" s="52"/>
-      <c r="H92" s="53"/>
+      <c r="B92" s="42"/>
+      <c r="C92" s="42"/>
+      <c r="D92" s="42"/>
+      <c r="E92" s="50"/>
+      <c r="F92" s="50"/>
+      <c r="G92" s="50"/>
+      <c r="H92" s="51"/>
     </row>
     <row r="93" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A93" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B93" s="44"/>
-      <c r="C93" s="44"/>
-      <c r="D93" s="44"/>
-      <c r="E93" s="44"/>
-      <c r="F93" s="44"/>
-      <c r="G93" s="44"/>
-      <c r="H93" s="54"/>
+      <c r="B93" s="43"/>
+      <c r="C93" s="43"/>
+      <c r="D93" s="43"/>
+      <c r="E93" s="43"/>
+      <c r="F93" s="43"/>
+      <c r="G93" s="43"/>
+      <c r="H93" s="52"/>
     </row>
     <row r="94" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A94" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="B94" s="45"/>
-      <c r="C94" s="50"/>
-      <c r="D94" s="50"/>
+      <c r="A94" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="B94" s="40"/>
+      <c r="C94" s="48"/>
+      <c r="D94" s="48"/>
     </row>
     <row r="95" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B95" s="41"/>
-      <c r="C95" s="50"/>
-      <c r="D95" s="50"/>
+        <v>107</v>
+      </c>
+      <c r="B95" s="40"/>
+      <c r="C95" s="48"/>
+      <c r="D95" s="48"/>
     </row>
     <row r="96" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="B96" s="41"/>
-      <c r="C96" s="50"/>
-      <c r="D96" s="50"/>
+        <v>55</v>
+      </c>
+      <c r="B96" s="40"/>
+      <c r="C96" s="48"/>
+      <c r="D96" s="48"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B97" s="41"/>
-      <c r="C97" s="50"/>
-      <c r="D97" s="50"/>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="B97" s="40"/>
+      <c r="C97" s="48"/>
+      <c r="D97" s="48"/>
+    </row>
+    <row r="98" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B98" s="41"/>
-      <c r="C98" s="50"/>
-      <c r="D98" s="50"/>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="B98" s="40"/>
+      <c r="C98" s="48"/>
+      <c r="D98" s="48"/>
+      <c r="E98" s="48"/>
+      <c r="F98" s="48"/>
+      <c r="G98" s="44"/>
+      <c r="H98" s="44"/>
+      <c r="I98" s="44"/>
+    </row>
+    <row r="99" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="B99" s="41"/>
-      <c r="C99" s="50"/>
-      <c r="D99" s="50"/>
+        <v>68</v>
+      </c>
+      <c r="B99" s="40"/>
+      <c r="C99" s="48"/>
+      <c r="D99" s="48"/>
+      <c r="E99" s="48"/>
+      <c r="F99" s="48"/>
+      <c r="G99" s="44"/>
+      <c r="H99" s="44"/>
+      <c r="I99" s="44"/>
     </row>
     <row r="100" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B100" s="41"/>
-      <c r="C100" s="50"/>
-      <c r="D100" s="50"/>
-      <c r="E100" s="50"/>
-      <c r="F100" s="50"/>
-      <c r="G100" s="46"/>
-      <c r="H100" s="46"/>
-      <c r="I100" s="46"/>
+        <v>117</v>
+      </c>
+      <c r="B100" s="40"/>
+      <c r="C100" s="48"/>
+      <c r="D100" s="48"/>
+      <c r="E100" s="48"/>
+      <c r="F100" s="48"/>
+      <c r="G100" s="44"/>
+      <c r="H100" s="44"/>
+      <c r="I100" s="44"/>
     </row>
     <row r="101" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B101" s="41"/>
-      <c r="C101" s="50"/>
-      <c r="D101" s="50"/>
-      <c r="E101" s="50"/>
-      <c r="F101" s="50"/>
-      <c r="G101" s="46"/>
-      <c r="H101" s="46"/>
-      <c r="I101" s="46"/>
-    </row>
-    <row r="102" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="B101" s="40"/>
+      <c r="C101" s="48"/>
+      <c r="D101" s="48"/>
+      <c r="E101" s="48"/>
+      <c r="F101" s="48"/>
+      <c r="G101" s="44"/>
+      <c r="H101" s="44"/>
+      <c r="I101" s="44"/>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="B102" s="41"/>
-      <c r="C102" s="50"/>
-      <c r="D102" s="50"/>
-      <c r="E102" s="50"/>
-      <c r="F102" s="50"/>
-      <c r="G102" s="46"/>
-      <c r="H102" s="46"/>
-      <c r="I102" s="46"/>
-    </row>
-    <row r="103" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="B102" s="40"/>
+      <c r="C102" s="48"/>
+      <c r="D102" s="48"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B103" s="41"/>
-      <c r="C103" s="50"/>
-      <c r="D103" s="50"/>
-      <c r="E103" s="50"/>
-      <c r="F103" s="50"/>
-      <c r="G103" s="46"/>
-      <c r="H103" s="46"/>
-      <c r="I103" s="46"/>
+        <v>57</v>
+      </c>
+      <c r="B103" s="40"/>
+      <c r="C103" s="48"/>
+      <c r="D103" s="48"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B104" s="41"/>
-      <c r="C104" s="50"/>
-      <c r="D104" s="50"/>
+        <v>58</v>
+      </c>
+      <c r="B104" s="40"/>
+      <c r="C104" s="48"/>
+      <c r="D104" s="48"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B105" s="41"/>
-      <c r="C105" s="50"/>
-      <c r="D105" s="50"/>
+        <v>118</v>
+      </c>
+      <c r="B105" s="40"/>
+      <c r="C105" s="48"/>
+      <c r="D105" s="48"/>
+      <c r="E105" s="48"/>
+      <c r="F105" s="48"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B106" s="41"/>
-      <c r="C106" s="50"/>
-      <c r="D106" s="50"/>
+      <c r="A106" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="B106" s="68"/>
+      <c r="C106" s="72"/>
+      <c r="D106" s="72"/>
+      <c r="E106" s="72"/>
+      <c r="F106" s="72"/>
+      <c r="G106"/>
+      <c r="H106"/>
+      <c r="I106"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B107" s="41"/>
-      <c r="C107" s="50"/>
-      <c r="D107" s="50"/>
-      <c r="E107" s="50"/>
-      <c r="F107" s="50"/>
+      <c r="A107" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="B107" s="54"/>
+      <c r="C107" s="71"/>
+      <c r="D107" s="71"/>
+      <c r="E107" s="72"/>
+      <c r="F107" s="72"/>
+      <c r="G107"/>
+      <c r="H107"/>
+      <c r="I107"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="55" t="s">
-        <v>88</v>
-      </c>
-      <c r="B108" s="70"/>
-      <c r="C108" s="74"/>
-      <c r="D108" s="74"/>
-      <c r="E108" s="74"/>
-      <c r="F108" s="74"/>
+      <c r="A108" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="B108" s="54"/>
+      <c r="C108" s="72"/>
+      <c r="D108" s="72"/>
+      <c r="E108" s="72"/>
+      <c r="F108" s="72"/>
       <c r="G108"/>
       <c r="H108"/>
       <c r="I108"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="B109" s="56"/>
-      <c r="C109" s="73"/>
-      <c r="D109" s="73"/>
-      <c r="E109" s="74"/>
-      <c r="F109" s="74"/>
+      <c r="A109" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="B109" s="54"/>
+      <c r="C109" s="72"/>
+      <c r="D109" s="72"/>
+      <c r="E109" s="72"/>
+      <c r="F109" s="72"/>
       <c r="G109"/>
       <c r="H109"/>
       <c r="I109"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="56" t="s">
-        <v>95</v>
-      </c>
-      <c r="B110" s="56"/>
-      <c r="C110" s="74"/>
-      <c r="D110" s="74"/>
-      <c r="E110" s="74"/>
-      <c r="F110" s="74"/>
+      <c r="A110" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="B110" s="54"/>
+      <c r="C110" s="72"/>
+      <c r="D110" s="72"/>
+      <c r="E110" s="72"/>
+      <c r="F110" s="72"/>
       <c r="G110"/>
       <c r="H110"/>
       <c r="I110"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="56" t="s">
-        <v>133</v>
-      </c>
-      <c r="B111" s="56"/>
-      <c r="C111" s="74"/>
-      <c r="D111" s="74"/>
-      <c r="E111" s="74"/>
-      <c r="F111" s="74"/>
+      <c r="A111" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="B111" s="54"/>
+      <c r="C111" s="72"/>
+      <c r="D111" s="72"/>
+      <c r="E111" s="72"/>
+      <c r="F111" s="72"/>
       <c r="G111"/>
       <c r="H111"/>
       <c r="I111"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="56" t="s">
-        <v>141</v>
-      </c>
-      <c r="B112" s="56"/>
-      <c r="C112" s="74"/>
-      <c r="D112" s="74"/>
-      <c r="E112" s="74"/>
-      <c r="F112" s="74"/>
+      <c r="A112" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="B112" s="54"/>
+      <c r="C112" s="71"/>
+      <c r="D112" s="71"/>
+      <c r="E112" s="72"/>
+      <c r="F112" s="72"/>
       <c r="G112"/>
       <c r="H112"/>
       <c r="I112"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="56" t="s">
+      <c r="A113" s="54" t="s">
         <v>96</v>
       </c>
-      <c r="B113" s="56"/>
-      <c r="C113" s="74"/>
-      <c r="D113" s="74"/>
-      <c r="E113" s="74"/>
-      <c r="F113" s="74"/>
+      <c r="B113" s="54"/>
+      <c r="C113" s="72"/>
+      <c r="D113" s="72"/>
+      <c r="E113" s="72"/>
+      <c r="F113" s="72"/>
       <c r="G113"/>
       <c r="H113"/>
       <c r="I113"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="B114" s="56"/>
-      <c r="C114" s="73"/>
-      <c r="D114" s="73"/>
-      <c r="E114" s="74"/>
-      <c r="F114" s="74"/>
+      <c r="A114" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="B114" s="54"/>
+      <c r="C114" s="72"/>
+      <c r="D114" s="72"/>
+      <c r="E114" s="72"/>
+      <c r="F114" s="72"/>
       <c r="G114"/>
       <c r="H114"/>
       <c r="I114"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="56" t="s">
-        <v>97</v>
-      </c>
-      <c r="B115" s="56"/>
-      <c r="C115" s="74"/>
-      <c r="D115" s="74"/>
-      <c r="E115" s="74"/>
-      <c r="F115" s="74"/>
+      <c r="A115" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="B115" s="54"/>
+      <c r="C115" s="72"/>
+      <c r="D115" s="72"/>
+      <c r="E115" s="72"/>
+      <c r="F115" s="72"/>
       <c r="G115"/>
       <c r="H115"/>
       <c r="I115"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="56" t="s">
-        <v>134</v>
-      </c>
-      <c r="B116" s="56"/>
-      <c r="C116" s="74"/>
-      <c r="D116" s="74"/>
-      <c r="E116" s="74"/>
-      <c r="F116" s="74"/>
+      <c r="A116" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="B116" s="54"/>
+      <c r="C116" s="72"/>
+      <c r="D116" s="72"/>
+      <c r="E116" s="72"/>
+      <c r="F116" s="72"/>
       <c r="G116"/>
       <c r="H116"/>
       <c r="I116"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="56" t="s">
-        <v>142</v>
-      </c>
-      <c r="B117" s="56"/>
-      <c r="C117" s="74"/>
-      <c r="D117" s="74"/>
-      <c r="E117" s="74"/>
-      <c r="F117" s="74"/>
+      <c r="A117" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="B117" s="69"/>
+      <c r="C117" s="72"/>
+      <c r="D117" s="72"/>
+      <c r="E117" s="72"/>
+      <c r="F117" s="72"/>
       <c r="G117"/>
       <c r="H117"/>
       <c r="I117"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="56" t="s">
+      <c r="A118" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="B118" s="56"/>
-      <c r="C118" s="74"/>
-      <c r="D118" s="74"/>
-      <c r="E118" s="74"/>
-      <c r="F118" s="74"/>
+      <c r="B118" s="69"/>
+      <c r="C118" s="72"/>
+      <c r="D118" s="72"/>
+      <c r="E118" s="72"/>
+      <c r="F118" s="72"/>
       <c r="G118"/>
       <c r="H118"/>
       <c r="I118"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="57" t="s">
-        <v>91</v>
-      </c>
-      <c r="B119" s="71"/>
-      <c r="C119" s="74"/>
-      <c r="D119" s="74"/>
-      <c r="E119" s="74"/>
-      <c r="F119" s="74"/>
+      <c r="A119" s="55" t="s">
+        <v>133</v>
+      </c>
+      <c r="B119" s="69"/>
+      <c r="C119" s="72"/>
+      <c r="D119" s="72"/>
+      <c r="E119" s="72"/>
+      <c r="F119" s="72"/>
       <c r="G119"/>
       <c r="H119"/>
       <c r="I119"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="57" t="s">
-        <v>99</v>
-      </c>
-      <c r="B120" s="71"/>
-      <c r="C120" s="74"/>
-      <c r="D120" s="74"/>
-      <c r="E120" s="74"/>
-      <c r="F120" s="74"/>
+      <c r="A120" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="B120" s="69"/>
+      <c r="C120" s="72"/>
+      <c r="D120" s="72"/>
+      <c r="E120" s="72"/>
+      <c r="F120" s="72"/>
       <c r="G120"/>
       <c r="H120"/>
       <c r="I120"/>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="57" t="s">
-        <v>135</v>
-      </c>
-      <c r="B121" s="71"/>
-      <c r="C121" s="74"/>
-      <c r="D121" s="74"/>
-      <c r="E121" s="74"/>
-      <c r="F121" s="74"/>
+      <c r="A121" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="B121" s="69"/>
+      <c r="C121" s="72"/>
+      <c r="D121" s="72"/>
+      <c r="E121" s="72"/>
+      <c r="F121" s="72"/>
       <c r="G121"/>
       <c r="H121"/>
       <c r="I121"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="56" t="s">
-        <v>143</v>
-      </c>
-      <c r="B122" s="71"/>
-      <c r="C122" s="74"/>
-      <c r="D122" s="74"/>
-      <c r="E122" s="74"/>
-      <c r="F122" s="74"/>
+      <c r="A122" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="B122" s="69"/>
+      <c r="C122" s="72"/>
+      <c r="D122" s="72"/>
+      <c r="E122" s="72"/>
+      <c r="F122" s="72"/>
       <c r="G122"/>
       <c r="H122"/>
       <c r="I122"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="57" t="s">
+      <c r="A123" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="B123" s="71"/>
-      <c r="C123" s="74"/>
-      <c r="D123" s="74"/>
-      <c r="E123" s="74"/>
-      <c r="F123" s="74"/>
+      <c r="B123" s="69"/>
+      <c r="C123" s="72"/>
+      <c r="D123" s="72"/>
+      <c r="E123" s="72"/>
+      <c r="F123" s="72"/>
       <c r="G123"/>
       <c r="H123"/>
       <c r="I123"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="57" t="s">
-        <v>92</v>
-      </c>
-      <c r="B124" s="71"/>
-      <c r="C124" s="74"/>
-      <c r="D124" s="74"/>
-      <c r="E124" s="74"/>
-      <c r="F124" s="74"/>
+      <c r="A124" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="B124" s="69"/>
+      <c r="C124" s="72"/>
+      <c r="D124" s="72"/>
+      <c r="E124" s="72"/>
+      <c r="F124" s="72"/>
       <c r="G124"/>
       <c r="H124"/>
       <c r="I124"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="57" t="s">
-        <v>101</v>
-      </c>
-      <c r="B125" s="71"/>
-      <c r="C125" s="74"/>
-      <c r="D125" s="74"/>
-      <c r="E125" s="74"/>
-      <c r="F125" s="74"/>
+      <c r="A125" s="54" t="s">
+        <v>142</v>
+      </c>
+      <c r="B125" s="69"/>
+      <c r="C125" s="72"/>
+      <c r="D125" s="72"/>
+      <c r="E125" s="72"/>
+      <c r="F125" s="72"/>
       <c r="G125"/>
       <c r="H125"/>
       <c r="I125"/>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A126" s="57" t="s">
-        <v>136</v>
-      </c>
-      <c r="B126" s="71"/>
-      <c r="C126" s="74"/>
-      <c r="D126" s="74"/>
-      <c r="E126" s="74"/>
-      <c r="F126" s="74"/>
+      <c r="A126" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="B126" s="69"/>
+      <c r="C126" s="72"/>
+      <c r="D126" s="72"/>
+      <c r="E126" s="72"/>
+      <c r="F126" s="72"/>
       <c r="G126"/>
       <c r="H126"/>
       <c r="I126"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A127" s="56" t="s">
-        <v>144</v>
-      </c>
-      <c r="B127" s="71"/>
-      <c r="C127" s="74"/>
-      <c r="D127" s="74"/>
-      <c r="E127" s="74"/>
-      <c r="F127" s="74"/>
+      <c r="A127" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="B127" s="69"/>
+      <c r="C127" s="72"/>
+      <c r="D127" s="72"/>
+      <c r="E127" s="72"/>
+      <c r="F127" s="72"/>
       <c r="G127"/>
       <c r="H127"/>
       <c r="I127"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" s="57" t="s">
+      <c r="A128" s="55" t="s">
         <v>102</v>
       </c>
-      <c r="B128" s="71"/>
-      <c r="C128" s="74"/>
-      <c r="D128" s="74"/>
-      <c r="E128" s="74"/>
-      <c r="F128" s="74"/>
+      <c r="B128" s="69"/>
+      <c r="C128" s="72"/>
+      <c r="D128" s="72"/>
+      <c r="E128" s="73"/>
+      <c r="F128" s="72"/>
       <c r="G128"/>
       <c r="H128"/>
       <c r="I128"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="57" t="s">
-        <v>93</v>
-      </c>
-      <c r="B129" s="71"/>
-      <c r="C129" s="74"/>
-      <c r="D129" s="74"/>
-      <c r="E129" s="74"/>
-      <c r="F129" s="74"/>
+      <c r="A129" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="B129" s="69"/>
+      <c r="C129" s="72"/>
+      <c r="D129" s="72"/>
+      <c r="E129" s="73"/>
+      <c r="F129" s="72"/>
       <c r="G129"/>
       <c r="H129"/>
       <c r="I129"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="57" t="s">
-        <v>103</v>
-      </c>
-      <c r="B130" s="71"/>
-      <c r="C130" s="74"/>
-      <c r="D130" s="74"/>
-      <c r="E130" s="75"/>
-      <c r="F130" s="74"/>
+      <c r="A130" s="54" t="s">
+        <v>143</v>
+      </c>
+      <c r="B130" s="69"/>
+      <c r="C130" s="72"/>
+      <c r="D130" s="72"/>
+      <c r="E130" s="72"/>
+      <c r="F130" s="72"/>
       <c r="G130"/>
       <c r="H130"/>
       <c r="I130"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="57" t="s">
-        <v>137</v>
-      </c>
-      <c r="B131" s="71"/>
-      <c r="C131" s="74"/>
-      <c r="D131" s="74"/>
-      <c r="E131" s="75"/>
-      <c r="F131" s="74"/>
+      <c r="A131" s="55" t="s">
+        <v>103</v>
+      </c>
+      <c r="B131" s="69"/>
+      <c r="C131" s="72"/>
+      <c r="D131" s="72"/>
+      <c r="E131" s="72"/>
+      <c r="F131" s="72"/>
       <c r="G131"/>
       <c r="H131"/>
       <c r="I131"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="56" t="s">
-        <v>145</v>
-      </c>
-      <c r="B132" s="71"/>
-      <c r="C132" s="74"/>
-      <c r="D132" s="74"/>
-      <c r="E132" s="74"/>
-      <c r="F132" s="74"/>
+      <c r="A132" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="B132" s="54"/>
+      <c r="C132" s="72"/>
+      <c r="D132" s="72"/>
+      <c r="E132" s="72"/>
+      <c r="F132" s="72"/>
       <c r="G132"/>
       <c r="H132"/>
       <c r="I132"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="57" t="s">
+      <c r="A133" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="B133" s="71"/>
-      <c r="C133" s="74"/>
-      <c r="D133" s="74"/>
-      <c r="E133" s="74"/>
-      <c r="F133" s="74"/>
+      <c r="B133" s="54"/>
+      <c r="C133" s="72"/>
+      <c r="D133" s="72"/>
+      <c r="E133" s="72"/>
+      <c r="F133" s="72"/>
       <c r="G133"/>
       <c r="H133"/>
       <c r="I133"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="57" t="s">
-        <v>94</v>
-      </c>
-      <c r="B134" s="56"/>
-      <c r="C134" s="74"/>
-      <c r="D134" s="74"/>
-      <c r="E134" s="74"/>
-      <c r="F134" s="74"/>
+      <c r="A134" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="B134" s="54"/>
+      <c r="C134" s="72"/>
+      <c r="D134" s="72"/>
+      <c r="E134" s="72"/>
+      <c r="F134" s="72"/>
       <c r="G134"/>
       <c r="H134"/>
       <c r="I134"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A135" s="57" t="s">
-        <v>105</v>
-      </c>
-      <c r="B135" s="56"/>
-      <c r="C135" s="74"/>
-      <c r="D135" s="74"/>
-      <c r="E135" s="74"/>
-      <c r="F135" s="74"/>
+      <c r="A135" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="B135" s="54"/>
+      <c r="C135" s="72"/>
+      <c r="D135" s="72"/>
+      <c r="E135" s="72"/>
+      <c r="F135" s="72"/>
       <c r="G135"/>
       <c r="H135"/>
       <c r="I135"/>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A136" s="57" t="s">
-        <v>138</v>
-      </c>
-      <c r="B136" s="56"/>
-      <c r="C136" s="74"/>
-      <c r="D136" s="74"/>
-      <c r="E136" s="74"/>
-      <c r="F136" s="74"/>
+      <c r="A136" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="B136" s="54"/>
+      <c r="C136" s="72"/>
+      <c r="D136" s="72"/>
+      <c r="E136" s="72"/>
+      <c r="F136" s="72"/>
       <c r="G136"/>
       <c r="H136"/>
       <c r="I136"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A137" s="56" t="s">
-        <v>146</v>
-      </c>
-      <c r="B137" s="56"/>
-      <c r="C137" s="74"/>
-      <c r="D137" s="74"/>
-      <c r="E137" s="74"/>
-      <c r="F137" s="74"/>
+      <c r="A137" s="55" t="s">
+        <v>124</v>
+      </c>
+      <c r="B137" s="54"/>
+      <c r="C137" s="72"/>
+      <c r="D137" s="72"/>
+      <c r="E137" s="72"/>
+      <c r="F137" s="72"/>
       <c r="G137"/>
       <c r="H137"/>
       <c r="I137"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="57" t="s">
-        <v>106</v>
-      </c>
-      <c r="B138" s="56"/>
-      <c r="C138" s="74"/>
-      <c r="D138" s="74"/>
-      <c r="E138" s="74"/>
-      <c r="F138" s="74"/>
+      <c r="A138" s="55" t="s">
+        <v>125</v>
+      </c>
+      <c r="B138" s="54"/>
+      <c r="C138" s="72"/>
+      <c r="D138" s="72"/>
+      <c r="E138" s="72"/>
+      <c r="F138" s="72"/>
       <c r="G138"/>
       <c r="H138"/>
       <c r="I138"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A139" s="57" t="s">
-        <v>126</v>
-      </c>
-      <c r="B139" s="56"/>
-      <c r="C139" s="74"/>
-      <c r="D139" s="74"/>
-      <c r="E139" s="74"/>
-      <c r="F139" s="74"/>
+      <c r="A139" s="55" t="s">
+        <v>137</v>
+      </c>
+      <c r="B139" s="54"/>
+      <c r="C139" s="72"/>
+      <c r="D139" s="72"/>
+      <c r="E139" s="72"/>
+      <c r="F139" s="72"/>
       <c r="G139"/>
       <c r="H139"/>
       <c r="I139"/>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A140" s="57" t="s">
-        <v>127</v>
-      </c>
-      <c r="B140" s="56"/>
-      <c r="C140" s="74"/>
-      <c r="D140" s="74"/>
-      <c r="E140" s="74"/>
-      <c r="F140" s="74"/>
+      <c r="A140" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="B140" s="54"/>
+      <c r="C140" s="72"/>
+      <c r="D140" s="72"/>
+      <c r="E140" s="72"/>
+      <c r="F140" s="72"/>
       <c r="G140"/>
       <c r="H140"/>
       <c r="I140"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A141" s="57" t="s">
-        <v>139</v>
-      </c>
-      <c r="B141" s="56"/>
-      <c r="C141" s="74"/>
-      <c r="D141" s="74"/>
-      <c r="E141" s="74"/>
-      <c r="F141" s="74"/>
+      <c r="A141" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="B141" s="70"/>
+      <c r="C141" s="72"/>
+      <c r="D141" s="72"/>
+      <c r="E141" s="72"/>
+      <c r="F141" s="72"/>
       <c r="G141"/>
       <c r="H141"/>
       <c r="I141"/>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A142" s="56" t="s">
-        <v>147</v>
-      </c>
-      <c r="B142" s="56"/>
-      <c r="C142" s="74"/>
-      <c r="D142" s="74"/>
-      <c r="E142" s="74"/>
-      <c r="F142" s="74"/>
-      <c r="G142"/>
-      <c r="H142"/>
-      <c r="I142"/>
+      <c r="C142" s="48"/>
+      <c r="D142" s="48"/>
+      <c r="E142" s="48"/>
+      <c r="F142" s="48"/>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A143" s="58" t="s">
-        <v>128</v>
-      </c>
-      <c r="B143" s="72"/>
-      <c r="C143" s="74"/>
-      <c r="D143" s="74"/>
-      <c r="E143" s="74"/>
-      <c r="F143" s="74"/>
-      <c r="G143"/>
-      <c r="H143"/>
-      <c r="I143"/>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C144" s="50"/>
-      <c r="D144" s="50"/>
-      <c r="E144" s="50"/>
-      <c r="F144" s="50"/>
-    </row>
-    <row r="145" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C145" s="50"/>
-      <c r="D145" s="50"/>
-      <c r="E145" s="50"/>
-      <c r="F145" s="50"/>
+      <c r="C143" s="48"/>
+      <c r="D143" s="48"/>
+      <c r="E143" s="48"/>
+      <c r="F143" s="48"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
@@ -4548,7 +4524,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B94:D107 B76:D80 B86:D88</xm:sqref>
+          <xm:sqref>B76:D80 B86:D88 B94:D105</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Simplify GUI with some loops
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="144">
   <si>
     <t>recent_time</t>
   </si>
@@ -333,12 +333,6 @@
   </si>
   <si>
     <t>econ_saturation_xpertacf</t>
-  </si>
-  <si>
-    <t>output_by_scenario</t>
-  </si>
-  <si>
-    <t>output_horizontally</t>
   </si>
   <si>
     <t>report_start_time</t>
@@ -2463,10 +2457,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP143"/>
+  <dimension ref="A1:BP141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2888,7 +2882,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B41" s="61"/>
       <c r="C41" s="61"/>
@@ -2901,7 +2895,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B42" s="61"/>
       <c r="C42" s="61"/>
@@ -2914,7 +2908,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B43" s="61"/>
       <c r="C43" s="61"/>
@@ -2927,7 +2921,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B44" s="61"/>
       <c r="C44" s="61"/>
@@ -2940,7 +2934,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B45" s="61"/>
       <c r="C45" s="61"/>
@@ -2963,7 +2957,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B47" s="24"/>
       <c r="C47" s="24"/>
@@ -3027,7 +3021,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B54" s="29"/>
       <c r="C54" s="58"/>
@@ -3035,7 +3029,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B55" s="29"/>
       <c r="C55" s="58"/>
@@ -3043,7 +3037,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B56" s="29"/>
       <c r="C56" s="58"/>
@@ -3067,7 +3061,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B59" s="28"/>
       <c r="C59" s="57"/>
@@ -3105,7 +3099,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B63" s="28"/>
       <c r="C63" s="57"/>
@@ -3116,7 +3110,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B64" s="28"/>
       <c r="C64" s="57"/>
@@ -3127,7 +3121,7 @@
     </row>
     <row r="65" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B65" s="28"/>
       <c r="C65" s="57"/>
@@ -3138,7 +3132,7 @@
     </row>
     <row r="66" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B66" s="63"/>
       <c r="C66" s="65"/>
@@ -3151,7 +3145,7 @@
     </row>
     <row r="67" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B67" s="63"/>
       <c r="C67" s="65"/>
@@ -3164,7 +3158,7 @@
     </row>
     <row r="68" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B68" s="63"/>
       <c r="C68" s="65"/>
@@ -3177,7 +3171,7 @@
     </row>
     <row r="69" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B69" s="28"/>
       <c r="C69" s="57"/>
@@ -3188,7 +3182,7 @@
     </row>
     <row r="70" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B70" s="28"/>
       <c r="C70" s="57"/>
@@ -3888,7 +3882,7 @@
     </row>
     <row r="94" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="B94" s="40"/>
       <c r="C94" s="48"/>
@@ -3896,31 +3890,41 @@
     </row>
     <row r="95" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A95" s="13" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="B95" s="40"/>
       <c r="C95" s="48"/>
       <c r="D95" s="48"/>
     </row>
-    <row r="96" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="13" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B96" s="40"/>
       <c r="C96" s="48"/>
       <c r="D96" s="48"/>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E96" s="48"/>
+      <c r="F96" s="48"/>
+      <c r="G96" s="44"/>
+      <c r="H96" s="44"/>
+      <c r="I96" s="44"/>
+    </row>
+    <row r="97" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A97" s="13" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="B97" s="40"/>
       <c r="C97" s="48"/>
       <c r="D97" s="48"/>
+      <c r="E97" s="48"/>
+      <c r="F97" s="48"/>
+      <c r="G97" s="44"/>
+      <c r="H97" s="44"/>
+      <c r="I97" s="44"/>
     </row>
     <row r="98" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="13" t="s">
-        <v>67</v>
+        <v>115</v>
       </c>
       <c r="B98" s="40"/>
       <c r="C98" s="48"/>
@@ -3933,7 +3937,7 @@
     </row>
     <row r="99" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="13" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B99" s="40"/>
       <c r="C99" s="48"/>
@@ -3944,35 +3948,25 @@
       <c r="H99" s="44"/>
       <c r="I99" s="44"/>
     </row>
-    <row r="100" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="13" t="s">
-        <v>117</v>
+        <v>56</v>
       </c>
       <c r="B100" s="40"/>
       <c r="C100" s="48"/>
       <c r="D100" s="48"/>
-      <c r="E100" s="48"/>
-      <c r="F100" s="48"/>
-      <c r="G100" s="44"/>
-      <c r="H100" s="44"/>
-      <c r="I100" s="44"/>
-    </row>
-    <row r="101" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="13" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="B101" s="40"/>
       <c r="C101" s="48"/>
       <c r="D101" s="48"/>
-      <c r="E101" s="48"/>
-      <c r="F101" s="48"/>
-      <c r="G101" s="44"/>
-      <c r="H101" s="44"/>
-      <c r="I101" s="44"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B102" s="40"/>
       <c r="C102" s="48"/>
@@ -3980,35 +3974,45 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="13" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
       <c r="B103" s="40"/>
       <c r="C103" s="48"/>
       <c r="D103" s="48"/>
+      <c r="E103" s="48"/>
+      <c r="F103" s="48"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B104" s="40"/>
-      <c r="C104" s="48"/>
-      <c r="D104" s="48"/>
+      <c r="A104" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="B104" s="68"/>
+      <c r="C104" s="72"/>
+      <c r="D104" s="72"/>
+      <c r="E104" s="72"/>
+      <c r="F104" s="72"/>
+      <c r="G104"/>
+      <c r="H104"/>
+      <c r="I104"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="B105" s="40"/>
-      <c r="C105" s="48"/>
-      <c r="D105" s="48"/>
-      <c r="E105" s="48"/>
-      <c r="F105" s="48"/>
+      <c r="A105" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="B105" s="54"/>
+      <c r="C105" s="71"/>
+      <c r="D105" s="71"/>
+      <c r="E105" s="72"/>
+      <c r="F105" s="72"/>
+      <c r="G105"/>
+      <c r="H105"/>
+      <c r="I105"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="53" t="s">
-        <v>87</v>
-      </c>
-      <c r="B106" s="68"/>
+      <c r="A106" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="B106" s="54"/>
       <c r="C106" s="72"/>
       <c r="D106" s="72"/>
       <c r="E106" s="72"/>
@@ -4019,11 +4023,11 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="54" t="s">
-        <v>88</v>
+        <v>129</v>
       </c>
       <c r="B107" s="54"/>
-      <c r="C107" s="71"/>
-      <c r="D107" s="71"/>
+      <c r="C107" s="72"/>
+      <c r="D107" s="72"/>
       <c r="E107" s="72"/>
       <c r="F107" s="72"/>
       <c r="G107"/>
@@ -4032,7 +4036,7 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="54" t="s">
-        <v>94</v>
+        <v>137</v>
       </c>
       <c r="B108" s="54"/>
       <c r="C108" s="72"/>
@@ -4045,7 +4049,7 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="54" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="B109" s="54"/>
       <c r="C109" s="72"/>
@@ -4058,11 +4062,11 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="54" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="B110" s="54"/>
-      <c r="C110" s="72"/>
-      <c r="D110" s="72"/>
+      <c r="C110" s="71"/>
+      <c r="D110" s="71"/>
       <c r="E110" s="72"/>
       <c r="F110" s="72"/>
       <c r="G110"/>
@@ -4071,7 +4075,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="54" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B111" s="54"/>
       <c r="C111" s="72"/>
@@ -4084,11 +4088,11 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="54" t="s">
-        <v>89</v>
+        <v>130</v>
       </c>
       <c r="B112" s="54"/>
-      <c r="C112" s="71"/>
-      <c r="D112" s="71"/>
+      <c r="C112" s="72"/>
+      <c r="D112" s="72"/>
       <c r="E112" s="72"/>
       <c r="F112" s="72"/>
       <c r="G112"/>
@@ -4097,7 +4101,7 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="54" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="B113" s="54"/>
       <c r="C113" s="72"/>
@@ -4110,7 +4114,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="54" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="B114" s="54"/>
       <c r="C114" s="72"/>
@@ -4122,10 +4126,10 @@
       <c r="I114"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="54" t="s">
-        <v>140</v>
-      </c>
-      <c r="B115" s="54"/>
+      <c r="A115" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="B115" s="69"/>
       <c r="C115" s="72"/>
       <c r="D115" s="72"/>
       <c r="E115" s="72"/>
@@ -4135,10 +4139,10 @@
       <c r="I115"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="B116" s="54"/>
+      <c r="A116" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B116" s="69"/>
       <c r="C116" s="72"/>
       <c r="D116" s="72"/>
       <c r="E116" s="72"/>
@@ -4149,7 +4153,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="55" t="s">
-        <v>90</v>
+        <v>131</v>
       </c>
       <c r="B117" s="69"/>
       <c r="C117" s="72"/>
@@ -4161,8 +4165,8 @@
       <c r="I117"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="55" t="s">
-        <v>98</v>
+      <c r="A118" s="54" t="s">
+        <v>139</v>
       </c>
       <c r="B118" s="69"/>
       <c r="C118" s="72"/>
@@ -4175,7 +4179,7 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="55" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="B119" s="69"/>
       <c r="C119" s="72"/>
@@ -4187,8 +4191,8 @@
       <c r="I119"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="54" t="s">
-        <v>141</v>
+      <c r="A120" s="55" t="s">
+        <v>91</v>
       </c>
       <c r="B120" s="69"/>
       <c r="C120" s="72"/>
@@ -4201,7 +4205,7 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="55" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B121" s="69"/>
       <c r="C121" s="72"/>
@@ -4214,7 +4218,7 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="55" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="B122" s="69"/>
       <c r="C122" s="72"/>
@@ -4226,8 +4230,8 @@
       <c r="I122"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="55" t="s">
-        <v>100</v>
+      <c r="A123" s="54" t="s">
+        <v>140</v>
       </c>
       <c r="B123" s="69"/>
       <c r="C123" s="72"/>
@@ -4240,7 +4244,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="55" t="s">
-        <v>134</v>
+        <v>101</v>
       </c>
       <c r="B124" s="69"/>
       <c r="C124" s="72"/>
@@ -4252,8 +4256,8 @@
       <c r="I124"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="54" t="s">
-        <v>142</v>
+      <c r="A125" s="55" t="s">
+        <v>92</v>
       </c>
       <c r="B125" s="69"/>
       <c r="C125" s="72"/>
@@ -4266,12 +4270,12 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="55" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B126" s="69"/>
       <c r="C126" s="72"/>
       <c r="D126" s="72"/>
-      <c r="E126" s="72"/>
+      <c r="E126" s="73"/>
       <c r="F126" s="72"/>
       <c r="G126"/>
       <c r="H126"/>
@@ -4279,25 +4283,25 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="55" t="s">
-        <v>92</v>
+        <v>133</v>
       </c>
       <c r="B127" s="69"/>
       <c r="C127" s="72"/>
       <c r="D127" s="72"/>
-      <c r="E127" s="72"/>
+      <c r="E127" s="73"/>
       <c r="F127" s="72"/>
       <c r="G127"/>
       <c r="H127"/>
       <c r="I127"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" s="55" t="s">
-        <v>102</v>
+      <c r="A128" s="54" t="s">
+        <v>141</v>
       </c>
       <c r="B128" s="69"/>
       <c r="C128" s="72"/>
       <c r="D128" s="72"/>
-      <c r="E128" s="73"/>
+      <c r="E128" s="72"/>
       <c r="F128" s="72"/>
       <c r="G128"/>
       <c r="H128"/>
@@ -4305,22 +4309,22 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="55" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="B129" s="69"/>
       <c r="C129" s="72"/>
       <c r="D129" s="72"/>
-      <c r="E129" s="73"/>
+      <c r="E129" s="72"/>
       <c r="F129" s="72"/>
       <c r="G129"/>
       <c r="H129"/>
       <c r="I129"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="54" t="s">
-        <v>143</v>
-      </c>
-      <c r="B130" s="69"/>
+      <c r="A130" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="B130" s="54"/>
       <c r="C130" s="72"/>
       <c r="D130" s="72"/>
       <c r="E130" s="72"/>
@@ -4331,9 +4335,9 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="B131" s="69"/>
+        <v>104</v>
+      </c>
+      <c r="B131" s="54"/>
       <c r="C131" s="72"/>
       <c r="D131" s="72"/>
       <c r="E131" s="72"/>
@@ -4344,7 +4348,7 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="55" t="s">
-        <v>93</v>
+        <v>134</v>
       </c>
       <c r="B132" s="54"/>
       <c r="C132" s="72"/>
@@ -4356,8 +4360,8 @@
       <c r="I132"/>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="55" t="s">
-        <v>104</v>
+      <c r="A133" s="54" t="s">
+        <v>142</v>
       </c>
       <c r="B133" s="54"/>
       <c r="C133" s="72"/>
@@ -4370,7 +4374,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="55" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
       <c r="B134" s="54"/>
       <c r="C134" s="72"/>
@@ -4382,8 +4386,8 @@
       <c r="I134"/>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A135" s="54" t="s">
-        <v>144</v>
+      <c r="A135" s="55" t="s">
+        <v>122</v>
       </c>
       <c r="B135" s="54"/>
       <c r="C135" s="72"/>
@@ -4396,7 +4400,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="55" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="B136" s="54"/>
       <c r="C136" s="72"/>
@@ -4409,7 +4413,7 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="55" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B137" s="54"/>
       <c r="C137" s="72"/>
@@ -4421,8 +4425,8 @@
       <c r="I137"/>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="55" t="s">
-        <v>125</v>
+      <c r="A138" s="54" t="s">
+        <v>143</v>
       </c>
       <c r="B138" s="54"/>
       <c r="C138" s="72"/>
@@ -4434,10 +4438,10 @@
       <c r="I138"/>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A139" s="55" t="s">
-        <v>137</v>
-      </c>
-      <c r="B139" s="54"/>
+      <c r="A139" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="B139" s="70"/>
       <c r="C139" s="72"/>
       <c r="D139" s="72"/>
       <c r="E139" s="72"/>
@@ -4447,42 +4451,16 @@
       <c r="I139"/>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A140" s="54" t="s">
-        <v>145</v>
-      </c>
-      <c r="B140" s="54"/>
-      <c r="C140" s="72"/>
-      <c r="D140" s="72"/>
-      <c r="E140" s="72"/>
-      <c r="F140" s="72"/>
-      <c r="G140"/>
-      <c r="H140"/>
-      <c r="I140"/>
+      <c r="C140" s="48"/>
+      <c r="D140" s="48"/>
+      <c r="E140" s="48"/>
+      <c r="F140" s="48"/>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A141" s="56" t="s">
-        <v>126</v>
-      </c>
-      <c r="B141" s="70"/>
-      <c r="C141" s="72"/>
-      <c r="D141" s="72"/>
-      <c r="E141" s="72"/>
-      <c r="F141" s="72"/>
-      <c r="G141"/>
-      <c r="H141"/>
-      <c r="I141"/>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C142" s="48"/>
-      <c r="D142" s="48"/>
-      <c r="E142" s="48"/>
-      <c r="F142" s="48"/>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C143" s="48"/>
-      <c r="D143" s="48"/>
-      <c r="E143" s="48"/>
-      <c r="F143" s="48"/>
+      <c r="C141" s="48"/>
+      <c r="D141" s="48"/>
+      <c r="E141" s="48"/>
+      <c r="F141" s="48"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
@@ -4524,7 +4502,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B76:D80 B86:D88 B94:D105</xm:sqref>
+          <xm:sqref>B76:D80 B86:D88 B94:D103</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
More checkboxes to GUI
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="135">
   <si>
     <t>recent_time</t>
   </si>
@@ -182,15 +182,6 @@
     <t>active</t>
   </si>
   <si>
-    <t>output_flow_diagram</t>
-  </si>
-  <si>
-    <t>output_fractions</t>
-  </si>
-  <si>
-    <t>output_scaleups</t>
-  </si>
-  <si>
     <t>tb_prop_early_progression_age0to5</t>
   </si>
   <si>
@@ -215,12 +206,6 @@
     <t>tb_multiplier_child_infectiousness_age10up</t>
   </si>
   <si>
-    <t>output_by_age</t>
-  </si>
-  <si>
-    <t>output_age_fractions</t>
-  </si>
-  <si>
     <t>comorbidity_diabetes</t>
   </si>
   <si>
@@ -260,9 +245,6 @@
     <t>early_time</t>
   </si>
   <si>
-    <t>output_comorbidity_fractions</t>
-  </si>
-  <si>
     <t>program_prop_acf_detections_per_round</t>
   </si>
   <si>
@@ -360,12 +342,6 @@
   </si>
   <si>
     <t>output_age_calculations</t>
-  </si>
-  <si>
-    <t>output_plot_economics</t>
-  </si>
-  <si>
-    <t>output_compartment_populations</t>
   </si>
   <si>
     <t>program_nns_smearacf</t>
@@ -2454,10 +2430,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP140"/>
+  <dimension ref="A1:BP132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2476,7 +2452,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -2509,7 +2485,7 @@
     </row>
     <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -2519,7 +2495,7 @@
     </row>
     <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -2529,7 +2505,7 @@
     </row>
     <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
@@ -2549,7 +2525,7 @@
     </row>
     <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -2559,7 +2535,7 @@
     </row>
     <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -2569,7 +2545,7 @@
     </row>
     <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
@@ -2779,7 +2755,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
@@ -2789,7 +2765,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B32" s="23"/>
       <c r="C32" s="23"/>
@@ -2849,7 +2825,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B38" s="25"/>
       <c r="C38" s="25"/>
@@ -2859,7 +2835,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B39" s="25"/>
       <c r="C39" s="25"/>
@@ -2869,7 +2845,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B40" s="25"/>
       <c r="C40" s="25"/>
@@ -2879,7 +2855,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B41" s="61"/>
       <c r="C41" s="61"/>
@@ -2892,7 +2868,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B42" s="61"/>
       <c r="C42" s="61"/>
@@ -2905,7 +2881,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B43" s="61"/>
       <c r="C43" s="61"/>
@@ -2918,7 +2894,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B44" s="61"/>
       <c r="C44" s="61"/>
@@ -2931,7 +2907,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B45" s="61"/>
       <c r="C45" s="61"/>
@@ -2954,7 +2930,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B47" s="24"/>
       <c r="C47" s="24"/>
@@ -2964,7 +2940,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B48" s="26"/>
       <c r="C48" s="26"/>
@@ -2994,7 +2970,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B51" s="28"/>
       <c r="C51" s="57"/>
@@ -3018,7 +2994,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B54" s="29"/>
       <c r="C54" s="58"/>
@@ -3026,7 +3002,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B55" s="29"/>
       <c r="C55" s="58"/>
@@ -3034,7 +3010,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B56" s="29"/>
       <c r="C56" s="58"/>
@@ -3058,7 +3034,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B59" s="28"/>
       <c r="C59" s="57"/>
@@ -3096,7 +3072,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B63" s="28"/>
       <c r="C63" s="57"/>
@@ -3107,7 +3083,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B64" s="28"/>
       <c r="C64" s="57"/>
@@ -3118,7 +3094,7 @@
     </row>
     <row r="65" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B65" s="28"/>
       <c r="C65" s="57"/>
@@ -3129,7 +3105,7 @@
     </row>
     <row r="66" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B66" s="63"/>
       <c r="C66" s="65"/>
@@ -3142,7 +3118,7 @@
     </row>
     <row r="67" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B67" s="63"/>
       <c r="C67" s="65"/>
@@ -3155,7 +3131,7 @@
     </row>
     <row r="68" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B68" s="63"/>
       <c r="C68" s="65"/>
@@ -3168,7 +3144,7 @@
     </row>
     <row r="69" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B69" s="28"/>
       <c r="C69" s="57"/>
@@ -3179,7 +3155,7 @@
     </row>
     <row r="70" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B70" s="28"/>
       <c r="C70" s="57"/>
@@ -3190,7 +3166,7 @@
     </row>
     <row r="71" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B71" s="30"/>
       <c r="C71" s="57"/>
@@ -3367,7 +3343,7 @@
     </row>
     <row r="76" spans="1:68" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B76" s="34"/>
       <c r="C76" s="57"/>
@@ -3439,7 +3415,7 @@
     </row>
     <row r="77" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B77" s="33"/>
       <c r="C77" s="57"/>
@@ -3452,7 +3428,7 @@
     </row>
     <row r="78" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B78" s="33"/>
       <c r="C78" s="57"/>
@@ -3465,7 +3441,7 @@
     </row>
     <row r="79" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B79" s="33"/>
       <c r="C79" s="57"/>
@@ -3478,7 +3454,7 @@
     </row>
     <row r="80" spans="1:68" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B80" s="35"/>
       <c r="C80" s="57"/>
@@ -3550,7 +3526,7 @@
     </row>
     <row r="81" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B81" s="36"/>
       <c r="C81" s="59"/>
@@ -3563,7 +3539,7 @@
     </row>
     <row r="82" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B82" s="36"/>
       <c r="C82" s="59"/>
@@ -3576,7 +3552,7 @@
     </row>
     <row r="83" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B83" s="36"/>
       <c r="C83" s="59"/>
@@ -3589,7 +3565,7 @@
     </row>
     <row r="84" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B84" s="36"/>
       <c r="C84" s="59"/>
@@ -3602,7 +3578,7 @@
     </row>
     <row r="85" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B85" s="37"/>
       <c r="C85" s="59"/>
@@ -3877,105 +3853,128 @@
       <c r="G93" s="43"/>
       <c r="H93" s="52"/>
     </row>
-    <row r="94" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B94" s="40"/>
       <c r="C94" s="48"/>
       <c r="D94" s="48"/>
-    </row>
-    <row r="95" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B95" s="40"/>
-      <c r="C95" s="48"/>
-      <c r="D95" s="48"/>
-      <c r="E95" s="48"/>
-      <c r="F95" s="48"/>
-      <c r="G95" s="44"/>
-      <c r="H95" s="44"/>
-      <c r="I95" s="44"/>
-    </row>
-    <row r="96" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B96" s="40"/>
-      <c r="C96" s="48"/>
-      <c r="D96" s="48"/>
-      <c r="E96" s="48"/>
-      <c r="F96" s="48"/>
-      <c r="G96" s="44"/>
-      <c r="H96" s="44"/>
-      <c r="I96" s="44"/>
-    </row>
-    <row r="97" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="B97" s="40"/>
-      <c r="C97" s="48"/>
-      <c r="D97" s="48"/>
-      <c r="E97" s="48"/>
-      <c r="F97" s="48"/>
-      <c r="G97" s="44"/>
-      <c r="H97" s="44"/>
-      <c r="I97" s="44"/>
-    </row>
-    <row r="98" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="13" t="s">
+      <c r="E94" s="48"/>
+      <c r="F94" s="48"/>
+      <c r="G94" s="44"/>
+      <c r="H94" s="44"/>
+      <c r="I94" s="44"/>
+    </row>
+    <row r="95" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A95" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="B95" s="68"/>
+      <c r="C95" s="72"/>
+      <c r="D95" s="72"/>
+      <c r="E95" s="72"/>
+      <c r="F95" s="72"/>
+      <c r="G95"/>
+      <c r="H95"/>
+      <c r="I95"/>
+    </row>
+    <row r="96" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A96" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="B98" s="40"/>
-      <c r="C98" s="48"/>
-      <c r="D98" s="48"/>
-      <c r="E98" s="48"/>
-      <c r="F98" s="48"/>
-      <c r="G98" s="44"/>
-      <c r="H98" s="44"/>
-      <c r="I98" s="44"/>
+      <c r="B96" s="54"/>
+      <c r="C96" s="71"/>
+      <c r="D96" s="71"/>
+      <c r="E96" s="72"/>
+      <c r="F96" s="72"/>
+      <c r="G96"/>
+      <c r="H96"/>
+      <c r="I96"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="B97" s="54"/>
+      <c r="C97" s="72"/>
+      <c r="D97" s="72"/>
+      <c r="E97" s="72"/>
+      <c r="F97" s="72"/>
+      <c r="G97"/>
+      <c r="H97"/>
+      <c r="I97"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B98" s="54"/>
+      <c r="C98" s="72"/>
+      <c r="D98" s="72"/>
+      <c r="E98" s="72"/>
+      <c r="F98" s="72"/>
+      <c r="G98"/>
+      <c r="H98"/>
+      <c r="I98"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B99" s="40"/>
-      <c r="C99" s="48"/>
-      <c r="D99" s="48"/>
+      <c r="A99" s="54" t="s">
+        <v>128</v>
+      </c>
+      <c r="B99" s="54"/>
+      <c r="C99" s="72"/>
+      <c r="D99" s="72"/>
+      <c r="E99" s="72"/>
+      <c r="F99" s="72"/>
+      <c r="G99"/>
+      <c r="H99"/>
+      <c r="I99"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="B100" s="40"/>
-      <c r="C100" s="48"/>
-      <c r="D100" s="48"/>
+      <c r="A100" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="B100" s="54"/>
+      <c r="C100" s="72"/>
+      <c r="D100" s="72"/>
+      <c r="E100" s="72"/>
+      <c r="F100" s="72"/>
+      <c r="G100"/>
+      <c r="H100"/>
+      <c r="I100"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="B101" s="40"/>
-      <c r="C101" s="48"/>
-      <c r="D101" s="48"/>
+      <c r="A101" s="54" t="s">
+        <v>82</v>
+      </c>
+      <c r="B101" s="54"/>
+      <c r="C101" s="71"/>
+      <c r="D101" s="71"/>
+      <c r="E101" s="72"/>
+      <c r="F101" s="72"/>
+      <c r="G101"/>
+      <c r="H101"/>
+      <c r="I101"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="B102" s="40"/>
-      <c r="C102" s="48"/>
-      <c r="D102" s="48"/>
-      <c r="E102" s="48"/>
-      <c r="F102" s="48"/>
+      <c r="A102" s="54" t="s">
+        <v>89</v>
+      </c>
+      <c r="B102" s="54"/>
+      <c r="C102" s="72"/>
+      <c r="D102" s="72"/>
+      <c r="E102" s="72"/>
+      <c r="F102" s="72"/>
+      <c r="G102"/>
+      <c r="H102"/>
+      <c r="I102"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="B103" s="68"/>
+      <c r="A103" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="B103" s="54"/>
       <c r="C103" s="72"/>
       <c r="D103" s="72"/>
       <c r="E103" s="72"/>
@@ -3986,11 +3985,11 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="54" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="B104" s="54"/>
-      <c r="C104" s="71"/>
-      <c r="D104" s="71"/>
+      <c r="C104" s="72"/>
+      <c r="D104" s="72"/>
       <c r="E104" s="72"/>
       <c r="F104" s="72"/>
       <c r="G104"/>
@@ -3999,7 +3998,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="54" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B105" s="54"/>
       <c r="C105" s="72"/>
@@ -4011,10 +4010,10 @@
       <c r="I105"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="54" t="s">
-        <v>128</v>
-      </c>
-      <c r="B106" s="54"/>
+      <c r="A106" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="B106" s="69"/>
       <c r="C106" s="72"/>
       <c r="D106" s="72"/>
       <c r="E106" s="72"/>
@@ -4024,10 +4023,10 @@
       <c r="I106"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="54" t="s">
-        <v>136</v>
-      </c>
-      <c r="B107" s="54"/>
+      <c r="A107" s="55" t="s">
+        <v>91</v>
+      </c>
+      <c r="B107" s="69"/>
       <c r="C107" s="72"/>
       <c r="D107" s="72"/>
       <c r="E107" s="72"/>
@@ -4037,10 +4036,10 @@
       <c r="I107"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="54" t="s">
-        <v>94</v>
-      </c>
-      <c r="B108" s="54"/>
+      <c r="A108" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="B108" s="69"/>
       <c r="C108" s="72"/>
       <c r="D108" s="72"/>
       <c r="E108" s="72"/>
@@ -4051,11 +4050,11 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="B109" s="54"/>
-      <c r="C109" s="71"/>
-      <c r="D109" s="71"/>
+        <v>130</v>
+      </c>
+      <c r="B109" s="69"/>
+      <c r="C109" s="72"/>
+      <c r="D109" s="72"/>
       <c r="E109" s="72"/>
       <c r="F109" s="72"/>
       <c r="G109"/>
@@ -4063,10 +4062,10 @@
       <c r="I109"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="B110" s="54"/>
+      <c r="A110" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="B110" s="69"/>
       <c r="C110" s="72"/>
       <c r="D110" s="72"/>
       <c r="E110" s="72"/>
@@ -4076,10 +4075,10 @@
       <c r="I110"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="54" t="s">
-        <v>129</v>
-      </c>
-      <c r="B111" s="54"/>
+      <c r="A111" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="B111" s="69"/>
       <c r="C111" s="72"/>
       <c r="D111" s="72"/>
       <c r="E111" s="72"/>
@@ -4089,10 +4088,10 @@
       <c r="I111"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="54" t="s">
-        <v>137</v>
-      </c>
-      <c r="B112" s="54"/>
+      <c r="A112" s="55" t="s">
+        <v>93</v>
+      </c>
+      <c r="B112" s="69"/>
       <c r="C112" s="72"/>
       <c r="D112" s="72"/>
       <c r="E112" s="72"/>
@@ -4102,10 +4101,10 @@
       <c r="I112"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="B113" s="54"/>
+      <c r="A113" s="55" t="s">
+        <v>123</v>
+      </c>
+      <c r="B113" s="69"/>
       <c r="C113" s="72"/>
       <c r="D113" s="72"/>
       <c r="E113" s="72"/>
@@ -4115,8 +4114,8 @@
       <c r="I113"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="55" t="s">
-        <v>89</v>
+      <c r="A114" s="54" t="s">
+        <v>131</v>
       </c>
       <c r="B114" s="69"/>
       <c r="C114" s="72"/>
@@ -4129,7 +4128,7 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="55" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B115" s="69"/>
       <c r="C115" s="72"/>
@@ -4142,7 +4141,7 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="55" t="s">
-        <v>130</v>
+        <v>85</v>
       </c>
       <c r="B116" s="69"/>
       <c r="C116" s="72"/>
@@ -4154,13 +4153,13 @@
       <c r="I116"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="54" t="s">
-        <v>138</v>
+      <c r="A117" s="55" t="s">
+        <v>95</v>
       </c>
       <c r="B117" s="69"/>
       <c r="C117" s="72"/>
       <c r="D117" s="72"/>
-      <c r="E117" s="72"/>
+      <c r="E117" s="73"/>
       <c r="F117" s="72"/>
       <c r="G117"/>
       <c r="H117"/>
@@ -4168,20 +4167,20 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="55" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="B118" s="69"/>
       <c r="C118" s="72"/>
       <c r="D118" s="72"/>
-      <c r="E118" s="72"/>
+      <c r="E118" s="73"/>
       <c r="F118" s="72"/>
       <c r="G118"/>
       <c r="H118"/>
       <c r="I118"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="55" t="s">
-        <v>90</v>
+      <c r="A119" s="54" t="s">
+        <v>132</v>
       </c>
       <c r="B119" s="69"/>
       <c r="C119" s="72"/>
@@ -4194,7 +4193,7 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="55" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B120" s="69"/>
       <c r="C120" s="72"/>
@@ -4207,9 +4206,9 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="55" t="s">
-        <v>131</v>
-      </c>
-      <c r="B121" s="69"/>
+        <v>86</v>
+      </c>
+      <c r="B121" s="54"/>
       <c r="C121" s="72"/>
       <c r="D121" s="72"/>
       <c r="E121" s="72"/>
@@ -4219,10 +4218,10 @@
       <c r="I121"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="54" t="s">
-        <v>139</v>
-      </c>
-      <c r="B122" s="69"/>
+      <c r="A122" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="B122" s="54"/>
       <c r="C122" s="72"/>
       <c r="D122" s="72"/>
       <c r="E122" s="72"/>
@@ -4233,9 +4232,9 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="55" t="s">
-        <v>100</v>
-      </c>
-      <c r="B123" s="69"/>
+        <v>125</v>
+      </c>
+      <c r="B123" s="54"/>
       <c r="C123" s="72"/>
       <c r="D123" s="72"/>
       <c r="E123" s="72"/>
@@ -4245,10 +4244,10 @@
       <c r="I123"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="B124" s="69"/>
+      <c r="A124" s="54" t="s">
+        <v>133</v>
+      </c>
+      <c r="B124" s="54"/>
       <c r="C124" s="72"/>
       <c r="D124" s="72"/>
       <c r="E124" s="72"/>
@@ -4259,12 +4258,12 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="55" t="s">
-        <v>101</v>
-      </c>
-      <c r="B125" s="69"/>
+        <v>98</v>
+      </c>
+      <c r="B125" s="54"/>
       <c r="C125" s="72"/>
       <c r="D125" s="72"/>
-      <c r="E125" s="73"/>
+      <c r="E125" s="72"/>
       <c r="F125" s="72"/>
       <c r="G125"/>
       <c r="H125"/>
@@ -4272,22 +4271,22 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="55" t="s">
-        <v>132</v>
-      </c>
-      <c r="B126" s="69"/>
+        <v>113</v>
+      </c>
+      <c r="B126" s="54"/>
       <c r="C126" s="72"/>
       <c r="D126" s="72"/>
-      <c r="E126" s="73"/>
+      <c r="E126" s="72"/>
       <c r="F126" s="72"/>
       <c r="G126"/>
       <c r="H126"/>
       <c r="I126"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A127" s="54" t="s">
-        <v>140</v>
-      </c>
-      <c r="B127" s="69"/>
+      <c r="A127" s="55" t="s">
+        <v>114</v>
+      </c>
+      <c r="B127" s="54"/>
       <c r="C127" s="72"/>
       <c r="D127" s="72"/>
       <c r="E127" s="72"/>
@@ -4298,9 +4297,9 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="55" t="s">
-        <v>102</v>
-      </c>
-      <c r="B128" s="69"/>
+        <v>126</v>
+      </c>
+      <c r="B128" s="54"/>
       <c r="C128" s="72"/>
       <c r="D128" s="72"/>
       <c r="E128" s="72"/>
@@ -4310,8 +4309,8 @@
       <c r="I128"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="55" t="s">
-        <v>92</v>
+      <c r="A129" s="54" t="s">
+        <v>134</v>
       </c>
       <c r="B129" s="54"/>
       <c r="C129" s="72"/>
@@ -4323,10 +4322,10 @@
       <c r="I129"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="55" t="s">
-        <v>103</v>
-      </c>
-      <c r="B130" s="54"/>
+      <c r="A130" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="B130" s="70"/>
       <c r="C130" s="72"/>
       <c r="D130" s="72"/>
       <c r="E130" s="72"/>
@@ -4336,120 +4335,16 @@
       <c r="I130"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="55" t="s">
-        <v>133</v>
-      </c>
-      <c r="B131" s="54"/>
-      <c r="C131" s="72"/>
-      <c r="D131" s="72"/>
-      <c r="E131" s="72"/>
-      <c r="F131" s="72"/>
-      <c r="G131"/>
-      <c r="H131"/>
-      <c r="I131"/>
+      <c r="C131" s="48"/>
+      <c r="D131" s="48"/>
+      <c r="E131" s="48"/>
+      <c r="F131" s="48"/>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="54" t="s">
-        <v>141</v>
-      </c>
-      <c r="B132" s="54"/>
-      <c r="C132" s="72"/>
-      <c r="D132" s="72"/>
-      <c r="E132" s="72"/>
-      <c r="F132" s="72"/>
-      <c r="G132"/>
-      <c r="H132"/>
-      <c r="I132"/>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="55" t="s">
-        <v>104</v>
-      </c>
-      <c r="B133" s="54"/>
-      <c r="C133" s="72"/>
-      <c r="D133" s="72"/>
-      <c r="E133" s="72"/>
-      <c r="F133" s="72"/>
-      <c r="G133"/>
-      <c r="H133"/>
-      <c r="I133"/>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A134" s="55" t="s">
-        <v>121</v>
-      </c>
-      <c r="B134" s="54"/>
-      <c r="C134" s="72"/>
-      <c r="D134" s="72"/>
-      <c r="E134" s="72"/>
-      <c r="F134" s="72"/>
-      <c r="G134"/>
-      <c r="H134"/>
-      <c r="I134"/>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A135" s="55" t="s">
-        <v>122</v>
-      </c>
-      <c r="B135" s="54"/>
-      <c r="C135" s="72"/>
-      <c r="D135" s="72"/>
-      <c r="E135" s="72"/>
-      <c r="F135" s="72"/>
-      <c r="G135"/>
-      <c r="H135"/>
-      <c r="I135"/>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A136" s="55" t="s">
-        <v>134</v>
-      </c>
-      <c r="B136" s="54"/>
-      <c r="C136" s="72"/>
-      <c r="D136" s="72"/>
-      <c r="E136" s="72"/>
-      <c r="F136" s="72"/>
-      <c r="G136"/>
-      <c r="H136"/>
-      <c r="I136"/>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A137" s="54" t="s">
-        <v>142</v>
-      </c>
-      <c r="B137" s="54"/>
-      <c r="C137" s="72"/>
-      <c r="D137" s="72"/>
-      <c r="E137" s="72"/>
-      <c r="F137" s="72"/>
-      <c r="G137"/>
-      <c r="H137"/>
-      <c r="I137"/>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A138" s="56" t="s">
-        <v>123</v>
-      </c>
-      <c r="B138" s="70"/>
-      <c r="C138" s="72"/>
-      <c r="D138" s="72"/>
-      <c r="E138" s="72"/>
-      <c r="F138" s="72"/>
-      <c r="G138"/>
-      <c r="H138"/>
-      <c r="I138"/>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C139" s="48"/>
-      <c r="D139" s="48"/>
-      <c r="E139" s="48"/>
-      <c r="F139" s="48"/>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C140" s="48"/>
-      <c r="D140" s="48"/>
-      <c r="E140" s="48"/>
-      <c r="F140" s="48"/>
+      <c r="C132" s="48"/>
+      <c r="D132" s="48"/>
+      <c r="E132" s="48"/>
+      <c r="F132" s="48"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
@@ -4491,7 +4386,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B76:D80 B86:D88 B94:D102</xm:sqref>
+          <xm:sqref>B76:D80 B86:D88 B94:D94</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Move last boolean out of spreadsheets
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="134">
   <si>
     <t>recent_time</t>
   </si>
@@ -339,9 +339,6 @@
   </si>
   <si>
     <t>plot_start_time</t>
-  </si>
-  <si>
-    <t>output_age_calculations</t>
   </si>
   <si>
     <t>program_nns_smearacf</t>
@@ -2430,10 +2427,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP132"/>
+  <dimension ref="A1:BP131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2855,7 +2852,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B41" s="61"/>
       <c r="C41" s="61"/>
@@ -2868,7 +2865,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B42" s="61"/>
       <c r="C42" s="61"/>
@@ -2881,7 +2878,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B43" s="61"/>
       <c r="C43" s="61"/>
@@ -2894,7 +2891,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B44" s="61"/>
       <c r="C44" s="61"/>
@@ -2907,7 +2904,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B45" s="61"/>
       <c r="C45" s="61"/>
@@ -3034,7 +3031,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B59" s="28"/>
       <c r="C59" s="57"/>
@@ -3105,7 +3102,7 @@
     </row>
     <row r="66" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B66" s="63"/>
       <c r="C66" s="65"/>
@@ -3118,7 +3115,7 @@
     </row>
     <row r="67" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B67" s="63"/>
       <c r="C67" s="65"/>
@@ -3131,7 +3128,7 @@
     </row>
     <row r="68" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B68" s="63"/>
       <c r="C68" s="65"/>
@@ -3845,34 +3842,38 @@
       <c r="A93" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B93" s="43"/>
-      <c r="C93" s="43"/>
+      <c r="B93" s="43">
+        <v>5</v>
+      </c>
+      <c r="C93" s="43">
+        <v>15</v>
+      </c>
       <c r="D93" s="43"/>
       <c r="E93" s="43"/>
       <c r="F93" s="43"/>
       <c r="G93" s="43"/>
       <c r="H93" s="52"/>
     </row>
-    <row r="94" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B94" s="40"/>
-      <c r="C94" s="48"/>
-      <c r="D94" s="48"/>
-      <c r="E94" s="48"/>
-      <c r="F94" s="48"/>
-      <c r="G94" s="44"/>
-      <c r="H94" s="44"/>
-      <c r="I94" s="44"/>
+    <row r="94" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A94" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="B94" s="68"/>
+      <c r="C94" s="72"/>
+      <c r="D94" s="72"/>
+      <c r="E94" s="72"/>
+      <c r="F94" s="72"/>
+      <c r="G94"/>
+      <c r="H94"/>
+      <c r="I94"/>
     </row>
     <row r="95" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A95" s="53" t="s">
-        <v>80</v>
-      </c>
-      <c r="B95" s="68"/>
-      <c r="C95" s="72"/>
-      <c r="D95" s="72"/>
+      <c r="A95" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="B95" s="54"/>
+      <c r="C95" s="71"/>
+      <c r="D95" s="71"/>
       <c r="E95" s="72"/>
       <c r="F95" s="72"/>
       <c r="G95"/>
@@ -3881,11 +3882,11 @@
     </row>
     <row r="96" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A96" s="54" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B96" s="54"/>
-      <c r="C96" s="71"/>
-      <c r="D96" s="71"/>
+      <c r="C96" s="72"/>
+      <c r="D96" s="72"/>
       <c r="E96" s="72"/>
       <c r="F96" s="72"/>
       <c r="G96"/>
@@ -3894,7 +3895,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="54" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="B97" s="54"/>
       <c r="C97" s="72"/>
@@ -3907,7 +3908,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="54" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B98" s="54"/>
       <c r="C98" s="72"/>
@@ -3920,7 +3921,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="54" t="s">
-        <v>128</v>
+        <v>88</v>
       </c>
       <c r="B99" s="54"/>
       <c r="C99" s="72"/>
@@ -3933,11 +3934,11 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="54" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B100" s="54"/>
-      <c r="C100" s="72"/>
-      <c r="D100" s="72"/>
+      <c r="C100" s="71"/>
+      <c r="D100" s="71"/>
       <c r="E100" s="72"/>
       <c r="F100" s="72"/>
       <c r="G100"/>
@@ -3946,11 +3947,11 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="54" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B101" s="54"/>
-      <c r="C101" s="71"/>
-      <c r="D101" s="71"/>
+      <c r="C101" s="72"/>
+      <c r="D101" s="72"/>
       <c r="E101" s="72"/>
       <c r="F101" s="72"/>
       <c r="G101"/>
@@ -3959,7 +3960,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="54" t="s">
-        <v>89</v>
+        <v>120</v>
       </c>
       <c r="B102" s="54"/>
       <c r="C102" s="72"/>
@@ -3972,7 +3973,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="54" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B103" s="54"/>
       <c r="C103" s="72"/>
@@ -3985,7 +3986,7 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="54" t="s">
-        <v>129</v>
+        <v>90</v>
       </c>
       <c r="B104" s="54"/>
       <c r="C104" s="72"/>
@@ -3997,10 +3998,10 @@
       <c r="I104"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="B105" s="54"/>
+      <c r="A105" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="B105" s="69"/>
       <c r="C105" s="72"/>
       <c r="D105" s="72"/>
       <c r="E105" s="72"/>
@@ -4011,7 +4012,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="55" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="B106" s="69"/>
       <c r="C106" s="72"/>
@@ -4024,7 +4025,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="55" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="B107" s="69"/>
       <c r="C107" s="72"/>
@@ -4036,8 +4037,8 @@
       <c r="I107"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="55" t="s">
-        <v>122</v>
+      <c r="A108" s="54" t="s">
+        <v>129</v>
       </c>
       <c r="B108" s="69"/>
       <c r="C108" s="72"/>
@@ -4049,8 +4050,8 @@
       <c r="I108"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="54" t="s">
-        <v>130</v>
+      <c r="A109" s="55" t="s">
+        <v>92</v>
       </c>
       <c r="B109" s="69"/>
       <c r="C109" s="72"/>
@@ -4063,7 +4064,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="55" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B110" s="69"/>
       <c r="C110" s="72"/>
@@ -4076,7 +4077,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="55" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B111" s="69"/>
       <c r="C111" s="72"/>
@@ -4089,7 +4090,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="55" t="s">
-        <v>93</v>
+        <v>122</v>
       </c>
       <c r="B112" s="69"/>
       <c r="C112" s="72"/>
@@ -4101,8 +4102,8 @@
       <c r="I112"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="55" t="s">
-        <v>123</v>
+      <c r="A113" s="54" t="s">
+        <v>130</v>
       </c>
       <c r="B113" s="69"/>
       <c r="C113" s="72"/>
@@ -4114,8 +4115,8 @@
       <c r="I113"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="54" t="s">
-        <v>131</v>
+      <c r="A114" s="55" t="s">
+        <v>94</v>
       </c>
       <c r="B114" s="69"/>
       <c r="C114" s="72"/>
@@ -4128,7 +4129,7 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="55" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B115" s="69"/>
       <c r="C115" s="72"/>
@@ -4141,12 +4142,12 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="55" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B116" s="69"/>
       <c r="C116" s="72"/>
       <c r="D116" s="72"/>
-      <c r="E116" s="72"/>
+      <c r="E116" s="73"/>
       <c r="F116" s="72"/>
       <c r="G116"/>
       <c r="H116"/>
@@ -4154,7 +4155,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="55" t="s">
-        <v>95</v>
+        <v>123</v>
       </c>
       <c r="B117" s="69"/>
       <c r="C117" s="72"/>
@@ -4166,21 +4167,21 @@
       <c r="I117"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="55" t="s">
-        <v>124</v>
+      <c r="A118" s="54" t="s">
+        <v>131</v>
       </c>
       <c r="B118" s="69"/>
       <c r="C118" s="72"/>
       <c r="D118" s="72"/>
-      <c r="E118" s="73"/>
+      <c r="E118" s="72"/>
       <c r="F118" s="72"/>
       <c r="G118"/>
       <c r="H118"/>
       <c r="I118"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="54" t="s">
-        <v>132</v>
+      <c r="A119" s="55" t="s">
+        <v>96</v>
       </c>
       <c r="B119" s="69"/>
       <c r="C119" s="72"/>
@@ -4193,9 +4194,9 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="B120" s="69"/>
+        <v>86</v>
+      </c>
+      <c r="B120" s="54"/>
       <c r="C120" s="72"/>
       <c r="D120" s="72"/>
       <c r="E120" s="72"/>
@@ -4206,7 +4207,7 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="55" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="B121" s="54"/>
       <c r="C121" s="72"/>
@@ -4219,7 +4220,7 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="55" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="B122" s="54"/>
       <c r="C122" s="72"/>
@@ -4231,8 +4232,8 @@
       <c r="I122"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="55" t="s">
-        <v>125</v>
+      <c r="A123" s="54" t="s">
+        <v>132</v>
       </c>
       <c r="B123" s="54"/>
       <c r="C123" s="72"/>
@@ -4244,8 +4245,8 @@
       <c r="I123"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="54" t="s">
-        <v>133</v>
+      <c r="A124" s="55" t="s">
+        <v>98</v>
       </c>
       <c r="B124" s="54"/>
       <c r="C124" s="72"/>
@@ -4258,7 +4259,7 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="55" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B125" s="54"/>
       <c r="C125" s="72"/>
@@ -4284,7 +4285,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="55" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B127" s="54"/>
       <c r="C127" s="72"/>
@@ -4296,8 +4297,8 @@
       <c r="I127"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" s="55" t="s">
-        <v>126</v>
+      <c r="A128" s="54" t="s">
+        <v>133</v>
       </c>
       <c r="B128" s="54"/>
       <c r="C128" s="72"/>
@@ -4309,10 +4310,10 @@
       <c r="I128"/>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="54" t="s">
-        <v>134</v>
-      </c>
-      <c r="B129" s="54"/>
+      <c r="A129" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="B129" s="70"/>
       <c r="C129" s="72"/>
       <c r="D129" s="72"/>
       <c r="E129" s="72"/>
@@ -4322,29 +4323,16 @@
       <c r="I129"/>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A130" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B130" s="70"/>
-      <c r="C130" s="72"/>
-      <c r="D130" s="72"/>
-      <c r="E130" s="72"/>
-      <c r="F130" s="72"/>
-      <c r="G130"/>
-      <c r="H130"/>
-      <c r="I130"/>
+      <c r="C130" s="48"/>
+      <c r="D130" s="48"/>
+      <c r="E130" s="48"/>
+      <c r="F130" s="48"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C131" s="48"/>
       <c r="D131" s="48"/>
       <c r="E131" s="48"/>
       <c r="F131" s="48"/>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C132" s="48"/>
-      <c r="D132" s="48"/>
-      <c r="E132" s="48"/>
-      <c r="F132" s="48"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
@@ -4386,7 +4374,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B76:D80 B86:D88 B94:D94</xm:sqref>
+          <xm:sqref>B76:D80 B86:D88</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
First dropdown box implemented in GUI
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="133">
   <si>
     <t>recent_time</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>age_breakpoints</t>
-  </si>
-  <si>
-    <t>integration</t>
   </si>
   <si>
     <t>explicit</t>
@@ -2427,10 +2424,10 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP131"/>
+  <dimension ref="A1:BP130"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2446,10 +2443,10 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -2461,7 +2458,7 @@
     </row>
     <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -2472,7 +2469,7 @@
     </row>
     <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="23"/>
       <c r="C3" s="23"/>
@@ -2482,7 +2479,7 @@
     </row>
     <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="23"/>
       <c r="C4" s="23"/>
@@ -2492,7 +2489,7 @@
     </row>
     <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -2502,7 +2499,7 @@
     </row>
     <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
@@ -2512,7 +2509,7 @@
     </row>
     <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
@@ -2522,7 +2519,7 @@
     </row>
     <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -2532,7 +2529,7 @@
     </row>
     <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -2542,7 +2539,7 @@
     </row>
     <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
@@ -2552,7 +2549,7 @@
     </row>
     <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -2562,7 +2559,7 @@
     </row>
     <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -2572,7 +2569,7 @@
     </row>
     <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -2582,7 +2579,7 @@
     </row>
     <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
@@ -2592,7 +2589,7 @@
     </row>
     <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
@@ -2602,7 +2599,7 @@
     </row>
     <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="24"/>
       <c r="C16" s="24"/>
@@ -2612,7 +2609,7 @@
     </row>
     <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="24"/>
       <c r="C17" s="24"/>
@@ -2622,7 +2619,7 @@
     </row>
     <row r="18" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" s="23"/>
       <c r="C18" s="23"/>
@@ -2632,7 +2629,7 @@
     </row>
     <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
@@ -2642,7 +2639,7 @@
     </row>
     <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
@@ -2652,7 +2649,7 @@
     </row>
     <row r="21" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="23"/>
       <c r="C21" s="23"/>
@@ -2662,7 +2659,7 @@
     </row>
     <row r="22" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
@@ -2672,7 +2669,7 @@
     </row>
     <row r="23" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
@@ -2682,7 +2679,7 @@
     </row>
     <row r="24" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B24" s="23"/>
       <c r="C24" s="23"/>
@@ -2692,7 +2689,7 @@
     </row>
     <row r="25" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="23"/>
       <c r="C25" s="23"/>
@@ -2702,7 +2699,7 @@
     </row>
     <row r="26" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="23"/>
       <c r="C26" s="23"/>
@@ -2712,7 +2709,7 @@
     </row>
     <row r="27" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B27" s="23"/>
       <c r="C27" s="23"/>
@@ -2722,7 +2719,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B28" s="23"/>
       <c r="C28" s="23"/>
@@ -2732,7 +2729,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="23"/>
       <c r="C29" s="23"/>
@@ -2742,7 +2739,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" s="23"/>
       <c r="C30" s="23"/>
@@ -2752,7 +2749,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
@@ -2762,7 +2759,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="23"/>
       <c r="C32" s="23"/>
@@ -2772,7 +2769,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>
@@ -2782,7 +2779,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B34" s="23"/>
       <c r="C34" s="23"/>
@@ -2792,7 +2789,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="23"/>
       <c r="C35" s="23"/>
@@ -2802,7 +2799,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" s="23"/>
       <c r="C36" s="23"/>
@@ -2812,7 +2809,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B37" s="25"/>
       <c r="C37" s="25"/>
@@ -2822,7 +2819,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B38" s="25"/>
       <c r="C38" s="25"/>
@@ -2832,7 +2829,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B39" s="25"/>
       <c r="C39" s="25"/>
@@ -2842,7 +2839,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B40" s="25"/>
       <c r="C40" s="25"/>
@@ -2852,7 +2849,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B41" s="61"/>
       <c r="C41" s="61"/>
@@ -2865,7 +2862,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B42" s="61"/>
       <c r="C42" s="61"/>
@@ -2878,7 +2875,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B43" s="61"/>
       <c r="C43" s="61"/>
@@ -2891,7 +2888,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B44" s="61"/>
       <c r="C44" s="61"/>
@@ -2904,7 +2901,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B45" s="61"/>
       <c r="C45" s="61"/>
@@ -2917,7 +2914,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="24"/>
       <c r="C46" s="24"/>
@@ -2927,7 +2924,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B47" s="24"/>
       <c r="C47" s="24"/>
@@ -2937,7 +2934,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B48" s="26"/>
       <c r="C48" s="26"/>
@@ -2947,7 +2944,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B49" s="27">
         <v>0.05</v>
@@ -2959,7 +2956,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B50" s="28"/>
       <c r="C50" s="57"/>
@@ -2967,7 +2964,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B51" s="28"/>
       <c r="C51" s="57"/>
@@ -2975,7 +2972,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B52" s="28"/>
       <c r="C52" s="57"/>
@@ -2983,7 +2980,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B53" s="28"/>
       <c r="C53" s="57"/>
@@ -2991,7 +2988,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B54" s="29"/>
       <c r="C54" s="58"/>
@@ -2999,7 +2996,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B55" s="29"/>
       <c r="C55" s="58"/>
@@ -3007,7 +3004,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B56" s="29"/>
       <c r="C56" s="58"/>
@@ -3023,7 +3020,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B58" s="28"/>
       <c r="C58" s="57"/>
@@ -3031,7 +3028,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B59" s="28"/>
       <c r="C59" s="57"/>
@@ -3039,7 +3036,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B60" s="28"/>
       <c r="C60" s="57"/>
@@ -3047,7 +3044,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B61" s="28"/>
       <c r="C61" s="57"/>
@@ -3058,7 +3055,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B62" s="28"/>
       <c r="C62" s="57"/>
@@ -3069,7 +3066,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B63" s="28"/>
       <c r="C63" s="57"/>
@@ -3080,7 +3077,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B64" s="28"/>
       <c r="C64" s="57"/>
@@ -3091,7 +3088,7 @@
     </row>
     <row r="65" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B65" s="28"/>
       <c r="C65" s="57"/>
@@ -3102,7 +3099,7 @@
     </row>
     <row r="66" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B66" s="63"/>
       <c r="C66" s="65"/>
@@ -3115,7 +3112,7 @@
     </row>
     <row r="67" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B67" s="63"/>
       <c r="C67" s="65"/>
@@ -3128,7 +3125,7 @@
     </row>
     <row r="68" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B68" s="63"/>
       <c r="C68" s="65"/>
@@ -3141,7 +3138,7 @@
     </row>
     <row r="69" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B69" s="28"/>
       <c r="C69" s="57"/>
@@ -3152,7 +3149,7 @@
     </row>
     <row r="70" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B70" s="28"/>
       <c r="C70" s="57"/>
@@ -3163,7 +3160,7 @@
     </row>
     <row r="71" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B71" s="30"/>
       <c r="C71" s="57"/>
@@ -3174,7 +3171,7 @@
     </row>
     <row r="72" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B72" s="31"/>
       <c r="C72" s="57"/>
@@ -3185,7 +3182,7 @@
     </row>
     <row r="73" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B73" s="32"/>
       <c r="C73" s="57"/>
@@ -3340,7 +3337,7 @@
     </row>
     <row r="76" spans="1:68" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B76" s="34"/>
       <c r="C76" s="57"/>
@@ -3412,7 +3409,7 @@
     </row>
     <row r="77" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B77" s="33"/>
       <c r="C77" s="57"/>
@@ -3425,7 +3422,7 @@
     </row>
     <row r="78" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B78" s="33"/>
       <c r="C78" s="57"/>
@@ -3438,7 +3435,7 @@
     </row>
     <row r="79" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B79" s="33"/>
       <c r="C79" s="57"/>
@@ -3451,7 +3448,7 @@
     </row>
     <row r="80" spans="1:68" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B80" s="35"/>
       <c r="C80" s="57"/>
@@ -3523,7 +3520,7 @@
     </row>
     <row r="81" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B81" s="36"/>
       <c r="C81" s="59"/>
@@ -3536,7 +3533,7 @@
     </row>
     <row r="82" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B82" s="36"/>
       <c r="C82" s="59"/>
@@ -3549,7 +3546,7 @@
     </row>
     <row r="83" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B83" s="36"/>
       <c r="C83" s="59"/>
@@ -3562,7 +3559,7 @@
     </row>
     <row r="84" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B84" s="36"/>
       <c r="C84" s="59"/>
@@ -3575,7 +3572,7 @@
     </row>
     <row r="85" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B85" s="37"/>
       <c r="C85" s="59"/>
@@ -3804,7 +3801,7 @@
     </row>
     <row r="89" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A89" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B89" s="40"/>
       <c r="C89" s="48"/>
@@ -3812,55 +3809,60 @@
     </row>
     <row r="90" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A90" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B90" s="41"/>
       <c r="C90" s="60"/>
       <c r="D90" s="60"/>
     </row>
     <row r="91" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A91" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B91" s="40"/>
-      <c r="C91" s="48"/>
-      <c r="D91" s="48"/>
+      <c r="A91" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B91" s="42"/>
+      <c r="C91" s="42"/>
+      <c r="D91" s="42"/>
+      <c r="E91" s="50"/>
+      <c r="F91" s="50"/>
+      <c r="G91" s="50"/>
+      <c r="H91" s="51"/>
     </row>
     <row r="92" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A92" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B92" s="42"/>
-      <c r="C92" s="42"/>
-      <c r="D92" s="42"/>
-      <c r="E92" s="50"/>
-      <c r="F92" s="50"/>
-      <c r="G92" s="50"/>
-      <c r="H92" s="51"/>
+      <c r="A92" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B92" s="43">
+        <v>5</v>
+      </c>
+      <c r="C92" s="43">
+        <v>15</v>
+      </c>
+      <c r="D92" s="43"/>
+      <c r="E92" s="43"/>
+      <c r="F92" s="43"/>
+      <c r="G92" s="43"/>
+      <c r="H92" s="52"/>
     </row>
     <row r="93" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A93" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B93" s="43">
-        <v>5</v>
-      </c>
-      <c r="C93" s="43">
-        <v>15</v>
-      </c>
-      <c r="D93" s="43"/>
-      <c r="E93" s="43"/>
-      <c r="F93" s="43"/>
-      <c r="G93" s="43"/>
-      <c r="H93" s="52"/>
+      <c r="A93" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93" s="68"/>
+      <c r="C93" s="72"/>
+      <c r="D93" s="72"/>
+      <c r="E93" s="72"/>
+      <c r="F93" s="72"/>
+      <c r="G93"/>
+      <c r="H93"/>
+      <c r="I93"/>
     </row>
     <row r="94" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A94" s="53" t="s">
+      <c r="A94" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="B94" s="68"/>
-      <c r="C94" s="72"/>
-      <c r="D94" s="72"/>
+      <c r="B94" s="54"/>
+      <c r="C94" s="71"/>
+      <c r="D94" s="71"/>
       <c r="E94" s="72"/>
       <c r="F94" s="72"/>
       <c r="G94"/>
@@ -3869,11 +3871,11 @@
     </row>
     <row r="95" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A95" s="54" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B95" s="54"/>
-      <c r="C95" s="71"/>
-      <c r="D95" s="71"/>
+      <c r="C95" s="72"/>
+      <c r="D95" s="72"/>
       <c r="E95" s="72"/>
       <c r="F95" s="72"/>
       <c r="G95"/>
@@ -3882,7 +3884,7 @@
     </row>
     <row r="96" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A96" s="54" t="s">
-        <v>87</v>
+        <v>118</v>
       </c>
       <c r="B96" s="54"/>
       <c r="C96" s="72"/>
@@ -3895,7 +3897,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="54" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B97" s="54"/>
       <c r="C97" s="72"/>
@@ -3908,7 +3910,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="54" t="s">
-        <v>127</v>
+        <v>87</v>
       </c>
       <c r="B98" s="54"/>
       <c r="C98" s="72"/>
@@ -3921,11 +3923,11 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="54" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B99" s="54"/>
-      <c r="C99" s="72"/>
-      <c r="D99" s="72"/>
+      <c r="C99" s="71"/>
+      <c r="D99" s="71"/>
       <c r="E99" s="72"/>
       <c r="F99" s="72"/>
       <c r="G99"/>
@@ -3934,11 +3936,11 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="54" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B100" s="54"/>
-      <c r="C100" s="71"/>
-      <c r="D100" s="71"/>
+      <c r="C100" s="72"/>
+      <c r="D100" s="72"/>
       <c r="E100" s="72"/>
       <c r="F100" s="72"/>
       <c r="G100"/>
@@ -3947,7 +3949,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="54" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="B101" s="54"/>
       <c r="C101" s="72"/>
@@ -3960,7 +3962,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="54" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B102" s="54"/>
       <c r="C102" s="72"/>
@@ -3973,7 +3975,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="54" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
       <c r="B103" s="54"/>
       <c r="C103" s="72"/>
@@ -3985,10 +3987,10 @@
       <c r="I103"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="54" t="s">
-        <v>90</v>
-      </c>
-      <c r="B104" s="54"/>
+      <c r="A104" s="55" t="s">
+        <v>82</v>
+      </c>
+      <c r="B104" s="69"/>
       <c r="C104" s="72"/>
       <c r="D104" s="72"/>
       <c r="E104" s="72"/>
@@ -3999,7 +4001,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="55" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B105" s="69"/>
       <c r="C105" s="72"/>
@@ -4012,7 +4014,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="55" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
       <c r="B106" s="69"/>
       <c r="C106" s="72"/>
@@ -4024,8 +4026,8 @@
       <c r="I106"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="55" t="s">
-        <v>121</v>
+      <c r="A107" s="54" t="s">
+        <v>128</v>
       </c>
       <c r="B107" s="69"/>
       <c r="C107" s="72"/>
@@ -4037,8 +4039,8 @@
       <c r="I107"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="54" t="s">
-        <v>129</v>
+      <c r="A108" s="55" t="s">
+        <v>91</v>
       </c>
       <c r="B108" s="69"/>
       <c r="C108" s="72"/>
@@ -4051,7 +4053,7 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="55" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B109" s="69"/>
       <c r="C109" s="72"/>
@@ -4064,7 +4066,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="55" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="B110" s="69"/>
       <c r="C110" s="72"/>
@@ -4077,7 +4079,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="55" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="B111" s="69"/>
       <c r="C111" s="72"/>
@@ -4089,8 +4091,8 @@
       <c r="I111"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="55" t="s">
-        <v>122</v>
+      <c r="A112" s="54" t="s">
+        <v>129</v>
       </c>
       <c r="B112" s="69"/>
       <c r="C112" s="72"/>
@@ -4102,8 +4104,8 @@
       <c r="I112"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="54" t="s">
-        <v>130</v>
+      <c r="A113" s="55" t="s">
+        <v>93</v>
       </c>
       <c r="B113" s="69"/>
       <c r="C113" s="72"/>
@@ -4116,7 +4118,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="55" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B114" s="69"/>
       <c r="C114" s="72"/>
@@ -4129,12 +4131,12 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="55" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B115" s="69"/>
       <c r="C115" s="72"/>
       <c r="D115" s="72"/>
-      <c r="E115" s="72"/>
+      <c r="E115" s="73"/>
       <c r="F115" s="72"/>
       <c r="G115"/>
       <c r="H115"/>
@@ -4142,7 +4144,7 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="55" t="s">
-        <v>95</v>
+        <v>122</v>
       </c>
       <c r="B116" s="69"/>
       <c r="C116" s="72"/>
@@ -4154,21 +4156,21 @@
       <c r="I116"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="55" t="s">
-        <v>123</v>
+      <c r="A117" s="54" t="s">
+        <v>130</v>
       </c>
       <c r="B117" s="69"/>
       <c r="C117" s="72"/>
       <c r="D117" s="72"/>
-      <c r="E117" s="73"/>
+      <c r="E117" s="72"/>
       <c r="F117" s="72"/>
       <c r="G117"/>
       <c r="H117"/>
       <c r="I117"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="54" t="s">
-        <v>131</v>
+      <c r="A118" s="55" t="s">
+        <v>95</v>
       </c>
       <c r="B118" s="69"/>
       <c r="C118" s="72"/>
@@ -4181,9 +4183,9 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="B119" s="69"/>
+        <v>85</v>
+      </c>
+      <c r="B119" s="54"/>
       <c r="C119" s="72"/>
       <c r="D119" s="72"/>
       <c r="E119" s="72"/>
@@ -4194,7 +4196,7 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="55" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B120" s="54"/>
       <c r="C120" s="72"/>
@@ -4207,7 +4209,7 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="55" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="B121" s="54"/>
       <c r="C121" s="72"/>
@@ -4219,8 +4221,8 @@
       <c r="I121"/>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="55" t="s">
-        <v>124</v>
+      <c r="A122" s="54" t="s">
+        <v>131</v>
       </c>
       <c r="B122" s="54"/>
       <c r="C122" s="72"/>
@@ -4232,8 +4234,8 @@
       <c r="I122"/>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="54" t="s">
-        <v>132</v>
+      <c r="A123" s="55" t="s">
+        <v>97</v>
       </c>
       <c r="B123" s="54"/>
       <c r="C123" s="72"/>
@@ -4246,7 +4248,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="55" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="B124" s="54"/>
       <c r="C124" s="72"/>
@@ -4272,7 +4274,7 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="55" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B126" s="54"/>
       <c r="C126" s="72"/>
@@ -4284,8 +4286,8 @@
       <c r="I126"/>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A127" s="55" t="s">
-        <v>125</v>
+      <c r="A127" s="54" t="s">
+        <v>132</v>
       </c>
       <c r="B127" s="54"/>
       <c r="C127" s="72"/>
@@ -4297,10 +4299,10 @@
       <c r="I127"/>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" s="54" t="s">
-        <v>133</v>
-      </c>
-      <c r="B128" s="54"/>
+      <c r="A128" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="B128" s="70"/>
       <c r="C128" s="72"/>
       <c r="D128" s="72"/>
       <c r="E128" s="72"/>
@@ -4309,30 +4311,17 @@
       <c r="H128"/>
       <c r="I128"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="56" t="s">
-        <v>114</v>
-      </c>
-      <c r="B129" s="70"/>
-      <c r="C129" s="72"/>
-      <c r="D129" s="72"/>
-      <c r="E129" s="72"/>
-      <c r="F129" s="72"/>
-      <c r="G129"/>
-      <c r="H129"/>
-      <c r="I129"/>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C129" s="48"/>
+      <c r="D129" s="48"/>
+      <c r="E129" s="48"/>
+      <c r="F129" s="48"/>
+    </row>
+    <row r="130" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C130" s="48"/>
       <c r="D130" s="48"/>
       <c r="E130" s="48"/>
       <c r="F130" s="48"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C131" s="48"/>
-      <c r="D131" s="48"/>
-      <c r="E131" s="48"/>
-      <c r="F131" s="48"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="7">
@@ -4352,7 +4341,7 @@
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B92:D92">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B91:D91">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -4369,18 +4358,12 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="363" yWindow="440" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="363" yWindow="440" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
           <xm:sqref>B76:D80 B86:D88</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$C$2:$C$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B91:D91</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4403,32 +4386,32 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
         <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Neaten model running section of GUI
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="122">
   <si>
     <t>recent_time</t>
   </si>
@@ -41,9 +41,6 @@
     <t>explicit</t>
   </si>
   <si>
-    <t>fitting_method</t>
-  </si>
-  <si>
     <t>scenario_end_time</t>
   </si>
   <si>
@@ -201,36 +198,6 @@
   </si>
   <si>
     <t>tb_multiplier_child_infectiousness_age10up</t>
-  </si>
-  <si>
-    <t>comorbidity_diabetes</t>
-  </si>
-  <si>
-    <t>comorbidity_hiv</t>
-  </si>
-  <si>
-    <t>comorbidity_prison</t>
-  </si>
-  <si>
-    <t>comorbidity_remote</t>
-  </si>
-  <si>
-    <t>comorbidity_poverty</t>
-  </si>
-  <si>
-    <t>comorb_prop_prison</t>
-  </si>
-  <si>
-    <t>comorb_prop_poverty</t>
-  </si>
-  <si>
-    <t>comorb_prop_remote</t>
-  </si>
-  <si>
-    <t>comorb_prop_hiv</t>
-  </si>
-  <si>
-    <t>comorb_prop_diabetes</t>
   </si>
   <si>
     <t>program_prop_treatment_support_improvement</t>
@@ -1365,7 +1332,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1389,9 +1356,7 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="12" fillId="9" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -1408,13 +1373,8 @@
     <xf numFmtId="1" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="12" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="12" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="12" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1435,7 +1395,6 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1454,6 +1413,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2424,437 +2384,437 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP130"/>
+  <dimension ref="A1:BP119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="25.5703125" style="44" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="49" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="49" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="49"/>
+    <col min="2" max="4" width="25.5703125" style="37" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="42" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="42" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="42"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
+        <v>15</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
     </row>
     <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="44"/>
+        <v>21</v>
+      </c>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="37"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
+        <v>22</v>
+      </c>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
+        <v>58</v>
+      </c>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
     </row>
     <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="48"/>
-      <c r="F5" s="48"/>
+        <v>59</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
     </row>
     <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
+        <v>60</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
     </row>
     <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="48"/>
+        <v>23</v>
+      </c>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
     </row>
     <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
+        <v>53</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
     </row>
     <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
+        <v>54</v>
+      </c>
+      <c r="B9" s="21"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
     </row>
     <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
+        <v>55</v>
+      </c>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
     </row>
     <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
+        <v>24</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
     </row>
     <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="48"/>
-      <c r="F12" s="48"/>
+        <v>25</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
     </row>
     <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="48"/>
-      <c r="F13" s="48"/>
+        <v>26</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
     </row>
     <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
+        <v>27</v>
+      </c>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
     </row>
     <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
+        <v>41</v>
+      </c>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
     </row>
     <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
+        <v>42</v>
+      </c>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
     </row>
     <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
+        <v>43</v>
+      </c>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
     </row>
     <row r="18" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
+        <v>28</v>
+      </c>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
     </row>
     <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
+        <v>29</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
     </row>
     <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
+        <v>30</v>
+      </c>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
     </row>
     <row r="21" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
+        <v>31</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
     </row>
     <row r="22" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
+        <v>32</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
     </row>
     <row r="23" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="48"/>
-      <c r="F23" s="48"/>
+        <v>33</v>
+      </c>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
     </row>
     <row r="24" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="48"/>
+        <v>34</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
     </row>
     <row r="25" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="48"/>
-      <c r="F25" s="48"/>
+        <v>35</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
     </row>
     <row r="26" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="48"/>
-      <c r="F26" s="48"/>
+        <v>36</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
     </row>
     <row r="27" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="48"/>
-      <c r="F27" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="48"/>
-      <c r="F28" s="48"/>
+        <v>38</v>
+      </c>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="48"/>
-      <c r="F29" s="48"/>
+        <v>39</v>
+      </c>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="48"/>
-      <c r="F30" s="48"/>
+        <v>40</v>
+      </c>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="48"/>
-      <c r="F31" s="48"/>
+        <v>56</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="48"/>
-      <c r="F32" s="48"/>
+        <v>57</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
+        <v>44</v>
+      </c>
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="48"/>
-      <c r="F34" s="48"/>
+        <v>45</v>
+      </c>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="48"/>
-      <c r="F35" s="48"/>
+        <v>46</v>
+      </c>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="48"/>
-      <c r="F36" s="48"/>
+        <v>47</v>
+      </c>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="48"/>
+        <v>48</v>
+      </c>
+      <c r="B37" s="23"/>
+      <c r="C37" s="23"/>
+      <c r="D37" s="23"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="48"/>
-      <c r="F38" s="48"/>
+        <v>61</v>
+      </c>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="41"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="48"/>
-      <c r="F39" s="48"/>
+        <v>64</v>
+      </c>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="48"/>
-      <c r="F40" s="48"/>
+        <v>65</v>
+      </c>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="41"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B41" s="61"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="61"/>
-      <c r="E41" s="62"/>
+        <v>96</v>
+      </c>
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="54"/>
       <c r="F41"/>
       <c r="G41"/>
       <c r="H41"/>
@@ -2862,12 +2822,12 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B42" s="61"/>
-      <c r="C42" s="61"/>
-      <c r="D42" s="61"/>
-      <c r="E42" s="62"/>
+        <v>97</v>
+      </c>
+      <c r="B42" s="53"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="53"/>
+      <c r="E42" s="54"/>
       <c r="F42"/>
       <c r="G42"/>
       <c r="H42"/>
@@ -2875,12 +2835,12 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B43" s="61"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="61"/>
-      <c r="E43" s="62"/>
+        <v>98</v>
+      </c>
+      <c r="B43" s="53"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="54"/>
       <c r="F43"/>
       <c r="G43"/>
       <c r="H43"/>
@@ -2888,12 +2848,12 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B44" s="61"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="61"/>
-      <c r="E44" s="62"/>
+        <v>114</v>
+      </c>
+      <c r="B44" s="53"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="53"/>
+      <c r="E44" s="54"/>
       <c r="F44"/>
       <c r="G44"/>
       <c r="H44"/>
@@ -2901,12 +2861,12 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B45" s="61"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="61"/>
-      <c r="E45" s="62"/>
+        <v>99</v>
+      </c>
+      <c r="B45" s="53"/>
+      <c r="C45" s="53"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="54"/>
       <c r="F45"/>
       <c r="G45"/>
       <c r="H45"/>
@@ -2914,295 +2874,295 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
+        <v>49</v>
+      </c>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="41"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B47" s="24"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
+        <v>93</v>
+      </c>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="41"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B48" s="26"/>
-      <c r="C48" s="26"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
+        <v>66</v>
+      </c>
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="41"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B49" s="27">
+        <v>13</v>
+      </c>
+      <c r="B49" s="25">
         <v>0.05</v>
       </c>
-      <c r="C49" s="48"/>
-      <c r="D49" s="48"/>
-      <c r="E49" s="44"/>
-      <c r="F49" s="44"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B50" s="28"/>
-      <c r="C50" s="57"/>
-      <c r="D50" s="57"/>
+        <v>50</v>
+      </c>
+      <c r="B50" s="26"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="50"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B51" s="28"/>
-      <c r="C51" s="57"/>
-      <c r="D51" s="57"/>
+        <v>63</v>
+      </c>
+      <c r="B51" s="26"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B52" s="28"/>
-      <c r="C52" s="57"/>
-      <c r="D52" s="57"/>
+        <v>11</v>
+      </c>
+      <c r="B52" s="26"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="50"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B53" s="28"/>
-      <c r="C53" s="57"/>
-      <c r="D53" s="57"/>
+        <v>12</v>
+      </c>
+      <c r="B53" s="26"/>
+      <c r="C53" s="50"/>
+      <c r="D53" s="50"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B54" s="29"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="58"/>
+        <v>90</v>
+      </c>
+      <c r="B54" s="27"/>
+      <c r="C54" s="51"/>
+      <c r="D54" s="51"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B55" s="29"/>
-      <c r="C55" s="58"/>
-      <c r="D55" s="58"/>
+        <v>91</v>
+      </c>
+      <c r="B55" s="27"/>
+      <c r="C55" s="51"/>
+      <c r="D55" s="51"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B56" s="29"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="58"/>
+        <v>92</v>
+      </c>
+      <c r="B56" s="27"/>
+      <c r="C56" s="51"/>
+      <c r="D56" s="51"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="28"/>
-      <c r="C57" s="57"/>
-      <c r="D57" s="57"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="50"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B58" s="28"/>
-      <c r="C58" s="57"/>
-      <c r="D58" s="57"/>
+        <v>9</v>
+      </c>
+      <c r="B58" s="26"/>
+      <c r="C58" s="50"/>
+      <c r="D58" s="50"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B59" s="28"/>
-      <c r="C59" s="57"/>
-      <c r="D59" s="57"/>
+        <v>106</v>
+      </c>
+      <c r="B59" s="26"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="50"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B60" s="28"/>
-      <c r="C60" s="57"/>
-      <c r="D60" s="57"/>
+        <v>11</v>
+      </c>
+      <c r="B60" s="26"/>
+      <c r="C60" s="50"/>
+      <c r="D60" s="50"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B61" s="28"/>
-      <c r="C61" s="57"/>
-      <c r="D61" s="57"/>
-      <c r="E61" s="64"/>
-      <c r="F61" s="64"/>
-      <c r="G61" s="64"/>
+        <v>12</v>
+      </c>
+      <c r="B61" s="26"/>
+      <c r="C61" s="50"/>
+      <c r="D61" s="50"/>
+      <c r="E61" s="56"/>
+      <c r="F61" s="56"/>
+      <c r="G61" s="56"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B62" s="28"/>
-      <c r="C62" s="57"/>
-      <c r="D62" s="57"/>
-      <c r="E62" s="64"/>
-      <c r="F62" s="64"/>
-      <c r="G62" s="64"/>
+        <v>8</v>
+      </c>
+      <c r="B62" s="26"/>
+      <c r="C62" s="50"/>
+      <c r="D62" s="50"/>
+      <c r="E62" s="56"/>
+      <c r="F62" s="56"/>
+      <c r="G62" s="56"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B63" s="28"/>
-      <c r="C63" s="57"/>
-      <c r="D63" s="57"/>
-      <c r="E63" s="64"/>
-      <c r="F63" s="64"/>
-      <c r="G63" s="64"/>
+        <v>87</v>
+      </c>
+      <c r="B63" s="26"/>
+      <c r="C63" s="50"/>
+      <c r="D63" s="50"/>
+      <c r="E63" s="56"/>
+      <c r="F63" s="56"/>
+      <c r="G63" s="56"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B64" s="28"/>
-      <c r="C64" s="57"/>
-      <c r="D64" s="57"/>
-      <c r="E64" s="64"/>
-      <c r="F64" s="64"/>
-      <c r="G64" s="64"/>
+        <v>88</v>
+      </c>
+      <c r="B64" s="26"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="56"/>
+      <c r="F64" s="56"/>
+      <c r="G64" s="56"/>
     </row>
     <row r="65" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B65" s="28"/>
-      <c r="C65" s="57"/>
-      <c r="D65" s="57"/>
-      <c r="E65" s="64"/>
-      <c r="F65" s="64"/>
-      <c r="G65" s="64"/>
+        <v>89</v>
+      </c>
+      <c r="B65" s="26"/>
+      <c r="C65" s="50"/>
+      <c r="D65" s="50"/>
+      <c r="E65" s="56"/>
+      <c r="F65" s="56"/>
+      <c r="G65" s="56"/>
     </row>
     <row r="66" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B66" s="63"/>
-      <c r="C66" s="65"/>
-      <c r="D66" s="65"/>
-      <c r="E66" s="66"/>
-      <c r="F66" s="67"/>
-      <c r="G66" s="67"/>
+        <v>103</v>
+      </c>
+      <c r="B66" s="55"/>
+      <c r="C66" s="57"/>
+      <c r="D66" s="57"/>
+      <c r="E66" s="58"/>
+      <c r="F66" s="59"/>
+      <c r="G66" s="59"/>
       <c r="H66"/>
       <c r="I66"/>
     </row>
     <row r="67" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B67" s="63"/>
-      <c r="C67" s="65"/>
-      <c r="D67" s="65"/>
-      <c r="E67" s="66"/>
-      <c r="F67" s="67"/>
-      <c r="G67" s="67"/>
+        <v>104</v>
+      </c>
+      <c r="B67" s="55"/>
+      <c r="C67" s="57"/>
+      <c r="D67" s="57"/>
+      <c r="E67" s="58"/>
+      <c r="F67" s="59"/>
+      <c r="G67" s="59"/>
       <c r="H67"/>
       <c r="I67"/>
     </row>
     <row r="68" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B68" s="63"/>
-      <c r="C68" s="65"/>
-      <c r="D68" s="65"/>
-      <c r="E68" s="66"/>
-      <c r="F68" s="67"/>
-      <c r="G68" s="67"/>
+        <v>105</v>
+      </c>
+      <c r="B68" s="55"/>
+      <c r="C68" s="57"/>
+      <c r="D68" s="57"/>
+      <c r="E68" s="58"/>
+      <c r="F68" s="59"/>
+      <c r="G68" s="59"/>
       <c r="H68"/>
       <c r="I68"/>
     </row>
     <row r="69" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B69" s="28"/>
-      <c r="C69" s="57"/>
-      <c r="D69" s="57"/>
-      <c r="E69" s="64"/>
-      <c r="F69" s="64"/>
-      <c r="G69" s="64"/>
+        <v>95</v>
+      </c>
+      <c r="B69" s="26"/>
+      <c r="C69" s="50"/>
+      <c r="D69" s="50"/>
+      <c r="E69" s="56"/>
+      <c r="F69" s="56"/>
+      <c r="G69" s="56"/>
     </row>
     <row r="70" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B70" s="28"/>
-      <c r="C70" s="57"/>
-      <c r="D70" s="57"/>
-      <c r="E70" s="64"/>
-      <c r="F70" s="64"/>
-      <c r="G70" s="64"/>
+        <v>94</v>
+      </c>
+      <c r="B70" s="26"/>
+      <c r="C70" s="50"/>
+      <c r="D70" s="50"/>
+      <c r="E70" s="56"/>
+      <c r="F70" s="56"/>
+      <c r="G70" s="56"/>
     </row>
     <row r="71" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B71" s="30"/>
-      <c r="C71" s="57"/>
-      <c r="D71" s="57"/>
-      <c r="E71" s="64"/>
-      <c r="F71" s="64"/>
-      <c r="G71" s="64"/>
+        <v>67</v>
+      </c>
+      <c r="B71" s="28"/>
+      <c r="C71" s="50"/>
+      <c r="D71" s="50"/>
+      <c r="E71" s="56"/>
+      <c r="F71" s="56"/>
+      <c r="G71" s="56"/>
     </row>
     <row r="72" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B72" s="31"/>
-      <c r="C72" s="57"/>
-      <c r="D72" s="57"/>
-      <c r="E72" s="64"/>
-      <c r="F72" s="64"/>
-      <c r="G72" s="64"/>
+        <v>51</v>
+      </c>
+      <c r="B72" s="29"/>
+      <c r="C72" s="50"/>
+      <c r="D72" s="50"/>
+      <c r="E72" s="56"/>
+      <c r="F72" s="56"/>
+      <c r="G72" s="56"/>
     </row>
     <row r="73" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B73" s="32"/>
-      <c r="C73" s="57"/>
-      <c r="D73" s="57"/>
-      <c r="E73" s="64"/>
-      <c r="F73" s="64"/>
-      <c r="G73" s="64"/>
+        <v>52</v>
+      </c>
+      <c r="B73" s="30"/>
+      <c r="C73" s="50"/>
+      <c r="D73" s="50"/>
+      <c r="E73" s="56"/>
+      <c r="F73" s="56"/>
+      <c r="G73" s="56"/>
     </row>
     <row r="74" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B74" s="33"/>
-      <c r="C74" s="57"/>
-      <c r="D74" s="57"/>
-      <c r="E74" s="48"/>
-      <c r="F74" s="48"/>
-      <c r="G74" s="48"/>
-      <c r="H74" s="44"/>
-      <c r="I74" s="44"/>
+      <c r="B74" s="31"/>
+      <c r="C74" s="50"/>
+      <c r="D74" s="50"/>
+      <c r="E74" s="41"/>
+      <c r="F74" s="41"/>
+      <c r="G74" s="41"/>
+      <c r="H74" s="37"/>
+      <c r="I74" s="37"/>
       <c r="J74" s="15"/>
       <c r="K74" s="15"/>
       <c r="L74" s="15"/>
@@ -3267,14 +3227,14 @@
       <c r="A75" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B75" s="33"/>
-      <c r="C75" s="57"/>
-      <c r="D75" s="57"/>
-      <c r="E75" s="48"/>
-      <c r="F75" s="48"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="44"/>
-      <c r="I75" s="44"/>
+      <c r="B75" s="31"/>
+      <c r="C75" s="50"/>
+      <c r="D75" s="50"/>
+      <c r="E75" s="41"/>
+      <c r="F75" s="41"/>
+      <c r="G75" s="41"/>
+      <c r="H75" s="37"/>
+      <c r="I75" s="37"/>
       <c r="J75" s="15"/>
       <c r="K75" s="15"/>
       <c r="L75" s="15"/>
@@ -3335,18 +3295,18 @@
       <c r="BO75" s="15"/>
       <c r="BP75" s="15"/>
     </row>
-    <row r="76" spans="1:68" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="B76" s="34"/>
-      <c r="C76" s="57"/>
-      <c r="D76" s="57"/>
-      <c r="E76" s="48"/>
-      <c r="F76" s="48"/>
-      <c r="G76" s="48"/>
-      <c r="H76" s="44"/>
-      <c r="I76" s="44"/>
+    <row r="76" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A76" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76" s="66"/>
+      <c r="C76" s="41"/>
+      <c r="D76" s="41"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="37"/>
+      <c r="G76" s="37"/>
+      <c r="H76" s="37"/>
+      <c r="I76" s="37"/>
       <c r="J76" s="15"/>
       <c r="K76" s="15"/>
       <c r="L76" s="15"/>
@@ -3407,925 +3367,669 @@
       <c r="BO76" s="15"/>
       <c r="BP76" s="15"/>
     </row>
-    <row r="77" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B77" s="33"/>
-      <c r="C77" s="57"/>
-      <c r="D77" s="57"/>
-      <c r="E77" s="44"/>
-      <c r="F77" s="44"/>
-      <c r="G77" s="44"/>
-      <c r="H77" s="44"/>
-      <c r="I77" s="44"/>
-    </row>
-    <row r="78" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="11" t="s">
-        <v>65</v>
+        <v>4</v>
+      </c>
+      <c r="B77" s="32"/>
+      <c r="C77" s="41"/>
+      <c r="D77" s="41"/>
+      <c r="E77" s="37"/>
+      <c r="F77" s="37"/>
+      <c r="G77" s="37"/>
+      <c r="H77" s="37"/>
+      <c r="I77" s="37"/>
+      <c r="J77" s="15"/>
+      <c r="K77" s="15"/>
+      <c r="L77" s="15"/>
+      <c r="M77" s="15"/>
+      <c r="N77" s="15"/>
+      <c r="O77" s="15"/>
+      <c r="P77" s="15"/>
+      <c r="Q77" s="15"/>
+      <c r="R77" s="15"/>
+      <c r="S77" s="15"/>
+      <c r="T77" s="15"/>
+      <c r="U77" s="15"/>
+      <c r="V77" s="15"/>
+      <c r="W77" s="15"/>
+      <c r="X77" s="15"/>
+      <c r="Y77" s="15"/>
+      <c r="Z77" s="15"/>
+      <c r="AA77" s="15"/>
+      <c r="AB77" s="15"/>
+      <c r="AC77" s="15"/>
+      <c r="AD77" s="15"/>
+      <c r="AE77" s="15"/>
+      <c r="AF77" s="15"/>
+      <c r="AG77" s="15"/>
+      <c r="AH77" s="15"/>
+      <c r="AI77" s="15"/>
+      <c r="AJ77" s="15"/>
+      <c r="AK77" s="15"/>
+      <c r="AL77" s="15"/>
+      <c r="AM77" s="15"/>
+      <c r="AN77" s="15"/>
+      <c r="AO77" s="15"/>
+      <c r="AP77" s="15"/>
+      <c r="AQ77" s="15"/>
+      <c r="AR77" s="15"/>
+      <c r="AS77" s="15"/>
+      <c r="AT77" s="15"/>
+      <c r="AU77" s="15"/>
+      <c r="AV77" s="15"/>
+      <c r="AW77" s="15"/>
+      <c r="AX77" s="15"/>
+      <c r="AY77" s="15"/>
+      <c r="AZ77" s="15"/>
+      <c r="BA77" s="15"/>
+      <c r="BB77" s="15"/>
+      <c r="BC77" s="15"/>
+      <c r="BD77" s="15"/>
+      <c r="BE77" s="15"/>
+      <c r="BF77" s="15"/>
+      <c r="BG77" s="15"/>
+      <c r="BH77" s="15"/>
+      <c r="BI77" s="15"/>
+      <c r="BJ77" s="15"/>
+      <c r="BK77" s="15"/>
+      <c r="BL77" s="15"/>
+      <c r="BM77" s="15"/>
+      <c r="BN77" s="15"/>
+      <c r="BO77" s="15"/>
+      <c r="BP77" s="15"/>
+    </row>
+    <row r="78" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A78" s="12" t="s">
+        <v>5</v>
       </c>
       <c r="B78" s="33"/>
-      <c r="C78" s="57"/>
-      <c r="D78" s="57"/>
-      <c r="E78" s="44"/>
-      <c r="F78" s="44"/>
-      <c r="G78" s="44"/>
-      <c r="H78" s="44"/>
-      <c r="I78" s="44"/>
-    </row>
-    <row r="79" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B79" s="33"/>
-      <c r="C79" s="57"/>
-      <c r="D79" s="57"/>
-      <c r="E79" s="44"/>
-      <c r="F79" s="44"/>
-      <c r="G79" s="44"/>
-      <c r="H79" s="44"/>
-      <c r="I79" s="44"/>
-    </row>
-    <row r="80" spans="1:68" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="12" t="s">
-        <v>62</v>
+      <c r="C78" s="41"/>
+      <c r="D78" s="41"/>
+      <c r="E78" s="37"/>
+      <c r="F78" s="37"/>
+      <c r="G78" s="37"/>
+      <c r="H78" s="37"/>
+      <c r="I78" s="37"/>
+      <c r="J78" s="15"/>
+      <c r="K78" s="15"/>
+      <c r="L78" s="15"/>
+      <c r="M78" s="15"/>
+      <c r="N78" s="15"/>
+      <c r="O78" s="15"/>
+      <c r="P78" s="15"/>
+      <c r="Q78" s="15"/>
+      <c r="R78" s="15"/>
+      <c r="S78" s="15"/>
+      <c r="T78" s="15"/>
+      <c r="U78" s="15"/>
+      <c r="V78" s="15"/>
+      <c r="W78" s="15"/>
+      <c r="X78" s="15"/>
+      <c r="Y78" s="15"/>
+      <c r="Z78" s="15"/>
+      <c r="AA78" s="15"/>
+      <c r="AB78" s="15"/>
+      <c r="AC78" s="15"/>
+      <c r="AD78" s="15"/>
+      <c r="AE78" s="15"/>
+      <c r="AF78" s="15"/>
+      <c r="AG78" s="15"/>
+      <c r="AH78" s="15"/>
+      <c r="AI78" s="15"/>
+      <c r="AJ78" s="15"/>
+      <c r="AK78" s="15"/>
+      <c r="AL78" s="15"/>
+      <c r="AM78" s="15"/>
+      <c r="AN78" s="15"/>
+      <c r="AO78" s="15"/>
+      <c r="AP78" s="15"/>
+      <c r="AQ78" s="15"/>
+      <c r="AR78" s="15"/>
+      <c r="AS78" s="15"/>
+      <c r="AT78" s="15"/>
+      <c r="AU78" s="15"/>
+      <c r="AV78" s="15"/>
+      <c r="AW78" s="15"/>
+      <c r="AX78" s="15"/>
+      <c r="AY78" s="15"/>
+      <c r="AZ78" s="15"/>
+      <c r="BA78" s="15"/>
+      <c r="BB78" s="15"/>
+      <c r="BC78" s="15"/>
+      <c r="BD78" s="15"/>
+      <c r="BE78" s="15"/>
+      <c r="BF78" s="15"/>
+      <c r="BG78" s="15"/>
+      <c r="BH78" s="15"/>
+      <c r="BI78" s="15"/>
+      <c r="BJ78" s="15"/>
+      <c r="BK78" s="15"/>
+      <c r="BL78" s="15"/>
+      <c r="BM78" s="15"/>
+      <c r="BN78" s="15"/>
+      <c r="BO78" s="15"/>
+      <c r="BP78" s="15"/>
+    </row>
+    <row r="79" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A79" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B79" s="34"/>
+      <c r="C79" s="52"/>
+      <c r="D79" s="52"/>
+    </row>
+    <row r="80" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A80" s="17" t="s">
+        <v>10</v>
       </c>
       <c r="B80" s="35"/>
-      <c r="C80" s="57"/>
-      <c r="D80" s="57"/>
-      <c r="E80" s="44"/>
-      <c r="F80" s="44"/>
-      <c r="G80" s="44"/>
+      <c r="C80" s="35"/>
+      <c r="D80" s="35"/>
+      <c r="E80" s="43"/>
+      <c r="F80" s="43"/>
+      <c r="G80" s="43"/>
       <c r="H80" s="44"/>
-      <c r="I80" s="44"/>
-      <c r="J80" s="15"/>
-      <c r="K80" s="15"/>
-      <c r="L80" s="15"/>
-      <c r="M80" s="15"/>
-      <c r="N80" s="15"/>
-      <c r="O80" s="15"/>
-      <c r="P80" s="15"/>
-      <c r="Q80" s="15"/>
-      <c r="R80" s="15"/>
-      <c r="S80" s="15"/>
-      <c r="T80" s="15"/>
-      <c r="U80" s="15"/>
-      <c r="V80" s="15"/>
-      <c r="W80" s="15"/>
-      <c r="X80" s="15"/>
-      <c r="Y80" s="15"/>
-      <c r="Z80" s="15"/>
-      <c r="AA80" s="15"/>
-      <c r="AB80" s="15"/>
-      <c r="AC80" s="15"/>
-      <c r="AD80" s="15"/>
-      <c r="AE80" s="15"/>
-      <c r="AF80" s="15"/>
-      <c r="AG80" s="15"/>
-      <c r="AH80" s="15"/>
-      <c r="AI80" s="15"/>
-      <c r="AJ80" s="15"/>
-      <c r="AK80" s="15"/>
-      <c r="AL80" s="15"/>
-      <c r="AM80" s="15"/>
-      <c r="AN80" s="15"/>
-      <c r="AO80" s="15"/>
-      <c r="AP80" s="15"/>
-      <c r="AQ80" s="15"/>
-      <c r="AR80" s="15"/>
-      <c r="AS80" s="15"/>
-      <c r="AT80" s="15"/>
-      <c r="AU80" s="15"/>
-      <c r="AV80" s="15"/>
-      <c r="AW80" s="15"/>
-      <c r="AX80" s="15"/>
-      <c r="AY80" s="15"/>
-      <c r="AZ80" s="15"/>
-      <c r="BA80" s="15"/>
-      <c r="BB80" s="15"/>
-      <c r="BC80" s="15"/>
-      <c r="BD80" s="15"/>
-      <c r="BE80" s="15"/>
-      <c r="BF80" s="15"/>
-      <c r="BG80" s="15"/>
-      <c r="BH80" s="15"/>
-      <c r="BI80" s="15"/>
-      <c r="BJ80" s="15"/>
-      <c r="BK80" s="15"/>
-      <c r="BL80" s="15"/>
-      <c r="BM80" s="15"/>
-      <c r="BN80" s="15"/>
-      <c r="BO80" s="15"/>
-      <c r="BP80" s="15"/>
-    </row>
-    <row r="81" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B81" s="36"/>
-      <c r="C81" s="59"/>
-      <c r="D81" s="59"/>
-      <c r="E81" s="44"/>
-      <c r="F81" s="44"/>
-      <c r="G81" s="44"/>
-      <c r="H81" s="44"/>
-      <c r="I81" s="44"/>
-    </row>
-    <row r="82" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="11" t="s">
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" s="36">
+        <v>5</v>
+      </c>
+      <c r="C81" s="36">
+        <v>15</v>
+      </c>
+      <c r="D81" s="36"/>
+      <c r="E81" s="36"/>
+      <c r="F81" s="36"/>
+      <c r="G81" s="36"/>
+      <c r="H81" s="45"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="B82" s="36"/>
-      <c r="C82" s="59"/>
-      <c r="D82" s="59"/>
-      <c r="E82" s="44"/>
-      <c r="F82" s="44"/>
-      <c r="G82" s="44"/>
-      <c r="H82" s="44"/>
-      <c r="I82" s="44"/>
-    </row>
-    <row r="83" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="11" t="s">
+      <c r="B82" s="60"/>
+      <c r="C82" s="64"/>
+      <c r="D82" s="64"/>
+      <c r="E82" s="64"/>
+      <c r="F82" s="64"/>
+      <c r="G82"/>
+      <c r="H82"/>
+      <c r="I82"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="47" t="s">
         <v>69</v>
       </c>
-      <c r="B83" s="36"/>
-      <c r="C83" s="59"/>
-      <c r="D83" s="59"/>
-      <c r="E83" s="44"/>
-      <c r="F83" s="44"/>
-      <c r="G83" s="44"/>
-      <c r="H83" s="44"/>
-      <c r="I83" s="44"/>
-    </row>
-    <row r="84" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="11" t="s">
+      <c r="B83" s="47"/>
+      <c r="C83" s="63"/>
+      <c r="D83" s="63"/>
+      <c r="E83" s="64"/>
+      <c r="F83" s="64"/>
+      <c r="G83"/>
+      <c r="H83"/>
+      <c r="I83"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="B84" s="47"/>
+      <c r="C84" s="64"/>
+      <c r="D84" s="64"/>
+      <c r="E84" s="64"/>
+      <c r="F84" s="64"/>
+      <c r="G84"/>
+      <c r="H84"/>
+      <c r="I84"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="B85" s="47"/>
+      <c r="C85" s="64"/>
+      <c r="D85" s="64"/>
+      <c r="E85" s="64"/>
+      <c r="F85" s="64"/>
+      <c r="G85"/>
+      <c r="H85"/>
+      <c r="I85"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="B86" s="47"/>
+      <c r="C86" s="64"/>
+      <c r="D86" s="64"/>
+      <c r="E86" s="64"/>
+      <c r="F86" s="64"/>
+      <c r="G86"/>
+      <c r="H86"/>
+      <c r="I86"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="B87" s="47"/>
+      <c r="C87" s="64"/>
+      <c r="D87" s="64"/>
+      <c r="E87" s="64"/>
+      <c r="F87" s="64"/>
+      <c r="G87"/>
+      <c r="H87"/>
+      <c r="I87"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="B84" s="36"/>
-      <c r="C84" s="59"/>
-      <c r="D84" s="59"/>
-      <c r="E84" s="44"/>
-      <c r="F84" s="44"/>
-      <c r="G84" s="44"/>
-      <c r="H84" s="44"/>
-      <c r="I84" s="44"/>
-    </row>
-    <row r="85" spans="1:68" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="12" t="s">
+      <c r="B88" s="47"/>
+      <c r="C88" s="63"/>
+      <c r="D88" s="63"/>
+      <c r="E88" s="64"/>
+      <c r="F88" s="64"/>
+      <c r="G88"/>
+      <c r="H88"/>
+      <c r="I88"/>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B89" s="47"/>
+      <c r="C89" s="64"/>
+      <c r="D89" s="64"/>
+      <c r="E89" s="64"/>
+      <c r="F89" s="64"/>
+      <c r="G89"/>
+      <c r="H89"/>
+      <c r="I89"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="B90" s="47"/>
+      <c r="C90" s="64"/>
+      <c r="D90" s="64"/>
+      <c r="E90" s="64"/>
+      <c r="F90" s="64"/>
+      <c r="G90"/>
+      <c r="H90"/>
+      <c r="I90"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="B91" s="47"/>
+      <c r="C91" s="64"/>
+      <c r="D91" s="64"/>
+      <c r="E91" s="64"/>
+      <c r="F91" s="64"/>
+      <c r="G91"/>
+      <c r="H91"/>
+      <c r="I91"/>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B92" s="47"/>
+      <c r="C92" s="64"/>
+      <c r="D92" s="64"/>
+      <c r="E92" s="64"/>
+      <c r="F92" s="64"/>
+      <c r="G92"/>
+      <c r="H92"/>
+      <c r="I92"/>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="B85" s="37"/>
-      <c r="C85" s="59"/>
-      <c r="D85" s="59"/>
-      <c r="E85" s="44"/>
-      <c r="F85" s="44"/>
-      <c r="G85" s="44"/>
-      <c r="H85" s="44"/>
-      <c r="I85" s="44"/>
-    </row>
-    <row r="86" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A86" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B86" s="38"/>
-      <c r="C86" s="48"/>
-      <c r="D86" s="48"/>
-      <c r="E86" s="44"/>
-      <c r="F86" s="44"/>
-      <c r="G86" s="44"/>
-      <c r="H86" s="44"/>
-      <c r="I86" s="44"/>
-      <c r="J86" s="15"/>
-      <c r="K86" s="15"/>
-      <c r="L86" s="15"/>
-      <c r="M86" s="15"/>
-      <c r="N86" s="15"/>
-      <c r="O86" s="15"/>
-      <c r="P86" s="15"/>
-      <c r="Q86" s="15"/>
-      <c r="R86" s="15"/>
-      <c r="S86" s="15"/>
-      <c r="T86" s="15"/>
-      <c r="U86" s="15"/>
-      <c r="V86" s="15"/>
-      <c r="W86" s="15"/>
-      <c r="X86" s="15"/>
-      <c r="Y86" s="15"/>
-      <c r="Z86" s="15"/>
-      <c r="AA86" s="15"/>
-      <c r="AB86" s="15"/>
-      <c r="AC86" s="15"/>
-      <c r="AD86" s="15"/>
-      <c r="AE86" s="15"/>
-      <c r="AF86" s="15"/>
-      <c r="AG86" s="15"/>
-      <c r="AH86" s="15"/>
-      <c r="AI86" s="15"/>
-      <c r="AJ86" s="15"/>
-      <c r="AK86" s="15"/>
-      <c r="AL86" s="15"/>
-      <c r="AM86" s="15"/>
-      <c r="AN86" s="15"/>
-      <c r="AO86" s="15"/>
-      <c r="AP86" s="15"/>
-      <c r="AQ86" s="15"/>
-      <c r="AR86" s="15"/>
-      <c r="AS86" s="15"/>
-      <c r="AT86" s="15"/>
-      <c r="AU86" s="15"/>
-      <c r="AV86" s="15"/>
-      <c r="AW86" s="15"/>
-      <c r="AX86" s="15"/>
-      <c r="AY86" s="15"/>
-      <c r="AZ86" s="15"/>
-      <c r="BA86" s="15"/>
-      <c r="BB86" s="15"/>
-      <c r="BC86" s="15"/>
-      <c r="BD86" s="15"/>
-      <c r="BE86" s="15"/>
-      <c r="BF86" s="15"/>
-      <c r="BG86" s="15"/>
-      <c r="BH86" s="15"/>
-      <c r="BI86" s="15"/>
-      <c r="BJ86" s="15"/>
-      <c r="BK86" s="15"/>
-      <c r="BL86" s="15"/>
-      <c r="BM86" s="15"/>
-      <c r="BN86" s="15"/>
-      <c r="BO86" s="15"/>
-      <c r="BP86" s="15"/>
-    </row>
-    <row r="87" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A87" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B87" s="38"/>
-      <c r="C87" s="48"/>
-      <c r="D87" s="48"/>
-      <c r="E87" s="44"/>
-      <c r="F87" s="44"/>
-      <c r="G87" s="44"/>
-      <c r="H87" s="44"/>
-      <c r="I87" s="44"/>
-      <c r="J87" s="15"/>
-      <c r="K87" s="15"/>
-      <c r="L87" s="15"/>
-      <c r="M87" s="15"/>
-      <c r="N87" s="15"/>
-      <c r="O87" s="15"/>
-      <c r="P87" s="15"/>
-      <c r="Q87" s="15"/>
-      <c r="R87" s="15"/>
-      <c r="S87" s="15"/>
-      <c r="T87" s="15"/>
-      <c r="U87" s="15"/>
-      <c r="V87" s="15"/>
-      <c r="W87" s="15"/>
-      <c r="X87" s="15"/>
-      <c r="Y87" s="15"/>
-      <c r="Z87" s="15"/>
-      <c r="AA87" s="15"/>
-      <c r="AB87" s="15"/>
-      <c r="AC87" s="15"/>
-      <c r="AD87" s="15"/>
-      <c r="AE87" s="15"/>
-      <c r="AF87" s="15"/>
-      <c r="AG87" s="15"/>
-      <c r="AH87" s="15"/>
-      <c r="AI87" s="15"/>
-      <c r="AJ87" s="15"/>
-      <c r="AK87" s="15"/>
-      <c r="AL87" s="15"/>
-      <c r="AM87" s="15"/>
-      <c r="AN87" s="15"/>
-      <c r="AO87" s="15"/>
-      <c r="AP87" s="15"/>
-      <c r="AQ87" s="15"/>
-      <c r="AR87" s="15"/>
-      <c r="AS87" s="15"/>
-      <c r="AT87" s="15"/>
-      <c r="AU87" s="15"/>
-      <c r="AV87" s="15"/>
-      <c r="AW87" s="15"/>
-      <c r="AX87" s="15"/>
-      <c r="AY87" s="15"/>
-      <c r="AZ87" s="15"/>
-      <c r="BA87" s="15"/>
-      <c r="BB87" s="15"/>
-      <c r="BC87" s="15"/>
-      <c r="BD87" s="15"/>
-      <c r="BE87" s="15"/>
-      <c r="BF87" s="15"/>
-      <c r="BG87" s="15"/>
-      <c r="BH87" s="15"/>
-      <c r="BI87" s="15"/>
-      <c r="BJ87" s="15"/>
-      <c r="BK87" s="15"/>
-      <c r="BL87" s="15"/>
-      <c r="BM87" s="15"/>
-      <c r="BN87" s="15"/>
-      <c r="BO87" s="15"/>
-      <c r="BP87" s="15"/>
-    </row>
-    <row r="88" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A88" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B88" s="39"/>
-      <c r="C88" s="48"/>
-      <c r="D88" s="48"/>
-      <c r="E88" s="44"/>
-      <c r="F88" s="44"/>
-      <c r="G88" s="44"/>
-      <c r="H88" s="44"/>
-      <c r="I88" s="44"/>
-      <c r="J88" s="15"/>
-      <c r="K88" s="15"/>
-      <c r="L88" s="15"/>
-      <c r="M88" s="15"/>
-      <c r="N88" s="15"/>
-      <c r="O88" s="15"/>
-      <c r="P88" s="15"/>
-      <c r="Q88" s="15"/>
-      <c r="R88" s="15"/>
-      <c r="S88" s="15"/>
-      <c r="T88" s="15"/>
-      <c r="U88" s="15"/>
-      <c r="V88" s="15"/>
-      <c r="W88" s="15"/>
-      <c r="X88" s="15"/>
-      <c r="Y88" s="15"/>
-      <c r="Z88" s="15"/>
-      <c r="AA88" s="15"/>
-      <c r="AB88" s="15"/>
-      <c r="AC88" s="15"/>
-      <c r="AD88" s="15"/>
-      <c r="AE88" s="15"/>
-      <c r="AF88" s="15"/>
-      <c r="AG88" s="15"/>
-      <c r="AH88" s="15"/>
-      <c r="AI88" s="15"/>
-      <c r="AJ88" s="15"/>
-      <c r="AK88" s="15"/>
-      <c r="AL88" s="15"/>
-      <c r="AM88" s="15"/>
-      <c r="AN88" s="15"/>
-      <c r="AO88" s="15"/>
-      <c r="AP88" s="15"/>
-      <c r="AQ88" s="15"/>
-      <c r="AR88" s="15"/>
-      <c r="AS88" s="15"/>
-      <c r="AT88" s="15"/>
-      <c r="AU88" s="15"/>
-      <c r="AV88" s="15"/>
-      <c r="AW88" s="15"/>
-      <c r="AX88" s="15"/>
-      <c r="AY88" s="15"/>
-      <c r="AZ88" s="15"/>
-      <c r="BA88" s="15"/>
-      <c r="BB88" s="15"/>
-      <c r="BC88" s="15"/>
-      <c r="BD88" s="15"/>
-      <c r="BE88" s="15"/>
-      <c r="BF88" s="15"/>
-      <c r="BG88" s="15"/>
-      <c r="BH88" s="15"/>
-      <c r="BI88" s="15"/>
-      <c r="BJ88" s="15"/>
-      <c r="BK88" s="15"/>
-      <c r="BL88" s="15"/>
-      <c r="BM88" s="15"/>
-      <c r="BN88" s="15"/>
-      <c r="BO88" s="15"/>
-      <c r="BP88" s="15"/>
-    </row>
-    <row r="89" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A89" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B89" s="40"/>
-      <c r="C89" s="48"/>
-      <c r="D89" s="48"/>
-    </row>
-    <row r="90" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A90" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B90" s="41"/>
-      <c r="C90" s="60"/>
-      <c r="D90" s="60"/>
-    </row>
-    <row r="91" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A91" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B91" s="42"/>
-      <c r="C91" s="42"/>
-      <c r="D91" s="42"/>
-      <c r="E91" s="50"/>
-      <c r="F91" s="50"/>
-      <c r="G91" s="50"/>
-      <c r="H91" s="51"/>
-    </row>
-    <row r="92" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A92" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B92" s="43">
-        <v>5</v>
-      </c>
-      <c r="C92" s="43">
-        <v>15</v>
-      </c>
-      <c r="D92" s="43"/>
-      <c r="E92" s="43"/>
-      <c r="F92" s="43"/>
-      <c r="G92" s="43"/>
-      <c r="H92" s="52"/>
-    </row>
-    <row r="93" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A93" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="B93" s="68"/>
-      <c r="C93" s="72"/>
-      <c r="D93" s="72"/>
-      <c r="E93" s="72"/>
-      <c r="F93" s="72"/>
+      <c r="B93" s="61"/>
+      <c r="C93" s="64"/>
+      <c r="D93" s="64"/>
+      <c r="E93" s="64"/>
+      <c r="F93" s="64"/>
       <c r="G93"/>
       <c r="H93"/>
       <c r="I93"/>
     </row>
-    <row r="94" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A94" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="B94" s="54"/>
-      <c r="C94" s="71"/>
-      <c r="D94" s="71"/>
-      <c r="E94" s="72"/>
-      <c r="F94" s="72"/>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B94" s="61"/>
+      <c r="C94" s="64"/>
+      <c r="D94" s="64"/>
+      <c r="E94" s="64"/>
+      <c r="F94" s="64"/>
       <c r="G94"/>
       <c r="H94"/>
       <c r="I94"/>
     </row>
-    <row r="95" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A95" s="54" t="s">
-        <v>86</v>
-      </c>
-      <c r="B95" s="54"/>
-      <c r="C95" s="72"/>
-      <c r="D95" s="72"/>
-      <c r="E95" s="72"/>
-      <c r="F95" s="72"/>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="B95" s="61"/>
+      <c r="C95" s="64"/>
+      <c r="D95" s="64"/>
+      <c r="E95" s="64"/>
+      <c r="F95" s="64"/>
       <c r="G95"/>
       <c r="H95"/>
       <c r="I95"/>
     </row>
-    <row r="96" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A96" s="54" t="s">
-        <v>118</v>
-      </c>
-      <c r="B96" s="54"/>
-      <c r="C96" s="72"/>
-      <c r="D96" s="72"/>
-      <c r="E96" s="72"/>
-      <c r="F96" s="72"/>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="B96" s="61"/>
+      <c r="C96" s="64"/>
+      <c r="D96" s="64"/>
+      <c r="E96" s="64"/>
+      <c r="F96" s="64"/>
       <c r="G96"/>
       <c r="H96"/>
       <c r="I96"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="54" t="s">
-        <v>126</v>
-      </c>
-      <c r="B97" s="54"/>
-      <c r="C97" s="72"/>
-      <c r="D97" s="72"/>
-      <c r="E97" s="72"/>
-      <c r="F97" s="72"/>
+      <c r="A97" s="48" t="s">
+        <v>80</v>
+      </c>
+      <c r="B97" s="61"/>
+      <c r="C97" s="64"/>
+      <c r="D97" s="64"/>
+      <c r="E97" s="64"/>
+      <c r="F97" s="64"/>
       <c r="G97"/>
       <c r="H97"/>
       <c r="I97"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="54" t="s">
-        <v>87</v>
-      </c>
-      <c r="B98" s="54"/>
-      <c r="C98" s="72"/>
-      <c r="D98" s="72"/>
-      <c r="E98" s="72"/>
-      <c r="F98" s="72"/>
+      <c r="A98" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="B98" s="61"/>
+      <c r="C98" s="64"/>
+      <c r="D98" s="64"/>
+      <c r="E98" s="64"/>
+      <c r="F98" s="64"/>
       <c r="G98"/>
       <c r="H98"/>
       <c r="I98"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="54" t="s">
+      <c r="A99" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="B99" s="54"/>
-      <c r="C99" s="71"/>
-      <c r="D99" s="71"/>
-      <c r="E99" s="72"/>
-      <c r="F99" s="72"/>
+      <c r="B99" s="61"/>
+      <c r="C99" s="64"/>
+      <c r="D99" s="64"/>
+      <c r="E99" s="64"/>
+      <c r="F99" s="64"/>
       <c r="G99"/>
       <c r="H99"/>
       <c r="I99"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="54" t="s">
-        <v>88</v>
-      </c>
-      <c r="B100" s="54"/>
-      <c r="C100" s="72"/>
-      <c r="D100" s="72"/>
-      <c r="E100" s="72"/>
-      <c r="F100" s="72"/>
+      <c r="A100" s="48" t="s">
+        <v>110</v>
+      </c>
+      <c r="B100" s="61"/>
+      <c r="C100" s="64"/>
+      <c r="D100" s="64"/>
+      <c r="E100" s="64"/>
+      <c r="F100" s="64"/>
       <c r="G100"/>
       <c r="H100"/>
       <c r="I100"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="54" t="s">
-        <v>119</v>
-      </c>
-      <c r="B101" s="54"/>
-      <c r="C101" s="72"/>
-      <c r="D101" s="72"/>
-      <c r="E101" s="72"/>
-      <c r="F101" s="72"/>
+      <c r="A101" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="B101" s="61"/>
+      <c r="C101" s="64"/>
+      <c r="D101" s="64"/>
+      <c r="E101" s="64"/>
+      <c r="F101" s="64"/>
       <c r="G101"/>
       <c r="H101"/>
       <c r="I101"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="B102" s="54"/>
-      <c r="C102" s="72"/>
-      <c r="D102" s="72"/>
-      <c r="E102" s="72"/>
-      <c r="F102" s="72"/>
+      <c r="A102" s="48" t="s">
+        <v>82</v>
+      </c>
+      <c r="B102" s="61"/>
+      <c r="C102" s="64"/>
+      <c r="D102" s="64"/>
+      <c r="E102" s="64"/>
+      <c r="F102" s="64"/>
       <c r="G102"/>
       <c r="H102"/>
       <c r="I102"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="54" t="s">
-        <v>89</v>
-      </c>
-      <c r="B103" s="54"/>
-      <c r="C103" s="72"/>
-      <c r="D103" s="72"/>
-      <c r="E103" s="72"/>
-      <c r="F103" s="72"/>
+      <c r="A103" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B103" s="61"/>
+      <c r="C103" s="64"/>
+      <c r="D103" s="64"/>
+      <c r="E103" s="64"/>
+      <c r="F103" s="64"/>
       <c r="G103"/>
       <c r="H103"/>
       <c r="I103"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="55" t="s">
-        <v>82</v>
-      </c>
-      <c r="B104" s="69"/>
-      <c r="C104" s="72"/>
-      <c r="D104" s="72"/>
-      <c r="E104" s="72"/>
-      <c r="F104" s="72"/>
+      <c r="A104" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="B104" s="61"/>
+      <c r="C104" s="64"/>
+      <c r="D104" s="64"/>
+      <c r="E104" s="65"/>
+      <c r="F104" s="64"/>
       <c r="G104"/>
       <c r="H104"/>
       <c r="I104"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="55" t="s">
-        <v>90</v>
-      </c>
-      <c r="B105" s="69"/>
-      <c r="C105" s="72"/>
-      <c r="D105" s="72"/>
-      <c r="E105" s="72"/>
-      <c r="F105" s="72"/>
+      <c r="A105" s="48" t="s">
+        <v>111</v>
+      </c>
+      <c r="B105" s="61"/>
+      <c r="C105" s="64"/>
+      <c r="D105" s="64"/>
+      <c r="E105" s="65"/>
+      <c r="F105" s="64"/>
       <c r="G105"/>
       <c r="H105"/>
       <c r="I105"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="55" t="s">
-        <v>120</v>
-      </c>
-      <c r="B106" s="69"/>
-      <c r="C106" s="72"/>
-      <c r="D106" s="72"/>
-      <c r="E106" s="72"/>
-      <c r="F106" s="72"/>
+      <c r="A106" s="47" t="s">
+        <v>119</v>
+      </c>
+      <c r="B106" s="61"/>
+      <c r="C106" s="64"/>
+      <c r="D106" s="64"/>
+      <c r="E106" s="64"/>
+      <c r="F106" s="64"/>
       <c r="G106"/>
       <c r="H106"/>
       <c r="I106"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="54" t="s">
-        <v>128</v>
-      </c>
-      <c r="B107" s="69"/>
-      <c r="C107" s="72"/>
-      <c r="D107" s="72"/>
-      <c r="E107" s="72"/>
-      <c r="F107" s="72"/>
+      <c r="A107" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="B107" s="61"/>
+      <c r="C107" s="64"/>
+      <c r="D107" s="64"/>
+      <c r="E107" s="64"/>
+      <c r="F107" s="64"/>
       <c r="G107"/>
       <c r="H107"/>
       <c r="I107"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="55" t="s">
-        <v>91</v>
-      </c>
-      <c r="B108" s="69"/>
-      <c r="C108" s="72"/>
-      <c r="D108" s="72"/>
-      <c r="E108" s="72"/>
-      <c r="F108" s="72"/>
+      <c r="A108" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="B108" s="47"/>
+      <c r="C108" s="64"/>
+      <c r="D108" s="64"/>
+      <c r="E108" s="64"/>
+      <c r="F108" s="64"/>
       <c r="G108"/>
       <c r="H108"/>
       <c r="I108"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="55" t="s">
-        <v>83</v>
-      </c>
-      <c r="B109" s="69"/>
-      <c r="C109" s="72"/>
-      <c r="D109" s="72"/>
-      <c r="E109" s="72"/>
-      <c r="F109" s="72"/>
+      <c r="A109" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="B109" s="47"/>
+      <c r="C109" s="64"/>
+      <c r="D109" s="64"/>
+      <c r="E109" s="64"/>
+      <c r="F109" s="64"/>
       <c r="G109"/>
       <c r="H109"/>
       <c r="I109"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="55" t="s">
-        <v>92</v>
-      </c>
-      <c r="B110" s="69"/>
-      <c r="C110" s="72"/>
-      <c r="D110" s="72"/>
-      <c r="E110" s="72"/>
-      <c r="F110" s="72"/>
+      <c r="A110" s="48" t="s">
+        <v>112</v>
+      </c>
+      <c r="B110" s="47"/>
+      <c r="C110" s="64"/>
+      <c r="D110" s="64"/>
+      <c r="E110" s="64"/>
+      <c r="F110" s="64"/>
       <c r="G110"/>
       <c r="H110"/>
       <c r="I110"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="55" t="s">
-        <v>121</v>
-      </c>
-      <c r="B111" s="69"/>
-      <c r="C111" s="72"/>
-      <c r="D111" s="72"/>
-      <c r="E111" s="72"/>
-      <c r="F111" s="72"/>
+      <c r="A111" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="B111" s="47"/>
+      <c r="C111" s="64"/>
+      <c r="D111" s="64"/>
+      <c r="E111" s="64"/>
+      <c r="F111" s="64"/>
       <c r="G111"/>
       <c r="H111"/>
       <c r="I111"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="54" t="s">
-        <v>129</v>
-      </c>
-      <c r="B112" s="69"/>
-      <c r="C112" s="72"/>
-      <c r="D112" s="72"/>
-      <c r="E112" s="72"/>
-      <c r="F112" s="72"/>
+      <c r="A112" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="B112" s="47"/>
+      <c r="C112" s="64"/>
+      <c r="D112" s="64"/>
+      <c r="E112" s="64"/>
+      <c r="F112" s="64"/>
       <c r="G112"/>
       <c r="H112"/>
       <c r="I112"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="55" t="s">
-        <v>93</v>
-      </c>
-      <c r="B113" s="69"/>
-      <c r="C113" s="72"/>
-      <c r="D113" s="72"/>
-      <c r="E113" s="72"/>
-      <c r="F113" s="72"/>
+      <c r="A113" s="48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B113" s="47"/>
+      <c r="C113" s="64"/>
+      <c r="D113" s="64"/>
+      <c r="E113" s="64"/>
+      <c r="F113" s="64"/>
       <c r="G113"/>
       <c r="H113"/>
       <c r="I113"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="55" t="s">
-        <v>84</v>
-      </c>
-      <c r="B114" s="69"/>
-      <c r="C114" s="72"/>
-      <c r="D114" s="72"/>
-      <c r="E114" s="72"/>
-      <c r="F114" s="72"/>
+      <c r="A114" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B114" s="47"/>
+      <c r="C114" s="64"/>
+      <c r="D114" s="64"/>
+      <c r="E114" s="64"/>
+      <c r="F114" s="64"/>
       <c r="G114"/>
       <c r="H114"/>
       <c r="I114"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="55" t="s">
-        <v>94</v>
-      </c>
-      <c r="B115" s="69"/>
-      <c r="C115" s="72"/>
-      <c r="D115" s="72"/>
-      <c r="E115" s="73"/>
-      <c r="F115" s="72"/>
+      <c r="A115" s="48" t="s">
+        <v>113</v>
+      </c>
+      <c r="B115" s="47"/>
+      <c r="C115" s="64"/>
+      <c r="D115" s="64"/>
+      <c r="E115" s="64"/>
+      <c r="F115" s="64"/>
       <c r="G115"/>
       <c r="H115"/>
       <c r="I115"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="55" t="s">
-        <v>122</v>
-      </c>
-      <c r="B116" s="69"/>
-      <c r="C116" s="72"/>
-      <c r="D116" s="72"/>
-      <c r="E116" s="73"/>
-      <c r="F116" s="72"/>
+      <c r="A116" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="B116" s="47"/>
+      <c r="C116" s="64"/>
+      <c r="D116" s="64"/>
+      <c r="E116" s="64"/>
+      <c r="F116" s="64"/>
       <c r="G116"/>
       <c r="H116"/>
       <c r="I116"/>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="54" t="s">
-        <v>130</v>
-      </c>
-      <c r="B117" s="69"/>
-      <c r="C117" s="72"/>
-      <c r="D117" s="72"/>
-      <c r="E117" s="72"/>
-      <c r="F117" s="72"/>
+      <c r="A117" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B117" s="62"/>
+      <c r="C117" s="64"/>
+      <c r="D117" s="64"/>
+      <c r="E117" s="64"/>
+      <c r="F117" s="64"/>
       <c r="G117"/>
       <c r="H117"/>
       <c r="I117"/>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="55" t="s">
-        <v>95</v>
-      </c>
-      <c r="B118" s="69"/>
-      <c r="C118" s="72"/>
-      <c r="D118" s="72"/>
-      <c r="E118" s="72"/>
-      <c r="F118" s="72"/>
-      <c r="G118"/>
-      <c r="H118"/>
-      <c r="I118"/>
+      <c r="C118" s="41"/>
+      <c r="D118" s="41"/>
+      <c r="E118" s="41"/>
+      <c r="F118" s="41"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="B119" s="54"/>
-      <c r="C119" s="72"/>
-      <c r="D119" s="72"/>
-      <c r="E119" s="72"/>
-      <c r="F119" s="72"/>
-      <c r="G119"/>
-      <c r="H119"/>
-      <c r="I119"/>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="55" t="s">
-        <v>96</v>
-      </c>
-      <c r="B120" s="54"/>
-      <c r="C120" s="72"/>
-      <c r="D120" s="72"/>
-      <c r="E120" s="72"/>
-      <c r="F120" s="72"/>
-      <c r="G120"/>
-      <c r="H120"/>
-      <c r="I120"/>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="55" t="s">
-        <v>123</v>
-      </c>
-      <c r="B121" s="54"/>
-      <c r="C121" s="72"/>
-      <c r="D121" s="72"/>
-      <c r="E121" s="72"/>
-      <c r="F121" s="72"/>
-      <c r="G121"/>
-      <c r="H121"/>
-      <c r="I121"/>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="54" t="s">
-        <v>131</v>
-      </c>
-      <c r="B122" s="54"/>
-      <c r="C122" s="72"/>
-      <c r="D122" s="72"/>
-      <c r="E122" s="72"/>
-      <c r="F122" s="72"/>
-      <c r="G122"/>
-      <c r="H122"/>
-      <c r="I122"/>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="55" t="s">
-        <v>97</v>
-      </c>
-      <c r="B123" s="54"/>
-      <c r="C123" s="72"/>
-      <c r="D123" s="72"/>
-      <c r="E123" s="72"/>
-      <c r="F123" s="72"/>
-      <c r="G123"/>
-      <c r="H123"/>
-      <c r="I123"/>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A124" s="55" t="s">
-        <v>111</v>
-      </c>
-      <c r="B124" s="54"/>
-      <c r="C124" s="72"/>
-      <c r="D124" s="72"/>
-      <c r="E124" s="72"/>
-      <c r="F124" s="72"/>
-      <c r="G124"/>
-      <c r="H124"/>
-      <c r="I124"/>
-    </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="55" t="s">
-        <v>112</v>
-      </c>
-      <c r="B125" s="54"/>
-      <c r="C125" s="72"/>
-      <c r="D125" s="72"/>
-      <c r="E125" s="72"/>
-      <c r="F125" s="72"/>
-      <c r="G125"/>
-      <c r="H125"/>
-      <c r="I125"/>
-    </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A126" s="55" t="s">
-        <v>124</v>
-      </c>
-      <c r="B126" s="54"/>
-      <c r="C126" s="72"/>
-      <c r="D126" s="72"/>
-      <c r="E126" s="72"/>
-      <c r="F126" s="72"/>
-      <c r="G126"/>
-      <c r="H126"/>
-      <c r="I126"/>
-    </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A127" s="54" t="s">
-        <v>132</v>
-      </c>
-      <c r="B127" s="54"/>
-      <c r="C127" s="72"/>
-      <c r="D127" s="72"/>
-      <c r="E127" s="72"/>
-      <c r="F127" s="72"/>
-      <c r="G127"/>
-      <c r="H127"/>
-      <c r="I127"/>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A128" s="56" t="s">
-        <v>113</v>
-      </c>
-      <c r="B128" s="70"/>
-      <c r="C128" s="72"/>
-      <c r="D128" s="72"/>
-      <c r="E128" s="72"/>
-      <c r="F128" s="72"/>
-      <c r="G128"/>
-      <c r="H128"/>
-      <c r="I128"/>
-    </row>
-    <row r="129" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C129" s="48"/>
-      <c r="D129" s="48"/>
-      <c r="E129" s="48"/>
-      <c r="F129" s="48"/>
-    </row>
-    <row r="130" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C130" s="48"/>
-      <c r="D130" s="48"/>
-      <c r="E130" s="48"/>
-      <c r="F130" s="48"/>
+      <c r="C119" s="41"/>
+      <c r="D119" s="41"/>
+      <c r="E119" s="41"/>
+      <c r="F119" s="41"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="363" yWindow="440" count="7">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B89:D89 B74:D75">
+  <dataValidations xWindow="363" yWindow="440" count="6">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74:D75">
       <formula1>0</formula1>
       <formula2>10</formula2>
     </dataValidation>
@@ -4333,7 +4037,7 @@
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B90:D90">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79:D79">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
@@ -4341,17 +4045,13 @@
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B91:D91">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B80:D80">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B49:D49">
       <formula1>0</formula1>
       <formula2>100</formula2>
-    </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B81:D85">
-      <formula1>0</formula1>
-      <formula2>1</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4363,7 +4063,7 @@
           <x14:formula1>
             <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>B76:D80 B86:D88</xm:sqref>
+          <xm:sqref>B76:D78</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4386,7 +4086,7 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -4397,21 +4097,21 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move elaborations to GUI from sheets
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="119">
   <si>
     <t>recent_time</t>
   </si>
@@ -24,15 +24,6 @@
   </si>
   <si>
     <t>n_strains</t>
-  </si>
-  <si>
-    <t>is_lowquality</t>
-  </si>
-  <si>
-    <t>is_amplification</t>
-  </si>
-  <si>
-    <t>is_misassignment</t>
   </si>
   <si>
     <t>age_breakpoints</t>
@@ -1332,7 +1323,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1356,7 +1347,6 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="12" fillId="9" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
@@ -1373,8 +1363,6 @@
     <xf numFmtId="1" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="12" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="12" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1413,7 +1401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="12" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2384,437 +2372,437 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP119"/>
+  <dimension ref="A1:BP116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="52.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="25.5703125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="42" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="42" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="42"/>
+    <col min="2" max="4" width="25.5703125" style="34" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="39" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="39" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="39"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
+        <v>12</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
     </row>
     <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="37"/>
+        <v>18</v>
+      </c>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
+        <v>19</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
+        <v>55</v>
+      </c>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
     </row>
     <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+        <v>56</v>
+      </c>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
     </row>
     <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+        <v>57</v>
+      </c>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
     </row>
     <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+        <v>20</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
     </row>
     <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+        <v>50</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
     </row>
     <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+        <v>51</v>
+      </c>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+        <v>52</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
     </row>
     <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+        <v>21</v>
+      </c>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
     </row>
     <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
+        <v>22</v>
+      </c>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
     </row>
     <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
+        <v>23</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
     </row>
     <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
+        <v>24</v>
+      </c>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
     </row>
     <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
+        <v>38</v>
+      </c>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
     </row>
     <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
+        <v>39</v>
+      </c>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
     </row>
     <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
+        <v>40</v>
+      </c>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
     </row>
     <row r="18" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
+        <v>25</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
     </row>
     <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
+        <v>26</v>
+      </c>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
     </row>
     <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
+        <v>27</v>
+      </c>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
     </row>
     <row r="21" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
+        <v>28</v>
+      </c>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
     </row>
     <row r="22" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
+        <v>29</v>
+      </c>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
     </row>
     <row r="23" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
+        <v>30</v>
+      </c>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
     </row>
     <row r="24" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
+        <v>31</v>
+      </c>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
     </row>
     <row r="25" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
+        <v>32</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+        <v>33</v>
+      </c>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
     </row>
     <row r="27" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
+        <v>34</v>
+      </c>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="38"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+        <v>35</v>
+      </c>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
+        <v>36</v>
+      </c>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
+        <v>37</v>
+      </c>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
+        <v>53</v>
+      </c>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
+        <v>54</v>
+      </c>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="38"/>
+      <c r="F32" s="38"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
+        <v>41</v>
+      </c>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
+        <v>42</v>
+      </c>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
+        <v>43</v>
+      </c>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="38"/>
+      <c r="F35" s="38"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+        <v>44</v>
+      </c>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+        <v>45</v>
+      </c>
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B38" s="23"/>
-      <c r="C38" s="23"/>
-      <c r="D38" s="23"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="41"/>
+        <v>58</v>
+      </c>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" s="23"/>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
+        <v>61</v>
+      </c>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B40" s="23"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
+        <v>62</v>
+      </c>
+      <c r="B40" s="22"/>
+      <c r="C40" s="22"/>
+      <c r="D40" s="22"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B41" s="53"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
-      <c r="E41" s="54"/>
+        <v>93</v>
+      </c>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="51"/>
       <c r="F41"/>
       <c r="G41"/>
       <c r="H41"/>
@@ -2822,12 +2810,12 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="53"/>
-      <c r="E42" s="54"/>
+        <v>94</v>
+      </c>
+      <c r="B42" s="50"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="51"/>
       <c r="F42"/>
       <c r="G42"/>
       <c r="H42"/>
@@ -2835,12 +2823,12 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B43" s="53"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="54"/>
+        <v>95</v>
+      </c>
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="51"/>
       <c r="F43"/>
       <c r="G43"/>
       <c r="H43"/>
@@ -2848,12 +2836,12 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B44" s="53"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="54"/>
+        <v>111</v>
+      </c>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="51"/>
       <c r="F44"/>
       <c r="G44"/>
       <c r="H44"/>
@@ -2861,12 +2849,12 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" s="53"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="54"/>
+        <v>96</v>
+      </c>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="51"/>
       <c r="F45"/>
       <c r="G45"/>
       <c r="H45"/>
@@ -2874,295 +2862,295 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="41"/>
+        <v>46</v>
+      </c>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="38"/>
+      <c r="F46" s="38"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
+        <v>90</v>
+      </c>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="38"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="41"/>
+        <v>63</v>
+      </c>
+      <c r="B48" s="23"/>
+      <c r="C48" s="23"/>
+      <c r="D48" s="23"/>
+      <c r="E48" s="38"/>
+      <c r="F48" s="38"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49" s="25">
+        <v>10</v>
+      </c>
+      <c r="B49" s="24">
         <v>0.05</v>
       </c>
-      <c r="C49" s="41"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="38"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="26"/>
-      <c r="C50" s="50"/>
-      <c r="D50" s="50"/>
+        <v>47</v>
+      </c>
+      <c r="B50" s="25"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="47"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B51" s="26"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50"/>
+        <v>60</v>
+      </c>
+      <c r="B51" s="25"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B52" s="26"/>
-      <c r="C52" s="50"/>
-      <c r="D52" s="50"/>
+        <v>8</v>
+      </c>
+      <c r="B52" s="25"/>
+      <c r="C52" s="47"/>
+      <c r="D52" s="47"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B53" s="26"/>
-      <c r="C53" s="50"/>
-      <c r="D53" s="50"/>
+        <v>9</v>
+      </c>
+      <c r="B53" s="25"/>
+      <c r="C53" s="47"/>
+      <c r="D53" s="47"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
+        <v>87</v>
+      </c>
+      <c r="B54" s="26"/>
+      <c r="C54" s="48"/>
+      <c r="D54" s="48"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B55" s="27"/>
-      <c r="C55" s="51"/>
-      <c r="D55" s="51"/>
+        <v>88</v>
+      </c>
+      <c r="B55" s="26"/>
+      <c r="C55" s="48"/>
+      <c r="D55" s="48"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B56" s="27"/>
-      <c r="C56" s="51"/>
-      <c r="D56" s="51"/>
+        <v>89</v>
+      </c>
+      <c r="B56" s="26"/>
+      <c r="C56" s="48"/>
+      <c r="D56" s="48"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="26"/>
-      <c r="C57" s="50"/>
-      <c r="D57" s="50"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B58" s="26"/>
-      <c r="C58" s="50"/>
-      <c r="D58" s="50"/>
+        <v>6</v>
+      </c>
+      <c r="B58" s="25"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="47"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B59" s="26"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="50"/>
+        <v>103</v>
+      </c>
+      <c r="B59" s="25"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="47"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B60" s="26"/>
-      <c r="C60" s="50"/>
-      <c r="D60" s="50"/>
+        <v>8</v>
+      </c>
+      <c r="B60" s="25"/>
+      <c r="C60" s="47"/>
+      <c r="D60" s="47"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B61" s="26"/>
-      <c r="C61" s="50"/>
-      <c r="D61" s="50"/>
-      <c r="E61" s="56"/>
-      <c r="F61" s="56"/>
-      <c r="G61" s="56"/>
+        <v>9</v>
+      </c>
+      <c r="B61" s="25"/>
+      <c r="C61" s="47"/>
+      <c r="D61" s="47"/>
+      <c r="E61" s="53"/>
+      <c r="F61" s="53"/>
+      <c r="G61" s="53"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B62" s="26"/>
-      <c r="C62" s="50"/>
-      <c r="D62" s="50"/>
-      <c r="E62" s="56"/>
-      <c r="F62" s="56"/>
-      <c r="G62" s="56"/>
+        <v>5</v>
+      </c>
+      <c r="B62" s="25"/>
+      <c r="C62" s="47"/>
+      <c r="D62" s="47"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="53"/>
+      <c r="G62" s="53"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B63" s="26"/>
-      <c r="C63" s="50"/>
-      <c r="D63" s="50"/>
-      <c r="E63" s="56"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="56"/>
+        <v>84</v>
+      </c>
+      <c r="B63" s="25"/>
+      <c r="C63" s="47"/>
+      <c r="D63" s="47"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+      <c r="G63" s="53"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B64" s="26"/>
-      <c r="C64" s="50"/>
-      <c r="D64" s="50"/>
-      <c r="E64" s="56"/>
-      <c r="F64" s="56"/>
-      <c r="G64" s="56"/>
+        <v>85</v>
+      </c>
+      <c r="B64" s="25"/>
+      <c r="C64" s="47"/>
+      <c r="D64" s="47"/>
+      <c r="E64" s="53"/>
+      <c r="F64" s="53"/>
+      <c r="G64" s="53"/>
     </row>
     <row r="65" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B65" s="26"/>
-      <c r="C65" s="50"/>
-      <c r="D65" s="50"/>
-      <c r="E65" s="56"/>
-      <c r="F65" s="56"/>
-      <c r="G65" s="56"/>
+        <v>86</v>
+      </c>
+      <c r="B65" s="25"/>
+      <c r="C65" s="47"/>
+      <c r="D65" s="47"/>
+      <c r="E65" s="53"/>
+      <c r="F65" s="53"/>
+      <c r="G65" s="53"/>
     </row>
     <row r="66" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B66" s="55"/>
-      <c r="C66" s="57"/>
-      <c r="D66" s="57"/>
-      <c r="E66" s="58"/>
-      <c r="F66" s="59"/>
-      <c r="G66" s="59"/>
+        <v>100</v>
+      </c>
+      <c r="B66" s="52"/>
+      <c r="C66" s="54"/>
+      <c r="D66" s="54"/>
+      <c r="E66" s="55"/>
+      <c r="F66" s="56"/>
+      <c r="G66" s="56"/>
       <c r="H66"/>
       <c r="I66"/>
     </row>
     <row r="67" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B67" s="55"/>
-      <c r="C67" s="57"/>
-      <c r="D67" s="57"/>
-      <c r="E67" s="58"/>
-      <c r="F67" s="59"/>
-      <c r="G67" s="59"/>
+        <v>101</v>
+      </c>
+      <c r="B67" s="52"/>
+      <c r="C67" s="54"/>
+      <c r="D67" s="54"/>
+      <c r="E67" s="55"/>
+      <c r="F67" s="56"/>
+      <c r="G67" s="56"/>
       <c r="H67"/>
       <c r="I67"/>
     </row>
     <row r="68" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B68" s="55"/>
-      <c r="C68" s="57"/>
-      <c r="D68" s="57"/>
-      <c r="E68" s="58"/>
-      <c r="F68" s="59"/>
-      <c r="G68" s="59"/>
+        <v>102</v>
+      </c>
+      <c r="B68" s="52"/>
+      <c r="C68" s="54"/>
+      <c r="D68" s="54"/>
+      <c r="E68" s="55"/>
+      <c r="F68" s="56"/>
+      <c r="G68" s="56"/>
       <c r="H68"/>
       <c r="I68"/>
     </row>
     <row r="69" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B69" s="26"/>
-      <c r="C69" s="50"/>
-      <c r="D69" s="50"/>
-      <c r="E69" s="56"/>
-      <c r="F69" s="56"/>
-      <c r="G69" s="56"/>
+        <v>92</v>
+      </c>
+      <c r="B69" s="25"/>
+      <c r="C69" s="47"/>
+      <c r="D69" s="47"/>
+      <c r="E69" s="53"/>
+      <c r="F69" s="53"/>
+      <c r="G69" s="53"/>
     </row>
     <row r="70" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B70" s="26"/>
-      <c r="C70" s="50"/>
-      <c r="D70" s="50"/>
-      <c r="E70" s="56"/>
-      <c r="F70" s="56"/>
-      <c r="G70" s="56"/>
+        <v>91</v>
+      </c>
+      <c r="B70" s="25"/>
+      <c r="C70" s="47"/>
+      <c r="D70" s="47"/>
+      <c r="E70" s="53"/>
+      <c r="F70" s="53"/>
+      <c r="G70" s="53"/>
     </row>
     <row r="71" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B71" s="28"/>
-      <c r="C71" s="50"/>
-      <c r="D71" s="50"/>
-      <c r="E71" s="56"/>
-      <c r="F71" s="56"/>
-      <c r="G71" s="56"/>
+        <v>64</v>
+      </c>
+      <c r="B71" s="27"/>
+      <c r="C71" s="47"/>
+      <c r="D71" s="47"/>
+      <c r="E71" s="53"/>
+      <c r="F71" s="53"/>
+      <c r="G71" s="53"/>
     </row>
     <row r="72" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B72" s="29"/>
-      <c r="C72" s="50"/>
-      <c r="D72" s="50"/>
-      <c r="E72" s="56"/>
-      <c r="F72" s="56"/>
-      <c r="G72" s="56"/>
+        <v>48</v>
+      </c>
+      <c r="B72" s="28"/>
+      <c r="C72" s="47"/>
+      <c r="D72" s="47"/>
+      <c r="E72" s="53"/>
+      <c r="F72" s="53"/>
+      <c r="G72" s="53"/>
     </row>
     <row r="73" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B73" s="30"/>
-      <c r="C73" s="50"/>
-      <c r="D73" s="50"/>
-      <c r="E73" s="56"/>
-      <c r="F73" s="56"/>
-      <c r="G73" s="56"/>
+        <v>49</v>
+      </c>
+      <c r="B73" s="29"/>
+      <c r="C73" s="47"/>
+      <c r="D73" s="47"/>
+      <c r="E73" s="53"/>
+      <c r="F73" s="53"/>
+      <c r="G73" s="53"/>
     </row>
     <row r="74" spans="1:68" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B74" s="31"/>
-      <c r="C74" s="50"/>
-      <c r="D74" s="50"/>
-      <c r="E74" s="41"/>
-      <c r="F74" s="41"/>
-      <c r="G74" s="41"/>
-      <c r="H74" s="37"/>
-      <c r="I74" s="37"/>
+      <c r="B74" s="30"/>
+      <c r="C74" s="47"/>
+      <c r="D74" s="47"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="38"/>
+      <c r="G74" s="38"/>
+      <c r="H74" s="34"/>
+      <c r="I74" s="34"/>
       <c r="J74" s="15"/>
       <c r="K74" s="15"/>
       <c r="L74" s="15"/>
@@ -3224,17 +3212,17 @@
       <c r="BP74" s="15"/>
     </row>
     <row r="75" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A75" s="11" t="s">
+      <c r="A75" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B75" s="31"/>
-      <c r="C75" s="50"/>
-      <c r="D75" s="50"/>
-      <c r="E75" s="41"/>
-      <c r="F75" s="41"/>
-      <c r="G75" s="41"/>
-      <c r="H75" s="37"/>
-      <c r="I75" s="37"/>
+      <c r="B75" s="63"/>
+      <c r="C75" s="47"/>
+      <c r="D75" s="47"/>
+      <c r="E75" s="38"/>
+      <c r="F75" s="38"/>
+      <c r="G75" s="38"/>
+      <c r="H75" s="34"/>
+      <c r="I75" s="34"/>
       <c r="J75" s="15"/>
       <c r="K75" s="15"/>
       <c r="L75" s="15"/>
@@ -3296,736 +3284,520 @@
       <c r="BP75" s="15"/>
     </row>
     <row r="76" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A76" s="19" t="s">
+      <c r="A76" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B76" s="31"/>
+      <c r="C76" s="49"/>
+      <c r="D76" s="49"/>
+    </row>
+    <row r="77" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A77" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B77" s="32"/>
+      <c r="C77" s="32"/>
+      <c r="D77" s="32"/>
+      <c r="E77" s="40"/>
+      <c r="F77" s="40"/>
+      <c r="G77" s="40"/>
+      <c r="H77" s="41"/>
+    </row>
+    <row r="78" spans="1:68" x14ac:dyDescent="0.25">
+      <c r="A78" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B76" s="66"/>
-      <c r="C76" s="41"/>
-      <c r="D76" s="41"/>
-      <c r="E76" s="37"/>
-      <c r="F76" s="37"/>
-      <c r="G76" s="37"/>
-      <c r="H76" s="37"/>
-      <c r="I76" s="37"/>
-      <c r="J76" s="15"/>
-      <c r="K76" s="15"/>
-      <c r="L76" s="15"/>
-      <c r="M76" s="15"/>
-      <c r="N76" s="15"/>
-      <c r="O76" s="15"/>
-      <c r="P76" s="15"/>
-      <c r="Q76" s="15"/>
-      <c r="R76" s="15"/>
-      <c r="S76" s="15"/>
-      <c r="T76" s="15"/>
-      <c r="U76" s="15"/>
-      <c r="V76" s="15"/>
-      <c r="W76" s="15"/>
-      <c r="X76" s="15"/>
-      <c r="Y76" s="15"/>
-      <c r="Z76" s="15"/>
-      <c r="AA76" s="15"/>
-      <c r="AB76" s="15"/>
-      <c r="AC76" s="15"/>
-      <c r="AD76" s="15"/>
-      <c r="AE76" s="15"/>
-      <c r="AF76" s="15"/>
-      <c r="AG76" s="15"/>
-      <c r="AH76" s="15"/>
-      <c r="AI76" s="15"/>
-      <c r="AJ76" s="15"/>
-      <c r="AK76" s="15"/>
-      <c r="AL76" s="15"/>
-      <c r="AM76" s="15"/>
-      <c r="AN76" s="15"/>
-      <c r="AO76" s="15"/>
-      <c r="AP76" s="15"/>
-      <c r="AQ76" s="15"/>
-      <c r="AR76" s="15"/>
-      <c r="AS76" s="15"/>
-      <c r="AT76" s="15"/>
-      <c r="AU76" s="15"/>
-      <c r="AV76" s="15"/>
-      <c r="AW76" s="15"/>
-      <c r="AX76" s="15"/>
-      <c r="AY76" s="15"/>
-      <c r="AZ76" s="15"/>
-      <c r="BA76" s="15"/>
-      <c r="BB76" s="15"/>
-      <c r="BC76" s="15"/>
-      <c r="BD76" s="15"/>
-      <c r="BE76" s="15"/>
-      <c r="BF76" s="15"/>
-      <c r="BG76" s="15"/>
-      <c r="BH76" s="15"/>
-      <c r="BI76" s="15"/>
-      <c r="BJ76" s="15"/>
-      <c r="BK76" s="15"/>
-      <c r="BL76" s="15"/>
-      <c r="BM76" s="15"/>
-      <c r="BN76" s="15"/>
-      <c r="BO76" s="15"/>
-      <c r="BP76" s="15"/>
-    </row>
-    <row r="77" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A77" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B77" s="32"/>
-      <c r="C77" s="41"/>
-      <c r="D77" s="41"/>
-      <c r="E77" s="37"/>
-      <c r="F77" s="37"/>
-      <c r="G77" s="37"/>
-      <c r="H77" s="37"/>
-      <c r="I77" s="37"/>
-      <c r="J77" s="15"/>
-      <c r="K77" s="15"/>
-      <c r="L77" s="15"/>
-      <c r="M77" s="15"/>
-      <c r="N77" s="15"/>
-      <c r="O77" s="15"/>
-      <c r="P77" s="15"/>
-      <c r="Q77" s="15"/>
-      <c r="R77" s="15"/>
-      <c r="S77" s="15"/>
-      <c r="T77" s="15"/>
-      <c r="U77" s="15"/>
-      <c r="V77" s="15"/>
-      <c r="W77" s="15"/>
-      <c r="X77" s="15"/>
-      <c r="Y77" s="15"/>
-      <c r="Z77" s="15"/>
-      <c r="AA77" s="15"/>
-      <c r="AB77" s="15"/>
-      <c r="AC77" s="15"/>
-      <c r="AD77" s="15"/>
-      <c r="AE77" s="15"/>
-      <c r="AF77" s="15"/>
-      <c r="AG77" s="15"/>
-      <c r="AH77" s="15"/>
-      <c r="AI77" s="15"/>
-      <c r="AJ77" s="15"/>
-      <c r="AK77" s="15"/>
-      <c r="AL77" s="15"/>
-      <c r="AM77" s="15"/>
-      <c r="AN77" s="15"/>
-      <c r="AO77" s="15"/>
-      <c r="AP77" s="15"/>
-      <c r="AQ77" s="15"/>
-      <c r="AR77" s="15"/>
-      <c r="AS77" s="15"/>
-      <c r="AT77" s="15"/>
-      <c r="AU77" s="15"/>
-      <c r="AV77" s="15"/>
-      <c r="AW77" s="15"/>
-      <c r="AX77" s="15"/>
-      <c r="AY77" s="15"/>
-      <c r="AZ77" s="15"/>
-      <c r="BA77" s="15"/>
-      <c r="BB77" s="15"/>
-      <c r="BC77" s="15"/>
-      <c r="BD77" s="15"/>
-      <c r="BE77" s="15"/>
-      <c r="BF77" s="15"/>
-      <c r="BG77" s="15"/>
-      <c r="BH77" s="15"/>
-      <c r="BI77" s="15"/>
-      <c r="BJ77" s="15"/>
-      <c r="BK77" s="15"/>
-      <c r="BL77" s="15"/>
-      <c r="BM77" s="15"/>
-      <c r="BN77" s="15"/>
-      <c r="BO77" s="15"/>
-      <c r="BP77" s="15"/>
-    </row>
-    <row r="78" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A78" s="12" t="s">
+      <c r="B78" s="33">
         <v>5</v>
       </c>
-      <c r="B78" s="33"/>
-      <c r="C78" s="41"/>
-      <c r="D78" s="41"/>
-      <c r="E78" s="37"/>
-      <c r="F78" s="37"/>
-      <c r="G78" s="37"/>
-      <c r="H78" s="37"/>
-      <c r="I78" s="37"/>
-      <c r="J78" s="15"/>
-      <c r="K78" s="15"/>
-      <c r="L78" s="15"/>
-      <c r="M78" s="15"/>
-      <c r="N78" s="15"/>
-      <c r="O78" s="15"/>
-      <c r="P78" s="15"/>
-      <c r="Q78" s="15"/>
-      <c r="R78" s="15"/>
-      <c r="S78" s="15"/>
-      <c r="T78" s="15"/>
-      <c r="U78" s="15"/>
-      <c r="V78" s="15"/>
-      <c r="W78" s="15"/>
-      <c r="X78" s="15"/>
-      <c r="Y78" s="15"/>
-      <c r="Z78" s="15"/>
-      <c r="AA78" s="15"/>
-      <c r="AB78" s="15"/>
-      <c r="AC78" s="15"/>
-      <c r="AD78" s="15"/>
-      <c r="AE78" s="15"/>
-      <c r="AF78" s="15"/>
-      <c r="AG78" s="15"/>
-      <c r="AH78" s="15"/>
-      <c r="AI78" s="15"/>
-      <c r="AJ78" s="15"/>
-      <c r="AK78" s="15"/>
-      <c r="AL78" s="15"/>
-      <c r="AM78" s="15"/>
-      <c r="AN78" s="15"/>
-      <c r="AO78" s="15"/>
-      <c r="AP78" s="15"/>
-      <c r="AQ78" s="15"/>
-      <c r="AR78" s="15"/>
-      <c r="AS78" s="15"/>
-      <c r="AT78" s="15"/>
-      <c r="AU78" s="15"/>
-      <c r="AV78" s="15"/>
-      <c r="AW78" s="15"/>
-      <c r="AX78" s="15"/>
-      <c r="AY78" s="15"/>
-      <c r="AZ78" s="15"/>
-      <c r="BA78" s="15"/>
-      <c r="BB78" s="15"/>
-      <c r="BC78" s="15"/>
-      <c r="BD78" s="15"/>
-      <c r="BE78" s="15"/>
-      <c r="BF78" s="15"/>
-      <c r="BG78" s="15"/>
-      <c r="BH78" s="15"/>
-      <c r="BI78" s="15"/>
-      <c r="BJ78" s="15"/>
-      <c r="BK78" s="15"/>
-      <c r="BL78" s="15"/>
-      <c r="BM78" s="15"/>
-      <c r="BN78" s="15"/>
-      <c r="BO78" s="15"/>
-      <c r="BP78" s="15"/>
+      <c r="C78" s="33">
+        <v>15</v>
+      </c>
+      <c r="D78" s="33"/>
+      <c r="E78" s="33"/>
+      <c r="F78" s="33"/>
+      <c r="G78" s="33"/>
+      <c r="H78" s="42"/>
     </row>
     <row r="79" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A79" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B79" s="34"/>
-      <c r="C79" s="52"/>
-      <c r="D79" s="52"/>
+      <c r="A79" s="43" t="s">
+        <v>65</v>
+      </c>
+      <c r="B79" s="57"/>
+      <c r="C79" s="61"/>
+      <c r="D79" s="61"/>
+      <c r="E79" s="61"/>
+      <c r="F79" s="61"/>
+      <c r="G79"/>
+      <c r="H79"/>
+      <c r="I79"/>
     </row>
     <row r="80" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B80" s="35"/>
-      <c r="C80" s="35"/>
-      <c r="D80" s="35"/>
-      <c r="E80" s="43"/>
-      <c r="F80" s="43"/>
-      <c r="G80" s="43"/>
-      <c r="H80" s="44"/>
+      <c r="A80" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="B80" s="44"/>
+      <c r="C80" s="60"/>
+      <c r="D80" s="60"/>
+      <c r="E80" s="61"/>
+      <c r="F80" s="61"/>
+      <c r="G80"/>
+      <c r="H80"/>
+      <c r="I80"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B81" s="36">
-        <v>5</v>
-      </c>
-      <c r="C81" s="36">
-        <v>15</v>
-      </c>
-      <c r="D81" s="36"/>
-      <c r="E81" s="36"/>
-      <c r="F81" s="36"/>
-      <c r="G81" s="36"/>
-      <c r="H81" s="45"/>
+      <c r="A81" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="B81" s="44"/>
+      <c r="C81" s="61"/>
+      <c r="D81" s="61"/>
+      <c r="E81" s="61"/>
+      <c r="F81" s="61"/>
+      <c r="G81"/>
+      <c r="H81"/>
+      <c r="I81"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="B82" s="60"/>
-      <c r="C82" s="64"/>
-      <c r="D82" s="64"/>
-      <c r="E82" s="64"/>
-      <c r="F82" s="64"/>
+      <c r="A82" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="B82" s="44"/>
+      <c r="C82" s="61"/>
+      <c r="D82" s="61"/>
+      <c r="E82" s="61"/>
+      <c r="F82" s="61"/>
       <c r="G82"/>
       <c r="H82"/>
       <c r="I82"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="47" t="s">
-        <v>69</v>
-      </c>
-      <c r="B83" s="47"/>
-      <c r="C83" s="63"/>
-      <c r="D83" s="63"/>
-      <c r="E83" s="64"/>
-      <c r="F83" s="64"/>
+      <c r="A83" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="B83" s="44"/>
+      <c r="C83" s="61"/>
+      <c r="D83" s="61"/>
+      <c r="E83" s="61"/>
+      <c r="F83" s="61"/>
       <c r="G83"/>
       <c r="H83"/>
       <c r="I83"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="B84" s="47"/>
-      <c r="C84" s="64"/>
-      <c r="D84" s="64"/>
-      <c r="E84" s="64"/>
-      <c r="F84" s="64"/>
+      <c r="A84" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="B84" s="44"/>
+      <c r="C84" s="61"/>
+      <c r="D84" s="61"/>
+      <c r="E84" s="61"/>
+      <c r="F84" s="61"/>
       <c r="G84"/>
       <c r="H84"/>
       <c r="I84"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="47" t="s">
-        <v>107</v>
-      </c>
-      <c r="B85" s="47"/>
-      <c r="C85" s="64"/>
-      <c r="D85" s="64"/>
-      <c r="E85" s="64"/>
-      <c r="F85" s="64"/>
+      <c r="A85" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B85" s="44"/>
+      <c r="C85" s="60"/>
+      <c r="D85" s="60"/>
+      <c r="E85" s="61"/>
+      <c r="F85" s="61"/>
       <c r="G85"/>
       <c r="H85"/>
       <c r="I85"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="B86" s="47"/>
-      <c r="C86" s="64"/>
-      <c r="D86" s="64"/>
-      <c r="E86" s="64"/>
-      <c r="F86" s="64"/>
+      <c r="A86" s="44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B86" s="44"/>
+      <c r="C86" s="61"/>
+      <c r="D86" s="61"/>
+      <c r="E86" s="61"/>
+      <c r="F86" s="61"/>
       <c r="G86"/>
       <c r="H86"/>
       <c r="I86"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="47" t="s">
-        <v>76</v>
-      </c>
-      <c r="B87" s="47"/>
-      <c r="C87" s="64"/>
-      <c r="D87" s="64"/>
-      <c r="E87" s="64"/>
-      <c r="F87" s="64"/>
+      <c r="A87" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B87" s="44"/>
+      <c r="C87" s="61"/>
+      <c r="D87" s="61"/>
+      <c r="E87" s="61"/>
+      <c r="F87" s="61"/>
       <c r="G87"/>
       <c r="H87"/>
       <c r="I87"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="B88" s="47"/>
-      <c r="C88" s="63"/>
-      <c r="D88" s="63"/>
-      <c r="E88" s="64"/>
-      <c r="F88" s="64"/>
+      <c r="A88" s="44" t="s">
+        <v>113</v>
+      </c>
+      <c r="B88" s="44"/>
+      <c r="C88" s="61"/>
+      <c r="D88" s="61"/>
+      <c r="E88" s="61"/>
+      <c r="F88" s="61"/>
       <c r="G88"/>
       <c r="H88"/>
       <c r="I88"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="47" t="s">
-        <v>77</v>
-      </c>
-      <c r="B89" s="47"/>
-      <c r="C89" s="64"/>
-      <c r="D89" s="64"/>
-      <c r="E89" s="64"/>
-      <c r="F89" s="64"/>
+      <c r="A89" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B89" s="44"/>
+      <c r="C89" s="61"/>
+      <c r="D89" s="61"/>
+      <c r="E89" s="61"/>
+      <c r="F89" s="61"/>
       <c r="G89"/>
       <c r="H89"/>
       <c r="I89"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="47" t="s">
-        <v>108</v>
-      </c>
-      <c r="B90" s="47"/>
-      <c r="C90" s="64"/>
-      <c r="D90" s="64"/>
-      <c r="E90" s="64"/>
-      <c r="F90" s="64"/>
+      <c r="A90" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="B90" s="58"/>
+      <c r="C90" s="61"/>
+      <c r="D90" s="61"/>
+      <c r="E90" s="61"/>
+      <c r="F90" s="61"/>
       <c r="G90"/>
       <c r="H90"/>
       <c r="I90"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="B91" s="47"/>
-      <c r="C91" s="64"/>
-      <c r="D91" s="64"/>
-      <c r="E91" s="64"/>
-      <c r="F91" s="64"/>
+      <c r="A91" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B91" s="58"/>
+      <c r="C91" s="61"/>
+      <c r="D91" s="61"/>
+      <c r="E91" s="61"/>
+      <c r="F91" s="61"/>
       <c r="G91"/>
       <c r="H91"/>
       <c r="I91"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="47" t="s">
-        <v>78</v>
-      </c>
-      <c r="B92" s="47"/>
-      <c r="C92" s="64"/>
-      <c r="D92" s="64"/>
-      <c r="E92" s="64"/>
-      <c r="F92" s="64"/>
+      <c r="A92" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="B92" s="58"/>
+      <c r="C92" s="61"/>
+      <c r="D92" s="61"/>
+      <c r="E92" s="61"/>
+      <c r="F92" s="61"/>
       <c r="G92"/>
       <c r="H92"/>
       <c r="I92"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="B93" s="61"/>
-      <c r="C93" s="64"/>
-      <c r="D93" s="64"/>
-      <c r="E93" s="64"/>
-      <c r="F93" s="64"/>
+      <c r="A93" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="B93" s="58"/>
+      <c r="C93" s="61"/>
+      <c r="D93" s="61"/>
+      <c r="E93" s="61"/>
+      <c r="F93" s="61"/>
       <c r="G93"/>
       <c r="H93"/>
       <c r="I93"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="B94" s="61"/>
-      <c r="C94" s="64"/>
-      <c r="D94" s="64"/>
-      <c r="E94" s="64"/>
-      <c r="F94" s="64"/>
+      <c r="A94" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="B94" s="58"/>
+      <c r="C94" s="61"/>
+      <c r="D94" s="61"/>
+      <c r="E94" s="61"/>
+      <c r="F94" s="61"/>
       <c r="G94"/>
       <c r="H94"/>
       <c r="I94"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="48" t="s">
-        <v>109</v>
-      </c>
-      <c r="B95" s="61"/>
-      <c r="C95" s="64"/>
-      <c r="D95" s="64"/>
-      <c r="E95" s="64"/>
-      <c r="F95" s="64"/>
+      <c r="A95" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B95" s="58"/>
+      <c r="C95" s="61"/>
+      <c r="D95" s="61"/>
+      <c r="E95" s="61"/>
+      <c r="F95" s="61"/>
       <c r="G95"/>
       <c r="H95"/>
       <c r="I95"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="47" t="s">
-        <v>117</v>
-      </c>
-      <c r="B96" s="61"/>
-      <c r="C96" s="64"/>
-      <c r="D96" s="64"/>
-      <c r="E96" s="64"/>
-      <c r="F96" s="64"/>
+      <c r="A96" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="B96" s="58"/>
+      <c r="C96" s="61"/>
+      <c r="D96" s="61"/>
+      <c r="E96" s="61"/>
+      <c r="F96" s="61"/>
       <c r="G96"/>
       <c r="H96"/>
       <c r="I96"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="B97" s="61"/>
-      <c r="C97" s="64"/>
-      <c r="D97" s="64"/>
-      <c r="E97" s="64"/>
-      <c r="F97" s="64"/>
+      <c r="A97" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="B97" s="58"/>
+      <c r="C97" s="61"/>
+      <c r="D97" s="61"/>
+      <c r="E97" s="61"/>
+      <c r="F97" s="61"/>
       <c r="G97"/>
       <c r="H97"/>
       <c r="I97"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="48" t="s">
-        <v>72</v>
-      </c>
-      <c r="B98" s="61"/>
-      <c r="C98" s="64"/>
-      <c r="D98" s="64"/>
-      <c r="E98" s="64"/>
-      <c r="F98" s="64"/>
+      <c r="A98" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="B98" s="58"/>
+      <c r="C98" s="61"/>
+      <c r="D98" s="61"/>
+      <c r="E98" s="61"/>
+      <c r="F98" s="61"/>
       <c r="G98"/>
       <c r="H98"/>
       <c r="I98"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="48" t="s">
-        <v>81</v>
-      </c>
-      <c r="B99" s="61"/>
-      <c r="C99" s="64"/>
-      <c r="D99" s="64"/>
-      <c r="E99" s="64"/>
-      <c r="F99" s="64"/>
+      <c r="A99" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B99" s="58"/>
+      <c r="C99" s="61"/>
+      <c r="D99" s="61"/>
+      <c r="E99" s="61"/>
+      <c r="F99" s="61"/>
       <c r="G99"/>
       <c r="H99"/>
       <c r="I99"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="48" t="s">
-        <v>110</v>
-      </c>
-      <c r="B100" s="61"/>
-      <c r="C100" s="64"/>
-      <c r="D100" s="64"/>
-      <c r="E100" s="64"/>
-      <c r="F100" s="64"/>
+      <c r="A100" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B100" s="58"/>
+      <c r="C100" s="61"/>
+      <c r="D100" s="61"/>
+      <c r="E100" s="61"/>
+      <c r="F100" s="61"/>
       <c r="G100"/>
       <c r="H100"/>
       <c r="I100"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="47" t="s">
-        <v>118</v>
-      </c>
-      <c r="B101" s="61"/>
-      <c r="C101" s="64"/>
-      <c r="D101" s="64"/>
-      <c r="E101" s="64"/>
-      <c r="F101" s="64"/>
+      <c r="A101" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B101" s="58"/>
+      <c r="C101" s="61"/>
+      <c r="D101" s="61"/>
+      <c r="E101" s="62"/>
+      <c r="F101" s="61"/>
       <c r="G101"/>
       <c r="H101"/>
       <c r="I101"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="48" t="s">
-        <v>82</v>
-      </c>
-      <c r="B102" s="61"/>
-      <c r="C102" s="64"/>
-      <c r="D102" s="64"/>
-      <c r="E102" s="64"/>
-      <c r="F102" s="64"/>
+      <c r="A102" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="B102" s="58"/>
+      <c r="C102" s="61"/>
+      <c r="D102" s="61"/>
+      <c r="E102" s="62"/>
+      <c r="F102" s="61"/>
       <c r="G102"/>
       <c r="H102"/>
       <c r="I102"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="48" t="s">
-        <v>73</v>
-      </c>
-      <c r="B103" s="61"/>
-      <c r="C103" s="64"/>
-      <c r="D103" s="64"/>
-      <c r="E103" s="64"/>
-      <c r="F103" s="64"/>
+      <c r="A103" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="B103" s="58"/>
+      <c r="C103" s="61"/>
+      <c r="D103" s="61"/>
+      <c r="E103" s="61"/>
+      <c r="F103" s="61"/>
       <c r="G103"/>
       <c r="H103"/>
       <c r="I103"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="B104" s="61"/>
-      <c r="C104" s="64"/>
-      <c r="D104" s="64"/>
-      <c r="E104" s="65"/>
-      <c r="F104" s="64"/>
+      <c r="A104" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B104" s="58"/>
+      <c r="C104" s="61"/>
+      <c r="D104" s="61"/>
+      <c r="E104" s="61"/>
+      <c r="F104" s="61"/>
       <c r="G104"/>
       <c r="H104"/>
       <c r="I104"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="48" t="s">
-        <v>111</v>
-      </c>
-      <c r="B105" s="61"/>
-      <c r="C105" s="64"/>
-      <c r="D105" s="64"/>
-      <c r="E105" s="65"/>
-      <c r="F105" s="64"/>
+      <c r="A105" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="B105" s="44"/>
+      <c r="C105" s="61"/>
+      <c r="D105" s="61"/>
+      <c r="E105" s="61"/>
+      <c r="F105" s="61"/>
       <c r="G105"/>
       <c r="H105"/>
       <c r="I105"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="B106" s="61"/>
-      <c r="C106" s="64"/>
-      <c r="D106" s="64"/>
-      <c r="E106" s="64"/>
-      <c r="F106" s="64"/>
+      <c r="A106" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B106" s="44"/>
+      <c r="C106" s="61"/>
+      <c r="D106" s="61"/>
+      <c r="E106" s="61"/>
+      <c r="F106" s="61"/>
       <c r="G106"/>
       <c r="H106"/>
       <c r="I106"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="B107" s="61"/>
-      <c r="C107" s="64"/>
-      <c r="D107" s="64"/>
-      <c r="E107" s="64"/>
-      <c r="F107" s="64"/>
+      <c r="A107" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B107" s="44"/>
+      <c r="C107" s="61"/>
+      <c r="D107" s="61"/>
+      <c r="E107" s="61"/>
+      <c r="F107" s="61"/>
       <c r="G107"/>
       <c r="H107"/>
       <c r="I107"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="48" t="s">
-        <v>74</v>
-      </c>
-      <c r="B108" s="47"/>
-      <c r="C108" s="64"/>
-      <c r="D108" s="64"/>
-      <c r="E108" s="64"/>
-      <c r="F108" s="64"/>
+      <c r="A108" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="B108" s="44"/>
+      <c r="C108" s="61"/>
+      <c r="D108" s="61"/>
+      <c r="E108" s="61"/>
+      <c r="F108" s="61"/>
       <c r="G108"/>
       <c r="H108"/>
       <c r="I108"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="48" t="s">
-        <v>85</v>
-      </c>
-      <c r="B109" s="47"/>
-      <c r="C109" s="64"/>
-      <c r="D109" s="64"/>
-      <c r="E109" s="64"/>
-      <c r="F109" s="64"/>
+      <c r="A109" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B109" s="44"/>
+      <c r="C109" s="61"/>
+      <c r="D109" s="61"/>
+      <c r="E109" s="61"/>
+      <c r="F109" s="61"/>
       <c r="G109"/>
       <c r="H109"/>
       <c r="I109"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="48" t="s">
-        <v>112</v>
-      </c>
-      <c r="B110" s="47"/>
-      <c r="C110" s="64"/>
-      <c r="D110" s="64"/>
-      <c r="E110" s="64"/>
-      <c r="F110" s="64"/>
+      <c r="A110" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B110" s="44"/>
+      <c r="C110" s="61"/>
+      <c r="D110" s="61"/>
+      <c r="E110" s="61"/>
+      <c r="F110" s="61"/>
       <c r="G110"/>
       <c r="H110"/>
       <c r="I110"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="47" t="s">
-        <v>120</v>
-      </c>
-      <c r="B111" s="47"/>
-      <c r="C111" s="64"/>
-      <c r="D111" s="64"/>
-      <c r="E111" s="64"/>
-      <c r="F111" s="64"/>
+      <c r="A111" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="B111" s="44"/>
+      <c r="C111" s="61"/>
+      <c r="D111" s="61"/>
+      <c r="E111" s="61"/>
+      <c r="F111" s="61"/>
       <c r="G111"/>
       <c r="H111"/>
       <c r="I111"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="B112" s="47"/>
-      <c r="C112" s="64"/>
-      <c r="D112" s="64"/>
-      <c r="E112" s="64"/>
-      <c r="F112" s="64"/>
+      <c r="A112" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="B112" s="44"/>
+      <c r="C112" s="61"/>
+      <c r="D112" s="61"/>
+      <c r="E112" s="61"/>
+      <c r="F112" s="61"/>
       <c r="G112"/>
       <c r="H112"/>
       <c r="I112"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="48" t="s">
-        <v>100</v>
-      </c>
-      <c r="B113" s="47"/>
-      <c r="C113" s="64"/>
-      <c r="D113" s="64"/>
-      <c r="E113" s="64"/>
-      <c r="F113" s="64"/>
+      <c r="A113" s="44" t="s">
+        <v>118</v>
+      </c>
+      <c r="B113" s="44"/>
+      <c r="C113" s="61"/>
+      <c r="D113" s="61"/>
+      <c r="E113" s="61"/>
+      <c r="F113" s="61"/>
       <c r="G113"/>
       <c r="H113"/>
       <c r="I113"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="B114" s="47"/>
-      <c r="C114" s="64"/>
-      <c r="D114" s="64"/>
-      <c r="E114" s="64"/>
-      <c r="F114" s="64"/>
+      <c r="A114" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B114" s="59"/>
+      <c r="C114" s="61"/>
+      <c r="D114" s="61"/>
+      <c r="E114" s="61"/>
+      <c r="F114" s="61"/>
       <c r="G114"/>
       <c r="H114"/>
       <c r="I114"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="48" t="s">
-        <v>113</v>
-      </c>
-      <c r="B115" s="47"/>
-      <c r="C115" s="64"/>
-      <c r="D115" s="64"/>
-      <c r="E115" s="64"/>
-      <c r="F115" s="64"/>
-      <c r="G115"/>
-      <c r="H115"/>
-      <c r="I115"/>
+      <c r="C115" s="38"/>
+      <c r="D115" s="38"/>
+      <c r="E115" s="38"/>
+      <c r="F115" s="38"/>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="47" t="s">
-        <v>121</v>
-      </c>
-      <c r="B116" s="47"/>
-      <c r="C116" s="64"/>
-      <c r="D116" s="64"/>
-      <c r="E116" s="64"/>
-      <c r="F116" s="64"/>
-      <c r="G116"/>
-      <c r="H116"/>
-      <c r="I116"/>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="B117" s="62"/>
-      <c r="C117" s="64"/>
-      <c r="D117" s="64"/>
-      <c r="E117" s="64"/>
-      <c r="F117" s="64"/>
-      <c r="G117"/>
-      <c r="H117"/>
-      <c r="I117"/>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C118" s="41"/>
-      <c r="D118" s="41"/>
-      <c r="E118" s="41"/>
-      <c r="F118" s="41"/>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C119" s="41"/>
-      <c r="D119" s="41"/>
-      <c r="E119" s="41"/>
-      <c r="F119" s="41"/>
+      <c r="C116" s="38"/>
+      <c r="D116" s="38"/>
+      <c r="E116" s="38"/>
+      <c r="F116" s="38"/>
     </row>
   </sheetData>
   <dataValidations xWindow="363" yWindow="440" count="6">
@@ -4037,7 +3809,7 @@
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B79:D79">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B76:D76">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
@@ -4045,7 +3817,7 @@
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B80:D80">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B77:D77">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -4056,18 +3828,6 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="363" yWindow="440" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>dropdown_lists!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B76:D78</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4086,32 +3846,32 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All model stratification moved to GUI
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,15 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="117">
   <si>
     <t>recent_time</t>
-  </si>
-  <si>
-    <t>n_organs</t>
-  </si>
-  <si>
-    <t>n_strains</t>
   </si>
   <si>
     <t>age_breakpoints</t>
@@ -382,7 +376,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -454,13 +448,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="5" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -474,7 +461,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -485,12 +472,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB9DAED"/>
         <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -1321,79 +1302,75 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="12" fillId="9" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="8" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="12" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="12" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="7" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="2" fontId="11" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="6" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="12" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="9" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="8" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="6" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="8" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1401,7 +1378,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="12" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="664">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -2372,437 +2348,437 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:BP116"/>
+  <dimension ref="A1:I114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="25.5703125" style="34" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="39" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="39" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="39"/>
+    <col min="1" max="1" width="52.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="25.5703125" style="30" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="35" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="35" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="35" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="35" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="35"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
+      <c r="A1" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="34"/>
+        <v>16</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+        <v>17</v>
+      </c>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
+        <v>53</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+        <v>54</v>
+      </c>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
+        <v>55</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
     </row>
     <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
+        <v>18</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
+        <v>48</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
+        <v>49</v>
+      </c>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
     </row>
     <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
+        <v>50</v>
+      </c>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
     </row>
     <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
+        <v>19</v>
+      </c>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
     </row>
     <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
+        <v>20</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
     </row>
     <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
+        <v>21</v>
+      </c>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
     </row>
     <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
+        <v>22</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
     </row>
     <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
+        <v>36</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="34"/>
     </row>
     <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
+        <v>37</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
     </row>
     <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
+        <v>38</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
     </row>
     <row r="18" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
+        <v>23</v>
+      </c>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
     </row>
     <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
+        <v>24</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
     </row>
     <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
+        <v>25</v>
+      </c>
+      <c r="B20" s="17"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
     </row>
     <row r="21" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
+        <v>26</v>
+      </c>
+      <c r="B21" s="17"/>
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
     </row>
     <row r="22" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="38"/>
-      <c r="F22" s="38"/>
+        <v>27</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
     </row>
     <row r="23" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
+        <v>28</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
     </row>
     <row r="24" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
+        <v>29</v>
+      </c>
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
     </row>
     <row r="25" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
+        <v>30</v>
+      </c>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
     </row>
     <row r="26" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
+        <v>31</v>
+      </c>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
     </row>
     <row r="27" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
+        <v>32</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
+        <v>33</v>
+      </c>
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
+        <v>34</v>
+      </c>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
+        <v>35</v>
+      </c>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
+        <v>51</v>
+      </c>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
+        <v>52</v>
+      </c>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
+        <v>39</v>
+      </c>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
+        <v>40</v>
+      </c>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="38"/>
-      <c r="F35" s="38"/>
+        <v>41</v>
+      </c>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="38"/>
-      <c r="F36" s="38"/>
+        <v>42</v>
+      </c>
+      <c r="B36" s="17"/>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B37" s="22"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="22"/>
-      <c r="E37" s="38"/>
-      <c r="F37" s="38"/>
+        <v>43</v>
+      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="B38" s="22"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="22"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="38"/>
+        <v>56</v>
+      </c>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="34"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="38"/>
-      <c r="F39" s="38"/>
+        <v>59</v>
+      </c>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="34"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" s="22"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="38"/>
-      <c r="F40" s="38"/>
+        <v>60</v>
+      </c>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="34"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="51"/>
+        <v>91</v>
+      </c>
+      <c r="B41" s="46"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="47"/>
       <c r="F41"/>
       <c r="G41"/>
       <c r="H41"/>
@@ -2810,12 +2786,12 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B42" s="50"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="50"/>
-      <c r="E42" s="51"/>
+        <v>92</v>
+      </c>
+      <c r="B42" s="46"/>
+      <c r="C42" s="46"/>
+      <c r="D42" s="46"/>
+      <c r="E42" s="47"/>
       <c r="F42"/>
       <c r="G42"/>
       <c r="H42"/>
@@ -2823,12 +2799,12 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B43" s="50"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="50"/>
-      <c r="E43" s="51"/>
+        <v>93</v>
+      </c>
+      <c r="B43" s="46"/>
+      <c r="C43" s="46"/>
+      <c r="D43" s="46"/>
+      <c r="E43" s="47"/>
       <c r="F43"/>
       <c r="G43"/>
       <c r="H43"/>
@@ -2836,12 +2812,12 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B44" s="50"/>
-      <c r="C44" s="50"/>
-      <c r="D44" s="50"/>
-      <c r="E44" s="51"/>
+        <v>109</v>
+      </c>
+      <c r="B44" s="46"/>
+      <c r="C44" s="46"/>
+      <c r="D44" s="46"/>
+      <c r="E44" s="47"/>
       <c r="F44"/>
       <c r="G44"/>
       <c r="H44"/>
@@ -2849,12 +2825,12 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B45" s="50"/>
-      <c r="C45" s="50"/>
-      <c r="D45" s="50"/>
-      <c r="E45" s="51"/>
+        <v>94</v>
+      </c>
+      <c r="B45" s="46"/>
+      <c r="C45" s="46"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="47"/>
       <c r="F45"/>
       <c r="G45"/>
       <c r="H45"/>
@@ -2862,954 +2838,802 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
-      <c r="D46" s="21"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
+        <v>44</v>
+      </c>
+      <c r="B46" s="18"/>
+      <c r="C46" s="18"/>
+      <c r="D46" s="18"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
+        <v>88</v>
+      </c>
+      <c r="B47" s="18"/>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B48" s="23"/>
-      <c r="C48" s="23"/>
-      <c r="D48" s="23"/>
-      <c r="E48" s="38"/>
-      <c r="F48" s="38"/>
+        <v>61</v>
+      </c>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="34"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B49" s="24">
+        <v>8</v>
+      </c>
+      <c r="B49" s="21">
         <v>0.05</v>
       </c>
-      <c r="C49" s="38"/>
-      <c r="D49" s="38"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B50" s="25"/>
-      <c r="C50" s="47"/>
-      <c r="D50" s="47"/>
+        <v>45</v>
+      </c>
+      <c r="B50" s="22"/>
+      <c r="C50" s="43"/>
+      <c r="D50" s="43"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B51" s="25"/>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
+        <v>58</v>
+      </c>
+      <c r="B51" s="22"/>
+      <c r="C51" s="43"/>
+      <c r="D51" s="43"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B52" s="25"/>
-      <c r="C52" s="47"/>
-      <c r="D52" s="47"/>
+        <v>6</v>
+      </c>
+      <c r="B52" s="22"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="43"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="47"/>
-      <c r="D53" s="47"/>
+        <v>7</v>
+      </c>
+      <c r="B53" s="22"/>
+      <c r="C53" s="43"/>
+      <c r="D53" s="43"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B54" s="26"/>
-      <c r="C54" s="48"/>
-      <c r="D54" s="48"/>
+        <v>85</v>
+      </c>
+      <c r="B54" s="23"/>
+      <c r="C54" s="44"/>
+      <c r="D54" s="44"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="B55" s="26"/>
-      <c r="C55" s="48"/>
-      <c r="D55" s="48"/>
+        <v>86</v>
+      </c>
+      <c r="B55" s="23"/>
+      <c r="C55" s="44"/>
+      <c r="D55" s="44"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B56" s="26"/>
-      <c r="C56" s="48"/>
-      <c r="D56" s="48"/>
+        <v>87</v>
+      </c>
+      <c r="B56" s="23"/>
+      <c r="C56" s="44"/>
+      <c r="D56" s="44"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="25"/>
-      <c r="C57" s="47"/>
-      <c r="D57" s="47"/>
+      <c r="B57" s="22"/>
+      <c r="C57" s="43"/>
+      <c r="D57" s="43"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B58" s="25"/>
-      <c r="C58" s="47"/>
-      <c r="D58" s="47"/>
+        <v>4</v>
+      </c>
+      <c r="B58" s="22"/>
+      <c r="C58" s="43"/>
+      <c r="D58" s="43"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B59" s="25"/>
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
+        <v>101</v>
+      </c>
+      <c r="B59" s="22"/>
+      <c r="C59" s="43"/>
+      <c r="D59" s="43"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B60" s="25"/>
-      <c r="C60" s="47"/>
-      <c r="D60" s="47"/>
+        <v>6</v>
+      </c>
+      <c r="B60" s="22"/>
+      <c r="C60" s="43"/>
+      <c r="D60" s="43"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B61" s="25"/>
-      <c r="C61" s="47"/>
-      <c r="D61" s="47"/>
-      <c r="E61" s="53"/>
-      <c r="F61" s="53"/>
-      <c r="G61" s="53"/>
+        <v>7</v>
+      </c>
+      <c r="B61" s="22"/>
+      <c r="C61" s="43"/>
+      <c r="D61" s="43"/>
+      <c r="E61" s="49"/>
+      <c r="F61" s="49"/>
+      <c r="G61" s="49"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B62" s="25"/>
-      <c r="C62" s="47"/>
-      <c r="D62" s="47"/>
-      <c r="E62" s="53"/>
-      <c r="F62" s="53"/>
-      <c r="G62" s="53"/>
+        <v>3</v>
+      </c>
+      <c r="B62" s="22"/>
+      <c r="C62" s="43"/>
+      <c r="D62" s="43"/>
+      <c r="E62" s="49"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="49"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B63" s="25"/>
-      <c r="C63" s="47"/>
-      <c r="D63" s="47"/>
-      <c r="E63" s="53"/>
-      <c r="F63" s="53"/>
-      <c r="G63" s="53"/>
+        <v>82</v>
+      </c>
+      <c r="B63" s="22"/>
+      <c r="C63" s="43"/>
+      <c r="D63" s="43"/>
+      <c r="E63" s="49"/>
+      <c r="F63" s="49"/>
+      <c r="G63" s="49"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B64" s="25"/>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
-      <c r="E64" s="53"/>
-      <c r="F64" s="53"/>
-      <c r="G64" s="53"/>
-    </row>
-    <row r="65" spans="1:68" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="B64" s="22"/>
+      <c r="C64" s="43"/>
+      <c r="D64" s="43"/>
+      <c r="E64" s="49"/>
+      <c r="F64" s="49"/>
+      <c r="G64" s="49"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B65" s="25"/>
-      <c r="C65" s="47"/>
-      <c r="D65" s="47"/>
-      <c r="E65" s="53"/>
-      <c r="F65" s="53"/>
-      <c r="G65" s="53"/>
-    </row>
-    <row r="66" spans="1:68" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="B65" s="22"/>
+      <c r="C65" s="43"/>
+      <c r="D65" s="43"/>
+      <c r="E65" s="49"/>
+      <c r="F65" s="49"/>
+      <c r="G65" s="49"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="B66" s="52"/>
-      <c r="C66" s="54"/>
-      <c r="D66" s="54"/>
-      <c r="E66" s="55"/>
-      <c r="F66" s="56"/>
-      <c r="G66" s="56"/>
+        <v>98</v>
+      </c>
+      <c r="B66" s="48"/>
+      <c r="C66" s="50"/>
+      <c r="D66" s="50"/>
+      <c r="E66" s="51"/>
+      <c r="F66" s="52"/>
+      <c r="G66" s="52"/>
       <c r="H66"/>
       <c r="I66"/>
     </row>
-    <row r="67" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B67" s="52"/>
-      <c r="C67" s="54"/>
-      <c r="D67" s="54"/>
-      <c r="E67" s="55"/>
-      <c r="F67" s="56"/>
-      <c r="G67" s="56"/>
+        <v>99</v>
+      </c>
+      <c r="B67" s="48"/>
+      <c r="C67" s="50"/>
+      <c r="D67" s="50"/>
+      <c r="E67" s="51"/>
+      <c r="F67" s="52"/>
+      <c r="G67" s="52"/>
       <c r="H67"/>
       <c r="I67"/>
     </row>
-    <row r="68" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B68" s="52"/>
-      <c r="C68" s="54"/>
-      <c r="D68" s="54"/>
-      <c r="E68" s="55"/>
-      <c r="F68" s="56"/>
-      <c r="G68" s="56"/>
+        <v>100</v>
+      </c>
+      <c r="B68" s="48"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="50"/>
+      <c r="E68" s="51"/>
+      <c r="F68" s="52"/>
+      <c r="G68" s="52"/>
       <c r="H68"/>
       <c r="I68"/>
     </row>
-    <row r="69" spans="1:68" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B69" s="25"/>
-      <c r="C69" s="47"/>
-      <c r="D69" s="47"/>
-      <c r="E69" s="53"/>
-      <c r="F69" s="53"/>
-      <c r="G69" s="53"/>
-    </row>
-    <row r="70" spans="1:68" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="B69" s="22"/>
+      <c r="C69" s="43"/>
+      <c r="D69" s="43"/>
+      <c r="E69" s="49"/>
+      <c r="F69" s="49"/>
+      <c r="G69" s="49"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="B70" s="25"/>
-      <c r="C70" s="47"/>
-      <c r="D70" s="47"/>
-      <c r="E70" s="53"/>
-      <c r="F70" s="53"/>
-      <c r="G70" s="53"/>
-    </row>
-    <row r="71" spans="1:68" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="B70" s="22"/>
+      <c r="C70" s="43"/>
+      <c r="D70" s="43"/>
+      <c r="E70" s="49"/>
+      <c r="F70" s="49"/>
+      <c r="G70" s="49"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71" s="24"/>
+      <c r="C71" s="43"/>
+      <c r="D71" s="43"/>
+      <c r="E71" s="49"/>
+      <c r="F71" s="49"/>
+      <c r="G71" s="49"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B72" s="25"/>
+      <c r="C72" s="43"/>
+      <c r="D72" s="43"/>
+      <c r="E72" s="49"/>
+      <c r="F72" s="49"/>
+      <c r="G72" s="49"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B73" s="26"/>
+      <c r="C73" s="43"/>
+      <c r="D73" s="43"/>
+      <c r="E73" s="49"/>
+      <c r="F73" s="49"/>
+      <c r="G73" s="49"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B74" s="27"/>
+      <c r="C74" s="45"/>
+      <c r="D74" s="45"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" s="28"/>
+      <c r="C75" s="28"/>
+      <c r="D75" s="28"/>
+      <c r="E75" s="36"/>
+      <c r="F75" s="36"/>
+      <c r="G75" s="36"/>
+      <c r="H75" s="37"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="29"/>
+      <c r="C76" s="29"/>
+      <c r="D76" s="29"/>
+      <c r="E76" s="29"/>
+      <c r="F76" s="29"/>
+      <c r="G76" s="29"/>
+      <c r="H76" s="38"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="B77" s="53"/>
+      <c r="C77" s="57"/>
+      <c r="D77" s="57"/>
+      <c r="E77" s="57"/>
+      <c r="F77" s="57"/>
+      <c r="G77"/>
+      <c r="H77"/>
+      <c r="I77"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B71" s="27"/>
-      <c r="C71" s="47"/>
-      <c r="D71" s="47"/>
-      <c r="E71" s="53"/>
-      <c r="F71" s="53"/>
-      <c r="G71" s="53"/>
-    </row>
-    <row r="72" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A72" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B72" s="28"/>
-      <c r="C72" s="47"/>
-      <c r="D72" s="47"/>
-      <c r="E72" s="53"/>
-      <c r="F72" s="53"/>
-      <c r="G72" s="53"/>
-    </row>
-    <row r="73" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A73" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B73" s="29"/>
-      <c r="C73" s="47"/>
-      <c r="D73" s="47"/>
-      <c r="E73" s="53"/>
-      <c r="F73" s="53"/>
-      <c r="G73" s="53"/>
-    </row>
-    <row r="74" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A74" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="B74" s="30"/>
-      <c r="C74" s="47"/>
-      <c r="D74" s="47"/>
-      <c r="E74" s="38"/>
-      <c r="F74" s="38"/>
-      <c r="G74" s="38"/>
-      <c r="H74" s="34"/>
-      <c r="I74" s="34"/>
-      <c r="J74" s="15"/>
-      <c r="K74" s="15"/>
-      <c r="L74" s="15"/>
-      <c r="M74" s="15"/>
-      <c r="N74" s="15"/>
-      <c r="O74" s="15"/>
-      <c r="P74" s="15"/>
-      <c r="Q74" s="15"/>
-      <c r="R74" s="15"/>
-      <c r="S74" s="15"/>
-      <c r="T74" s="15"/>
-      <c r="U74" s="15"/>
-      <c r="V74" s="15"/>
-      <c r="W74" s="15"/>
-      <c r="X74" s="15"/>
-      <c r="Y74" s="15"/>
-      <c r="Z74" s="15"/>
-      <c r="AA74" s="15"/>
-      <c r="AB74" s="15"/>
-      <c r="AC74" s="15"/>
-      <c r="AD74" s="15"/>
-      <c r="AE74" s="15"/>
-      <c r="AF74" s="15"/>
-      <c r="AG74" s="15"/>
-      <c r="AH74" s="15"/>
-      <c r="AI74" s="15"/>
-      <c r="AJ74" s="15"/>
-      <c r="AK74" s="15"/>
-      <c r="AL74" s="15"/>
-      <c r="AM74" s="15"/>
-      <c r="AN74" s="15"/>
-      <c r="AO74" s="15"/>
-      <c r="AP74" s="15"/>
-      <c r="AQ74" s="15"/>
-      <c r="AR74" s="15"/>
-      <c r="AS74" s="15"/>
-      <c r="AT74" s="15"/>
-      <c r="AU74" s="15"/>
-      <c r="AV74" s="15"/>
-      <c r="AW74" s="15"/>
-      <c r="AX74" s="15"/>
-      <c r="AY74" s="15"/>
-      <c r="AZ74" s="15"/>
-      <c r="BA74" s="15"/>
-      <c r="BB74" s="15"/>
-      <c r="BC74" s="15"/>
-      <c r="BD74" s="15"/>
-      <c r="BE74" s="15"/>
-      <c r="BF74" s="15"/>
-      <c r="BG74" s="15"/>
-      <c r="BH74" s="15"/>
-      <c r="BI74" s="15"/>
-      <c r="BJ74" s="15"/>
-      <c r="BK74" s="15"/>
-      <c r="BL74" s="15"/>
-      <c r="BM74" s="15"/>
-      <c r="BN74" s="15"/>
-      <c r="BO74" s="15"/>
-      <c r="BP74" s="15"/>
-    </row>
-    <row r="75" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A75" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B75" s="63"/>
-      <c r="C75" s="47"/>
-      <c r="D75" s="47"/>
-      <c r="E75" s="38"/>
-      <c r="F75" s="38"/>
-      <c r="G75" s="38"/>
-      <c r="H75" s="34"/>
-      <c r="I75" s="34"/>
-      <c r="J75" s="15"/>
-      <c r="K75" s="15"/>
-      <c r="L75" s="15"/>
-      <c r="M75" s="15"/>
-      <c r="N75" s="15"/>
-      <c r="O75" s="15"/>
-      <c r="P75" s="15"/>
-      <c r="Q75" s="15"/>
-      <c r="R75" s="15"/>
-      <c r="S75" s="15"/>
-      <c r="T75" s="15"/>
-      <c r="U75" s="15"/>
-      <c r="V75" s="15"/>
-      <c r="W75" s="15"/>
-      <c r="X75" s="15"/>
-      <c r="Y75" s="15"/>
-      <c r="Z75" s="15"/>
-      <c r="AA75" s="15"/>
-      <c r="AB75" s="15"/>
-      <c r="AC75" s="15"/>
-      <c r="AD75" s="15"/>
-      <c r="AE75" s="15"/>
-      <c r="AF75" s="15"/>
-      <c r="AG75" s="15"/>
-      <c r="AH75" s="15"/>
-      <c r="AI75" s="15"/>
-      <c r="AJ75" s="15"/>
-      <c r="AK75" s="15"/>
-      <c r="AL75" s="15"/>
-      <c r="AM75" s="15"/>
-      <c r="AN75" s="15"/>
-      <c r="AO75" s="15"/>
-      <c r="AP75" s="15"/>
-      <c r="AQ75" s="15"/>
-      <c r="AR75" s="15"/>
-      <c r="AS75" s="15"/>
-      <c r="AT75" s="15"/>
-      <c r="AU75" s="15"/>
-      <c r="AV75" s="15"/>
-      <c r="AW75" s="15"/>
-      <c r="AX75" s="15"/>
-      <c r="AY75" s="15"/>
-      <c r="AZ75" s="15"/>
-      <c r="BA75" s="15"/>
-      <c r="BB75" s="15"/>
-      <c r="BC75" s="15"/>
-      <c r="BD75" s="15"/>
-      <c r="BE75" s="15"/>
-      <c r="BF75" s="15"/>
-      <c r="BG75" s="15"/>
-      <c r="BH75" s="15"/>
-      <c r="BI75" s="15"/>
-      <c r="BJ75" s="15"/>
-      <c r="BK75" s="15"/>
-      <c r="BL75" s="15"/>
-      <c r="BM75" s="15"/>
-      <c r="BN75" s="15"/>
-      <c r="BO75" s="15"/>
-      <c r="BP75" s="15"/>
-    </row>
-    <row r="76" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A76" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B76" s="31"/>
-      <c r="C76" s="49"/>
-      <c r="D76" s="49"/>
-    </row>
-    <row r="77" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A77" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B77" s="32"/>
-      <c r="C77" s="32"/>
-      <c r="D77" s="32"/>
-      <c r="E77" s="40"/>
-      <c r="F77" s="40"/>
-      <c r="G77" s="40"/>
-      <c r="H77" s="41"/>
-    </row>
-    <row r="78" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A78" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B78" s="33">
-        <v>5</v>
-      </c>
-      <c r="C78" s="33">
-        <v>15</v>
-      </c>
-      <c r="D78" s="33"/>
-      <c r="E78" s="33"/>
-      <c r="F78" s="33"/>
-      <c r="G78" s="33"/>
-      <c r="H78" s="42"/>
-    </row>
-    <row r="79" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A79" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="B79" s="57"/>
-      <c r="C79" s="61"/>
-      <c r="D79" s="61"/>
-      <c r="E79" s="61"/>
-      <c r="F79" s="61"/>
+      <c r="B78" s="40"/>
+      <c r="C78" s="56"/>
+      <c r="D78" s="56"/>
+      <c r="E78" s="57"/>
+      <c r="F78" s="57"/>
+      <c r="G78"/>
+      <c r="H78"/>
+      <c r="I78"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B79" s="40"/>
+      <c r="C79" s="57"/>
+      <c r="D79" s="57"/>
+      <c r="E79" s="57"/>
+      <c r="F79" s="57"/>
       <c r="G79"/>
       <c r="H79"/>
       <c r="I79"/>
     </row>
-    <row r="80" spans="1:68" x14ac:dyDescent="0.25">
-      <c r="A80" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="B80" s="44"/>
-      <c r="C80" s="60"/>
-      <c r="D80" s="60"/>
-      <c r="E80" s="61"/>
-      <c r="F80" s="61"/>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="40" t="s">
+        <v>102</v>
+      </c>
+      <c r="B80" s="40"/>
+      <c r="C80" s="57"/>
+      <c r="D80" s="57"/>
+      <c r="E80" s="57"/>
+      <c r="F80" s="57"/>
       <c r="G80"/>
       <c r="H80"/>
       <c r="I80"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="44" t="s">
-        <v>72</v>
-      </c>
-      <c r="B81" s="44"/>
-      <c r="C81" s="61"/>
-      <c r="D81" s="61"/>
-      <c r="E81" s="61"/>
-      <c r="F81" s="61"/>
+      <c r="A81" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B81" s="40"/>
+      <c r="C81" s="57"/>
+      <c r="D81" s="57"/>
+      <c r="E81" s="57"/>
+      <c r="F81" s="57"/>
       <c r="G81"/>
       <c r="H81"/>
       <c r="I81"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="B82" s="44"/>
-      <c r="C82" s="61"/>
-      <c r="D82" s="61"/>
-      <c r="E82" s="61"/>
-      <c r="F82" s="61"/>
+      <c r="A82" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="B82" s="40"/>
+      <c r="C82" s="57"/>
+      <c r="D82" s="57"/>
+      <c r="E82" s="57"/>
+      <c r="F82" s="57"/>
       <c r="G82"/>
       <c r="H82"/>
       <c r="I82"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="B83" s="44"/>
-      <c r="C83" s="61"/>
-      <c r="D83" s="61"/>
-      <c r="E83" s="61"/>
-      <c r="F83" s="61"/>
+      <c r="A83" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B83" s="40"/>
+      <c r="C83" s="56"/>
+      <c r="D83" s="56"/>
+      <c r="E83" s="57"/>
+      <c r="F83" s="57"/>
       <c r="G83"/>
       <c r="H83"/>
       <c r="I83"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="B84" s="44"/>
-      <c r="C84" s="61"/>
-      <c r="D84" s="61"/>
-      <c r="E84" s="61"/>
-      <c r="F84" s="61"/>
+      <c r="A84" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B84" s="40"/>
+      <c r="C84" s="57"/>
+      <c r="D84" s="57"/>
+      <c r="E84" s="57"/>
+      <c r="F84" s="57"/>
       <c r="G84"/>
       <c r="H84"/>
       <c r="I84"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="B85" s="44"/>
-      <c r="C85" s="60"/>
-      <c r="D85" s="60"/>
-      <c r="E85" s="61"/>
-      <c r="F85" s="61"/>
+      <c r="A85" s="40" t="s">
+        <v>103</v>
+      </c>
+      <c r="B85" s="40"/>
+      <c r="C85" s="57"/>
+      <c r="D85" s="57"/>
+      <c r="E85" s="57"/>
+      <c r="F85" s="57"/>
       <c r="G85"/>
       <c r="H85"/>
       <c r="I85"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="44" t="s">
-        <v>74</v>
-      </c>
-      <c r="B86" s="44"/>
-      <c r="C86" s="61"/>
-      <c r="D86" s="61"/>
-      <c r="E86" s="61"/>
-      <c r="F86" s="61"/>
+      <c r="A86" s="40" t="s">
+        <v>111</v>
+      </c>
+      <c r="B86" s="40"/>
+      <c r="C86" s="57"/>
+      <c r="D86" s="57"/>
+      <c r="E86" s="57"/>
+      <c r="F86" s="57"/>
       <c r="G86"/>
       <c r="H86"/>
       <c r="I86"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="B87" s="44"/>
-      <c r="C87" s="61"/>
-      <c r="D87" s="61"/>
-      <c r="E87" s="61"/>
-      <c r="F87" s="61"/>
+      <c r="A87" s="40" t="s">
+        <v>73</v>
+      </c>
+      <c r="B87" s="40"/>
+      <c r="C87" s="57"/>
+      <c r="D87" s="57"/>
+      <c r="E87" s="57"/>
+      <c r="F87" s="57"/>
       <c r="G87"/>
       <c r="H87"/>
       <c r="I87"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="44" t="s">
-        <v>113</v>
-      </c>
-      <c r="B88" s="44"/>
-      <c r="C88" s="61"/>
-      <c r="D88" s="61"/>
-      <c r="E88" s="61"/>
-      <c r="F88" s="61"/>
+      <c r="A88" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B88" s="54"/>
+      <c r="C88" s="57"/>
+      <c r="D88" s="57"/>
+      <c r="E88" s="57"/>
+      <c r="F88" s="57"/>
       <c r="G88"/>
       <c r="H88"/>
       <c r="I88"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="44" t="s">
-        <v>75</v>
-      </c>
-      <c r="B89" s="44"/>
-      <c r="C89" s="61"/>
-      <c r="D89" s="61"/>
-      <c r="E89" s="61"/>
-      <c r="F89" s="61"/>
+      <c r="A89" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B89" s="54"/>
+      <c r="C89" s="57"/>
+      <c r="D89" s="57"/>
+      <c r="E89" s="57"/>
+      <c r="F89" s="57"/>
       <c r="G89"/>
       <c r="H89"/>
       <c r="I89"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="B90" s="58"/>
-      <c r="C90" s="61"/>
-      <c r="D90" s="61"/>
-      <c r="E90" s="61"/>
-      <c r="F90" s="61"/>
+      <c r="A90" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="B90" s="54"/>
+      <c r="C90" s="57"/>
+      <c r="D90" s="57"/>
+      <c r="E90" s="57"/>
+      <c r="F90" s="57"/>
       <c r="G90"/>
       <c r="H90"/>
       <c r="I90"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="B91" s="58"/>
-      <c r="C91" s="61"/>
-      <c r="D91" s="61"/>
-      <c r="E91" s="61"/>
-      <c r="F91" s="61"/>
+      <c r="A91" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="B91" s="54"/>
+      <c r="C91" s="57"/>
+      <c r="D91" s="57"/>
+      <c r="E91" s="57"/>
+      <c r="F91" s="57"/>
       <c r="G91"/>
       <c r="H91"/>
       <c r="I91"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="45" t="s">
-        <v>106</v>
-      </c>
-      <c r="B92" s="58"/>
-      <c r="C92" s="61"/>
-      <c r="D92" s="61"/>
-      <c r="E92" s="61"/>
-      <c r="F92" s="61"/>
+      <c r="A92" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B92" s="54"/>
+      <c r="C92" s="57"/>
+      <c r="D92" s="57"/>
+      <c r="E92" s="57"/>
+      <c r="F92" s="57"/>
       <c r="G92"/>
       <c r="H92"/>
       <c r="I92"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="B93" s="58"/>
-      <c r="C93" s="61"/>
-      <c r="D93" s="61"/>
-      <c r="E93" s="61"/>
-      <c r="F93" s="61"/>
+      <c r="A93" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="B93" s="54"/>
+      <c r="C93" s="57"/>
+      <c r="D93" s="57"/>
+      <c r="E93" s="57"/>
+      <c r="F93" s="57"/>
       <c r="G93"/>
       <c r="H93"/>
       <c r="I93"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="B94" s="58"/>
-      <c r="C94" s="61"/>
-      <c r="D94" s="61"/>
-      <c r="E94" s="61"/>
-      <c r="F94" s="61"/>
+      <c r="A94" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B94" s="54"/>
+      <c r="C94" s="57"/>
+      <c r="D94" s="57"/>
+      <c r="E94" s="57"/>
+      <c r="F94" s="57"/>
       <c r="G94"/>
       <c r="H94"/>
       <c r="I94"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="45" t="s">
-        <v>69</v>
-      </c>
-      <c r="B95" s="58"/>
-      <c r="C95" s="61"/>
-      <c r="D95" s="61"/>
-      <c r="E95" s="61"/>
-      <c r="F95" s="61"/>
+      <c r="A95" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="B95" s="54"/>
+      <c r="C95" s="57"/>
+      <c r="D95" s="57"/>
+      <c r="E95" s="57"/>
+      <c r="F95" s="57"/>
       <c r="G95"/>
       <c r="H95"/>
       <c r="I95"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="B96" s="58"/>
-      <c r="C96" s="61"/>
-      <c r="D96" s="61"/>
-      <c r="E96" s="61"/>
-      <c r="F96" s="61"/>
+      <c r="A96" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="B96" s="54"/>
+      <c r="C96" s="57"/>
+      <c r="D96" s="57"/>
+      <c r="E96" s="57"/>
+      <c r="F96" s="57"/>
       <c r="G96"/>
       <c r="H96"/>
       <c r="I96"/>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="B97" s="58"/>
-      <c r="C97" s="61"/>
-      <c r="D97" s="61"/>
-      <c r="E97" s="61"/>
-      <c r="F97" s="61"/>
+      <c r="A97" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B97" s="54"/>
+      <c r="C97" s="57"/>
+      <c r="D97" s="57"/>
+      <c r="E97" s="57"/>
+      <c r="F97" s="57"/>
       <c r="G97"/>
       <c r="H97"/>
       <c r="I97"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="B98" s="58"/>
-      <c r="C98" s="61"/>
-      <c r="D98" s="61"/>
-      <c r="E98" s="61"/>
-      <c r="F98" s="61"/>
+      <c r="A98" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="B98" s="54"/>
+      <c r="C98" s="57"/>
+      <c r="D98" s="57"/>
+      <c r="E98" s="57"/>
+      <c r="F98" s="57"/>
       <c r="G98"/>
       <c r="H98"/>
       <c r="I98"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="B99" s="58"/>
-      <c r="C99" s="61"/>
-      <c r="D99" s="61"/>
-      <c r="E99" s="61"/>
-      <c r="F99" s="61"/>
+      <c r="A99" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="B99" s="54"/>
+      <c r="C99" s="57"/>
+      <c r="D99" s="57"/>
+      <c r="E99" s="58"/>
+      <c r="F99" s="57"/>
       <c r="G99"/>
       <c r="H99"/>
       <c r="I99"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="B100" s="58"/>
-      <c r="C100" s="61"/>
-      <c r="D100" s="61"/>
-      <c r="E100" s="61"/>
-      <c r="F100" s="61"/>
+      <c r="A100" s="41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B100" s="54"/>
+      <c r="C100" s="57"/>
+      <c r="D100" s="57"/>
+      <c r="E100" s="58"/>
+      <c r="F100" s="57"/>
       <c r="G100"/>
       <c r="H100"/>
       <c r="I100"/>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="B101" s="58"/>
-      <c r="C101" s="61"/>
-      <c r="D101" s="61"/>
-      <c r="E101" s="62"/>
-      <c r="F101" s="61"/>
+      <c r="A101" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B101" s="54"/>
+      <c r="C101" s="57"/>
+      <c r="D101" s="57"/>
+      <c r="E101" s="57"/>
+      <c r="F101" s="57"/>
       <c r="G101"/>
       <c r="H101"/>
       <c r="I101"/>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="45" t="s">
-        <v>108</v>
-      </c>
-      <c r="B102" s="58"/>
-      <c r="C102" s="61"/>
-      <c r="D102" s="61"/>
-      <c r="E102" s="62"/>
-      <c r="F102" s="61"/>
+      <c r="A102" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B102" s="54"/>
+      <c r="C102" s="57"/>
+      <c r="D102" s="57"/>
+      <c r="E102" s="57"/>
+      <c r="F102" s="57"/>
       <c r="G102"/>
       <c r="H102"/>
       <c r="I102"/>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="B103" s="58"/>
-      <c r="C103" s="61"/>
-      <c r="D103" s="61"/>
-      <c r="E103" s="61"/>
-      <c r="F103" s="61"/>
+      <c r="A103" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B103" s="40"/>
+      <c r="C103" s="57"/>
+      <c r="D103" s="57"/>
+      <c r="E103" s="57"/>
+      <c r="F103" s="57"/>
       <c r="G103"/>
       <c r="H103"/>
       <c r="I103"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="45" t="s">
-        <v>81</v>
-      </c>
-      <c r="B104" s="58"/>
-      <c r="C104" s="61"/>
-      <c r="D104" s="61"/>
-      <c r="E104" s="61"/>
-      <c r="F104" s="61"/>
+      <c r="A104" s="41" t="s">
+        <v>80</v>
+      </c>
+      <c r="B104" s="40"/>
+      <c r="C104" s="57"/>
+      <c r="D104" s="57"/>
+      <c r="E104" s="57"/>
+      <c r="F104" s="57"/>
       <c r="G104"/>
       <c r="H104"/>
       <c r="I104"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="45" t="s">
-        <v>71</v>
-      </c>
-      <c r="B105" s="44"/>
-      <c r="C105" s="61"/>
-      <c r="D105" s="61"/>
-      <c r="E105" s="61"/>
-      <c r="F105" s="61"/>
+      <c r="A105" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="B105" s="40"/>
+      <c r="C105" s="57"/>
+      <c r="D105" s="57"/>
+      <c r="E105" s="57"/>
+      <c r="F105" s="57"/>
       <c r="G105"/>
       <c r="H105"/>
       <c r="I105"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="B106" s="44"/>
-      <c r="C106" s="61"/>
-      <c r="D106" s="61"/>
-      <c r="E106" s="61"/>
-      <c r="F106" s="61"/>
+      <c r="A106" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="B106" s="40"/>
+      <c r="C106" s="57"/>
+      <c r="D106" s="57"/>
+      <c r="E106" s="57"/>
+      <c r="F106" s="57"/>
       <c r="G106"/>
       <c r="H106"/>
       <c r="I106"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="45" t="s">
-        <v>109</v>
-      </c>
-      <c r="B107" s="44"/>
-      <c r="C107" s="61"/>
-      <c r="D107" s="61"/>
-      <c r="E107" s="61"/>
-      <c r="F107" s="61"/>
+      <c r="A107" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="B107" s="40"/>
+      <c r="C107" s="57"/>
+      <c r="D107" s="57"/>
+      <c r="E107" s="57"/>
+      <c r="F107" s="57"/>
       <c r="G107"/>
       <c r="H107"/>
       <c r="I107"/>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="B108" s="44"/>
-      <c r="C108" s="61"/>
-      <c r="D108" s="61"/>
-      <c r="E108" s="61"/>
-      <c r="F108" s="61"/>
+      <c r="A108" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="B108" s="40"/>
+      <c r="C108" s="57"/>
+      <c r="D108" s="57"/>
+      <c r="E108" s="57"/>
+      <c r="F108" s="57"/>
       <c r="G108"/>
       <c r="H108"/>
       <c r="I108"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="B109" s="44"/>
-      <c r="C109" s="61"/>
-      <c r="D109" s="61"/>
-      <c r="E109" s="61"/>
-      <c r="F109" s="61"/>
+      <c r="A109" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="B109" s="40"/>
+      <c r="C109" s="57"/>
+      <c r="D109" s="57"/>
+      <c r="E109" s="57"/>
+      <c r="F109" s="57"/>
       <c r="G109"/>
       <c r="H109"/>
       <c r="I109"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="45" t="s">
-        <v>97</v>
-      </c>
-      <c r="B110" s="44"/>
-      <c r="C110" s="61"/>
-      <c r="D110" s="61"/>
-      <c r="E110" s="61"/>
-      <c r="F110" s="61"/>
+      <c r="A110" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="B110" s="40"/>
+      <c r="C110" s="57"/>
+      <c r="D110" s="57"/>
+      <c r="E110" s="57"/>
+      <c r="F110" s="57"/>
       <c r="G110"/>
       <c r="H110"/>
       <c r="I110"/>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="45" t="s">
-        <v>98</v>
-      </c>
-      <c r="B111" s="44"/>
-      <c r="C111" s="61"/>
-      <c r="D111" s="61"/>
-      <c r="E111" s="61"/>
-      <c r="F111" s="61"/>
+      <c r="A111" s="40" t="s">
+        <v>116</v>
+      </c>
+      <c r="B111" s="40"/>
+      <c r="C111" s="57"/>
+      <c r="D111" s="57"/>
+      <c r="E111" s="57"/>
+      <c r="F111" s="57"/>
       <c r="G111"/>
       <c r="H111"/>
       <c r="I111"/>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="B112" s="44"/>
-      <c r="C112" s="61"/>
-      <c r="D112" s="61"/>
-      <c r="E112" s="61"/>
-      <c r="F112" s="61"/>
+      <c r="A112" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="B112" s="55"/>
+      <c r="C112" s="57"/>
+      <c r="D112" s="57"/>
+      <c r="E112" s="57"/>
+      <c r="F112" s="57"/>
       <c r="G112"/>
       <c r="H112"/>
       <c r="I112"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="44" t="s">
-        <v>118</v>
-      </c>
-      <c r="B113" s="44"/>
-      <c r="C113" s="61"/>
-      <c r="D113" s="61"/>
-      <c r="E113" s="61"/>
-      <c r="F113" s="61"/>
-      <c r="G113"/>
-      <c r="H113"/>
-      <c r="I113"/>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="46" t="s">
-        <v>99</v>
-      </c>
-      <c r="B114" s="59"/>
-      <c r="C114" s="61"/>
-      <c r="D114" s="61"/>
-      <c r="E114" s="61"/>
-      <c r="F114" s="61"/>
-      <c r="G114"/>
-      <c r="H114"/>
-      <c r="I114"/>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C115" s="38"/>
-      <c r="D115" s="38"/>
-      <c r="E115" s="38"/>
-      <c r="F115" s="38"/>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C116" s="38"/>
-      <c r="D116" s="38"/>
-      <c r="E116" s="38"/>
-      <c r="F116" s="38"/>
+    <row r="113" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C113" s="34"/>
+      <c r="D113" s="34"/>
+      <c r="E113" s="34"/>
+      <c r="F113" s="34"/>
+    </row>
+    <row r="114" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C114" s="34"/>
+      <c r="D114" s="34"/>
+      <c r="E114" s="34"/>
+      <c r="F114" s="34"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="363" yWindow="440" count="6">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74:D75">
-      <formula1>0</formula1>
-      <formula2>10</formula2>
-    </dataValidation>
+  <dataValidations xWindow="363" yWindow="440" count="5">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B72:D73">
       <formula1>0</formula1>
       <formula2>10000000000</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B76:D76">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B74:D74">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
@@ -3817,7 +3641,7 @@
       <formula1>-10000</formula1>
       <formula2>10000</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B77:D77">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75:D75">
       <formula1>1</formula1>
       <formula2>100</formula2>
     </dataValidation>
@@ -3846,32 +3670,32 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove more rows from control panel
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -15,27 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
-  <si>
-    <t>recent_time</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>age_breakpoints</t>
   </si>
   <si>
     <t>explicit</t>
-  </si>
-  <si>
-    <t>scenario_end_time</t>
-  </si>
-  <si>
-    <t>current_time</t>
-  </si>
-  <si>
-    <t>scenario_start_time</t>
-  </si>
-  <si>
-    <t>scenario_full_time</t>
   </si>
   <si>
     <t>country</t>
@@ -56,52 +41,7 @@
     <t>runge_kutta</t>
   </si>
   <si>
-    <t>start_time</t>
-  </si>
-  <si>
     <t>Fiji</t>
-  </si>
-  <si>
-    <t>early_time</t>
-  </si>
-  <si>
-    <t>economics_start_time</t>
-  </si>
-  <si>
-    <t>report_start_time</t>
-  </si>
-  <si>
-    <t>report_end_time</t>
-  </si>
-  <si>
-    <t>report_step_time</t>
-  </si>
-  <si>
-    <t>start_mdr_introduce_time</t>
-  </si>
-  <si>
-    <t>end_mdr_introduce_time</t>
-  </si>
-  <si>
-    <t>xdr_introduce_time</t>
-  </si>
-  <si>
-    <t>plot_end_time</t>
-  </si>
-  <si>
-    <t>plot_start_time</t>
-  </si>
-  <si>
-    <t>cost_curve_start_time</t>
-  </si>
-  <si>
-    <t>cost_curve_end_time</t>
-  </si>
-  <si>
-    <t>cost_curve_step_time</t>
-  </si>
-  <si>
-    <t>reference_time</t>
   </si>
 </sst>
 </file>
@@ -111,7 +51,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,20 +89,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="3" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="6" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -182,7 +108,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,23 +129,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -288,23 +203,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="664">
+  <cellStyleXfs count="663">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
@@ -968,45 +868,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="9" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="9" fillId="4" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="663" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="664">
+  <cellStyles count="663">
     <cellStyle name="Comma 2" xfId="4"/>
     <cellStyle name="Comma 2 2" xfId="5"/>
-    <cellStyle name="Input" xfId="663" builtinId="20"/>
     <cellStyle name="Input 2" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="6"/>
@@ -1972,288 +1853,67 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="25.5703125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="14"/>
+    <col min="1" max="1" width="52.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="25.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="10" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>7</v>
+      <c r="A1" s="3" t="s">
+        <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>14</v>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
+      <c r="A2" s="11" t="s">
+        <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
+      <c r="B2" s="12">
+        <v>5</v>
+      </c>
+      <c r="C2" s="12">
+        <v>15</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18"/>
-      <c r="I18"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19"/>
-      <c r="I19"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20"/>
-      <c r="I20"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
-        <v>1</v>
-      </c>
-      <c r="B24" s="23">
-        <v>5</v>
-      </c>
-      <c r="C24" s="23">
-        <v>15</v>
-      </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="24"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="363" yWindow="440" count="1">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:D23">
-      <formula1>-10000</formula1>
-      <formula2>10000</formula2>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2274,32 +1934,32 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move country selection to GUI
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -8,40 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="control_panel" sheetId="4" r:id="rId1"/>
-    <sheet name="dropdown_lists" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>age_breakpoints</t>
-  </si>
-  <si>
-    <t>explicit</t>
-  </si>
-  <si>
-    <t>country</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>scipy</t>
-  </si>
-  <si>
-    <t>na</t>
-  </si>
-  <si>
-    <t>runge_kutta</t>
-  </si>
-  <si>
-    <t>Fiji</t>
   </si>
 </sst>
 </file>
@@ -51,7 +26,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,23 +55,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="6" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,7 +68,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,14 +87,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -154,15 +108,6 @@
       </top>
       <bottom style="thin">
         <color theme="0"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -869,21 +814,15 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="663">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -1853,117 +1792,51 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="52.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="25.5703125" style="5" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" style="10" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="10" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="10"/>
+    <col min="1" max="1" width="52.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="25.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>8</v>
+      <c r="B1" s="6">
+        <v>5</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
+      <c r="C1" s="6">
+        <v>15</v>
+      </c>
+      <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="7"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="12">
-        <v>5</v>
-      </c>
-      <c r="C2" s="12">
-        <v>15</v>
-      </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="0" tint="-4.9989318521683403E-2"/>
-  </sheetPr>
-  <dimension ref="A2:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection password="D0CB" sheet="1" objects="1" scenarios="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Remove all information from control panel
</commit_message>
<xml_diff>
--- a/autumn/xls/control_panel.xlsx
+++ b/autumn/xls/control_panel.xlsx
@@ -14,11 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>age_breakpoints</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26,7 +22,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,19 +52,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="6" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -81,14 +70,8 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -111,43 +94,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="663">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -814,15 +760,12 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="663">
     <cellStyle name="Comma 2" xfId="4"/>
@@ -1792,9 +1735,11 @@
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1807,33 +1752,17 @@
     <col min="9" max="9" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6">
-        <v>5</v>
-      </c>
-      <c r="C1" s="6">
-        <v>15</v>
-      </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="7"/>
+    <row r="1" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>